<commit_message>
study: add 30 word
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
     <sheet name="Update_ea9e" sheetId="2" r:id="rId2"/>
+    <sheet name="Update_3987" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -398,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -429,7 +430,7 @@
     <row r="2">
       <c r="A2" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>e9589940-742b-43f2-ac65-fc45bb80e027</v>
+        <v>2855e402-1dfa-4dc2-8840-cebd848fa19c</v>
       </c>
       <c r="B2">
         <v>26</v>
@@ -450,7 +451,7 @@
     <row r="3">
       <c r="A3" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>df96699a-5763-442b-95fc-cbb91f19f173</v>
+        <v>d90b062b-c464-4c5c-bf4d-2d250fee42b4</v>
       </c>
       <c r="B3">
         <v>26</v>
@@ -471,7 +472,7 @@
     <row r="4">
       <c r="A4" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>b404c93e-c748-4648-9faf-190a9ad5dba8</v>
+        <v>d670b0d5-a0f9-4e3d-be7e-7539b709f4bf</v>
       </c>
       <c r="B4">
         <v>26</v>
@@ -492,7 +493,7 @@
     <row r="5">
       <c r="A5" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>7c8e0bd5-ee8c-41f0-bdc6-7d308bfa4ab5</v>
+        <v>0b08724a-3034-4e5c-9eed-a809189bff3a</v>
       </c>
       <c r="B5">
         <v>26</v>
@@ -513,7 +514,7 @@
     <row r="6">
       <c r="A6" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>9f86076e-64fe-4a74-aaba-1d8f05735eac</v>
+        <v>4152b846-3f6e-4b76-b48c-320c8d9bf98d</v>
       </c>
       <c r="B6">
         <v>26</v>
@@ -534,7 +535,7 @@
     <row r="7">
       <c r="A7" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>559fe9af-e60b-4194-83d4-fc1806e45563</v>
+        <v>f9c612cb-22a0-4f9d-a949-c179e45f0655</v>
       </c>
       <c r="B7">
         <v>26</v>
@@ -555,7 +556,7 @@
     <row r="8">
       <c r="A8" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>4b845d2c-e2c1-4fdd-8548-32d690072f4e</v>
+        <v>53af5326-467e-4e15-a189-ec4723760626</v>
       </c>
       <c r="B8">
         <v>26</v>
@@ -576,7 +577,7 @@
     <row r="9">
       <c r="A9" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>9d47ec42-31eb-4357-bfc0-45d200872d21</v>
+        <v>faab9a2e-d127-4a38-abf1-879e33beef60</v>
       </c>
       <c r="B9">
         <v>26</v>
@@ -597,7 +598,7 @@
     <row r="10">
       <c r="A10" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>4ff90ae3-5e15-4a78-94f0-735775606ffa</v>
+        <v>da3b1816-173a-4493-ad15-7beb97e72ba5</v>
       </c>
       <c r="B10">
         <v>26</v>
@@ -618,7 +619,7 @@
     <row r="11">
       <c r="A11" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>a71d8989-9fc3-4461-9b1c-aee9819e51f1</v>
+        <v>e98b5079-2952-47db-afac-31e8e8b2ded1</v>
       </c>
       <c r="B11">
         <v>26</v>
@@ -639,7 +640,7 @@
     <row r="12">
       <c r="A12" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>28ba2cea-e9b7-444f-bf0c-5f414436bfba</v>
+        <v>6834a067-2935-4767-b07e-7e28c2af50bc</v>
       </c>
       <c r="B12">
         <v>26</v>
@@ -660,7 +661,7 @@
     <row r="13">
       <c r="A13" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>8aa2c4b0-1c7c-4945-82fa-8382cdf4ab6f</v>
+        <v>eec73fe0-6f13-4d23-b16e-304b453fd1eb</v>
       </c>
       <c r="B13">
         <v>26</v>
@@ -681,7 +682,7 @@
     <row r="14">
       <c r="A14" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>2cb14656-58ab-4802-975a-080e7e9be699</v>
+        <v>d82e9755-cb4a-4e76-b2d1-c22e9bbd3e4a</v>
       </c>
       <c r="B14">
         <v>26</v>
@@ -702,7 +703,7 @@
     <row r="15">
       <c r="A15" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>7acaa11d-729f-42b7-9f09-0955a4f7d42c</v>
+        <v>80af4f65-e319-4276-abc7-c4b93cfb684f</v>
       </c>
       <c r="B15">
         <v>26</v>
@@ -723,7 +724,7 @@
     <row r="16">
       <c r="A16" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>1b1a8ac3-85cf-492c-8008-e9953d15f894</v>
+        <v>66eb9a3b-e5cf-4572-af26-c0ced46a6a41</v>
       </c>
       <c r="B16">
         <v>26</v>
@@ -744,7 +745,7 @@
     <row r="17">
       <c r="A17" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>c128256f-c15c-4d39-8060-be37724208b0</v>
+        <v>6d66f4e3-1575-453b-9c56-b2e35ae6f572</v>
       </c>
       <c r="B17">
         <v>26</v>
@@ -765,7 +766,7 @@
     <row r="18">
       <c r="A18" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>38610c4a-fe8b-4d51-8168-17aa92f7ff9d</v>
+        <v>c61cf54e-76e9-4c4f-a546-be16ad5e5bcf</v>
       </c>
       <c r="B18">
         <v>26</v>
@@ -786,7 +787,7 @@
     <row r="19">
       <c r="A19" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>9f62ae08-61be-4094-804d-cc8013c0a33e</v>
+        <v>75d97f77-6607-497c-a34c-c08e4276bc76</v>
       </c>
       <c r="B19">
         <v>26</v>
@@ -807,7 +808,7 @@
     <row r="20">
       <c r="A20" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>63b355e6-86e1-4e37-9a68-1b9447be1780</v>
+        <v>e2745e17-f355-4999-984f-246339ace9e7</v>
       </c>
       <c r="B20">
         <v>26</v>
@@ -828,7 +829,7 @@
     <row r="21">
       <c r="A21" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>d7aeac52-22a8-48c9-b3dc-9c983249b645</v>
+        <v>d883b560-e598-4399-b67a-fbd255f88070</v>
       </c>
       <c r="B21">
         <v>26</v>
@@ -849,7 +850,7 @@
     <row r="22">
       <c r="A22" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>52a8de1b-1439-4e9f-8889-7ca55f5db9d4</v>
+        <v>861042fb-7382-4b86-b5dc-6f8a0f267c2b</v>
       </c>
       <c r="B22">
         <v>26</v>
@@ -870,7 +871,7 @@
     <row r="23">
       <c r="A23" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>acf897b0-c82a-4b38-a0ec-7b014ca4e7f1</v>
+        <v>2c327c19-447e-45c6-8278-14aa65293f96</v>
       </c>
       <c r="B23">
         <v>26</v>
@@ -891,7 +892,7 @@
     <row r="24">
       <c r="A24" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>e802aafa-29e6-435e-ac76-b39e6011f747</v>
+        <v>1c7e5e1d-737d-4a0f-9124-6e6415aaab50</v>
       </c>
       <c r="B24">
         <v>26</v>
@@ -912,7 +913,7 @@
     <row r="25">
       <c r="A25" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>43076760-6d75-4fe1-a6a3-dbf273a1ed69</v>
+        <v>046efda8-e3b4-4698-a754-cacebf1c90e0</v>
       </c>
       <c r="B25">
         <v>26</v>
@@ -933,7 +934,7 @@
     <row r="26">
       <c r="A26" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>15049f9d-7c2c-4f70-b7dd-d6fcb78f6f94</v>
+        <v>7040324e-e5a2-44f4-9535-b2cc9cbdb924</v>
       </c>
       <c r="B26">
         <v>26</v>
@@ -954,7 +955,7 @@
     <row r="27">
       <c r="A27" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>0f3bd34e-ee98-4fee-b98b-23644a117b3c</v>
+        <v>988a2983-945c-4cf0-ba48-152e92f249c4</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -975,7 +976,7 @@
     <row r="28">
       <c r="A28" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>04388592-876e-4575-adcd-e0fe1be365b3</v>
+        <v>928cac87-df35-4693-90eb-0b7ac9ba4f7c</v>
       </c>
       <c r="B28">
         <v>26</v>
@@ -996,7 +997,7 @@
     <row r="29">
       <c r="A29" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>7344acb7-f1a2-4fc1-b76e-94122a109c7a</v>
+        <v>470241db-5ef4-4605-923a-0f067329f20f</v>
       </c>
       <c r="B29">
         <v>26</v>
@@ -1017,7 +1018,7 @@
     <row r="30">
       <c r="A30" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>5677ba8e-838f-4b4f-b705-0df492ebdf1b</v>
+        <v>972036e4-0ba9-4393-b01e-adb398bcbf0c</v>
       </c>
       <c r="B30">
         <v>26</v>
@@ -1038,7 +1039,7 @@
     <row r="31">
       <c r="A31" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>e36b0ed5-6805-48e8-ad47-328b2dfa37ec</v>
+        <v>fefbe098-b8f8-40ef-87d2-ea757ae401e2</v>
       </c>
       <c r="B31">
         <v>26</v>
@@ -1059,7 +1060,7 @@
     <row r="32">
       <c r="A32" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>3208a29f-cd43-40f0-a981-777899ce22c0</v>
+        <v>7ced7a2e-75de-4804-ac90-20e3e958d965</v>
       </c>
       <c r="B32">
         <v>27</v>
@@ -1080,7 +1081,7 @@
     <row r="33">
       <c r="A33" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>ee5e822f-b746-4dcf-8c93-863f4fcf61f0</v>
+        <v>4b5d71f1-69c8-4d40-917c-56ed60fa341a</v>
       </c>
       <c r="B33">
         <v>27</v>
@@ -1101,7 +1102,7 @@
     <row r="34">
       <c r="A34" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>19720a6e-bfec-46ab-a32d-98ff082191a7</v>
+        <v>f249b615-9ce7-490b-aeb1-e7fb50956f75</v>
       </c>
       <c r="B34">
         <v>27</v>
@@ -1122,7 +1123,7 @@
     <row r="35">
       <c r="A35" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>fdc92382-011c-40e3-a9c5-499c24fccbae</v>
+        <v>33645007-d97b-4e05-9fbb-18ce6453df08</v>
       </c>
       <c r="B35">
         <v>27</v>
@@ -1143,7 +1144,7 @@
     <row r="36">
       <c r="A36" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>94ad9cc2-958c-450f-820f-10508e3e81c3</v>
+        <v>c1f5fd98-6823-4cd2-8332-437b40d1cdbb</v>
       </c>
       <c r="B36">
         <v>27</v>
@@ -1164,7 +1165,7 @@
     <row r="37">
       <c r="A37" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>77310ddb-be92-4c78-8912-8012f9026c38</v>
+        <v>9e32b63e-6f9b-484a-a3cf-03b2554b0c81</v>
       </c>
       <c r="B37">
         <v>27</v>
@@ -1185,7 +1186,7 @@
     <row r="38">
       <c r="A38" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>a800480b-6b2f-4c5f-9279-9ac2416d7189</v>
+        <v>3af0b7f7-7574-4b56-bf9b-afbdc9d94496</v>
       </c>
       <c r="B38">
         <v>27</v>
@@ -1206,7 +1207,7 @@
     <row r="39">
       <c r="A39" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>c2ea6b48-2f8f-420f-9655-6b55b0e784d6</v>
+        <v>cd2a5828-bdf8-445c-81a1-3926ae9be2da</v>
       </c>
       <c r="B39">
         <v>27</v>
@@ -1227,7 +1228,7 @@
     <row r="40">
       <c r="A40" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>961ae097-bbd2-4be2-b313-094621395203</v>
+        <v>123fb41c-f345-498c-a994-9a9b27e98bf8</v>
       </c>
       <c r="B40">
         <v>27</v>
@@ -1248,7 +1249,7 @@
     <row r="41">
       <c r="A41" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>880b0225-c9b1-4bdd-8ed7-93e6220d7346</v>
+        <v>87d2b191-c73b-403f-96bc-6f392d27e7b2</v>
       </c>
       <c r="B41">
         <v>27</v>
@@ -1269,7 +1270,7 @@
     <row r="42">
       <c r="A42" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>d288a6d6-a293-416d-8b1f-4f3d01131e7f</v>
+        <v>5a4867f1-271f-4ee0-865d-7d7eb2b42d5d</v>
       </c>
       <c r="B42">
         <v>27</v>
@@ -1290,7 +1291,7 @@
     <row r="43">
       <c r="A43" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>c9daf53e-22ab-4e9d-8eb3-d36471ceb17f</v>
+        <v>3423a5df-5518-4d10-9006-6b46aef0c92f</v>
       </c>
       <c r="B43">
         <v>27</v>
@@ -1311,7 +1312,7 @@
     <row r="44">
       <c r="A44" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>4077b92e-d763-449e-accf-f4cf450bddb8</v>
+        <v>dac664bf-4d84-4185-9955-6184e4705180</v>
       </c>
       <c r="B44">
         <v>27</v>
@@ -1332,7 +1333,7 @@
     <row r="45">
       <c r="A45" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>ff459de3-e4f7-413a-821d-8205032383d7</v>
+        <v>8d87d414-5e8f-41e4-8024-820fa8e2834f</v>
       </c>
       <c r="B45">
         <v>27</v>
@@ -1353,7 +1354,7 @@
     <row r="46">
       <c r="A46" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>3ab2b1c9-7355-4d3c-9b89-8797da83a013</v>
+        <v>999e1a08-f844-4088-a0eb-d43b316c22f6</v>
       </c>
       <c r="B46">
         <v>27</v>
@@ -1374,7 +1375,7 @@
     <row r="47">
       <c r="A47" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>8f6ad1e1-0aa4-409c-a69f-5bacf2a68b0a</v>
+        <v>f3268128-5bfc-4b77-b848-87fd19d76a2d</v>
       </c>
       <c r="B47">
         <v>27</v>
@@ -1395,7 +1396,7 @@
     <row r="48">
       <c r="A48" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>5b58d634-aaa6-406c-9146-9a2ade88aed4</v>
+        <v>abf03747-d6bf-4469-9f81-fdf87f96dce3</v>
       </c>
       <c r="B48">
         <v>27</v>
@@ -1416,7 +1417,7 @@
     <row r="49">
       <c r="A49" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>6e8ad717-d117-427e-9279-a45e9219729c</v>
+        <v>cba5a361-0281-4457-a39e-8fff93b461df</v>
       </c>
       <c r="B49">
         <v>27</v>
@@ -1437,7 +1438,7 @@
     <row r="50">
       <c r="A50" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>c456e86d-ec7c-4d45-bcb7-3274a394c455</v>
+        <v>ba407704-b048-4ddc-b6ff-92559d5fe029</v>
       </c>
       <c r="B50">
         <v>27</v>
@@ -1458,7 +1459,7 @@
     <row r="51">
       <c r="A51" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>84f34f22-2fc4-42a9-a379-016b2d32bd27</v>
+        <v>a23819c9-7af3-4246-a061-633cfade115b</v>
       </c>
       <c r="B51">
         <v>27</v>
@@ -1479,7 +1480,7 @@
     <row r="52">
       <c r="A52" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>e4a3eb62-d8da-43d9-ad02-2381e98beeb0</v>
+        <v>bacb314f-3d07-4d2c-ad43-ee564b779903</v>
       </c>
       <c r="B52">
         <v>27</v>
@@ -1500,7 +1501,7 @@
     <row r="53">
       <c r="A53" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>249f29dc-63c9-4c07-958a-715d411f0fa1</v>
+        <v>a499a65c-f6a4-43bf-b3af-7414b2c94310</v>
       </c>
       <c r="B53">
         <v>27</v>
@@ -1521,7 +1522,7 @@
     <row r="54">
       <c r="A54" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>ed08c637-8021-49df-b96e-11b99461fd79</v>
+        <v>48d3d3eb-d568-4c77-8488-43c41b7afbf5</v>
       </c>
       <c r="B54">
         <v>27</v>
@@ -1542,7 +1543,7 @@
     <row r="55">
       <c r="A55" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>fd1e295f-870f-4951-a3d2-338a4c66acee</v>
+        <v>0aa13e64-c9da-42cf-98a6-ea7b261bfbc8</v>
       </c>
       <c r="B55">
         <v>27</v>
@@ -1563,7 +1564,7 @@
     <row r="56">
       <c r="A56" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>72cfa590-d7e9-4a64-830a-a29b0527af30</v>
+        <v>200b047e-f499-4d66-99d8-fbca132dfb75</v>
       </c>
       <c r="B56">
         <v>27</v>
@@ -1584,7 +1585,7 @@
     <row r="57">
       <c r="A57" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>4abb9347-8561-40c4-9763-175c5bd472f2</v>
+        <v>3b253e28-0230-47de-a666-91be77248828</v>
       </c>
       <c r="B57">
         <v>27</v>
@@ -1605,7 +1606,7 @@
     <row r="58">
       <c r="A58" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>6ecb16e9-54fc-4a3b-ba96-4c22542beefa</v>
+        <v>4334038f-c1b7-49a5-98f1-62b1237f3ab0</v>
       </c>
       <c r="B58">
         <v>27</v>
@@ -1626,7 +1627,7 @@
     <row r="59">
       <c r="A59" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>d09efba9-808b-404a-899c-686f3af486b3</v>
+        <v>5d8f29ff-7d1d-4e1e-82e1-34512516151c</v>
       </c>
       <c r="B59">
         <v>27</v>
@@ -1647,7 +1648,7 @@
     <row r="60">
       <c r="A60" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>f91e3b67-dc1a-448b-b69a-f6cf708fc839</v>
+        <v>85f0b61e-0ab3-4e0f-a3ef-060ce867161f</v>
       </c>
       <c r="B60">
         <v>27</v>
@@ -1668,7 +1669,7 @@
     <row r="61">
       <c r="A61" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>b1e22646-acd3-4f2c-b655-0c647a0b88f2</v>
+        <v>575c63cd-6cd4-43a1-b29d-d6b8960530e0</v>
       </c>
       <c r="B61">
         <v>27</v>
@@ -1689,7 +1690,7 @@
     <row r="62">
       <c r="A62" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>7537ced0-edd5-41b1-9372-2001d3458cd8</v>
+        <v>fb90b861-646a-4dd4-b647-a4cc017bc8aa</v>
       </c>
       <c r="B62">
         <v>28</v>
@@ -1710,7 +1711,7 @@
     <row r="63">
       <c r="A63" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>27ffff20-c05d-4bd9-adba-beb4139629a5</v>
+        <v>cbb60ea8-e319-4ef2-a23f-3d0a72e8a76d</v>
       </c>
       <c r="B63">
         <v>28</v>
@@ -1731,7 +1732,7 @@
     <row r="64">
       <c r="A64" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>3a2594b0-4677-4970-8022-74fc6b86aa9b</v>
+        <v>6567b1a7-ce1d-4054-873f-8febe4c8c136</v>
       </c>
       <c r="B64">
         <v>28</v>
@@ -1752,7 +1753,7 @@
     <row r="65">
       <c r="A65" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>2714de7f-867b-4a2d-bd49-32627164a79f</v>
+        <v>f0d6988c-f4a0-484b-b07f-71769fed5a9d</v>
       </c>
       <c r="B65">
         <v>28</v>
@@ -1773,7 +1774,7 @@
     <row r="66">
       <c r="A66" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>ce6c5dd8-b42c-47cb-93b4-df482a6f7f63</v>
+        <v>8b0ee883-6437-4353-b875-c394855058aa</v>
       </c>
       <c r="B66">
         <v>28</v>
@@ -1794,7 +1795,7 @@
     <row r="67">
       <c r="A67" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>a7887bd5-fea2-4053-9659-2996e7912f5f</v>
+        <v>f4140d64-523c-47a1-a31d-a55a487858ad</v>
       </c>
       <c r="B67">
         <v>28</v>
@@ -1815,7 +1816,7 @@
     <row r="68">
       <c r="A68" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>9fa0f6e5-eab4-49d8-903c-5a5d5e9b9fe6</v>
+        <v>e1e7a71f-4e39-419e-a77b-86d1a1e534e9</v>
       </c>
       <c r="B68">
         <v>28</v>
@@ -1836,7 +1837,7 @@
     <row r="69">
       <c r="A69" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>dab81130-0d84-4c31-92fa-61fe23ce815e</v>
+        <v>7ec6e054-a925-4b6d-868e-7edae103be2d</v>
       </c>
       <c r="B69">
         <v>28</v>
@@ -1857,7 +1858,7 @@
     <row r="70">
       <c r="A70" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>6c50b6c3-429d-4ea8-b0b7-577239200ebd</v>
+        <v>baac48ef-2267-4932-b04b-f8b85153bcf8</v>
       </c>
       <c r="B70">
         <v>28</v>
@@ -1878,7 +1879,7 @@
     <row r="71">
       <c r="A71" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>67ea425c-c978-46ff-b6ca-1fb5e78fc9f4</v>
+        <v>b3a79e76-a9ed-453a-affb-d11df6cb336e</v>
       </c>
       <c r="B71">
         <v>28</v>
@@ -1899,7 +1900,7 @@
     <row r="72">
       <c r="A72" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>fef2d6ba-22e3-4581-90b9-007f05b11c58</v>
+        <v>74975ac4-5195-4360-a509-f8abcd51c71d</v>
       </c>
       <c r="B72">
         <v>28</v>
@@ -1920,7 +1921,7 @@
     <row r="73">
       <c r="A73" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>8bbb0350-9bdb-49c0-87b5-9f1a4cc59ba4</v>
+        <v>8af0b848-c984-475f-af71-c73c9cf77b8b</v>
       </c>
       <c r="B73">
         <v>28</v>
@@ -1935,7 +1936,7 @@
     <row r="74">
       <c r="A74" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>b5f240ec-c5f0-413b-a02f-f1938c8ba8c8</v>
+        <v>b631dad9-b82c-47b5-b18e-a505891c7e86</v>
       </c>
       <c r="B74">
         <v>28</v>
@@ -1956,7 +1957,7 @@
     <row r="75">
       <c r="A75" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>b3b854ea-ae11-4e9f-a8fd-64994ac9dbbf</v>
+        <v>d7be64cc-0840-44db-9e09-27cf029efff2</v>
       </c>
       <c r="B75">
         <v>28</v>
@@ -1977,7 +1978,7 @@
     <row r="76">
       <c r="A76" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>28a056a6-afc8-4573-b795-129679e826fd</v>
+        <v>7c51af5a-2c08-40d7-9b59-971579e83fcd</v>
       </c>
       <c r="B76">
         <v>28</v>
@@ -1998,7 +1999,7 @@
     <row r="77">
       <c r="A77" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>a83f5781-c10b-4059-b678-f5017c3bfd91</v>
+        <v>f9d5999c-a156-41b9-800c-a7802ca98ea5</v>
       </c>
       <c r="B77">
         <v>28</v>
@@ -2019,7 +2020,7 @@
     <row r="78">
       <c r="A78" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>c851cfa6-da17-4115-bfba-e73ad76bad11</v>
+        <v>c8a1854a-ae84-41f5-a5d4-a1d0aa910d2c</v>
       </c>
       <c r="B78">
         <v>28</v>
@@ -2037,7 +2038,7 @@
     <row r="79">
       <c r="A79" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>7df8e698-06b4-4ed7-be9e-55f134bd1398</v>
+        <v>e3abb703-a37a-4308-96b6-b20859e2a6aa</v>
       </c>
       <c r="B79">
         <v>28</v>
@@ -2058,7 +2059,7 @@
     <row r="80">
       <c r="A80" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>158fe7a4-efef-4a53-b28c-89efeb6d300a</v>
+        <v>dfa9fc23-b0d1-4e81-865b-13d53416db11</v>
       </c>
       <c r="B80">
         <v>28</v>
@@ -2079,7 +2080,7 @@
     <row r="81">
       <c r="A81" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>98d438f9-e8b5-470e-9413-e9da43789b60</v>
+        <v>e9792faa-117f-408c-8aa4-bb141f602092</v>
       </c>
       <c r="B81">
         <v>28</v>
@@ -2100,7 +2101,7 @@
     <row r="82">
       <c r="A82" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>0ef71b05-a9f0-4c83-96d8-ef620421699f</v>
+        <v>9c9784a3-bc25-46fe-99fb-cb54224c9f86</v>
       </c>
       <c r="B82">
         <v>28</v>
@@ -2121,7 +2122,7 @@
     <row r="83">
       <c r="A83" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>bf37e4d2-1ace-45b0-92fa-c09b9579ba53</v>
+        <v>6842266a-c5ab-4119-a535-872c36da4757</v>
       </c>
       <c r="B83">
         <v>28</v>
@@ -2142,7 +2143,7 @@
     <row r="84">
       <c r="A84" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>282ee767-dd0b-456f-8e48-a59f2ec0ada4</v>
+        <v>d2a15da2-9ea7-48ec-ac1c-31958d2a9169</v>
       </c>
       <c r="B84">
         <v>28</v>
@@ -2163,7 +2164,7 @@
     <row r="85">
       <c r="A85" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>4b5365bb-45cc-471f-93f9-fdd6365503db</v>
+        <v>2c2dbe0d-943c-43ab-ba45-c532ffa886ae</v>
       </c>
       <c r="B85">
         <v>28</v>
@@ -2184,7 +2185,7 @@
     <row r="86">
       <c r="A86" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>d170c824-40b3-4d23-85bc-dac94d473ef6</v>
+        <v>41542f1d-741d-4a47-8a81-a1d09a9a966b</v>
       </c>
       <c r="B86">
         <v>28</v>
@@ -2205,7 +2206,7 @@
     <row r="87">
       <c r="A87" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>6bc2356b-925a-4b5e-a5f8-d18885512916</v>
+        <v>6e66b3ef-3ec5-4743-9860-7418a93dce27</v>
       </c>
       <c r="B87">
         <v>28</v>
@@ -2226,7 +2227,7 @@
     <row r="88">
       <c r="A88" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>deaadcab-99d2-4f62-9991-d8ea1255331a</v>
+        <v>1188e571-d666-4bf9-81ee-46334eabd388</v>
       </c>
       <c r="B88">
         <v>28</v>
@@ -2247,7 +2248,7 @@
     <row r="89">
       <c r="A89" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>aaeea09b-0891-4adf-a60a-f1b9819850d7</v>
+        <v>c8f79e81-dc8c-4f22-805d-0f1945deadcd</v>
       </c>
       <c r="B89">
         <v>28</v>
@@ -2268,7 +2269,7 @@
     <row r="90">
       <c r="A90" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>a72056af-f2b4-47fa-99d4-23d65d468706</v>
+        <v>df9891a5-2a7a-4754-91d7-ff7fffc40477</v>
       </c>
       <c r="B90">
         <v>28</v>
@@ -2289,7 +2290,7 @@
     <row r="91">
       <c r="A91" t="str">
         <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>649d019d-0852-4490-94ad-2d14e1e266f1</v>
+        <v>f1186873-4969-486d-bd89-9a0695b5388f</v>
       </c>
       <c r="B91">
         <v>28</v>
@@ -2305,12 +2306,642 @@
       </c>
       <c r="F91" t="str">
         <v>prefer something to something</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>a2b1778e-1bde-4f07-8efc-386e9629f6dc</v>
+      </c>
+      <c r="B92">
+        <v>29</v>
+      </c>
+      <c r="C92" t="str">
+        <v>Câu cá</v>
+      </c>
+      <c r="D92" t="str">
+        <v>Fishing</v>
+      </c>
+      <c r="E92" t="str">
+        <v>My dad and I go fishing every day</v>
+      </c>
+      <c r="F92" t="str">
+        <v>Go fishing</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>cf990805-78a4-450b-9080-8d1407d56334</v>
+      </c>
+      <c r="B93">
+        <v>29</v>
+      </c>
+      <c r="C93" t="str">
+        <v>Vận động viên</v>
+      </c>
+      <c r="D93" t="str">
+        <v>Athlete</v>
+      </c>
+      <c r="E93" t="str">
+        <v>Olumpic athletes train hard to complete</v>
+      </c>
+      <c r="F93" t="str">
+        <v>An Olympic athlete</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>b6a3f27f-b5f1-4f59-a13a-5a3b1d198402</v>
+      </c>
+      <c r="B94">
+        <v>29</v>
+      </c>
+      <c r="C94" t="str">
+        <v>Môn đấu vật</v>
+      </c>
+      <c r="D94" t="str">
+        <v>Wrestling</v>
+      </c>
+      <c r="E94" t="str">
+        <v>Wrestling matches are popular in the US</v>
+      </c>
+      <c r="F94" t="str">
+        <v>a wrestling match</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>f903164f-992c-4ff7-bdd0-9796bb39e5eb</v>
+      </c>
+      <c r="B95">
+        <v>29</v>
+      </c>
+      <c r="C95" t="str">
+        <v>Chuyên nghiệp</v>
+      </c>
+      <c r="D95" t="str">
+        <v>Professional</v>
+      </c>
+      <c r="E95" t="str">
+        <v>He was a professional soccer player</v>
+      </c>
+      <c r="F95" t="str">
+        <v>a professional soccer player</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>f38ea113-6eed-41a7-864c-9fd8eb997c46</v>
+      </c>
+      <c r="B96">
+        <v>29</v>
+      </c>
+      <c r="C96" t="str">
+        <v>Hàng năm</v>
+      </c>
+      <c r="D96" t="str">
+        <v>Annual</v>
+      </c>
+      <c r="E96" t="str">
+        <v>The company has annual meetings for us</v>
+      </c>
+      <c r="F96" t="str">
+        <v>an annual meeting</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>cec821bf-15bc-4c73-85e6-328b2b004fd1</v>
+      </c>
+      <c r="B97">
+        <v>29</v>
+      </c>
+      <c r="C97" t="str">
+        <v>Giải đấu</v>
+      </c>
+      <c r="D97" t="str">
+        <v>Tournament</v>
+      </c>
+      <c r="E97" t="str">
+        <v>What an exciting soccer tournament!</v>
+      </c>
+      <c r="F97" t="str">
+        <v>A soccer tournament</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>ddae4d17-2487-4c91-b15b-62ec664e7e93</v>
+      </c>
+      <c r="B98">
+        <v>29</v>
+      </c>
+      <c r="C98" t="str">
+        <v>Huấn luyện viên</v>
+      </c>
+      <c r="D98" t="str">
+        <v>Coach</v>
+      </c>
+      <c r="E98" t="str">
+        <v>The team coach trains us hard</v>
+      </c>
+      <c r="F98" t="str">
+        <v>the team coach</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>9c573cff-4ddd-4aec-83ca-2f88d870993e</v>
+      </c>
+      <c r="B99">
+        <v>29</v>
+      </c>
+      <c r="C99" t="str">
+        <v>Trận đấu</v>
+      </c>
+      <c r="D99" t="str">
+        <v>Match</v>
+      </c>
+      <c r="E99" t="str">
+        <v>There is a soccer match tonight</v>
+      </c>
+      <c r="F99" t="str">
+        <v>a soccer match</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>dd72f5c5-8548-436c-bd33-79ddb20c7437</v>
+      </c>
+      <c r="B100">
+        <v>29</v>
+      </c>
+      <c r="C100" t="str">
+        <v>Đánh bại</v>
+      </c>
+      <c r="D100" t="str">
+        <v>Beat</v>
+      </c>
+      <c r="E100" t="str">
+        <v>They beat their opponents in the first round</v>
+      </c>
+      <c r="F100" t="str">
+        <v>beat something or somebody</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>b1892029-56ff-4cbe-984a-c7dab29a9977</v>
+      </c>
+      <c r="B101">
+        <v>29</v>
+      </c>
+      <c r="C101" t="str">
+        <v>Đối thủ</v>
+      </c>
+      <c r="D101" t="str">
+        <v>opponent</v>
+      </c>
+      <c r="E101" t="str">
+        <v>She is my opponent in chess</v>
+      </c>
+      <c r="F101" t="str">
+        <v>one's oppponent in something</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>1e190ed8-33a8-4e71-b7b2-fa84c7c02941</v>
+      </c>
+      <c r="B102">
+        <v>29</v>
+      </c>
+      <c r="C102" t="str">
+        <v>Môn thể thao</v>
+      </c>
+      <c r="D102" t="str">
+        <v>Athletics</v>
+      </c>
+      <c r="E102" t="str">
+        <v>Football, soccer, and baseball are types of atheletics</v>
+      </c>
+      <c r="F102" t="str">
+        <v>Types of athletics</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>d38353fc-5f4f-472c-ac04-668987f0a4a7</v>
+      </c>
+      <c r="B103">
+        <v>29</v>
+      </c>
+      <c r="C103" t="str">
+        <v>Bóng rỗ</v>
+      </c>
+      <c r="D103" t="str">
+        <v>Basketball</v>
+      </c>
+      <c r="E103" t="str">
+        <v>I am the captain of the basketball team</v>
+      </c>
+      <c r="F103" t="str">
+        <v>a basketball team</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>ef65ce51-588d-4574-aabf-54d79f5fccc8</v>
+      </c>
+      <c r="B104">
+        <v>29</v>
+      </c>
+      <c r="C104" t="str">
+        <v>Người chơi</v>
+      </c>
+      <c r="D104" t="str">
+        <v>Player</v>
+      </c>
+      <c r="E104" t="str">
+        <v>he is the best soccer player here</v>
+      </c>
+      <c r="F104" t="str">
+        <v>a soccer player</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>b7c13a10-8f6b-4bc0-adf4-4efd66aa87fc</v>
+      </c>
+      <c r="B105">
+        <v>29</v>
+      </c>
+      <c r="C105" t="str">
+        <v xml:space="preserve">Liên đoàn </v>
+      </c>
+      <c r="D105" t="str">
+        <v>League</v>
+      </c>
+      <c r="E105" t="str">
+        <v>My sone plays for a soccer league</v>
+      </c>
+      <c r="F105" t="str">
+        <v>A soccer league</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>cbf03296-0921-4040-90d4-199fd9d5c23b</v>
+      </c>
+      <c r="B106">
+        <v>29</v>
+      </c>
+      <c r="C106" t="str">
+        <v>Giải vô địch</v>
+      </c>
+      <c r="D106" t="str">
+        <v>Championship</v>
+      </c>
+      <c r="E106" t="str">
+        <v>Are you ready for the basketball championship</v>
+      </c>
+      <c r="F106" t="str">
+        <v>a basketball championship</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>5029497b-8c66-41b8-8d0a-4bfe381c4286</v>
+      </c>
+      <c r="B107">
+        <v>29</v>
+      </c>
+      <c r="C107" t="str">
+        <v>Đội trưởng</v>
+      </c>
+      <c r="D107" t="str">
+        <v>Captain</v>
+      </c>
+      <c r="E107" t="str">
+        <v>we vote for a team camtain</v>
+      </c>
+      <c r="F107" t="str">
+        <v>team captain</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>c2fb9123-f320-4cc1-a7fa-d38da99a5fc1</v>
+      </c>
+      <c r="B108">
+        <v>29</v>
+      </c>
+      <c r="C108" t="str">
+        <v>Ghi điểm</v>
+      </c>
+      <c r="D108" t="str">
+        <v>score</v>
+      </c>
+      <c r="E108" t="str">
+        <v>He scored a goal for the team</v>
+      </c>
+      <c r="F108" t="str">
+        <v>score a goal</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>a52a7a35-9823-4ea9-87c9-6dec37ecf622</v>
+      </c>
+      <c r="B109">
+        <v>29</v>
+      </c>
+      <c r="C109" t="str">
+        <v>Danh hiệu</v>
+      </c>
+      <c r="D109" t="str">
+        <v>Title</v>
+      </c>
+      <c r="E109" t="str">
+        <v>The team won the title with a goal in the last minute</v>
+      </c>
+      <c r="F109" t="str">
+        <v>win the title</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>916d379b-cba3-40d9-a67f-a71d48b74a2f</v>
+      </c>
+      <c r="B110">
+        <v>29</v>
+      </c>
+      <c r="C110" t="str">
+        <v>Lưới</v>
+      </c>
+      <c r="D110" t="str">
+        <v>net</v>
+      </c>
+      <c r="E110" t="str">
+        <v>The fishing net has holes in it</v>
+      </c>
+      <c r="F110" t="str">
+        <v>a fishing net</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>463b16e3-432e-446b-bea0-a0f2b3da5f06</v>
+      </c>
+      <c r="B111">
+        <v>29</v>
+      </c>
+      <c r="C111" t="str">
+        <v>Anh hùng</v>
+      </c>
+      <c r="D111" t="str">
+        <v>hero</v>
+      </c>
+      <c r="E111" t="str">
+        <v>The fireman became a local hero</v>
+      </c>
+      <c r="F111" t="str">
+        <v>a local hero</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>39de71b0-d5b5-48c9-8f4d-95b2e2f50af6</v>
+      </c>
+      <c r="B112">
+        <v>29</v>
+      </c>
+      <c r="C112" t="str">
+        <v>Môn đạp xe</v>
+      </c>
+      <c r="D112" t="str">
+        <v>Cycling</v>
+      </c>
+      <c r="E112" t="str">
+        <v>She went cycling down the hill</v>
+      </c>
+      <c r="F112" t="str">
+        <v>go cycling</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>aae25fe9-c463-44f6-8403-64b3ab4901df</v>
+      </c>
+      <c r="B113">
+        <v>29</v>
+      </c>
+      <c r="C113" t="str">
+        <v>Sân vận động</v>
+      </c>
+      <c r="D113" t="str">
+        <v>Stadium</v>
+      </c>
+      <c r="E113" t="str">
+        <v>Where is the biggest sports stadium in hanoi</v>
+      </c>
+      <c r="F113" t="str">
+        <v>A sport stadium</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>a8bd58e5-0590-4ebb-9b28-1b10efe4f691</v>
+      </c>
+      <c r="B114">
+        <v>29</v>
+      </c>
+      <c r="C114" t="str">
+        <v>Người thắng cuộc</v>
+      </c>
+      <c r="D114" t="str">
+        <v>Winner</v>
+      </c>
+      <c r="E114" t="str">
+        <v>The actor is an award winner</v>
+      </c>
+      <c r="F114" t="str">
+        <v>an award winer</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>b553acc6-a0c9-417a-b2d9-d77e5fd33909</v>
+      </c>
+      <c r="B115">
+        <v>29</v>
+      </c>
+      <c r="C115" t="str">
+        <v>Môn đánh golf</v>
+      </c>
+      <c r="D115" t="str">
+        <v>Golf</v>
+      </c>
+      <c r="E115" t="str">
+        <v>Businessmen love to play golf</v>
+      </c>
+      <c r="F115" t="str">
+        <v>play golf</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>c9b2d631-4c95-4cbf-b5c6-51760a9800c8</v>
+      </c>
+      <c r="B116">
+        <v>29</v>
+      </c>
+      <c r="C116" t="str">
+        <v>Đánh</v>
+      </c>
+      <c r="D116" t="str">
+        <v>Strike</v>
+      </c>
+      <c r="E116" t="str">
+        <v>He strikes the golf ball perfectly</v>
+      </c>
+      <c r="F116" t="str">
+        <v>strike the ball</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>6c846374-0b04-4261-a1fc-abb952bde9d0</v>
+      </c>
+      <c r="B117">
+        <v>29</v>
+      </c>
+      <c r="C117" t="str">
+        <v>Đích, mục tiêu</v>
+      </c>
+      <c r="D117" t="str">
+        <v>target</v>
+      </c>
+      <c r="E117" t="str">
+        <v>He shot the arrow and hit the target</v>
+      </c>
+      <c r="F117" t="str">
+        <v>hit the target</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>7c39a7bf-0223-4d67-bf19-bc70d6260a4c</v>
+      </c>
+      <c r="B118">
+        <v>29</v>
+      </c>
+      <c r="C118" t="str">
+        <v>Tối đa</v>
+      </c>
+      <c r="D118" t="str">
+        <v>maximum</v>
+      </c>
+      <c r="E118" t="str">
+        <v>The maximum amount for storage is 256GB</v>
+      </c>
+      <c r="F118" t="str">
+        <v>the maximum amount</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>727a487b-ea11-4357-8b3a-cfd78069fedb</v>
+      </c>
+      <c r="B119">
+        <v>29</v>
+      </c>
+      <c r="C119" t="str">
+        <v>Lướt</v>
+      </c>
+      <c r="D119" t="str">
+        <v>Surf</v>
+      </c>
+      <c r="E119" t="str">
+        <v>In hawaii, you must surf the waves</v>
+      </c>
+      <c r="F119" t="str">
+        <v>surf the wave</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>86cb971a-bdd1-45d0-9169-17ef0fb2990e</v>
+      </c>
+      <c r="B120">
+        <v>29</v>
+      </c>
+      <c r="C120" t="str">
+        <v>Không may</v>
+      </c>
+      <c r="D120" t="str">
+        <v>unfortunately</v>
+      </c>
+      <c r="E120" t="str">
+        <v>Unfortunately, I won't be able to attend the meeting</v>
+      </c>
+      <c r="F120" t="str">
+        <v>unfortunately, I won't</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <f>LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
+        <v>2805d4a5-2450-4193-92b7-19d2357bd4d9</v>
+      </c>
+      <c r="B121">
+        <v>29</v>
+      </c>
+      <c r="C121" t="str">
+        <v>Trân trọng, đánh giá cao</v>
+      </c>
+      <c r="D121" t="str">
+        <v>Appreciate</v>
+      </c>
+      <c r="E121" t="str">
+        <v>I appreciate the help you gave me</v>
+      </c>
+      <c r="F121" t="str">
+        <v>appreciate somebody or something</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G91"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G121"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4143,8 +4774,2443 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:F91"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F121"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>unitId</v>
+      </c>
+      <c r="C1" t="str">
+        <v>word</v>
+      </c>
+      <c r="D1" t="str">
+        <v>answers</v>
+      </c>
+      <c r="E1" t="str">
+        <v>sentences</v>
+      </c>
+      <c r="F1" t="str">
+        <v>phrases</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2855e402-1dfa-4dc2-8840-cebd848fa19c</v>
+      </c>
+      <c r="B2">
+        <v>26</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Chương trình</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Show</v>
+      </c>
+      <c r="E2" t="str">
+        <v>I watch TV shows on my television</v>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>d90b062b-c464-4c5c-bf4d-2d250fee42b4</v>
+      </c>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Cảnh</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Scene</v>
+      </c>
+      <c r="E3" t="str">
+        <v>The crew needs to film a scene</v>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>d670b0d5-a0f9-4e3d-be7e-7539b709f4bf</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Nam diễn viên</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Actor</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Who is the lead actor in titanic</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>0b08724a-3034-4e5c-9eed-a809189bff3a</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Thuộc âm nhạc</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Musical</v>
+      </c>
+      <c r="E5" t="str">
+        <v xml:space="preserve">The audience loved the musical performance </v>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>4152b846-3f6e-4b76-b48c-320c8d9bf98d</v>
+      </c>
+      <c r="B6">
+        <v>26</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Nhạc phim</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Soundtrack</v>
+      </c>
+      <c r="E6" t="str">
+        <v>The soundtrack of this movie is great</v>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>f9c612cb-22a0-4f9d-a949-c179e45f0655</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Thuộc lịch sử</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Historical</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Albert Einstein is an important historical figure</v>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>53af5326-467e-4e15-a189-ec4723760626</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Bí ẩn</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Mystery</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Nobody can solve the mystery of the Bermuda triangle</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>faab9a2e-d127-4a38-abf1-879e33beef60</v>
+      </c>
+      <c r="B9">
+        <v>26</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Tội ác</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Crime</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Stealing money is a serious crime</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>da3b1816-173a-4493-ad15-7beb97e72ba5</v>
+      </c>
+      <c r="B10">
+        <v>26</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Đoạn kết</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Ending</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Fairy tales have happy endings</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>e98b5079-2952-47db-afac-31e8e8b2ded1</v>
+      </c>
+      <c r="B11">
+        <v>26</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Tiết lộ</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Reveal</v>
+      </c>
+      <c r="E11" t="str">
+        <v>The magician never reveals the truth</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>6834a067-2935-4767-b07e-7e28c2af50bc</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Phim giật gân</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Thriller</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Thriller movies are scary</v>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>eec73fe0-6f13-4d23-b16e-304b453fd1eb</v>
+      </c>
+      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Xưởng, không gian sáng tạo</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Studio</v>
+      </c>
+      <c r="E13" t="str">
+        <v>She teaches us at her dance studio</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>d82e9755-cb4a-4e76-b2d1-c22e9bbd3e4a</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Bối cảnh, khung cảnh</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Setting</v>
+      </c>
+      <c r="E14" t="str">
+        <v xml:space="preserve">What a beautiful setting this city is </v>
+      </c>
+      <c r="F14" t="str">
+        <v>A beautiful setting</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>80af4f65-e319-4276-abc7-c4b93cfb684f</v>
+      </c>
+      <c r="B15">
+        <v>26</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Điều viễn tưởng</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Fiction</v>
+      </c>
+      <c r="E15" t="str">
+        <v>She wrote fiction on aliens and love</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>66eb9a3b-e5cf-4572-af26-c0ced46a6a41</v>
+      </c>
+      <c r="B16">
+        <v>26</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Sự việc kịch tính</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Drama</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Teens like to watch drama series</v>
+      </c>
+      <c r="F16" t="str">
+        <v>A drama series</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>6d66f4e3-1575-453b-9c56-b2e35ae6f572</v>
+      </c>
+      <c r="B17">
+        <v>26</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Đạo diễn</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Director</v>
+      </c>
+      <c r="E17" t="str">
+        <v>The young film director deserves our recognition</v>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>c61cf54e-76e9-4c4f-a546-be16ad5e5bcf</v>
+      </c>
+      <c r="B18">
+        <v>26</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Ra mắt</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Come out</v>
+      </c>
+      <c r="E18" t="str">
+        <v>When is her album coming out?</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Something new comes out</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>75d97f77-6607-497c-a34c-c08e4276bc76</v>
+      </c>
+      <c r="B19">
+        <v>26</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Nhân vật</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Character</v>
+      </c>
+      <c r="E19" t="str">
+        <v>The main character in "Batman" is mysterious</v>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>e2745e17-f355-4999-984f-246339ace9e7</v>
+      </c>
+      <c r="B20">
+        <v>26</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Nữ diễn viên</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Actress</v>
+      </c>
+      <c r="E20" t="str">
+        <v>She was a good actress back then</v>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>d883b560-e598-4399-b67a-fbd255f88070</v>
+      </c>
+      <c r="B21">
+        <v>26</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Kỳ lạ, kỳ quặc</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Odd</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Hanging out with odd people is fun</v>
+      </c>
+      <c r="F21" t="str">
+        <v>An odd person</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>861042fb-7382-4b86-b5dc-6f8a0f267c2b</v>
+      </c>
+      <c r="B22">
+        <v>26</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Màn hình</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Screen</v>
+      </c>
+      <c r="E22" t="str">
+        <v>The laptop has a big computer screen</v>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>2c327c19-447e-45c6-8278-14aa65293f96</v>
+      </c>
+      <c r="B23">
+        <v>26</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Hành động</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Action</v>
+      </c>
+      <c r="E23" t="str">
+        <v>My favorite action movie is Fast and Furious</v>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>1c7e5e1d-737d-4a0f-9124-6e6415aaab50</v>
+      </c>
+      <c r="B24">
+        <v>26</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Chuyến phiêu lưu</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Adventure</v>
+      </c>
+      <c r="E24" t="str">
+        <v>I seek an adventure of a lifetime</v>
+      </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>046efda8-e3b4-4698-a754-cacebf1c90e0</v>
+      </c>
+      <c r="B25">
+        <v>26</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Phim tài liệu</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Documentary</v>
+      </c>
+      <c r="E25" t="str">
+        <v>I watched that documentary film on Netflix</v>
+      </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>7040324e-e5a2-44f4-9535-b2cc9cbdb924</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Góc</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Angle</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Tilt your head to a 45 angle</v>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>988a2983-945c-4cf0-ba48-152e92f249c4</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Thấy khó hiểu</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Confused</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Are you confused about the instructions?</v>
+      </c>
+      <c r="F27" t="str">
+        <v>Confused about something</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>928cac87-df35-4693-90eb-0b7ac9ba4f7c</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Cuộc hội thoại, lời thoại</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Dialogue</v>
+      </c>
+      <c r="E28" t="str">
+        <v>The dialogue with my therapist helped me</v>
+      </c>
+      <c r="F28" t="str">
+        <v>Dialogue with somebody</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>470241db-5ef4-4605-923a-0f067329f20f</v>
+      </c>
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Tác phẩm thành công</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Hit</v>
+      </c>
+      <c r="E29" t="str">
+        <v>His book became a big hit</v>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>972036e4-0ba9-4393-b01e-adb398bcbf0c</v>
+      </c>
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Tuyệt vời</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Wonderful</v>
+      </c>
+      <c r="E30" t="str">
+        <v>I am grateful for the wonderful opportunity</v>
+      </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>fefbe098-b8f8-40ef-87d2-ea757ae401e2</v>
+      </c>
+      <c r="B31">
+        <v>26</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Tài giỏi, tuyệt vời</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Brilliant</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Thank you for the brilliant idea</v>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>7ced7a2e-75de-4804-ac90-20e3e958d965</v>
+      </c>
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Khiêm tốn</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Modest</v>
+      </c>
+      <c r="E32" t="str">
+        <v>You are too modest! You are gifted.</v>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>4b5d71f1-69c8-4d40-917c-56ed60fa341a</v>
+      </c>
+      <c r="B33">
+        <v>27</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Có năng khiếu</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Gifted</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Do you consider yourself a gifted musican?</v>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>f249b615-9ce7-490b-aeb1-e7fb50956f75</v>
+      </c>
+      <c r="B34">
+        <v>27</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Ngành giải trí</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Showbiz</v>
+      </c>
+      <c r="E34" t="str">
+        <v>People in showbiz are movie stars</v>
+      </c>
+      <c r="F34" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>33645007-d97b-4e05-9fbb-18ce6453df08</v>
+      </c>
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Kênh</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Channel</v>
+      </c>
+      <c r="E35" t="str">
+        <v>The show is live on the VTV3 channel</v>
+      </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>c1f5fd98-6823-4cd2-8332-437b40d1cdbb</v>
+      </c>
+      <c r="B36">
+        <v>27</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Truyền thông</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Media</v>
+      </c>
+      <c r="E36" t="str">
+        <v>My mom posts so many pictures on social media</v>
+      </c>
+      <c r="F36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>9e32b63e-6f9b-484a-a3cf-03b2554b0c81</v>
+      </c>
+      <c r="B37">
+        <v>27</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Nổi tiếng</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Well-known</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Is he a well-known actor?</v>
+      </c>
+      <c r="F37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>3af0b7f7-7574-4b56-bf9b-afbdc9d94496</v>
+      </c>
+      <c r="B38">
+        <v>27</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Nhận ra</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Recognize</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Did you recognize me on stage?</v>
+      </c>
+      <c r="F38" t="str">
+        <v>Recognize somebody or something</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>cd2a5828-bdf8-445c-81a1-3926ae9be2da</v>
+      </c>
+      <c r="B39">
+        <v>27</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Người hâm mộ</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Fan</v>
+      </c>
+      <c r="E39" t="str">
+        <v>My girlfriend is a big soccer fan</v>
+      </c>
+      <c r="F39" t="str">
+        <v>A soccer fan</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>123fb41c-f345-498c-a994-9a9b27e98bf8</v>
+      </c>
+      <c r="B40">
+        <v>27</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Đăng ký</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Subscribe</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Please subscribe to step up english youtube channel</v>
+      </c>
+      <c r="F40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>87d2b191-c73b-403f-96bc-6f392d27e7b2</v>
+      </c>
+      <c r="B41">
+        <v>27</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Hét to</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Sceam</v>
+      </c>
+      <c r="E41" t="str">
+        <v>They screamed out loud for help</v>
+      </c>
+      <c r="F41" t="str">
+        <v>Scream out loud</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>5a4867f1-271f-4ee0-865d-7d7eb2b42d5d</v>
+      </c>
+      <c r="B42">
+        <v>27</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Buồn cười</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Funny</v>
+      </c>
+      <c r="E42" t="str">
+        <v>The funny story made me laugh hard</v>
+      </c>
+      <c r="F42" t="str">
+        <v>A funny story</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>3423a5df-5518-4d10-9006-6b46aef0c92f</v>
+      </c>
+      <c r="B43">
+        <v>27</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Hiện nay</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Currently</v>
+      </c>
+      <c r="E43" t="str">
+        <v>I am currently working as a front-end developer</v>
+      </c>
+      <c r="F43" t="str">
+        <v>Currently working as something</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>dac664bf-4d84-4185-9955-6184e4705180</v>
+      </c>
+      <c r="B44">
+        <v>27</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Lan truyền nhanh</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Viral</v>
+      </c>
+      <c r="E44" t="str">
+        <v>The video went viral on Facebook</v>
+      </c>
+      <c r="F44" t="str">
+        <v>Go viral</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>8d87d414-5e8f-41e4-8024-820fa8e2834f</v>
+      </c>
+      <c r="B45">
+        <v>27</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Màn biểu diễn</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Performance</v>
+      </c>
+      <c r="E45" t="str">
+        <v>The opera singer delivered an outstanding performance</v>
+      </c>
+      <c r="F45" t="str">
+        <v>Deliver an outstanding performance</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>999e1a08-f844-4088-a0eb-d43b316c22f6</v>
+      </c>
+      <c r="B46">
+        <v>27</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Quá khứ</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Past</v>
+      </c>
+      <c r="E46" t="str">
+        <v>I used to live abroad in the past</v>
+      </c>
+      <c r="F46" t="str">
+        <v>In the past</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>f3268128-5bfc-4b77-b848-87fd19d76a2d</v>
+      </c>
+      <c r="B47">
+        <v>27</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Trở nên</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Become</v>
+      </c>
+      <c r="E47" t="str">
+        <v>I want to become a person of influence</v>
+      </c>
+      <c r="F47" t="str">
+        <v>Become somebody or something</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>abf03747-d6bf-4469-9f81-fdf87f96dce3</v>
+      </c>
+      <c r="B48">
+        <v>27</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Toàn cầu</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Global</v>
+      </c>
+      <c r="E48" t="str">
+        <v>The singer's talent made her go global</v>
+      </c>
+      <c r="F48" t="str">
+        <v>Go global</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>cba5a361-0281-4457-a39e-8fff93b461df</v>
+      </c>
+      <c r="B49">
+        <v>27</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Lên tiếng</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Speak out</v>
+      </c>
+      <c r="E49" t="str">
+        <v>She bravely spoke out against her boss</v>
+      </c>
+      <c r="F49" t="str">
+        <v>Speak out against somebody or something</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>ba407704-b048-4ddc-b6ff-92559d5fe029</v>
+      </c>
+      <c r="B50">
+        <v>27</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Xứng đáng</v>
+      </c>
+      <c r="D50" t="str">
+        <v>Deserve</v>
+      </c>
+      <c r="E50" t="str">
+        <v>I deserve ice cream after work</v>
+      </c>
+      <c r="F50" t="str">
+        <v>Deserve something</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>a23819c9-7af3-4246-a061-633cfade115b</v>
+      </c>
+      <c r="B51">
+        <v>27</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Trực tiếp</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Live</v>
+      </c>
+      <c r="E51" t="str">
+        <v>The band did a live performance</v>
+      </c>
+      <c r="F51" t="str">
+        <v>A live performance</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>bacb314f-3d07-4d2c-ad43-ee564b779903</v>
+      </c>
+      <c r="B52">
+        <v>27</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Giải thưởng</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Award</v>
+      </c>
+      <c r="E52" t="str">
+        <v>She received an award for her acting</v>
+      </c>
+      <c r="F52" t="str">
+        <v>Receive an award</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>a499a65c-f6a4-43bf-b3af-7414b2c94310</v>
+      </c>
+      <c r="B53">
+        <v>27</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Danh dự</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Honor</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Welcome, you are my guest of honor</v>
+      </c>
+      <c r="F53" t="str">
+        <v>The guest of honor</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>48d3d3eb-d568-4c77-8488-43c41b7afbf5</v>
+      </c>
+      <c r="B54">
+        <v>27</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Việc thiện nguyện</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Charity</v>
+      </c>
+      <c r="E54" t="str">
+        <v>We should do charity for the disadvantaged</v>
+      </c>
+      <c r="F54" t="str">
+        <v>Do charity for somebody</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>0aa13e64-c9da-42cf-98a6-ea7b261bfbc8</v>
+      </c>
+      <c r="B55">
+        <v>27</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Tình nguyện</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Volunteer</v>
+      </c>
+      <c r="E55" t="str">
+        <v>She volunteered to clean the car</v>
+      </c>
+      <c r="F55" t="str">
+        <v>Volunteer to do something</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>200b047e-f499-4d66-99d8-fbca132dfb75</v>
+      </c>
+      <c r="B56">
+        <v>27</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Vụ bê bối</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Scandal</v>
+      </c>
+      <c r="E56" t="str">
+        <v>He created the scandal to attract attention</v>
+      </c>
+      <c r="F56" t="str">
+        <v>Create a scandal</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>3b253e28-0230-47de-a666-91be77248828</v>
+      </c>
+      <c r="B57">
+        <v>27</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Tin đồn</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Rumor</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Rumor has it that you got the job!</v>
+      </c>
+      <c r="F57" t="str">
+        <v>Rumor has it that</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>4334038f-c1b7-49a5-98f1-62b1237f3ab0</v>
+      </c>
+      <c r="B58">
+        <v>27</v>
+      </c>
+      <c r="C58" t="str">
+        <v>Tiểu sử</v>
+      </c>
+      <c r="D58" t="str">
+        <v>Biography</v>
+      </c>
+      <c r="E58" t="str">
+        <v>They wrote a biography of her life</v>
+      </c>
+      <c r="F58" t="str">
+        <v>A biography of something</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>5d8f29ff-7d1d-4e1e-82e1-34512516151c</v>
+      </c>
+      <c r="B59">
+        <v>27</v>
+      </c>
+      <c r="C59" t="str">
+        <v>Ngưỡng mộ</v>
+      </c>
+      <c r="D59" t="str">
+        <v>Admire</v>
+      </c>
+      <c r="E59" t="str">
+        <v>I admire my student's passion</v>
+      </c>
+      <c r="F59" t="str">
+        <v>Admire somebody or something</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>85f0b61e-0ab3-4e0f-a3ef-060ce867161f</v>
+      </c>
+      <c r="B60">
+        <v>27</v>
+      </c>
+      <c r="C60" t="str">
+        <v>Ngưỡng mộ</v>
+      </c>
+      <c r="D60" t="str">
+        <v>Look up to</v>
+      </c>
+      <c r="E60" t="str">
+        <v>I look up to my father very much</v>
+      </c>
+      <c r="F60" t="str">
+        <v>Look up to somebody</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>575c63cd-6cd4-43a1-b29d-d6b8960530e0</v>
+      </c>
+      <c r="B61">
+        <v>27</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Đáp ứng tiêu chuẩn</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Live up to</v>
+      </c>
+      <c r="E61" t="str">
+        <v>He lived up to my parent's expectations</v>
+      </c>
+      <c r="F61" t="str">
+        <v>Live up to my parent's expectations</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>fb90b861-646a-4dd4-b647-a4cc017bc8aa</v>
+      </c>
+      <c r="B62">
+        <v>28</v>
+      </c>
+      <c r="C62" t="str">
+        <v>Buổi hòa nhạc</v>
+      </c>
+      <c r="D62" t="str">
+        <v>Concert</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Let's go to a concert tonight!</v>
+      </c>
+      <c r="F62" t="str">
+        <v>Go to a concert</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>cbb60ea8-e319-4ef2-a23f-3d0a72e8a76d</v>
+      </c>
+      <c r="B63">
+        <v>28</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Trò xếp hình, trò giải đố</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Puzzle</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Crassword puzzles are for everyone to play</v>
+      </c>
+      <c r="F63" t="str">
+        <v>A crossword puzzle</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>6567b1a7-ce1d-4054-873f-8febe4c8c136</v>
+      </c>
+      <c r="B64">
+        <v>28</v>
+      </c>
+      <c r="C64" t="str">
+        <v>Đoán</v>
+      </c>
+      <c r="D64" t="str">
+        <v>Guess</v>
+      </c>
+      <c r="E64" t="str">
+        <v>Can you guess my age</v>
+      </c>
+      <c r="F64" t="str">
+        <v>Guess something</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>f0d6988c-f4a0-484b-b07f-71769fed5a9d</v>
+      </c>
+      <c r="B65">
+        <v>28</v>
+      </c>
+      <c r="C65" t="str">
+        <v>Tin Tường</v>
+      </c>
+      <c r="D65" t="str">
+        <v>Keen</v>
+      </c>
+      <c r="E65" t="str">
+        <v>She has a keen eye for fashion</v>
+      </c>
+      <c r="F65" t="str">
+        <v>A keen eye for something</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>8b0ee883-6437-4353-b875-c394855058aa</v>
+      </c>
+      <c r="B66">
+        <v>28</v>
+      </c>
+      <c r="C66" t="str">
+        <v>Đan</v>
+      </c>
+      <c r="D66" t="str">
+        <v>Knit</v>
+      </c>
+      <c r="E66" t="str">
+        <v>Grandma loves to knit scarves</v>
+      </c>
+      <c r="F66" t="str">
+        <v>Knit something</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>f4140d64-523c-47a1-a31d-a55a487858ad</v>
+      </c>
+      <c r="B67">
+        <v>28</v>
+      </c>
+      <c r="C67" t="str">
+        <v>Tiểu thuyết</v>
+      </c>
+      <c r="D67" t="str">
+        <v>Novel</v>
+      </c>
+      <c r="E67" t="str">
+        <v>The author wrote two best-selling novels</v>
+      </c>
+      <c r="F67" t="str">
+        <v>A best-selling novel</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>e1e7a71f-4e39-419e-a77b-86d1a1e534e9</v>
+      </c>
+      <c r="B68">
+        <v>28</v>
+      </c>
+      <c r="C68" t="str">
+        <v>Bộ sưu tập</v>
+      </c>
+      <c r="D68" t="str">
+        <v>Collection</v>
+      </c>
+      <c r="E68" t="str">
+        <v>He has a collection of vinyl records</v>
+      </c>
+      <c r="F68" t="str">
+        <v>Collection of something</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>7ec6e054-a925-4b6d-868e-7edae103be2d</v>
+      </c>
+      <c r="B69">
+        <v>28</v>
+      </c>
+      <c r="C69" t="str">
+        <v>Chèo thuyền</v>
+      </c>
+      <c r="D69" t="str">
+        <v>Sail</v>
+      </c>
+      <c r="E69" t="str">
+        <v>Can we sail a boat tomorrow?</v>
+      </c>
+      <c r="F69" t="str">
+        <v>Sail a boat</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>baac48ef-2267-4932-b04b-f8b85153bcf8</v>
+      </c>
+      <c r="B70">
+        <v>28</v>
+      </c>
+      <c r="C70" t="str">
+        <v>Có hứng thú</v>
+      </c>
+      <c r="D70" t="str">
+        <v>Interested</v>
+      </c>
+      <c r="E70" t="str">
+        <v>Are you interested in the arts?</v>
+      </c>
+      <c r="F70" t="str">
+        <v>Interested in something or somebody</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>b3a79e76-a9ed-453a-affb-d11df6cb336e</v>
+      </c>
+      <c r="B71">
+        <v>28</v>
+      </c>
+      <c r="C71" t="str">
+        <v>Nhiếp ảnh</v>
+      </c>
+      <c r="D71" t="str">
+        <v>Photography</v>
+      </c>
+      <c r="E71" t="str">
+        <v>The artist mainly does digital photography</v>
+      </c>
+      <c r="F71" t="str">
+        <v>Digital photography</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>74975ac4-5195-4360-a509-f8abcd51c71d</v>
+      </c>
+      <c r="B72">
+        <v>28</v>
+      </c>
+      <c r="C72" t="str">
+        <v>Hướng dẫn cách làm</v>
+      </c>
+      <c r="D72" t="str">
+        <v>Tutorial</v>
+      </c>
+      <c r="E72" t="str">
+        <v>Check out her step-by-step tutorial on makeup</v>
+      </c>
+      <c r="F72" t="str">
+        <v>Step-by-Step tutorial</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>8af0b848-c984-475f-af71-c73c9cf77b8b</v>
+      </c>
+      <c r="B73">
+        <v>28</v>
+      </c>
+      <c r="C73" t="str">
+        <v>Nhật ký bằng video</v>
+      </c>
+      <c r="D73" t="str">
+        <v>Vlogs</v>
+      </c>
+      <c r="E73" t="str">
+        <v/>
+      </c>
+      <c r="F73" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>b631dad9-b82c-47b5-b18e-a505891c7e86</v>
+      </c>
+      <c r="B74">
+        <v>28</v>
+      </c>
+      <c r="C74" t="str">
+        <v>Đội, nhóm</v>
+      </c>
+      <c r="D74" t="str">
+        <v>Team</v>
+      </c>
+      <c r="E74" t="str">
+        <v>The soccer team won 5-1</v>
+      </c>
+      <c r="F74" t="str">
+        <v>A soccer team</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>d7be64cc-0840-44db-9e09-27cf029efff2</v>
+      </c>
+      <c r="B75">
+        <v>28</v>
+      </c>
+      <c r="C75" t="str">
+        <v>Thử</v>
+      </c>
+      <c r="D75" t="str">
+        <v>Try out</v>
+      </c>
+      <c r="E75" t="str">
+        <v>Would you try out a new method of cooking?</v>
+      </c>
+      <c r="F75" t="str">
+        <v>Try out a new method</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>7c51af5a-2c08-40d7-9b59-971579e83fcd</v>
+      </c>
+      <c r="B76">
+        <v>28</v>
+      </c>
+      <c r="C76" t="str">
+        <v>Tham gia</v>
+      </c>
+      <c r="D76" t="str">
+        <v>Participate</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Please participate more in class</v>
+      </c>
+      <c r="F76" t="str">
+        <v>Participate in something</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>f9d5999c-a156-41b9-800c-a7802ca98ea5</v>
+      </c>
+      <c r="B77">
+        <v>28</v>
+      </c>
+      <c r="C77" t="str">
+        <v>Chương trình</v>
+      </c>
+      <c r="D77" t="str">
+        <v>Program</v>
+      </c>
+      <c r="E77" t="str">
+        <v>She works for a news program</v>
+      </c>
+      <c r="F77" t="str">
+        <v>A news program</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>c8a1854a-ae84-41f5-a5d4-a1d0aa910d2c</v>
+      </c>
+      <c r="B78">
+        <v>28</v>
+      </c>
+      <c r="C78" t="str">
+        <v>Hoạt hình</v>
+      </c>
+      <c r="D78" t="str">
+        <v>Cartoon</v>
+      </c>
+      <c r="E78" t="str">
+        <v>Mickey mouse is a walt disney cartoon</v>
+      </c>
+      <c r="F78" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>e3abb703-a37a-4308-96b6-b20859e2a6aa</v>
+      </c>
+      <c r="B79">
+        <v>28</v>
+      </c>
+      <c r="C79" t="str">
+        <v>Thể loại</v>
+      </c>
+      <c r="D79" t="str">
+        <v>Genre</v>
+      </c>
+      <c r="E79" t="str">
+        <v>What music genre do you listen to?</v>
+      </c>
+      <c r="F79" t="str">
+        <v>Music genre</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>dfa9fc23-b0d1-4e81-865b-13d53416db11</v>
+      </c>
+      <c r="B80">
+        <v>28</v>
+      </c>
+      <c r="C80" t="str">
+        <v>Phim hài</v>
+      </c>
+      <c r="D80" t="str">
+        <v>Comedy</v>
+      </c>
+      <c r="E80" t="str">
+        <v>My friend loves watching remoantic comedies</v>
+      </c>
+      <c r="F80" t="str">
+        <v>A romantic comedy</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>e9792faa-117f-408c-8aa4-bb141f602092</v>
+      </c>
+      <c r="B81">
+        <v>28</v>
+      </c>
+      <c r="C81" t="str">
+        <v>Trèo</v>
+      </c>
+      <c r="D81" t="str">
+        <v>Climb</v>
+      </c>
+      <c r="E81" t="str">
+        <v>The cat climbed up the tree</v>
+      </c>
+      <c r="F81" t="str">
+        <v>Climb up something</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>9c9784a3-bc25-46fe-99fb-cb54224c9f86</v>
+      </c>
+      <c r="B82">
+        <v>28</v>
+      </c>
+      <c r="C82" t="str">
+        <v>Sự thích thú, niềm vui</v>
+      </c>
+      <c r="D82" t="str">
+        <v>Pleasure</v>
+      </c>
+      <c r="E82" t="str">
+        <v>The kids find pleasure in singing</v>
+      </c>
+      <c r="F82" t="str">
+        <v>Take or find pleasure in doing something</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>6842266a-c5ab-4119-a535-872c36da4757</v>
+      </c>
+      <c r="B83">
+        <v>28</v>
+      </c>
+      <c r="C83" t="str">
+        <v>Trong nhà</v>
+      </c>
+      <c r="D83" t="str">
+        <v>Indoor</v>
+      </c>
+      <c r="E83" t="str">
+        <v>The hotel's indoor swimming pool is huge!</v>
+      </c>
+      <c r="F83" t="str">
+        <v>An indoor swimming pool</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>d2a15da2-9ea7-48ec-ac1c-31958d2a9169</v>
+      </c>
+      <c r="B84">
+        <v>28</v>
+      </c>
+      <c r="C84" t="str">
+        <v>Chuyến nghỉ dưỡng, kỳ nghỉ</v>
+      </c>
+      <c r="D84" t="str">
+        <v>Holiday</v>
+      </c>
+      <c r="E84" t="str">
+        <v>I do not work on holiday</v>
+      </c>
+      <c r="F84" t="str">
+        <v>On holiday</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>2c2dbe0d-943c-43ab-ba45-c532ffa886ae</v>
+      </c>
+      <c r="B85">
+        <v>28</v>
+      </c>
+      <c r="C85" t="str">
+        <v>Chuyến đi</v>
+      </c>
+      <c r="D85" t="str">
+        <v>Ride</v>
+      </c>
+      <c r="E85" t="str">
+        <v>We are in for a bumpy ride</v>
+      </c>
+      <c r="F85" t="str">
+        <v>A bumpy ride</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>41542f1d-741d-4a47-8a81-a1d09a9a966b</v>
+      </c>
+      <c r="B86">
+        <v>28</v>
+      </c>
+      <c r="C86" t="str">
+        <v>Có ý nghĩa</v>
+      </c>
+      <c r="D86" t="str">
+        <v>Meaningful</v>
+      </c>
+      <c r="E86" t="str">
+        <v>I strive to do meaningful work</v>
+      </c>
+      <c r="F86" t="str">
+        <v>Meaningful work</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>6e66b3ef-3ec5-4743-9860-7418a93dce27</v>
+      </c>
+      <c r="B87">
+        <v>28</v>
+      </c>
+      <c r="C87" t="str">
+        <v>Việc cấm trại</v>
+      </c>
+      <c r="D87" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="E87" t="str">
+        <v>We are going on a camping trip</v>
+      </c>
+      <c r="F87" t="str">
+        <v>A camping trip</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>1188e571-d666-4bf9-81ee-46334eabd388</v>
+      </c>
+      <c r="B88">
+        <v>28</v>
+      </c>
+      <c r="C88" t="str">
+        <v>Hợp tác</v>
+      </c>
+      <c r="D88" t="str">
+        <v>Cooperate</v>
+      </c>
+      <c r="E88" t="str">
+        <v>You have to cooperate with here</v>
+      </c>
+      <c r="F88" t="str">
+        <v>Cooperate with something or somebody</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>c8f79e81-dc8c-4f22-805d-0f1945deadcd</v>
+      </c>
+      <c r="B89">
+        <v>28</v>
+      </c>
+      <c r="C89" t="str">
+        <v>Lều</v>
+      </c>
+      <c r="D89" t="str">
+        <v>Tent</v>
+      </c>
+      <c r="E89" t="str">
+        <v>Please put up the tent for me</v>
+      </c>
+      <c r="F89" t="str">
+        <v>Put up a tent</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>df9891a5-2a7a-4754-91d7-ff7fffc40477</v>
+      </c>
+      <c r="B90">
+        <v>28</v>
+      </c>
+      <c r="C90" t="str">
+        <v>Hứng thú với</v>
+      </c>
+      <c r="D90" t="str">
+        <v>Go in for</v>
+      </c>
+      <c r="E90" t="str">
+        <v>My sister decides to go in for a debate competition</v>
+      </c>
+      <c r="F90" t="str">
+        <v>Go in for a competition</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>f1186873-4969-486d-bd89-9a0695b5388f</v>
+      </c>
+      <c r="B91">
+        <v>28</v>
+      </c>
+      <c r="C91" t="str">
+        <v>Thích hơn</v>
+      </c>
+      <c r="D91" t="str">
+        <v>Prefer</v>
+      </c>
+      <c r="E91" t="str">
+        <v>She prefers eating apples to pears</v>
+      </c>
+      <c r="F91" t="str">
+        <v>Prefer something to something</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>a2b1778e-1bde-4f07-8efc-386e9629f6dc</v>
+      </c>
+      <c r="B92">
+        <v>29</v>
+      </c>
+      <c r="C92" t="str">
+        <v>Câu cá</v>
+      </c>
+      <c r="D92" t="str">
+        <v>Fishing</v>
+      </c>
+      <c r="E92" t="str">
+        <v>My dad and I go fishing every day</v>
+      </c>
+      <c r="F92" t="str">
+        <v>Go fishing</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>cf990805-78a4-450b-9080-8d1407d56334</v>
+      </c>
+      <c r="B93">
+        <v>29</v>
+      </c>
+      <c r="C93" t="str">
+        <v>Vận động viên</v>
+      </c>
+      <c r="D93" t="str">
+        <v>Athlete</v>
+      </c>
+      <c r="E93" t="str">
+        <v>Olumpic athletes train hard to complete</v>
+      </c>
+      <c r="F93" t="str">
+        <v>An Olympic athlete</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>b6a3f27f-b5f1-4f59-a13a-5a3b1d198402</v>
+      </c>
+      <c r="B94">
+        <v>29</v>
+      </c>
+      <c r="C94" t="str">
+        <v>Môn đấu vật</v>
+      </c>
+      <c r="D94" t="str">
+        <v>Wrestling</v>
+      </c>
+      <c r="E94" t="str">
+        <v>Wrestling matches are popular in the US</v>
+      </c>
+      <c r="F94" t="str">
+        <v>A wrestling match</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>f903164f-992c-4ff7-bdd0-9796bb39e5eb</v>
+      </c>
+      <c r="B95">
+        <v>29</v>
+      </c>
+      <c r="C95" t="str">
+        <v>Chuyên nghiệp</v>
+      </c>
+      <c r="D95" t="str">
+        <v>Professional</v>
+      </c>
+      <c r="E95" t="str">
+        <v>He was a professional soccer player</v>
+      </c>
+      <c r="F95" t="str">
+        <v>A professional soccer player</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>f38ea113-6eed-41a7-864c-9fd8eb997c46</v>
+      </c>
+      <c r="B96">
+        <v>29</v>
+      </c>
+      <c r="C96" t="str">
+        <v>Hàng năm</v>
+      </c>
+      <c r="D96" t="str">
+        <v>Annual</v>
+      </c>
+      <c r="E96" t="str">
+        <v>The company has annual meetings for us</v>
+      </c>
+      <c r="F96" t="str">
+        <v>An annual meeting</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>cec821bf-15bc-4c73-85e6-328b2b004fd1</v>
+      </c>
+      <c r="B97">
+        <v>29</v>
+      </c>
+      <c r="C97" t="str">
+        <v>Giải đấu</v>
+      </c>
+      <c r="D97" t="str">
+        <v>Tournament</v>
+      </c>
+      <c r="E97" t="str">
+        <v>What an exciting soccer tournament!</v>
+      </c>
+      <c r="F97" t="str">
+        <v>A soccer tournament</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>ddae4d17-2487-4c91-b15b-62ec664e7e93</v>
+      </c>
+      <c r="B98">
+        <v>29</v>
+      </c>
+      <c r="C98" t="str">
+        <v>Huấn luyện viên</v>
+      </c>
+      <c r="D98" t="str">
+        <v>Coach</v>
+      </c>
+      <c r="E98" t="str">
+        <v>The team coach trains us hard</v>
+      </c>
+      <c r="F98" t="str">
+        <v>The team coach</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>9c573cff-4ddd-4aec-83ca-2f88d870993e</v>
+      </c>
+      <c r="B99">
+        <v>29</v>
+      </c>
+      <c r="C99" t="str">
+        <v>Trận đấu</v>
+      </c>
+      <c r="D99" t="str">
+        <v>Match</v>
+      </c>
+      <c r="E99" t="str">
+        <v>There is a soccer match tonight</v>
+      </c>
+      <c r="F99" t="str">
+        <v>A soccer match</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>dd72f5c5-8548-436c-bd33-79ddb20c7437</v>
+      </c>
+      <c r="B100">
+        <v>29</v>
+      </c>
+      <c r="C100" t="str">
+        <v>Đánh bại</v>
+      </c>
+      <c r="D100" t="str">
+        <v>Beat</v>
+      </c>
+      <c r="E100" t="str">
+        <v>They beat their opponents in the first round</v>
+      </c>
+      <c r="F100" t="str">
+        <v>Beat something or somebody</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>b1892029-56ff-4cbe-984a-c7dab29a9977</v>
+      </c>
+      <c r="B101">
+        <v>29</v>
+      </c>
+      <c r="C101" t="str">
+        <v>Đối thủ</v>
+      </c>
+      <c r="D101" t="str">
+        <v>Opponent</v>
+      </c>
+      <c r="E101" t="str">
+        <v>She is my opponent in chess</v>
+      </c>
+      <c r="F101" t="str">
+        <v>One's oppponent in something</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>1e190ed8-33a8-4e71-b7b2-fa84c7c02941</v>
+      </c>
+      <c r="B102">
+        <v>29</v>
+      </c>
+      <c r="C102" t="str">
+        <v>Môn thể thao</v>
+      </c>
+      <c r="D102" t="str">
+        <v>Athletics</v>
+      </c>
+      <c r="E102" t="str">
+        <v>Football, soccer, and baseball are types of atheletics</v>
+      </c>
+      <c r="F102" t="str">
+        <v>Types of athletics</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>d38353fc-5f4f-472c-ac04-668987f0a4a7</v>
+      </c>
+      <c r="B103">
+        <v>29</v>
+      </c>
+      <c r="C103" t="str">
+        <v>Bóng rỗ</v>
+      </c>
+      <c r="D103" t="str">
+        <v>Basketball</v>
+      </c>
+      <c r="E103" t="str">
+        <v>I am the captain of the basketball team</v>
+      </c>
+      <c r="F103" t="str">
+        <v>A basketball team</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>ef65ce51-588d-4574-aabf-54d79f5fccc8</v>
+      </c>
+      <c r="B104">
+        <v>29</v>
+      </c>
+      <c r="C104" t="str">
+        <v>Người chơi</v>
+      </c>
+      <c r="D104" t="str">
+        <v>Player</v>
+      </c>
+      <c r="E104" t="str">
+        <v>He is the best soccer player here</v>
+      </c>
+      <c r="F104" t="str">
+        <v>A soccer player</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>b7c13a10-8f6b-4bc0-adf4-4efd66aa87fc</v>
+      </c>
+      <c r="B105">
+        <v>29</v>
+      </c>
+      <c r="C105" t="str">
+        <v xml:space="preserve">Liên đoàn </v>
+      </c>
+      <c r="D105" t="str">
+        <v>League</v>
+      </c>
+      <c r="E105" t="str">
+        <v>My sone plays for a soccer league</v>
+      </c>
+      <c r="F105" t="str">
+        <v>A soccer league</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>cbf03296-0921-4040-90d4-199fd9d5c23b</v>
+      </c>
+      <c r="B106">
+        <v>29</v>
+      </c>
+      <c r="C106" t="str">
+        <v>Giải vô địch</v>
+      </c>
+      <c r="D106" t="str">
+        <v>Championship</v>
+      </c>
+      <c r="E106" t="str">
+        <v>Are you ready for the basketball championship</v>
+      </c>
+      <c r="F106" t="str">
+        <v>A basketball championship</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>5029497b-8c66-41b8-8d0a-4bfe381c4286</v>
+      </c>
+      <c r="B107">
+        <v>29</v>
+      </c>
+      <c r="C107" t="str">
+        <v>Đội trưởng</v>
+      </c>
+      <c r="D107" t="str">
+        <v>Captain</v>
+      </c>
+      <c r="E107" t="str">
+        <v>We vote for a team camtain</v>
+      </c>
+      <c r="F107" t="str">
+        <v>Team captain</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>c2fb9123-f320-4cc1-a7fa-d38da99a5fc1</v>
+      </c>
+      <c r="B108">
+        <v>29</v>
+      </c>
+      <c r="C108" t="str">
+        <v>Ghi điểm</v>
+      </c>
+      <c r="D108" t="str">
+        <v>Score</v>
+      </c>
+      <c r="E108" t="str">
+        <v>He scored a goal for the team</v>
+      </c>
+      <c r="F108" t="str">
+        <v>Score a goal</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>a52a7a35-9823-4ea9-87c9-6dec37ecf622</v>
+      </c>
+      <c r="B109">
+        <v>29</v>
+      </c>
+      <c r="C109" t="str">
+        <v>Danh hiệu</v>
+      </c>
+      <c r="D109" t="str">
+        <v>Title</v>
+      </c>
+      <c r="E109" t="str">
+        <v>The team won the title with a goal in the last minute</v>
+      </c>
+      <c r="F109" t="str">
+        <v>Win the title</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>916d379b-cba3-40d9-a67f-a71d48b74a2f</v>
+      </c>
+      <c r="B110">
+        <v>29</v>
+      </c>
+      <c r="C110" t="str">
+        <v>Lưới</v>
+      </c>
+      <c r="D110" t="str">
+        <v>Net</v>
+      </c>
+      <c r="E110" t="str">
+        <v>The fishing net has holes in it</v>
+      </c>
+      <c r="F110" t="str">
+        <v>A fishing net</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>463b16e3-432e-446b-bea0-a0f2b3da5f06</v>
+      </c>
+      <c r="B111">
+        <v>29</v>
+      </c>
+      <c r="C111" t="str">
+        <v>Anh hùng</v>
+      </c>
+      <c r="D111" t="str">
+        <v>Hero</v>
+      </c>
+      <c r="E111" t="str">
+        <v>The fireman became a local hero</v>
+      </c>
+      <c r="F111" t="str">
+        <v>A local hero</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>39de71b0-d5b5-48c9-8f4d-95b2e2f50af6</v>
+      </c>
+      <c r="B112">
+        <v>29</v>
+      </c>
+      <c r="C112" t="str">
+        <v>Môn đạp xe</v>
+      </c>
+      <c r="D112" t="str">
+        <v>Cycling</v>
+      </c>
+      <c r="E112" t="str">
+        <v>She went cycling down the hill</v>
+      </c>
+      <c r="F112" t="str">
+        <v>Go cycling</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>aae25fe9-c463-44f6-8403-64b3ab4901df</v>
+      </c>
+      <c r="B113">
+        <v>29</v>
+      </c>
+      <c r="C113" t="str">
+        <v>Sân vận động</v>
+      </c>
+      <c r="D113" t="str">
+        <v>Stadium</v>
+      </c>
+      <c r="E113" t="str">
+        <v>Where is the biggest sports stadium in hanoi</v>
+      </c>
+      <c r="F113" t="str">
+        <v>A sport stadium</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>a8bd58e5-0590-4ebb-9b28-1b10efe4f691</v>
+      </c>
+      <c r="B114">
+        <v>29</v>
+      </c>
+      <c r="C114" t="str">
+        <v>Người thắng cuộc</v>
+      </c>
+      <c r="D114" t="str">
+        <v>Winner</v>
+      </c>
+      <c r="E114" t="str">
+        <v>The actor is an award winner</v>
+      </c>
+      <c r="F114" t="str">
+        <v>An award winer</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>b553acc6-a0c9-417a-b2d9-d77e5fd33909</v>
+      </c>
+      <c r="B115">
+        <v>29</v>
+      </c>
+      <c r="C115" t="str">
+        <v>Môn đánh golf</v>
+      </c>
+      <c r="D115" t="str">
+        <v>Golf</v>
+      </c>
+      <c r="E115" t="str">
+        <v>Businessmen love to play golf</v>
+      </c>
+      <c r="F115" t="str">
+        <v>Play golf</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>c9b2d631-4c95-4cbf-b5c6-51760a9800c8</v>
+      </c>
+      <c r="B116">
+        <v>29</v>
+      </c>
+      <c r="C116" t="str">
+        <v>Đánh</v>
+      </c>
+      <c r="D116" t="str">
+        <v>Strike</v>
+      </c>
+      <c r="E116" t="str">
+        <v>He strikes the golf ball perfectly</v>
+      </c>
+      <c r="F116" t="str">
+        <v>Strike the ball</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>6c846374-0b04-4261-a1fc-abb952bde9d0</v>
+      </c>
+      <c r="B117">
+        <v>29</v>
+      </c>
+      <c r="C117" t="str">
+        <v>Đích, mục tiêu</v>
+      </c>
+      <c r="D117" t="str">
+        <v>Target</v>
+      </c>
+      <c r="E117" t="str">
+        <v>He shot the arrow and hit the target</v>
+      </c>
+      <c r="F117" t="str">
+        <v>Hit the target</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>7c39a7bf-0223-4d67-bf19-bc70d6260a4c</v>
+      </c>
+      <c r="B118">
+        <v>29</v>
+      </c>
+      <c r="C118" t="str">
+        <v>Tối đa</v>
+      </c>
+      <c r="D118" t="str">
+        <v>Maximum</v>
+      </c>
+      <c r="E118" t="str">
+        <v>The maximum amount for storage is 256GB</v>
+      </c>
+      <c r="F118" t="str">
+        <v>The maximum amount</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>727a487b-ea11-4357-8b3a-cfd78069fedb</v>
+      </c>
+      <c r="B119">
+        <v>29</v>
+      </c>
+      <c r="C119" t="str">
+        <v>Lướt</v>
+      </c>
+      <c r="D119" t="str">
+        <v>Surf</v>
+      </c>
+      <c r="E119" t="str">
+        <v>In hawaii, you must surf the waves</v>
+      </c>
+      <c r="F119" t="str">
+        <v>Surf the wave</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>86cb971a-bdd1-45d0-9169-17ef0fb2990e</v>
+      </c>
+      <c r="B120">
+        <v>29</v>
+      </c>
+      <c r="C120" t="str">
+        <v>Không may</v>
+      </c>
+      <c r="D120" t="str">
+        <v>Unfortunately</v>
+      </c>
+      <c r="E120" t="str">
+        <v>Unfortunately, I won't be able to attend the meeting</v>
+      </c>
+      <c r="F120" t="str">
+        <v>Unfortunately, I won't</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>2805d4a5-2450-4193-92b7-19d2357bd4d9</v>
+      </c>
+      <c r="B121">
+        <v>29</v>
+      </c>
+      <c r="C121" t="str">
+        <v>Trân trọng, đánh giá cao</v>
+      </c>
+      <c r="D121" t="str">
+        <v>Appreciate</v>
+      </c>
+      <c r="E121" t="str">
+        <v>I appreciate the help you gave me</v>
+      </c>
+      <c r="F121" t="str">
+        <v>Appreciate somebody or something</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F121"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add search function
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -6,6 +6,7 @@
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
     <sheet name="Update_ea9e" sheetId="2" r:id="rId2"/>
     <sheet name="Update_3987" sheetId="3" r:id="rId3"/>
+    <sheet name="Update_da6e" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -7213,4 +7214,2438 @@
     <ignoredError numberStoredAsText="1" sqref="A1:F121"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F121"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>unitId</v>
+      </c>
+      <c r="C1" t="str">
+        <v>word</v>
+      </c>
+      <c r="D1" t="str">
+        <v>answers</v>
+      </c>
+      <c r="E1" t="str">
+        <v>sentences</v>
+      </c>
+      <c r="F1" t="str">
+        <v>phrases</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2855e402-1dfa-4dc2-8840-cebd848fa19c</v>
+      </c>
+      <c r="B2">
+        <v>26</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Chương trình</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Show</v>
+      </c>
+      <c r="E2" t="str">
+        <v>I watch TV shows on my television</v>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>d90b062b-c464-4c5c-bf4d-2d250fee42b4</v>
+      </c>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Cảnh</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Scene</v>
+      </c>
+      <c r="E3" t="str">
+        <v>The crew needs to film a scene</v>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>d670b0d5-a0f9-4e3d-be7e-7539b709f4bf</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Nam diễn viên</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Actor</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Who is the lead actor in titanic</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>0b08724a-3034-4e5c-9eed-a809189bff3a</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Thuộc âm nhạc</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Musical</v>
+      </c>
+      <c r="E5" t="str">
+        <v xml:space="preserve">The audience loved the musical performance </v>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>4152b846-3f6e-4b76-b48c-320c8d9bf98d</v>
+      </c>
+      <c r="B6">
+        <v>26</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Nhạc phim</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Soundtrack</v>
+      </c>
+      <c r="E6" t="str">
+        <v>The soundtrack of this movie is great</v>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>f9c612cb-22a0-4f9d-a949-c179e45f0655</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Thuộc lịch sử</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Historical</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Albert Einstein is an important historical figure</v>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>53af5326-467e-4e15-a189-ec4723760626</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Bí ẩn</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Mystery</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Nobody can solve the mystery of the Bermuda triangle</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>faab9a2e-d127-4a38-abf1-879e33beef60</v>
+      </c>
+      <c r="B9">
+        <v>26</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Tội ác</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Crime</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Stealing money is a serious crime</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>da3b1816-173a-4493-ad15-7beb97e72ba5</v>
+      </c>
+      <c r="B10">
+        <v>26</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Đoạn kết</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Ending</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Fairy tales have happy endings</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>e98b5079-2952-47db-afac-31e8e8b2ded1</v>
+      </c>
+      <c r="B11">
+        <v>26</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Tiết lộ</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Reveal</v>
+      </c>
+      <c r="E11" t="str">
+        <v>The magician never reveals the truth</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>6834a067-2935-4767-b07e-7e28c2af50bc</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Phim giật gân</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Thriller</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Thriller movies are scary</v>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>eec73fe0-6f13-4d23-b16e-304b453fd1eb</v>
+      </c>
+      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Xưởng, không gian sáng tạo</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Studio</v>
+      </c>
+      <c r="E13" t="str">
+        <v>She teaches us at her dance studio</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>d82e9755-cb4a-4e76-b2d1-c22e9bbd3e4a</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Bối cảnh, khung cảnh</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Setting</v>
+      </c>
+      <c r="E14" t="str">
+        <v xml:space="preserve">What a beautiful setting this city is </v>
+      </c>
+      <c r="F14" t="str">
+        <v>A beautiful setting</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>80af4f65-e319-4276-abc7-c4b93cfb684f</v>
+      </c>
+      <c r="B15">
+        <v>26</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Điều viễn tưởng</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Fiction</v>
+      </c>
+      <c r="E15" t="str">
+        <v>She wrote fiction on aliens and love</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>66eb9a3b-e5cf-4572-af26-c0ced46a6a41</v>
+      </c>
+      <c r="B16">
+        <v>26</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Sự việc kịch tính</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Drama</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Teens like to watch drama series</v>
+      </c>
+      <c r="F16" t="str">
+        <v>A drama series</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>6d66f4e3-1575-453b-9c56-b2e35ae6f572</v>
+      </c>
+      <c r="B17">
+        <v>26</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Đạo diễn</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Director</v>
+      </c>
+      <c r="E17" t="str">
+        <v>The young film director deserves our recognition</v>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>c61cf54e-76e9-4c4f-a546-be16ad5e5bcf</v>
+      </c>
+      <c r="B18">
+        <v>26</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Ra mắt</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Come out</v>
+      </c>
+      <c r="E18" t="str">
+        <v>When is her album coming out?</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Something new comes out</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>75d97f77-6607-497c-a34c-c08e4276bc76</v>
+      </c>
+      <c r="B19">
+        <v>26</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Nhân vật</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Character</v>
+      </c>
+      <c r="E19" t="str">
+        <v>The main character in "Batman" is mysterious</v>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>e2745e17-f355-4999-984f-246339ace9e7</v>
+      </c>
+      <c r="B20">
+        <v>26</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Nữ diễn viên</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Actress</v>
+      </c>
+      <c r="E20" t="str">
+        <v>She was a good actress back then</v>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>d883b560-e598-4399-b67a-fbd255f88070</v>
+      </c>
+      <c r="B21">
+        <v>26</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Kỳ lạ, kỳ quặc</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Odd</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Hanging out with odd people is fun</v>
+      </c>
+      <c r="F21" t="str">
+        <v>An odd person</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>861042fb-7382-4b86-b5dc-6f8a0f267c2b</v>
+      </c>
+      <c r="B22">
+        <v>26</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Màn hình</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Screen</v>
+      </c>
+      <c r="E22" t="str">
+        <v>The laptop has a big computer screen</v>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>2c327c19-447e-45c6-8278-14aa65293f96</v>
+      </c>
+      <c r="B23">
+        <v>26</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Hành động</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Action</v>
+      </c>
+      <c r="E23" t="str">
+        <v>My favorite action movie is Fast and Furious</v>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>1c7e5e1d-737d-4a0f-9124-6e6415aaab50</v>
+      </c>
+      <c r="B24">
+        <v>26</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Chuyến phiêu lưu</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Adventure</v>
+      </c>
+      <c r="E24" t="str">
+        <v>I seek an adventure of a lifetime</v>
+      </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>046efda8-e3b4-4698-a754-cacebf1c90e0</v>
+      </c>
+      <c r="B25">
+        <v>26</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Phim tài liệu</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Documentary</v>
+      </c>
+      <c r="E25" t="str">
+        <v>I watched that documentary film on Netflix</v>
+      </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>7040324e-e5a2-44f4-9535-b2cc9cbdb924</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Góc</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Angle</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Tilt your head to a 45 angle</v>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>988a2983-945c-4cf0-ba48-152e92f249c4</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Thấy khó hiểu</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Confused</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Are you confused about the instructions?</v>
+      </c>
+      <c r="F27" t="str">
+        <v>Confused about something</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>928cac87-df35-4693-90eb-0b7ac9ba4f7c</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Cuộc hội thoại, lời thoại</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Dialogue</v>
+      </c>
+      <c r="E28" t="str">
+        <v>The dialogue with my therapist helped me</v>
+      </c>
+      <c r="F28" t="str">
+        <v>Dialogue with somebody</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>470241db-5ef4-4605-923a-0f067329f20f</v>
+      </c>
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Tác phẩm thành công</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Hit</v>
+      </c>
+      <c r="E29" t="str">
+        <v>His book became a big hit</v>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>972036e4-0ba9-4393-b01e-adb398bcbf0c</v>
+      </c>
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Tuyệt vời</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Wonderful</v>
+      </c>
+      <c r="E30" t="str">
+        <v>I am grateful for the wonderful opportunity</v>
+      </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>fefbe098-b8f8-40ef-87d2-ea757ae401e2</v>
+      </c>
+      <c r="B31">
+        <v>26</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Tài giỏi, tuyệt vời</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Brilliant</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Thank you for the brilliant idea</v>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>7ced7a2e-75de-4804-ac90-20e3e958d965</v>
+      </c>
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Khiêm tốn</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Modest</v>
+      </c>
+      <c r="E32" t="str">
+        <v>You are too modest! You are gifted.</v>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>4b5d71f1-69c8-4d40-917c-56ed60fa341a</v>
+      </c>
+      <c r="B33">
+        <v>27</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Có năng khiếu</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Gifted</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Do you consider yourself a gifted musican?</v>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>f249b615-9ce7-490b-aeb1-e7fb50956f75</v>
+      </c>
+      <c r="B34">
+        <v>27</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Ngành giải trí</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Showbiz</v>
+      </c>
+      <c r="E34" t="str">
+        <v>People in showbiz are movie stars</v>
+      </c>
+      <c r="F34" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>33645007-d97b-4e05-9fbb-18ce6453df08</v>
+      </c>
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Kênh</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Channel</v>
+      </c>
+      <c r="E35" t="str">
+        <v>The show is live on the VTV3 channel</v>
+      </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>c1f5fd98-6823-4cd2-8332-437b40d1cdbb</v>
+      </c>
+      <c r="B36">
+        <v>27</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Truyền thông</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Media</v>
+      </c>
+      <c r="E36" t="str">
+        <v>My mom posts so many pictures on social media</v>
+      </c>
+      <c r="F36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>9e32b63e-6f9b-484a-a3cf-03b2554b0c81</v>
+      </c>
+      <c r="B37">
+        <v>27</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Nổi tiếng</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Well-known</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Is he a well-known actor?</v>
+      </c>
+      <c r="F37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>3af0b7f7-7574-4b56-bf9b-afbdc9d94496</v>
+      </c>
+      <c r="B38">
+        <v>27</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Nhận ra</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Recognize</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Did you recognize me on stage?</v>
+      </c>
+      <c r="F38" t="str">
+        <v>Recognize somebody or something</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>cd2a5828-bdf8-445c-81a1-3926ae9be2da</v>
+      </c>
+      <c r="B39">
+        <v>27</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Người hâm mộ</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Fan</v>
+      </c>
+      <c r="E39" t="str">
+        <v>My girlfriend is a big soccer fan</v>
+      </c>
+      <c r="F39" t="str">
+        <v>A soccer fan</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>123fb41c-f345-498c-a994-9a9b27e98bf8</v>
+      </c>
+      <c r="B40">
+        <v>27</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Đăng ký</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Subscribe</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Please subscribe to step up english youtube channel</v>
+      </c>
+      <c r="F40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>87d2b191-c73b-403f-96bc-6f392d27e7b2</v>
+      </c>
+      <c r="B41">
+        <v>27</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Hét to</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Sceam</v>
+      </c>
+      <c r="E41" t="str">
+        <v>They screamed out loud for help</v>
+      </c>
+      <c r="F41" t="str">
+        <v>Scream out loud</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>5a4867f1-271f-4ee0-865d-7d7eb2b42d5d</v>
+      </c>
+      <c r="B42">
+        <v>27</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Buồn cười</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Funny</v>
+      </c>
+      <c r="E42" t="str">
+        <v>The funny story made me laugh hard</v>
+      </c>
+      <c r="F42" t="str">
+        <v>A funny story</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>3423a5df-5518-4d10-9006-6b46aef0c92f</v>
+      </c>
+      <c r="B43">
+        <v>27</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Hiện nay</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Currently</v>
+      </c>
+      <c r="E43" t="str">
+        <v>I am currently working as a front-end developer</v>
+      </c>
+      <c r="F43" t="str">
+        <v>Currently working as something</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>dac664bf-4d84-4185-9955-6184e4705180</v>
+      </c>
+      <c r="B44">
+        <v>27</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Lan truyền nhanh</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Viral</v>
+      </c>
+      <c r="E44" t="str">
+        <v>The video went viral on Facebook</v>
+      </c>
+      <c r="F44" t="str">
+        <v>Go viral</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>8d87d414-5e8f-41e4-8024-820fa8e2834f</v>
+      </c>
+      <c r="B45">
+        <v>27</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Màn biểu diễn</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Performance</v>
+      </c>
+      <c r="E45" t="str">
+        <v>The opera singer delivered an outstanding performance</v>
+      </c>
+      <c r="F45" t="str">
+        <v>Deliver an outstanding performance</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>999e1a08-f844-4088-a0eb-d43b316c22f6</v>
+      </c>
+      <c r="B46">
+        <v>27</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Quá khứ</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Past</v>
+      </c>
+      <c r="E46" t="str">
+        <v>I used to live abroad in the past</v>
+      </c>
+      <c r="F46" t="str">
+        <v>In the past</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>f3268128-5bfc-4b77-b848-87fd19d76a2d</v>
+      </c>
+      <c r="B47">
+        <v>27</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Trở nên</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Become</v>
+      </c>
+      <c r="E47" t="str">
+        <v>I want to become a person of influence</v>
+      </c>
+      <c r="F47" t="str">
+        <v>Become somebody or something</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>abf03747-d6bf-4469-9f81-fdf87f96dce3</v>
+      </c>
+      <c r="B48">
+        <v>27</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Toàn cầu</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Global</v>
+      </c>
+      <c r="E48" t="str">
+        <v>The singer's talent made her go global</v>
+      </c>
+      <c r="F48" t="str">
+        <v>Go global</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>cba5a361-0281-4457-a39e-8fff93b461df</v>
+      </c>
+      <c r="B49">
+        <v>27</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Lên tiếng</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Speak out</v>
+      </c>
+      <c r="E49" t="str">
+        <v>She bravely spoke out against her boss</v>
+      </c>
+      <c r="F49" t="str">
+        <v>Speak out against somebody or something</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>ba407704-b048-4ddc-b6ff-92559d5fe029</v>
+      </c>
+      <c r="B50">
+        <v>27</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Xứng đáng</v>
+      </c>
+      <c r="D50" t="str">
+        <v>Deserve</v>
+      </c>
+      <c r="E50" t="str">
+        <v>I deserve ice cream after work</v>
+      </c>
+      <c r="F50" t="str">
+        <v>Deserve something</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>a23819c9-7af3-4246-a061-633cfade115b</v>
+      </c>
+      <c r="B51">
+        <v>27</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Trực tiếp</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Live</v>
+      </c>
+      <c r="E51" t="str">
+        <v>The band did a live performance</v>
+      </c>
+      <c r="F51" t="str">
+        <v>A live performance</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>bacb314f-3d07-4d2c-ad43-ee564b779903</v>
+      </c>
+      <c r="B52">
+        <v>27</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Giải thưởng</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Award</v>
+      </c>
+      <c r="E52" t="str">
+        <v>She received an award for her acting</v>
+      </c>
+      <c r="F52" t="str">
+        <v>Receive an award</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>a499a65c-f6a4-43bf-b3af-7414b2c94310</v>
+      </c>
+      <c r="B53">
+        <v>27</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Danh dự</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Honor</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Welcome, you are my guest of honor</v>
+      </c>
+      <c r="F53" t="str">
+        <v>The guest of honor</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>48d3d3eb-d568-4c77-8488-43c41b7afbf5</v>
+      </c>
+      <c r="B54">
+        <v>27</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Việc thiện nguyện</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Charity</v>
+      </c>
+      <c r="E54" t="str">
+        <v>We should do charity for the disadvantaged</v>
+      </c>
+      <c r="F54" t="str">
+        <v>Do charity for somebody</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>0aa13e64-c9da-42cf-98a6-ea7b261bfbc8</v>
+      </c>
+      <c r="B55">
+        <v>27</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Tình nguyện</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Volunteer</v>
+      </c>
+      <c r="E55" t="str">
+        <v>She volunteered to clean the car</v>
+      </c>
+      <c r="F55" t="str">
+        <v>Volunteer to do something</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>200b047e-f499-4d66-99d8-fbca132dfb75</v>
+      </c>
+      <c r="B56">
+        <v>27</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Vụ bê bối</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Scandal</v>
+      </c>
+      <c r="E56" t="str">
+        <v>He created the scandal to attract attention</v>
+      </c>
+      <c r="F56" t="str">
+        <v>Create a scandal</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>3b253e28-0230-47de-a666-91be77248828</v>
+      </c>
+      <c r="B57">
+        <v>27</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Tin đồn</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Rumor</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Rumor has it that you got the job!</v>
+      </c>
+      <c r="F57" t="str">
+        <v>Rumor has it that</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>4334038f-c1b7-49a5-98f1-62b1237f3ab0</v>
+      </c>
+      <c r="B58">
+        <v>27</v>
+      </c>
+      <c r="C58" t="str">
+        <v>Tiểu sử</v>
+      </c>
+      <c r="D58" t="str">
+        <v>Biography</v>
+      </c>
+      <c r="E58" t="str">
+        <v>They wrote a biography of her life</v>
+      </c>
+      <c r="F58" t="str">
+        <v>A biography of something</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>5d8f29ff-7d1d-4e1e-82e1-34512516151c</v>
+      </c>
+      <c r="B59">
+        <v>27</v>
+      </c>
+      <c r="C59" t="str">
+        <v>Ngưỡng mộ</v>
+      </c>
+      <c r="D59" t="str">
+        <v>Admire</v>
+      </c>
+      <c r="E59" t="str">
+        <v>I admire my student's passion</v>
+      </c>
+      <c r="F59" t="str">
+        <v>Admire somebody or something</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>85f0b61e-0ab3-4e0f-a3ef-060ce867161f</v>
+      </c>
+      <c r="B60">
+        <v>27</v>
+      </c>
+      <c r="C60" t="str">
+        <v>Ngưỡng mộ</v>
+      </c>
+      <c r="D60" t="str">
+        <v>Look up to</v>
+      </c>
+      <c r="E60" t="str">
+        <v>I look up to my father very much</v>
+      </c>
+      <c r="F60" t="str">
+        <v>Look up to somebody</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>575c63cd-6cd4-43a1-b29d-d6b8960530e0</v>
+      </c>
+      <c r="B61">
+        <v>27</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Đáp ứng tiêu chuẩn</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Live up to</v>
+      </c>
+      <c r="E61" t="str">
+        <v>He lived up to my parent's expectations</v>
+      </c>
+      <c r="F61" t="str">
+        <v>Live up to my parent's expectations</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>fb90b861-646a-4dd4-b647-a4cc017bc8aa</v>
+      </c>
+      <c r="B62">
+        <v>28</v>
+      </c>
+      <c r="C62" t="str">
+        <v>Buổi hòa nhạc</v>
+      </c>
+      <c r="D62" t="str">
+        <v>Concert</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Let's go to a concert tonight!</v>
+      </c>
+      <c r="F62" t="str">
+        <v>Go to a concert</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>cbb60ea8-e319-4ef2-a23f-3d0a72e8a76d</v>
+      </c>
+      <c r="B63">
+        <v>28</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Trò xếp hình, trò giải đố</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Puzzle</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Crassword puzzles are for everyone to play</v>
+      </c>
+      <c r="F63" t="str">
+        <v>A crossword puzzle</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>6567b1a7-ce1d-4054-873f-8febe4c8c136</v>
+      </c>
+      <c r="B64">
+        <v>28</v>
+      </c>
+      <c r="C64" t="str">
+        <v>Đoán</v>
+      </c>
+      <c r="D64" t="str">
+        <v>Guess</v>
+      </c>
+      <c r="E64" t="str">
+        <v>Can you guess my age</v>
+      </c>
+      <c r="F64" t="str">
+        <v>Guess something</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>f0d6988c-f4a0-484b-b07f-71769fed5a9d</v>
+      </c>
+      <c r="B65">
+        <v>28</v>
+      </c>
+      <c r="C65" t="str">
+        <v>Tin Tường</v>
+      </c>
+      <c r="D65" t="str">
+        <v>Keen</v>
+      </c>
+      <c r="E65" t="str">
+        <v>She has a keen eye for fashion</v>
+      </c>
+      <c r="F65" t="str">
+        <v>A keen eye for something</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>8b0ee883-6437-4353-b875-c394855058aa</v>
+      </c>
+      <c r="B66">
+        <v>28</v>
+      </c>
+      <c r="C66" t="str">
+        <v>Đan</v>
+      </c>
+      <c r="D66" t="str">
+        <v>Knit</v>
+      </c>
+      <c r="E66" t="str">
+        <v>Grandma loves to knit scarves</v>
+      </c>
+      <c r="F66" t="str">
+        <v>Knit something</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>f4140d64-523c-47a1-a31d-a55a487858ad</v>
+      </c>
+      <c r="B67">
+        <v>28</v>
+      </c>
+      <c r="C67" t="str">
+        <v>Tiểu thuyết</v>
+      </c>
+      <c r="D67" t="str">
+        <v>Novel</v>
+      </c>
+      <c r="E67" t="str">
+        <v>The author wrote two best-selling novels</v>
+      </c>
+      <c r="F67" t="str">
+        <v>A best-selling novel</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>e1e7a71f-4e39-419e-a77b-86d1a1e534e9</v>
+      </c>
+      <c r="B68">
+        <v>28</v>
+      </c>
+      <c r="C68" t="str">
+        <v>Bộ sưu tập</v>
+      </c>
+      <c r="D68" t="str">
+        <v>Collection</v>
+      </c>
+      <c r="E68" t="str">
+        <v>He has a collection of vinyl records</v>
+      </c>
+      <c r="F68" t="str">
+        <v>Collection of something</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>7ec6e054-a925-4b6d-868e-7edae103be2d</v>
+      </c>
+      <c r="B69">
+        <v>28</v>
+      </c>
+      <c r="C69" t="str">
+        <v>Chèo thuyền</v>
+      </c>
+      <c r="D69" t="str">
+        <v>Sail</v>
+      </c>
+      <c r="E69" t="str">
+        <v>Can we sail a boat tomorrow?</v>
+      </c>
+      <c r="F69" t="str">
+        <v>Sail a boat</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>baac48ef-2267-4932-b04b-f8b85153bcf8</v>
+      </c>
+      <c r="B70">
+        <v>28</v>
+      </c>
+      <c r="C70" t="str">
+        <v>Có hứng thú</v>
+      </c>
+      <c r="D70" t="str">
+        <v>Interested</v>
+      </c>
+      <c r="E70" t="str">
+        <v>Are you interested in the arts?</v>
+      </c>
+      <c r="F70" t="str">
+        <v>Interested in something or somebody</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>b3a79e76-a9ed-453a-affb-d11df6cb336e</v>
+      </c>
+      <c r="B71">
+        <v>28</v>
+      </c>
+      <c r="C71" t="str">
+        <v>Nhiếp ảnh</v>
+      </c>
+      <c r="D71" t="str">
+        <v>Photography</v>
+      </c>
+      <c r="E71" t="str">
+        <v>The artist mainly does digital photography</v>
+      </c>
+      <c r="F71" t="str">
+        <v>Digital photography</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>74975ac4-5195-4360-a509-f8abcd51c71d</v>
+      </c>
+      <c r="B72">
+        <v>28</v>
+      </c>
+      <c r="C72" t="str">
+        <v>Hướng dẫn cách làm</v>
+      </c>
+      <c r="D72" t="str">
+        <v>Tutorial</v>
+      </c>
+      <c r="E72" t="str">
+        <v>Check out her step-by-step tutorial on makeup</v>
+      </c>
+      <c r="F72" t="str">
+        <v>Step-by-Step tutorial</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>8af0b848-c984-475f-af71-c73c9cf77b8b</v>
+      </c>
+      <c r="B73">
+        <v>28</v>
+      </c>
+      <c r="C73" t="str">
+        <v>Nhật ký bằng video</v>
+      </c>
+      <c r="D73" t="str">
+        <v>Vlogs</v>
+      </c>
+      <c r="E73" t="str">
+        <v/>
+      </c>
+      <c r="F73" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>b631dad9-b82c-47b5-b18e-a505891c7e86</v>
+      </c>
+      <c r="B74">
+        <v>28</v>
+      </c>
+      <c r="C74" t="str">
+        <v>Đội, nhóm</v>
+      </c>
+      <c r="D74" t="str">
+        <v>Team</v>
+      </c>
+      <c r="E74" t="str">
+        <v>The soccer team won 5-1</v>
+      </c>
+      <c r="F74" t="str">
+        <v>A soccer team</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>d7be64cc-0840-44db-9e09-27cf029efff2</v>
+      </c>
+      <c r="B75">
+        <v>28</v>
+      </c>
+      <c r="C75" t="str">
+        <v>Thử</v>
+      </c>
+      <c r="D75" t="str">
+        <v>Try out</v>
+      </c>
+      <c r="E75" t="str">
+        <v>Would you try out a new method of cooking?</v>
+      </c>
+      <c r="F75" t="str">
+        <v>Try out a new method</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>7c51af5a-2c08-40d7-9b59-971579e83fcd</v>
+      </c>
+      <c r="B76">
+        <v>28</v>
+      </c>
+      <c r="C76" t="str">
+        <v>Tham gia</v>
+      </c>
+      <c r="D76" t="str">
+        <v>Participate</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Please participate more in class</v>
+      </c>
+      <c r="F76" t="str">
+        <v>Participate in something</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>f9d5999c-a156-41b9-800c-a7802ca98ea5</v>
+      </c>
+      <c r="B77">
+        <v>28</v>
+      </c>
+      <c r="C77" t="str">
+        <v>Chương trình</v>
+      </c>
+      <c r="D77" t="str">
+        <v>Program</v>
+      </c>
+      <c r="E77" t="str">
+        <v>She works for a news program</v>
+      </c>
+      <c r="F77" t="str">
+        <v>A news program</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>c8a1854a-ae84-41f5-a5d4-a1d0aa910d2c</v>
+      </c>
+      <c r="B78">
+        <v>28</v>
+      </c>
+      <c r="C78" t="str">
+        <v>Hoạt hình</v>
+      </c>
+      <c r="D78" t="str">
+        <v>Cartoon</v>
+      </c>
+      <c r="E78" t="str">
+        <v>Mickey mouse is a walt disney cartoon</v>
+      </c>
+      <c r="F78" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>e3abb703-a37a-4308-96b6-b20859e2a6aa</v>
+      </c>
+      <c r="B79">
+        <v>28</v>
+      </c>
+      <c r="C79" t="str">
+        <v>Thể loại</v>
+      </c>
+      <c r="D79" t="str">
+        <v>Genre</v>
+      </c>
+      <c r="E79" t="str">
+        <v>What music genre do you listen to?</v>
+      </c>
+      <c r="F79" t="str">
+        <v>Music genre</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>dfa9fc23-b0d1-4e81-865b-13d53416db11</v>
+      </c>
+      <c r="B80">
+        <v>28</v>
+      </c>
+      <c r="C80" t="str">
+        <v>Phim hài</v>
+      </c>
+      <c r="D80" t="str">
+        <v>Comedy</v>
+      </c>
+      <c r="E80" t="str">
+        <v>My friend loves watching remoantic comedies</v>
+      </c>
+      <c r="F80" t="str">
+        <v>A romantic comedy</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>e9792faa-117f-408c-8aa4-bb141f602092</v>
+      </c>
+      <c r="B81">
+        <v>28</v>
+      </c>
+      <c r="C81" t="str">
+        <v>Trèo</v>
+      </c>
+      <c r="D81" t="str">
+        <v>Climb</v>
+      </c>
+      <c r="E81" t="str">
+        <v>The cat climbed up the tree</v>
+      </c>
+      <c r="F81" t="str">
+        <v>Climb up something</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>9c9784a3-bc25-46fe-99fb-cb54224c9f86</v>
+      </c>
+      <c r="B82">
+        <v>28</v>
+      </c>
+      <c r="C82" t="str">
+        <v>Sự thích thú, niềm vui</v>
+      </c>
+      <c r="D82" t="str">
+        <v>Pleasure</v>
+      </c>
+      <c r="E82" t="str">
+        <v>The kids find pleasure in singing</v>
+      </c>
+      <c r="F82" t="str">
+        <v>Take or find pleasure in doing something</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>6842266a-c5ab-4119-a535-872c36da4757</v>
+      </c>
+      <c r="B83">
+        <v>28</v>
+      </c>
+      <c r="C83" t="str">
+        <v>Trong nhà</v>
+      </c>
+      <c r="D83" t="str">
+        <v>Indoor</v>
+      </c>
+      <c r="E83" t="str">
+        <v>The hotel's indoor swimming pool is huge!</v>
+      </c>
+      <c r="F83" t="str">
+        <v>An indoor swimming pool</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>d2a15da2-9ea7-48ec-ac1c-31958d2a9169</v>
+      </c>
+      <c r="B84">
+        <v>28</v>
+      </c>
+      <c r="C84" t="str">
+        <v>Chuyến nghỉ dưỡng, kỳ nghỉ</v>
+      </c>
+      <c r="D84" t="str">
+        <v>Holiday</v>
+      </c>
+      <c r="E84" t="str">
+        <v>I do not work on holiday</v>
+      </c>
+      <c r="F84" t="str">
+        <v>On holiday</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>2c2dbe0d-943c-43ab-ba45-c532ffa886ae</v>
+      </c>
+      <c r="B85">
+        <v>28</v>
+      </c>
+      <c r="C85" t="str">
+        <v>Chuyến đi</v>
+      </c>
+      <c r="D85" t="str">
+        <v>Ride</v>
+      </c>
+      <c r="E85" t="str">
+        <v>We are in for a bumpy ride</v>
+      </c>
+      <c r="F85" t="str">
+        <v>A bumpy ride</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>41542f1d-741d-4a47-8a81-a1d09a9a966b</v>
+      </c>
+      <c r="B86">
+        <v>28</v>
+      </c>
+      <c r="C86" t="str">
+        <v>Có ý nghĩa</v>
+      </c>
+      <c r="D86" t="str">
+        <v>Meaningful</v>
+      </c>
+      <c r="E86" t="str">
+        <v>I strive to do meaningful work</v>
+      </c>
+      <c r="F86" t="str">
+        <v>Meaningful work</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>6e66b3ef-3ec5-4743-9860-7418a93dce27</v>
+      </c>
+      <c r="B87">
+        <v>28</v>
+      </c>
+      <c r="C87" t="str">
+        <v>Việc cấm trại</v>
+      </c>
+      <c r="D87" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="E87" t="str">
+        <v>We are going on a camping trip</v>
+      </c>
+      <c r="F87" t="str">
+        <v>A camping trip</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>1188e571-d666-4bf9-81ee-46334eabd388</v>
+      </c>
+      <c r="B88">
+        <v>28</v>
+      </c>
+      <c r="C88" t="str">
+        <v>Hợp tác</v>
+      </c>
+      <c r="D88" t="str">
+        <v>Cooperate</v>
+      </c>
+      <c r="E88" t="str">
+        <v>You have to cooperate with here</v>
+      </c>
+      <c r="F88" t="str">
+        <v>Cooperate with something or somebody</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>c8f79e81-dc8c-4f22-805d-0f1945deadcd</v>
+      </c>
+      <c r="B89">
+        <v>28</v>
+      </c>
+      <c r="C89" t="str">
+        <v>Lều</v>
+      </c>
+      <c r="D89" t="str">
+        <v>Tent</v>
+      </c>
+      <c r="E89" t="str">
+        <v>Please put up the tent for me</v>
+      </c>
+      <c r="F89" t="str">
+        <v>Put up a tent</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>df9891a5-2a7a-4754-91d7-ff7fffc40477</v>
+      </c>
+      <c r="B90">
+        <v>28</v>
+      </c>
+      <c r="C90" t="str">
+        <v>Hứng thú với</v>
+      </c>
+      <c r="D90" t="str">
+        <v>Go in for</v>
+      </c>
+      <c r="E90" t="str">
+        <v>My sister decides to go in for a debate competition</v>
+      </c>
+      <c r="F90" t="str">
+        <v>Go in for a competition</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>f1186873-4969-486d-bd89-9a0695b5388f</v>
+      </c>
+      <c r="B91">
+        <v>28</v>
+      </c>
+      <c r="C91" t="str">
+        <v>Thích hơn</v>
+      </c>
+      <c r="D91" t="str">
+        <v>Prefer</v>
+      </c>
+      <c r="E91" t="str">
+        <v>She prefers eating apples to pears</v>
+      </c>
+      <c r="F91" t="str">
+        <v>Prefer something to something</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>a2b1778e-1bde-4f07-8efc-386e9629f6dc</v>
+      </c>
+      <c r="B92">
+        <v>29</v>
+      </c>
+      <c r="C92" t="str">
+        <v>Câu cá</v>
+      </c>
+      <c r="D92" t="str">
+        <v>Fishing</v>
+      </c>
+      <c r="E92" t="str">
+        <v>My dad and I go fishing every day</v>
+      </c>
+      <c r="F92" t="str">
+        <v>Go fishing</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>cf990805-78a4-450b-9080-8d1407d56334</v>
+      </c>
+      <c r="B93">
+        <v>29</v>
+      </c>
+      <c r="C93" t="str">
+        <v>Vận động viên</v>
+      </c>
+      <c r="D93" t="str">
+        <v>Athlete</v>
+      </c>
+      <c r="E93" t="str">
+        <v>Olumpic athletes train hard to complete</v>
+      </c>
+      <c r="F93" t="str">
+        <v>An Olympic athlete</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>b6a3f27f-b5f1-4f59-a13a-5a3b1d198402</v>
+      </c>
+      <c r="B94">
+        <v>29</v>
+      </c>
+      <c r="C94" t="str">
+        <v>Môn đấu vật</v>
+      </c>
+      <c r="D94" t="str">
+        <v>Wrestling</v>
+      </c>
+      <c r="E94" t="str">
+        <v>Wrestling matches are popular in the US</v>
+      </c>
+      <c r="F94" t="str">
+        <v>A wrestling match</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>f903164f-992c-4ff7-bdd0-9796bb39e5eb</v>
+      </c>
+      <c r="B95">
+        <v>29</v>
+      </c>
+      <c r="C95" t="str">
+        <v>Chuyên nghiệp</v>
+      </c>
+      <c r="D95" t="str">
+        <v>Professional</v>
+      </c>
+      <c r="E95" t="str">
+        <v>He was a professional soccer player</v>
+      </c>
+      <c r="F95" t="str">
+        <v>A professional soccer player</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>f38ea113-6eed-41a7-864c-9fd8eb997c46</v>
+      </c>
+      <c r="B96">
+        <v>29</v>
+      </c>
+      <c r="C96" t="str">
+        <v>Hàng năm</v>
+      </c>
+      <c r="D96" t="str">
+        <v>Annual</v>
+      </c>
+      <c r="E96" t="str">
+        <v>The company has annual meetings for us</v>
+      </c>
+      <c r="F96" t="str">
+        <v>An annual meeting</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>cec821bf-15bc-4c73-85e6-328b2b004fd1</v>
+      </c>
+      <c r="B97">
+        <v>29</v>
+      </c>
+      <c r="C97" t="str">
+        <v>Giải đấu</v>
+      </c>
+      <c r="D97" t="str">
+        <v>Tournament</v>
+      </c>
+      <c r="E97" t="str">
+        <v>What an exciting soccer tournament!</v>
+      </c>
+      <c r="F97" t="str">
+        <v>A soccer tournament</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>ddae4d17-2487-4c91-b15b-62ec664e7e93</v>
+      </c>
+      <c r="B98">
+        <v>29</v>
+      </c>
+      <c r="C98" t="str">
+        <v>Huấn luyện viên</v>
+      </c>
+      <c r="D98" t="str">
+        <v>Coach</v>
+      </c>
+      <c r="E98" t="str">
+        <v>The team coach trains us hard</v>
+      </c>
+      <c r="F98" t="str">
+        <v>The team coach</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>9c573cff-4ddd-4aec-83ca-2f88d870993e</v>
+      </c>
+      <c r="B99">
+        <v>29</v>
+      </c>
+      <c r="C99" t="str">
+        <v>Trận đấu</v>
+      </c>
+      <c r="D99" t="str">
+        <v>Match</v>
+      </c>
+      <c r="E99" t="str">
+        <v>There is a soccer match tonight</v>
+      </c>
+      <c r="F99" t="str">
+        <v>A soccer match</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>dd72f5c5-8548-436c-bd33-79ddb20c7437</v>
+      </c>
+      <c r="B100">
+        <v>29</v>
+      </c>
+      <c r="C100" t="str">
+        <v>Đánh bại</v>
+      </c>
+      <c r="D100" t="str">
+        <v>Beat</v>
+      </c>
+      <c r="E100" t="str">
+        <v>They beat their opponents in the first round</v>
+      </c>
+      <c r="F100" t="str">
+        <v>Beat something or somebody</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>b1892029-56ff-4cbe-984a-c7dab29a9977</v>
+      </c>
+      <c r="B101">
+        <v>29</v>
+      </c>
+      <c r="C101" t="str">
+        <v>Đối thủ</v>
+      </c>
+      <c r="D101" t="str">
+        <v>Opponent</v>
+      </c>
+      <c r="E101" t="str">
+        <v>She is my opponent in chess</v>
+      </c>
+      <c r="F101" t="str">
+        <v>One's oppponent in something</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>1e190ed8-33a8-4e71-b7b2-fa84c7c02941</v>
+      </c>
+      <c r="B102">
+        <v>29</v>
+      </c>
+      <c r="C102" t="str">
+        <v>Môn thể thao</v>
+      </c>
+      <c r="D102" t="str">
+        <v>Athletics</v>
+      </c>
+      <c r="E102" t="str">
+        <v>Football, soccer, and baseball are types of atheletics</v>
+      </c>
+      <c r="F102" t="str">
+        <v>Types of athletics</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>d38353fc-5f4f-472c-ac04-668987f0a4a7</v>
+      </c>
+      <c r="B103">
+        <v>29</v>
+      </c>
+      <c r="C103" t="str">
+        <v>Bóng rỗ</v>
+      </c>
+      <c r="D103" t="str">
+        <v>Basketball</v>
+      </c>
+      <c r="E103" t="str">
+        <v>I am the captain of the basketball team</v>
+      </c>
+      <c r="F103" t="str">
+        <v>A basketball team</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>ef65ce51-588d-4574-aabf-54d79f5fccc8</v>
+      </c>
+      <c r="B104">
+        <v>29</v>
+      </c>
+      <c r="C104" t="str">
+        <v>Người chơi</v>
+      </c>
+      <c r="D104" t="str">
+        <v>Player</v>
+      </c>
+      <c r="E104" t="str">
+        <v>He is the best soccer player here</v>
+      </c>
+      <c r="F104" t="str">
+        <v>A soccer player</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>b7c13a10-8f6b-4bc0-adf4-4efd66aa87fc</v>
+      </c>
+      <c r="B105">
+        <v>29</v>
+      </c>
+      <c r="C105" t="str">
+        <v xml:space="preserve">Liên đoàn </v>
+      </c>
+      <c r="D105" t="str">
+        <v>League</v>
+      </c>
+      <c r="E105" t="str">
+        <v>My sone plays for a soccer league</v>
+      </c>
+      <c r="F105" t="str">
+        <v>A soccer league</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>cbf03296-0921-4040-90d4-199fd9d5c23b</v>
+      </c>
+      <c r="B106">
+        <v>29</v>
+      </c>
+      <c r="C106" t="str">
+        <v>Giải vô địch</v>
+      </c>
+      <c r="D106" t="str">
+        <v>Championship</v>
+      </c>
+      <c r="E106" t="str">
+        <v>Are you ready for the basketball championship</v>
+      </c>
+      <c r="F106" t="str">
+        <v>A basketball championship</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>5029497b-8c66-41b8-8d0a-4bfe381c4286</v>
+      </c>
+      <c r="B107">
+        <v>29</v>
+      </c>
+      <c r="C107" t="str">
+        <v>Đội trưởng</v>
+      </c>
+      <c r="D107" t="str">
+        <v>Captain</v>
+      </c>
+      <c r="E107" t="str">
+        <v>We vote for a team camtain</v>
+      </c>
+      <c r="F107" t="str">
+        <v>Team captain</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>c2fb9123-f320-4cc1-a7fa-d38da99a5fc1</v>
+      </c>
+      <c r="B108">
+        <v>29</v>
+      </c>
+      <c r="C108" t="str">
+        <v>Ghi điểm</v>
+      </c>
+      <c r="D108" t="str">
+        <v>Score</v>
+      </c>
+      <c r="E108" t="str">
+        <v>He scored a goal for the team</v>
+      </c>
+      <c r="F108" t="str">
+        <v>Score a goal</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>a52a7a35-9823-4ea9-87c9-6dec37ecf622</v>
+      </c>
+      <c r="B109">
+        <v>29</v>
+      </c>
+      <c r="C109" t="str">
+        <v>Danh hiệu</v>
+      </c>
+      <c r="D109" t="str">
+        <v>Title</v>
+      </c>
+      <c r="E109" t="str">
+        <v>The team won the title with a goal in the last minute</v>
+      </c>
+      <c r="F109" t="str">
+        <v>Win the title</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>916d379b-cba3-40d9-a67f-a71d48b74a2f</v>
+      </c>
+      <c r="B110">
+        <v>29</v>
+      </c>
+      <c r="C110" t="str">
+        <v>Lưới</v>
+      </c>
+      <c r="D110" t="str">
+        <v>Net</v>
+      </c>
+      <c r="E110" t="str">
+        <v>The fishing net has holes in it</v>
+      </c>
+      <c r="F110" t="str">
+        <v>A fishing net</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>463b16e3-432e-446b-bea0-a0f2b3da5f06</v>
+      </c>
+      <c r="B111">
+        <v>29</v>
+      </c>
+      <c r="C111" t="str">
+        <v>Anh hùng</v>
+      </c>
+      <c r="D111" t="str">
+        <v>Hero</v>
+      </c>
+      <c r="E111" t="str">
+        <v>The fireman became a local hero</v>
+      </c>
+      <c r="F111" t="str">
+        <v>A local hero</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>39de71b0-d5b5-48c9-8f4d-95b2e2f50af6</v>
+      </c>
+      <c r="B112">
+        <v>29</v>
+      </c>
+      <c r="C112" t="str">
+        <v>Môn đạp xe</v>
+      </c>
+      <c r="D112" t="str">
+        <v>Cycling</v>
+      </c>
+      <c r="E112" t="str">
+        <v>She went cycling down the hill</v>
+      </c>
+      <c r="F112" t="str">
+        <v>Go cycling</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>aae25fe9-c463-44f6-8403-64b3ab4901df</v>
+      </c>
+      <c r="B113">
+        <v>29</v>
+      </c>
+      <c r="C113" t="str">
+        <v>Sân vận động</v>
+      </c>
+      <c r="D113" t="str">
+        <v>Stadium</v>
+      </c>
+      <c r="E113" t="str">
+        <v>Where is the biggest sports stadium in hanoi</v>
+      </c>
+      <c r="F113" t="str">
+        <v>A sport stadium</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>a8bd58e5-0590-4ebb-9b28-1b10efe4f691</v>
+      </c>
+      <c r="B114">
+        <v>29</v>
+      </c>
+      <c r="C114" t="str">
+        <v>Người thắng cuộc</v>
+      </c>
+      <c r="D114" t="str">
+        <v>Winner</v>
+      </c>
+      <c r="E114" t="str">
+        <v>The actor is an award winner</v>
+      </c>
+      <c r="F114" t="str">
+        <v>An award winer</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>b553acc6-a0c9-417a-b2d9-d77e5fd33909</v>
+      </c>
+      <c r="B115">
+        <v>29</v>
+      </c>
+      <c r="C115" t="str">
+        <v>Môn đánh golf</v>
+      </c>
+      <c r="D115" t="str">
+        <v>Golf</v>
+      </c>
+      <c r="E115" t="str">
+        <v>Businessmen love to play golf</v>
+      </c>
+      <c r="F115" t="str">
+        <v>Play golf</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>c9b2d631-4c95-4cbf-b5c6-51760a9800c8</v>
+      </c>
+      <c r="B116">
+        <v>29</v>
+      </c>
+      <c r="C116" t="str">
+        <v>Đánh</v>
+      </c>
+      <c r="D116" t="str">
+        <v>Strike</v>
+      </c>
+      <c r="E116" t="str">
+        <v>He strikes the golf ball perfectly</v>
+      </c>
+      <c r="F116" t="str">
+        <v>Strike the ball</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>6c846374-0b04-4261-a1fc-abb952bde9d0</v>
+      </c>
+      <c r="B117">
+        <v>29</v>
+      </c>
+      <c r="C117" t="str">
+        <v>Đích, mục tiêu</v>
+      </c>
+      <c r="D117" t="str">
+        <v>Target</v>
+      </c>
+      <c r="E117" t="str">
+        <v>He shot the arrow and hit the target</v>
+      </c>
+      <c r="F117" t="str">
+        <v>Hit the target</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>7c39a7bf-0223-4d67-bf19-bc70d6260a4c</v>
+      </c>
+      <c r="B118">
+        <v>29</v>
+      </c>
+      <c r="C118" t="str">
+        <v>Tối đa</v>
+      </c>
+      <c r="D118" t="str">
+        <v>Maximum</v>
+      </c>
+      <c r="E118" t="str">
+        <v>The maximum amount for storage is 256GB</v>
+      </c>
+      <c r="F118" t="str">
+        <v>The maximum amount</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>727a487b-ea11-4357-8b3a-cfd78069fedb</v>
+      </c>
+      <c r="B119">
+        <v>29</v>
+      </c>
+      <c r="C119" t="str">
+        <v>Lướt</v>
+      </c>
+      <c r="D119" t="str">
+        <v>Surf</v>
+      </c>
+      <c r="E119" t="str">
+        <v>In hawaii, you must surf the waves</v>
+      </c>
+      <c r="F119" t="str">
+        <v>Surf the wave</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>86cb971a-bdd1-45d0-9169-17ef0fb2990e</v>
+      </c>
+      <c r="B120">
+        <v>29</v>
+      </c>
+      <c r="C120" t="str">
+        <v>Không may</v>
+      </c>
+      <c r="D120" t="str">
+        <v>Unfortunately</v>
+      </c>
+      <c r="E120" t="str">
+        <v>Unfortunately, I won't be able to attend the meeting</v>
+      </c>
+      <c r="F120" t="str">
+        <v>Unfortunately, I won't</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>2805d4a5-2450-4193-92b7-19d2357bd4d9</v>
+      </c>
+      <c r="B121">
+        <v>29</v>
+      </c>
+      <c r="C121" t="str">
+        <v>Trân trọng, đánh giá cao</v>
+      </c>
+      <c r="D121" t="str">
+        <v>Appreciate</v>
+      </c>
+      <c r="E121" t="str">
+        <v>I appreciate the help you gave me</v>
+      </c>
+      <c r="F121" t="str">
+        <v>Appreciate somebody or something</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F121"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add login with google account and add feature filter with unit
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -7,6 +7,7 @@
     <sheet name="Update_ea9e" sheetId="2" r:id="rId2"/>
     <sheet name="Update_3987" sheetId="3" r:id="rId3"/>
     <sheet name="Update_da6e" sheetId="4" r:id="rId4"/>
+    <sheet name="Update_b82e" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -9648,4 +9649,2438 @@
     <ignoredError numberStoredAsText="1" sqref="A1:F121"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F121"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>unitId</v>
+      </c>
+      <c r="C1" t="str">
+        <v>word</v>
+      </c>
+      <c r="D1" t="str">
+        <v>answers</v>
+      </c>
+      <c r="E1" t="str">
+        <v>sentences</v>
+      </c>
+      <c r="F1" t="str">
+        <v>phrases</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2855e402-1dfa-4dc2-8840-cebd848fa19c</v>
+      </c>
+      <c r="B2">
+        <v>26</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Chương trình</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Show</v>
+      </c>
+      <c r="E2" t="str">
+        <v>I watch TV shows on my television</v>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>d90b062b-c464-4c5c-bf4d-2d250fee42b4</v>
+      </c>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Cảnh</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Scene</v>
+      </c>
+      <c r="E3" t="str">
+        <v>The crew needs to film a scene</v>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>d670b0d5-a0f9-4e3d-be7e-7539b709f4bf</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Nam diễn viên</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Actor</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Who is the lead actor in titanic</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>0b08724a-3034-4e5c-9eed-a809189bff3a</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Thuộc âm nhạc</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Musical</v>
+      </c>
+      <c r="E5" t="str">
+        <v xml:space="preserve">The audience loved the musical performance </v>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>4152b846-3f6e-4b76-b48c-320c8d9bf98d</v>
+      </c>
+      <c r="B6">
+        <v>26</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Nhạc phim</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Soundtrack</v>
+      </c>
+      <c r="E6" t="str">
+        <v>The soundtrack of this movie is great</v>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>f9c612cb-22a0-4f9d-a949-c179e45f0655</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Thuộc lịch sử</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Historical</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Albert Einstein is an important historical figure</v>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>53af5326-467e-4e15-a189-ec4723760626</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Bí ẩn</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Mystery</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Nobody can solve the mystery of the Bermuda triangle</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>faab9a2e-d127-4a38-abf1-879e33beef60</v>
+      </c>
+      <c r="B9">
+        <v>26</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Tội ác</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Crime</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Stealing money is a serious crime</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>da3b1816-173a-4493-ad15-7beb97e72ba5</v>
+      </c>
+      <c r="B10">
+        <v>26</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Đoạn kết</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Ending</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Fairy tales have happy endings</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>e98b5079-2952-47db-afac-31e8e8b2ded1</v>
+      </c>
+      <c r="B11">
+        <v>26</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Tiết lộ</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Reveal</v>
+      </c>
+      <c r="E11" t="str">
+        <v>The magician never reveals the truth</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>6834a067-2935-4767-b07e-7e28c2af50bc</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Phim giật gân</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Thriller</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Thriller movies are scary</v>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>eec73fe0-6f13-4d23-b16e-304b453fd1eb</v>
+      </c>
+      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Xưởng, không gian sáng tạo</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Studio</v>
+      </c>
+      <c r="E13" t="str">
+        <v>She teaches us at her dance studio</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>d82e9755-cb4a-4e76-b2d1-c22e9bbd3e4a</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Bối cảnh, khung cảnh</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Setting</v>
+      </c>
+      <c r="E14" t="str">
+        <v xml:space="preserve">What a beautiful setting this city is </v>
+      </c>
+      <c r="F14" t="str">
+        <v>A beautiful setting</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>80af4f65-e319-4276-abc7-c4b93cfb684f</v>
+      </c>
+      <c r="B15">
+        <v>26</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Điều viễn tưởng</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Fiction</v>
+      </c>
+      <c r="E15" t="str">
+        <v>She wrote fiction on aliens and love</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>66eb9a3b-e5cf-4572-af26-c0ced46a6a41</v>
+      </c>
+      <c r="B16">
+        <v>26</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Sự việc kịch tính</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Drama</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Teens like to watch drama series</v>
+      </c>
+      <c r="F16" t="str">
+        <v>A drama series</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>6d66f4e3-1575-453b-9c56-b2e35ae6f572</v>
+      </c>
+      <c r="B17">
+        <v>26</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Đạo diễn</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Director</v>
+      </c>
+      <c r="E17" t="str">
+        <v>The young film director deserves our recognition</v>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>c61cf54e-76e9-4c4f-a546-be16ad5e5bcf</v>
+      </c>
+      <c r="B18">
+        <v>26</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Ra mắt</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Come out</v>
+      </c>
+      <c r="E18" t="str">
+        <v>When is her album coming out?</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Something new comes out</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>75d97f77-6607-497c-a34c-c08e4276bc76</v>
+      </c>
+      <c r="B19">
+        <v>26</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Nhân vật</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Character</v>
+      </c>
+      <c r="E19" t="str">
+        <v>The main character in "Batman" is mysterious</v>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>e2745e17-f355-4999-984f-246339ace9e7</v>
+      </c>
+      <c r="B20">
+        <v>26</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Nữ diễn viên</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Actress</v>
+      </c>
+      <c r="E20" t="str">
+        <v>She was a good actress back then</v>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>d883b560-e598-4399-b67a-fbd255f88070</v>
+      </c>
+      <c r="B21">
+        <v>26</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Kỳ lạ, kỳ quặc</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Odd</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Hanging out with odd people is fun</v>
+      </c>
+      <c r="F21" t="str">
+        <v>An odd person</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>861042fb-7382-4b86-b5dc-6f8a0f267c2b</v>
+      </c>
+      <c r="B22">
+        <v>26</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Màn hình</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Screen</v>
+      </c>
+      <c r="E22" t="str">
+        <v>The laptop has a big computer screen</v>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>2c327c19-447e-45c6-8278-14aa65293f96</v>
+      </c>
+      <c r="B23">
+        <v>26</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Hành động</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Action</v>
+      </c>
+      <c r="E23" t="str">
+        <v>My favorite action movie is Fast and Furious</v>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>1c7e5e1d-737d-4a0f-9124-6e6415aaab50</v>
+      </c>
+      <c r="B24">
+        <v>26</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Chuyến phiêu lưu</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Adventure</v>
+      </c>
+      <c r="E24" t="str">
+        <v>I seek an adventure of a lifetime</v>
+      </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>046efda8-e3b4-4698-a754-cacebf1c90e0</v>
+      </c>
+      <c r="B25">
+        <v>26</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Phim tài liệu</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Documentary</v>
+      </c>
+      <c r="E25" t="str">
+        <v>I watched that documentary film on Netflix</v>
+      </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>7040324e-e5a2-44f4-9535-b2cc9cbdb924</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Góc</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Angle</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Tilt your head to a 45 angle</v>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>988a2983-945c-4cf0-ba48-152e92f249c4</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Thấy khó hiểu</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Confused</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Are you confused about the instructions?</v>
+      </c>
+      <c r="F27" t="str">
+        <v>Confused about something</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>928cac87-df35-4693-90eb-0b7ac9ba4f7c</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Cuộc hội thoại, lời thoại</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Dialogue</v>
+      </c>
+      <c r="E28" t="str">
+        <v>The dialogue with my therapist helped me</v>
+      </c>
+      <c r="F28" t="str">
+        <v>Dialogue with somebody</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>470241db-5ef4-4605-923a-0f067329f20f</v>
+      </c>
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Tác phẩm thành công</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Hit</v>
+      </c>
+      <c r="E29" t="str">
+        <v>His book became a big hit</v>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>972036e4-0ba9-4393-b01e-adb398bcbf0c</v>
+      </c>
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Tuyệt vời</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Wonderful</v>
+      </c>
+      <c r="E30" t="str">
+        <v>I am grateful for the wonderful opportunity</v>
+      </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>fefbe098-b8f8-40ef-87d2-ea757ae401e2</v>
+      </c>
+      <c r="B31">
+        <v>26</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Tài giỏi, tuyệt vời</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Brilliant</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Thank you for the brilliant idea</v>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>7ced7a2e-75de-4804-ac90-20e3e958d965</v>
+      </c>
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Khiêm tốn</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Modest</v>
+      </c>
+      <c r="E32" t="str">
+        <v>You are too modest! You are gifted.</v>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>4b5d71f1-69c8-4d40-917c-56ed60fa341a</v>
+      </c>
+      <c r="B33">
+        <v>27</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Có năng khiếu</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Gifted</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Do you consider yourself a gifted musican?</v>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>f249b615-9ce7-490b-aeb1-e7fb50956f75</v>
+      </c>
+      <c r="B34">
+        <v>27</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Ngành giải trí</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Showbiz</v>
+      </c>
+      <c r="E34" t="str">
+        <v>People in showbiz are movie stars</v>
+      </c>
+      <c r="F34" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>33645007-d97b-4e05-9fbb-18ce6453df08</v>
+      </c>
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Kênh</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Channel</v>
+      </c>
+      <c r="E35" t="str">
+        <v>The show is live on the VTV3 channel</v>
+      </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>c1f5fd98-6823-4cd2-8332-437b40d1cdbb</v>
+      </c>
+      <c r="B36">
+        <v>27</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Truyền thông</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Media</v>
+      </c>
+      <c r="E36" t="str">
+        <v>My mom posts so many pictures on social media</v>
+      </c>
+      <c r="F36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>9e32b63e-6f9b-484a-a3cf-03b2554b0c81</v>
+      </c>
+      <c r="B37">
+        <v>27</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Nổi tiếng</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Well-known</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Is he a well-known actor?</v>
+      </c>
+      <c r="F37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>3af0b7f7-7574-4b56-bf9b-afbdc9d94496</v>
+      </c>
+      <c r="B38">
+        <v>27</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Nhận ra</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Recognize</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Did you recognize me on stage?</v>
+      </c>
+      <c r="F38" t="str">
+        <v>Recognize somebody or something</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>cd2a5828-bdf8-445c-81a1-3926ae9be2da</v>
+      </c>
+      <c r="B39">
+        <v>27</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Người hâm mộ</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Fan</v>
+      </c>
+      <c r="E39" t="str">
+        <v>My girlfriend is a big soccer fan</v>
+      </c>
+      <c r="F39" t="str">
+        <v>A soccer fan</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>123fb41c-f345-498c-a994-9a9b27e98bf8</v>
+      </c>
+      <c r="B40">
+        <v>27</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Đăng ký</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Subscribe</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Please subscribe to step up english youtube channel</v>
+      </c>
+      <c r="F40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>87d2b191-c73b-403f-96bc-6f392d27e7b2</v>
+      </c>
+      <c r="B41">
+        <v>27</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Hét to</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Sceam</v>
+      </c>
+      <c r="E41" t="str">
+        <v>They screamed out loud for help</v>
+      </c>
+      <c r="F41" t="str">
+        <v>Scream out loud</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>5a4867f1-271f-4ee0-865d-7d7eb2b42d5d</v>
+      </c>
+      <c r="B42">
+        <v>27</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Buồn cười</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Funny</v>
+      </c>
+      <c r="E42" t="str">
+        <v>The funny story made me laugh hard</v>
+      </c>
+      <c r="F42" t="str">
+        <v>A funny story</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>3423a5df-5518-4d10-9006-6b46aef0c92f</v>
+      </c>
+      <c r="B43">
+        <v>27</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Hiện nay</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Currently</v>
+      </c>
+      <c r="E43" t="str">
+        <v>I am currently working as a front-end developer</v>
+      </c>
+      <c r="F43" t="str">
+        <v>Currently working as something</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>dac664bf-4d84-4185-9955-6184e4705180</v>
+      </c>
+      <c r="B44">
+        <v>27</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Lan truyền nhanh</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Viral</v>
+      </c>
+      <c r="E44" t="str">
+        <v>The video went viral on Facebook</v>
+      </c>
+      <c r="F44" t="str">
+        <v>Go viral</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>8d87d414-5e8f-41e4-8024-820fa8e2834f</v>
+      </c>
+      <c r="B45">
+        <v>27</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Màn biểu diễn</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Performance</v>
+      </c>
+      <c r="E45" t="str">
+        <v>The opera singer delivered an outstanding performance</v>
+      </c>
+      <c r="F45" t="str">
+        <v>Deliver an outstanding performance</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>999e1a08-f844-4088-a0eb-d43b316c22f6</v>
+      </c>
+      <c r="B46">
+        <v>27</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Quá khứ</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Past</v>
+      </c>
+      <c r="E46" t="str">
+        <v>I used to live abroad in the past</v>
+      </c>
+      <c r="F46" t="str">
+        <v>In the past</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>f3268128-5bfc-4b77-b848-87fd19d76a2d</v>
+      </c>
+      <c r="B47">
+        <v>27</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Trở nên</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Become</v>
+      </c>
+      <c r="E47" t="str">
+        <v>I want to become a person of influence</v>
+      </c>
+      <c r="F47" t="str">
+        <v>Become somebody or something</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>abf03747-d6bf-4469-9f81-fdf87f96dce3</v>
+      </c>
+      <c r="B48">
+        <v>27</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Toàn cầu</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Global</v>
+      </c>
+      <c r="E48" t="str">
+        <v>The singer's talent made her go global</v>
+      </c>
+      <c r="F48" t="str">
+        <v>Go global</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>cba5a361-0281-4457-a39e-8fff93b461df</v>
+      </c>
+      <c r="B49">
+        <v>27</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Lên tiếng</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Speak out</v>
+      </c>
+      <c r="E49" t="str">
+        <v>She bravely spoke out against her boss</v>
+      </c>
+      <c r="F49" t="str">
+        <v>Speak out against somebody or something</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>ba407704-b048-4ddc-b6ff-92559d5fe029</v>
+      </c>
+      <c r="B50">
+        <v>27</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Xứng đáng</v>
+      </c>
+      <c r="D50" t="str">
+        <v>Deserve</v>
+      </c>
+      <c r="E50" t="str">
+        <v>I deserve ice cream after work</v>
+      </c>
+      <c r="F50" t="str">
+        <v>Deserve something</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>a23819c9-7af3-4246-a061-633cfade115b</v>
+      </c>
+      <c r="B51">
+        <v>27</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Trực tiếp</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Live</v>
+      </c>
+      <c r="E51" t="str">
+        <v>The band did a live performance</v>
+      </c>
+      <c r="F51" t="str">
+        <v>A live performance</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>bacb314f-3d07-4d2c-ad43-ee564b779903</v>
+      </c>
+      <c r="B52">
+        <v>27</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Giải thưởng</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Award</v>
+      </c>
+      <c r="E52" t="str">
+        <v>She received an award for her acting</v>
+      </c>
+      <c r="F52" t="str">
+        <v>Receive an award</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>a499a65c-f6a4-43bf-b3af-7414b2c94310</v>
+      </c>
+      <c r="B53">
+        <v>27</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Danh dự</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Honor</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Welcome, you are my guest of honor</v>
+      </c>
+      <c r="F53" t="str">
+        <v>The guest of honor</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>48d3d3eb-d568-4c77-8488-43c41b7afbf5</v>
+      </c>
+      <c r="B54">
+        <v>27</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Việc thiện nguyện</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Charity</v>
+      </c>
+      <c r="E54" t="str">
+        <v>We should do charity for the disadvantaged</v>
+      </c>
+      <c r="F54" t="str">
+        <v>Do charity for somebody</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>0aa13e64-c9da-42cf-98a6-ea7b261bfbc8</v>
+      </c>
+      <c r="B55">
+        <v>27</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Tình nguyện</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Volunteer</v>
+      </c>
+      <c r="E55" t="str">
+        <v>She volunteered to clean the car</v>
+      </c>
+      <c r="F55" t="str">
+        <v>Volunteer to do something</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>200b047e-f499-4d66-99d8-fbca132dfb75</v>
+      </c>
+      <c r="B56">
+        <v>27</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Vụ bê bối</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Scandal</v>
+      </c>
+      <c r="E56" t="str">
+        <v>He created the scandal to attract attention</v>
+      </c>
+      <c r="F56" t="str">
+        <v>Create a scandal</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>3b253e28-0230-47de-a666-91be77248828</v>
+      </c>
+      <c r="B57">
+        <v>27</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Tin đồn</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Rumor</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Rumor has it that you got the job!</v>
+      </c>
+      <c r="F57" t="str">
+        <v>Rumor has it that</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>4334038f-c1b7-49a5-98f1-62b1237f3ab0</v>
+      </c>
+      <c r="B58">
+        <v>27</v>
+      </c>
+      <c r="C58" t="str">
+        <v>Tiểu sử</v>
+      </c>
+      <c r="D58" t="str">
+        <v>Biography</v>
+      </c>
+      <c r="E58" t="str">
+        <v>They wrote a biography of her life</v>
+      </c>
+      <c r="F58" t="str">
+        <v>A biography of something</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>5d8f29ff-7d1d-4e1e-82e1-34512516151c</v>
+      </c>
+      <c r="B59">
+        <v>27</v>
+      </c>
+      <c r="C59" t="str">
+        <v>Ngưỡng mộ</v>
+      </c>
+      <c r="D59" t="str">
+        <v>Admire</v>
+      </c>
+      <c r="E59" t="str">
+        <v>I admire my student's passion</v>
+      </c>
+      <c r="F59" t="str">
+        <v>Admire somebody or something</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>85f0b61e-0ab3-4e0f-a3ef-060ce867161f</v>
+      </c>
+      <c r="B60">
+        <v>27</v>
+      </c>
+      <c r="C60" t="str">
+        <v>Ngưỡng mộ</v>
+      </c>
+      <c r="D60" t="str">
+        <v>Look up to</v>
+      </c>
+      <c r="E60" t="str">
+        <v>I look up to my father very much</v>
+      </c>
+      <c r="F60" t="str">
+        <v>Look up to somebody</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>575c63cd-6cd4-43a1-b29d-d6b8960530e0</v>
+      </c>
+      <c r="B61">
+        <v>27</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Đáp ứng tiêu chuẩn</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Live up to</v>
+      </c>
+      <c r="E61" t="str">
+        <v>He lived up to my parent's expectations</v>
+      </c>
+      <c r="F61" t="str">
+        <v>Live up to my parent's expectations</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>fb90b861-646a-4dd4-b647-a4cc017bc8aa</v>
+      </c>
+      <c r="B62">
+        <v>28</v>
+      </c>
+      <c r="C62" t="str">
+        <v>Buổi hòa nhạc</v>
+      </c>
+      <c r="D62" t="str">
+        <v>Concert</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Let's go to a concert tonight!</v>
+      </c>
+      <c r="F62" t="str">
+        <v>Go to a concert</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>cbb60ea8-e319-4ef2-a23f-3d0a72e8a76d</v>
+      </c>
+      <c r="B63">
+        <v>28</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Trò xếp hình, trò giải đố</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Puzzle</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Crassword puzzles are for everyone to play</v>
+      </c>
+      <c r="F63" t="str">
+        <v>A crossword puzzle</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>6567b1a7-ce1d-4054-873f-8febe4c8c136</v>
+      </c>
+      <c r="B64">
+        <v>28</v>
+      </c>
+      <c r="C64" t="str">
+        <v>Đoán</v>
+      </c>
+      <c r="D64" t="str">
+        <v>Guess</v>
+      </c>
+      <c r="E64" t="str">
+        <v>Can you guess my age</v>
+      </c>
+      <c r="F64" t="str">
+        <v>Guess something</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>f0d6988c-f4a0-484b-b07f-71769fed5a9d</v>
+      </c>
+      <c r="B65">
+        <v>28</v>
+      </c>
+      <c r="C65" t="str">
+        <v>Tin Tường</v>
+      </c>
+      <c r="D65" t="str">
+        <v>Keen</v>
+      </c>
+      <c r="E65" t="str">
+        <v>She has a keen eye for fashion</v>
+      </c>
+      <c r="F65" t="str">
+        <v>A keen eye for something</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>8b0ee883-6437-4353-b875-c394855058aa</v>
+      </c>
+      <c r="B66">
+        <v>28</v>
+      </c>
+      <c r="C66" t="str">
+        <v>Đan</v>
+      </c>
+      <c r="D66" t="str">
+        <v>Knit</v>
+      </c>
+      <c r="E66" t="str">
+        <v>Grandma loves to knit scarves</v>
+      </c>
+      <c r="F66" t="str">
+        <v>Knit something</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>f4140d64-523c-47a1-a31d-a55a487858ad</v>
+      </c>
+      <c r="B67">
+        <v>28</v>
+      </c>
+      <c r="C67" t="str">
+        <v>Tiểu thuyết</v>
+      </c>
+      <c r="D67" t="str">
+        <v>Novel</v>
+      </c>
+      <c r="E67" t="str">
+        <v>The author wrote two best-selling novels</v>
+      </c>
+      <c r="F67" t="str">
+        <v>A best-selling novel</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>e1e7a71f-4e39-419e-a77b-86d1a1e534e9</v>
+      </c>
+      <c r="B68">
+        <v>28</v>
+      </c>
+      <c r="C68" t="str">
+        <v>Bộ sưu tập</v>
+      </c>
+      <c r="D68" t="str">
+        <v>Collection</v>
+      </c>
+      <c r="E68" t="str">
+        <v>He has a collection of vinyl records</v>
+      </c>
+      <c r="F68" t="str">
+        <v>Collection of something</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>7ec6e054-a925-4b6d-868e-7edae103be2d</v>
+      </c>
+      <c r="B69">
+        <v>28</v>
+      </c>
+      <c r="C69" t="str">
+        <v>Chèo thuyền</v>
+      </c>
+      <c r="D69" t="str">
+        <v>Sail</v>
+      </c>
+      <c r="E69" t="str">
+        <v>Can we sail a boat tomorrow?</v>
+      </c>
+      <c r="F69" t="str">
+        <v>Sail a boat</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>baac48ef-2267-4932-b04b-f8b85153bcf8</v>
+      </c>
+      <c r="B70">
+        <v>28</v>
+      </c>
+      <c r="C70" t="str">
+        <v>Có hứng thú</v>
+      </c>
+      <c r="D70" t="str">
+        <v>Interested</v>
+      </c>
+      <c r="E70" t="str">
+        <v>Are you interested in the arts?</v>
+      </c>
+      <c r="F70" t="str">
+        <v>Interested in something or somebody</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>b3a79e76-a9ed-453a-affb-d11df6cb336e</v>
+      </c>
+      <c r="B71">
+        <v>28</v>
+      </c>
+      <c r="C71" t="str">
+        <v>Nhiếp ảnh</v>
+      </c>
+      <c r="D71" t="str">
+        <v>Photography</v>
+      </c>
+      <c r="E71" t="str">
+        <v>The artist mainly does digital photography</v>
+      </c>
+      <c r="F71" t="str">
+        <v>Digital photography</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>74975ac4-5195-4360-a509-f8abcd51c71d</v>
+      </c>
+      <c r="B72">
+        <v>28</v>
+      </c>
+      <c r="C72" t="str">
+        <v>Hướng dẫn cách làm</v>
+      </c>
+      <c r="D72" t="str">
+        <v>Tutorial</v>
+      </c>
+      <c r="E72" t="str">
+        <v>Check out her step-by-step tutorial on makeup</v>
+      </c>
+      <c r="F72" t="str">
+        <v>Step-by-Step tutorial</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>8af0b848-c984-475f-af71-c73c9cf77b8b</v>
+      </c>
+      <c r="B73">
+        <v>28</v>
+      </c>
+      <c r="C73" t="str">
+        <v>Nhật ký bằng video</v>
+      </c>
+      <c r="D73" t="str">
+        <v>Vlogs</v>
+      </c>
+      <c r="E73" t="str">
+        <v/>
+      </c>
+      <c r="F73" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>b631dad9-b82c-47b5-b18e-a505891c7e86</v>
+      </c>
+      <c r="B74">
+        <v>28</v>
+      </c>
+      <c r="C74" t="str">
+        <v>Đội, nhóm</v>
+      </c>
+      <c r="D74" t="str">
+        <v>Team</v>
+      </c>
+      <c r="E74" t="str">
+        <v>The soccer team won 5-1</v>
+      </c>
+      <c r="F74" t="str">
+        <v>A soccer team</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>d7be64cc-0840-44db-9e09-27cf029efff2</v>
+      </c>
+      <c r="B75">
+        <v>28</v>
+      </c>
+      <c r="C75" t="str">
+        <v>Thử</v>
+      </c>
+      <c r="D75" t="str">
+        <v>Try out</v>
+      </c>
+      <c r="E75" t="str">
+        <v>Would you try out a new method of cooking?</v>
+      </c>
+      <c r="F75" t="str">
+        <v>Try out a new method</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>7c51af5a-2c08-40d7-9b59-971579e83fcd</v>
+      </c>
+      <c r="B76">
+        <v>28</v>
+      </c>
+      <c r="C76" t="str">
+        <v>Tham gia</v>
+      </c>
+      <c r="D76" t="str">
+        <v>Participate</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Please participate more in class</v>
+      </c>
+      <c r="F76" t="str">
+        <v>Participate in something</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>f9d5999c-a156-41b9-800c-a7802ca98ea5</v>
+      </c>
+      <c r="B77">
+        <v>28</v>
+      </c>
+      <c r="C77" t="str">
+        <v>Chương trình</v>
+      </c>
+      <c r="D77" t="str">
+        <v>Program</v>
+      </c>
+      <c r="E77" t="str">
+        <v>She works for a news program</v>
+      </c>
+      <c r="F77" t="str">
+        <v>A news program</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>c8a1854a-ae84-41f5-a5d4-a1d0aa910d2c</v>
+      </c>
+      <c r="B78">
+        <v>28</v>
+      </c>
+      <c r="C78" t="str">
+        <v>Hoạt hình</v>
+      </c>
+      <c r="D78" t="str">
+        <v>Cartoon</v>
+      </c>
+      <c r="E78" t="str">
+        <v>Mickey mouse is a walt disney cartoon</v>
+      </c>
+      <c r="F78" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>e3abb703-a37a-4308-96b6-b20859e2a6aa</v>
+      </c>
+      <c r="B79">
+        <v>28</v>
+      </c>
+      <c r="C79" t="str">
+        <v>Thể loại</v>
+      </c>
+      <c r="D79" t="str">
+        <v>Genre</v>
+      </c>
+      <c r="E79" t="str">
+        <v>What music genre do you listen to?</v>
+      </c>
+      <c r="F79" t="str">
+        <v>Music genre</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>dfa9fc23-b0d1-4e81-865b-13d53416db11</v>
+      </c>
+      <c r="B80">
+        <v>28</v>
+      </c>
+      <c r="C80" t="str">
+        <v>Phim hài</v>
+      </c>
+      <c r="D80" t="str">
+        <v>Comedy</v>
+      </c>
+      <c r="E80" t="str">
+        <v>My friend loves watching remoantic comedies</v>
+      </c>
+      <c r="F80" t="str">
+        <v>A romantic comedy</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>e9792faa-117f-408c-8aa4-bb141f602092</v>
+      </c>
+      <c r="B81">
+        <v>28</v>
+      </c>
+      <c r="C81" t="str">
+        <v>Trèo</v>
+      </c>
+      <c r="D81" t="str">
+        <v>Climb</v>
+      </c>
+      <c r="E81" t="str">
+        <v>The cat climbed up the tree</v>
+      </c>
+      <c r="F81" t="str">
+        <v>Climb up something</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>9c9784a3-bc25-46fe-99fb-cb54224c9f86</v>
+      </c>
+      <c r="B82">
+        <v>28</v>
+      </c>
+      <c r="C82" t="str">
+        <v>Sự thích thú, niềm vui</v>
+      </c>
+      <c r="D82" t="str">
+        <v>Pleasure</v>
+      </c>
+      <c r="E82" t="str">
+        <v>The kids find pleasure in singing</v>
+      </c>
+      <c r="F82" t="str">
+        <v>Take or find pleasure in doing something</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>6842266a-c5ab-4119-a535-872c36da4757</v>
+      </c>
+      <c r="B83">
+        <v>28</v>
+      </c>
+      <c r="C83" t="str">
+        <v>Trong nhà</v>
+      </c>
+      <c r="D83" t="str">
+        <v>Indoor</v>
+      </c>
+      <c r="E83" t="str">
+        <v>The hotel's indoor swimming pool is huge!</v>
+      </c>
+      <c r="F83" t="str">
+        <v>An indoor swimming pool</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>d2a15da2-9ea7-48ec-ac1c-31958d2a9169</v>
+      </c>
+      <c r="B84">
+        <v>28</v>
+      </c>
+      <c r="C84" t="str">
+        <v>Chuyến nghỉ dưỡng, kỳ nghỉ</v>
+      </c>
+      <c r="D84" t="str">
+        <v>Holiday</v>
+      </c>
+      <c r="E84" t="str">
+        <v>I do not work on holiday</v>
+      </c>
+      <c r="F84" t="str">
+        <v>On holiday</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>2c2dbe0d-943c-43ab-ba45-c532ffa886ae</v>
+      </c>
+      <c r="B85">
+        <v>28</v>
+      </c>
+      <c r="C85" t="str">
+        <v>Chuyến đi</v>
+      </c>
+      <c r="D85" t="str">
+        <v>Ride</v>
+      </c>
+      <c r="E85" t="str">
+        <v>We are in for a bumpy ride</v>
+      </c>
+      <c r="F85" t="str">
+        <v>A bumpy ride</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>41542f1d-741d-4a47-8a81-a1d09a9a966b</v>
+      </c>
+      <c r="B86">
+        <v>28</v>
+      </c>
+      <c r="C86" t="str">
+        <v>Có ý nghĩa</v>
+      </c>
+      <c r="D86" t="str">
+        <v>Meaningful</v>
+      </c>
+      <c r="E86" t="str">
+        <v>I strive to do meaningful work</v>
+      </c>
+      <c r="F86" t="str">
+        <v>Meaningful work</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>6e66b3ef-3ec5-4743-9860-7418a93dce27</v>
+      </c>
+      <c r="B87">
+        <v>28</v>
+      </c>
+      <c r="C87" t="str">
+        <v>Việc cấm trại</v>
+      </c>
+      <c r="D87" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="E87" t="str">
+        <v>We are going on a camping trip</v>
+      </c>
+      <c r="F87" t="str">
+        <v>A camping trip</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>1188e571-d666-4bf9-81ee-46334eabd388</v>
+      </c>
+      <c r="B88">
+        <v>28</v>
+      </c>
+      <c r="C88" t="str">
+        <v>Hợp tác</v>
+      </c>
+      <c r="D88" t="str">
+        <v>Cooperate</v>
+      </c>
+      <c r="E88" t="str">
+        <v>You have to cooperate with here</v>
+      </c>
+      <c r="F88" t="str">
+        <v>Cooperate with something or somebody</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>c8f79e81-dc8c-4f22-805d-0f1945deadcd</v>
+      </c>
+      <c r="B89">
+        <v>28</v>
+      </c>
+      <c r="C89" t="str">
+        <v>Lều</v>
+      </c>
+      <c r="D89" t="str">
+        <v>Tent</v>
+      </c>
+      <c r="E89" t="str">
+        <v>Please put up the tent for me</v>
+      </c>
+      <c r="F89" t="str">
+        <v>Put up a tent</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>df9891a5-2a7a-4754-91d7-ff7fffc40477</v>
+      </c>
+      <c r="B90">
+        <v>28</v>
+      </c>
+      <c r="C90" t="str">
+        <v>Hứng thú với</v>
+      </c>
+      <c r="D90" t="str">
+        <v>Go in for</v>
+      </c>
+      <c r="E90" t="str">
+        <v>My sister decides to go in for a debate competition</v>
+      </c>
+      <c r="F90" t="str">
+        <v>Go in for a competition</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>f1186873-4969-486d-bd89-9a0695b5388f</v>
+      </c>
+      <c r="B91">
+        <v>28</v>
+      </c>
+      <c r="C91" t="str">
+        <v>Thích hơn</v>
+      </c>
+      <c r="D91" t="str">
+        <v>Prefer</v>
+      </c>
+      <c r="E91" t="str">
+        <v>She prefers eating apples to pears</v>
+      </c>
+      <c r="F91" t="str">
+        <v>Prefer something to something</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>a2b1778e-1bde-4f07-8efc-386e9629f6dc</v>
+      </c>
+      <c r="B92">
+        <v>29</v>
+      </c>
+      <c r="C92" t="str">
+        <v>Câu cá</v>
+      </c>
+      <c r="D92" t="str">
+        <v>Fishing</v>
+      </c>
+      <c r="E92" t="str">
+        <v>My dad and I go fishing every day</v>
+      </c>
+      <c r="F92" t="str">
+        <v>Go fishing</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>cf990805-78a4-450b-9080-8d1407d56334</v>
+      </c>
+      <c r="B93">
+        <v>29</v>
+      </c>
+      <c r="C93" t="str">
+        <v>Vận động viên</v>
+      </c>
+      <c r="D93" t="str">
+        <v>Athlete</v>
+      </c>
+      <c r="E93" t="str">
+        <v>Olumpic athletes train hard to complete</v>
+      </c>
+      <c r="F93" t="str">
+        <v>An Olympic athlete</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>b6a3f27f-b5f1-4f59-a13a-5a3b1d198402</v>
+      </c>
+      <c r="B94">
+        <v>29</v>
+      </c>
+      <c r="C94" t="str">
+        <v>Môn đấu vật</v>
+      </c>
+      <c r="D94" t="str">
+        <v>Wrestling</v>
+      </c>
+      <c r="E94" t="str">
+        <v>Wrestling matches are popular in the US</v>
+      </c>
+      <c r="F94" t="str">
+        <v>A wrestling match</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>f903164f-992c-4ff7-bdd0-9796bb39e5eb</v>
+      </c>
+      <c r="B95">
+        <v>29</v>
+      </c>
+      <c r="C95" t="str">
+        <v>Chuyên nghiệp</v>
+      </c>
+      <c r="D95" t="str">
+        <v>Professional</v>
+      </c>
+      <c r="E95" t="str">
+        <v>He was a professional soccer player</v>
+      </c>
+      <c r="F95" t="str">
+        <v>A professional soccer player</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>f38ea113-6eed-41a7-864c-9fd8eb997c46</v>
+      </c>
+      <c r="B96">
+        <v>29</v>
+      </c>
+      <c r="C96" t="str">
+        <v>Hàng năm</v>
+      </c>
+      <c r="D96" t="str">
+        <v>Annual</v>
+      </c>
+      <c r="E96" t="str">
+        <v>The company has annual meetings for us</v>
+      </c>
+      <c r="F96" t="str">
+        <v>An annual meeting</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>cec821bf-15bc-4c73-85e6-328b2b004fd1</v>
+      </c>
+      <c r="B97">
+        <v>29</v>
+      </c>
+      <c r="C97" t="str">
+        <v>Giải đấu</v>
+      </c>
+      <c r="D97" t="str">
+        <v>Tournament</v>
+      </c>
+      <c r="E97" t="str">
+        <v>What an exciting soccer tournament!</v>
+      </c>
+      <c r="F97" t="str">
+        <v>A soccer tournament</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>ddae4d17-2487-4c91-b15b-62ec664e7e93</v>
+      </c>
+      <c r="B98">
+        <v>29</v>
+      </c>
+      <c r="C98" t="str">
+        <v>Huấn luyện viên</v>
+      </c>
+      <c r="D98" t="str">
+        <v>Coach</v>
+      </c>
+      <c r="E98" t="str">
+        <v>The team coach trains us hard</v>
+      </c>
+      <c r="F98" t="str">
+        <v>The team coach</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>9c573cff-4ddd-4aec-83ca-2f88d870993e</v>
+      </c>
+      <c r="B99">
+        <v>29</v>
+      </c>
+      <c r="C99" t="str">
+        <v>Trận đấu</v>
+      </c>
+      <c r="D99" t="str">
+        <v>Match</v>
+      </c>
+      <c r="E99" t="str">
+        <v>There is a soccer match tonight</v>
+      </c>
+      <c r="F99" t="str">
+        <v>A soccer match</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>dd72f5c5-8548-436c-bd33-79ddb20c7437</v>
+      </c>
+      <c r="B100">
+        <v>29</v>
+      </c>
+      <c r="C100" t="str">
+        <v>Đánh bại</v>
+      </c>
+      <c r="D100" t="str">
+        <v>Beat</v>
+      </c>
+      <c r="E100" t="str">
+        <v>They beat their opponents in the first round</v>
+      </c>
+      <c r="F100" t="str">
+        <v>Beat something or somebody</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>b1892029-56ff-4cbe-984a-c7dab29a9977</v>
+      </c>
+      <c r="B101">
+        <v>29</v>
+      </c>
+      <c r="C101" t="str">
+        <v>Đối thủ</v>
+      </c>
+      <c r="D101" t="str">
+        <v>Opponent</v>
+      </c>
+      <c r="E101" t="str">
+        <v>She is my opponent in chess</v>
+      </c>
+      <c r="F101" t="str">
+        <v>One's oppponent in something</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>1e190ed8-33a8-4e71-b7b2-fa84c7c02941</v>
+      </c>
+      <c r="B102">
+        <v>29</v>
+      </c>
+      <c r="C102" t="str">
+        <v>Môn thể thao</v>
+      </c>
+      <c r="D102" t="str">
+        <v>Athletics</v>
+      </c>
+      <c r="E102" t="str">
+        <v>Football, soccer, and baseball are types of atheletics</v>
+      </c>
+      <c r="F102" t="str">
+        <v>Types of athletics</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>d38353fc-5f4f-472c-ac04-668987f0a4a7</v>
+      </c>
+      <c r="B103">
+        <v>29</v>
+      </c>
+      <c r="C103" t="str">
+        <v>Bóng rỗ</v>
+      </c>
+      <c r="D103" t="str">
+        <v>Basketball</v>
+      </c>
+      <c r="E103" t="str">
+        <v>I am the captain of the basketball team</v>
+      </c>
+      <c r="F103" t="str">
+        <v>A basketball team</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>ef65ce51-588d-4574-aabf-54d79f5fccc8</v>
+      </c>
+      <c r="B104">
+        <v>29</v>
+      </c>
+      <c r="C104" t="str">
+        <v>Người chơi</v>
+      </c>
+      <c r="D104" t="str">
+        <v>Player</v>
+      </c>
+      <c r="E104" t="str">
+        <v>He is the best soccer player here</v>
+      </c>
+      <c r="F104" t="str">
+        <v>A soccer player</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>b7c13a10-8f6b-4bc0-adf4-4efd66aa87fc</v>
+      </c>
+      <c r="B105">
+        <v>29</v>
+      </c>
+      <c r="C105" t="str">
+        <v xml:space="preserve">Liên đoàn </v>
+      </c>
+      <c r="D105" t="str">
+        <v>League</v>
+      </c>
+      <c r="E105" t="str">
+        <v>My sone plays for a soccer league</v>
+      </c>
+      <c r="F105" t="str">
+        <v>A soccer league</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>cbf03296-0921-4040-90d4-199fd9d5c23b</v>
+      </c>
+      <c r="B106">
+        <v>29</v>
+      </c>
+      <c r="C106" t="str">
+        <v>Giải vô địch</v>
+      </c>
+      <c r="D106" t="str">
+        <v>Championship</v>
+      </c>
+      <c r="E106" t="str">
+        <v>Are you ready for the basketball championship</v>
+      </c>
+      <c r="F106" t="str">
+        <v>A basketball championship</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>5029497b-8c66-41b8-8d0a-4bfe381c4286</v>
+      </c>
+      <c r="B107">
+        <v>29</v>
+      </c>
+      <c r="C107" t="str">
+        <v>Đội trưởng</v>
+      </c>
+      <c r="D107" t="str">
+        <v>Captain</v>
+      </c>
+      <c r="E107" t="str">
+        <v>We vote for a team camtain</v>
+      </c>
+      <c r="F107" t="str">
+        <v>Team captain</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>c2fb9123-f320-4cc1-a7fa-d38da99a5fc1</v>
+      </c>
+      <c r="B108">
+        <v>29</v>
+      </c>
+      <c r="C108" t="str">
+        <v>Ghi điểm</v>
+      </c>
+      <c r="D108" t="str">
+        <v>Score</v>
+      </c>
+      <c r="E108" t="str">
+        <v>He scored a goal for the team</v>
+      </c>
+      <c r="F108" t="str">
+        <v>Score a goal</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>a52a7a35-9823-4ea9-87c9-6dec37ecf622</v>
+      </c>
+      <c r="B109">
+        <v>29</v>
+      </c>
+      <c r="C109" t="str">
+        <v>Danh hiệu</v>
+      </c>
+      <c r="D109" t="str">
+        <v>Title</v>
+      </c>
+      <c r="E109" t="str">
+        <v>The team won the title with a goal in the last minute</v>
+      </c>
+      <c r="F109" t="str">
+        <v>Win the title</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>916d379b-cba3-40d9-a67f-a71d48b74a2f</v>
+      </c>
+      <c r="B110">
+        <v>29</v>
+      </c>
+      <c r="C110" t="str">
+        <v>Lưới</v>
+      </c>
+      <c r="D110" t="str">
+        <v>Net</v>
+      </c>
+      <c r="E110" t="str">
+        <v>The fishing net has holes in it</v>
+      </c>
+      <c r="F110" t="str">
+        <v>A fishing net</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>463b16e3-432e-446b-bea0-a0f2b3da5f06</v>
+      </c>
+      <c r="B111">
+        <v>29</v>
+      </c>
+      <c r="C111" t="str">
+        <v>Anh hùng</v>
+      </c>
+      <c r="D111" t="str">
+        <v>Hero</v>
+      </c>
+      <c r="E111" t="str">
+        <v>The fireman became a local hero</v>
+      </c>
+      <c r="F111" t="str">
+        <v>A local hero</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>39de71b0-d5b5-48c9-8f4d-95b2e2f50af6</v>
+      </c>
+      <c r="B112">
+        <v>29</v>
+      </c>
+      <c r="C112" t="str">
+        <v>Môn đạp xe</v>
+      </c>
+      <c r="D112" t="str">
+        <v>Cycling</v>
+      </c>
+      <c r="E112" t="str">
+        <v>She went cycling down the hill</v>
+      </c>
+      <c r="F112" t="str">
+        <v>Go cycling</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>aae25fe9-c463-44f6-8403-64b3ab4901df</v>
+      </c>
+      <c r="B113">
+        <v>29</v>
+      </c>
+      <c r="C113" t="str">
+        <v>Sân vận động</v>
+      </c>
+      <c r="D113" t="str">
+        <v>Stadium</v>
+      </c>
+      <c r="E113" t="str">
+        <v>Where is the biggest sports stadium in hanoi</v>
+      </c>
+      <c r="F113" t="str">
+        <v>A sport stadium</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>a8bd58e5-0590-4ebb-9b28-1b10efe4f691</v>
+      </c>
+      <c r="B114">
+        <v>29</v>
+      </c>
+      <c r="C114" t="str">
+        <v>Người thắng cuộc</v>
+      </c>
+      <c r="D114" t="str">
+        <v>Winner</v>
+      </c>
+      <c r="E114" t="str">
+        <v>The actor is an award winner</v>
+      </c>
+      <c r="F114" t="str">
+        <v>An award winer</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>b553acc6-a0c9-417a-b2d9-d77e5fd33909</v>
+      </c>
+      <c r="B115">
+        <v>29</v>
+      </c>
+      <c r="C115" t="str">
+        <v>Môn đánh golf</v>
+      </c>
+      <c r="D115" t="str">
+        <v>Golf</v>
+      </c>
+      <c r="E115" t="str">
+        <v>Businessmen love to play golf</v>
+      </c>
+      <c r="F115" t="str">
+        <v>Play golf</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>c9b2d631-4c95-4cbf-b5c6-51760a9800c8</v>
+      </c>
+      <c r="B116">
+        <v>29</v>
+      </c>
+      <c r="C116" t="str">
+        <v>Đánh</v>
+      </c>
+      <c r="D116" t="str">
+        <v>Strike</v>
+      </c>
+      <c r="E116" t="str">
+        <v>He strikes the golf ball perfectly</v>
+      </c>
+      <c r="F116" t="str">
+        <v>Strike the ball</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>6c846374-0b04-4261-a1fc-abb952bde9d0</v>
+      </c>
+      <c r="B117">
+        <v>29</v>
+      </c>
+      <c r="C117" t="str">
+        <v>Đích, mục tiêu</v>
+      </c>
+      <c r="D117" t="str">
+        <v>Target</v>
+      </c>
+      <c r="E117" t="str">
+        <v>He shot the arrow and hit the target</v>
+      </c>
+      <c r="F117" t="str">
+        <v>Hit the target</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>7c39a7bf-0223-4d67-bf19-bc70d6260a4c</v>
+      </c>
+      <c r="B118">
+        <v>29</v>
+      </c>
+      <c r="C118" t="str">
+        <v>Tối đa</v>
+      </c>
+      <c r="D118" t="str">
+        <v>Maximum</v>
+      </c>
+      <c r="E118" t="str">
+        <v>The maximum amount for storage is 256GB</v>
+      </c>
+      <c r="F118" t="str">
+        <v>The maximum amount</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>727a487b-ea11-4357-8b3a-cfd78069fedb</v>
+      </c>
+      <c r="B119">
+        <v>29</v>
+      </c>
+      <c r="C119" t="str">
+        <v>Lướt</v>
+      </c>
+      <c r="D119" t="str">
+        <v>Surf</v>
+      </c>
+      <c r="E119" t="str">
+        <v>In hawaii, you must surf the waves</v>
+      </c>
+      <c r="F119" t="str">
+        <v>Surf the wave</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>86cb971a-bdd1-45d0-9169-17ef0fb2990e</v>
+      </c>
+      <c r="B120">
+        <v>29</v>
+      </c>
+      <c r="C120" t="str">
+        <v>Không may</v>
+      </c>
+      <c r="D120" t="str">
+        <v>Unfortunately</v>
+      </c>
+      <c r="E120" t="str">
+        <v>Unfortunately, I won't be able to attend the meeting</v>
+      </c>
+      <c r="F120" t="str">
+        <v>Unfortunately, I won't</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>2805d4a5-2450-4193-92b7-19d2357bd4d9</v>
+      </c>
+      <c r="B121">
+        <v>29</v>
+      </c>
+      <c r="C121" t="str">
+        <v>Trân trọng, đánh giá cao</v>
+      </c>
+      <c r="D121" t="str">
+        <v>Appreciate</v>
+      </c>
+      <c r="E121" t="str">
+        <v>I appreciate the help you gave me</v>
+      </c>
+      <c r="F121" t="str">
+        <v>Appreciate somebody or something</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F121"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: release unit 7 and 1/3 unit 8
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DB93DE-1701-7A4F-93DE-069B7423BCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382A33FF-43AD-B04E-99D2-A22F96C920D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50740" yWindow="-960" windowWidth="33600" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46760" yWindow="-1780" windowWidth="33600" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="1542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1671">
   <si>
     <t>ID</t>
   </si>
@@ -4657,6 +4657,393 @@
   </si>
   <si>
     <t>Write a summary</t>
+  </si>
+  <si>
+    <t>Thư ký</t>
+  </si>
+  <si>
+    <t>Secretary</t>
+  </si>
+  <si>
+    <t>She works as a secretary for our manager</t>
+  </si>
+  <si>
+    <t>Work as a secretary</t>
+  </si>
+  <si>
+    <t>Tập tài liệu</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>she tells me to create a new folder on the computer</t>
+  </si>
+  <si>
+    <t>create a new folder</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Print</t>
+  </si>
+  <si>
+    <t>I print our photos on a cup</t>
+  </si>
+  <si>
+    <t>print something on something</t>
+  </si>
+  <si>
+    <t>colleague</t>
+  </si>
+  <si>
+    <t>Đồng nghiệp</t>
+  </si>
+  <si>
+    <t>Our male colleagues prepare gifts for women's day</t>
+  </si>
+  <si>
+    <t>a male colleague</t>
+  </si>
+  <si>
+    <t>Báo cáo</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>I stay up late to write a report</t>
+  </si>
+  <si>
+    <t>write a report</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>The due date for the next payment is today</t>
+  </si>
+  <si>
+    <t>due date</t>
+  </si>
+  <si>
+    <t>Đến hạn</t>
+  </si>
+  <si>
+    <t>Kỳ thực tập</t>
+  </si>
+  <si>
+    <t>Internship</t>
+  </si>
+  <si>
+    <t>My friend gets an internship at EY</t>
+  </si>
+  <si>
+    <t>get an internship / được nhận vào thực tập</t>
+  </si>
+  <si>
+    <t>Hoãn lại</t>
+  </si>
+  <si>
+    <t>Put off</t>
+  </si>
+  <si>
+    <t>She puts off going to the dentist until Sunday</t>
+  </si>
+  <si>
+    <t>put off doing something</t>
+  </si>
+  <si>
+    <t>Thiết bị</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>His job is to install equipment for laboratories</t>
+  </si>
+  <si>
+    <t>install equipment</t>
+  </si>
+  <si>
+    <t>Giải pháp</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>We cannot find a solution to the problem</t>
+  </si>
+  <si>
+    <t>find a solution</t>
+  </si>
+  <si>
+    <t>Chức năng</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Video call is a useful function of FB</t>
+  </si>
+  <si>
+    <t>a useful function</t>
+  </si>
+  <si>
+    <t>Bàn giao</t>
+  </si>
+  <si>
+    <t>hand over</t>
+  </si>
+  <si>
+    <t>He finally hands over the project to his boss</t>
+  </si>
+  <si>
+    <t>hand over something to somebody</t>
+  </si>
+  <si>
+    <t>Hạn chót</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>I work overtime to meet the deadline</t>
+  </si>
+  <si>
+    <t>meet a deadline / kịp hạn chót</t>
+  </si>
+  <si>
+    <t>Cuộc họp</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>we aare well-prepared to attend the meeting</t>
+  </si>
+  <si>
+    <t>attend a meeting</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Our dog is considered a family member</t>
+  </si>
+  <si>
+    <t>a family member</t>
+  </si>
+  <si>
+    <t>Thành viên</t>
+  </si>
+  <si>
+    <t>Bài thuyết trình</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Candidates need to give a presentation on Monday</t>
+  </si>
+  <si>
+    <t>give a presentation</t>
+  </si>
+  <si>
+    <t>Chấp nhận</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>His parents do not approve of his girlfriend</t>
+  </si>
+  <si>
+    <t>Approve of somebody or something</t>
+  </si>
+  <si>
+    <t>Conference</t>
+  </si>
+  <si>
+    <t>Hội thảo</t>
+  </si>
+  <si>
+    <t>They organize a conference about technology every year</t>
+  </si>
+  <si>
+    <t>organize a conference</t>
+  </si>
+  <si>
+    <t>Khách hàng</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>We are all shopee's potential clients</t>
+  </si>
+  <si>
+    <t>a potential client / khách hàng tiềm năng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lỗi </t>
+  </si>
+  <si>
+    <t>Fault</t>
+  </si>
+  <si>
+    <t>It's not my fault</t>
+  </si>
+  <si>
+    <t>not my fault</t>
+  </si>
+  <si>
+    <t>U08_01</t>
+  </si>
+  <si>
+    <t>U08_02</t>
+  </si>
+  <si>
+    <t>U08_03</t>
+  </si>
+  <si>
+    <t>U08_04</t>
+  </si>
+  <si>
+    <t>U08_05</t>
+  </si>
+  <si>
+    <t>U08_06</t>
+  </si>
+  <si>
+    <t>U08_07</t>
+  </si>
+  <si>
+    <t>U08_08</t>
+  </si>
+  <si>
+    <t>U08_09</t>
+  </si>
+  <si>
+    <t>U08_10</t>
+  </si>
+  <si>
+    <t>Hủy</t>
+  </si>
+  <si>
+    <t>Call off</t>
+  </si>
+  <si>
+    <t>He calls off the meeting all of a sudden</t>
+  </si>
+  <si>
+    <t>Call off something</t>
+  </si>
+  <si>
+    <t>Con dấu, con tem</t>
+  </si>
+  <si>
+    <t>Stamp</t>
+  </si>
+  <si>
+    <t>She puts a stamp on the envelope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">put a stamp on </t>
+  </si>
+  <si>
+    <t>Ý kiến phản hồi</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Customers are encouraged to provide feedbacks to us</t>
+  </si>
+  <si>
+    <t>Implement a strategy</t>
+  </si>
+  <si>
+    <t>Thực hiện</t>
+  </si>
+  <si>
+    <t>Carry out</t>
+  </si>
+  <si>
+    <t>They carry out the research on customers' behaviors</t>
+  </si>
+  <si>
+    <t>carry out something</t>
+  </si>
+  <si>
+    <t>Chiến lược</t>
+  </si>
+  <si>
+    <t>Provide feedback</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>It is crucial to implement a new strategy</t>
+  </si>
+  <si>
+    <t>Trợ lý</t>
+  </si>
+  <si>
+    <t>Assistant</t>
+  </si>
+  <si>
+    <t>She applies to be a teaching assistant</t>
+  </si>
+  <si>
+    <t>A teaching assistant / trợ giảng</t>
+  </si>
+  <si>
+    <t>nghỉ hưu</t>
+  </si>
+  <si>
+    <t>Retire</t>
+  </si>
+  <si>
+    <t>Aging forces him to retire from his job</t>
+  </si>
+  <si>
+    <t>retire from something / nghỉ hưu khỏi việc gì đó</t>
+  </si>
+  <si>
+    <t>Mang tính chuyên gia</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>Whe should seek expert advice before deciding</t>
+  </si>
+  <si>
+    <t>expert advice / tư vấn chuyên môn</t>
+  </si>
+  <si>
+    <t>Handle</t>
+  </si>
+  <si>
+    <t>He handles the situation gracefully</t>
+  </si>
+  <si>
+    <t>handle a situation</t>
+  </si>
+  <si>
+    <t>Bao gồm</t>
+  </si>
+  <si>
+    <t>Involve</t>
+  </si>
+  <si>
+    <t>Banking involves a lot of measuring</t>
+  </si>
+  <si>
+    <t>involve something</t>
   </si>
 </sst>
 </file>
@@ -5014,10 +5401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G331"/>
+  <dimension ref="A1:G341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G191" sqref="G191"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9200,19 +9587,19 @@
         <v>7</v>
       </c>
       <c r="C182" t="s">
-        <v>1503</v>
+        <v>1632</v>
       </c>
       <c r="D182" t="s">
-        <v>1504</v>
+        <v>1633</v>
       </c>
       <c r="E182" t="s">
-        <v>1505</v>
+        <v>1634</v>
       </c>
       <c r="F182" t="s">
-        <v>1506</v>
+        <v>1635</v>
       </c>
       <c r="G182" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,16 +9610,16 @@
         <v>7</v>
       </c>
       <c r="C183" t="s">
-        <v>1507</v>
+        <v>1636</v>
       </c>
       <c r="D183" t="s">
-        <v>1508</v>
+        <v>1637</v>
       </c>
       <c r="E183" t="s">
-        <v>1509</v>
+        <v>1638</v>
       </c>
       <c r="F183" t="s">
-        <v>1510</v>
+        <v>1639</v>
       </c>
       <c r="G183" t="s">
         <v>28</v>
@@ -9246,19 +9633,19 @@
         <v>7</v>
       </c>
       <c r="C184" t="s">
-        <v>1511</v>
+        <v>1640</v>
       </c>
       <c r="D184" t="s">
-        <v>1512</v>
+        <v>1641</v>
       </c>
       <c r="E184" t="s">
-        <v>1513</v>
+        <v>1642</v>
       </c>
       <c r="F184" t="s">
-        <v>1514</v>
+        <v>1649</v>
       </c>
       <c r="G184" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
@@ -9269,16 +9656,16 @@
         <v>7</v>
       </c>
       <c r="C185" t="s">
-        <v>1515</v>
+        <v>1644</v>
       </c>
       <c r="D185" t="s">
-        <v>1516</v>
+        <v>1645</v>
       </c>
       <c r="E185" t="s">
-        <v>1517</v>
+        <v>1646</v>
       </c>
       <c r="F185" t="s">
-        <v>1518</v>
+        <v>1647</v>
       </c>
       <c r="G185" t="s">
         <v>12</v>
@@ -9292,16 +9679,16 @@
         <v>7</v>
       </c>
       <c r="C186" t="s">
-        <v>332</v>
+        <v>1648</v>
       </c>
       <c r="D186" t="s">
-        <v>1519</v>
+        <v>1650</v>
       </c>
       <c r="E186" t="s">
-        <v>1520</v>
+        <v>1651</v>
       </c>
       <c r="F186" t="s">
-        <v>1521</v>
+        <v>1643</v>
       </c>
       <c r="G186" t="s">
         <v>28</v>
@@ -9315,16 +9702,16 @@
         <v>7</v>
       </c>
       <c r="C187" t="s">
-        <v>1522</v>
+        <v>1652</v>
       </c>
       <c r="D187" t="s">
-        <v>1523</v>
+        <v>1653</v>
       </c>
       <c r="E187" t="s">
-        <v>1524</v>
+        <v>1654</v>
       </c>
       <c r="F187" t="s">
-        <v>1525</v>
+        <v>1655</v>
       </c>
       <c r="G187" t="s">
         <v>28</v>
@@ -9338,19 +9725,19 @@
         <v>7</v>
       </c>
       <c r="C188" t="s">
-        <v>1526</v>
+        <v>1656</v>
       </c>
       <c r="D188" t="s">
-        <v>1527</v>
+        <v>1657</v>
       </c>
       <c r="E188" t="s">
-        <v>1528</v>
+        <v>1658</v>
       </c>
       <c r="F188" t="s">
-        <v>1529</v>
+        <v>1659</v>
       </c>
       <c r="G188" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
@@ -9361,19 +9748,19 @@
         <v>7</v>
       </c>
       <c r="C189" t="s">
-        <v>1530</v>
+        <v>1660</v>
       </c>
       <c r="D189" t="s">
-        <v>1531</v>
+        <v>1661</v>
       </c>
       <c r="E189" t="s">
-        <v>1532</v>
+        <v>1662</v>
       </c>
       <c r="F189" t="s">
-        <v>1533</v>
+        <v>1663</v>
       </c>
       <c r="G189" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
@@ -9384,19 +9771,19 @@
         <v>7</v>
       </c>
       <c r="C190" t="s">
-        <v>1534</v>
+        <v>830</v>
       </c>
       <c r="D190" t="s">
-        <v>1535</v>
+        <v>1664</v>
       </c>
       <c r="E190" t="s">
-        <v>1536</v>
+        <v>1665</v>
       </c>
       <c r="F190" t="s">
-        <v>1537</v>
+        <v>1666</v>
       </c>
       <c r="G190" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
@@ -9407,19 +9794,19 @@
         <v>7</v>
       </c>
       <c r="C191" t="s">
-        <v>1538</v>
+        <v>1667</v>
       </c>
       <c r="D191" t="s">
-        <v>1539</v>
+        <v>1668</v>
       </c>
       <c r="E191" t="s">
-        <v>1540</v>
+        <v>1669</v>
       </c>
       <c r="F191" t="s">
-        <v>1541</v>
+        <v>1670</v>
       </c>
       <c r="G191" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
@@ -9429,434 +9816,764 @@
       <c r="B192">
         <v>7</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C192" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D192" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E192" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F192" t="s">
+        <v>1545</v>
+      </c>
+      <c r="G192" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>1484</v>
       </c>
       <c r="B193">
         <v>7</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C193" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D193" t="s">
+        <v>1547</v>
+      </c>
+      <c r="E193" t="s">
+        <v>1548</v>
+      </c>
+      <c r="F193" t="s">
+        <v>1549</v>
+      </c>
+      <c r="G193" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>1485</v>
       </c>
       <c r="B194">
         <v>7</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C194" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D194" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E194" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F194" t="s">
+        <v>1553</v>
+      </c>
+      <c r="G194" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>1486</v>
       </c>
       <c r="B195">
         <v>7</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C195" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D195" t="s">
+        <v>1554</v>
+      </c>
+      <c r="E195" t="s">
+        <v>1556</v>
+      </c>
+      <c r="F195" t="s">
+        <v>1557</v>
+      </c>
+      <c r="G195" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>1487</v>
       </c>
       <c r="B196">
         <v>7</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C196" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D196" t="s">
+        <v>1559</v>
+      </c>
+      <c r="E196" t="s">
+        <v>1560</v>
+      </c>
+      <c r="F196" t="s">
+        <v>1561</v>
+      </c>
+      <c r="G196" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>1488</v>
       </c>
       <c r="B197">
         <v>7</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C197" t="s">
+        <v>1565</v>
+      </c>
+      <c r="D197" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E197" t="s">
+        <v>1563</v>
+      </c>
+      <c r="F197" t="s">
+        <v>1564</v>
+      </c>
+      <c r="G197" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>1489</v>
       </c>
       <c r="B198">
         <v>7</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C198" t="s">
+        <v>1566</v>
+      </c>
+      <c r="D198" t="s">
+        <v>1567</v>
+      </c>
+      <c r="E198" t="s">
+        <v>1568</v>
+      </c>
+      <c r="F198" t="s">
+        <v>1569</v>
+      </c>
+      <c r="G198" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>1490</v>
       </c>
       <c r="B199">
         <v>7</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C199" t="s">
+        <v>1570</v>
+      </c>
+      <c r="D199" t="s">
+        <v>1571</v>
+      </c>
+      <c r="E199" t="s">
+        <v>1572</v>
+      </c>
+      <c r="F199" t="s">
+        <v>1573</v>
+      </c>
+      <c r="G199" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>1491</v>
       </c>
       <c r="B200">
         <v>7</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C200" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D200" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E200" t="s">
+        <v>1576</v>
+      </c>
+      <c r="F200" t="s">
+        <v>1577</v>
+      </c>
+      <c r="G200" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>1492</v>
       </c>
       <c r="B201">
         <v>7</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C201" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D201" t="s">
+        <v>1579</v>
+      </c>
+      <c r="E201" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F201" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G201" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>1493</v>
       </c>
       <c r="B202">
         <v>7</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C202" t="s">
+        <v>1582</v>
+      </c>
+      <c r="D202" t="s">
+        <v>1583</v>
+      </c>
+      <c r="E202" t="s">
+        <v>1584</v>
+      </c>
+      <c r="F202" t="s">
+        <v>1585</v>
+      </c>
+      <c r="G202" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>1494</v>
       </c>
       <c r="B203">
         <v>7</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C203" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D203" t="s">
+        <v>1587</v>
+      </c>
+      <c r="E203" t="s">
+        <v>1588</v>
+      </c>
+      <c r="F203" t="s">
+        <v>1589</v>
+      </c>
+      <c r="G203" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>1495</v>
       </c>
       <c r="B204">
         <v>7</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C204" t="s">
+        <v>1590</v>
+      </c>
+      <c r="D204" t="s">
+        <v>1591</v>
+      </c>
+      <c r="E204" t="s">
+        <v>1592</v>
+      </c>
+      <c r="F204" t="s">
+        <v>1593</v>
+      </c>
+      <c r="G204" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>1496</v>
       </c>
       <c r="B205">
         <v>7</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C205" t="s">
+        <v>1594</v>
+      </c>
+      <c r="D205" t="s">
+        <v>1595</v>
+      </c>
+      <c r="E205" t="s">
+        <v>1596</v>
+      </c>
+      <c r="F205" t="s">
+        <v>1597</v>
+      </c>
+      <c r="G205" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>1497</v>
       </c>
       <c r="B206">
         <v>7</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C206" t="s">
+        <v>1601</v>
+      </c>
+      <c r="D206" t="s">
+        <v>1598</v>
+      </c>
+      <c r="E206" t="s">
+        <v>1599</v>
+      </c>
+      <c r="F206" t="s">
+        <v>1600</v>
+      </c>
+      <c r="G206" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>1498</v>
       </c>
       <c r="B207">
         <v>7</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C207" t="s">
+        <v>1602</v>
+      </c>
+      <c r="D207" t="s">
+        <v>1603</v>
+      </c>
+      <c r="E207" t="s">
+        <v>1604</v>
+      </c>
+      <c r="F207" t="s">
+        <v>1605</v>
+      </c>
+      <c r="G207" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>1499</v>
       </c>
       <c r="B208">
         <v>7</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C208" t="s">
+        <v>1606</v>
+      </c>
+      <c r="D208" t="s">
+        <v>1607</v>
+      </c>
+      <c r="E208" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F208" t="s">
+        <v>1609</v>
+      </c>
+      <c r="G208" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>1500</v>
       </c>
       <c r="B209">
         <v>7</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C209" t="s">
+        <v>1611</v>
+      </c>
+      <c r="D209" t="s">
+        <v>1610</v>
+      </c>
+      <c r="E209" t="s">
+        <v>1612</v>
+      </c>
+      <c r="F209" t="s">
+        <v>1613</v>
+      </c>
+      <c r="G209" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>1501</v>
       </c>
       <c r="B210">
         <v>7</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C210" t="s">
+        <v>1614</v>
+      </c>
+      <c r="D210" t="s">
+        <v>1615</v>
+      </c>
+      <c r="E210" t="s">
+        <v>1616</v>
+      </c>
+      <c r="F210" t="s">
+        <v>1617</v>
+      </c>
+      <c r="G210" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>1502</v>
       </c>
       <c r="B211">
         <v>7</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C211" t="s">
+        <v>1618</v>
+      </c>
+      <c r="D211" t="s">
+        <v>1619</v>
+      </c>
+      <c r="E211" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F211" t="s">
+        <v>1621</v>
+      </c>
+      <c r="G211" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B212">
+        <v>8</v>
+      </c>
+      <c r="C212" t="s">
+        <v>1503</v>
+      </c>
+      <c r="D212" t="s">
+        <v>1504</v>
+      </c>
+      <c r="E212" t="s">
+        <v>1505</v>
+      </c>
+      <c r="F212" t="s">
+        <v>1506</v>
+      </c>
+      <c r="G212" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B213">
+        <v>8</v>
+      </c>
+      <c r="C213" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D213" t="s">
+        <v>1508</v>
+      </c>
+      <c r="E213" t="s">
+        <v>1509</v>
+      </c>
+      <c r="F213" t="s">
+        <v>1510</v>
+      </c>
+      <c r="G213" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B214">
+        <v>8</v>
+      </c>
+      <c r="C214" t="s">
+        <v>1511</v>
+      </c>
+      <c r="D214" t="s">
+        <v>1512</v>
+      </c>
+      <c r="E214" t="s">
+        <v>1513</v>
+      </c>
+      <c r="F214" t="s">
+        <v>1514</v>
+      </c>
+      <c r="G214" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B215">
+        <v>8</v>
+      </c>
+      <c r="C215" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D215" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E215" t="s">
+        <v>1517</v>
+      </c>
+      <c r="F215" t="s">
+        <v>1518</v>
+      </c>
+      <c r="G215" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B216">
+        <v>8</v>
+      </c>
+      <c r="C216" t="s">
+        <v>332</v>
+      </c>
+      <c r="D216" t="s">
+        <v>1519</v>
+      </c>
+      <c r="E216" t="s">
+        <v>1520</v>
+      </c>
+      <c r="F216" t="s">
+        <v>1521</v>
+      </c>
+      <c r="G216" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B217">
+        <v>8</v>
+      </c>
+      <c r="C217" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D217" t="s">
+        <v>1523</v>
+      </c>
+      <c r="E217" t="s">
+        <v>1524</v>
+      </c>
+      <c r="F217" t="s">
+        <v>1525</v>
+      </c>
+      <c r="G217" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B218">
+        <v>8</v>
+      </c>
+      <c r="C218" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D218" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E218" t="s">
+        <v>1528</v>
+      </c>
+      <c r="F218" t="s">
+        <v>1529</v>
+      </c>
+      <c r="G218" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>1629</v>
+      </c>
+      <c r="B219">
+        <v>8</v>
+      </c>
+      <c r="C219" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D219" t="s">
+        <v>1531</v>
+      </c>
+      <c r="E219" t="s">
+        <v>1532</v>
+      </c>
+      <c r="F219" t="s">
+        <v>1533</v>
+      </c>
+      <c r="G219" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B220">
+        <v>8</v>
+      </c>
+      <c r="C220" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D220" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E220" t="s">
+        <v>1536</v>
+      </c>
+      <c r="F220" t="s">
+        <v>1537</v>
+      </c>
+      <c r="G220" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B221">
+        <v>8</v>
+      </c>
+      <c r="C221" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D221" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E221" t="s">
+        <v>1540</v>
+      </c>
+      <c r="F221" t="s">
+        <v>1541</v>
+      </c>
+      <c r="G221" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
         <v>907</v>
-      </c>
-      <c r="B212">
-        <v>26</v>
-      </c>
-      <c r="C212" t="s">
-        <v>908</v>
-      </c>
-      <c r="D212" t="s">
-        <v>909</v>
-      </c>
-      <c r="E212" t="s">
-        <v>910</v>
-      </c>
-      <c r="F212" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>912</v>
-      </c>
-      <c r="B213">
-        <v>26</v>
-      </c>
-      <c r="C213" t="s">
-        <v>913</v>
-      </c>
-      <c r="D213" t="s">
-        <v>914</v>
-      </c>
-      <c r="E213" t="s">
-        <v>915</v>
-      </c>
-      <c r="F213" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>916</v>
-      </c>
-      <c r="B214">
-        <v>26</v>
-      </c>
-      <c r="C214" t="s">
-        <v>917</v>
-      </c>
-      <c r="D214" t="s">
-        <v>918</v>
-      </c>
-      <c r="E214" t="s">
-        <v>919</v>
-      </c>
-      <c r="F214" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
-        <v>920</v>
-      </c>
-      <c r="B215">
-        <v>26</v>
-      </c>
-      <c r="C215" t="s">
-        <v>921</v>
-      </c>
-      <c r="D215" t="s">
-        <v>922</v>
-      </c>
-      <c r="E215" t="s">
-        <v>923</v>
-      </c>
-      <c r="F215" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
-        <v>924</v>
-      </c>
-      <c r="B216">
-        <v>26</v>
-      </c>
-      <c r="C216" t="s">
-        <v>925</v>
-      </c>
-      <c r="D216" t="s">
-        <v>926</v>
-      </c>
-      <c r="E216" t="s">
-        <v>927</v>
-      </c>
-      <c r="F216" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A217" t="s">
-        <v>928</v>
-      </c>
-      <c r="B217">
-        <v>26</v>
-      </c>
-      <c r="C217" t="s">
-        <v>929</v>
-      </c>
-      <c r="D217" t="s">
-        <v>930</v>
-      </c>
-      <c r="E217" t="s">
-        <v>931</v>
-      </c>
-      <c r="F217" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
-        <v>932</v>
-      </c>
-      <c r="B218">
-        <v>26</v>
-      </c>
-      <c r="C218" t="s">
-        <v>933</v>
-      </c>
-      <c r="D218" t="s">
-        <v>934</v>
-      </c>
-      <c r="E218" t="s">
-        <v>935</v>
-      </c>
-      <c r="F218" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
-        <v>936</v>
-      </c>
-      <c r="B219">
-        <v>26</v>
-      </c>
-      <c r="C219" t="s">
-        <v>937</v>
-      </c>
-      <c r="D219" t="s">
-        <v>938</v>
-      </c>
-      <c r="E219" t="s">
-        <v>939</v>
-      </c>
-      <c r="F219" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
-        <v>940</v>
-      </c>
-      <c r="B220">
-        <v>26</v>
-      </c>
-      <c r="C220" t="s">
-        <v>941</v>
-      </c>
-      <c r="D220" t="s">
-        <v>942</v>
-      </c>
-      <c r="E220" t="s">
-        <v>943</v>
-      </c>
-      <c r="F220" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A221" t="s">
-        <v>944</v>
-      </c>
-      <c r="B221">
-        <v>26</v>
-      </c>
-      <c r="C221" t="s">
-        <v>945</v>
-      </c>
-      <c r="D221" t="s">
-        <v>946</v>
-      </c>
-      <c r="E221" t="s">
-        <v>947</v>
-      </c>
-      <c r="F221" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A222" t="s">
-        <v>948</v>
       </c>
       <c r="B222">
         <v>26</v>
       </c>
       <c r="C222" t="s">
-        <v>949</v>
+        <v>908</v>
       </c>
       <c r="D222" t="s">
-        <v>950</v>
+        <v>909</v>
       </c>
       <c r="E222" t="s">
-        <v>951</v>
+        <v>910</v>
       </c>
       <c r="F222" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>952</v>
+        <v>912</v>
       </c>
       <c r="B223">
         <v>26</v>
       </c>
       <c r="C223" t="s">
-        <v>953</v>
+        <v>913</v>
       </c>
       <c r="D223" t="s">
-        <v>954</v>
+        <v>914</v>
       </c>
       <c r="E223" t="s">
-        <v>955</v>
+        <v>915</v>
       </c>
       <c r="F223" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>956</v>
+        <v>916</v>
       </c>
       <c r="B224">
         <v>26</v>
       </c>
       <c r="C224" t="s">
-        <v>957</v>
+        <v>917</v>
       </c>
       <c r="D224" t="s">
-        <v>958</v>
+        <v>918</v>
       </c>
       <c r="E224" t="s">
-        <v>959</v>
+        <v>919</v>
       </c>
       <c r="F224" t="s">
-        <v>960</v>
+        <v>911</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>961</v>
+        <v>920</v>
       </c>
       <c r="B225">
         <v>26</v>
       </c>
       <c r="C225" t="s">
-        <v>962</v>
+        <v>921</v>
       </c>
       <c r="D225" t="s">
-        <v>963</v>
+        <v>922</v>
       </c>
       <c r="E225" t="s">
-        <v>964</v>
+        <v>923</v>
       </c>
       <c r="F225" t="s">
         <v>911</v>
@@ -9864,39 +10581,39 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>965</v>
+        <v>924</v>
       </c>
       <c r="B226">
         <v>26</v>
       </c>
       <c r="C226" t="s">
-        <v>966</v>
+        <v>925</v>
       </c>
       <c r="D226" t="s">
-        <v>967</v>
+        <v>926</v>
       </c>
       <c r="E226" t="s">
-        <v>968</v>
+        <v>927</v>
       </c>
       <c r="F226" t="s">
-        <v>969</v>
+        <v>911</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>970</v>
+        <v>928</v>
       </c>
       <c r="B227">
         <v>26</v>
       </c>
       <c r="C227" t="s">
-        <v>971</v>
+        <v>929</v>
       </c>
       <c r="D227" t="s">
-        <v>972</v>
+        <v>930</v>
       </c>
       <c r="E227" t="s">
-        <v>973</v>
+        <v>931</v>
       </c>
       <c r="F227" t="s">
         <v>911</v>
@@ -9904,39 +10621,39 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>974</v>
+        <v>932</v>
       </c>
       <c r="B228">
         <v>26</v>
       </c>
       <c r="C228" t="s">
-        <v>975</v>
+        <v>933</v>
       </c>
       <c r="D228" t="s">
-        <v>976</v>
+        <v>934</v>
       </c>
       <c r="E228" t="s">
-        <v>977</v>
+        <v>935</v>
       </c>
       <c r="F228" t="s">
-        <v>978</v>
+        <v>911</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>979</v>
+        <v>936</v>
       </c>
       <c r="B229">
         <v>26</v>
       </c>
       <c r="C229" t="s">
-        <v>980</v>
+        <v>937</v>
       </c>
       <c r="D229" t="s">
-        <v>981</v>
+        <v>938</v>
       </c>
       <c r="E229" t="s">
-        <v>982</v>
+        <v>939</v>
       </c>
       <c r="F229" t="s">
         <v>911</v>
@@ -9944,19 +10661,19 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>983</v>
+        <v>940</v>
       </c>
       <c r="B230">
         <v>26</v>
       </c>
       <c r="C230" t="s">
-        <v>984</v>
+        <v>941</v>
       </c>
       <c r="D230" t="s">
-        <v>985</v>
+        <v>942</v>
       </c>
       <c r="E230" t="s">
-        <v>986</v>
+        <v>943</v>
       </c>
       <c r="F230" t="s">
         <v>911</v>
@@ -9964,39 +10681,39 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>987</v>
+        <v>944</v>
       </c>
       <c r="B231">
         <v>26</v>
       </c>
       <c r="C231" t="s">
-        <v>988</v>
+        <v>945</v>
       </c>
       <c r="D231" t="s">
-        <v>989</v>
+        <v>946</v>
       </c>
       <c r="E231" t="s">
-        <v>990</v>
+        <v>947</v>
       </c>
       <c r="F231" t="s">
-        <v>991</v>
+        <v>911</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>992</v>
+        <v>948</v>
       </c>
       <c r="B232">
         <v>26</v>
       </c>
       <c r="C232" t="s">
-        <v>993</v>
+        <v>949</v>
       </c>
       <c r="D232" t="s">
-        <v>994</v>
+        <v>950</v>
       </c>
       <c r="E232" t="s">
-        <v>995</v>
+        <v>951</v>
       </c>
       <c r="F232" t="s">
         <v>911</v>
@@ -10004,19 +10721,19 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>996</v>
+        <v>952</v>
       </c>
       <c r="B233">
         <v>26</v>
       </c>
       <c r="C233" t="s">
-        <v>997</v>
+        <v>953</v>
       </c>
       <c r="D233" t="s">
-        <v>998</v>
+        <v>954</v>
       </c>
       <c r="E233" t="s">
-        <v>999</v>
+        <v>955</v>
       </c>
       <c r="F233" t="s">
         <v>911</v>
@@ -10024,39 +10741,39 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>1000</v>
+        <v>956</v>
       </c>
       <c r="B234">
         <v>26</v>
       </c>
       <c r="C234" t="s">
-        <v>1001</v>
+        <v>957</v>
       </c>
       <c r="D234" t="s">
-        <v>1002</v>
+        <v>958</v>
       </c>
       <c r="E234" t="s">
-        <v>1003</v>
+        <v>959</v>
       </c>
       <c r="F234" t="s">
-        <v>911</v>
+        <v>960</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>1004</v>
+        <v>961</v>
       </c>
       <c r="B235">
         <v>26</v>
       </c>
       <c r="C235" t="s">
-        <v>1005</v>
+        <v>962</v>
       </c>
       <c r="D235" t="s">
-        <v>1006</v>
+        <v>963</v>
       </c>
       <c r="E235" t="s">
-        <v>1007</v>
+        <v>964</v>
       </c>
       <c r="F235" t="s">
         <v>911</v>
@@ -10064,79 +10781,79 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>1008</v>
+        <v>965</v>
       </c>
       <c r="B236">
         <v>26</v>
       </c>
       <c r="C236" t="s">
-        <v>1009</v>
+        <v>966</v>
       </c>
       <c r="D236" t="s">
-        <v>1010</v>
+        <v>967</v>
       </c>
       <c r="E236" t="s">
-        <v>1011</v>
+        <v>968</v>
       </c>
       <c r="F236" t="s">
-        <v>911</v>
+        <v>969</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>1012</v>
+        <v>970</v>
       </c>
       <c r="B237">
         <v>26</v>
       </c>
       <c r="C237" t="s">
-        <v>1013</v>
+        <v>971</v>
       </c>
       <c r="D237" t="s">
-        <v>1014</v>
+        <v>972</v>
       </c>
       <c r="E237" t="s">
-        <v>1015</v>
+        <v>973</v>
       </c>
       <c r="F237" t="s">
-        <v>1016</v>
+        <v>911</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>1017</v>
+        <v>974</v>
       </c>
       <c r="B238">
         <v>26</v>
       </c>
       <c r="C238" t="s">
-        <v>1018</v>
+        <v>975</v>
       </c>
       <c r="D238" t="s">
-        <v>1019</v>
+        <v>976</v>
       </c>
       <c r="E238" t="s">
-        <v>1020</v>
+        <v>977</v>
       </c>
       <c r="F238" t="s">
-        <v>1021</v>
+        <v>978</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>1022</v>
+        <v>979</v>
       </c>
       <c r="B239">
         <v>26</v>
       </c>
       <c r="C239" t="s">
-        <v>1023</v>
+        <v>980</v>
       </c>
       <c r="D239" t="s">
-        <v>1024</v>
+        <v>981</v>
       </c>
       <c r="E239" t="s">
-        <v>1025</v>
+        <v>982</v>
       </c>
       <c r="F239" t="s">
         <v>911</v>
@@ -10144,19 +10861,19 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>1026</v>
+        <v>983</v>
       </c>
       <c r="B240">
         <v>26</v>
       </c>
       <c r="C240" t="s">
-        <v>447</v>
+        <v>984</v>
       </c>
       <c r="D240" t="s">
-        <v>1027</v>
+        <v>985</v>
       </c>
       <c r="E240" t="s">
-        <v>1028</v>
+        <v>986</v>
       </c>
       <c r="F240" t="s">
         <v>911</v>
@@ -10164,39 +10881,39 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>1029</v>
+        <v>987</v>
       </c>
       <c r="B241">
         <v>26</v>
       </c>
       <c r="C241" t="s">
-        <v>1030</v>
+        <v>988</v>
       </c>
       <c r="D241" t="s">
-        <v>1031</v>
+        <v>989</v>
       </c>
       <c r="E241" t="s">
-        <v>1032</v>
+        <v>990</v>
       </c>
       <c r="F241" t="s">
-        <v>911</v>
+        <v>991</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>1033</v>
+        <v>992</v>
       </c>
       <c r="B242">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C242" t="s">
-        <v>1034</v>
+        <v>993</v>
       </c>
       <c r="D242" t="s">
-        <v>1035</v>
+        <v>994</v>
       </c>
       <c r="E242" t="s">
-        <v>1036</v>
+        <v>995</v>
       </c>
       <c r="F242" t="s">
         <v>911</v>
@@ -10204,19 +10921,19 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>1037</v>
+        <v>996</v>
       </c>
       <c r="B243">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C243" t="s">
-        <v>1038</v>
+        <v>997</v>
       </c>
       <c r="D243" t="s">
-        <v>1039</v>
+        <v>998</v>
       </c>
       <c r="E243" t="s">
-        <v>1040</v>
+        <v>999</v>
       </c>
       <c r="F243" t="s">
         <v>911</v>
@@ -10224,19 +10941,19 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>1041</v>
+        <v>1000</v>
       </c>
       <c r="B244">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C244" t="s">
-        <v>1042</v>
+        <v>1001</v>
       </c>
       <c r="D244" t="s">
-        <v>1043</v>
+        <v>1002</v>
       </c>
       <c r="E244" t="s">
-        <v>1044</v>
+        <v>1003</v>
       </c>
       <c r="F244" t="s">
         <v>911</v>
@@ -10244,19 +10961,19 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>1045</v>
+        <v>1004</v>
       </c>
       <c r="B245">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C245" t="s">
-        <v>1046</v>
+        <v>1005</v>
       </c>
       <c r="D245" t="s">
-        <v>1047</v>
+        <v>1006</v>
       </c>
       <c r="E245" t="s">
-        <v>1048</v>
+        <v>1007</v>
       </c>
       <c r="F245" t="s">
         <v>911</v>
@@ -10264,19 +10981,19 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>1049</v>
+        <v>1008</v>
       </c>
       <c r="B246">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C246" t="s">
-        <v>1050</v>
+        <v>1009</v>
       </c>
       <c r="D246" t="s">
-        <v>1051</v>
+        <v>1010</v>
       </c>
       <c r="E246" t="s">
-        <v>1052</v>
+        <v>1011</v>
       </c>
       <c r="F246" t="s">
         <v>911</v>
@@ -10284,79 +11001,79 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>1053</v>
+        <v>1012</v>
       </c>
       <c r="B247">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C247" t="s">
-        <v>1054</v>
+        <v>1013</v>
       </c>
       <c r="D247" t="s">
-        <v>1055</v>
+        <v>1014</v>
       </c>
       <c r="E247" t="s">
-        <v>1056</v>
+        <v>1015</v>
       </c>
       <c r="F247" t="s">
-        <v>911</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>1057</v>
+        <v>1017</v>
       </c>
       <c r="B248">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C248" t="s">
-        <v>1058</v>
+        <v>1018</v>
       </c>
       <c r="D248" t="s">
-        <v>1059</v>
+        <v>1019</v>
       </c>
       <c r="E248" t="s">
-        <v>1060</v>
+        <v>1020</v>
       </c>
       <c r="F248" t="s">
-        <v>1061</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>1062</v>
+        <v>1022</v>
       </c>
       <c r="B249">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C249" t="s">
-        <v>1063</v>
+        <v>1023</v>
       </c>
       <c r="D249" t="s">
-        <v>1064</v>
+        <v>1024</v>
       </c>
       <c r="E249" t="s">
-        <v>1065</v>
+        <v>1025</v>
       </c>
       <c r="F249" t="s">
-        <v>1066</v>
+        <v>911</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>1067</v>
+        <v>1026</v>
       </c>
       <c r="B250">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C250" t="s">
-        <v>1068</v>
+        <v>447</v>
       </c>
       <c r="D250" t="s">
-        <v>1069</v>
+        <v>1027</v>
       </c>
       <c r="E250" t="s">
-        <v>1070</v>
+        <v>1028</v>
       </c>
       <c r="F250" t="s">
         <v>911</v>
@@ -10364,1612 +11081,1812 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>1071</v>
+        <v>1029</v>
       </c>
       <c r="B251">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C251" t="s">
-        <v>1072</v>
+        <v>1030</v>
       </c>
       <c r="D251" t="s">
-        <v>1073</v>
+        <v>1031</v>
       </c>
       <c r="E251" t="s">
-        <v>1074</v>
+        <v>1032</v>
       </c>
       <c r="F251" t="s">
-        <v>1075</v>
+        <v>911</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>1076</v>
+        <v>1033</v>
       </c>
       <c r="B252">
         <v>27</v>
       </c>
       <c r="C252" t="s">
-        <v>1077</v>
+        <v>1034</v>
       </c>
       <c r="D252" t="s">
-        <v>1078</v>
+        <v>1035</v>
       </c>
       <c r="E252" t="s">
-        <v>1079</v>
+        <v>1036</v>
       </c>
       <c r="F252" t="s">
-        <v>1080</v>
+        <v>911</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>1081</v>
+        <v>1037</v>
       </c>
       <c r="B253">
         <v>27</v>
       </c>
       <c r="C253" t="s">
-        <v>1082</v>
+        <v>1038</v>
       </c>
       <c r="D253" t="s">
-        <v>1083</v>
+        <v>1039</v>
       </c>
       <c r="E253" t="s">
-        <v>1084</v>
+        <v>1040</v>
       </c>
       <c r="F253" t="s">
-        <v>1085</v>
+        <v>911</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>1086</v>
+        <v>1041</v>
       </c>
       <c r="B254">
         <v>27</v>
       </c>
       <c r="C254" t="s">
-        <v>1087</v>
+        <v>1042</v>
       </c>
       <c r="D254" t="s">
-        <v>1088</v>
+        <v>1043</v>
       </c>
       <c r="E254" t="s">
-        <v>1089</v>
+        <v>1044</v>
       </c>
       <c r="F254" t="s">
-        <v>1090</v>
+        <v>911</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>1091</v>
+        <v>1045</v>
       </c>
       <c r="B255">
         <v>27</v>
       </c>
       <c r="C255" t="s">
-        <v>1092</v>
+        <v>1046</v>
       </c>
       <c r="D255" t="s">
-        <v>1093</v>
+        <v>1047</v>
       </c>
       <c r="E255" t="s">
-        <v>1094</v>
+        <v>1048</v>
       </c>
       <c r="F255" t="s">
-        <v>1095</v>
+        <v>911</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>1096</v>
+        <v>1049</v>
       </c>
       <c r="B256">
         <v>27</v>
       </c>
       <c r="C256" t="s">
-        <v>1097</v>
+        <v>1050</v>
       </c>
       <c r="D256" t="s">
-        <v>1098</v>
+        <v>1051</v>
       </c>
       <c r="E256" t="s">
-        <v>1099</v>
+        <v>1052</v>
       </c>
       <c r="F256" t="s">
-        <v>1100</v>
+        <v>911</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>1101</v>
+        <v>1053</v>
       </c>
       <c r="B257">
         <v>27</v>
       </c>
       <c r="C257" t="s">
-        <v>1102</v>
+        <v>1054</v>
       </c>
       <c r="D257" t="s">
-        <v>1103</v>
+        <v>1055</v>
       </c>
       <c r="E257" t="s">
-        <v>1104</v>
+        <v>1056</v>
       </c>
       <c r="F257" t="s">
-        <v>1105</v>
+        <v>911</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>1106</v>
+        <v>1057</v>
       </c>
       <c r="B258">
         <v>27</v>
       </c>
       <c r="C258" t="s">
-        <v>1107</v>
+        <v>1058</v>
       </c>
       <c r="D258" t="s">
-        <v>1108</v>
+        <v>1059</v>
       </c>
       <c r="E258" t="s">
-        <v>1109</v>
+        <v>1060</v>
       </c>
       <c r="F258" t="s">
-        <v>1110</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>1111</v>
+        <v>1062</v>
       </c>
       <c r="B259">
         <v>27</v>
       </c>
       <c r="C259" t="s">
-        <v>1112</v>
+        <v>1063</v>
       </c>
       <c r="D259" t="s">
-        <v>1113</v>
+        <v>1064</v>
       </c>
       <c r="E259" t="s">
-        <v>1114</v>
+        <v>1065</v>
       </c>
       <c r="F259" t="s">
-        <v>1115</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>1116</v>
+        <v>1067</v>
       </c>
       <c r="B260">
         <v>27</v>
       </c>
       <c r="C260" t="s">
-        <v>1117</v>
+        <v>1068</v>
       </c>
       <c r="D260" t="s">
-        <v>1118</v>
+        <v>1069</v>
       </c>
       <c r="E260" t="s">
-        <v>1119</v>
+        <v>1070</v>
       </c>
       <c r="F260" t="s">
-        <v>1120</v>
+        <v>911</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>1121</v>
+        <v>1071</v>
       </c>
       <c r="B261">
         <v>27</v>
       </c>
       <c r="C261" t="s">
-        <v>1122</v>
+        <v>1072</v>
       </c>
       <c r="D261" t="s">
-        <v>1123</v>
+        <v>1073</v>
       </c>
       <c r="E261" t="s">
-        <v>1124</v>
+        <v>1074</v>
       </c>
       <c r="F261" t="s">
-        <v>1125</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>1126</v>
+        <v>1076</v>
       </c>
       <c r="B262">
         <v>27</v>
       </c>
       <c r="C262" t="s">
-        <v>1127</v>
+        <v>1077</v>
       </c>
       <c r="D262" t="s">
-        <v>1128</v>
+        <v>1078</v>
       </c>
       <c r="E262" t="s">
-        <v>1129</v>
+        <v>1079</v>
       </c>
       <c r="F262" t="s">
-        <v>1130</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>1131</v>
+        <v>1081</v>
       </c>
       <c r="B263">
         <v>27</v>
       </c>
       <c r="C263" t="s">
-        <v>1132</v>
+        <v>1082</v>
       </c>
       <c r="D263" t="s">
-        <v>1133</v>
+        <v>1083</v>
       </c>
       <c r="E263" t="s">
-        <v>1134</v>
+        <v>1084</v>
       </c>
       <c r="F263" t="s">
-        <v>1135</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>1136</v>
+        <v>1086</v>
       </c>
       <c r="B264">
         <v>27</v>
       </c>
       <c r="C264" t="s">
-        <v>1137</v>
+        <v>1087</v>
       </c>
       <c r="D264" t="s">
-        <v>1138</v>
+        <v>1088</v>
       </c>
       <c r="E264" t="s">
-        <v>1139</v>
+        <v>1089</v>
       </c>
       <c r="F264" t="s">
-        <v>1140</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>1141</v>
+        <v>1091</v>
       </c>
       <c r="B265">
         <v>27</v>
       </c>
       <c r="C265" t="s">
-        <v>1142</v>
+        <v>1092</v>
       </c>
       <c r="D265" t="s">
-        <v>1143</v>
+        <v>1093</v>
       </c>
       <c r="E265" t="s">
-        <v>1144</v>
+        <v>1094</v>
       </c>
       <c r="F265" t="s">
-        <v>1145</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>1146</v>
+        <v>1096</v>
       </c>
       <c r="B266">
         <v>27</v>
       </c>
       <c r="C266" t="s">
-        <v>1147</v>
+        <v>1097</v>
       </c>
       <c r="D266" t="s">
-        <v>1148</v>
+        <v>1098</v>
       </c>
       <c r="E266" t="s">
-        <v>1149</v>
+        <v>1099</v>
       </c>
       <c r="F266" t="s">
-        <v>1150</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>1151</v>
+        <v>1101</v>
       </c>
       <c r="B267">
         <v>27</v>
       </c>
       <c r="C267" t="s">
-        <v>1152</v>
+        <v>1102</v>
       </c>
       <c r="D267" t="s">
-        <v>1153</v>
+        <v>1103</v>
       </c>
       <c r="E267" t="s">
-        <v>1154</v>
+        <v>1104</v>
       </c>
       <c r="F267" t="s">
-        <v>1155</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>1156</v>
+        <v>1106</v>
       </c>
       <c r="B268">
         <v>27</v>
       </c>
       <c r="C268" t="s">
-        <v>1157</v>
+        <v>1107</v>
       </c>
       <c r="D268" t="s">
-        <v>1158</v>
+        <v>1108</v>
       </c>
       <c r="E268" t="s">
-        <v>1159</v>
+        <v>1109</v>
       </c>
       <c r="F268" t="s">
-        <v>1160</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>1161</v>
+        <v>1111</v>
       </c>
       <c r="B269">
         <v>27</v>
       </c>
       <c r="C269" t="s">
-        <v>1162</v>
+        <v>1112</v>
       </c>
       <c r="D269" t="s">
-        <v>1163</v>
+        <v>1113</v>
       </c>
       <c r="E269" t="s">
-        <v>1164</v>
+        <v>1114</v>
       </c>
       <c r="F269" t="s">
-        <v>1165</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>1166</v>
+        <v>1116</v>
       </c>
       <c r="B270">
         <v>27</v>
       </c>
       <c r="C270" t="s">
-        <v>1162</v>
+        <v>1117</v>
       </c>
       <c r="D270" t="s">
-        <v>1167</v>
+        <v>1118</v>
       </c>
       <c r="E270" t="s">
-        <v>1168</v>
+        <v>1119</v>
       </c>
       <c r="F270" t="s">
-        <v>1169</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>1170</v>
+        <v>1121</v>
       </c>
       <c r="B271">
         <v>27</v>
       </c>
       <c r="C271" t="s">
-        <v>1171</v>
+        <v>1122</v>
       </c>
       <c r="D271" t="s">
-        <v>1172</v>
+        <v>1123</v>
       </c>
       <c r="E271" t="s">
-        <v>1173</v>
+        <v>1124</v>
       </c>
       <c r="F271" t="s">
-        <v>1174</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>1175</v>
+        <v>1126</v>
       </c>
       <c r="B272">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C272" t="s">
-        <v>1176</v>
+        <v>1127</v>
       </c>
       <c r="D272" t="s">
-        <v>1177</v>
+        <v>1128</v>
       </c>
       <c r="E272" t="s">
-        <v>1178</v>
+        <v>1129</v>
       </c>
       <c r="F272" t="s">
-        <v>1179</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>1180</v>
+        <v>1131</v>
       </c>
       <c r="B273">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C273" t="s">
-        <v>1181</v>
+        <v>1132</v>
       </c>
       <c r="D273" t="s">
-        <v>1182</v>
+        <v>1133</v>
       </c>
       <c r="E273" t="s">
-        <v>1183</v>
+        <v>1134</v>
       </c>
       <c r="F273" t="s">
-        <v>1184</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>1185</v>
+        <v>1136</v>
       </c>
       <c r="B274">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C274" t="s">
-        <v>1186</v>
+        <v>1137</v>
       </c>
       <c r="D274" t="s">
-        <v>1187</v>
+        <v>1138</v>
       </c>
       <c r="E274" t="s">
-        <v>1188</v>
+        <v>1139</v>
       </c>
       <c r="F274" t="s">
-        <v>1189</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>1190</v>
+        <v>1141</v>
       </c>
       <c r="B275">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C275" t="s">
-        <v>1191</v>
+        <v>1142</v>
       </c>
       <c r="D275" t="s">
-        <v>1192</v>
+        <v>1143</v>
       </c>
       <c r="E275" t="s">
-        <v>1193</v>
+        <v>1144</v>
       </c>
       <c r="F275" t="s">
-        <v>1194</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>1195</v>
+        <v>1146</v>
       </c>
       <c r="B276">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C276" t="s">
-        <v>1196</v>
+        <v>1147</v>
       </c>
       <c r="D276" t="s">
-        <v>1197</v>
+        <v>1148</v>
       </c>
       <c r="E276" t="s">
-        <v>1198</v>
+        <v>1149</v>
       </c>
       <c r="F276" t="s">
-        <v>1199</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>1200</v>
+        <v>1151</v>
       </c>
       <c r="B277">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C277" t="s">
-        <v>1201</v>
+        <v>1152</v>
       </c>
       <c r="D277" t="s">
-        <v>1202</v>
+        <v>1153</v>
       </c>
       <c r="E277" t="s">
-        <v>1203</v>
+        <v>1154</v>
       </c>
       <c r="F277" t="s">
-        <v>1204</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>1205</v>
+        <v>1156</v>
       </c>
       <c r="B278">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C278" t="s">
-        <v>1206</v>
+        <v>1157</v>
       </c>
       <c r="D278" t="s">
-        <v>1207</v>
+        <v>1158</v>
       </c>
       <c r="E278" t="s">
-        <v>1208</v>
+        <v>1159</v>
       </c>
       <c r="F278" t="s">
-        <v>1209</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>1210</v>
+        <v>1161</v>
       </c>
       <c r="B279">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C279" t="s">
-        <v>1211</v>
+        <v>1162</v>
       </c>
       <c r="D279" t="s">
-        <v>1212</v>
+        <v>1163</v>
       </c>
       <c r="E279" t="s">
-        <v>1213</v>
+        <v>1164</v>
       </c>
       <c r="F279" t="s">
-        <v>1214</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>1215</v>
+        <v>1166</v>
       </c>
       <c r="B280">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C280" t="s">
-        <v>1216</v>
+        <v>1162</v>
       </c>
       <c r="D280" t="s">
-        <v>1217</v>
+        <v>1167</v>
       </c>
       <c r="E280" t="s">
-        <v>1218</v>
+        <v>1168</v>
       </c>
       <c r="F280" t="s">
-        <v>1219</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>1220</v>
+        <v>1170</v>
       </c>
       <c r="B281">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C281" t="s">
-        <v>1221</v>
+        <v>1171</v>
       </c>
       <c r="D281" t="s">
-        <v>1222</v>
+        <v>1172</v>
       </c>
       <c r="E281" t="s">
-        <v>1223</v>
+        <v>1173</v>
       </c>
       <c r="F281" t="s">
-        <v>1224</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>1225</v>
+        <v>1175</v>
       </c>
       <c r="B282">
         <v>28</v>
       </c>
       <c r="C282" t="s">
-        <v>1226</v>
+        <v>1176</v>
       </c>
       <c r="D282" t="s">
-        <v>1227</v>
+        <v>1177</v>
       </c>
       <c r="E282" t="s">
-        <v>1228</v>
+        <v>1178</v>
       </c>
       <c r="F282" t="s">
-        <v>1229</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>1230</v>
+        <v>1180</v>
       </c>
       <c r="B283">
         <v>28</v>
       </c>
       <c r="C283" t="s">
-        <v>1231</v>
+        <v>1181</v>
       </c>
       <c r="D283" t="s">
-        <v>1232</v>
+        <v>1182</v>
+      </c>
+      <c r="E283" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F283" t="s">
+        <v>1184</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>1233</v>
+        <v>1185</v>
       </c>
       <c r="B284">
         <v>28</v>
       </c>
       <c r="C284" t="s">
-        <v>1234</v>
+        <v>1186</v>
       </c>
       <c r="D284" t="s">
-        <v>1235</v>
+        <v>1187</v>
       </c>
       <c r="E284" t="s">
-        <v>1236</v>
+        <v>1188</v>
       </c>
       <c r="F284" t="s">
-        <v>1237</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>1238</v>
+        <v>1190</v>
       </c>
       <c r="B285">
         <v>28</v>
       </c>
       <c r="C285" t="s">
-        <v>1239</v>
+        <v>1191</v>
       </c>
       <c r="D285" t="s">
-        <v>1240</v>
+        <v>1192</v>
       </c>
       <c r="E285" t="s">
-        <v>1241</v>
+        <v>1193</v>
       </c>
       <c r="F285" t="s">
-        <v>1242</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>1243</v>
+        <v>1195</v>
       </c>
       <c r="B286">
         <v>28</v>
       </c>
       <c r="C286" t="s">
-        <v>1244</v>
+        <v>1196</v>
       </c>
       <c r="D286" t="s">
-        <v>1245</v>
+        <v>1197</v>
       </c>
       <c r="E286" t="s">
-        <v>1246</v>
+        <v>1198</v>
       </c>
       <c r="F286" t="s">
-        <v>1247</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>1248</v>
+        <v>1200</v>
       </c>
       <c r="B287">
         <v>28</v>
       </c>
       <c r="C287" t="s">
-        <v>908</v>
+        <v>1201</v>
       </c>
       <c r="D287" t="s">
-        <v>1249</v>
+        <v>1202</v>
       </c>
       <c r="E287" t="s">
-        <v>1250</v>
+        <v>1203</v>
       </c>
       <c r="F287" t="s">
-        <v>1251</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>1252</v>
+        <v>1205</v>
       </c>
       <c r="B288">
         <v>28</v>
       </c>
       <c r="C288" t="s">
-        <v>1253</v>
+        <v>1206</v>
       </c>
       <c r="D288" t="s">
-        <v>1254</v>
+        <v>1207</v>
       </c>
       <c r="E288" t="s">
-        <v>1255</v>
+        <v>1208</v>
+      </c>
+      <c r="F288" t="s">
+        <v>1209</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>1256</v>
+        <v>1210</v>
       </c>
       <c r="B289">
         <v>28</v>
       </c>
       <c r="C289" t="s">
-        <v>1257</v>
+        <v>1211</v>
       </c>
       <c r="D289" t="s">
-        <v>1258</v>
+        <v>1212</v>
       </c>
       <c r="E289" t="s">
-        <v>1259</v>
+        <v>1213</v>
       </c>
       <c r="F289" t="s">
-        <v>1260</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>1261</v>
+        <v>1215</v>
       </c>
       <c r="B290">
         <v>28</v>
       </c>
       <c r="C290" t="s">
-        <v>1262</v>
+        <v>1216</v>
       </c>
       <c r="D290" t="s">
-        <v>1263</v>
+        <v>1217</v>
       </c>
       <c r="E290" t="s">
-        <v>1264</v>
+        <v>1218</v>
       </c>
       <c r="F290" t="s">
-        <v>1265</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>1266</v>
+        <v>1220</v>
       </c>
       <c r="B291">
         <v>28</v>
       </c>
       <c r="C291" t="s">
-        <v>1267</v>
+        <v>1221</v>
       </c>
       <c r="D291" t="s">
-        <v>1268</v>
+        <v>1222</v>
       </c>
       <c r="E291" t="s">
-        <v>1269</v>
+        <v>1223</v>
       </c>
       <c r="F291" t="s">
-        <v>1270</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>1271</v>
+        <v>1225</v>
       </c>
       <c r="B292">
         <v>28</v>
       </c>
       <c r="C292" t="s">
-        <v>1272</v>
+        <v>1226</v>
       </c>
       <c r="D292" t="s">
-        <v>1273</v>
+        <v>1227</v>
       </c>
       <c r="E292" t="s">
-        <v>1274</v>
+        <v>1228</v>
       </c>
       <c r="F292" t="s">
-        <v>1275</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>1276</v>
+        <v>1230</v>
       </c>
       <c r="B293">
         <v>28</v>
       </c>
       <c r="C293" t="s">
-        <v>1277</v>
+        <v>1231</v>
       </c>
       <c r="D293" t="s">
-        <v>1278</v>
-      </c>
-      <c r="E293" t="s">
-        <v>1279</v>
-      </c>
-      <c r="F293" t="s">
-        <v>1280</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>1281</v>
+        <v>1233</v>
       </c>
       <c r="B294">
         <v>28</v>
       </c>
       <c r="C294" t="s">
-        <v>1282</v>
+        <v>1234</v>
       </c>
       <c r="D294" t="s">
-        <v>1283</v>
+        <v>1235</v>
       </c>
       <c r="E294" t="s">
-        <v>1284</v>
+        <v>1236</v>
       </c>
       <c r="F294" t="s">
-        <v>1285</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>1286</v>
+        <v>1238</v>
       </c>
       <c r="B295">
         <v>28</v>
       </c>
       <c r="C295" t="s">
-        <v>1287</v>
+        <v>1239</v>
       </c>
       <c r="D295" t="s">
-        <v>1288</v>
+        <v>1240</v>
       </c>
       <c r="E295" t="s">
-        <v>1289</v>
+        <v>1241</v>
       </c>
       <c r="F295" t="s">
-        <v>1290</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>1291</v>
+        <v>1243</v>
       </c>
       <c r="B296">
         <v>28</v>
       </c>
       <c r="C296" t="s">
-        <v>1292</v>
+        <v>1244</v>
       </c>
       <c r="D296" t="s">
-        <v>1293</v>
+        <v>1245</v>
       </c>
       <c r="E296" t="s">
-        <v>1294</v>
+        <v>1246</v>
       </c>
       <c r="F296" t="s">
-        <v>1295</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>1296</v>
+        <v>1248</v>
       </c>
       <c r="B297">
         <v>28</v>
       </c>
       <c r="C297" t="s">
-        <v>1297</v>
+        <v>908</v>
       </c>
       <c r="D297" t="s">
-        <v>1298</v>
+        <v>1249</v>
       </c>
       <c r="E297" t="s">
-        <v>1299</v>
+        <v>1250</v>
       </c>
       <c r="F297" t="s">
-        <v>1300</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>1301</v>
+        <v>1252</v>
       </c>
       <c r="B298">
         <v>28</v>
       </c>
       <c r="C298" t="s">
-        <v>1302</v>
+        <v>1253</v>
       </c>
       <c r="D298" t="s">
-        <v>1303</v>
+        <v>1254</v>
       </c>
       <c r="E298" t="s">
-        <v>1304</v>
-      </c>
-      <c r="F298" t="s">
-        <v>1305</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>1306</v>
+        <v>1256</v>
       </c>
       <c r="B299">
         <v>28</v>
       </c>
       <c r="C299" t="s">
-        <v>1307</v>
+        <v>1257</v>
       </c>
       <c r="D299" t="s">
-        <v>1308</v>
+        <v>1258</v>
       </c>
       <c r="E299" t="s">
-        <v>1309</v>
+        <v>1259</v>
       </c>
       <c r="F299" t="s">
-        <v>1310</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>1311</v>
+        <v>1261</v>
       </c>
       <c r="B300">
         <v>28</v>
       </c>
       <c r="C300" t="s">
-        <v>1312</v>
+        <v>1262</v>
       </c>
       <c r="D300" t="s">
-        <v>1313</v>
+        <v>1263</v>
       </c>
       <c r="E300" t="s">
-        <v>1314</v>
+        <v>1264</v>
       </c>
       <c r="F300" t="s">
-        <v>1315</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>1316</v>
+        <v>1266</v>
       </c>
       <c r="B301">
         <v>28</v>
       </c>
       <c r="C301" t="s">
-        <v>1317</v>
+        <v>1267</v>
       </c>
       <c r="D301" t="s">
-        <v>1318</v>
+        <v>1268</v>
       </c>
       <c r="E301" t="s">
-        <v>1319</v>
+        <v>1269</v>
       </c>
       <c r="F301" t="s">
-        <v>1320</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>1321</v>
+        <v>1271</v>
       </c>
       <c r="B302">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C302" t="s">
-        <v>1322</v>
+        <v>1272</v>
       </c>
       <c r="D302" t="s">
-        <v>1323</v>
+        <v>1273</v>
       </c>
       <c r="E302" t="s">
-        <v>1324</v>
+        <v>1274</v>
       </c>
       <c r="F302" t="s">
-        <v>1325</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>1326</v>
+        <v>1276</v>
       </c>
       <c r="B303">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C303" t="s">
-        <v>1327</v>
+        <v>1277</v>
       </c>
       <c r="D303" t="s">
-        <v>1328</v>
+        <v>1278</v>
       </c>
       <c r="E303" t="s">
-        <v>1329</v>
+        <v>1279</v>
       </c>
       <c r="F303" t="s">
-        <v>1330</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>1331</v>
+        <v>1281</v>
       </c>
       <c r="B304">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C304" t="s">
-        <v>1332</v>
+        <v>1282</v>
       </c>
       <c r="D304" t="s">
-        <v>1333</v>
+        <v>1283</v>
       </c>
       <c r="E304" t="s">
-        <v>1334</v>
+        <v>1284</v>
       </c>
       <c r="F304" t="s">
-        <v>1335</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>1336</v>
+        <v>1286</v>
       </c>
       <c r="B305">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C305" t="s">
-        <v>1337</v>
+        <v>1287</v>
       </c>
       <c r="D305" t="s">
-        <v>1338</v>
+        <v>1288</v>
       </c>
       <c r="E305" t="s">
-        <v>1339</v>
+        <v>1289</v>
       </c>
       <c r="F305" t="s">
-        <v>1340</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>1341</v>
+        <v>1291</v>
       </c>
       <c r="B306">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C306" t="s">
-        <v>1342</v>
+        <v>1292</v>
       </c>
       <c r="D306" t="s">
-        <v>1343</v>
+        <v>1293</v>
       </c>
       <c r="E306" t="s">
-        <v>1344</v>
+        <v>1294</v>
       </c>
       <c r="F306" t="s">
-        <v>1345</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>1346</v>
+        <v>1296</v>
       </c>
       <c r="B307">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C307" t="s">
-        <v>1347</v>
+        <v>1297</v>
       </c>
       <c r="D307" t="s">
-        <v>1348</v>
+        <v>1298</v>
       </c>
       <c r="E307" t="s">
-        <v>1349</v>
+        <v>1299</v>
       </c>
       <c r="F307" t="s">
-        <v>1350</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>1351</v>
+        <v>1301</v>
       </c>
       <c r="B308">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C308" t="s">
-        <v>1352</v>
+        <v>1302</v>
       </c>
       <c r="D308" t="s">
-        <v>1353</v>
+        <v>1303</v>
       </c>
       <c r="E308" t="s">
-        <v>1354</v>
+        <v>1304</v>
       </c>
       <c r="F308" t="s">
-        <v>1355</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>1356</v>
+        <v>1306</v>
       </c>
       <c r="B309">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C309" t="s">
-        <v>1357</v>
+        <v>1307</v>
       </c>
       <c r="D309" t="s">
-        <v>1358</v>
+        <v>1308</v>
       </c>
       <c r="E309" t="s">
-        <v>1359</v>
+        <v>1309</v>
       </c>
       <c r="F309" t="s">
-        <v>1360</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>1361</v>
+        <v>1311</v>
       </c>
       <c r="B310">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C310" t="s">
-        <v>1362</v>
+        <v>1312</v>
       </c>
       <c r="D310" t="s">
-        <v>1363</v>
+        <v>1313</v>
       </c>
       <c r="E310" t="s">
-        <v>1364</v>
+        <v>1314</v>
       </c>
       <c r="F310" t="s">
-        <v>1365</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>1366</v>
+        <v>1316</v>
       </c>
       <c r="B311">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C311" t="s">
-        <v>1367</v>
+        <v>1317</v>
       </c>
       <c r="D311" t="s">
-        <v>1368</v>
+        <v>1318</v>
       </c>
       <c r="E311" t="s">
-        <v>1369</v>
+        <v>1319</v>
       </c>
       <c r="F311" t="s">
-        <v>1370</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>1371</v>
+        <v>1321</v>
       </c>
       <c r="B312">
         <v>29</v>
       </c>
       <c r="C312" t="s">
-        <v>1372</v>
+        <v>1322</v>
       </c>
       <c r="D312" t="s">
-        <v>1373</v>
+        <v>1323</v>
       </c>
       <c r="E312" t="s">
-        <v>1374</v>
+        <v>1324</v>
       </c>
       <c r="F312" t="s">
-        <v>1375</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>1376</v>
+        <v>1326</v>
       </c>
       <c r="B313">
         <v>29</v>
       </c>
       <c r="C313" t="s">
-        <v>1377</v>
+        <v>1327</v>
       </c>
       <c r="D313" t="s">
-        <v>1378</v>
+        <v>1328</v>
       </c>
       <c r="E313" t="s">
-        <v>1379</v>
+        <v>1329</v>
       </c>
       <c r="F313" t="s">
-        <v>1380</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>1381</v>
+        <v>1331</v>
       </c>
       <c r="B314">
         <v>29</v>
       </c>
       <c r="C314" t="s">
-        <v>1382</v>
+        <v>1332</v>
       </c>
       <c r="D314" t="s">
-        <v>1383</v>
+        <v>1333</v>
       </c>
       <c r="E314" t="s">
-        <v>1384</v>
+        <v>1334</v>
       </c>
       <c r="F314" t="s">
-        <v>1385</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>1386</v>
+        <v>1336</v>
       </c>
       <c r="B315">
         <v>29</v>
       </c>
       <c r="C315" t="s">
-        <v>1387</v>
+        <v>1337</v>
       </c>
       <c r="D315" t="s">
-        <v>1388</v>
+        <v>1338</v>
       </c>
       <c r="E315" t="s">
-        <v>1389</v>
+        <v>1339</v>
       </c>
       <c r="F315" t="s">
-        <v>1390</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>1391</v>
+        <v>1341</v>
       </c>
       <c r="B316">
         <v>29</v>
       </c>
       <c r="C316" t="s">
-        <v>1392</v>
+        <v>1342</v>
       </c>
       <c r="D316" t="s">
-        <v>1393</v>
+        <v>1343</v>
       </c>
       <c r="E316" t="s">
-        <v>1394</v>
+        <v>1344</v>
       </c>
       <c r="F316" t="s">
-        <v>1395</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>1396</v>
+        <v>1346</v>
       </c>
       <c r="B317">
         <v>29</v>
       </c>
       <c r="C317" t="s">
-        <v>1397</v>
+        <v>1347</v>
       </c>
       <c r="D317" t="s">
-        <v>1398</v>
+        <v>1348</v>
       </c>
       <c r="E317" t="s">
-        <v>1399</v>
+        <v>1349</v>
       </c>
       <c r="F317" t="s">
-        <v>1400</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>1401</v>
+        <v>1351</v>
       </c>
       <c r="B318">
         <v>29</v>
       </c>
       <c r="C318" t="s">
-        <v>1402</v>
+        <v>1352</v>
       </c>
       <c r="D318" t="s">
-        <v>1403</v>
+        <v>1353</v>
       </c>
       <c r="E318" t="s">
-        <v>1404</v>
+        <v>1354</v>
       </c>
       <c r="F318" t="s">
-        <v>1405</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>1406</v>
+        <v>1356</v>
       </c>
       <c r="B319">
         <v>29</v>
       </c>
       <c r="C319" t="s">
-        <v>1407</v>
+        <v>1357</v>
       </c>
       <c r="D319" t="s">
-        <v>1408</v>
+        <v>1358</v>
       </c>
       <c r="E319" t="s">
-        <v>1409</v>
+        <v>1359</v>
       </c>
       <c r="F319" t="s">
-        <v>1410</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>1411</v>
+        <v>1361</v>
       </c>
       <c r="B320">
         <v>29</v>
       </c>
       <c r="C320" t="s">
-        <v>1412</v>
+        <v>1362</v>
       </c>
       <c r="D320" t="s">
-        <v>1413</v>
+        <v>1363</v>
       </c>
       <c r="E320" t="s">
-        <v>1414</v>
+        <v>1364</v>
       </c>
       <c r="F320" t="s">
-        <v>1415</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>1416</v>
+        <v>1366</v>
       </c>
       <c r="B321">
         <v>29</v>
       </c>
       <c r="C321" t="s">
-        <v>1417</v>
+        <v>1367</v>
       </c>
       <c r="D321" t="s">
-        <v>1418</v>
+        <v>1368</v>
       </c>
       <c r="E321" t="s">
-        <v>1419</v>
+        <v>1369</v>
       </c>
       <c r="F321" t="s">
-        <v>1420</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>1421</v>
+        <v>1371</v>
       </c>
       <c r="B322">
         <v>29</v>
       </c>
       <c r="C322" t="s">
-        <v>1422</v>
+        <v>1372</v>
       </c>
       <c r="D322" t="s">
-        <v>1423</v>
+        <v>1373</v>
       </c>
       <c r="E322" t="s">
-        <v>1424</v>
+        <v>1374</v>
       </c>
       <c r="F322" t="s">
-        <v>1425</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>1426</v>
+        <v>1376</v>
       </c>
       <c r="B323">
         <v>29</v>
       </c>
       <c r="C323" t="s">
-        <v>1427</v>
+        <v>1377</v>
       </c>
       <c r="D323" t="s">
-        <v>1428</v>
+        <v>1378</v>
       </c>
       <c r="E323" t="s">
-        <v>1429</v>
+        <v>1379</v>
       </c>
       <c r="F323" t="s">
-        <v>1430</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>1431</v>
+        <v>1381</v>
       </c>
       <c r="B324">
         <v>29</v>
       </c>
       <c r="C324" t="s">
-        <v>1432</v>
+        <v>1382</v>
       </c>
       <c r="D324" t="s">
-        <v>1433</v>
+        <v>1383</v>
       </c>
       <c r="E324" t="s">
-        <v>1434</v>
+        <v>1384</v>
       </c>
       <c r="F324" t="s">
-        <v>1435</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>1436</v>
+        <v>1386</v>
       </c>
       <c r="B325">
         <v>29</v>
       </c>
       <c r="C325" t="s">
-        <v>1437</v>
+        <v>1387</v>
       </c>
       <c r="D325" t="s">
-        <v>1438</v>
+        <v>1388</v>
       </c>
       <c r="E325" t="s">
-        <v>1439</v>
+        <v>1389</v>
       </c>
       <c r="F325" t="s">
-        <v>1440</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>1441</v>
+        <v>1391</v>
       </c>
       <c r="B326">
         <v>29</v>
       </c>
       <c r="C326" t="s">
-        <v>1442</v>
+        <v>1392</v>
       </c>
       <c r="D326" t="s">
-        <v>1443</v>
+        <v>1393</v>
       </c>
       <c r="E326" t="s">
-        <v>1444</v>
+        <v>1394</v>
       </c>
       <c r="F326" t="s">
-        <v>1445</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>1446</v>
+        <v>1396</v>
       </c>
       <c r="B327">
         <v>29</v>
       </c>
       <c r="C327" t="s">
-        <v>1447</v>
+        <v>1397</v>
       </c>
       <c r="D327" t="s">
-        <v>1448</v>
+        <v>1398</v>
       </c>
       <c r="E327" t="s">
-        <v>1449</v>
+        <v>1399</v>
       </c>
       <c r="F327" t="s">
-        <v>1450</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>1451</v>
+        <v>1401</v>
       </c>
       <c r="B328">
         <v>29</v>
       </c>
       <c r="C328" t="s">
-        <v>1452</v>
+        <v>1402</v>
       </c>
       <c r="D328" t="s">
-        <v>1453</v>
+        <v>1403</v>
       </c>
       <c r="E328" t="s">
-        <v>1454</v>
+        <v>1404</v>
       </c>
       <c r="F328" t="s">
-        <v>1455</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>1456</v>
+        <v>1406</v>
       </c>
       <c r="B329">
         <v>29</v>
       </c>
       <c r="C329" t="s">
-        <v>1457</v>
+        <v>1407</v>
       </c>
       <c r="D329" t="s">
-        <v>1458</v>
+        <v>1408</v>
       </c>
       <c r="E329" t="s">
-        <v>1459</v>
+        <v>1409</v>
       </c>
       <c r="F329" t="s">
-        <v>1460</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>1461</v>
+        <v>1411</v>
       </c>
       <c r="B330">
         <v>29</v>
       </c>
       <c r="C330" t="s">
-        <v>1462</v>
+        <v>1412</v>
       </c>
       <c r="D330" t="s">
-        <v>1463</v>
+        <v>1413</v>
       </c>
       <c r="E330" t="s">
-        <v>1464</v>
+        <v>1414</v>
       </c>
       <c r="F330" t="s">
-        <v>1465</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>1466</v>
+        <v>1416</v>
       </c>
       <c r="B331">
         <v>29</v>
       </c>
       <c r="C331" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D331" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E331" t="s">
+        <v>1419</v>
+      </c>
+      <c r="F331" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B332">
+        <v>29</v>
+      </c>
+      <c r="C332" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D332" t="s">
+        <v>1423</v>
+      </c>
+      <c r="E332" t="s">
+        <v>1424</v>
+      </c>
+      <c r="F332" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B333">
+        <v>29</v>
+      </c>
+      <c r="C333" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D333" t="s">
+        <v>1428</v>
+      </c>
+      <c r="E333" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F333" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B334">
+        <v>29</v>
+      </c>
+      <c r="C334" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D334" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E334" t="s">
+        <v>1434</v>
+      </c>
+      <c r="F334" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A335" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B335">
+        <v>29</v>
+      </c>
+      <c r="C335" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D335" t="s">
+        <v>1438</v>
+      </c>
+      <c r="E335" t="s">
+        <v>1439</v>
+      </c>
+      <c r="F335" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A336" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B336">
+        <v>29</v>
+      </c>
+      <c r="C336" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D336" t="s">
+        <v>1443</v>
+      </c>
+      <c r="E336" t="s">
+        <v>1444</v>
+      </c>
+      <c r="F336" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B337">
+        <v>29</v>
+      </c>
+      <c r="C337" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D337" t="s">
+        <v>1448</v>
+      </c>
+      <c r="E337" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F337" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B338">
+        <v>29</v>
+      </c>
+      <c r="C338" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D338" t="s">
+        <v>1453</v>
+      </c>
+      <c r="E338" t="s">
+        <v>1454</v>
+      </c>
+      <c r="F338" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A339" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B339">
+        <v>29</v>
+      </c>
+      <c r="C339" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D339" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E339" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F339" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A340" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B340">
+        <v>29</v>
+      </c>
+      <c r="C340" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D340" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E340" t="s">
+        <v>1464</v>
+      </c>
+      <c r="F340" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A341" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B341">
+        <v>29</v>
+      </c>
+      <c r="C341" t="s">
         <v>1467</v>
       </c>
-      <c r="D331" t="s">
+      <c r="D341" t="s">
         <v>1468</v>
       </c>
-      <c r="E331" t="s">
+      <c r="E341" t="s">
         <v>1469</v>
       </c>
-      <c r="F331" t="s">
+      <c r="F341" t="s">
         <v>1470</v>
       </c>
     </row>
@@ -11977,7 +12894,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A212:G331 A1:B1 D1:G1 A2:G181" numberStoredAsText="1"/>
+    <ignoredError sqref="A222:G341 A1:B1 D1:G1 A2:G181" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -12001,7 +12918,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>67e55b48-7fca-45c8-8ed6-814cbb364d30</v>
+        <v>4da16d99-2110-4bdc-95c0-f300b8a9ce45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add unit 8 some remain  word
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382A33FF-43AD-B04E-99D2-A22F96C920D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A358393-979E-924B-8A0E-D329A49992F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46760" yWindow="-1780" windowWidth="33600" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50340" yWindow="1900" windowWidth="33600" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="1770">
   <si>
     <t>ID</t>
   </si>
@@ -5044,6 +5044,303 @@
   </si>
   <si>
     <t>involve something</t>
+  </si>
+  <si>
+    <t>U08_11</t>
+  </si>
+  <si>
+    <t>U08_12</t>
+  </si>
+  <si>
+    <t>U08_13</t>
+  </si>
+  <si>
+    <t>U08_14</t>
+  </si>
+  <si>
+    <t>U08_15</t>
+  </si>
+  <si>
+    <t>U08_16</t>
+  </si>
+  <si>
+    <t>U08_17</t>
+  </si>
+  <si>
+    <t>U08_18</t>
+  </si>
+  <si>
+    <t>U08_19</t>
+  </si>
+  <si>
+    <t>U08_20</t>
+  </si>
+  <si>
+    <t>U08_21</t>
+  </si>
+  <si>
+    <t>U08_22</t>
+  </si>
+  <si>
+    <t>U08_23</t>
+  </si>
+  <si>
+    <t>U08_24</t>
+  </si>
+  <si>
+    <t>U08_25</t>
+  </si>
+  <si>
+    <t>U08_26</t>
+  </si>
+  <si>
+    <t>U08_27</t>
+  </si>
+  <si>
+    <t>U08_28</t>
+  </si>
+  <si>
+    <t>U08_29</t>
+  </si>
+  <si>
+    <t>U08_30</t>
+  </si>
+  <si>
+    <t>Bài giảng</t>
+  </si>
+  <si>
+    <t>Lecture</t>
+  </si>
+  <si>
+    <t>A professor from harvard is giving a lecture</t>
+  </si>
+  <si>
+    <t>give a lecture</t>
+  </si>
+  <si>
+    <t>Sách giáo khoa</t>
+  </si>
+  <si>
+    <t>Textbook</t>
+  </si>
+  <si>
+    <t>I love reading school textbooks</t>
+  </si>
+  <si>
+    <t>a school textbook</t>
+  </si>
+  <si>
+    <t>Hóa học</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>Why is organic chemistry so difficult?</t>
+  </si>
+  <si>
+    <t>organic chemistry</t>
+  </si>
+  <si>
+    <t>Lịch sử</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Electricity was an important invention in human history</t>
+  </si>
+  <si>
+    <t>in human history</t>
+  </si>
+  <si>
+    <t>Toán</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Our math teacher is quite young</t>
+  </si>
+  <si>
+    <t>a math teacher</t>
+  </si>
+  <si>
+    <t>Vật lý</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>The physics lesson really bores me</t>
+  </si>
+  <si>
+    <t>A physics lesson</t>
+  </si>
+  <si>
+    <t>Môn học</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Math is my favorite subject at school</t>
+  </si>
+  <si>
+    <t>subject at school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Văn học </t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>He is reading a piece of classical literature</t>
+  </si>
+  <si>
+    <t>a piece of literature</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>The topic of our conversation is stress management</t>
+  </si>
+  <si>
+    <t>The topic of conversation</t>
+  </si>
+  <si>
+    <t>Chủ đề</t>
+  </si>
+  <si>
+    <t>Cuối cùng</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>He is in the final year of college</t>
+  </si>
+  <si>
+    <t>final year</t>
+  </si>
+  <si>
+    <t>Vở, sổ</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>I found a personal notebook in the trash</t>
+  </si>
+  <si>
+    <t>a personal notebook</t>
+  </si>
+  <si>
+    <t>Blank</t>
+  </si>
+  <si>
+    <t>Please write your address on the blank page</t>
+  </si>
+  <si>
+    <t>a blank page</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trống </t>
+  </si>
+  <si>
+    <t>Please include your full name in the application</t>
+  </si>
+  <si>
+    <t>include something in something</t>
+  </si>
+  <si>
+    <t>Kỳ học</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>The spring semester usually starts in January</t>
+  </si>
+  <si>
+    <t>The spring semester</t>
+  </si>
+  <si>
+    <t>TÒ mò</t>
+  </si>
+  <si>
+    <t>curious</t>
+  </si>
+  <si>
+    <t>Se is extremely curious about his background</t>
+  </si>
+  <si>
+    <t>curious about something</t>
+  </si>
+  <si>
+    <t>Có thể</t>
+  </si>
+  <si>
+    <t>Possible</t>
+  </si>
+  <si>
+    <t>Is it possible to reschuedule my class?</t>
+  </si>
+  <si>
+    <t>possible to do something</t>
+  </si>
+  <si>
+    <t>Kỳ vọng</t>
+  </si>
+  <si>
+    <t>Expect</t>
+  </si>
+  <si>
+    <t>She expects a present from her boyfriend</t>
+  </si>
+  <si>
+    <t>expect something from somebody</t>
+  </si>
+  <si>
+    <t>Tụt lại phía sau</t>
+  </si>
+  <si>
+    <t>Fall behind</t>
+  </si>
+  <si>
+    <t>She always falls behind everyone in the class</t>
+  </si>
+  <si>
+    <t>fall behind somebody or something</t>
+  </si>
+  <si>
+    <t>Tìm tới</t>
+  </si>
+  <si>
+    <t>Turn to</t>
+  </si>
+  <si>
+    <t>I turn to my classmate for help</t>
+  </si>
+  <si>
+    <t>Turn to somebody to for help</t>
+  </si>
+  <si>
+    <t>Cải thiện</t>
+  </si>
+  <si>
+    <t>Improve</t>
+  </si>
+  <si>
+    <t>I try to improve my pronunciation</t>
+  </si>
+  <si>
+    <t>try to improve something</t>
   </si>
 </sst>
 </file>
@@ -5401,10 +5698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G341"/>
+  <dimension ref="A1:G361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+    <sheetView tabSelected="1" topLeftCell="B218" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G241" sqref="G241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10501,719 +10798,779 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>907</v>
+        <v>1671</v>
       </c>
       <c r="B222">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>908</v>
+        <v>1691</v>
       </c>
       <c r="D222" t="s">
-        <v>909</v>
+        <v>1692</v>
       </c>
       <c r="E222" t="s">
-        <v>910</v>
+        <v>1693</v>
       </c>
       <c r="F222" t="s">
-        <v>911</v>
+        <v>1694</v>
+      </c>
+      <c r="G222" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>912</v>
+        <v>1672</v>
       </c>
       <c r="B223">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>913</v>
+        <v>1695</v>
       </c>
       <c r="D223" t="s">
-        <v>914</v>
+        <v>1696</v>
       </c>
       <c r="E223" t="s">
-        <v>915</v>
+        <v>1697</v>
       </c>
       <c r="F223" t="s">
-        <v>911</v>
+        <v>1698</v>
+      </c>
+      <c r="G223" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>916</v>
+        <v>1673</v>
       </c>
       <c r="B224">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>917</v>
+        <v>1699</v>
       </c>
       <c r="D224" t="s">
-        <v>918</v>
+        <v>1700</v>
       </c>
       <c r="E224" t="s">
-        <v>919</v>
+        <v>1701</v>
       </c>
       <c r="F224" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1702</v>
+      </c>
+      <c r="G224" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>920</v>
+        <v>1674</v>
       </c>
       <c r="B225">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>921</v>
+        <v>1703</v>
       </c>
       <c r="D225" t="s">
-        <v>922</v>
+        <v>1704</v>
       </c>
       <c r="E225" t="s">
-        <v>923</v>
+        <v>1705</v>
       </c>
       <c r="F225" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1706</v>
+      </c>
+      <c r="G225" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>924</v>
+        <v>1675</v>
       </c>
       <c r="B226">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C226" t="s">
-        <v>925</v>
+        <v>1707</v>
       </c>
       <c r="D226" t="s">
-        <v>926</v>
+        <v>1708</v>
       </c>
       <c r="E226" t="s">
-        <v>927</v>
+        <v>1709</v>
       </c>
       <c r="F226" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1710</v>
+      </c>
+      <c r="G226" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>928</v>
+        <v>1676</v>
       </c>
       <c r="B227">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C227" t="s">
-        <v>929</v>
+        <v>1711</v>
       </c>
       <c r="D227" t="s">
-        <v>930</v>
+        <v>1712</v>
       </c>
       <c r="E227" t="s">
-        <v>931</v>
+        <v>1713</v>
       </c>
       <c r="F227" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1714</v>
+      </c>
+      <c r="G227" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>932</v>
+        <v>1677</v>
       </c>
       <c r="B228">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C228" t="s">
-        <v>933</v>
+        <v>1715</v>
       </c>
       <c r="D228" t="s">
-        <v>934</v>
+        <v>1716</v>
       </c>
       <c r="E228" t="s">
-        <v>935</v>
+        <v>1717</v>
       </c>
       <c r="F228" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1718</v>
+      </c>
+      <c r="G228" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>936</v>
+        <v>1678</v>
       </c>
       <c r="B229">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C229" t="s">
-        <v>937</v>
+        <v>1719</v>
       </c>
       <c r="D229" t="s">
-        <v>938</v>
+        <v>1720</v>
       </c>
       <c r="E229" t="s">
-        <v>939</v>
+        <v>1721</v>
       </c>
       <c r="F229" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1722</v>
+      </c>
+      <c r="G229" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>940</v>
+        <v>1679</v>
       </c>
       <c r="B230">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C230" t="s">
-        <v>941</v>
+        <v>1726</v>
       </c>
       <c r="D230" t="s">
-        <v>942</v>
+        <v>1723</v>
       </c>
       <c r="E230" t="s">
-        <v>943</v>
+        <v>1724</v>
       </c>
       <c r="F230" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1725</v>
+      </c>
+      <c r="G230" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>944</v>
+        <v>1680</v>
       </c>
       <c r="B231">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C231" t="s">
-        <v>945</v>
+        <v>1727</v>
       </c>
       <c r="D231" t="s">
-        <v>946</v>
+        <v>1728</v>
       </c>
       <c r="E231" t="s">
-        <v>947</v>
+        <v>1729</v>
       </c>
       <c r="F231" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1730</v>
+      </c>
+      <c r="G231" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>948</v>
+        <v>1681</v>
       </c>
       <c r="B232">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C232" t="s">
-        <v>949</v>
+        <v>1731</v>
       </c>
       <c r="D232" t="s">
-        <v>950</v>
+        <v>1732</v>
       </c>
       <c r="E232" t="s">
-        <v>951</v>
+        <v>1733</v>
       </c>
       <c r="F232" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1734</v>
+      </c>
+      <c r="G232" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>952</v>
+        <v>1682</v>
       </c>
       <c r="B233">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C233" t="s">
-        <v>953</v>
+        <v>1739</v>
       </c>
       <c r="D233" t="s">
-        <v>954</v>
+        <v>1735</v>
       </c>
       <c r="E233" t="s">
-        <v>955</v>
+        <v>1736</v>
       </c>
       <c r="F233" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1737</v>
+      </c>
+      <c r="G233" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>956</v>
+        <v>1683</v>
       </c>
       <c r="B234">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C234" t="s">
-        <v>957</v>
+        <v>1667</v>
       </c>
       <c r="D234" t="s">
-        <v>958</v>
+        <v>1738</v>
       </c>
       <c r="E234" t="s">
-        <v>959</v>
+        <v>1740</v>
       </c>
       <c r="F234" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1741</v>
+      </c>
+      <c r="G234" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>961</v>
+        <v>1684</v>
       </c>
       <c r="B235">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C235" t="s">
-        <v>962</v>
+        <v>1742</v>
       </c>
       <c r="D235" t="s">
-        <v>963</v>
+        <v>1743</v>
       </c>
       <c r="E235" t="s">
-        <v>964</v>
+        <v>1744</v>
       </c>
       <c r="F235" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1745</v>
+      </c>
+      <c r="G235" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>965</v>
+        <v>1685</v>
       </c>
       <c r="B236">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C236" t="s">
-        <v>966</v>
+        <v>1746</v>
       </c>
       <c r="D236" t="s">
-        <v>967</v>
+        <v>1747</v>
       </c>
       <c r="E236" t="s">
-        <v>968</v>
+        <v>1748</v>
       </c>
       <c r="F236" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1749</v>
+      </c>
+      <c r="G236" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>970</v>
+        <v>1686</v>
       </c>
       <c r="B237">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>971</v>
+        <v>1750</v>
       </c>
       <c r="D237" t="s">
-        <v>972</v>
+        <v>1751</v>
       </c>
       <c r="E237" t="s">
-        <v>973</v>
+        <v>1752</v>
       </c>
       <c r="F237" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1753</v>
+      </c>
+      <c r="G237" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>974</v>
+        <v>1687</v>
       </c>
       <c r="B238">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C238" t="s">
-        <v>975</v>
+        <v>1754</v>
       </c>
       <c r="D238" t="s">
-        <v>976</v>
+        <v>1755</v>
       </c>
       <c r="E238" t="s">
-        <v>977</v>
+        <v>1756</v>
       </c>
       <c r="F238" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1757</v>
+      </c>
+      <c r="G238" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>979</v>
+        <v>1688</v>
       </c>
       <c r="B239">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C239" t="s">
-        <v>980</v>
+        <v>1758</v>
       </c>
       <c r="D239" t="s">
-        <v>981</v>
+        <v>1759</v>
       </c>
       <c r="E239" t="s">
-        <v>982</v>
+        <v>1760</v>
       </c>
       <c r="F239" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1761</v>
+      </c>
+      <c r="G239" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>983</v>
+        <v>1689</v>
       </c>
       <c r="B240">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C240" t="s">
-        <v>984</v>
+        <v>1762</v>
       </c>
       <c r="D240" t="s">
-        <v>985</v>
+        <v>1763</v>
       </c>
       <c r="E240" t="s">
-        <v>986</v>
+        <v>1764</v>
       </c>
       <c r="F240" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1765</v>
+      </c>
+      <c r="G240" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>987</v>
+        <v>1690</v>
       </c>
       <c r="B241">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C241" t="s">
-        <v>988</v>
+        <v>1766</v>
       </c>
       <c r="D241" t="s">
-        <v>989</v>
+        <v>1767</v>
       </c>
       <c r="E241" t="s">
-        <v>990</v>
+        <v>1768</v>
       </c>
       <c r="F241" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1769</v>
+      </c>
+      <c r="G241" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>992</v>
+        <v>907</v>
       </c>
       <c r="B242">
         <v>26</v>
       </c>
       <c r="C242" t="s">
-        <v>993</v>
+        <v>908</v>
       </c>
       <c r="D242" t="s">
-        <v>994</v>
+        <v>909</v>
       </c>
       <c r="E242" t="s">
-        <v>995</v>
+        <v>910</v>
       </c>
       <c r="F242" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>996</v>
+        <v>912</v>
       </c>
       <c r="B243">
         <v>26</v>
       </c>
       <c r="C243" t="s">
-        <v>997</v>
+        <v>913</v>
       </c>
       <c r="D243" t="s">
-        <v>998</v>
+        <v>914</v>
       </c>
       <c r="E243" t="s">
-        <v>999</v>
+        <v>915</v>
       </c>
       <c r="F243" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>1000</v>
+        <v>916</v>
       </c>
       <c r="B244">
         <v>26</v>
       </c>
       <c r="C244" t="s">
-        <v>1001</v>
+        <v>917</v>
       </c>
       <c r="D244" t="s">
-        <v>1002</v>
+        <v>918</v>
       </c>
       <c r="E244" t="s">
-        <v>1003</v>
+        <v>919</v>
       </c>
       <c r="F244" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>1004</v>
+        <v>920</v>
       </c>
       <c r="B245">
         <v>26</v>
       </c>
       <c r="C245" t="s">
-        <v>1005</v>
+        <v>921</v>
       </c>
       <c r="D245" t="s">
-        <v>1006</v>
+        <v>922</v>
       </c>
       <c r="E245" t="s">
-        <v>1007</v>
+        <v>923</v>
       </c>
       <c r="F245" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>1008</v>
+        <v>924</v>
       </c>
       <c r="B246">
         <v>26</v>
       </c>
       <c r="C246" t="s">
-        <v>1009</v>
+        <v>925</v>
       </c>
       <c r="D246" t="s">
-        <v>1010</v>
+        <v>926</v>
       </c>
       <c r="E246" t="s">
-        <v>1011</v>
+        <v>927</v>
       </c>
       <c r="F246" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>1012</v>
+        <v>928</v>
       </c>
       <c r="B247">
         <v>26</v>
       </c>
       <c r="C247" t="s">
-        <v>1013</v>
+        <v>929</v>
       </c>
       <c r="D247" t="s">
-        <v>1014</v>
+        <v>930</v>
       </c>
       <c r="E247" t="s">
-        <v>1015</v>
+        <v>931</v>
       </c>
       <c r="F247" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>1017</v>
+        <v>932</v>
       </c>
       <c r="B248">
         <v>26</v>
       </c>
       <c r="C248" t="s">
-        <v>1018</v>
+        <v>933</v>
       </c>
       <c r="D248" t="s">
-        <v>1019</v>
+        <v>934</v>
       </c>
       <c r="E248" t="s">
-        <v>1020</v>
+        <v>935</v>
       </c>
       <c r="F248" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>1022</v>
+        <v>936</v>
       </c>
       <c r="B249">
         <v>26</v>
       </c>
       <c r="C249" t="s">
-        <v>1023</v>
+        <v>937</v>
       </c>
       <c r="D249" t="s">
-        <v>1024</v>
+        <v>938</v>
       </c>
       <c r="E249" t="s">
-        <v>1025</v>
+        <v>939</v>
       </c>
       <c r="F249" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>1026</v>
+        <v>940</v>
       </c>
       <c r="B250">
         <v>26</v>
       </c>
       <c r="C250" t="s">
-        <v>447</v>
+        <v>941</v>
       </c>
       <c r="D250" t="s">
-        <v>1027</v>
+        <v>942</v>
       </c>
       <c r="E250" t="s">
-        <v>1028</v>
+        <v>943</v>
       </c>
       <c r="F250" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>1029</v>
+        <v>944</v>
       </c>
       <c r="B251">
         <v>26</v>
       </c>
       <c r="C251" t="s">
-        <v>1030</v>
+        <v>945</v>
       </c>
       <c r="D251" t="s">
-        <v>1031</v>
+        <v>946</v>
       </c>
       <c r="E251" t="s">
-        <v>1032</v>
+        <v>947</v>
       </c>
       <c r="F251" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>1033</v>
+        <v>948</v>
       </c>
       <c r="B252">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C252" t="s">
-        <v>1034</v>
+        <v>949</v>
       </c>
       <c r="D252" t="s">
-        <v>1035</v>
+        <v>950</v>
       </c>
       <c r="E252" t="s">
-        <v>1036</v>
+        <v>951</v>
       </c>
       <c r="F252" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>1037</v>
+        <v>952</v>
       </c>
       <c r="B253">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C253" t="s">
-        <v>1038</v>
+        <v>953</v>
       </c>
       <c r="D253" t="s">
-        <v>1039</v>
+        <v>954</v>
       </c>
       <c r="E253" t="s">
-        <v>1040</v>
+        <v>955</v>
       </c>
       <c r="F253" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>1041</v>
+        <v>956</v>
       </c>
       <c r="B254">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C254" t="s">
-        <v>1042</v>
+        <v>957</v>
       </c>
       <c r="D254" t="s">
-        <v>1043</v>
+        <v>958</v>
       </c>
       <c r="E254" t="s">
-        <v>1044</v>
+        <v>959</v>
       </c>
       <c r="F254" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>1045</v>
+        <v>961</v>
       </c>
       <c r="B255">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C255" t="s">
-        <v>1046</v>
+        <v>962</v>
       </c>
       <c r="D255" t="s">
-        <v>1047</v>
+        <v>963</v>
       </c>
       <c r="E255" t="s">
-        <v>1048</v>
+        <v>964</v>
       </c>
       <c r="F255" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>1049</v>
+        <v>965</v>
       </c>
       <c r="B256">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C256" t="s">
-        <v>1050</v>
+        <v>966</v>
       </c>
       <c r="D256" t="s">
-        <v>1051</v>
+        <v>967</v>
       </c>
       <c r="E256" t="s">
-        <v>1052</v>
+        <v>968</v>
       </c>
       <c r="F256" t="s">
-        <v>911</v>
+        <v>969</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>1053</v>
+        <v>970</v>
       </c>
       <c r="B257">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C257" t="s">
-        <v>1054</v>
+        <v>971</v>
       </c>
       <c r="D257" t="s">
-        <v>1055</v>
+        <v>972</v>
       </c>
       <c r="E257" t="s">
-        <v>1056</v>
+        <v>973</v>
       </c>
       <c r="F257" t="s">
         <v>911</v>
@@ -11221,59 +11578,59 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>1057</v>
+        <v>974</v>
       </c>
       <c r="B258">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C258" t="s">
-        <v>1058</v>
+        <v>975</v>
       </c>
       <c r="D258" t="s">
-        <v>1059</v>
+        <v>976</v>
       </c>
       <c r="E258" t="s">
-        <v>1060</v>
+        <v>977</v>
       </c>
       <c r="F258" t="s">
-        <v>1061</v>
+        <v>978</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>1062</v>
+        <v>979</v>
       </c>
       <c r="B259">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C259" t="s">
-        <v>1063</v>
+        <v>980</v>
       </c>
       <c r="D259" t="s">
-        <v>1064</v>
+        <v>981</v>
       </c>
       <c r="E259" t="s">
-        <v>1065</v>
+        <v>982</v>
       </c>
       <c r="F259" t="s">
-        <v>1066</v>
+        <v>911</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>1067</v>
+        <v>983</v>
       </c>
       <c r="B260">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C260" t="s">
-        <v>1068</v>
+        <v>984</v>
       </c>
       <c r="D260" t="s">
-        <v>1069</v>
+        <v>985</v>
       </c>
       <c r="E260" t="s">
-        <v>1070</v>
+        <v>986</v>
       </c>
       <c r="F260" t="s">
         <v>911</v>
@@ -11281,1612 +11638,2012 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>1071</v>
+        <v>987</v>
       </c>
       <c r="B261">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C261" t="s">
-        <v>1072</v>
+        <v>988</v>
       </c>
       <c r="D261" t="s">
-        <v>1073</v>
+        <v>989</v>
       </c>
       <c r="E261" t="s">
-        <v>1074</v>
+        <v>990</v>
       </c>
       <c r="F261" t="s">
-        <v>1075</v>
+        <v>991</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>1076</v>
+        <v>992</v>
       </c>
       <c r="B262">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C262" t="s">
-        <v>1077</v>
+        <v>993</v>
       </c>
       <c r="D262" t="s">
-        <v>1078</v>
+        <v>994</v>
       </c>
       <c r="E262" t="s">
-        <v>1079</v>
+        <v>995</v>
       </c>
       <c r="F262" t="s">
-        <v>1080</v>
+        <v>911</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>1081</v>
+        <v>996</v>
       </c>
       <c r="B263">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C263" t="s">
-        <v>1082</v>
+        <v>997</v>
       </c>
       <c r="D263" t="s">
-        <v>1083</v>
+        <v>998</v>
       </c>
       <c r="E263" t="s">
-        <v>1084</v>
+        <v>999</v>
       </c>
       <c r="F263" t="s">
-        <v>1085</v>
+        <v>911</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>1086</v>
+        <v>1000</v>
       </c>
       <c r="B264">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C264" t="s">
-        <v>1087</v>
+        <v>1001</v>
       </c>
       <c r="D264" t="s">
-        <v>1088</v>
+        <v>1002</v>
       </c>
       <c r="E264" t="s">
-        <v>1089</v>
+        <v>1003</v>
       </c>
       <c r="F264" t="s">
-        <v>1090</v>
+        <v>911</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>1091</v>
+        <v>1004</v>
       </c>
       <c r="B265">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C265" t="s">
-        <v>1092</v>
+        <v>1005</v>
       </c>
       <c r="D265" t="s">
-        <v>1093</v>
+        <v>1006</v>
       </c>
       <c r="E265" t="s">
-        <v>1094</v>
+        <v>1007</v>
       </c>
       <c r="F265" t="s">
-        <v>1095</v>
+        <v>911</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>1096</v>
+        <v>1008</v>
       </c>
       <c r="B266">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C266" t="s">
-        <v>1097</v>
+        <v>1009</v>
       </c>
       <c r="D266" t="s">
-        <v>1098</v>
+        <v>1010</v>
       </c>
       <c r="E266" t="s">
-        <v>1099</v>
+        <v>1011</v>
       </c>
       <c r="F266" t="s">
-        <v>1100</v>
+        <v>911</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>1101</v>
+        <v>1012</v>
       </c>
       <c r="B267">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C267" t="s">
-        <v>1102</v>
+        <v>1013</v>
       </c>
       <c r="D267" t="s">
-        <v>1103</v>
+        <v>1014</v>
       </c>
       <c r="E267" t="s">
-        <v>1104</v>
+        <v>1015</v>
       </c>
       <c r="F267" t="s">
-        <v>1105</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>1106</v>
+        <v>1017</v>
       </c>
       <c r="B268">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C268" t="s">
-        <v>1107</v>
+        <v>1018</v>
       </c>
       <c r="D268" t="s">
-        <v>1108</v>
+        <v>1019</v>
       </c>
       <c r="E268" t="s">
-        <v>1109</v>
+        <v>1020</v>
       </c>
       <c r="F268" t="s">
-        <v>1110</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>1111</v>
+        <v>1022</v>
       </c>
       <c r="B269">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C269" t="s">
-        <v>1112</v>
+        <v>1023</v>
       </c>
       <c r="D269" t="s">
-        <v>1113</v>
+        <v>1024</v>
       </c>
       <c r="E269" t="s">
-        <v>1114</v>
+        <v>1025</v>
       </c>
       <c r="F269" t="s">
-        <v>1115</v>
+        <v>911</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>1116</v>
+        <v>1026</v>
       </c>
       <c r="B270">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C270" t="s">
-        <v>1117</v>
+        <v>447</v>
       </c>
       <c r="D270" t="s">
-        <v>1118</v>
+        <v>1027</v>
       </c>
       <c r="E270" t="s">
-        <v>1119</v>
+        <v>1028</v>
       </c>
       <c r="F270" t="s">
-        <v>1120</v>
+        <v>911</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>1121</v>
+        <v>1029</v>
       </c>
       <c r="B271">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C271" t="s">
-        <v>1122</v>
+        <v>1030</v>
       </c>
       <c r="D271" t="s">
-        <v>1123</v>
+        <v>1031</v>
       </c>
       <c r="E271" t="s">
-        <v>1124</v>
+        <v>1032</v>
       </c>
       <c r="F271" t="s">
-        <v>1125</v>
+        <v>911</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>1126</v>
+        <v>1033</v>
       </c>
       <c r="B272">
         <v>27</v>
       </c>
       <c r="C272" t="s">
-        <v>1127</v>
+        <v>1034</v>
       </c>
       <c r="D272" t="s">
-        <v>1128</v>
+        <v>1035</v>
       </c>
       <c r="E272" t="s">
-        <v>1129</v>
+        <v>1036</v>
       </c>
       <c r="F272" t="s">
-        <v>1130</v>
+        <v>911</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>1131</v>
+        <v>1037</v>
       </c>
       <c r="B273">
         <v>27</v>
       </c>
       <c r="C273" t="s">
-        <v>1132</v>
+        <v>1038</v>
       </c>
       <c r="D273" t="s">
-        <v>1133</v>
+        <v>1039</v>
       </c>
       <c r="E273" t="s">
-        <v>1134</v>
+        <v>1040</v>
       </c>
       <c r="F273" t="s">
-        <v>1135</v>
+        <v>911</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>1136</v>
+        <v>1041</v>
       </c>
       <c r="B274">
         <v>27</v>
       </c>
       <c r="C274" t="s">
-        <v>1137</v>
+        <v>1042</v>
       </c>
       <c r="D274" t="s">
-        <v>1138</v>
+        <v>1043</v>
       </c>
       <c r="E274" t="s">
-        <v>1139</v>
+        <v>1044</v>
       </c>
       <c r="F274" t="s">
-        <v>1140</v>
+        <v>911</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>1141</v>
+        <v>1045</v>
       </c>
       <c r="B275">
         <v>27</v>
       </c>
       <c r="C275" t="s">
-        <v>1142</v>
+        <v>1046</v>
       </c>
       <c r="D275" t="s">
-        <v>1143</v>
+        <v>1047</v>
       </c>
       <c r="E275" t="s">
-        <v>1144</v>
+        <v>1048</v>
       </c>
       <c r="F275" t="s">
-        <v>1145</v>
+        <v>911</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>1146</v>
+        <v>1049</v>
       </c>
       <c r="B276">
         <v>27</v>
       </c>
       <c r="C276" t="s">
-        <v>1147</v>
+        <v>1050</v>
       </c>
       <c r="D276" t="s">
-        <v>1148</v>
+        <v>1051</v>
       </c>
       <c r="E276" t="s">
-        <v>1149</v>
+        <v>1052</v>
       </c>
       <c r="F276" t="s">
-        <v>1150</v>
+        <v>911</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>1151</v>
+        <v>1053</v>
       </c>
       <c r="B277">
         <v>27</v>
       </c>
       <c r="C277" t="s">
-        <v>1152</v>
+        <v>1054</v>
       </c>
       <c r="D277" t="s">
-        <v>1153</v>
+        <v>1055</v>
       </c>
       <c r="E277" t="s">
-        <v>1154</v>
+        <v>1056</v>
       </c>
       <c r="F277" t="s">
-        <v>1155</v>
+        <v>911</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>1156</v>
+        <v>1057</v>
       </c>
       <c r="B278">
         <v>27</v>
       </c>
       <c r="C278" t="s">
-        <v>1157</v>
+        <v>1058</v>
       </c>
       <c r="D278" t="s">
-        <v>1158</v>
+        <v>1059</v>
       </c>
       <c r="E278" t="s">
-        <v>1159</v>
+        <v>1060</v>
       </c>
       <c r="F278" t="s">
-        <v>1160</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>1161</v>
+        <v>1062</v>
       </c>
       <c r="B279">
         <v>27</v>
       </c>
       <c r="C279" t="s">
-        <v>1162</v>
+        <v>1063</v>
       </c>
       <c r="D279" t="s">
-        <v>1163</v>
+        <v>1064</v>
       </c>
       <c r="E279" t="s">
-        <v>1164</v>
+        <v>1065</v>
       </c>
       <c r="F279" t="s">
-        <v>1165</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>1166</v>
+        <v>1067</v>
       </c>
       <c r="B280">
         <v>27</v>
       </c>
       <c r="C280" t="s">
-        <v>1162</v>
+        <v>1068</v>
       </c>
       <c r="D280" t="s">
-        <v>1167</v>
+        <v>1069</v>
       </c>
       <c r="E280" t="s">
-        <v>1168</v>
+        <v>1070</v>
       </c>
       <c r="F280" t="s">
-        <v>1169</v>
+        <v>911</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>1170</v>
+        <v>1071</v>
       </c>
       <c r="B281">
         <v>27</v>
       </c>
       <c r="C281" t="s">
-        <v>1171</v>
+        <v>1072</v>
       </c>
       <c r="D281" t="s">
-        <v>1172</v>
+        <v>1073</v>
       </c>
       <c r="E281" t="s">
-        <v>1173</v>
+        <v>1074</v>
       </c>
       <c r="F281" t="s">
-        <v>1174</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>1175</v>
+        <v>1076</v>
       </c>
       <c r="B282">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C282" t="s">
-        <v>1176</v>
+        <v>1077</v>
       </c>
       <c r="D282" t="s">
-        <v>1177</v>
+        <v>1078</v>
       </c>
       <c r="E282" t="s">
-        <v>1178</v>
+        <v>1079</v>
       </c>
       <c r="F282" t="s">
-        <v>1179</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>1180</v>
+        <v>1081</v>
       </c>
       <c r="B283">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C283" t="s">
-        <v>1181</v>
+        <v>1082</v>
       </c>
       <c r="D283" t="s">
-        <v>1182</v>
+        <v>1083</v>
       </c>
       <c r="E283" t="s">
-        <v>1183</v>
+        <v>1084</v>
       </c>
       <c r="F283" t="s">
-        <v>1184</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>1185</v>
+        <v>1086</v>
       </c>
       <c r="B284">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C284" t="s">
-        <v>1186</v>
+        <v>1087</v>
       </c>
       <c r="D284" t="s">
-        <v>1187</v>
+        <v>1088</v>
       </c>
       <c r="E284" t="s">
-        <v>1188</v>
+        <v>1089</v>
       </c>
       <c r="F284" t="s">
-        <v>1189</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>1190</v>
+        <v>1091</v>
       </c>
       <c r="B285">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C285" t="s">
-        <v>1191</v>
+        <v>1092</v>
       </c>
       <c r="D285" t="s">
-        <v>1192</v>
+        <v>1093</v>
       </c>
       <c r="E285" t="s">
-        <v>1193</v>
+        <v>1094</v>
       </c>
       <c r="F285" t="s">
-        <v>1194</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>1195</v>
+        <v>1096</v>
       </c>
       <c r="B286">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C286" t="s">
-        <v>1196</v>
+        <v>1097</v>
       </c>
       <c r="D286" t="s">
-        <v>1197</v>
+        <v>1098</v>
       </c>
       <c r="E286" t="s">
-        <v>1198</v>
+        <v>1099</v>
       </c>
       <c r="F286" t="s">
-        <v>1199</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>1200</v>
+        <v>1101</v>
       </c>
       <c r="B287">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C287" t="s">
-        <v>1201</v>
+        <v>1102</v>
       </c>
       <c r="D287" t="s">
-        <v>1202</v>
+        <v>1103</v>
       </c>
       <c r="E287" t="s">
-        <v>1203</v>
+        <v>1104</v>
       </c>
       <c r="F287" t="s">
-        <v>1204</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>1205</v>
+        <v>1106</v>
       </c>
       <c r="B288">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C288" t="s">
-        <v>1206</v>
+        <v>1107</v>
       </c>
       <c r="D288" t="s">
-        <v>1207</v>
+        <v>1108</v>
       </c>
       <c r="E288" t="s">
-        <v>1208</v>
+        <v>1109</v>
       </c>
       <c r="F288" t="s">
-        <v>1209</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>1210</v>
+        <v>1111</v>
       </c>
       <c r="B289">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C289" t="s">
-        <v>1211</v>
+        <v>1112</v>
       </c>
       <c r="D289" t="s">
-        <v>1212</v>
+        <v>1113</v>
       </c>
       <c r="E289" t="s">
-        <v>1213</v>
+        <v>1114</v>
       </c>
       <c r="F289" t="s">
-        <v>1214</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>1215</v>
+        <v>1116</v>
       </c>
       <c r="B290">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C290" t="s">
-        <v>1216</v>
+        <v>1117</v>
       </c>
       <c r="D290" t="s">
-        <v>1217</v>
+        <v>1118</v>
       </c>
       <c r="E290" t="s">
-        <v>1218</v>
+        <v>1119</v>
       </c>
       <c r="F290" t="s">
-        <v>1219</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>1220</v>
+        <v>1121</v>
       </c>
       <c r="B291">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C291" t="s">
-        <v>1221</v>
+        <v>1122</v>
       </c>
       <c r="D291" t="s">
-        <v>1222</v>
+        <v>1123</v>
       </c>
       <c r="E291" t="s">
-        <v>1223</v>
+        <v>1124</v>
       </c>
       <c r="F291" t="s">
-        <v>1224</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>1225</v>
+        <v>1126</v>
       </c>
       <c r="B292">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C292" t="s">
-        <v>1226</v>
+        <v>1127</v>
       </c>
       <c r="D292" t="s">
-        <v>1227</v>
+        <v>1128</v>
       </c>
       <c r="E292" t="s">
-        <v>1228</v>
+        <v>1129</v>
       </c>
       <c r="F292" t="s">
-        <v>1229</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>1230</v>
+        <v>1131</v>
       </c>
       <c r="B293">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C293" t="s">
-        <v>1231</v>
+        <v>1132</v>
       </c>
       <c r="D293" t="s">
-        <v>1232</v>
+        <v>1133</v>
+      </c>
+      <c r="E293" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F293" t="s">
+        <v>1135</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>1233</v>
+        <v>1136</v>
       </c>
       <c r="B294">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C294" t="s">
-        <v>1234</v>
+        <v>1137</v>
       </c>
       <c r="D294" t="s">
-        <v>1235</v>
+        <v>1138</v>
       </c>
       <c r="E294" t="s">
-        <v>1236</v>
+        <v>1139</v>
       </c>
       <c r="F294" t="s">
-        <v>1237</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>1238</v>
+        <v>1141</v>
       </c>
       <c r="B295">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C295" t="s">
-        <v>1239</v>
+        <v>1142</v>
       </c>
       <c r="D295" t="s">
-        <v>1240</v>
+        <v>1143</v>
       </c>
       <c r="E295" t="s">
-        <v>1241</v>
+        <v>1144</v>
       </c>
       <c r="F295" t="s">
-        <v>1242</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>1243</v>
+        <v>1146</v>
       </c>
       <c r="B296">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C296" t="s">
-        <v>1244</v>
+        <v>1147</v>
       </c>
       <c r="D296" t="s">
-        <v>1245</v>
+        <v>1148</v>
       </c>
       <c r="E296" t="s">
-        <v>1246</v>
+        <v>1149</v>
       </c>
       <c r="F296" t="s">
-        <v>1247</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>1248</v>
+        <v>1151</v>
       </c>
       <c r="B297">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C297" t="s">
-        <v>908</v>
+        <v>1152</v>
       </c>
       <c r="D297" t="s">
-        <v>1249</v>
+        <v>1153</v>
       </c>
       <c r="E297" t="s">
-        <v>1250</v>
+        <v>1154</v>
       </c>
       <c r="F297" t="s">
-        <v>1251</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>1252</v>
+        <v>1156</v>
       </c>
       <c r="B298">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C298" t="s">
-        <v>1253</v>
+        <v>1157</v>
       </c>
       <c r="D298" t="s">
-        <v>1254</v>
+        <v>1158</v>
       </c>
       <c r="E298" t="s">
-        <v>1255</v>
+        <v>1159</v>
+      </c>
+      <c r="F298" t="s">
+        <v>1160</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>1256</v>
+        <v>1161</v>
       </c>
       <c r="B299">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C299" t="s">
-        <v>1257</v>
+        <v>1162</v>
       </c>
       <c r="D299" t="s">
-        <v>1258</v>
+        <v>1163</v>
       </c>
       <c r="E299" t="s">
-        <v>1259</v>
+        <v>1164</v>
       </c>
       <c r="F299" t="s">
-        <v>1260</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>1261</v>
+        <v>1166</v>
       </c>
       <c r="B300">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C300" t="s">
-        <v>1262</v>
+        <v>1162</v>
       </c>
       <c r="D300" t="s">
-        <v>1263</v>
+        <v>1167</v>
       </c>
       <c r="E300" t="s">
-        <v>1264</v>
+        <v>1168</v>
       </c>
       <c r="F300" t="s">
-        <v>1265</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>1266</v>
+        <v>1170</v>
       </c>
       <c r="B301">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C301" t="s">
-        <v>1267</v>
+        <v>1171</v>
       </c>
       <c r="D301" t="s">
-        <v>1268</v>
+        <v>1172</v>
       </c>
       <c r="E301" t="s">
-        <v>1269</v>
+        <v>1173</v>
       </c>
       <c r="F301" t="s">
-        <v>1270</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>1271</v>
+        <v>1175</v>
       </c>
       <c r="B302">
         <v>28</v>
       </c>
       <c r="C302" t="s">
-        <v>1272</v>
+        <v>1176</v>
       </c>
       <c r="D302" t="s">
-        <v>1273</v>
+        <v>1177</v>
       </c>
       <c r="E302" t="s">
-        <v>1274</v>
+        <v>1178</v>
       </c>
       <c r="F302" t="s">
-        <v>1275</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>1276</v>
+        <v>1180</v>
       </c>
       <c r="B303">
         <v>28</v>
       </c>
       <c r="C303" t="s">
-        <v>1277</v>
+        <v>1181</v>
       </c>
       <c r="D303" t="s">
-        <v>1278</v>
+        <v>1182</v>
       </c>
       <c r="E303" t="s">
-        <v>1279</v>
+        <v>1183</v>
       </c>
       <c r="F303" t="s">
-        <v>1280</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>1281</v>
+        <v>1185</v>
       </c>
       <c r="B304">
         <v>28</v>
       </c>
       <c r="C304" t="s">
-        <v>1282</v>
+        <v>1186</v>
       </c>
       <c r="D304" t="s">
-        <v>1283</v>
+        <v>1187</v>
       </c>
       <c r="E304" t="s">
-        <v>1284</v>
+        <v>1188</v>
       </c>
       <c r="F304" t="s">
-        <v>1285</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>1286</v>
+        <v>1190</v>
       </c>
       <c r="B305">
         <v>28</v>
       </c>
       <c r="C305" t="s">
-        <v>1287</v>
+        <v>1191</v>
       </c>
       <c r="D305" t="s">
-        <v>1288</v>
+        <v>1192</v>
       </c>
       <c r="E305" t="s">
-        <v>1289</v>
+        <v>1193</v>
       </c>
       <c r="F305" t="s">
-        <v>1290</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>1291</v>
+        <v>1195</v>
       </c>
       <c r="B306">
         <v>28</v>
       </c>
       <c r="C306" t="s">
-        <v>1292</v>
+        <v>1196</v>
       </c>
       <c r="D306" t="s">
-        <v>1293</v>
+        <v>1197</v>
       </c>
       <c r="E306" t="s">
-        <v>1294</v>
+        <v>1198</v>
       </c>
       <c r="F306" t="s">
-        <v>1295</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>1296</v>
+        <v>1200</v>
       </c>
       <c r="B307">
         <v>28</v>
       </c>
       <c r="C307" t="s">
-        <v>1297</v>
+        <v>1201</v>
       </c>
       <c r="D307" t="s">
-        <v>1298</v>
+        <v>1202</v>
       </c>
       <c r="E307" t="s">
-        <v>1299</v>
+        <v>1203</v>
       </c>
       <c r="F307" t="s">
-        <v>1300</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>1301</v>
+        <v>1205</v>
       </c>
       <c r="B308">
         <v>28</v>
       </c>
       <c r="C308" t="s">
-        <v>1302</v>
+        <v>1206</v>
       </c>
       <c r="D308" t="s">
-        <v>1303</v>
+        <v>1207</v>
       </c>
       <c r="E308" t="s">
-        <v>1304</v>
+        <v>1208</v>
       </c>
       <c r="F308" t="s">
-        <v>1305</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>1306</v>
+        <v>1210</v>
       </c>
       <c r="B309">
         <v>28</v>
       </c>
       <c r="C309" t="s">
-        <v>1307</v>
+        <v>1211</v>
       </c>
       <c r="D309" t="s">
-        <v>1308</v>
+        <v>1212</v>
       </c>
       <c r="E309" t="s">
-        <v>1309</v>
+        <v>1213</v>
       </c>
       <c r="F309" t="s">
-        <v>1310</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>1311</v>
+        <v>1215</v>
       </c>
       <c r="B310">
         <v>28</v>
       </c>
       <c r="C310" t="s">
-        <v>1312</v>
+        <v>1216</v>
       </c>
       <c r="D310" t="s">
-        <v>1313</v>
+        <v>1217</v>
       </c>
       <c r="E310" t="s">
-        <v>1314</v>
+        <v>1218</v>
       </c>
       <c r="F310" t="s">
-        <v>1315</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>1316</v>
+        <v>1220</v>
       </c>
       <c r="B311">
         <v>28</v>
       </c>
       <c r="C311" t="s">
-        <v>1317</v>
+        <v>1221</v>
       </c>
       <c r="D311" t="s">
-        <v>1318</v>
+        <v>1222</v>
       </c>
       <c r="E311" t="s">
-        <v>1319</v>
+        <v>1223</v>
       </c>
       <c r="F311" t="s">
-        <v>1320</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>1321</v>
+        <v>1225</v>
       </c>
       <c r="B312">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C312" t="s">
-        <v>1322</v>
+        <v>1226</v>
       </c>
       <c r="D312" t="s">
-        <v>1323</v>
+        <v>1227</v>
       </c>
       <c r="E312" t="s">
-        <v>1324</v>
+        <v>1228</v>
       </c>
       <c r="F312" t="s">
-        <v>1325</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>1326</v>
+        <v>1230</v>
       </c>
       <c r="B313">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C313" t="s">
-        <v>1327</v>
+        <v>1231</v>
       </c>
       <c r="D313" t="s">
-        <v>1328</v>
-      </c>
-      <c r="E313" t="s">
-        <v>1329</v>
-      </c>
-      <c r="F313" t="s">
-        <v>1330</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>1331</v>
+        <v>1233</v>
       </c>
       <c r="B314">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C314" t="s">
-        <v>1332</v>
+        <v>1234</v>
       </c>
       <c r="D314" t="s">
-        <v>1333</v>
+        <v>1235</v>
       </c>
       <c r="E314" t="s">
-        <v>1334</v>
+        <v>1236</v>
       </c>
       <c r="F314" t="s">
-        <v>1335</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>1336</v>
+        <v>1238</v>
       </c>
       <c r="B315">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C315" t="s">
-        <v>1337</v>
+        <v>1239</v>
       </c>
       <c r="D315" t="s">
-        <v>1338</v>
+        <v>1240</v>
       </c>
       <c r="E315" t="s">
-        <v>1339</v>
+        <v>1241</v>
       </c>
       <c r="F315" t="s">
-        <v>1340</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>1341</v>
+        <v>1243</v>
       </c>
       <c r="B316">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C316" t="s">
-        <v>1342</v>
+        <v>1244</v>
       </c>
       <c r="D316" t="s">
-        <v>1343</v>
+        <v>1245</v>
       </c>
       <c r="E316" t="s">
-        <v>1344</v>
+        <v>1246</v>
       </c>
       <c r="F316" t="s">
-        <v>1345</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>1346</v>
+        <v>1248</v>
       </c>
       <c r="B317">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C317" t="s">
-        <v>1347</v>
+        <v>908</v>
       </c>
       <c r="D317" t="s">
-        <v>1348</v>
+        <v>1249</v>
       </c>
       <c r="E317" t="s">
-        <v>1349</v>
+        <v>1250</v>
       </c>
       <c r="F317" t="s">
-        <v>1350</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>1351</v>
+        <v>1252</v>
       </c>
       <c r="B318">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C318" t="s">
-        <v>1352</v>
+        <v>1253</v>
       </c>
       <c r="D318" t="s">
-        <v>1353</v>
+        <v>1254</v>
       </c>
       <c r="E318" t="s">
-        <v>1354</v>
-      </c>
-      <c r="F318" t="s">
-        <v>1355</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>1356</v>
+        <v>1256</v>
       </c>
       <c r="B319">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C319" t="s">
-        <v>1357</v>
+        <v>1257</v>
       </c>
       <c r="D319" t="s">
-        <v>1358</v>
+        <v>1258</v>
       </c>
       <c r="E319" t="s">
-        <v>1359</v>
+        <v>1259</v>
       </c>
       <c r="F319" t="s">
-        <v>1360</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>1361</v>
+        <v>1261</v>
       </c>
       <c r="B320">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C320" t="s">
-        <v>1362</v>
+        <v>1262</v>
       </c>
       <c r="D320" t="s">
-        <v>1363</v>
+        <v>1263</v>
       </c>
       <c r="E320" t="s">
-        <v>1364</v>
+        <v>1264</v>
       </c>
       <c r="F320" t="s">
-        <v>1365</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>1366</v>
+        <v>1266</v>
       </c>
       <c r="B321">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C321" t="s">
-        <v>1367</v>
+        <v>1267</v>
       </c>
       <c r="D321" t="s">
-        <v>1368</v>
+        <v>1268</v>
       </c>
       <c r="E321" t="s">
-        <v>1369</v>
+        <v>1269</v>
       </c>
       <c r="F321" t="s">
-        <v>1370</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>1371</v>
+        <v>1271</v>
       </c>
       <c r="B322">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C322" t="s">
-        <v>1372</v>
+        <v>1272</v>
       </c>
       <c r="D322" t="s">
-        <v>1373</v>
+        <v>1273</v>
       </c>
       <c r="E322" t="s">
-        <v>1374</v>
+        <v>1274</v>
       </c>
       <c r="F322" t="s">
-        <v>1375</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>1376</v>
+        <v>1276</v>
       </c>
       <c r="B323">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C323" t="s">
-        <v>1377</v>
+        <v>1277</v>
       </c>
       <c r="D323" t="s">
-        <v>1378</v>
+        <v>1278</v>
       </c>
       <c r="E323" t="s">
-        <v>1379</v>
+        <v>1279</v>
       </c>
       <c r="F323" t="s">
-        <v>1380</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>1381</v>
+        <v>1281</v>
       </c>
       <c r="B324">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C324" t="s">
-        <v>1382</v>
+        <v>1282</v>
       </c>
       <c r="D324" t="s">
-        <v>1383</v>
+        <v>1283</v>
       </c>
       <c r="E324" t="s">
-        <v>1384</v>
+        <v>1284</v>
       </c>
       <c r="F324" t="s">
-        <v>1385</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>1386</v>
+        <v>1286</v>
       </c>
       <c r="B325">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C325" t="s">
-        <v>1387</v>
+        <v>1287</v>
       </c>
       <c r="D325" t="s">
-        <v>1388</v>
+        <v>1288</v>
       </c>
       <c r="E325" t="s">
-        <v>1389</v>
+        <v>1289</v>
       </c>
       <c r="F325" t="s">
-        <v>1390</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>1391</v>
+        <v>1291</v>
       </c>
       <c r="B326">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C326" t="s">
-        <v>1392</v>
+        <v>1292</v>
       </c>
       <c r="D326" t="s">
-        <v>1393</v>
+        <v>1293</v>
       </c>
       <c r="E326" t="s">
-        <v>1394</v>
+        <v>1294</v>
       </c>
       <c r="F326" t="s">
-        <v>1395</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>1396</v>
+        <v>1296</v>
       </c>
       <c r="B327">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C327" t="s">
-        <v>1397</v>
+        <v>1297</v>
       </c>
       <c r="D327" t="s">
-        <v>1398</v>
+        <v>1298</v>
       </c>
       <c r="E327" t="s">
-        <v>1399</v>
+        <v>1299</v>
       </c>
       <c r="F327" t="s">
-        <v>1400</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>1401</v>
+        <v>1301</v>
       </c>
       <c r="B328">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C328" t="s">
-        <v>1402</v>
+        <v>1302</v>
       </c>
       <c r="D328" t="s">
-        <v>1403</v>
+        <v>1303</v>
       </c>
       <c r="E328" t="s">
-        <v>1404</v>
+        <v>1304</v>
       </c>
       <c r="F328" t="s">
-        <v>1405</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>1406</v>
+        <v>1306</v>
       </c>
       <c r="B329">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C329" t="s">
-        <v>1407</v>
+        <v>1307</v>
       </c>
       <c r="D329" t="s">
-        <v>1408</v>
+        <v>1308</v>
       </c>
       <c r="E329" t="s">
-        <v>1409</v>
+        <v>1309</v>
       </c>
       <c r="F329" t="s">
-        <v>1410</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>1411</v>
+        <v>1311</v>
       </c>
       <c r="B330">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C330" t="s">
-        <v>1412</v>
+        <v>1312</v>
       </c>
       <c r="D330" t="s">
-        <v>1413</v>
+        <v>1313</v>
       </c>
       <c r="E330" t="s">
-        <v>1414</v>
+        <v>1314</v>
       </c>
       <c r="F330" t="s">
-        <v>1415</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>1416</v>
+        <v>1316</v>
       </c>
       <c r="B331">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C331" t="s">
-        <v>1417</v>
+        <v>1317</v>
       </c>
       <c r="D331" t="s">
-        <v>1418</v>
+        <v>1318</v>
       </c>
       <c r="E331" t="s">
-        <v>1419</v>
+        <v>1319</v>
       </c>
       <c r="F331" t="s">
-        <v>1420</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>1421</v>
+        <v>1321</v>
       </c>
       <c r="B332">
         <v>29</v>
       </c>
       <c r="C332" t="s">
-        <v>1422</v>
+        <v>1322</v>
       </c>
       <c r="D332" t="s">
-        <v>1423</v>
+        <v>1323</v>
       </c>
       <c r="E332" t="s">
-        <v>1424</v>
+        <v>1324</v>
       </c>
       <c r="F332" t="s">
-        <v>1425</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>1426</v>
+        <v>1326</v>
       </c>
       <c r="B333">
         <v>29</v>
       </c>
       <c r="C333" t="s">
-        <v>1427</v>
+        <v>1327</v>
       </c>
       <c r="D333" t="s">
-        <v>1428</v>
+        <v>1328</v>
       </c>
       <c r="E333" t="s">
-        <v>1429</v>
+        <v>1329</v>
       </c>
       <c r="F333" t="s">
-        <v>1430</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>1431</v>
+        <v>1331</v>
       </c>
       <c r="B334">
         <v>29</v>
       </c>
       <c r="C334" t="s">
-        <v>1432</v>
+        <v>1332</v>
       </c>
       <c r="D334" t="s">
-        <v>1433</v>
+        <v>1333</v>
       </c>
       <c r="E334" t="s">
-        <v>1434</v>
+        <v>1334</v>
       </c>
       <c r="F334" t="s">
-        <v>1435</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>1436</v>
+        <v>1336</v>
       </c>
       <c r="B335">
         <v>29</v>
       </c>
       <c r="C335" t="s">
-        <v>1437</v>
+        <v>1337</v>
       </c>
       <c r="D335" t="s">
-        <v>1438</v>
+        <v>1338</v>
       </c>
       <c r="E335" t="s">
-        <v>1439</v>
+        <v>1339</v>
       </c>
       <c r="F335" t="s">
-        <v>1440</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>1441</v>
+        <v>1341</v>
       </c>
       <c r="B336">
         <v>29</v>
       </c>
       <c r="C336" t="s">
-        <v>1442</v>
+        <v>1342</v>
       </c>
       <c r="D336" t="s">
-        <v>1443</v>
+        <v>1343</v>
       </c>
       <c r="E336" t="s">
-        <v>1444</v>
+        <v>1344</v>
       </c>
       <c r="F336" t="s">
-        <v>1445</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>1446</v>
+        <v>1346</v>
       </c>
       <c r="B337">
         <v>29</v>
       </c>
       <c r="C337" t="s">
-        <v>1447</v>
+        <v>1347</v>
       </c>
       <c r="D337" t="s">
-        <v>1448</v>
+        <v>1348</v>
       </c>
       <c r="E337" t="s">
-        <v>1449</v>
+        <v>1349</v>
       </c>
       <c r="F337" t="s">
-        <v>1450</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>1451</v>
+        <v>1351</v>
       </c>
       <c r="B338">
         <v>29</v>
       </c>
       <c r="C338" t="s">
-        <v>1452</v>
+        <v>1352</v>
       </c>
       <c r="D338" t="s">
-        <v>1453</v>
+        <v>1353</v>
       </c>
       <c r="E338" t="s">
-        <v>1454</v>
+        <v>1354</v>
       </c>
       <c r="F338" t="s">
-        <v>1455</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>1456</v>
+        <v>1356</v>
       </c>
       <c r="B339">
         <v>29</v>
       </c>
       <c r="C339" t="s">
-        <v>1457</v>
+        <v>1357</v>
       </c>
       <c r="D339" t="s">
-        <v>1458</v>
+        <v>1358</v>
       </c>
       <c r="E339" t="s">
-        <v>1459</v>
+        <v>1359</v>
       </c>
       <c r="F339" t="s">
-        <v>1460</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>1461</v>
+        <v>1361</v>
       </c>
       <c r="B340">
         <v>29</v>
       </c>
       <c r="C340" t="s">
-        <v>1462</v>
+        <v>1362</v>
       </c>
       <c r="D340" t="s">
-        <v>1463</v>
+        <v>1363</v>
       </c>
       <c r="E340" t="s">
-        <v>1464</v>
+        <v>1364</v>
       </c>
       <c r="F340" t="s">
-        <v>1465</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>1466</v>
+        <v>1366</v>
       </c>
       <c r="B341">
         <v>29</v>
       </c>
       <c r="C341" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D341" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E341" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F341" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A342" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B342">
+        <v>29</v>
+      </c>
+      <c r="C342" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D342" t="s">
+        <v>1373</v>
+      </c>
+      <c r="E342" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F342" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A343" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B343">
+        <v>29</v>
+      </c>
+      <c r="C343" t="s">
+        <v>1377</v>
+      </c>
+      <c r="D343" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E343" t="s">
+        <v>1379</v>
+      </c>
+      <c r="F343" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A344" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B344">
+        <v>29</v>
+      </c>
+      <c r="C344" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D344" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E344" t="s">
+        <v>1384</v>
+      </c>
+      <c r="F344" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A345" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B345">
+        <v>29</v>
+      </c>
+      <c r="C345" t="s">
+        <v>1387</v>
+      </c>
+      <c r="D345" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E345" t="s">
+        <v>1389</v>
+      </c>
+      <c r="F345" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A346" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B346">
+        <v>29</v>
+      </c>
+      <c r="C346" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D346" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E346" t="s">
+        <v>1394</v>
+      </c>
+      <c r="F346" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A347" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B347">
+        <v>29</v>
+      </c>
+      <c r="C347" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D347" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E347" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F347" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A348" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B348">
+        <v>29</v>
+      </c>
+      <c r="C348" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D348" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E348" t="s">
+        <v>1404</v>
+      </c>
+      <c r="F348" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A349" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B349">
+        <v>29</v>
+      </c>
+      <c r="C349" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D349" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E349" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F349" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A350" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B350">
+        <v>29</v>
+      </c>
+      <c r="C350" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D350" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E350" t="s">
+        <v>1414</v>
+      </c>
+      <c r="F350" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A351" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B351">
+        <v>29</v>
+      </c>
+      <c r="C351" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D351" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E351" t="s">
+        <v>1419</v>
+      </c>
+      <c r="F351" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A352" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B352">
+        <v>29</v>
+      </c>
+      <c r="C352" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D352" t="s">
+        <v>1423</v>
+      </c>
+      <c r="E352" t="s">
+        <v>1424</v>
+      </c>
+      <c r="F352" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A353" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B353">
+        <v>29</v>
+      </c>
+      <c r="C353" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D353" t="s">
+        <v>1428</v>
+      </c>
+      <c r="E353" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F353" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A354" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B354">
+        <v>29</v>
+      </c>
+      <c r="C354" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D354" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E354" t="s">
+        <v>1434</v>
+      </c>
+      <c r="F354" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A355" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B355">
+        <v>29</v>
+      </c>
+      <c r="C355" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D355" t="s">
+        <v>1438</v>
+      </c>
+      <c r="E355" t="s">
+        <v>1439</v>
+      </c>
+      <c r="F355" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A356" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B356">
+        <v>29</v>
+      </c>
+      <c r="C356" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D356" t="s">
+        <v>1443</v>
+      </c>
+      <c r="E356" t="s">
+        <v>1444</v>
+      </c>
+      <c r="F356" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A357" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B357">
+        <v>29</v>
+      </c>
+      <c r="C357" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D357" t="s">
+        <v>1448</v>
+      </c>
+      <c r="E357" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F357" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A358" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B358">
+        <v>29</v>
+      </c>
+      <c r="C358" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D358" t="s">
+        <v>1453</v>
+      </c>
+      <c r="E358" t="s">
+        <v>1454</v>
+      </c>
+      <c r="F358" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A359" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B359">
+        <v>29</v>
+      </c>
+      <c r="C359" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D359" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E359" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F359" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A360" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B360">
+        <v>29</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D360" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E360" t="s">
+        <v>1464</v>
+      </c>
+      <c r="F360" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A361" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B361">
+        <v>29</v>
+      </c>
+      <c r="C361" t="s">
         <v>1467</v>
       </c>
-      <c r="D341" t="s">
+      <c r="D361" t="s">
         <v>1468</v>
       </c>
-      <c r="E341" t="s">
+      <c r="E361" t="s">
         <v>1469</v>
       </c>
-      <c r="F341" t="s">
+      <c r="F361" t="s">
         <v>1470</v>
       </c>
     </row>
@@ -12894,7 +13651,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A222:G341 A1:B1 D1:G1 A2:G181" numberStoredAsText="1"/>
+    <ignoredError sqref="A242:G361 A1:B1 D1:G1 A2:G181" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -12918,7 +13675,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>4da16d99-2110-4bdc-95c0-f300b8a9ce45</v>
+        <v>214718e4-59a8-40b3-a3dd-a78a6dcb4064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add 10 words in unit 21
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82A9587-B534-6F43-AB60-83B187E3E127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84126FD0-6632-F94B-825E-A47F33B48A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51240" yWindow="-2100" windowWidth="29840" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4534" uniqueCount="3851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4594" uniqueCount="3900">
   <si>
     <t>ID</t>
   </si>
@@ -11583,6 +11583,153 @@
   </si>
   <si>
     <t>ancient culture</t>
+  </si>
+  <si>
+    <t>U22_01</t>
+  </si>
+  <si>
+    <t>U22_02</t>
+  </si>
+  <si>
+    <t>U22_03</t>
+  </si>
+  <si>
+    <t>U22_04</t>
+  </si>
+  <si>
+    <t>U22_05</t>
+  </si>
+  <si>
+    <t>U22_06</t>
+  </si>
+  <si>
+    <t>U22_07</t>
+  </si>
+  <si>
+    <t>U22_08</t>
+  </si>
+  <si>
+    <t>U22_09</t>
+  </si>
+  <si>
+    <t>U22_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biên giới </t>
+  </si>
+  <si>
+    <t>Border</t>
+  </si>
+  <si>
+    <t>This train crosses the border between Austria and Germany</t>
+  </si>
+  <si>
+    <t>cross the border</t>
+  </si>
+  <si>
+    <t>Dây an toàn</t>
+  </si>
+  <si>
+    <t>Belt</t>
+  </si>
+  <si>
+    <t>Please fasten the seat belt whenever you sit down</t>
+  </si>
+  <si>
+    <t>fasten the seat belt / thắt dây an toàn</t>
+  </si>
+  <si>
+    <t>Dự định</t>
+  </si>
+  <si>
+    <t>intend</t>
+  </si>
+  <si>
+    <t>He intends to travel after graduation</t>
+  </si>
+  <si>
+    <t>intend to do something / có dự định làm gì đó</t>
+  </si>
+  <si>
+    <t>Thông báo</t>
+  </si>
+  <si>
+    <t>Announce</t>
+  </si>
+  <si>
+    <t>She announces her marriage to the whole family</t>
+  </si>
+  <si>
+    <t>announce something to somebody</t>
+  </si>
+  <si>
+    <t>Miễn thuế</t>
+  </si>
+  <si>
+    <t>Duty-free</t>
+  </si>
+  <si>
+    <t>That cologne is from a duty-free shop</t>
+  </si>
+  <si>
+    <t>Duty-free shop</t>
+  </si>
+  <si>
+    <t>Gây ấn tượng</t>
+  </si>
+  <si>
+    <t>Impressive</t>
+  </si>
+  <si>
+    <t>She has an impressive performance</t>
+  </si>
+  <si>
+    <t>an impressive performance</t>
+  </si>
+  <si>
+    <t>Việc đặt trưuocws</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>She calls to make a booking</t>
+  </si>
+  <si>
+    <t>make a booking</t>
+  </si>
+  <si>
+    <t>Người lớn</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I would like to book an adult ticket for this flight </t>
+  </si>
+  <si>
+    <t>an adult ticket</t>
+  </si>
+  <si>
+    <t>airline</t>
+  </si>
+  <si>
+    <t>Jetstar is a low-cost airline</t>
+  </si>
+  <si>
+    <t>a low-cost airline</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>We cancel the show due to th rain</t>
+  </si>
+  <si>
+    <t>cancel something</t>
+  </si>
+  <si>
+    <t>Hãng hàng không</t>
   </si>
 </sst>
 </file>
@@ -11947,10 +12094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G781"/>
+  <dimension ref="A1:G791"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B611" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F628" sqref="F628"/>
+    <sheetView tabSelected="1" topLeftCell="B624" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E634" sqref="E634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26478,229 +26625,249 @@
     </row>
     <row r="632" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A632" s="1" t="s">
-        <v>1828</v>
+        <v>3851</v>
       </c>
       <c r="B632" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C632" s="1" t="s">
-        <v>6</v>
+        <v>3861</v>
       </c>
       <c r="D632" s="1" t="s">
-        <v>7</v>
+        <v>3862</v>
       </c>
       <c r="E632" s="1" t="s">
-        <v>8</v>
+        <v>3863</v>
       </c>
       <c r="F632" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G632" s="1"/>
+        <v>3864</v>
+      </c>
+      <c r="G632" s="1" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="633" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A633" s="1" t="s">
-        <v>1829</v>
+        <v>3852</v>
       </c>
       <c r="B633" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C633" s="1" t="s">
-        <v>10</v>
+        <v>3865</v>
       </c>
       <c r="D633" s="1" t="s">
-        <v>11</v>
+        <v>3866</v>
       </c>
       <c r="E633" s="1" t="s">
-        <v>12</v>
+        <v>3867</v>
       </c>
       <c r="F633" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G633" s="1"/>
+        <v>3868</v>
+      </c>
+      <c r="G633" s="1" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="634" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A634" s="1" t="s">
-        <v>1830</v>
+        <v>3853</v>
       </c>
       <c r="B634" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C634" s="1" t="s">
-        <v>13</v>
+        <v>3869</v>
       </c>
       <c r="D634" s="1" t="s">
-        <v>14</v>
+        <v>3870</v>
       </c>
       <c r="E634" s="1" t="s">
-        <v>15</v>
+        <v>3871</v>
       </c>
       <c r="F634" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G634" s="1"/>
+        <v>3872</v>
+      </c>
+      <c r="G634" s="1" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A635" s="1" t="s">
-        <v>1831</v>
+        <v>3854</v>
       </c>
       <c r="B635" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C635" s="1" t="s">
-        <v>16</v>
+        <v>3873</v>
       </c>
       <c r="D635" s="1" t="s">
-        <v>17</v>
+        <v>3874</v>
       </c>
       <c r="E635" s="1" t="s">
-        <v>18</v>
+        <v>3875</v>
       </c>
       <c r="F635" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G635" s="1"/>
+        <v>3876</v>
+      </c>
+      <c r="G635" s="1" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="636" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A636" s="1" t="s">
-        <v>1832</v>
+        <v>3855</v>
       </c>
       <c r="B636" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C636" s="1" t="s">
-        <v>19</v>
+        <v>3877</v>
       </c>
       <c r="D636" s="1" t="s">
-        <v>20</v>
+        <v>3878</v>
       </c>
       <c r="E636" s="1" t="s">
-        <v>21</v>
+        <v>3879</v>
       </c>
       <c r="F636" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G636" s="1"/>
+        <v>3880</v>
+      </c>
+      <c r="G636" s="1" t="s">
+        <v>609</v>
+      </c>
     </row>
     <row r="637" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A637" s="1" t="s">
-        <v>1833</v>
+        <v>3856</v>
       </c>
       <c r="B637" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C637" s="1" t="s">
-        <v>22</v>
+        <v>3881</v>
       </c>
       <c r="D637" s="1" t="s">
-        <v>23</v>
+        <v>3882</v>
       </c>
       <c r="E637" s="1" t="s">
-        <v>24</v>
+        <v>3883</v>
       </c>
       <c r="F637" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G637" s="1"/>
+        <v>3884</v>
+      </c>
+      <c r="G637" s="1" t="s">
+        <v>609</v>
+      </c>
     </row>
     <row r="638" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A638" s="1" t="s">
-        <v>1834</v>
+        <v>3857</v>
       </c>
       <c r="B638" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C638" s="1" t="s">
-        <v>25</v>
+        <v>3885</v>
       </c>
       <c r="D638" s="1" t="s">
-        <v>26</v>
+        <v>3886</v>
       </c>
       <c r="E638" s="1" t="s">
-        <v>27</v>
+        <v>3887</v>
       </c>
       <c r="F638" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G638" s="1"/>
+        <v>3888</v>
+      </c>
+      <c r="G638" s="1" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="639" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A639" s="1" t="s">
-        <v>1835</v>
+        <v>3858</v>
       </c>
       <c r="B639" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C639" s="1" t="s">
-        <v>28</v>
+        <v>3889</v>
       </c>
       <c r="D639" s="1" t="s">
-        <v>29</v>
+        <v>3890</v>
       </c>
       <c r="E639" s="1" t="s">
-        <v>30</v>
+        <v>3891</v>
       </c>
       <c r="F639" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G639" s="1"/>
+        <v>3892</v>
+      </c>
+      <c r="G639" s="1" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="640" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A640" s="1" t="s">
-        <v>1836</v>
+        <v>3859</v>
       </c>
       <c r="B640" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C640" s="1" t="s">
-        <v>31</v>
+        <v>3899</v>
       </c>
       <c r="D640" s="1" t="s">
-        <v>32</v>
+        <v>3893</v>
       </c>
       <c r="E640" s="1" t="s">
-        <v>33</v>
+        <v>3894</v>
       </c>
       <c r="F640" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G640" s="1"/>
+        <v>3895</v>
+      </c>
+      <c r="G640" s="1" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="641" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A641" s="1" t="s">
-        <v>1837</v>
+        <v>3860</v>
       </c>
       <c r="B641" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C641" s="1" t="s">
-        <v>34</v>
+        <v>1472</v>
       </c>
       <c r="D641" s="1" t="s">
-        <v>35</v>
+        <v>3896</v>
       </c>
       <c r="E641" s="1" t="s">
-        <v>36</v>
+        <v>3897</v>
       </c>
       <c r="F641" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G641" s="1"/>
+        <v>3898</v>
+      </c>
+      <c r="G641" s="1" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="642" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A642" s="1" t="s">
-        <v>1838</v>
+        <v>1828</v>
       </c>
       <c r="B642" s="1">
         <v>26</v>
       </c>
       <c r="C642" s="1" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D642" s="1" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="E642" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F642" s="1" t="s">
         <v>9</v>
@@ -26709,19 +26876,19 @@
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A643" s="1" t="s">
-        <v>1839</v>
+        <v>1829</v>
       </c>
       <c r="B643" s="1">
         <v>26</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D643" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E643" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="F643" s="1" t="s">
         <v>9</v>
@@ -26730,40 +26897,40 @@
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A644" s="1" t="s">
-        <v>1840</v>
+        <v>1830</v>
       </c>
       <c r="B644" s="1">
         <v>26</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="D644" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E644" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F644" s="1" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="G644" s="1"/>
     </row>
     <row r="645" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A645" s="1" t="s">
-        <v>1841</v>
+        <v>1831</v>
       </c>
       <c r="B645" s="1">
         <v>26</v>
       </c>
       <c r="C645" s="1" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="D645" s="1" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E645" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="F645" s="1" t="s">
         <v>9</v>
@@ -26772,40 +26939,40 @@
     </row>
     <row r="646" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A646" s="1" t="s">
-        <v>1842</v>
+        <v>1832</v>
       </c>
       <c r="B646" s="1">
         <v>26</v>
       </c>
       <c r="C646" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D646" s="1" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="E646" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="F646" s="1" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="G646" s="1"/>
     </row>
     <row r="647" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A647" s="1" t="s">
-        <v>1843</v>
+        <v>1833</v>
       </c>
       <c r="B647" s="1">
         <v>26</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="D647" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E647" s="1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="F647" s="1" t="s">
         <v>9</v>
@@ -26814,40 +26981,40 @@
     </row>
     <row r="648" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A648" s="1" t="s">
-        <v>1844</v>
+        <v>1834</v>
       </c>
       <c r="B648" s="1">
         <v>26</v>
       </c>
       <c r="C648" s="1" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="D648" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="E648" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="F648" s="1" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="G648" s="1"/>
     </row>
     <row r="649" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A649" s="1" t="s">
-        <v>1845</v>
+        <v>1835</v>
       </c>
       <c r="B649" s="1">
         <v>26</v>
       </c>
       <c r="C649" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D649" s="1" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E649" s="1" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="F649" s="1" t="s">
         <v>9</v>
@@ -26856,19 +27023,19 @@
     </row>
     <row r="650" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A650" s="1" t="s">
-        <v>1846</v>
+        <v>1836</v>
       </c>
       <c r="B650" s="1">
         <v>26</v>
       </c>
       <c r="C650" s="1" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="D650" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E650" s="1" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="F650" s="1" t="s">
         <v>9</v>
@@ -26877,40 +27044,40 @@
     </row>
     <row r="651" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A651" s="1" t="s">
-        <v>1847</v>
+        <v>1837</v>
       </c>
       <c r="B651" s="1">
         <v>26</v>
       </c>
       <c r="C651" s="1" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="D651" s="1" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="E651" s="1" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="F651" s="1" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="G651" s="1"/>
     </row>
     <row r="652" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A652" s="1" t="s">
-        <v>1848</v>
+        <v>1838</v>
       </c>
       <c r="B652" s="1">
         <v>26</v>
       </c>
       <c r="C652" s="1" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="D652" s="1" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="E652" s="1" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F652" s="1" t="s">
         <v>9</v>
@@ -26919,19 +27086,19 @@
     </row>
     <row r="653" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A653" s="1" t="s">
-        <v>1849</v>
+        <v>1839</v>
       </c>
       <c r="B653" s="1">
         <v>26</v>
       </c>
       <c r="C653" s="1" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="D653" s="1" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="E653" s="1" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="F653" s="1" t="s">
         <v>9</v>
@@ -26940,40 +27107,40 @@
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A654" s="1" t="s">
-        <v>1850</v>
+        <v>1840</v>
       </c>
       <c r="B654" s="1">
         <v>26</v>
       </c>
       <c r="C654" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="D654" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="E654" s="1" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="F654" s="1" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="G654" s="1"/>
     </row>
     <row r="655" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A655" s="1" t="s">
-        <v>1851</v>
+        <v>1841</v>
       </c>
       <c r="B655" s="1">
         <v>26</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="D655" s="1" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="E655" s="1" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="F655" s="1" t="s">
         <v>9</v>
@@ -26982,82 +27149,82 @@
     </row>
     <row r="656" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A656" s="1" t="s">
-        <v>1852</v>
+        <v>1842</v>
       </c>
       <c r="B656" s="1">
         <v>26</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="D656" s="1" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="E656" s="1" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="F656" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="G656" s="1"/>
     </row>
     <row r="657" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A657" s="1" t="s">
-        <v>1853</v>
+        <v>1843</v>
       </c>
       <c r="B657" s="1">
         <v>26</v>
       </c>
       <c r="C657" s="1" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="D657" s="1" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="E657" s="1" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="F657" s="1" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="G657" s="1"/>
     </row>
     <row r="658" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A658" s="1" t="s">
-        <v>1854</v>
+        <v>1844</v>
       </c>
       <c r="B658" s="1">
         <v>26</v>
       </c>
       <c r="C658" s="1" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D658" s="1" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="E658" s="1" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="F658" s="1" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="G658" s="1"/>
     </row>
     <row r="659" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A659" s="1" t="s">
-        <v>1855</v>
+        <v>1845</v>
       </c>
       <c r="B659" s="1">
         <v>26</v>
       </c>
       <c r="C659" s="1" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="D659" s="1" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="E659" s="1" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="F659" s="1" t="s">
         <v>9</v>
@@ -27066,19 +27233,19 @@
     </row>
     <row r="660" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A660" s="1" t="s">
-        <v>1856</v>
+        <v>1846</v>
       </c>
       <c r="B660" s="1">
         <v>26</v>
       </c>
       <c r="C660" s="1" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="D660" s="1" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="E660" s="1" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="F660" s="1" t="s">
         <v>9</v>
@@ -27087,40 +27254,40 @@
     </row>
     <row r="661" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A661" s="1" t="s">
-        <v>1857</v>
+        <v>1847</v>
       </c>
       <c r="B661" s="1">
         <v>26</v>
       </c>
       <c r="C661" s="1" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="D661" s="1" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E661" s="1" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="F661" s="1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="G661" s="1"/>
     </row>
     <row r="662" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A662" s="1" t="s">
-        <v>1858</v>
+        <v>1848</v>
       </c>
       <c r="B662" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C662" s="1" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="D662" s="1" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="E662" s="1" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="F662" s="1" t="s">
         <v>9</v>
@@ -27129,19 +27296,19 @@
     </row>
     <row r="663" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A663" s="1" t="s">
-        <v>1859</v>
+        <v>1849</v>
       </c>
       <c r="B663" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C663" s="1" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="D663" s="1" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="E663" s="1" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="F663" s="1" t="s">
         <v>9</v>
@@ -27150,19 +27317,19 @@
     </row>
     <row r="664" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A664" s="1" t="s">
-        <v>1860</v>
+        <v>1850</v>
       </c>
       <c r="B664" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D664" s="1" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="E664" s="1" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="F664" s="1" t="s">
         <v>9</v>
@@ -27171,19 +27338,19 @@
     </row>
     <row r="665" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A665" s="1" t="s">
-        <v>1861</v>
+        <v>1851</v>
       </c>
       <c r="B665" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="D665" s="1" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="E665" s="1" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="F665" s="1" t="s">
         <v>9</v>
@@ -27192,19 +27359,19 @@
     </row>
     <row r="666" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A666" s="1" t="s">
-        <v>1862</v>
+        <v>1852</v>
       </c>
       <c r="B666" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="D666" s="1" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="E666" s="1" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="F666" s="1" t="s">
         <v>9</v>
@@ -27213,82 +27380,82 @@
     </row>
     <row r="667" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A667" s="1" t="s">
-        <v>1863</v>
+        <v>1853</v>
       </c>
       <c r="B667" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="D667" s="1" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="E667" s="1" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="F667" s="1" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="G667" s="1"/>
     </row>
     <row r="668" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A668" s="1" t="s">
-        <v>1864</v>
+        <v>1854</v>
       </c>
       <c r="B668" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="D668" s="1" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="E668" s="1" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="F668" s="1" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="G668" s="1"/>
     </row>
     <row r="669" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A669" s="1" t="s">
-        <v>1865</v>
+        <v>1855</v>
       </c>
       <c r="B669" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="D669" s="1" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="E669" s="1" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="F669" s="1" t="s">
-        <v>128</v>
+        <v>9</v>
       </c>
       <c r="G669" s="1"/>
     </row>
     <row r="670" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A670" s="1" t="s">
-        <v>1866</v>
+        <v>1856</v>
       </c>
       <c r="B670" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C670" s="1" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="D670" s="1" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="E670" s="1" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="F670" s="1" t="s">
         <v>9</v>
@@ -27297,2328 +27464,2538 @@
     </row>
     <row r="671" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A671" s="1" t="s">
-        <v>1867</v>
+        <v>1857</v>
       </c>
       <c r="B671" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="D671" s="1" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="E671" s="1" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="F671" s="1" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
       <c r="G671" s="1"/>
     </row>
     <row r="672" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A672" s="1" t="s">
-        <v>1868</v>
+        <v>1858</v>
       </c>
       <c r="B672" s="1">
         <v>27</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="D672" s="1" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="E672" s="1" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="F672" s="1" t="s">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="G672" s="1"/>
     </row>
     <row r="673" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A673" s="1" t="s">
-        <v>1869</v>
+        <v>1859</v>
       </c>
       <c r="B673" s="1">
         <v>27</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="D673" s="1" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="E673" s="1" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="F673" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="G673" s="1"/>
     </row>
     <row r="674" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A674" s="1" t="s">
-        <v>1870</v>
+        <v>1860</v>
       </c>
       <c r="B674" s="1">
         <v>27</v>
       </c>
       <c r="C674" s="1" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="D674" s="1" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="E674" s="1" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="F674" s="1" t="s">
-        <v>147</v>
+        <v>9</v>
       </c>
       <c r="G674" s="1"/>
     </row>
     <row r="675" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A675" s="1" t="s">
-        <v>1871</v>
+        <v>1861</v>
       </c>
       <c r="B675" s="1">
         <v>27</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="D675" s="1" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="E675" s="1" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="F675" s="1" t="s">
-        <v>151</v>
+        <v>9</v>
       </c>
       <c r="G675" s="1"/>
     </row>
     <row r="676" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A676" s="1" t="s">
-        <v>1872</v>
+        <v>1862</v>
       </c>
       <c r="B676" s="1">
         <v>27</v>
       </c>
       <c r="C676" s="1" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="D676" s="1" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="E676" s="1" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="F676" s="1" t="s">
-        <v>155</v>
+        <v>9</v>
       </c>
       <c r="G676" s="1"/>
     </row>
     <row r="677" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A677" s="1" t="s">
-        <v>1873</v>
+        <v>1863</v>
       </c>
       <c r="B677" s="1">
         <v>27</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="D677" s="1" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="E677" s="1" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="F677" s="1" t="s">
-        <v>159</v>
+        <v>9</v>
       </c>
       <c r="G677" s="1"/>
     </row>
     <row r="678" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A678" s="1" t="s">
-        <v>1874</v>
+        <v>1864</v>
       </c>
       <c r="B678" s="1">
         <v>27</v>
       </c>
       <c r="C678" s="1" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="D678" s="1" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="E678" s="1" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="F678" s="1" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
       <c r="G678" s="1"/>
     </row>
     <row r="679" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A679" s="1" t="s">
-        <v>1875</v>
+        <v>1865</v>
       </c>
       <c r="B679" s="1">
         <v>27</v>
       </c>
       <c r="C679" s="1" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="D679" s="1" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="E679" s="1" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="F679" s="1" t="s">
-        <v>167</v>
+        <v>128</v>
       </c>
       <c r="G679" s="1"/>
     </row>
     <row r="680" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A680" s="1" t="s">
-        <v>1876</v>
+        <v>1866</v>
       </c>
       <c r="B680" s="1">
         <v>27</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>168</v>
+        <v>129</v>
       </c>
       <c r="D680" s="1" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="E680" s="1" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="F680" s="1" t="s">
-        <v>171</v>
+        <v>9</v>
       </c>
       <c r="G680" s="1"/>
     </row>
     <row r="681" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A681" s="1" t="s">
-        <v>1877</v>
+        <v>1867</v>
       </c>
       <c r="B681" s="1">
         <v>27</v>
       </c>
       <c r="C681" s="1" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="D681" s="1" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="E681" s="1" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="F681" s="1" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="G681" s="1"/>
     </row>
     <row r="682" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A682" s="1" t="s">
-        <v>1878</v>
+        <v>1868</v>
       </c>
       <c r="B682" s="1">
         <v>27</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="D682" s="1" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
       <c r="E682" s="1" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="F682" s="1" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="G682" s="1"/>
     </row>
     <row r="683" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A683" s="1" t="s">
-        <v>1879</v>
+        <v>1869</v>
       </c>
       <c r="B683" s="1">
         <v>27</v>
       </c>
       <c r="C683" s="1" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="D683" s="1" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="E683" s="1" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="F683" s="1" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="G683" s="1"/>
     </row>
     <row r="684" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A684" s="1" t="s">
-        <v>1880</v>
+        <v>1870</v>
       </c>
       <c r="B684" s="1">
         <v>27</v>
       </c>
       <c r="C684" s="1" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="D684" s="1" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="E684" s="1" t="s">
-        <v>186</v>
+        <v>146</v>
       </c>
       <c r="F684" s="1" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
       <c r="G684" s="1"/>
     </row>
     <row r="685" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A685" s="1" t="s">
-        <v>1881</v>
+        <v>1871</v>
       </c>
       <c r="B685" s="1">
         <v>27</v>
       </c>
       <c r="C685" s="1" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="D685" s="1" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="E685" s="1" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="F685" s="1" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="G685" s="1"/>
     </row>
     <row r="686" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A686" s="1" t="s">
-        <v>1882</v>
+        <v>1872</v>
       </c>
       <c r="B686" s="1">
         <v>27</v>
       </c>
       <c r="C686" s="1" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="D686" s="1" t="s">
-        <v>193</v>
+        <v>153</v>
       </c>
       <c r="E686" s="1" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="F686" s="1" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="G686" s="1"/>
     </row>
     <row r="687" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A687" s="1" t="s">
-        <v>1883</v>
+        <v>1873</v>
       </c>
       <c r="B687" s="1">
         <v>27</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="D687" s="1" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="E687" s="1" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="F687" s="1" t="s">
-        <v>199</v>
+        <v>159</v>
       </c>
       <c r="G687" s="1"/>
     </row>
     <row r="688" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A688" s="1" t="s">
-        <v>1884</v>
+        <v>1874</v>
       </c>
       <c r="B688" s="1">
         <v>27</v>
       </c>
       <c r="C688" s="1" t="s">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="D688" s="1" t="s">
-        <v>201</v>
+        <v>161</v>
       </c>
       <c r="E688" s="1" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="F688" s="1" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="G688" s="1"/>
     </row>
     <row r="689" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A689" s="1" t="s">
-        <v>1885</v>
+        <v>1875</v>
       </c>
       <c r="B689" s="1">
         <v>27</v>
       </c>
       <c r="C689" s="1" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="D689" s="1" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="E689" s="1" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
       <c r="F689" s="1" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
       <c r="G689" s="1"/>
     </row>
     <row r="690" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A690" s="1" t="s">
-        <v>1886</v>
+        <v>1876</v>
       </c>
       <c r="B690" s="1">
         <v>27</v>
       </c>
       <c r="C690" s="1" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="D690" s="1" t="s">
-        <v>208</v>
+        <v>169</v>
       </c>
       <c r="E690" s="1" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="F690" s="1" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="G690" s="1"/>
     </row>
     <row r="691" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A691" s="1" t="s">
-        <v>1887</v>
+        <v>1877</v>
       </c>
       <c r="B691" s="1">
         <v>27</v>
       </c>
       <c r="C691" s="1" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="D691" s="1" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="E691" s="1" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F691" s="1" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="G691" s="1"/>
     </row>
     <row r="692" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A692" s="1" t="s">
-        <v>1888</v>
+        <v>1878</v>
       </c>
       <c r="B692" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C692" s="1" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="D692" s="1" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="E692" s="1" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="F692" s="1" t="s">
-        <v>218</v>
+        <v>179</v>
       </c>
       <c r="G692" s="1"/>
     </row>
     <row r="693" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A693" s="1" t="s">
-        <v>1889</v>
+        <v>1879</v>
       </c>
       <c r="B693" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C693" s="1" t="s">
-        <v>219</v>
+        <v>180</v>
       </c>
       <c r="D693" s="1" t="s">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="E693" s="1" t="s">
-        <v>221</v>
+        <v>182</v>
       </c>
       <c r="F693" s="1" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="G693" s="1"/>
     </row>
     <row r="694" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A694" s="1" t="s">
-        <v>1890</v>
+        <v>1880</v>
       </c>
       <c r="B694" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C694" s="1" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="D694" s="1" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="E694" s="1" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
       <c r="F694" s="1" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="G694" s="1"/>
     </row>
     <row r="695" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A695" s="1" t="s">
-        <v>1891</v>
+        <v>1881</v>
       </c>
       <c r="B695" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C695" s="1" t="s">
-        <v>227</v>
+        <v>188</v>
       </c>
       <c r="D695" s="1" t="s">
-        <v>228</v>
+        <v>189</v>
       </c>
       <c r="E695" s="1" t="s">
-        <v>229</v>
+        <v>190</v>
       </c>
       <c r="F695" s="1" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="G695" s="1"/>
     </row>
     <row r="696" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A696" s="1" t="s">
-        <v>1892</v>
+        <v>1882</v>
       </c>
       <c r="B696" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C696" s="1" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
       <c r="D696" s="1" t="s">
-        <v>232</v>
+        <v>193</v>
       </c>
       <c r="E696" s="1" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="F696" s="1" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="G696" s="1"/>
     </row>
     <row r="697" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A697" s="1" t="s">
-        <v>1893</v>
+        <v>1883</v>
       </c>
       <c r="B697" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C697" s="1" t="s">
-        <v>235</v>
+        <v>196</v>
       </c>
       <c r="D697" s="1" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="E697" s="1" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="F697" s="1" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="G697" s="1"/>
     </row>
     <row r="698" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A698" s="1" t="s">
-        <v>1894</v>
+        <v>1884</v>
       </c>
       <c r="B698" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C698" s="1" t="s">
-        <v>239</v>
+        <v>200</v>
       </c>
       <c r="D698" s="1" t="s">
-        <v>240</v>
+        <v>201</v>
       </c>
       <c r="E698" s="1" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
       <c r="F698" s="1" t="s">
-        <v>242</v>
+        <v>203</v>
       </c>
       <c r="G698" s="1"/>
     </row>
     <row r="699" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A699" s="1" t="s">
-        <v>1895</v>
+        <v>1885</v>
       </c>
       <c r="B699" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D699" s="1" t="s">
-        <v>244</v>
+        <v>205</v>
       </c>
       <c r="E699" s="1" t="s">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="F699" s="1" t="s">
-        <v>246</v>
+        <v>207</v>
       </c>
       <c r="G699" s="1"/>
     </row>
     <row r="700" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A700" s="1" t="s">
-        <v>1896</v>
+        <v>1886</v>
       </c>
       <c r="B700" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C700" s="1" t="s">
-        <v>247</v>
+        <v>204</v>
       </c>
       <c r="D700" s="1" t="s">
-        <v>248</v>
+        <v>208</v>
       </c>
       <c r="E700" s="1" t="s">
-        <v>249</v>
+        <v>209</v>
       </c>
       <c r="F700" s="1" t="s">
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="G700" s="1"/>
     </row>
     <row r="701" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A701" s="1" t="s">
-        <v>1897</v>
+        <v>1887</v>
       </c>
       <c r="B701" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C701" s="1" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="D701" s="1" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="E701" s="1" t="s">
-        <v>253</v>
+        <v>213</v>
       </c>
       <c r="F701" s="1" t="s">
-        <v>254</v>
+        <v>214</v>
       </c>
       <c r="G701" s="1"/>
     </row>
     <row r="702" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A702" s="1" t="s">
-        <v>1898</v>
+        <v>1888</v>
       </c>
       <c r="B702" s="1">
         <v>28</v>
       </c>
       <c r="C702" s="1" t="s">
-        <v>255</v>
+        <v>215</v>
       </c>
       <c r="D702" s="1" t="s">
-        <v>256</v>
+        <v>216</v>
       </c>
       <c r="E702" s="1" t="s">
-        <v>257</v>
+        <v>217</v>
       </c>
       <c r="F702" s="1" t="s">
-        <v>258</v>
+        <v>218</v>
       </c>
       <c r="G702" s="1"/>
     </row>
     <row r="703" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A703" s="1" t="s">
-        <v>1899</v>
+        <v>1889</v>
       </c>
       <c r="B703" s="1">
         <v>28</v>
       </c>
       <c r="C703" s="1" t="s">
-        <v>259</v>
+        <v>219</v>
       </c>
       <c r="D703" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E703" s="1"/>
-      <c r="F703" s="1"/>
+        <v>220</v>
+      </c>
+      <c r="E703" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F703" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G703" s="1"/>
     </row>
     <row r="704" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A704" s="1" t="s">
-        <v>1900</v>
+        <v>1890</v>
       </c>
       <c r="B704" s="1">
         <v>28</v>
       </c>
       <c r="C704" s="1" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="D704" s="1" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="E704" s="1" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="F704" s="1" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="G704" s="1"/>
     </row>
     <row r="705" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A705" s="1" t="s">
-        <v>1901</v>
+        <v>1891</v>
       </c>
       <c r="B705" s="1">
         <v>28</v>
       </c>
       <c r="C705" s="1" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="D705" s="1" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="E705" s="1" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="F705" s="1" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="G705" s="1"/>
     </row>
     <row r="706" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A706" s="1" t="s">
-        <v>1902</v>
+        <v>1892</v>
       </c>
       <c r="B706" s="1">
         <v>28</v>
       </c>
       <c r="C706" s="1" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="D706" s="1" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="E706" s="1" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="F706" s="1" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
       <c r="G706" s="1"/>
     </row>
     <row r="707" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A707" s="1" t="s">
-        <v>1903</v>
+        <v>1893</v>
       </c>
       <c r="B707" s="1">
         <v>28</v>
       </c>
       <c r="C707" s="1" t="s">
-        <v>6</v>
+        <v>235</v>
       </c>
       <c r="D707" s="1" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="E707" s="1" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
       <c r="F707" s="1" t="s">
-        <v>275</v>
+        <v>238</v>
       </c>
       <c r="G707" s="1"/>
     </row>
     <row r="708" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A708" s="1" t="s">
-        <v>1904</v>
+        <v>1894</v>
       </c>
       <c r="B708" s="1">
         <v>28</v>
       </c>
       <c r="C708" s="1" t="s">
-        <v>276</v>
+        <v>239</v>
       </c>
       <c r="D708" s="1" t="s">
-        <v>277</v>
+        <v>240</v>
       </c>
       <c r="E708" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F708" s="1"/>
+        <v>241</v>
+      </c>
+      <c r="F708" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="G708" s="1"/>
     </row>
     <row r="709" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A709" s="1" t="s">
-        <v>1905</v>
+        <v>1895</v>
       </c>
       <c r="B709" s="1">
         <v>28</v>
       </c>
       <c r="C709" s="1" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="D709" s="1" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="E709" s="1" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="F709" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="G709" s="1"/>
     </row>
     <row r="710" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A710" s="1" t="s">
-        <v>1906</v>
+        <v>1896</v>
       </c>
       <c r="B710" s="1">
         <v>28</v>
       </c>
       <c r="C710" s="1" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="D710" s="1" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="E710" s="1" t="s">
-        <v>285</v>
+        <v>249</v>
       </c>
       <c r="F710" s="1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="G710" s="1"/>
     </row>
     <row r="711" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A711" s="1" t="s">
-        <v>1907</v>
+        <v>1897</v>
       </c>
       <c r="B711" s="1">
         <v>28</v>
       </c>
       <c r="C711" s="1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="D711" s="1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="E711" s="1" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="F711" s="1" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="G711" s="1"/>
     </row>
     <row r="712" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A712" s="1" t="s">
-        <v>1908</v>
+        <v>1898</v>
       </c>
       <c r="B712" s="1">
         <v>28</v>
       </c>
       <c r="C712" s="1" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="D712" s="1" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
       <c r="E712" s="1" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
       <c r="F712" s="1" t="s">
-        <v>294</v>
+        <v>258</v>
       </c>
       <c r="G712" s="1"/>
     </row>
     <row r="713" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A713" s="1" t="s">
-        <v>1909</v>
+        <v>1899</v>
       </c>
       <c r="B713" s="1">
         <v>28</v>
       </c>
       <c r="C713" s="1" t="s">
-        <v>295</v>
+        <v>259</v>
       </c>
       <c r="D713" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E713" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F713" s="1" t="s">
-        <v>298</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="E713" s="1"/>
+      <c r="F713" s="1"/>
       <c r="G713" s="1"/>
     </row>
     <row r="714" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A714" s="1" t="s">
-        <v>1910</v>
+        <v>1900</v>
       </c>
       <c r="B714" s="1">
         <v>28</v>
       </c>
       <c r="C714" s="1" t="s">
-        <v>299</v>
+        <v>261</v>
       </c>
       <c r="D714" s="1" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
       <c r="E714" s="1" t="s">
-        <v>301</v>
+        <v>263</v>
       </c>
       <c r="F714" s="1" t="s">
-        <v>302</v>
+        <v>264</v>
       </c>
       <c r="G714" s="1"/>
     </row>
     <row r="715" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A715" s="1" t="s">
-        <v>1911</v>
+        <v>1901</v>
       </c>
       <c r="B715" s="1">
         <v>28</v>
       </c>
       <c r="C715" s="1" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
       <c r="D715" s="1" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="E715" s="1" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="F715" s="1" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="G715" s="1"/>
     </row>
     <row r="716" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A716" s="1" t="s">
-        <v>1912</v>
+        <v>1902</v>
       </c>
       <c r="B716" s="1">
         <v>28</v>
       </c>
       <c r="C716" s="1" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="D716" s="1" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="E716" s="1" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="F716" s="1" t="s">
-        <v>310</v>
+        <v>272</v>
       </c>
       <c r="G716" s="1"/>
     </row>
     <row r="717" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A717" s="1" t="s">
-        <v>1913</v>
+        <v>1903</v>
       </c>
       <c r="B717" s="1">
         <v>28</v>
       </c>
       <c r="C717" s="1" t="s">
-        <v>311</v>
+        <v>6</v>
       </c>
       <c r="D717" s="1" t="s">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="E717" s="1" t="s">
-        <v>313</v>
+        <v>274</v>
       </c>
       <c r="F717" s="1" t="s">
-        <v>314</v>
+        <v>275</v>
       </c>
       <c r="G717" s="1"/>
     </row>
     <row r="718" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A718" s="1" t="s">
-        <v>1914</v>
+        <v>1904</v>
       </c>
       <c r="B718" s="1">
         <v>28</v>
       </c>
       <c r="C718" s="1" t="s">
-        <v>315</v>
+        <v>276</v>
       </c>
       <c r="D718" s="1" t="s">
-        <v>316</v>
+        <v>277</v>
       </c>
       <c r="E718" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="F718" s="1" t="s">
-        <v>318</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="F718" s="1"/>
       <c r="G718" s="1"/>
     </row>
     <row r="719" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A719" s="1" t="s">
-        <v>1915</v>
+        <v>1905</v>
       </c>
       <c r="B719" s="1">
         <v>28</v>
       </c>
       <c r="C719" s="1" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="D719" s="1" t="s">
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="E719" s="1" t="s">
-        <v>321</v>
+        <v>281</v>
       </c>
       <c r="F719" s="1" t="s">
-        <v>322</v>
+        <v>282</v>
       </c>
       <c r="G719" s="1"/>
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A720" s="1" t="s">
-        <v>1916</v>
+        <v>1906</v>
       </c>
       <c r="B720" s="1">
         <v>28</v>
       </c>
       <c r="C720" s="1" t="s">
-        <v>323</v>
+        <v>283</v>
       </c>
       <c r="D720" s="1" t="s">
-        <v>324</v>
+        <v>284</v>
       </c>
       <c r="E720" s="1" t="s">
-        <v>325</v>
+        <v>285</v>
       </c>
       <c r="F720" s="1" t="s">
-        <v>326</v>
+        <v>286</v>
       </c>
       <c r="G720" s="1"/>
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A721" s="1" t="s">
-        <v>1917</v>
+        <v>1907</v>
       </c>
       <c r="B721" s="1">
         <v>28</v>
       </c>
       <c r="C721" s="1" t="s">
-        <v>327</v>
+        <v>287</v>
       </c>
       <c r="D721" s="1" t="s">
-        <v>328</v>
+        <v>288</v>
       </c>
       <c r="E721" s="1" t="s">
-        <v>329</v>
+        <v>289</v>
       </c>
       <c r="F721" s="1" t="s">
-        <v>330</v>
+        <v>290</v>
       </c>
       <c r="G721" s="1"/>
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A722" s="1" t="s">
-        <v>1918</v>
+        <v>1908</v>
       </c>
       <c r="B722" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C722" s="1" t="s">
-        <v>331</v>
+        <v>291</v>
       </c>
       <c r="D722" s="1" t="s">
-        <v>332</v>
+        <v>292</v>
       </c>
       <c r="E722" s="1" t="s">
-        <v>333</v>
+        <v>293</v>
       </c>
       <c r="F722" s="1" t="s">
-        <v>334</v>
+        <v>294</v>
       </c>
       <c r="G722" s="1"/>
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A723" s="1" t="s">
-        <v>1919</v>
+        <v>1909</v>
       </c>
       <c r="B723" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C723" s="1" t="s">
-        <v>335</v>
+        <v>295</v>
       </c>
       <c r="D723" s="1" t="s">
-        <v>336</v>
+        <v>296</v>
       </c>
       <c r="E723" s="1" t="s">
-        <v>337</v>
+        <v>297</v>
       </c>
       <c r="F723" s="1" t="s">
-        <v>338</v>
+        <v>298</v>
       </c>
       <c r="G723" s="1"/>
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A724" s="1" t="s">
-        <v>1920</v>
+        <v>1910</v>
       </c>
       <c r="B724" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C724" s="1" t="s">
-        <v>339</v>
+        <v>299</v>
       </c>
       <c r="D724" s="1" t="s">
-        <v>340</v>
+        <v>300</v>
       </c>
       <c r="E724" s="1" t="s">
-        <v>341</v>
+        <v>301</v>
       </c>
       <c r="F724" s="1" t="s">
-        <v>342</v>
+        <v>302</v>
       </c>
       <c r="G724" s="1"/>
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A725" s="1" t="s">
-        <v>1921</v>
+        <v>1911</v>
       </c>
       <c r="B725" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C725" s="1" t="s">
-        <v>343</v>
+        <v>303</v>
       </c>
       <c r="D725" s="1" t="s">
-        <v>344</v>
+        <v>304</v>
       </c>
       <c r="E725" s="1" t="s">
-        <v>345</v>
+        <v>305</v>
       </c>
       <c r="F725" s="1" t="s">
-        <v>346</v>
+        <v>306</v>
       </c>
       <c r="G725" s="1"/>
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A726" s="1" t="s">
-        <v>1922</v>
+        <v>1912</v>
       </c>
       <c r="B726" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C726" s="1" t="s">
-        <v>347</v>
+        <v>307</v>
       </c>
       <c r="D726" s="1" t="s">
-        <v>348</v>
+        <v>308</v>
       </c>
       <c r="E726" s="1" t="s">
-        <v>349</v>
+        <v>309</v>
       </c>
       <c r="F726" s="1" t="s">
-        <v>350</v>
+        <v>310</v>
       </c>
       <c r="G726" s="1"/>
     </row>
     <row r="727" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A727" s="1" t="s">
-        <v>1923</v>
+        <v>1913</v>
       </c>
       <c r="B727" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C727" s="1" t="s">
-        <v>351</v>
+        <v>311</v>
       </c>
       <c r="D727" s="1" t="s">
-        <v>352</v>
+        <v>312</v>
       </c>
       <c r="E727" s="1" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="F727" s="1" t="s">
-        <v>354</v>
+        <v>314</v>
       </c>
       <c r="G727" s="1"/>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A728" s="1" t="s">
-        <v>1924</v>
+        <v>1914</v>
       </c>
       <c r="B728" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C728" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="D728" s="1" t="s">
-        <v>356</v>
+        <v>316</v>
       </c>
       <c r="E728" s="1" t="s">
-        <v>357</v>
+        <v>317</v>
       </c>
       <c r="F728" s="1" t="s">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="G728" s="1"/>
     </row>
     <row r="729" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A729" s="1" t="s">
-        <v>1925</v>
+        <v>1915</v>
       </c>
       <c r="B729" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C729" s="1" t="s">
-        <v>359</v>
+        <v>319</v>
       </c>
       <c r="D729" s="1" t="s">
-        <v>360</v>
+        <v>320</v>
       </c>
       <c r="E729" s="1" t="s">
-        <v>361</v>
+        <v>321</v>
       </c>
       <c r="F729" s="1" t="s">
-        <v>362</v>
+        <v>322</v>
       </c>
       <c r="G729" s="1"/>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A730" s="1" t="s">
-        <v>1926</v>
+        <v>1916</v>
       </c>
       <c r="B730" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C730" s="1" t="s">
-        <v>363</v>
+        <v>323</v>
       </c>
       <c r="D730" s="1" t="s">
-        <v>364</v>
+        <v>324</v>
       </c>
       <c r="E730" s="1" t="s">
-        <v>365</v>
+        <v>325</v>
       </c>
       <c r="F730" s="1" t="s">
-        <v>366</v>
+        <v>326</v>
       </c>
       <c r="G730" s="1"/>
     </row>
     <row r="731" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A731" s="1" t="s">
-        <v>1927</v>
+        <v>1917</v>
       </c>
       <c r="B731" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C731" s="1" t="s">
-        <v>367</v>
+        <v>327</v>
       </c>
       <c r="D731" s="1" t="s">
-        <v>368</v>
+        <v>328</v>
       </c>
       <c r="E731" s="1" t="s">
-        <v>369</v>
+        <v>329</v>
       </c>
       <c r="F731" s="1" t="s">
-        <v>370</v>
+        <v>330</v>
       </c>
       <c r="G731" s="1"/>
     </row>
     <row r="732" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A732" s="1" t="s">
-        <v>1928</v>
+        <v>1918</v>
       </c>
       <c r="B732" s="1">
         <v>29</v>
       </c>
       <c r="C732" s="1" t="s">
-        <v>371</v>
+        <v>331</v>
       </c>
       <c r="D732" s="1" t="s">
-        <v>372</v>
+        <v>332</v>
       </c>
       <c r="E732" s="1" t="s">
-        <v>373</v>
+        <v>333</v>
       </c>
       <c r="F732" s="1" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="G732" s="1"/>
     </row>
     <row r="733" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A733" s="1" t="s">
-        <v>1929</v>
+        <v>1919</v>
       </c>
       <c r="B733" s="1">
         <v>29</v>
       </c>
       <c r="C733" s="1" t="s">
-        <v>375</v>
+        <v>335</v>
       </c>
       <c r="D733" s="1" t="s">
-        <v>376</v>
+        <v>336</v>
       </c>
       <c r="E733" s="1" t="s">
-        <v>377</v>
+        <v>337</v>
       </c>
       <c r="F733" s="1" t="s">
-        <v>378</v>
+        <v>338</v>
       </c>
       <c r="G733" s="1"/>
     </row>
     <row r="734" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A734" s="1" t="s">
-        <v>1930</v>
+        <v>1920</v>
       </c>
       <c r="B734" s="1">
         <v>29</v>
       </c>
       <c r="C734" s="1" t="s">
-        <v>379</v>
+        <v>339</v>
       </c>
       <c r="D734" s="1" t="s">
-        <v>380</v>
+        <v>340</v>
       </c>
       <c r="E734" s="1" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
       <c r="F734" s="1" t="s">
-        <v>382</v>
+        <v>342</v>
       </c>
       <c r="G734" s="1"/>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A735" s="1" t="s">
-        <v>1931</v>
+        <v>1921</v>
       </c>
       <c r="B735" s="1">
         <v>29</v>
       </c>
       <c r="C735" s="1" t="s">
-        <v>383</v>
+        <v>343</v>
       </c>
       <c r="D735" s="1" t="s">
-        <v>384</v>
+        <v>344</v>
       </c>
       <c r="E735" s="1" t="s">
-        <v>385</v>
+        <v>345</v>
       </c>
       <c r="F735" s="1" t="s">
-        <v>386</v>
+        <v>346</v>
       </c>
       <c r="G735" s="1"/>
     </row>
     <row r="736" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A736" s="1" t="s">
-        <v>1932</v>
+        <v>1922</v>
       </c>
       <c r="B736" s="1">
         <v>29</v>
       </c>
       <c r="C736" s="1" t="s">
-        <v>387</v>
+        <v>347</v>
       </c>
       <c r="D736" s="1" t="s">
-        <v>388</v>
+        <v>348</v>
       </c>
       <c r="E736" s="1" t="s">
-        <v>389</v>
+        <v>349</v>
       </c>
       <c r="F736" s="1" t="s">
-        <v>390</v>
+        <v>350</v>
       </c>
       <c r="G736" s="1"/>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A737" s="1" t="s">
-        <v>1933</v>
+        <v>1923</v>
       </c>
       <c r="B737" s="1">
         <v>29</v>
       </c>
       <c r="C737" s="1" t="s">
-        <v>391</v>
+        <v>351</v>
       </c>
       <c r="D737" s="1" t="s">
-        <v>392</v>
+        <v>352</v>
       </c>
       <c r="E737" s="1" t="s">
-        <v>393</v>
+        <v>353</v>
       </c>
       <c r="F737" s="1" t="s">
-        <v>394</v>
+        <v>354</v>
       </c>
       <c r="G737" s="1"/>
     </row>
     <row r="738" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A738" s="1" t="s">
-        <v>1934</v>
+        <v>1924</v>
       </c>
       <c r="B738" s="1">
         <v>29</v>
       </c>
       <c r="C738" s="1" t="s">
-        <v>395</v>
+        <v>355</v>
       </c>
       <c r="D738" s="1" t="s">
-        <v>396</v>
+        <v>356</v>
       </c>
       <c r="E738" s="1" t="s">
-        <v>397</v>
+        <v>357</v>
       </c>
       <c r="F738" s="1" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="G738" s="1"/>
     </row>
     <row r="739" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A739" s="1" t="s">
-        <v>1935</v>
+        <v>1925</v>
       </c>
       <c r="B739" s="1">
         <v>29</v>
       </c>
       <c r="C739" s="1" t="s">
-        <v>399</v>
+        <v>359</v>
       </c>
       <c r="D739" s="1" t="s">
-        <v>400</v>
+        <v>360</v>
       </c>
       <c r="E739" s="1" t="s">
-        <v>401</v>
+        <v>361</v>
       </c>
       <c r="F739" s="1" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
       <c r="G739" s="1"/>
     </row>
     <row r="740" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A740" s="1" t="s">
-        <v>1936</v>
+        <v>1926</v>
       </c>
       <c r="B740" s="1">
         <v>29</v>
       </c>
       <c r="C740" s="1" t="s">
-        <v>403</v>
+        <v>363</v>
       </c>
       <c r="D740" s="1" t="s">
-        <v>404</v>
+        <v>364</v>
       </c>
       <c r="E740" s="1" t="s">
-        <v>405</v>
+        <v>365</v>
       </c>
       <c r="F740" s="1" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="G740" s="1"/>
     </row>
     <row r="741" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A741" s="1" t="s">
-        <v>1937</v>
+        <v>1927</v>
       </c>
       <c r="B741" s="1">
         <v>29</v>
       </c>
       <c r="C741" s="1" t="s">
-        <v>407</v>
+        <v>367</v>
       </c>
       <c r="D741" s="1" t="s">
-        <v>408</v>
+        <v>368</v>
       </c>
       <c r="E741" s="1" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="F741" s="1" t="s">
-        <v>410</v>
+        <v>370</v>
       </c>
       <c r="G741" s="1"/>
     </row>
     <row r="742" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A742" s="1" t="s">
-        <v>1938</v>
+        <v>1928</v>
       </c>
       <c r="B742" s="1">
         <v>29</v>
       </c>
       <c r="C742" s="1" t="s">
-        <v>411</v>
+        <v>371</v>
       </c>
       <c r="D742" s="1" t="s">
-        <v>412</v>
+        <v>372</v>
       </c>
       <c r="E742" s="1" t="s">
-        <v>413</v>
+        <v>373</v>
       </c>
       <c r="F742" s="1" t="s">
-        <v>414</v>
+        <v>374</v>
       </c>
       <c r="G742" s="1"/>
     </row>
     <row r="743" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A743" s="1" t="s">
-        <v>1939</v>
+        <v>1929</v>
       </c>
       <c r="B743" s="1">
         <v>29</v>
       </c>
       <c r="C743" s="1" t="s">
-        <v>415</v>
+        <v>375</v>
       </c>
       <c r="D743" s="1" t="s">
-        <v>416</v>
+        <v>376</v>
       </c>
       <c r="E743" s="1" t="s">
-        <v>417</v>
+        <v>377</v>
       </c>
       <c r="F743" s="1" t="s">
-        <v>418</v>
+        <v>378</v>
       </c>
       <c r="G743" s="1"/>
     </row>
     <row r="744" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A744" s="1" t="s">
-        <v>1940</v>
+        <v>1930</v>
       </c>
       <c r="B744" s="1">
         <v>29</v>
       </c>
       <c r="C744" s="1" t="s">
-        <v>419</v>
+        <v>379</v>
       </c>
       <c r="D744" s="1" t="s">
-        <v>420</v>
+        <v>380</v>
       </c>
       <c r="E744" s="1" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="F744" s="1" t="s">
-        <v>422</v>
+        <v>382</v>
       </c>
       <c r="G744" s="1"/>
     </row>
     <row r="745" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A745" s="1" t="s">
-        <v>1941</v>
+        <v>1931</v>
       </c>
       <c r="B745" s="1">
         <v>29</v>
       </c>
       <c r="C745" s="1" t="s">
-        <v>423</v>
+        <v>383</v>
       </c>
       <c r="D745" s="1" t="s">
-        <v>424</v>
+        <v>384</v>
       </c>
       <c r="E745" s="1" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="F745" s="1" t="s">
-        <v>426</v>
+        <v>386</v>
       </c>
       <c r="G745" s="1"/>
     </row>
     <row r="746" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A746" s="1" t="s">
-        <v>1942</v>
+        <v>1932</v>
       </c>
       <c r="B746" s="1">
         <v>29</v>
       </c>
       <c r="C746" s="1" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="D746" s="1" t="s">
-        <v>428</v>
+        <v>388</v>
       </c>
       <c r="E746" s="1" t="s">
-        <v>429</v>
+        <v>389</v>
       </c>
       <c r="F746" s="1" t="s">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="G746" s="1"/>
     </row>
     <row r="747" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A747" s="1" t="s">
-        <v>1943</v>
+        <v>1933</v>
       </c>
       <c r="B747" s="1">
         <v>29</v>
       </c>
       <c r="C747" s="1" t="s">
-        <v>431</v>
+        <v>391</v>
       </c>
       <c r="D747" s="1" t="s">
-        <v>432</v>
+        <v>392</v>
       </c>
       <c r="E747" s="1" t="s">
-        <v>433</v>
+        <v>393</v>
       </c>
       <c r="F747" s="1" t="s">
-        <v>434</v>
+        <v>394</v>
       </c>
       <c r="G747" s="1"/>
     </row>
     <row r="748" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A748" s="1" t="s">
-        <v>1944</v>
+        <v>1934</v>
       </c>
       <c r="B748" s="1">
         <v>29</v>
       </c>
       <c r="C748" s="1" t="s">
-        <v>435</v>
+        <v>395</v>
       </c>
       <c r="D748" s="1" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="E748" s="1" t="s">
-        <v>437</v>
+        <v>397</v>
       </c>
       <c r="F748" s="1" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="G748" s="1"/>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A749" s="1" t="s">
-        <v>1945</v>
+        <v>1935</v>
       </c>
       <c r="B749" s="1">
         <v>29</v>
       </c>
       <c r="C749" s="1" t="s">
-        <v>439</v>
+        <v>399</v>
       </c>
       <c r="D749" s="1" t="s">
-        <v>440</v>
+        <v>400</v>
       </c>
       <c r="E749" s="1" t="s">
-        <v>441</v>
+        <v>401</v>
       </c>
       <c r="F749" s="1" t="s">
-        <v>442</v>
+        <v>402</v>
       </c>
       <c r="G749" s="1"/>
     </row>
     <row r="750" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A750" s="1" t="s">
-        <v>1946</v>
+        <v>1936</v>
       </c>
       <c r="B750" s="1">
         <v>29</v>
       </c>
       <c r="C750" s="1" t="s">
-        <v>443</v>
+        <v>403</v>
       </c>
       <c r="D750" s="1" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
       <c r="E750" s="1" t="s">
-        <v>445</v>
+        <v>405</v>
       </c>
       <c r="F750" s="1" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
       <c r="G750" s="1"/>
     </row>
     <row r="751" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A751" s="1" t="s">
-        <v>1947</v>
+        <v>1937</v>
       </c>
       <c r="B751" s="1">
         <v>29</v>
       </c>
       <c r="C751" s="1" t="s">
-        <v>447</v>
+        <v>407</v>
       </c>
       <c r="D751" s="1" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="E751" s="1" t="s">
-        <v>449</v>
+        <v>409</v>
       </c>
       <c r="F751" s="1" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="G751" s="1"/>
     </row>
     <row r="752" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A752" s="1" t="s">
-        <v>1948</v>
+        <v>1938</v>
       </c>
       <c r="B752" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C752" s="1" t="s">
-        <v>451</v>
+        <v>411</v>
       </c>
       <c r="D752" s="1" t="s">
-        <v>452</v>
+        <v>412</v>
       </c>
       <c r="E752" s="1" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
       <c r="F752" s="1" t="s">
-        <v>454</v>
+        <v>414</v>
       </c>
       <c r="G752" s="1"/>
     </row>
     <row r="753" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A753" s="1" t="s">
-        <v>1949</v>
+        <v>1939</v>
       </c>
       <c r="B753" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C753" s="1" t="s">
-        <v>455</v>
+        <v>415</v>
       </c>
       <c r="D753" s="1" t="s">
-        <v>456</v>
+        <v>416</v>
       </c>
       <c r="E753" s="1" t="s">
-        <v>457</v>
+        <v>417</v>
       </c>
       <c r="F753" s="1" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="G753" s="1"/>
     </row>
     <row r="754" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A754" s="1" t="s">
-        <v>1950</v>
+        <v>1940</v>
       </c>
       <c r="B754" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C754" s="1" t="s">
-        <v>459</v>
+        <v>419</v>
       </c>
       <c r="D754" s="1" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="E754" s="1" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="F754" s="1" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="G754" s="1"/>
     </row>
     <row r="755" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A755" s="1" t="s">
-        <v>1951</v>
+        <v>1941</v>
       </c>
       <c r="B755" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C755" s="1" t="s">
-        <v>463</v>
+        <v>423</v>
       </c>
       <c r="D755" s="1" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="E755" s="1" t="s">
-        <v>465</v>
+        <v>425</v>
       </c>
       <c r="F755" s="1" t="s">
-        <v>466</v>
+        <v>426</v>
       </c>
       <c r="G755" s="1"/>
     </row>
     <row r="756" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A756" s="1" t="s">
-        <v>1952</v>
+        <v>1942</v>
       </c>
       <c r="B756" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C756" s="1" t="s">
-        <v>467</v>
+        <v>427</v>
       </c>
       <c r="D756" s="1" t="s">
-        <v>468</v>
+        <v>428</v>
       </c>
       <c r="E756" s="1" t="s">
-        <v>469</v>
+        <v>429</v>
       </c>
       <c r="F756" s="1" t="s">
-        <v>470</v>
+        <v>430</v>
       </c>
       <c r="G756" s="1"/>
     </row>
     <row r="757" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A757" s="1" t="s">
-        <v>1953</v>
+        <v>1943</v>
       </c>
       <c r="B757" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C757" s="1" t="s">
-        <v>471</v>
+        <v>431</v>
       </c>
       <c r="D757" s="1" t="s">
-        <v>472</v>
+        <v>432</v>
       </c>
       <c r="E757" s="1" t="s">
-        <v>473</v>
+        <v>433</v>
       </c>
       <c r="F757" s="1" t="s">
-        <v>474</v>
+        <v>434</v>
       </c>
       <c r="G757" s="1"/>
     </row>
     <row r="758" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A758" s="1" t="s">
-        <v>1954</v>
+        <v>1944</v>
       </c>
       <c r="B758" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C758" s="1" t="s">
-        <v>475</v>
+        <v>435</v>
       </c>
       <c r="D758" s="1" t="s">
-        <v>476</v>
+        <v>436</v>
       </c>
       <c r="E758" s="1" t="s">
-        <v>477</v>
+        <v>437</v>
       </c>
       <c r="F758" s="1" t="s">
-        <v>478</v>
+        <v>438</v>
       </c>
       <c r="G758" s="1"/>
     </row>
     <row r="759" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A759" s="1" t="s">
-        <v>1955</v>
+        <v>1945</v>
       </c>
       <c r="B759" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C759" s="1" t="s">
-        <v>479</v>
+        <v>439</v>
       </c>
       <c r="D759" s="1" t="s">
-        <v>480</v>
+        <v>440</v>
       </c>
       <c r="E759" s="1" t="s">
-        <v>481</v>
+        <v>441</v>
       </c>
       <c r="F759" s="1" t="s">
-        <v>482</v>
+        <v>442</v>
       </c>
       <c r="G759" s="1"/>
     </row>
     <row r="760" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A760" s="1" t="s">
-        <v>1956</v>
+        <v>1946</v>
       </c>
       <c r="B760" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C760" s="1" t="s">
-        <v>483</v>
+        <v>443</v>
       </c>
       <c r="D760" s="1" t="s">
-        <v>484</v>
+        <v>444</v>
       </c>
       <c r="E760" s="1" t="s">
-        <v>485</v>
+        <v>445</v>
       </c>
       <c r="F760" s="1" t="s">
-        <v>486</v>
+        <v>446</v>
       </c>
       <c r="G760" s="1"/>
     </row>
     <row r="761" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A761" s="1" t="s">
-        <v>1957</v>
+        <v>1947</v>
       </c>
       <c r="B761" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C761" s="1" t="s">
-        <v>487</v>
+        <v>447</v>
       </c>
       <c r="D761" s="1" t="s">
-        <v>488</v>
+        <v>448</v>
       </c>
       <c r="E761" s="1" t="s">
-        <v>489</v>
+        <v>449</v>
       </c>
       <c r="F761" s="1" t="s">
-        <v>490</v>
+        <v>450</v>
       </c>
       <c r="G761" s="1"/>
     </row>
     <row r="762" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A762" s="1" t="s">
-        <v>1958</v>
+        <v>1948</v>
       </c>
       <c r="B762" s="1">
         <v>30</v>
       </c>
       <c r="C762" s="1" t="s">
-        <v>491</v>
+        <v>451</v>
       </c>
       <c r="D762" s="1" t="s">
-        <v>492</v>
+        <v>452</v>
       </c>
       <c r="E762" s="1" t="s">
-        <v>493</v>
+        <v>453</v>
       </c>
       <c r="F762" s="1" t="s">
-        <v>494</v>
+        <v>454</v>
       </c>
       <c r="G762" s="1"/>
     </row>
     <row r="763" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A763" s="1" t="s">
-        <v>1959</v>
+        <v>1949</v>
       </c>
       <c r="B763" s="1">
         <v>30</v>
       </c>
       <c r="C763" s="1" t="s">
-        <v>495</v>
+        <v>455</v>
       </c>
       <c r="D763" s="1" t="s">
-        <v>496</v>
+        <v>456</v>
       </c>
       <c r="E763" s="1" t="s">
-        <v>497</v>
+        <v>457</v>
       </c>
       <c r="F763" s="1" t="s">
-        <v>498</v>
+        <v>458</v>
       </c>
       <c r="G763" s="1"/>
     </row>
     <row r="764" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A764" s="1" t="s">
-        <v>1960</v>
+        <v>1950</v>
       </c>
       <c r="B764" s="1">
         <v>30</v>
       </c>
       <c r="C764" s="1" t="s">
-        <v>499</v>
+        <v>459</v>
       </c>
       <c r="D764" s="1" t="s">
-        <v>500</v>
+        <v>460</v>
       </c>
       <c r="E764" s="1" t="s">
-        <v>501</v>
+        <v>461</v>
       </c>
       <c r="F764" s="1" t="s">
-        <v>502</v>
+        <v>462</v>
       </c>
       <c r="G764" s="1"/>
     </row>
     <row r="765" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A765" s="1" t="s">
-        <v>1961</v>
+        <v>1951</v>
       </c>
       <c r="B765" s="1">
         <v>30</v>
       </c>
       <c r="C765" s="1" t="s">
-        <v>503</v>
+        <v>463</v>
       </c>
       <c r="D765" s="1" t="s">
-        <v>504</v>
+        <v>464</v>
       </c>
       <c r="E765" s="1" t="s">
-        <v>505</v>
+        <v>465</v>
       </c>
       <c r="F765" s="1" t="s">
-        <v>506</v>
+        <v>466</v>
       </c>
       <c r="G765" s="1"/>
     </row>
     <row r="766" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A766" s="1" t="s">
-        <v>1962</v>
+        <v>1952</v>
       </c>
       <c r="B766" s="1">
         <v>30</v>
       </c>
       <c r="C766" s="1" t="s">
-        <v>507</v>
+        <v>467</v>
       </c>
       <c r="D766" s="1" t="s">
-        <v>508</v>
+        <v>468</v>
       </c>
       <c r="E766" s="1" t="s">
-        <v>509</v>
+        <v>469</v>
       </c>
       <c r="F766" s="1" t="s">
-        <v>510</v>
+        <v>470</v>
       </c>
       <c r="G766" s="1"/>
     </row>
     <row r="767" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A767" s="1" t="s">
-        <v>1963</v>
+        <v>1953</v>
       </c>
       <c r="B767" s="1">
         <v>30</v>
       </c>
       <c r="C767" s="1" t="s">
-        <v>511</v>
+        <v>471</v>
       </c>
       <c r="D767" s="1" t="s">
-        <v>512</v>
+        <v>472</v>
       </c>
       <c r="E767" s="1" t="s">
-        <v>513</v>
+        <v>473</v>
       </c>
       <c r="F767" s="1" t="s">
-        <v>514</v>
+        <v>474</v>
       </c>
       <c r="G767" s="1"/>
     </row>
     <row r="768" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A768" s="1" t="s">
-        <v>1964</v>
+        <v>1954</v>
       </c>
       <c r="B768" s="1">
         <v>30</v>
       </c>
       <c r="C768" s="1" t="s">
-        <v>515</v>
+        <v>475</v>
       </c>
       <c r="D768" s="1" t="s">
-        <v>516</v>
+        <v>476</v>
       </c>
       <c r="E768" s="1" t="s">
-        <v>517</v>
+        <v>477</v>
       </c>
       <c r="F768" s="1" t="s">
-        <v>518</v>
+        <v>478</v>
       </c>
       <c r="G768" s="1"/>
     </row>
     <row r="769" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A769" s="1" t="s">
-        <v>1965</v>
+        <v>1955</v>
       </c>
       <c r="B769" s="1">
         <v>30</v>
       </c>
       <c r="C769" s="1" t="s">
-        <v>519</v>
+        <v>479</v>
       </c>
       <c r="D769" s="1" t="s">
-        <v>520</v>
+        <v>480</v>
       </c>
       <c r="E769" s="1" t="s">
-        <v>521</v>
+        <v>481</v>
       </c>
       <c r="F769" s="1" t="s">
-        <v>522</v>
+        <v>482</v>
       </c>
       <c r="G769" s="1"/>
     </row>
     <row r="770" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A770" s="1" t="s">
-        <v>1966</v>
+        <v>1956</v>
       </c>
       <c r="B770" s="1">
         <v>30</v>
       </c>
       <c r="C770" s="1" t="s">
-        <v>523</v>
+        <v>483</v>
       </c>
       <c r="D770" s="1" t="s">
-        <v>524</v>
+        <v>484</v>
       </c>
       <c r="E770" s="1" t="s">
-        <v>525</v>
+        <v>485</v>
       </c>
       <c r="F770" s="1" t="s">
-        <v>526</v>
+        <v>486</v>
       </c>
       <c r="G770" s="1"/>
     </row>
     <row r="771" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A771" s="1" t="s">
-        <v>1967</v>
+        <v>1957</v>
       </c>
       <c r="B771" s="1">
         <v>30</v>
       </c>
       <c r="C771" s="1" t="s">
-        <v>527</v>
+        <v>487</v>
       </c>
       <c r="D771" s="1" t="s">
-        <v>528</v>
+        <v>488</v>
       </c>
       <c r="E771" s="1" t="s">
-        <v>529</v>
+        <v>489</v>
       </c>
       <c r="F771" s="1" t="s">
-        <v>530</v>
+        <v>490</v>
       </c>
       <c r="G771" s="1"/>
     </row>
     <row r="772" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A772" s="1" t="s">
-        <v>1968</v>
+        <v>1958</v>
       </c>
       <c r="B772" s="1">
         <v>30</v>
       </c>
       <c r="C772" s="1" t="s">
-        <v>531</v>
+        <v>491</v>
       </c>
       <c r="D772" s="1" t="s">
-        <v>532</v>
+        <v>492</v>
       </c>
       <c r="E772" s="1" t="s">
-        <v>533</v>
+        <v>493</v>
       </c>
       <c r="F772" s="1" t="s">
-        <v>534</v>
+        <v>494</v>
       </c>
       <c r="G772" s="1"/>
     </row>
     <row r="773" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A773" s="1" t="s">
-        <v>1969</v>
+        <v>1959</v>
       </c>
       <c r="B773" s="1">
         <v>30</v>
       </c>
       <c r="C773" s="1" t="s">
-        <v>535</v>
+        <v>495</v>
       </c>
       <c r="D773" s="1" t="s">
-        <v>536</v>
+        <v>496</v>
       </c>
       <c r="E773" s="1" t="s">
-        <v>537</v>
+        <v>497</v>
       </c>
       <c r="F773" s="1" t="s">
-        <v>538</v>
+        <v>498</v>
       </c>
       <c r="G773" s="1"/>
     </row>
     <row r="774" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A774" s="1" t="s">
-        <v>1970</v>
+        <v>1960</v>
       </c>
       <c r="B774" s="1">
         <v>30</v>
       </c>
       <c r="C774" s="1" t="s">
-        <v>539</v>
+        <v>499</v>
       </c>
       <c r="D774" s="1" t="s">
-        <v>540</v>
+        <v>500</v>
       </c>
       <c r="E774" s="1" t="s">
-        <v>541</v>
+        <v>501</v>
       </c>
       <c r="F774" s="1" t="s">
-        <v>542</v>
+        <v>502</v>
       </c>
       <c r="G774" s="1"/>
     </row>
     <row r="775" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A775" s="1" t="s">
-        <v>1971</v>
+        <v>1961</v>
       </c>
       <c r="B775" s="1">
         <v>30</v>
       </c>
       <c r="C775" s="1" t="s">
-        <v>543</v>
+        <v>503</v>
       </c>
       <c r="D775" s="1" t="s">
-        <v>544</v>
+        <v>504</v>
       </c>
       <c r="E775" s="1" t="s">
-        <v>545</v>
+        <v>505</v>
       </c>
       <c r="F775" s="1" t="s">
-        <v>546</v>
+        <v>506</v>
       </c>
       <c r="G775" s="1"/>
     </row>
     <row r="776" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A776" s="1" t="s">
-        <v>1972</v>
+        <v>1962</v>
       </c>
       <c r="B776" s="1">
         <v>30</v>
       </c>
       <c r="C776" s="1" t="s">
-        <v>547</v>
+        <v>507</v>
       </c>
       <c r="D776" s="1" t="s">
-        <v>548</v>
+        <v>508</v>
       </c>
       <c r="E776" s="1" t="s">
-        <v>549</v>
+        <v>509</v>
       </c>
       <c r="F776" s="1" t="s">
-        <v>550</v>
+        <v>510</v>
       </c>
       <c r="G776" s="1"/>
     </row>
     <row r="777" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A777" s="1" t="s">
-        <v>1973</v>
+        <v>1963</v>
       </c>
       <c r="B777" s="1">
         <v>30</v>
       </c>
       <c r="C777" s="1" t="s">
-        <v>551</v>
+        <v>511</v>
       </c>
       <c r="D777" s="1" t="s">
-        <v>552</v>
+        <v>512</v>
       </c>
       <c r="E777" s="1" t="s">
-        <v>553</v>
+        <v>513</v>
       </c>
       <c r="F777" s="1" t="s">
-        <v>554</v>
+        <v>514</v>
       </c>
       <c r="G777" s="1"/>
     </row>
     <row r="778" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A778" s="1" t="s">
-        <v>1974</v>
+        <v>1964</v>
       </c>
       <c r="B778" s="1">
         <v>30</v>
       </c>
       <c r="C778" s="1" t="s">
-        <v>555</v>
+        <v>515</v>
       </c>
       <c r="D778" s="1" t="s">
-        <v>556</v>
+        <v>516</v>
       </c>
       <c r="E778" s="1" t="s">
-        <v>557</v>
+        <v>517</v>
       </c>
       <c r="F778" s="1" t="s">
-        <v>558</v>
+        <v>518</v>
       </c>
       <c r="G778" s="1"/>
     </row>
     <row r="779" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A779" s="1" t="s">
-        <v>1975</v>
+        <v>1965</v>
       </c>
       <c r="B779" s="1">
         <v>30</v>
       </c>
       <c r="C779" s="1" t="s">
-        <v>559</v>
+        <v>519</v>
       </c>
       <c r="D779" s="1" t="s">
-        <v>560</v>
+        <v>520</v>
       </c>
       <c r="E779" s="1" t="s">
-        <v>561</v>
+        <v>521</v>
       </c>
       <c r="F779" s="1" t="s">
-        <v>562</v>
+        <v>522</v>
       </c>
       <c r="G779" s="1"/>
     </row>
     <row r="780" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A780" s="1" t="s">
-        <v>1976</v>
+        <v>1966</v>
       </c>
       <c r="B780" s="1">
         <v>30</v>
       </c>
       <c r="C780" s="1" t="s">
-        <v>563</v>
+        <v>523</v>
       </c>
       <c r="D780" s="1" t="s">
-        <v>564</v>
+        <v>524</v>
       </c>
       <c r="E780" s="1" t="s">
-        <v>565</v>
+        <v>525</v>
       </c>
       <c r="F780" s="1" t="s">
-        <v>566</v>
+        <v>526</v>
       </c>
       <c r="G780" s="1"/>
     </row>
     <row r="781" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A781" s="1" t="s">
-        <v>1977</v>
+        <v>1967</v>
       </c>
       <c r="B781" s="1">
         <v>30</v>
       </c>
       <c r="C781" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D781" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="E781" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="F781" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G781" s="1"/>
+    </row>
+    <row r="782" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A782" s="1" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B782" s="1">
+        <v>30</v>
+      </c>
+      <c r="C782" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D782" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="E782" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="F782" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G782" s="1"/>
+    </row>
+    <row r="783" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A783" s="1" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B783" s="1">
+        <v>30</v>
+      </c>
+      <c r="C783" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D783" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E783" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="F783" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="G783" s="1"/>
+    </row>
+    <row r="784" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A784" s="1" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B784" s="1">
+        <v>30</v>
+      </c>
+      <c r="C784" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D784" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="E784" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="F784" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="G784" s="1"/>
+    </row>
+    <row r="785" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A785" s="1" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B785" s="1">
+        <v>30</v>
+      </c>
+      <c r="C785" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D785" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E785" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="F785" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="G785" s="1"/>
+    </row>
+    <row r="786" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A786" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B786" s="1">
+        <v>30</v>
+      </c>
+      <c r="C786" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D786" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="E786" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="F786" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="G786" s="1"/>
+    </row>
+    <row r="787" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A787" s="1" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B787" s="1">
+        <v>30</v>
+      </c>
+      <c r="C787" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D787" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="E787" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="F787" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="G787" s="1"/>
+    </row>
+    <row r="788" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A788" s="1" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B788" s="1">
+        <v>30</v>
+      </c>
+      <c r="C788" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D788" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E788" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="F788" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="G788" s="1"/>
+    </row>
+    <row r="789" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A789" s="1" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B789" s="1">
+        <v>30</v>
+      </c>
+      <c r="C789" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="D789" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="E789" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="F789" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="G789" s="1"/>
+    </row>
+    <row r="790" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A790" s="1" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B790" s="1">
+        <v>30</v>
+      </c>
+      <c r="C790" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="D790" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E790" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="F790" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="G790" s="1"/>
+    </row>
+    <row r="791" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A791" s="1" t="s">
+        <v>1977</v>
+      </c>
+      <c r="B791" s="1">
+        <v>30</v>
+      </c>
+      <c r="C791" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="D781" s="1" t="s">
+      <c r="D791" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="E781" s="1" t="s">
+      <c r="E791" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="F781" s="1" t="s">
+      <c r="F791" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="G781" s="1"/>
+      <c r="G791" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 31
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06F8F9F-D116-9244-BA32-D8837F9BDF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9DC9B5-C07C-E748-8B8D-AB1C870F3F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="500" windowWidth="22060" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5254" uniqueCount="4442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5434" uniqueCount="4592">
   <si>
     <t>ID</t>
   </si>
@@ -13356,6 +13356,456 @@
   </si>
   <si>
     <t>speak clearly</t>
+  </si>
+  <si>
+    <t>U31_01</t>
+  </si>
+  <si>
+    <t>Ví</t>
+  </si>
+  <si>
+    <t>Purse</t>
+  </si>
+  <si>
+    <t>You can carry your purse in the store</t>
+  </si>
+  <si>
+    <t>carry a purse / mang theo ví</t>
+  </si>
+  <si>
+    <t>U31_02</t>
+  </si>
+  <si>
+    <t>U31_03</t>
+  </si>
+  <si>
+    <t>U31_04</t>
+  </si>
+  <si>
+    <t>U31_05</t>
+  </si>
+  <si>
+    <t>U31_06</t>
+  </si>
+  <si>
+    <t>U31_07</t>
+  </si>
+  <si>
+    <t>U31_08</t>
+  </si>
+  <si>
+    <t>U31_09</t>
+  </si>
+  <si>
+    <t>U31_10</t>
+  </si>
+  <si>
+    <t>cắt giảm</t>
+  </si>
+  <si>
+    <t>Cut back on</t>
+  </si>
+  <si>
+    <t>The company has cut back on employees</t>
+  </si>
+  <si>
+    <t>cut back on something</t>
+  </si>
+  <si>
+    <t>Quà lưu niệm</t>
+  </si>
+  <si>
+    <t>Souvenir</t>
+  </si>
+  <si>
+    <t>Let's buy a gift at the souvenir shop</t>
+  </si>
+  <si>
+    <t>A souvenir shop</t>
+  </si>
+  <si>
+    <t>Món đồ</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>I'm missing an item in my order</t>
+  </si>
+  <si>
+    <t>missing an item / thiếu một món đồ</t>
+  </si>
+  <si>
+    <t>Trao đổi</t>
+  </si>
+  <si>
+    <t>Exchange</t>
+  </si>
+  <si>
+    <t>Can you exchange US dollars for Vietnamese dong?</t>
+  </si>
+  <si>
+    <t>exchange something for something</t>
+  </si>
+  <si>
+    <t>Lấy lại, nhận lại</t>
+  </si>
+  <si>
+    <t>Take back</t>
+  </si>
+  <si>
+    <t>the shop can take back faulty products</t>
+  </si>
+  <si>
+    <t>Take back something / nhận lại cái gì đó</t>
+  </si>
+  <si>
+    <t>Hoàn tiền</t>
+  </si>
+  <si>
+    <t>Refund</t>
+  </si>
+  <si>
+    <t>I will get a refund for the canceled flight</t>
+  </si>
+  <si>
+    <t>get a refund / được hoàn lại tiền</t>
+  </si>
+  <si>
+    <t>Nhập khẩu</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>Our restaurant imports meat from overseas</t>
+  </si>
+  <si>
+    <t>import something from somewhere</t>
+  </si>
+  <si>
+    <t>Việc giao hàng</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>Will you accept cash on delivery?</t>
+  </si>
+  <si>
+    <t>cash on delivery / thanh toán khi giao hàng</t>
+  </si>
+  <si>
+    <t>Nhận</t>
+  </si>
+  <si>
+    <t>Receive</t>
+  </si>
+  <si>
+    <t>They will receive the letter by tomorrow</t>
+  </si>
+  <si>
+    <t>Receive something</t>
+  </si>
+  <si>
+    <t>U31_11</t>
+  </si>
+  <si>
+    <t>U31_12</t>
+  </si>
+  <si>
+    <t>U31_13</t>
+  </si>
+  <si>
+    <t>U31_14</t>
+  </si>
+  <si>
+    <t>U31_15</t>
+  </si>
+  <si>
+    <t>U31_16</t>
+  </si>
+  <si>
+    <t>U31_17</t>
+  </si>
+  <si>
+    <t>U31_18</t>
+  </si>
+  <si>
+    <t>U31_19</t>
+  </si>
+  <si>
+    <t>U31_20</t>
+  </si>
+  <si>
+    <t>Trung tâm thương mại</t>
+  </si>
+  <si>
+    <t>Mall</t>
+  </si>
+  <si>
+    <t>The countryside only has one shopping mall</t>
+  </si>
+  <si>
+    <t>a shopping mall / một trung tâm mua sắm</t>
+  </si>
+  <si>
+    <t>Khuyến mãi, thỏa thuận</t>
+  </si>
+  <si>
+    <t>Business people make deals every day</t>
+  </si>
+  <si>
+    <t>deal</t>
+  </si>
+  <si>
+    <t>make a deal / đàm phán thỏa thuận</t>
+  </si>
+  <si>
+    <t>Đi khảo giá</t>
+  </si>
+  <si>
+    <t>Shop around</t>
+  </si>
+  <si>
+    <t>He takes his time shopping around for the best price</t>
+  </si>
+  <si>
+    <t>shop around for the best price / đi khảo giá để tìm mức giá tốt nhất</t>
+  </si>
+  <si>
+    <t>Chương trình khuyến mãi</t>
+  </si>
+  <si>
+    <t>Promotion</t>
+  </si>
+  <si>
+    <t>We are doing a special promotion</t>
+  </si>
+  <si>
+    <t>a special promotion</t>
+  </si>
+  <si>
+    <t>Chất lượng</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>My old shoes are of poor quality</t>
+  </si>
+  <si>
+    <t>poor quality / chất lượng kém</t>
+  </si>
+  <si>
+    <t>Giả</t>
+  </si>
+  <si>
+    <t>Fake</t>
+  </si>
+  <si>
+    <t>I accidentally bought a fake bag / tôi vô tình…</t>
+  </si>
+  <si>
+    <t>a fake bag</t>
+  </si>
+  <si>
+    <t>Mua</t>
+  </si>
+  <si>
+    <t>Purchase</t>
+  </si>
+  <si>
+    <t>They have enough money to purchase a car</t>
+  </si>
+  <si>
+    <t>purchase something</t>
+  </si>
+  <si>
+    <t>Khoản thanh toán</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>which payment method do you prefer?</t>
+  </si>
+  <si>
+    <t>Payment method</t>
+  </si>
+  <si>
+    <t>Phiếu giảm giá</t>
+  </si>
+  <si>
+    <t>Coupon</t>
+  </si>
+  <si>
+    <t>You can get discount coupons in the newspapers</t>
+  </si>
+  <si>
+    <t>a discount coupon</t>
+  </si>
+  <si>
+    <t>Bán hết sạch</t>
+  </si>
+  <si>
+    <t>Sell out</t>
+  </si>
+  <si>
+    <t>The theater quickly sold out of tickets</t>
+  </si>
+  <si>
+    <t>Sell out of tickets</t>
+  </si>
+  <si>
+    <t>U31_21</t>
+  </si>
+  <si>
+    <t>U31_22</t>
+  </si>
+  <si>
+    <t>U31_23</t>
+  </si>
+  <si>
+    <t>U31_24</t>
+  </si>
+  <si>
+    <t>U31_25</t>
+  </si>
+  <si>
+    <t>U31_26</t>
+  </si>
+  <si>
+    <t>U31_27</t>
+  </si>
+  <si>
+    <t>U31_28</t>
+  </si>
+  <si>
+    <t>U31_29</t>
+  </si>
+  <si>
+    <t>U31_30</t>
+  </si>
+  <si>
+    <t>Nhãn hàng</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Nike is a well-known brand for shoes</t>
+  </si>
+  <si>
+    <t>a well-known brand / một thương hiệu nổi tiếng</t>
+  </si>
+  <si>
+    <t>Gói hàng</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>A large package has arrived for you</t>
+  </si>
+  <si>
+    <t>A large package</t>
+  </si>
+  <si>
+    <t>Nhãn hiệu</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Always read the label carefully!</t>
+  </si>
+  <si>
+    <t>read the label / đọc nhãn hiệu</t>
+  </si>
+  <si>
+    <t>Lượng lớn, bó</t>
+  </si>
+  <si>
+    <t>Bunch</t>
+  </si>
+  <si>
+    <t>She bought a bunch of flowers for her mom</t>
+  </si>
+  <si>
+    <t>a bunch of something</t>
+  </si>
+  <si>
+    <t>Quầy thanh toán</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>We pay for the items at the checkout</t>
+  </si>
+  <si>
+    <t>at the checkout / tại quầy thanh toán</t>
+  </si>
+  <si>
+    <t>yêu cầu</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>I requested some information from the office</t>
+  </si>
+  <si>
+    <t>request something from somebody</t>
+  </si>
+  <si>
+    <t>Xếp hàng</t>
+  </si>
+  <si>
+    <t>Line up</t>
+  </si>
+  <si>
+    <t>The captain lined up the soldiers for the training</t>
+  </si>
+  <si>
+    <t>Line up something or somebody</t>
+  </si>
+  <si>
+    <t>Giỏ hàng</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>My shopping cart is full of food</t>
+  </si>
+  <si>
+    <t>A shopping cart</t>
+  </si>
+  <si>
+    <t>Nhân viên thu ngân</t>
+  </si>
+  <si>
+    <t>Cashier</t>
+  </si>
+  <si>
+    <t>You can checkout with the supermarket cashier</t>
+  </si>
+  <si>
+    <t>a supermarket cashier</t>
+  </si>
+  <si>
+    <t>Bán</t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>He sells ice cream for children in our neighborhood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sell something </t>
   </si>
 </sst>
 </file>
@@ -13720,20 +14170,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G901"/>
+  <dimension ref="A1:G931"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A728" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C752" sqref="C752"/>
+    <sheetView tabSelected="1" topLeftCell="B903" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E932" sqref="E932"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -31028,9 +31479,8 @@
       <c r="F752" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G752" s="1"/>
-    </row>
-    <row r="753" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="753" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A753" s="1" t="s">
         <v>1829</v>
       </c>
@@ -31049,9 +31499,8 @@
       <c r="F753" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G753" s="1"/>
-    </row>
-    <row r="754" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="754" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A754" s="1" t="s">
         <v>1830</v>
       </c>
@@ -31070,9 +31519,8 @@
       <c r="F754" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G754" s="1"/>
-    </row>
-    <row r="755" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="755" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A755" s="1" t="s">
         <v>1831</v>
       </c>
@@ -31091,9 +31539,8 @@
       <c r="F755" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G755" s="1"/>
-    </row>
-    <row r="756" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="756" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A756" s="1" t="s">
         <v>1832</v>
       </c>
@@ -31112,9 +31559,8 @@
       <c r="F756" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G756" s="1"/>
-    </row>
-    <row r="757" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="757" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A757" s="1" t="s">
         <v>1833</v>
       </c>
@@ -31133,9 +31579,8 @@
       <c r="F757" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G757" s="1"/>
-    </row>
-    <row r="758" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="758" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A758" s="1" t="s">
         <v>1834</v>
       </c>
@@ -31154,9 +31599,8 @@
       <c r="F758" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G758" s="1"/>
-    </row>
-    <row r="759" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="759" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A759" s="1" t="s">
         <v>1835</v>
       </c>
@@ -31175,9 +31619,8 @@
       <c r="F759" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G759" s="1"/>
-    </row>
-    <row r="760" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="760" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A760" s="1" t="s">
         <v>1836</v>
       </c>
@@ -31196,9 +31639,8 @@
       <c r="F760" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G760" s="1"/>
-    </row>
-    <row r="761" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="761" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A761" s="1" t="s">
         <v>1837</v>
       </c>
@@ -31217,9 +31659,8 @@
       <c r="F761" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G761" s="1"/>
-    </row>
-    <row r="762" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="762" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A762" s="1" t="s">
         <v>1838</v>
       </c>
@@ -31238,9 +31679,8 @@
       <c r="F762" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G762" s="1"/>
-    </row>
-    <row r="763" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="763" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A763" s="1" t="s">
         <v>1839</v>
       </c>
@@ -31259,9 +31699,8 @@
       <c r="F763" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G763" s="1"/>
-    </row>
-    <row r="764" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="764" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A764" s="1" t="s">
         <v>1840</v>
       </c>
@@ -31280,9 +31719,8 @@
       <c r="F764" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G764" s="1"/>
-    </row>
-    <row r="765" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="765" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A765" s="1" t="s">
         <v>1841</v>
       </c>
@@ -31301,9 +31739,8 @@
       <c r="F765" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G765" s="1"/>
-    </row>
-    <row r="766" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="766" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A766" s="1" t="s">
         <v>1842</v>
       </c>
@@ -31322,9 +31759,8 @@
       <c r="F766" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G766" s="1"/>
-    </row>
-    <row r="767" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="767" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A767" s="1" t="s">
         <v>1843</v>
       </c>
@@ -31343,9 +31779,8 @@
       <c r="F767" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G767" s="1"/>
-    </row>
-    <row r="768" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="768" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A768" s="1" t="s">
         <v>1844</v>
       </c>
@@ -31364,9 +31799,8 @@
       <c r="F768" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G768" s="1"/>
-    </row>
-    <row r="769" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="769" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A769" s="1" t="s">
         <v>1845</v>
       </c>
@@ -31385,9 +31819,8 @@
       <c r="F769" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G769" s="1"/>
-    </row>
-    <row r="770" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="770" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A770" s="1" t="s">
         <v>1846</v>
       </c>
@@ -31406,9 +31839,8 @@
       <c r="F770" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G770" s="1"/>
-    </row>
-    <row r="771" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="771" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A771" s="1" t="s">
         <v>1847</v>
       </c>
@@ -31427,9 +31859,8 @@
       <c r="F771" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G771" s="1"/>
-    </row>
-    <row r="772" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="772" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A772" s="1" t="s">
         <v>1848</v>
       </c>
@@ -31448,9 +31879,8 @@
       <c r="F772" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G772" s="1"/>
-    </row>
-    <row r="773" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="773" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A773" s="1" t="s">
         <v>1849</v>
       </c>
@@ -31469,9 +31899,8 @@
       <c r="F773" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G773" s="1"/>
-    </row>
-    <row r="774" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="774" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A774" s="1" t="s">
         <v>1850</v>
       </c>
@@ -31490,9 +31919,8 @@
       <c r="F774" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G774" s="1"/>
-    </row>
-    <row r="775" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="775" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A775" s="1" t="s">
         <v>1851</v>
       </c>
@@ -31511,9 +31939,8 @@
       <c r="F775" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G775" s="1"/>
-    </row>
-    <row r="776" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="776" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A776" s="1" t="s">
         <v>1852</v>
       </c>
@@ -31532,9 +31959,8 @@
       <c r="F776" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G776" s="1"/>
-    </row>
-    <row r="777" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="777" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A777" s="1" t="s">
         <v>1853</v>
       </c>
@@ -31553,9 +31979,8 @@
       <c r="F777" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G777" s="1"/>
-    </row>
-    <row r="778" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="778" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A778" s="1" t="s">
         <v>1854</v>
       </c>
@@ -31574,9 +31999,8 @@
       <c r="F778" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G778" s="1"/>
-    </row>
-    <row r="779" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="779" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A779" s="1" t="s">
         <v>1855</v>
       </c>
@@ -31595,9 +32019,8 @@
       <c r="F779" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G779" s="1"/>
-    </row>
-    <row r="780" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="780" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A780" s="1" t="s">
         <v>1856</v>
       </c>
@@ -31616,9 +32039,8 @@
       <c r="F780" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G780" s="1"/>
-    </row>
-    <row r="781" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="781" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A781" s="1" t="s">
         <v>1857</v>
       </c>
@@ -31637,9 +32059,8 @@
       <c r="F781" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G781" s="1"/>
-    </row>
-    <row r="782" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="782" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A782" s="1" t="s">
         <v>1858</v>
       </c>
@@ -31658,9 +32079,8 @@
       <c r="F782" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G782" s="1"/>
-    </row>
-    <row r="783" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="783" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A783" s="1" t="s">
         <v>1859</v>
       </c>
@@ -31679,9 +32099,8 @@
       <c r="F783" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G783" s="1"/>
-    </row>
-    <row r="784" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="784" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A784" s="1" t="s">
         <v>1860</v>
       </c>
@@ -31700,9 +32119,8 @@
       <c r="F784" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G784" s="1"/>
-    </row>
-    <row r="785" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="785" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A785" s="1" t="s">
         <v>1861</v>
       </c>
@@ -31721,9 +32139,8 @@
       <c r="F785" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G785" s="1"/>
-    </row>
-    <row r="786" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="786" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A786" s="1" t="s">
         <v>1862</v>
       </c>
@@ -31742,9 +32159,8 @@
       <c r="F786" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G786" s="1"/>
-    </row>
-    <row r="787" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="787" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A787" s="1" t="s">
         <v>1863</v>
       </c>
@@ -31763,9 +32179,8 @@
       <c r="F787" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G787" s="1"/>
-    </row>
-    <row r="788" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="788" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A788" s="1" t="s">
         <v>1864</v>
       </c>
@@ -31784,9 +32199,8 @@
       <c r="F788" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G788" s="1"/>
-    </row>
-    <row r="789" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="789" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A789" s="1" t="s">
         <v>1865</v>
       </c>
@@ -31805,9 +32219,8 @@
       <c r="F789" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G789" s="1"/>
-    </row>
-    <row r="790" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="790" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A790" s="1" t="s">
         <v>1866</v>
       </c>
@@ -31826,9 +32239,8 @@
       <c r="F790" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G790" s="1"/>
-    </row>
-    <row r="791" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="791" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A791" s="1" t="s">
         <v>1867</v>
       </c>
@@ -31847,9 +32259,8 @@
       <c r="F791" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G791" s="1"/>
-    </row>
-    <row r="792" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="792" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A792" s="1" t="s">
         <v>1868</v>
       </c>
@@ -31868,9 +32279,8 @@
       <c r="F792" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G792" s="1"/>
-    </row>
-    <row r="793" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="793" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A793" s="1" t="s">
         <v>1869</v>
       </c>
@@ -31889,9 +32299,8 @@
       <c r="F793" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G793" s="1"/>
-    </row>
-    <row r="794" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="794" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A794" s="1" t="s">
         <v>1870</v>
       </c>
@@ -31910,9 +32319,8 @@
       <c r="F794" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G794" s="1"/>
-    </row>
-    <row r="795" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="795" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A795" s="1" t="s">
         <v>1871</v>
       </c>
@@ -31931,9 +32339,8 @@
       <c r="F795" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G795" s="1"/>
-    </row>
-    <row r="796" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="796" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A796" s="1" t="s">
         <v>1872</v>
       </c>
@@ -31952,9 +32359,8 @@
       <c r="F796" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G796" s="1"/>
-    </row>
-    <row r="797" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="797" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A797" s="1" t="s">
         <v>1873</v>
       </c>
@@ -31973,9 +32379,8 @@
       <c r="F797" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G797" s="1"/>
-    </row>
-    <row r="798" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="798" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A798" s="1" t="s">
         <v>1874</v>
       </c>
@@ -31994,9 +32399,8 @@
       <c r="F798" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G798" s="1"/>
-    </row>
-    <row r="799" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="799" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A799" s="1" t="s">
         <v>1875</v>
       </c>
@@ -32015,9 +32419,8 @@
       <c r="F799" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G799" s="1"/>
-    </row>
-    <row r="800" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="800" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A800" s="1" t="s">
         <v>1876</v>
       </c>
@@ -32036,9 +32439,8 @@
       <c r="F800" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G800" s="1"/>
-    </row>
-    <row r="801" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="801" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A801" s="1" t="s">
         <v>1877</v>
       </c>
@@ -32057,9 +32459,8 @@
       <c r="F801" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G801" s="1"/>
-    </row>
-    <row r="802" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="802" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A802" s="1" t="s">
         <v>1878</v>
       </c>
@@ -32078,9 +32479,8 @@
       <c r="F802" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G802" s="1"/>
-    </row>
-    <row r="803" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="803" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A803" s="1" t="s">
         <v>1879</v>
       </c>
@@ -32099,9 +32499,8 @@
       <c r="F803" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G803" s="1"/>
-    </row>
-    <row r="804" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="804" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A804" s="1" t="s">
         <v>1880</v>
       </c>
@@ -32120,9 +32519,8 @@
       <c r="F804" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G804" s="1"/>
-    </row>
-    <row r="805" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="805" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A805" s="1" t="s">
         <v>1881</v>
       </c>
@@ -32141,9 +32539,8 @@
       <c r="F805" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="G805" s="1"/>
-    </row>
-    <row r="806" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="806" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A806" s="1" t="s">
         <v>1882</v>
       </c>
@@ -32162,9 +32559,8 @@
       <c r="F806" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G806" s="1"/>
-    </row>
-    <row r="807" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="807" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A807" s="1" t="s">
         <v>1883</v>
       </c>
@@ -32183,9 +32579,8 @@
       <c r="F807" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G807" s="1"/>
-    </row>
-    <row r="808" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="808" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A808" s="1" t="s">
         <v>1884</v>
       </c>
@@ -32204,9 +32599,8 @@
       <c r="F808" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G808" s="1"/>
-    </row>
-    <row r="809" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="809" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A809" s="1" t="s">
         <v>1885</v>
       </c>
@@ -32225,9 +32619,8 @@
       <c r="F809" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G809" s="1"/>
-    </row>
-    <row r="810" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="810" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A810" s="1" t="s">
         <v>1886</v>
       </c>
@@ -32246,9 +32639,8 @@
       <c r="F810" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G810" s="1"/>
-    </row>
-    <row r="811" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="811" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A811" s="1" t="s">
         <v>1887</v>
       </c>
@@ -32267,9 +32659,8 @@
       <c r="F811" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="G811" s="1"/>
-    </row>
-    <row r="812" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="812" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A812" s="1" t="s">
         <v>1888</v>
       </c>
@@ -32288,9 +32679,8 @@
       <c r="F812" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="G812" s="1"/>
-    </row>
-    <row r="813" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="813" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A813" s="1" t="s">
         <v>1889</v>
       </c>
@@ -32309,9 +32699,8 @@
       <c r="F813" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G813" s="1"/>
-    </row>
-    <row r="814" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="814" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A814" s="1" t="s">
         <v>1890</v>
       </c>
@@ -32330,9 +32719,8 @@
       <c r="F814" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="G814" s="1"/>
-    </row>
-    <row r="815" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="815" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A815" s="1" t="s">
         <v>1891</v>
       </c>
@@ -32351,9 +32739,8 @@
       <c r="F815" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G815" s="1"/>
-    </row>
-    <row r="816" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="816" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A816" s="1" t="s">
         <v>1892</v>
       </c>
@@ -32372,9 +32759,8 @@
       <c r="F816" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="G816" s="1"/>
-    </row>
-    <row r="817" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="817" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A817" s="1" t="s">
         <v>1893</v>
       </c>
@@ -32393,9 +32779,8 @@
       <c r="F817" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="G817" s="1"/>
-    </row>
-    <row r="818" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="818" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A818" s="1" t="s">
         <v>1894</v>
       </c>
@@ -32414,9 +32799,8 @@
       <c r="F818" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="G818" s="1"/>
-    </row>
-    <row r="819" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="819" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A819" s="1" t="s">
         <v>1895</v>
       </c>
@@ -32435,9 +32819,8 @@
       <c r="F819" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="G819" s="1"/>
-    </row>
-    <row r="820" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="820" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A820" s="1" t="s">
         <v>1896</v>
       </c>
@@ -32456,9 +32839,8 @@
       <c r="F820" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="G820" s="1"/>
-    </row>
-    <row r="821" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="821" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A821" s="1" t="s">
         <v>1897</v>
       </c>
@@ -32477,9 +32859,8 @@
       <c r="F821" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="G821" s="1"/>
-    </row>
-    <row r="822" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="822" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A822" s="1" t="s">
         <v>1898</v>
       </c>
@@ -32498,9 +32879,8 @@
       <c r="F822" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="G822" s="1"/>
-    </row>
-    <row r="823" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="823" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A823" s="1" t="s">
         <v>1899</v>
       </c>
@@ -32513,11 +32893,8 @@
       <c r="D823" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E823" s="1"/>
-      <c r="F823" s="1"/>
-      <c r="G823" s="1"/>
-    </row>
-    <row r="824" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="824" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A824" s="1" t="s">
         <v>1900</v>
       </c>
@@ -32536,9 +32913,8 @@
       <c r="F824" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G824" s="1"/>
-    </row>
-    <row r="825" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="825" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A825" s="1" t="s">
         <v>1901</v>
       </c>
@@ -32557,9 +32933,8 @@
       <c r="F825" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G825" s="1"/>
-    </row>
-    <row r="826" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="826" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A826" s="1" t="s">
         <v>1902</v>
       </c>
@@ -32578,9 +32953,8 @@
       <c r="F826" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G826" s="1"/>
-    </row>
-    <row r="827" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="827" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A827" s="1" t="s">
         <v>1903</v>
       </c>
@@ -32599,9 +32973,8 @@
       <c r="F827" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G827" s="1"/>
-    </row>
-    <row r="828" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="828" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A828" s="1" t="s">
         <v>1904</v>
       </c>
@@ -32617,10 +32990,8 @@
       <c r="E828" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="F828" s="1"/>
-      <c r="G828" s="1"/>
-    </row>
-    <row r="829" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="829" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A829" s="1" t="s">
         <v>1905</v>
       </c>
@@ -32639,9 +33010,8 @@
       <c r="F829" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="G829" s="1"/>
-    </row>
-    <row r="830" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="830" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A830" s="1" t="s">
         <v>1906</v>
       </c>
@@ -32660,9 +33030,8 @@
       <c r="F830" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G830" s="1"/>
-    </row>
-    <row r="831" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="831" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A831" s="1" t="s">
         <v>1907</v>
       </c>
@@ -32681,9 +33050,8 @@
       <c r="F831" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="G831" s="1"/>
-    </row>
-    <row r="832" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="832" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A832" s="1" t="s">
         <v>1908</v>
       </c>
@@ -32702,9 +33070,8 @@
       <c r="F832" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="G832" s="1"/>
-    </row>
-    <row r="833" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="833" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A833" s="1" t="s">
         <v>1909</v>
       </c>
@@ -32723,9 +33090,8 @@
       <c r="F833" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="G833" s="1"/>
-    </row>
-    <row r="834" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="834" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A834" s="1" t="s">
         <v>1910</v>
       </c>
@@ -32744,9 +33110,8 @@
       <c r="F834" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="G834" s="1"/>
-    </row>
-    <row r="835" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="835" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A835" s="1" t="s">
         <v>1911</v>
       </c>
@@ -32765,9 +33130,8 @@
       <c r="F835" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G835" s="1"/>
-    </row>
-    <row r="836" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="836" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A836" s="1" t="s">
         <v>1912</v>
       </c>
@@ -32786,9 +33150,8 @@
       <c r="F836" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="G836" s="1"/>
-    </row>
-    <row r="837" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="837" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A837" s="1" t="s">
         <v>1913</v>
       </c>
@@ -32807,9 +33170,8 @@
       <c r="F837" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G837" s="1"/>
-    </row>
-    <row r="838" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="838" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A838" s="1" t="s">
         <v>1914</v>
       </c>
@@ -32828,9 +33190,8 @@
       <c r="F838" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G838" s="1"/>
-    </row>
-    <row r="839" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="839" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A839" s="1" t="s">
         <v>1915</v>
       </c>
@@ -32849,9 +33210,8 @@
       <c r="F839" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="G839" s="1"/>
-    </row>
-    <row r="840" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="840" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A840" s="1" t="s">
         <v>1916</v>
       </c>
@@ -32870,9 +33230,8 @@
       <c r="F840" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="G840" s="1"/>
-    </row>
-    <row r="841" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="841" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A841" s="1" t="s">
         <v>1917</v>
       </c>
@@ -32891,9 +33250,8 @@
       <c r="F841" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="G841" s="1"/>
-    </row>
-    <row r="842" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="842" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A842" s="1" t="s">
         <v>1918</v>
       </c>
@@ -32912,9 +33270,8 @@
       <c r="F842" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="G842" s="1"/>
-    </row>
-    <row r="843" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="843" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A843" s="1" t="s">
         <v>1919</v>
       </c>
@@ -32933,9 +33290,8 @@
       <c r="F843" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="G843" s="1"/>
-    </row>
-    <row r="844" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="844" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A844" s="1" t="s">
         <v>1920</v>
       </c>
@@ -32954,9 +33310,8 @@
       <c r="F844" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="G844" s="1"/>
-    </row>
-    <row r="845" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="845" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A845" s="1" t="s">
         <v>1921</v>
       </c>
@@ -32975,9 +33330,8 @@
       <c r="F845" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="G845" s="1"/>
-    </row>
-    <row r="846" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="846" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A846" s="1" t="s">
         <v>1922</v>
       </c>
@@ -32996,9 +33350,8 @@
       <c r="F846" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="G846" s="1"/>
-    </row>
-    <row r="847" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="847" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A847" s="1" t="s">
         <v>1923</v>
       </c>
@@ -33017,9 +33370,8 @@
       <c r="F847" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="G847" s="1"/>
-    </row>
-    <row r="848" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="848" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A848" s="1" t="s">
         <v>1924</v>
       </c>
@@ -33038,9 +33390,8 @@
       <c r="F848" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="G848" s="1"/>
-    </row>
-    <row r="849" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="849" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A849" s="1" t="s">
         <v>1925</v>
       </c>
@@ -33059,9 +33410,8 @@
       <c r="F849" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="G849" s="1"/>
-    </row>
-    <row r="850" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="850" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A850" s="1" t="s">
         <v>1926</v>
       </c>
@@ -33080,9 +33430,8 @@
       <c r="F850" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="G850" s="1"/>
-    </row>
-    <row r="851" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="851" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A851" s="1" t="s">
         <v>1927</v>
       </c>
@@ -33101,9 +33450,8 @@
       <c r="F851" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="G851" s="1"/>
-    </row>
-    <row r="852" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="852" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A852" s="1" t="s">
         <v>1928</v>
       </c>
@@ -33122,9 +33470,8 @@
       <c r="F852" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="G852" s="1"/>
-    </row>
-    <row r="853" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="853" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A853" s="1" t="s">
         <v>1929</v>
       </c>
@@ -33143,9 +33490,8 @@
       <c r="F853" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="G853" s="1"/>
-    </row>
-    <row r="854" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="854" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A854" s="1" t="s">
         <v>1930</v>
       </c>
@@ -33164,9 +33510,8 @@
       <c r="F854" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="G854" s="1"/>
-    </row>
-    <row r="855" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="855" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A855" s="1" t="s">
         <v>1931</v>
       </c>
@@ -33185,9 +33530,8 @@
       <c r="F855" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="G855" s="1"/>
-    </row>
-    <row r="856" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="856" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A856" s="1" t="s">
         <v>1932</v>
       </c>
@@ -33206,9 +33550,8 @@
       <c r="F856" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="G856" s="1"/>
-    </row>
-    <row r="857" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="857" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A857" s="1" t="s">
         <v>1933</v>
       </c>
@@ -33227,9 +33570,8 @@
       <c r="F857" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="G857" s="1"/>
-    </row>
-    <row r="858" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="858" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A858" s="1" t="s">
         <v>1934</v>
       </c>
@@ -33248,9 +33590,8 @@
       <c r="F858" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="G858" s="1"/>
-    </row>
-    <row r="859" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="859" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A859" s="1" t="s">
         <v>1935</v>
       </c>
@@ -33269,9 +33610,8 @@
       <c r="F859" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="G859" s="1"/>
-    </row>
-    <row r="860" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="860" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A860" s="1" t="s">
         <v>1936</v>
       </c>
@@ -33290,9 +33630,8 @@
       <c r="F860" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="G860" s="1"/>
-    </row>
-    <row r="861" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="861" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A861" s="1" t="s">
         <v>1937</v>
       </c>
@@ -33311,9 +33650,8 @@
       <c r="F861" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="G861" s="1"/>
-    </row>
-    <row r="862" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="862" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A862" s="1" t="s">
         <v>1938</v>
       </c>
@@ -33332,9 +33670,8 @@
       <c r="F862" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="G862" s="1"/>
-    </row>
-    <row r="863" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="863" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A863" s="1" t="s">
         <v>1939</v>
       </c>
@@ -33353,9 +33690,8 @@
       <c r="F863" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="G863" s="1"/>
-    </row>
-    <row r="864" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="864" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A864" s="1" t="s">
         <v>1940</v>
       </c>
@@ -33374,9 +33710,8 @@
       <c r="F864" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G864" s="1"/>
-    </row>
-    <row r="865" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="865" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A865" s="1" t="s">
         <v>1941</v>
       </c>
@@ -33395,9 +33730,8 @@
       <c r="F865" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="G865" s="1"/>
-    </row>
-    <row r="866" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="866" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A866" s="1" t="s">
         <v>1942</v>
       </c>
@@ -33416,9 +33750,8 @@
       <c r="F866" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="G866" s="1"/>
-    </row>
-    <row r="867" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="867" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A867" s="1" t="s">
         <v>1943</v>
       </c>
@@ -33437,9 +33770,8 @@
       <c r="F867" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="G867" s="1"/>
-    </row>
-    <row r="868" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="868" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A868" s="1" t="s">
         <v>1944</v>
       </c>
@@ -33458,9 +33790,8 @@
       <c r="F868" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="G868" s="1"/>
-    </row>
-    <row r="869" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="869" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A869" s="1" t="s">
         <v>1945</v>
       </c>
@@ -33479,9 +33810,8 @@
       <c r="F869" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="G869" s="1"/>
-    </row>
-    <row r="870" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="870" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A870" s="1" t="s">
         <v>1946</v>
       </c>
@@ -33500,9 +33830,8 @@
       <c r="F870" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="G870" s="1"/>
-    </row>
-    <row r="871" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="871" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A871" s="1" t="s">
         <v>1947</v>
       </c>
@@ -33521,9 +33850,8 @@
       <c r="F871" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="G871" s="1"/>
-    </row>
-    <row r="872" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="872" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A872" s="1" t="s">
         <v>1948</v>
       </c>
@@ -33542,9 +33870,8 @@
       <c r="F872" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="G872" s="1"/>
-    </row>
-    <row r="873" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="873" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A873" s="1" t="s">
         <v>1949</v>
       </c>
@@ -33563,9 +33890,8 @@
       <c r="F873" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="G873" s="1"/>
-    </row>
-    <row r="874" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="874" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A874" s="1" t="s">
         <v>1950</v>
       </c>
@@ -33584,9 +33910,8 @@
       <c r="F874" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="G874" s="1"/>
-    </row>
-    <row r="875" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="875" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A875" s="1" t="s">
         <v>1951</v>
       </c>
@@ -33605,9 +33930,8 @@
       <c r="F875" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="G875" s="1"/>
-    </row>
-    <row r="876" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="876" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A876" s="1" t="s">
         <v>1952</v>
       </c>
@@ -33626,9 +33950,8 @@
       <c r="F876" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="G876" s="1"/>
-    </row>
-    <row r="877" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="877" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A877" s="1" t="s">
         <v>1953</v>
       </c>
@@ -33647,9 +33970,8 @@
       <c r="F877" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="G877" s="1"/>
-    </row>
-    <row r="878" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="878" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A878" s="1" t="s">
         <v>1954</v>
       </c>
@@ -33668,9 +33990,8 @@
       <c r="F878" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="G878" s="1"/>
-    </row>
-    <row r="879" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="879" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A879" s="1" t="s">
         <v>1955</v>
       </c>
@@ -33689,9 +34010,8 @@
       <c r="F879" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="G879" s="1"/>
-    </row>
-    <row r="880" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="880" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A880" s="1" t="s">
         <v>1956</v>
       </c>
@@ -33710,9 +34030,8 @@
       <c r="F880" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="G880" s="1"/>
-    </row>
-    <row r="881" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="881" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A881" s="1" t="s">
         <v>1957</v>
       </c>
@@ -33731,9 +34050,8 @@
       <c r="F881" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="G881" s="1"/>
-    </row>
-    <row r="882" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="882" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A882" s="1" t="s">
         <v>1958</v>
       </c>
@@ -33752,9 +34070,8 @@
       <c r="F882" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="G882" s="1"/>
-    </row>
-    <row r="883" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="883" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A883" s="1" t="s">
         <v>1959</v>
       </c>
@@ -33773,9 +34090,8 @@
       <c r="F883" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="G883" s="1"/>
-    </row>
-    <row r="884" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="884" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A884" s="1" t="s">
         <v>1960</v>
       </c>
@@ -33794,9 +34110,8 @@
       <c r="F884" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="G884" s="1"/>
-    </row>
-    <row r="885" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="885" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A885" s="1" t="s">
         <v>1961</v>
       </c>
@@ -33815,9 +34130,8 @@
       <c r="F885" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="G885" s="1"/>
-    </row>
-    <row r="886" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="886" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A886" s="1" t="s">
         <v>1962</v>
       </c>
@@ -33836,9 +34150,8 @@
       <c r="F886" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="G886" s="1"/>
-    </row>
-    <row r="887" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="887" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A887" s="1" t="s">
         <v>1963</v>
       </c>
@@ -33857,9 +34170,8 @@
       <c r="F887" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="G887" s="1"/>
-    </row>
-    <row r="888" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="888" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A888" s="1" t="s">
         <v>1964</v>
       </c>
@@ -33878,9 +34190,8 @@
       <c r="F888" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="G888" s="1"/>
-    </row>
-    <row r="889" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="889" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A889" s="1" t="s">
         <v>1965</v>
       </c>
@@ -33899,9 +34210,8 @@
       <c r="F889" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="G889" s="1"/>
-    </row>
-    <row r="890" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="890" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A890" s="1" t="s">
         <v>1966</v>
       </c>
@@ -33920,9 +34230,8 @@
       <c r="F890" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="G890" s="1"/>
-    </row>
-    <row r="891" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="891" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A891" s="1" t="s">
         <v>1967</v>
       </c>
@@ -33941,9 +34250,8 @@
       <c r="F891" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="G891" s="1"/>
-    </row>
-    <row r="892" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="892" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A892" s="1" t="s">
         <v>1968</v>
       </c>
@@ -33962,9 +34270,8 @@
       <c r="F892" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="G892" s="1"/>
-    </row>
-    <row r="893" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="893" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A893" s="1" t="s">
         <v>1969</v>
       </c>
@@ -33983,9 +34290,8 @@
       <c r="F893" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="G893" s="1"/>
-    </row>
-    <row r="894" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="894" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A894" s="1" t="s">
         <v>1970</v>
       </c>
@@ -34004,9 +34310,8 @@
       <c r="F894" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="G894" s="1"/>
-    </row>
-    <row r="895" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="895" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A895" s="1" t="s">
         <v>1971</v>
       </c>
@@ -34025,9 +34330,8 @@
       <c r="F895" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="G895" s="1"/>
-    </row>
-    <row r="896" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="896" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A896" s="1" t="s">
         <v>1972</v>
       </c>
@@ -34046,7 +34350,6 @@
       <c r="F896" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="G896" s="1"/>
     </row>
     <row r="897" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A897" s="1" t="s">
@@ -34067,7 +34370,6 @@
       <c r="F897" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="G897" s="1"/>
     </row>
     <row r="898" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A898" s="1" t="s">
@@ -34088,7 +34390,6 @@
       <c r="F898" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="G898" s="1"/>
     </row>
     <row r="899" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A899" s="1" t="s">
@@ -34109,7 +34410,6 @@
       <c r="F899" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="G899" s="1"/>
     </row>
     <row r="900" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A900" s="1" t="s">
@@ -34130,7 +34430,6 @@
       <c r="F900" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="G900" s="1"/>
     </row>
     <row r="901" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A901" s="1" t="s">
@@ -34151,7 +34450,696 @@
       <c r="F901" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="G901" s="1"/>
+    </row>
+    <row r="902" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A902" s="1" t="s">
+        <v>4442</v>
+      </c>
+      <c r="B902" s="1">
+        <v>31</v>
+      </c>
+      <c r="C902" s="1" t="s">
+        <v>4443</v>
+      </c>
+      <c r="D902" s="1" t="s">
+        <v>4444</v>
+      </c>
+      <c r="E902" s="1" t="s">
+        <v>4445</v>
+      </c>
+      <c r="F902" s="1" t="s">
+        <v>4446</v>
+      </c>
+      <c r="G902" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="903" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A903" s="1" t="s">
+        <v>4447</v>
+      </c>
+      <c r="B903" s="1">
+        <v>31</v>
+      </c>
+      <c r="C903" s="1" t="s">
+        <v>4456</v>
+      </c>
+      <c r="D903" s="1" t="s">
+        <v>4457</v>
+      </c>
+      <c r="E903" s="1" t="s">
+        <v>4458</v>
+      </c>
+      <c r="F903" s="1" t="s">
+        <v>4459</v>
+      </c>
+      <c r="G903" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="904" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A904" s="1" t="s">
+        <v>4448</v>
+      </c>
+      <c r="B904" s="1">
+        <v>31</v>
+      </c>
+      <c r="C904" s="1" t="s">
+        <v>4460</v>
+      </c>
+      <c r="D904" s="1" t="s">
+        <v>4461</v>
+      </c>
+      <c r="E904" s="1" t="s">
+        <v>4462</v>
+      </c>
+      <c r="F904" s="1" t="s">
+        <v>4463</v>
+      </c>
+      <c r="G904" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="905" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A905" s="1" t="s">
+        <v>4449</v>
+      </c>
+      <c r="B905" s="1">
+        <v>31</v>
+      </c>
+      <c r="C905" s="1" t="s">
+        <v>4464</v>
+      </c>
+      <c r="D905" s="1" t="s">
+        <v>4465</v>
+      </c>
+      <c r="E905" s="1" t="s">
+        <v>4466</v>
+      </c>
+      <c r="F905" s="1" t="s">
+        <v>4467</v>
+      </c>
+      <c r="G905" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="906" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A906" s="1" t="s">
+        <v>4450</v>
+      </c>
+      <c r="B906" s="1">
+        <v>31</v>
+      </c>
+      <c r="C906" s="1" t="s">
+        <v>4468</v>
+      </c>
+      <c r="D906" s="1" t="s">
+        <v>4469</v>
+      </c>
+      <c r="E906" s="1" t="s">
+        <v>4470</v>
+      </c>
+      <c r="F906" s="1" t="s">
+        <v>4471</v>
+      </c>
+      <c r="G906" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="907" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A907" s="1" t="s">
+        <v>4451</v>
+      </c>
+      <c r="B907" s="1">
+        <v>31</v>
+      </c>
+      <c r="C907" s="1" t="s">
+        <v>4472</v>
+      </c>
+      <c r="D907" s="1" t="s">
+        <v>4473</v>
+      </c>
+      <c r="E907" s="1" t="s">
+        <v>4474</v>
+      </c>
+      <c r="F907" s="1" t="s">
+        <v>4475</v>
+      </c>
+      <c r="G907" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="908" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A908" s="1" t="s">
+        <v>4452</v>
+      </c>
+      <c r="B908" s="1">
+        <v>31</v>
+      </c>
+      <c r="C908" s="1" t="s">
+        <v>4476</v>
+      </c>
+      <c r="D908" s="1" t="s">
+        <v>4477</v>
+      </c>
+      <c r="E908" s="1" t="s">
+        <v>4478</v>
+      </c>
+      <c r="F908" s="1" t="s">
+        <v>4479</v>
+      </c>
+      <c r="G908" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="909" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A909" s="1" t="s">
+        <v>4453</v>
+      </c>
+      <c r="B909" s="1">
+        <v>31</v>
+      </c>
+      <c r="C909" s="1" t="s">
+        <v>4480</v>
+      </c>
+      <c r="D909" s="1" t="s">
+        <v>4481</v>
+      </c>
+      <c r="E909" s="1" t="s">
+        <v>4482</v>
+      </c>
+      <c r="F909" s="1" t="s">
+        <v>4483</v>
+      </c>
+      <c r="G909" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="910" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A910" s="1" t="s">
+        <v>4454</v>
+      </c>
+      <c r="B910" s="1">
+        <v>31</v>
+      </c>
+      <c r="C910" s="1" t="s">
+        <v>4484</v>
+      </c>
+      <c r="D910" s="1" t="s">
+        <v>4485</v>
+      </c>
+      <c r="E910" s="1" t="s">
+        <v>4486</v>
+      </c>
+      <c r="F910" s="1" t="s">
+        <v>4487</v>
+      </c>
+      <c r="G910" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="911" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A911" s="1" t="s">
+        <v>4455</v>
+      </c>
+      <c r="B911" s="1">
+        <v>31</v>
+      </c>
+      <c r="C911" s="1" t="s">
+        <v>4488</v>
+      </c>
+      <c r="D911" s="1" t="s">
+        <v>4489</v>
+      </c>
+      <c r="E911" s="1" t="s">
+        <v>4490</v>
+      </c>
+      <c r="F911" s="1" t="s">
+        <v>4491</v>
+      </c>
+      <c r="G911" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="912" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A912" s="1" t="s">
+        <v>4492</v>
+      </c>
+      <c r="B912" s="1">
+        <v>31</v>
+      </c>
+      <c r="C912" s="1" t="s">
+        <v>4502</v>
+      </c>
+      <c r="D912" s="1" t="s">
+        <v>4503</v>
+      </c>
+      <c r="E912" s="1" t="s">
+        <v>4504</v>
+      </c>
+      <c r="F912" s="1" t="s">
+        <v>4505</v>
+      </c>
+      <c r="G912" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="913" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A913" s="1" t="s">
+        <v>4493</v>
+      </c>
+      <c r="B913" s="1">
+        <v>31</v>
+      </c>
+      <c r="C913" s="1" t="s">
+        <v>4506</v>
+      </c>
+      <c r="D913" s="1" t="s">
+        <v>4508</v>
+      </c>
+      <c r="E913" s="1" t="s">
+        <v>4507</v>
+      </c>
+      <c r="F913" s="1" t="s">
+        <v>4509</v>
+      </c>
+      <c r="G913" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="914" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A914" s="1" t="s">
+        <v>4494</v>
+      </c>
+      <c r="B914" s="1">
+        <v>31</v>
+      </c>
+      <c r="C914" s="1" t="s">
+        <v>4510</v>
+      </c>
+      <c r="D914" s="1" t="s">
+        <v>4511</v>
+      </c>
+      <c r="E914" s="1" t="s">
+        <v>4512</v>
+      </c>
+      <c r="F914" s="1" t="s">
+        <v>4513</v>
+      </c>
+      <c r="G914" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="915" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A915" s="1" t="s">
+        <v>4495</v>
+      </c>
+      <c r="B915" s="1">
+        <v>31</v>
+      </c>
+      <c r="C915" s="1" t="s">
+        <v>4514</v>
+      </c>
+      <c r="D915" s="1" t="s">
+        <v>4515</v>
+      </c>
+      <c r="E915" s="1" t="s">
+        <v>4516</v>
+      </c>
+      <c r="F915" s="1" t="s">
+        <v>4517</v>
+      </c>
+      <c r="G915" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="916" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A916" s="1" t="s">
+        <v>4496</v>
+      </c>
+      <c r="B916" s="1">
+        <v>31</v>
+      </c>
+      <c r="C916" s="1" t="s">
+        <v>4518</v>
+      </c>
+      <c r="D916" s="1" t="s">
+        <v>4519</v>
+      </c>
+      <c r="E916" s="1" t="s">
+        <v>4520</v>
+      </c>
+      <c r="F916" s="1" t="s">
+        <v>4521</v>
+      </c>
+      <c r="G916" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="917" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A917" s="1" t="s">
+        <v>4497</v>
+      </c>
+      <c r="B917" s="1">
+        <v>31</v>
+      </c>
+      <c r="C917" s="1" t="s">
+        <v>4522</v>
+      </c>
+      <c r="D917" s="1" t="s">
+        <v>4523</v>
+      </c>
+      <c r="E917" s="1" t="s">
+        <v>4524</v>
+      </c>
+      <c r="F917" s="1" t="s">
+        <v>4525</v>
+      </c>
+      <c r="G917" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="918" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A918" s="1" t="s">
+        <v>4498</v>
+      </c>
+      <c r="B918" s="1">
+        <v>31</v>
+      </c>
+      <c r="C918" s="1" t="s">
+        <v>4526</v>
+      </c>
+      <c r="D918" s="1" t="s">
+        <v>4527</v>
+      </c>
+      <c r="E918" s="1" t="s">
+        <v>4528</v>
+      </c>
+      <c r="F918" s="1" t="s">
+        <v>4529</v>
+      </c>
+      <c r="G918" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="919" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A919" s="1" t="s">
+        <v>4499</v>
+      </c>
+      <c r="B919" s="1">
+        <v>31</v>
+      </c>
+      <c r="C919" s="1" t="s">
+        <v>4530</v>
+      </c>
+      <c r="D919" s="1" t="s">
+        <v>4531</v>
+      </c>
+      <c r="E919" s="1" t="s">
+        <v>4532</v>
+      </c>
+      <c r="F919" s="1" t="s">
+        <v>4533</v>
+      </c>
+      <c r="G919" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="920" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A920" s="1" t="s">
+        <v>4500</v>
+      </c>
+      <c r="B920" s="1">
+        <v>31</v>
+      </c>
+      <c r="C920" s="1" t="s">
+        <v>4534</v>
+      </c>
+      <c r="D920" s="1" t="s">
+        <v>4535</v>
+      </c>
+      <c r="E920" s="1" t="s">
+        <v>4536</v>
+      </c>
+      <c r="F920" s="1" t="s">
+        <v>4537</v>
+      </c>
+      <c r="G920" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="921" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A921" s="1" t="s">
+        <v>4501</v>
+      </c>
+      <c r="B921" s="1">
+        <v>31</v>
+      </c>
+      <c r="C921" s="1" t="s">
+        <v>4538</v>
+      </c>
+      <c r="D921" s="1" t="s">
+        <v>4539</v>
+      </c>
+      <c r="E921" s="1" t="s">
+        <v>4540</v>
+      </c>
+      <c r="F921" s="1" t="s">
+        <v>4541</v>
+      </c>
+      <c r="G921" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="922" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A922" s="1" t="s">
+        <v>4542</v>
+      </c>
+      <c r="B922" s="1">
+        <v>31</v>
+      </c>
+      <c r="C922" s="1" t="s">
+        <v>4552</v>
+      </c>
+      <c r="D922" s="1" t="s">
+        <v>4553</v>
+      </c>
+      <c r="E922" s="1" t="s">
+        <v>4554</v>
+      </c>
+      <c r="F922" s="1" t="s">
+        <v>4555</v>
+      </c>
+      <c r="G922" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="923" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A923" s="1" t="s">
+        <v>4543</v>
+      </c>
+      <c r="B923" s="1">
+        <v>31</v>
+      </c>
+      <c r="C923" s="1" t="s">
+        <v>4556</v>
+      </c>
+      <c r="D923" s="1" t="s">
+        <v>4557</v>
+      </c>
+      <c r="E923" s="1" t="s">
+        <v>4558</v>
+      </c>
+      <c r="F923" s="1" t="s">
+        <v>4559</v>
+      </c>
+      <c r="G923" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="924" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A924" s="1" t="s">
+        <v>4544</v>
+      </c>
+      <c r="B924" s="1">
+        <v>31</v>
+      </c>
+      <c r="C924" s="1" t="s">
+        <v>4560</v>
+      </c>
+      <c r="D924" s="1" t="s">
+        <v>4561</v>
+      </c>
+      <c r="E924" s="1" t="s">
+        <v>4562</v>
+      </c>
+      <c r="F924" s="1" t="s">
+        <v>4563</v>
+      </c>
+      <c r="G924" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="925" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A925" s="1" t="s">
+        <v>4545</v>
+      </c>
+      <c r="B925" s="1">
+        <v>31</v>
+      </c>
+      <c r="C925" s="1" t="s">
+        <v>4564</v>
+      </c>
+      <c r="D925" s="1" t="s">
+        <v>4565</v>
+      </c>
+      <c r="E925" s="1" t="s">
+        <v>4566</v>
+      </c>
+      <c r="F925" s="1" t="s">
+        <v>4567</v>
+      </c>
+      <c r="G925" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="926" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A926" s="1" t="s">
+        <v>4546</v>
+      </c>
+      <c r="B926" s="1">
+        <v>31</v>
+      </c>
+      <c r="C926" s="1" t="s">
+        <v>4568</v>
+      </c>
+      <c r="D926" s="1" t="s">
+        <v>4569</v>
+      </c>
+      <c r="E926" s="1" t="s">
+        <v>4570</v>
+      </c>
+      <c r="F926" s="1" t="s">
+        <v>4571</v>
+      </c>
+      <c r="G926" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="927" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A927" s="1" t="s">
+        <v>4547</v>
+      </c>
+      <c r="B927" s="1">
+        <v>31</v>
+      </c>
+      <c r="C927" s="1" t="s">
+        <v>4572</v>
+      </c>
+      <c r="D927" s="1" t="s">
+        <v>4573</v>
+      </c>
+      <c r="E927" s="1" t="s">
+        <v>4574</v>
+      </c>
+      <c r="F927" s="1" t="s">
+        <v>4575</v>
+      </c>
+      <c r="G927" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="928" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A928" s="1" t="s">
+        <v>4548</v>
+      </c>
+      <c r="B928" s="1">
+        <v>31</v>
+      </c>
+      <c r="C928" s="1" t="s">
+        <v>4576</v>
+      </c>
+      <c r="D928" s="1" t="s">
+        <v>4577</v>
+      </c>
+      <c r="E928" s="1" t="s">
+        <v>4578</v>
+      </c>
+      <c r="F928" s="1" t="s">
+        <v>4579</v>
+      </c>
+      <c r="G928" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="929" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A929" s="1" t="s">
+        <v>4549</v>
+      </c>
+      <c r="B929" s="1">
+        <v>31</v>
+      </c>
+      <c r="C929" s="1" t="s">
+        <v>4580</v>
+      </c>
+      <c r="D929" s="1" t="s">
+        <v>4581</v>
+      </c>
+      <c r="E929" s="1" t="s">
+        <v>4582</v>
+      </c>
+      <c r="F929" s="1" t="s">
+        <v>4583</v>
+      </c>
+      <c r="G929" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="930" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A930" s="1" t="s">
+        <v>4550</v>
+      </c>
+      <c r="B930" s="1">
+        <v>31</v>
+      </c>
+      <c r="C930" s="1" t="s">
+        <v>4584</v>
+      </c>
+      <c r="D930" s="1" t="s">
+        <v>4585</v>
+      </c>
+      <c r="E930" s="1" t="s">
+        <v>4586</v>
+      </c>
+      <c r="F930" s="1" t="s">
+        <v>4587</v>
+      </c>
+      <c r="G930" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="931" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A931" s="1" t="s">
+        <v>4551</v>
+      </c>
+      <c r="B931" s="1">
+        <v>31</v>
+      </c>
+      <c r="C931" s="1" t="s">
+        <v>4588</v>
+      </c>
+      <c r="D931" s="1" t="s">
+        <v>4589</v>
+      </c>
+      <c r="E931" s="1" t="s">
+        <v>4590</v>
+      </c>
+      <c r="F931" s="1" t="s">
+        <v>4591</v>
+      </c>
+      <c r="G931" s="1" t="s">
+        <v>577</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
test: add unit 31 - 32
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9DC9B5-C07C-E748-8B8D-AB1C870F3F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A73661B-4D14-B144-9441-E8D6E08DD25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5434" uniqueCount="4592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5614" uniqueCount="4741">
   <si>
     <t>ID</t>
   </si>
@@ -13806,6 +13806,453 @@
   </si>
   <si>
     <t xml:space="preserve">sell something </t>
+  </si>
+  <si>
+    <t>U32_01</t>
+  </si>
+  <si>
+    <t>U32_02</t>
+  </si>
+  <si>
+    <t>U32_03</t>
+  </si>
+  <si>
+    <t>U32_04</t>
+  </si>
+  <si>
+    <t>U32_05</t>
+  </si>
+  <si>
+    <t>U32_06</t>
+  </si>
+  <si>
+    <t>U32_07</t>
+  </si>
+  <si>
+    <t>U32_08</t>
+  </si>
+  <si>
+    <t>U32_09</t>
+  </si>
+  <si>
+    <t>U32_10</t>
+  </si>
+  <si>
+    <t>U32_11</t>
+  </si>
+  <si>
+    <t>U32_12</t>
+  </si>
+  <si>
+    <t>U32_13</t>
+  </si>
+  <si>
+    <t>U32_14</t>
+  </si>
+  <si>
+    <t>U32_15</t>
+  </si>
+  <si>
+    <t>U32_16</t>
+  </si>
+  <si>
+    <t>U32_17</t>
+  </si>
+  <si>
+    <t>U32_18</t>
+  </si>
+  <si>
+    <t>U32_19</t>
+  </si>
+  <si>
+    <t>U32_20</t>
+  </si>
+  <si>
+    <t>U32_21</t>
+  </si>
+  <si>
+    <t>U32_22</t>
+  </si>
+  <si>
+    <t>U32_23</t>
+  </si>
+  <si>
+    <t>U32_24</t>
+  </si>
+  <si>
+    <t>U32_25</t>
+  </si>
+  <si>
+    <t>U32_26</t>
+  </si>
+  <si>
+    <t>U32_27</t>
+  </si>
+  <si>
+    <t>U32_28</t>
+  </si>
+  <si>
+    <t>U32_29</t>
+  </si>
+  <si>
+    <t>U32_30</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>The ruler has a rectangular shape</t>
+  </si>
+  <si>
+    <t>a rectangular shape / hình chữ nhật</t>
+  </si>
+  <si>
+    <t>Cổ áo</t>
+  </si>
+  <si>
+    <t>Collar</t>
+  </si>
+  <si>
+    <t>a shirt collar</t>
+  </si>
+  <si>
+    <t>My shirt collar is stained / … bị ố</t>
+  </si>
+  <si>
+    <t>Đường cong</t>
+  </si>
+  <si>
+    <t>Curve</t>
+  </si>
+  <si>
+    <t>The fast car took a sharp curve</t>
+  </si>
+  <si>
+    <t>a sharp curve / khúc cua gấp</t>
+  </si>
+  <si>
+    <t>Khuy áo</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>One of your shirt buttons is missing</t>
+  </si>
+  <si>
+    <t>a shirt button / một cái khuy áo</t>
+  </si>
+  <si>
+    <t>Túi</t>
+  </si>
+  <si>
+    <t>Pocket</t>
+  </si>
+  <si>
+    <t>The keys are in my pocket</t>
+  </si>
+  <si>
+    <t>in one's pocket</t>
+  </si>
+  <si>
+    <t>Tay áo</t>
+  </si>
+  <si>
+    <t>Sleeve</t>
+  </si>
+  <si>
+    <t>His shirt has short sleeves</t>
+  </si>
+  <si>
+    <t>a short sleeve / áo cộc tay</t>
+  </si>
+  <si>
+    <t>Tủ quần áo</t>
+  </si>
+  <si>
+    <t>Closet</t>
+  </si>
+  <si>
+    <t>the child is hiding in the closet</t>
+  </si>
+  <si>
+    <t>in the closet</t>
+  </si>
+  <si>
+    <t>Tất</t>
+  </si>
+  <si>
+    <t>Sock</t>
+  </si>
+  <si>
+    <t>Your christmas gift is a pair of socks</t>
+  </si>
+  <si>
+    <t>a pair of socks</t>
+  </si>
+  <si>
+    <t>Trang sức</t>
+  </si>
+  <si>
+    <t>Juwelry</t>
+  </si>
+  <si>
+    <t>Gold jewelry is expensive</t>
+  </si>
+  <si>
+    <t>gold jewelry</t>
+  </si>
+  <si>
+    <t>Vòng tay</t>
+  </si>
+  <si>
+    <t>Bracelet</t>
+  </si>
+  <si>
+    <t>she wears a diamond bracelet on her wrist</t>
+  </si>
+  <si>
+    <t>a diamond bracelet</t>
+  </si>
+  <si>
+    <t>Cửa hàng</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Apple now has retail stores in vietnam</t>
+  </si>
+  <si>
+    <t>a retail store / cửa hàng bán lẻ</t>
+  </si>
+  <si>
+    <t>Thắt</t>
+  </si>
+  <si>
+    <t>Tie</t>
+  </si>
+  <si>
+    <t>I don’t know how to tie a tie</t>
+  </si>
+  <si>
+    <t>tie a tie / thắt cà vạt</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>Leather</t>
+  </si>
+  <si>
+    <t>Bikers usually wear leather jackets</t>
+  </si>
+  <si>
+    <t>a leather jacket / áo khoác da</t>
+  </si>
+  <si>
+    <t>Vẻ đẹp</t>
+  </si>
+  <si>
+    <t>Beauty</t>
+  </si>
+  <si>
+    <t>The beauty of this view amazes me</t>
+  </si>
+  <si>
+    <t>beauty of something or somebody</t>
+  </si>
+  <si>
+    <t>Hợp</t>
+  </si>
+  <si>
+    <t>Suit</t>
+  </si>
+  <si>
+    <t>This hat suits you well</t>
+  </si>
+  <si>
+    <t>suit somebody well</t>
+  </si>
+  <si>
+    <t>Thử đồ</t>
+  </si>
+  <si>
+    <t>Try on</t>
+  </si>
+  <si>
+    <t>Why don’t you try on the dress?</t>
+  </si>
+  <si>
+    <t>try on something</t>
+  </si>
+  <si>
+    <t>Lỏng</t>
+  </si>
+  <si>
+    <t>Loose</t>
+  </si>
+  <si>
+    <t>can you fix my shirt's loose button?</t>
+  </si>
+  <si>
+    <t>a loose button</t>
+  </si>
+  <si>
+    <t>Quần</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>You need a new pair of pants</t>
+  </si>
+  <si>
+    <t>a pair of pants / một chiếc quần dài</t>
+  </si>
+  <si>
+    <t>Chật</t>
+  </si>
+  <si>
+    <t>Tight</t>
+  </si>
+  <si>
+    <t>These pants are too tight for me</t>
+  </si>
+  <si>
+    <t>too tight for somebody</t>
+  </si>
+  <si>
+    <t>Phần eo</t>
+  </si>
+  <si>
+    <t>Waist</t>
+  </si>
+  <si>
+    <t>His clothes are wet from the waist down</t>
+  </si>
+  <si>
+    <t>from the waist down / từ thắt lưng trở xuống</t>
+  </si>
+  <si>
+    <t>Kim cương</t>
+  </si>
+  <si>
+    <t>Diamond</t>
+  </si>
+  <si>
+    <t>The diamond rind he gave her was huge</t>
+  </si>
+  <si>
+    <t>a diamond ring</t>
+  </si>
+  <si>
+    <t>Mẫu họa tiết</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>I like the pattern on your shirt</t>
+  </si>
+  <si>
+    <t>the pattern on something</t>
+  </si>
+  <si>
+    <t>Hợp với</t>
+  </si>
+  <si>
+    <t>Go with</t>
+  </si>
+  <si>
+    <t>My new shirt goes with my favorite watch</t>
+  </si>
+  <si>
+    <t>go with something</t>
+  </si>
+  <si>
+    <t>Mảnh</t>
+  </si>
+  <si>
+    <t>Piece</t>
+  </si>
+  <si>
+    <t>This purse can go with any piece of clothing</t>
+  </si>
+  <si>
+    <t>a piece of clothing / món đồ thời trang</t>
+  </si>
+  <si>
+    <t>Khoe mẽ</t>
+  </si>
+  <si>
+    <t>Show off</t>
+  </si>
+  <si>
+    <t>He is showing off his new watch</t>
+  </si>
+  <si>
+    <t>show off something</t>
+  </si>
+  <si>
+    <t>Ngầu</t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>The new poster design looks cool</t>
+  </si>
+  <si>
+    <t>to look cool / trong thật ngầu</t>
+  </si>
+  <si>
+    <t>Nhiều màu sắc</t>
+  </si>
+  <si>
+    <t>Children always make the most colorful paintings</t>
+  </si>
+  <si>
+    <t>Colorful</t>
+  </si>
+  <si>
+    <t>A colorful painting / một bức tranh sặc sỡ</t>
+  </si>
+  <si>
+    <t>Thời trang</t>
+  </si>
+  <si>
+    <t>Fashion</t>
+  </si>
+  <si>
+    <t>She writes about the latest fashion trends</t>
+  </si>
+  <si>
+    <t>a fashion trend</t>
+  </si>
+  <si>
+    <t>Thanh lịch</t>
+  </si>
+  <si>
+    <t>Chic</t>
+  </si>
+  <si>
+    <t>The fashionista has a chic style</t>
+  </si>
+  <si>
+    <t>a chic style / phong cách thanh lịch</t>
+  </si>
+  <si>
+    <t>Gói lại</t>
+  </si>
+  <si>
+    <t>Wrap up</t>
+  </si>
+  <si>
+    <t>The cashier wrapped up the shirt for me</t>
+  </si>
+  <si>
+    <t>wrap up something</t>
   </si>
 </sst>
 </file>
@@ -14170,10 +14617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G931"/>
+  <dimension ref="A1:G961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B903" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E932" sqref="E932"/>
+    <sheetView tabSelected="1" topLeftCell="B930" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C953" sqref="C953"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35141,6 +35588,696 @@
         <v>577</v>
       </c>
     </row>
+    <row r="932" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A932" s="1" t="s">
+        <v>4592</v>
+      </c>
+      <c r="B932" s="1">
+        <v>32</v>
+      </c>
+      <c r="C932" s="1" t="s">
+        <v>2872</v>
+      </c>
+      <c r="D932" s="1" t="s">
+        <v>4622</v>
+      </c>
+      <c r="E932" s="1" t="s">
+        <v>4623</v>
+      </c>
+      <c r="F932" s="1" t="s">
+        <v>4624</v>
+      </c>
+      <c r="G932" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="933" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A933" s="1" t="s">
+        <v>4593</v>
+      </c>
+      <c r="B933" s="1">
+        <v>32</v>
+      </c>
+      <c r="C933" s="1" t="s">
+        <v>4625</v>
+      </c>
+      <c r="D933" s="1" t="s">
+        <v>4626</v>
+      </c>
+      <c r="E933" s="1" t="s">
+        <v>4628</v>
+      </c>
+      <c r="F933" s="1" t="s">
+        <v>4627</v>
+      </c>
+      <c r="G933" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="934" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A934" s="1" t="s">
+        <v>4594</v>
+      </c>
+      <c r="B934" s="1">
+        <v>32</v>
+      </c>
+      <c r="C934" s="1" t="s">
+        <v>4629</v>
+      </c>
+      <c r="D934" s="1" t="s">
+        <v>4630</v>
+      </c>
+      <c r="E934" s="1" t="s">
+        <v>4631</v>
+      </c>
+      <c r="F934" s="1" t="s">
+        <v>4632</v>
+      </c>
+      <c r="G934" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="935" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A935" s="1" t="s">
+        <v>4595</v>
+      </c>
+      <c r="B935" s="1">
+        <v>32</v>
+      </c>
+      <c r="C935" s="1" t="s">
+        <v>4633</v>
+      </c>
+      <c r="D935" s="1" t="s">
+        <v>4634</v>
+      </c>
+      <c r="E935" s="1" t="s">
+        <v>4635</v>
+      </c>
+      <c r="F935" s="1" t="s">
+        <v>4636</v>
+      </c>
+      <c r="G935" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="936" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A936" s="1" t="s">
+        <v>4596</v>
+      </c>
+      <c r="B936" s="1">
+        <v>32</v>
+      </c>
+      <c r="C936" s="1" t="s">
+        <v>4637</v>
+      </c>
+      <c r="D936" s="1" t="s">
+        <v>4638</v>
+      </c>
+      <c r="E936" s="1" t="s">
+        <v>4639</v>
+      </c>
+      <c r="F936" s="1" t="s">
+        <v>4640</v>
+      </c>
+      <c r="G936" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="937" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A937" s="1" t="s">
+        <v>4597</v>
+      </c>
+      <c r="B937" s="1">
+        <v>32</v>
+      </c>
+      <c r="C937" s="1" t="s">
+        <v>4641</v>
+      </c>
+      <c r="D937" s="1" t="s">
+        <v>4642</v>
+      </c>
+      <c r="E937" s="1" t="s">
+        <v>4643</v>
+      </c>
+      <c r="F937" s="1" t="s">
+        <v>4644</v>
+      </c>
+      <c r="G937" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="938" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A938" s="1" t="s">
+        <v>4598</v>
+      </c>
+      <c r="B938" s="1">
+        <v>32</v>
+      </c>
+      <c r="C938" s="1" t="s">
+        <v>4645</v>
+      </c>
+      <c r="D938" s="1" t="s">
+        <v>4646</v>
+      </c>
+      <c r="E938" s="1" t="s">
+        <v>4647</v>
+      </c>
+      <c r="F938" s="1" t="s">
+        <v>4648</v>
+      </c>
+      <c r="G938" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="939" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A939" s="1" t="s">
+        <v>4599</v>
+      </c>
+      <c r="B939" s="1">
+        <v>32</v>
+      </c>
+      <c r="C939" s="1" t="s">
+        <v>4649</v>
+      </c>
+      <c r="D939" s="1" t="s">
+        <v>4650</v>
+      </c>
+      <c r="E939" s="1" t="s">
+        <v>4651</v>
+      </c>
+      <c r="F939" s="1" t="s">
+        <v>4652</v>
+      </c>
+      <c r="G939" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="940" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A940" s="1" t="s">
+        <v>4600</v>
+      </c>
+      <c r="B940" s="1">
+        <v>32</v>
+      </c>
+      <c r="C940" s="1" t="s">
+        <v>4653</v>
+      </c>
+      <c r="D940" s="1" t="s">
+        <v>4654</v>
+      </c>
+      <c r="E940" s="1" t="s">
+        <v>4655</v>
+      </c>
+      <c r="F940" s="1" t="s">
+        <v>4656</v>
+      </c>
+      <c r="G940" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="941" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A941" s="1" t="s">
+        <v>4601</v>
+      </c>
+      <c r="B941" s="1">
+        <v>32</v>
+      </c>
+      <c r="C941" s="1" t="s">
+        <v>4657</v>
+      </c>
+      <c r="D941" s="1" t="s">
+        <v>4658</v>
+      </c>
+      <c r="E941" s="1" t="s">
+        <v>4659</v>
+      </c>
+      <c r="F941" s="1" t="s">
+        <v>4660</v>
+      </c>
+      <c r="G941" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="942" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A942" s="1" t="s">
+        <v>4602</v>
+      </c>
+      <c r="B942" s="1">
+        <v>32</v>
+      </c>
+      <c r="C942" s="1" t="s">
+        <v>4661</v>
+      </c>
+      <c r="D942" s="1" t="s">
+        <v>4662</v>
+      </c>
+      <c r="E942" s="1" t="s">
+        <v>4663</v>
+      </c>
+      <c r="F942" s="1" t="s">
+        <v>4664</v>
+      </c>
+      <c r="G942" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="943" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A943" s="1" t="s">
+        <v>4603</v>
+      </c>
+      <c r="B943" s="1">
+        <v>32</v>
+      </c>
+      <c r="C943" s="1" t="s">
+        <v>4665</v>
+      </c>
+      <c r="D943" s="1" t="s">
+        <v>4666</v>
+      </c>
+      <c r="E943" s="1" t="s">
+        <v>4667</v>
+      </c>
+      <c r="F943" s="1" t="s">
+        <v>4668</v>
+      </c>
+      <c r="G943" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="944" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A944" s="1" t="s">
+        <v>4604</v>
+      </c>
+      <c r="B944" s="1">
+        <v>32</v>
+      </c>
+      <c r="C944" s="1" t="s">
+        <v>4669</v>
+      </c>
+      <c r="D944" s="1" t="s">
+        <v>4670</v>
+      </c>
+      <c r="E944" s="1" t="s">
+        <v>4671</v>
+      </c>
+      <c r="F944" s="1" t="s">
+        <v>4672</v>
+      </c>
+      <c r="G944" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="945" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A945" s="1" t="s">
+        <v>4605</v>
+      </c>
+      <c r="B945" s="1">
+        <v>32</v>
+      </c>
+      <c r="C945" s="1" t="s">
+        <v>4673</v>
+      </c>
+      <c r="D945" s="1" t="s">
+        <v>4674</v>
+      </c>
+      <c r="E945" s="1" t="s">
+        <v>4675</v>
+      </c>
+      <c r="F945" s="1" t="s">
+        <v>4676</v>
+      </c>
+      <c r="G945" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="946" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A946" s="1" t="s">
+        <v>4606</v>
+      </c>
+      <c r="B946" s="1">
+        <v>32</v>
+      </c>
+      <c r="C946" s="1" t="s">
+        <v>4677</v>
+      </c>
+      <c r="D946" s="1" t="s">
+        <v>4678</v>
+      </c>
+      <c r="E946" s="1" t="s">
+        <v>4679</v>
+      </c>
+      <c r="F946" s="1" t="s">
+        <v>4680</v>
+      </c>
+      <c r="G946" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="947" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A947" s="1" t="s">
+        <v>4607</v>
+      </c>
+      <c r="B947" s="1">
+        <v>32</v>
+      </c>
+      <c r="C947" s="1" t="s">
+        <v>4681</v>
+      </c>
+      <c r="D947" s="1" t="s">
+        <v>4682</v>
+      </c>
+      <c r="E947" s="1" t="s">
+        <v>4683</v>
+      </c>
+      <c r="F947" s="1" t="s">
+        <v>4684</v>
+      </c>
+      <c r="G947" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="948" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A948" s="1" t="s">
+        <v>4608</v>
+      </c>
+      <c r="B948" s="1">
+        <v>32</v>
+      </c>
+      <c r="C948" s="1" t="s">
+        <v>4685</v>
+      </c>
+      <c r="D948" s="1" t="s">
+        <v>4686</v>
+      </c>
+      <c r="E948" s="1" t="s">
+        <v>4687</v>
+      </c>
+      <c r="F948" s="1" t="s">
+        <v>4688</v>
+      </c>
+      <c r="G948" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="949" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A949" s="1" t="s">
+        <v>4609</v>
+      </c>
+      <c r="B949" s="1">
+        <v>32</v>
+      </c>
+      <c r="C949" s="1" t="s">
+        <v>4689</v>
+      </c>
+      <c r="D949" s="1" t="s">
+        <v>4690</v>
+      </c>
+      <c r="E949" s="1" t="s">
+        <v>4691</v>
+      </c>
+      <c r="F949" s="1" t="s">
+        <v>4692</v>
+      </c>
+      <c r="G949" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="950" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A950" s="1" t="s">
+        <v>4610</v>
+      </c>
+      <c r="B950" s="1">
+        <v>32</v>
+      </c>
+      <c r="C950" s="1" t="s">
+        <v>4693</v>
+      </c>
+      <c r="D950" s="1" t="s">
+        <v>4694</v>
+      </c>
+      <c r="E950" s="1" t="s">
+        <v>4695</v>
+      </c>
+      <c r="F950" s="1" t="s">
+        <v>4696</v>
+      </c>
+      <c r="G950" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="951" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A951" s="1" t="s">
+        <v>4611</v>
+      </c>
+      <c r="B951" s="1">
+        <v>32</v>
+      </c>
+      <c r="C951" s="1" t="s">
+        <v>4697</v>
+      </c>
+      <c r="D951" s="1" t="s">
+        <v>4698</v>
+      </c>
+      <c r="E951" s="1" t="s">
+        <v>4699</v>
+      </c>
+      <c r="F951" s="1" t="s">
+        <v>4700</v>
+      </c>
+      <c r="G951" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="952" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A952" s="1" t="s">
+        <v>4612</v>
+      </c>
+      <c r="B952" s="1">
+        <v>32</v>
+      </c>
+      <c r="C952" s="1" t="s">
+        <v>4701</v>
+      </c>
+      <c r="D952" s="1" t="s">
+        <v>4702</v>
+      </c>
+      <c r="E952" s="1" t="s">
+        <v>4703</v>
+      </c>
+      <c r="F952" s="1" t="s">
+        <v>4704</v>
+      </c>
+      <c r="G952" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="953" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A953" s="1" t="s">
+        <v>4613</v>
+      </c>
+      <c r="B953" s="1">
+        <v>32</v>
+      </c>
+      <c r="C953" s="1" t="s">
+        <v>4705</v>
+      </c>
+      <c r="D953" s="1" t="s">
+        <v>4706</v>
+      </c>
+      <c r="E953" s="1" t="s">
+        <v>4707</v>
+      </c>
+      <c r="F953" s="1" t="s">
+        <v>4708</v>
+      </c>
+      <c r="G953" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="954" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A954" s="1" t="s">
+        <v>4614</v>
+      </c>
+      <c r="B954" s="1">
+        <v>32</v>
+      </c>
+      <c r="C954" s="1" t="s">
+        <v>4709</v>
+      </c>
+      <c r="D954" s="1" t="s">
+        <v>4710</v>
+      </c>
+      <c r="E954" s="1" t="s">
+        <v>4711</v>
+      </c>
+      <c r="F954" s="1" t="s">
+        <v>4712</v>
+      </c>
+      <c r="G954" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="955" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A955" s="1" t="s">
+        <v>4615</v>
+      </c>
+      <c r="B955" s="1">
+        <v>32</v>
+      </c>
+      <c r="C955" s="1" t="s">
+        <v>4713</v>
+      </c>
+      <c r="D955" s="1" t="s">
+        <v>4714</v>
+      </c>
+      <c r="E955" s="1" t="s">
+        <v>4715</v>
+      </c>
+      <c r="F955" s="1" t="s">
+        <v>4716</v>
+      </c>
+      <c r="G955" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="956" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A956" s="1" t="s">
+        <v>4616</v>
+      </c>
+      <c r="B956" s="1">
+        <v>32</v>
+      </c>
+      <c r="C956" s="1" t="s">
+        <v>4717</v>
+      </c>
+      <c r="D956" s="1" t="s">
+        <v>4718</v>
+      </c>
+      <c r="E956" s="1" t="s">
+        <v>4719</v>
+      </c>
+      <c r="F956" s="1" t="s">
+        <v>4720</v>
+      </c>
+      <c r="G956" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="957" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A957" s="1" t="s">
+        <v>4617</v>
+      </c>
+      <c r="B957" s="1">
+        <v>32</v>
+      </c>
+      <c r="C957" s="1" t="s">
+        <v>4721</v>
+      </c>
+      <c r="D957" s="1" t="s">
+        <v>4722</v>
+      </c>
+      <c r="E957" s="1" t="s">
+        <v>4723</v>
+      </c>
+      <c r="F957" s="1" t="s">
+        <v>4724</v>
+      </c>
+      <c r="G957" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="958" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A958" s="1" t="s">
+        <v>4618</v>
+      </c>
+      <c r="B958" s="1">
+        <v>32</v>
+      </c>
+      <c r="C958" s="1" t="s">
+        <v>4725</v>
+      </c>
+      <c r="D958" s="1" t="s">
+        <v>4727</v>
+      </c>
+      <c r="E958" s="1" t="s">
+        <v>4726</v>
+      </c>
+      <c r="F958" s="1" t="s">
+        <v>4728</v>
+      </c>
+      <c r="G958" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="959" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A959" s="1" t="s">
+        <v>4619</v>
+      </c>
+      <c r="B959" s="1">
+        <v>32</v>
+      </c>
+      <c r="C959" s="1" t="s">
+        <v>4729</v>
+      </c>
+      <c r="D959" s="1" t="s">
+        <v>4730</v>
+      </c>
+      <c r="E959" s="1" t="s">
+        <v>4731</v>
+      </c>
+      <c r="F959" s="1" t="s">
+        <v>4732</v>
+      </c>
+      <c r="G959" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="960" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A960" s="1" t="s">
+        <v>4620</v>
+      </c>
+      <c r="B960" s="1">
+        <v>32</v>
+      </c>
+      <c r="C960" s="1" t="s">
+        <v>4733</v>
+      </c>
+      <c r="D960" s="1" t="s">
+        <v>4734</v>
+      </c>
+      <c r="E960" s="1" t="s">
+        <v>4735</v>
+      </c>
+      <c r="F960" s="1" t="s">
+        <v>4736</v>
+      </c>
+      <c r="G960" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="961" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A961" s="1" t="s">
+        <v>4621</v>
+      </c>
+      <c r="B961" s="1">
+        <v>32</v>
+      </c>
+      <c r="C961" s="1" t="s">
+        <v>4737</v>
+      </c>
+      <c r="D961" s="1" t="s">
+        <v>4738</v>
+      </c>
+      <c r="E961" s="1" t="s">
+        <v>4739</v>
+      </c>
+      <c r="F961" s="1" t="s">
+        <v>4740</v>
+      </c>
+      <c r="G961" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 34
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF67DFF7-E784-DF48-A53F-49D5827979B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369FBD00-BA72-EC4E-ACAF-8BDA287E272C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5794" uniqueCount="4889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5974" uniqueCount="5038">
   <si>
     <t>ID</t>
   </si>
@@ -14697,6 +14697,453 @@
   </si>
   <si>
     <t>legend has it that / truyền thuyết kể lại rằng</t>
+  </si>
+  <si>
+    <t>U34_01</t>
+  </si>
+  <si>
+    <t>U34_02</t>
+  </si>
+  <si>
+    <t>U34_03</t>
+  </si>
+  <si>
+    <t>U34_04</t>
+  </si>
+  <si>
+    <t>U34_05</t>
+  </si>
+  <si>
+    <t>U34_06</t>
+  </si>
+  <si>
+    <t>U34_07</t>
+  </si>
+  <si>
+    <t>U34_08</t>
+  </si>
+  <si>
+    <t>U34_09</t>
+  </si>
+  <si>
+    <t>U34_10</t>
+  </si>
+  <si>
+    <t>U34_11</t>
+  </si>
+  <si>
+    <t>U34_12</t>
+  </si>
+  <si>
+    <t>U34_13</t>
+  </si>
+  <si>
+    <t>U34_14</t>
+  </si>
+  <si>
+    <t>U34_15</t>
+  </si>
+  <si>
+    <t>U34_16</t>
+  </si>
+  <si>
+    <t>U34_17</t>
+  </si>
+  <si>
+    <t>U34_18</t>
+  </si>
+  <si>
+    <t>U34_19</t>
+  </si>
+  <si>
+    <t>U34_20</t>
+  </si>
+  <si>
+    <t>U34_21</t>
+  </si>
+  <si>
+    <t>U34_22</t>
+  </si>
+  <si>
+    <t>U34_23</t>
+  </si>
+  <si>
+    <t>U34_24</t>
+  </si>
+  <si>
+    <t>U34_25</t>
+  </si>
+  <si>
+    <t>U34_26</t>
+  </si>
+  <si>
+    <t>U34_27</t>
+  </si>
+  <si>
+    <t>U34_28</t>
+  </si>
+  <si>
+    <t>U34_29</t>
+  </si>
+  <si>
+    <t>U34_30</t>
+  </si>
+  <si>
+    <t>Pháo hoa</t>
+  </si>
+  <si>
+    <t>Firework</t>
+  </si>
+  <si>
+    <t>We watch fireworks displays together every year</t>
+  </si>
+  <si>
+    <t>a fireworks display / màn trình diễn pháo hoa</t>
+  </si>
+  <si>
+    <t>Ăn mừng, tán dương</t>
+  </si>
+  <si>
+    <t>Celebrate</t>
+  </si>
+  <si>
+    <t>Let's celebrate your promotion this Friday!</t>
+  </si>
+  <si>
+    <t>Celebrate somebody or something</t>
+  </si>
+  <si>
+    <t>Phần lớn, chủ yếu</t>
+  </si>
+  <si>
+    <t>Mostly</t>
+  </si>
+  <si>
+    <t>The sauce is mostly cream.</t>
+  </si>
+  <si>
+    <t>To be mostly something / chủ yếu là thứ gì đó</t>
+  </si>
+  <si>
+    <t>Phong bì</t>
+  </si>
+  <si>
+    <t>Envelope</t>
+  </si>
+  <si>
+    <t>"Li xi" is a red envelope of money</t>
+  </si>
+  <si>
+    <t>an envelope of something</t>
+  </si>
+  <si>
+    <t>Kỳ lạ</t>
+  </si>
+  <si>
+    <t>Strange</t>
+  </si>
+  <si>
+    <t>There is a strange object in the sky</t>
+  </si>
+  <si>
+    <t>A strange object / một vật thể kỳ lạ</t>
+  </si>
+  <si>
+    <t>Hào phóng</t>
+  </si>
+  <si>
+    <t>Generous</t>
+  </si>
+  <si>
+    <t>My dad is generous with giving gifts.</t>
+  </si>
+  <si>
+    <t>to be generous with something / hào phóng trong chuyện gì đó</t>
+  </si>
+  <si>
+    <t>Thay vì</t>
+  </si>
+  <si>
+    <t>Instead</t>
+  </si>
+  <si>
+    <t>Instead of doing homework, she watched TV</t>
+  </si>
+  <si>
+    <t>Instead of doing something</t>
+  </si>
+  <si>
+    <t>Quần áo, trang phục</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>We can wear casual clothing to work</t>
+  </si>
+  <si>
+    <t>casual clothing / trang phục đời thường</t>
+  </si>
+  <si>
+    <t>Trưng bày</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>display something</t>
+  </si>
+  <si>
+    <t>We display furniture (đồ nội thất) in our store.</t>
+  </si>
+  <si>
+    <t>Hoàng gia</t>
+  </si>
+  <si>
+    <t>Royal</t>
+  </si>
+  <si>
+    <t>The royal family in Britain is well-known</t>
+  </si>
+  <si>
+    <t>The royal family / gia đình hoàng gia</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>The team came across a serious problem</t>
+  </si>
+  <si>
+    <t>a serious problem</t>
+  </si>
+  <si>
+    <t>Phản cảm</t>
+  </si>
+  <si>
+    <t>Offensive</t>
+  </si>
+  <si>
+    <t>The show was offensive to certain people</t>
+  </si>
+  <si>
+    <t>to be offensive to someone / gây phản cảm cho ai đó</t>
+  </si>
+  <si>
+    <t>Quốc ca</t>
+  </si>
+  <si>
+    <t>Anthem</t>
+  </si>
+  <si>
+    <t>Can you sing our country's national anthem?</t>
+  </si>
+  <si>
+    <t>The national anthem</t>
+  </si>
+  <si>
+    <t>Điểm nổi bật</t>
+  </si>
+  <si>
+    <t>Highlight</t>
+  </si>
+  <si>
+    <t>The highlight of the trip was seeing the Taj Mahal.</t>
+  </si>
+  <si>
+    <t>The highlight of something / điểm nhấn của cái gì đó</t>
+  </si>
+  <si>
+    <t>Mất dần đi, mai một</t>
+  </si>
+  <si>
+    <t>die out</t>
+  </si>
+  <si>
+    <t>Many family traditions are dying out.</t>
+  </si>
+  <si>
+    <t>traditions die out  / truyền thống mai một dần</t>
+  </si>
+  <si>
+    <t>Cưới</t>
+  </si>
+  <si>
+    <t>Marry</t>
+  </si>
+  <si>
+    <t>I want to marry her because I love her</t>
+  </si>
+  <si>
+    <t>Marry somebody</t>
+  </si>
+  <si>
+    <t>Truyền lại</t>
+  </si>
+  <si>
+    <t>Pass down</t>
+  </si>
+  <si>
+    <t>My grandparents passes down family stories to us</t>
+  </si>
+  <si>
+    <t>Pass down something</t>
+  </si>
+  <si>
+    <t>Tiệc</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>you are invited to my birthday party.</t>
+  </si>
+  <si>
+    <t>A birthday party</t>
+  </si>
+  <si>
+    <t>Nhẫn</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>He bought an expensive wedding ring.</t>
+  </si>
+  <si>
+    <t>A wedding ring</t>
+  </si>
+  <si>
+    <t>Mặt nạ</t>
+  </si>
+  <si>
+    <t>Mask</t>
+  </si>
+  <si>
+    <t>You must breathe through the gas mask.</t>
+  </si>
+  <si>
+    <t>a gas mask / mặt nạ phòng độc</t>
+  </si>
+  <si>
+    <t>Xã hội</t>
+  </si>
+  <si>
+    <t>Society</t>
+  </si>
+  <si>
+    <t>There are many problems in modern society</t>
+  </si>
+  <si>
+    <t>a modern society</t>
+  </si>
+  <si>
+    <t>Nghi lễ, buổi lễ</t>
+  </si>
+  <si>
+    <t>Ceremony</t>
+  </si>
+  <si>
+    <t>Our daughter's graduation ceremony is this Sunday</t>
+  </si>
+  <si>
+    <t>a graduation ceremony / buổi lể tốt nghiệp</t>
+  </si>
+  <si>
+    <t>Sự để tâm, sự kính trọng</t>
+  </si>
+  <si>
+    <t>Regard</t>
+  </si>
+  <si>
+    <t>has regard for somebody or something</t>
+  </si>
+  <si>
+    <t>He has no regard for my feelings. / Anh ta không để tâm cảm xúc của tôi chút nào</t>
+  </si>
+  <si>
+    <t>Nến</t>
+  </si>
+  <si>
+    <t>Candle</t>
+  </si>
+  <si>
+    <t>Make a wish on the burning candle</t>
+  </si>
+  <si>
+    <t>a buring candle / ngon nến đang cháy</t>
+  </si>
+  <si>
+    <t>Cái chết</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>The anniversary of our grandmother's death was yesterday</t>
+  </si>
+  <si>
+    <t>The anniversary of somebody's death</t>
+  </si>
+  <si>
+    <t>Nhiều</t>
+  </si>
+  <si>
+    <t>Various</t>
+  </si>
+  <si>
+    <t>Cakes come in various shapes and sizes</t>
+  </si>
+  <si>
+    <t>Various shapes and sizes</t>
+  </si>
+  <si>
+    <t>Cờ</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>Vietnam's flag has a big yellow star</t>
+  </si>
+  <si>
+    <t>A country's flag / lá cờ của một quốc gia</t>
+  </si>
+  <si>
+    <t>Sự khó khăn</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Old people have difficulty in reading small work</t>
+  </si>
+  <si>
+    <t>Have difficulty in doing something</t>
+  </si>
+  <si>
+    <t>Nhỏ</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>The minor incident didn't hurt me.</t>
+  </si>
+  <si>
+    <t>a minor incident</t>
+  </si>
+  <si>
+    <t>Đạo đức</t>
+  </si>
+  <si>
+    <t>Moral</t>
+  </si>
+  <si>
+    <t>To steal or not is a moral issue.</t>
+  </si>
+  <si>
+    <t>a moral issues / vấn đề đạo đức</t>
   </si>
 </sst>
 </file>
@@ -14750,10 +15197,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15068,10 +15516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G991"/>
+  <dimension ref="A1:G1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B972" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C992" sqref="C992"/>
+    <sheetView tabSelected="1" topLeftCell="B1001" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1022" sqref="C1022"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37572,6 +38020,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="992" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A992" s="2" t="s">
+        <v>4889</v>
+      </c>
+      <c r="B992" s="2">
+        <v>34</v>
+      </c>
+      <c r="C992" s="2" t="s">
+        <v>4919</v>
+      </c>
+      <c r="D992" s="2" t="s">
+        <v>4920</v>
+      </c>
+      <c r="E992" s="2" t="s">
+        <v>4921</v>
+      </c>
+      <c r="F992" s="2" t="s">
+        <v>4922</v>
+      </c>
+      <c r="G992" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="993" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A993" s="2" t="s">
+        <v>4890</v>
+      </c>
+      <c r="B993" s="2">
+        <v>34</v>
+      </c>
+      <c r="C993" s="2" t="s">
+        <v>4923</v>
+      </c>
+      <c r="D993" s="2" t="s">
+        <v>4924</v>
+      </c>
+      <c r="E993" s="2" t="s">
+        <v>4925</v>
+      </c>
+      <c r="F993" s="2" t="s">
+        <v>4926</v>
+      </c>
+      <c r="G993" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="994" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A994" s="2" t="s">
+        <v>4891</v>
+      </c>
+      <c r="B994" s="2">
+        <v>34</v>
+      </c>
+      <c r="C994" s="2" t="s">
+        <v>4927</v>
+      </c>
+      <c r="D994" s="2" t="s">
+        <v>4928</v>
+      </c>
+      <c r="E994" s="2" t="s">
+        <v>4929</v>
+      </c>
+      <c r="F994" s="2" t="s">
+        <v>4930</v>
+      </c>
+      <c r="G994" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="995" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A995" s="2" t="s">
+        <v>4892</v>
+      </c>
+      <c r="B995" s="2">
+        <v>34</v>
+      </c>
+      <c r="C995" s="2" t="s">
+        <v>4931</v>
+      </c>
+      <c r="D995" s="2" t="s">
+        <v>4932</v>
+      </c>
+      <c r="E995" s="2" t="s">
+        <v>4933</v>
+      </c>
+      <c r="F995" s="2" t="s">
+        <v>4934</v>
+      </c>
+      <c r="G995" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="996" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A996" s="2" t="s">
+        <v>4893</v>
+      </c>
+      <c r="B996" s="2">
+        <v>34</v>
+      </c>
+      <c r="C996" s="2" t="s">
+        <v>4935</v>
+      </c>
+      <c r="D996" s="2" t="s">
+        <v>4936</v>
+      </c>
+      <c r="E996" s="2" t="s">
+        <v>4937</v>
+      </c>
+      <c r="F996" s="2" t="s">
+        <v>4938</v>
+      </c>
+      <c r="G996" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="997" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A997" s="2" t="s">
+        <v>4894</v>
+      </c>
+      <c r="B997" s="2">
+        <v>34</v>
+      </c>
+      <c r="C997" s="2" t="s">
+        <v>4939</v>
+      </c>
+      <c r="D997" s="2" t="s">
+        <v>4940</v>
+      </c>
+      <c r="E997" s="2" t="s">
+        <v>4941</v>
+      </c>
+      <c r="F997" s="2" t="s">
+        <v>4942</v>
+      </c>
+      <c r="G997" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="998" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A998" s="2" t="s">
+        <v>4895</v>
+      </c>
+      <c r="B998" s="2">
+        <v>34</v>
+      </c>
+      <c r="C998" s="2" t="s">
+        <v>4943</v>
+      </c>
+      <c r="D998" s="2" t="s">
+        <v>4944</v>
+      </c>
+      <c r="E998" s="2" t="s">
+        <v>4945</v>
+      </c>
+      <c r="F998" s="2" t="s">
+        <v>4946</v>
+      </c>
+      <c r="G998" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="999" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A999" s="2" t="s">
+        <v>4896</v>
+      </c>
+      <c r="B999" s="2">
+        <v>34</v>
+      </c>
+      <c r="C999" s="2" t="s">
+        <v>4947</v>
+      </c>
+      <c r="D999" s="2" t="s">
+        <v>4948</v>
+      </c>
+      <c r="E999" s="2" t="s">
+        <v>4949</v>
+      </c>
+      <c r="F999" s="2" t="s">
+        <v>4950</v>
+      </c>
+      <c r="G999" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1000" s="2" t="s">
+        <v>4897</v>
+      </c>
+      <c r="B1000" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1000" s="2" t="s">
+        <v>4951</v>
+      </c>
+      <c r="D1000" s="2" t="s">
+        <v>4952</v>
+      </c>
+      <c r="E1000" s="2" t="s">
+        <v>4954</v>
+      </c>
+      <c r="F1000" s="2" t="s">
+        <v>4953</v>
+      </c>
+      <c r="G1000" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1001" s="2" t="s">
+        <v>4898</v>
+      </c>
+      <c r="B1001" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1001" s="2" t="s">
+        <v>4955</v>
+      </c>
+      <c r="D1001" s="2" t="s">
+        <v>4956</v>
+      </c>
+      <c r="E1001" s="2" t="s">
+        <v>4957</v>
+      </c>
+      <c r="F1001" s="2" t="s">
+        <v>4958</v>
+      </c>
+      <c r="G1001" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1002" s="2" t="s">
+        <v>4899</v>
+      </c>
+      <c r="B1002" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1002" s="2" t="s">
+        <v>2549</v>
+      </c>
+      <c r="D1002" s="2" t="s">
+        <v>4959</v>
+      </c>
+      <c r="E1002" s="2" t="s">
+        <v>4960</v>
+      </c>
+      <c r="F1002" s="2" t="s">
+        <v>4961</v>
+      </c>
+      <c r="G1002" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1003" s="2" t="s">
+        <v>4900</v>
+      </c>
+      <c r="B1003" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1003" s="2" t="s">
+        <v>4962</v>
+      </c>
+      <c r="D1003" s="2" t="s">
+        <v>4963</v>
+      </c>
+      <c r="E1003" s="2" t="s">
+        <v>4964</v>
+      </c>
+      <c r="F1003" s="2" t="s">
+        <v>4965</v>
+      </c>
+      <c r="G1003" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1004" s="2" t="s">
+        <v>4901</v>
+      </c>
+      <c r="B1004" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1004" s="2" t="s">
+        <v>4966</v>
+      </c>
+      <c r="D1004" s="2" t="s">
+        <v>4967</v>
+      </c>
+      <c r="E1004" s="2" t="s">
+        <v>4968</v>
+      </c>
+      <c r="F1004" s="2" t="s">
+        <v>4969</v>
+      </c>
+      <c r="G1004" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1005" s="2" t="s">
+        <v>4902</v>
+      </c>
+      <c r="B1005" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1005" s="3" t="s">
+        <v>4970</v>
+      </c>
+      <c r="D1005" s="2" t="s">
+        <v>4971</v>
+      </c>
+      <c r="E1005" s="2" t="s">
+        <v>4972</v>
+      </c>
+      <c r="F1005" s="2" t="s">
+        <v>4973</v>
+      </c>
+      <c r="G1005" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1006" s="2" t="s">
+        <v>4903</v>
+      </c>
+      <c r="B1006" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1006" s="2" t="s">
+        <v>4974</v>
+      </c>
+      <c r="D1006" s="2" t="s">
+        <v>4975</v>
+      </c>
+      <c r="E1006" s="2" t="s">
+        <v>4976</v>
+      </c>
+      <c r="F1006" s="2" t="s">
+        <v>4977</v>
+      </c>
+      <c r="G1006" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1007" s="2" t="s">
+        <v>4904</v>
+      </c>
+      <c r="B1007" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1007" s="2" t="s">
+        <v>4978</v>
+      </c>
+      <c r="D1007" s="2" t="s">
+        <v>4979</v>
+      </c>
+      <c r="E1007" s="2" t="s">
+        <v>4980</v>
+      </c>
+      <c r="F1007" s="2" t="s">
+        <v>4981</v>
+      </c>
+      <c r="G1007" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1008" s="2" t="s">
+        <v>4905</v>
+      </c>
+      <c r="B1008" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1008" s="2" t="s">
+        <v>4982</v>
+      </c>
+      <c r="D1008" s="2" t="s">
+        <v>4983</v>
+      </c>
+      <c r="E1008" s="2" t="s">
+        <v>4984</v>
+      </c>
+      <c r="F1008" s="2" t="s">
+        <v>4985</v>
+      </c>
+      <c r="G1008" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1009" s="2" t="s">
+        <v>4906</v>
+      </c>
+      <c r="B1009" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1009" s="2" t="s">
+        <v>4986</v>
+      </c>
+      <c r="D1009" s="2" t="s">
+        <v>4987</v>
+      </c>
+      <c r="E1009" s="2" t="s">
+        <v>4988</v>
+      </c>
+      <c r="F1009" s="2" t="s">
+        <v>4989</v>
+      </c>
+      <c r="G1009" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1010" s="2" t="s">
+        <v>4907</v>
+      </c>
+      <c r="B1010" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1010" s="2" t="s">
+        <v>4990</v>
+      </c>
+      <c r="D1010" s="2" t="s">
+        <v>4991</v>
+      </c>
+      <c r="E1010" s="2" t="s">
+        <v>4992</v>
+      </c>
+      <c r="F1010" s="2" t="s">
+        <v>4993</v>
+      </c>
+      <c r="G1010" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1011" s="2" t="s">
+        <v>4908</v>
+      </c>
+      <c r="B1011" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1011" s="2" t="s">
+        <v>4994</v>
+      </c>
+      <c r="D1011" s="2" t="s">
+        <v>4995</v>
+      </c>
+      <c r="E1011" s="2" t="s">
+        <v>4996</v>
+      </c>
+      <c r="F1011" s="2" t="s">
+        <v>4997</v>
+      </c>
+      <c r="G1011" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1012" s="2" t="s">
+        <v>4909</v>
+      </c>
+      <c r="B1012" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1012" s="2" t="s">
+        <v>4998</v>
+      </c>
+      <c r="D1012" s="2" t="s">
+        <v>4999</v>
+      </c>
+      <c r="E1012" s="2" t="s">
+        <v>5000</v>
+      </c>
+      <c r="F1012" s="2" t="s">
+        <v>5001</v>
+      </c>
+      <c r="G1012" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1013" s="2" t="s">
+        <v>4910</v>
+      </c>
+      <c r="B1013" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1013" s="2" t="s">
+        <v>5002</v>
+      </c>
+      <c r="D1013" s="2" t="s">
+        <v>5003</v>
+      </c>
+      <c r="E1013" s="2" t="s">
+        <v>5004</v>
+      </c>
+      <c r="F1013" s="2" t="s">
+        <v>5005</v>
+      </c>
+      <c r="G1013" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1014" s="2" t="s">
+        <v>4911</v>
+      </c>
+      <c r="B1014" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1014" s="2" t="s">
+        <v>5006</v>
+      </c>
+      <c r="D1014" s="2" t="s">
+        <v>5007</v>
+      </c>
+      <c r="E1014" s="2" t="s">
+        <v>5009</v>
+      </c>
+      <c r="F1014" s="2" t="s">
+        <v>5008</v>
+      </c>
+      <c r="G1014" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1015" s="2" t="s">
+        <v>4912</v>
+      </c>
+      <c r="B1015" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1015" s="2" t="s">
+        <v>5010</v>
+      </c>
+      <c r="D1015" s="2" t="s">
+        <v>5011</v>
+      </c>
+      <c r="E1015" s="2" t="s">
+        <v>5012</v>
+      </c>
+      <c r="F1015" s="2" t="s">
+        <v>5013</v>
+      </c>
+      <c r="G1015" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1016" s="2" t="s">
+        <v>4913</v>
+      </c>
+      <c r="B1016" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1016" s="2" t="s">
+        <v>5014</v>
+      </c>
+      <c r="D1016" s="2" t="s">
+        <v>5015</v>
+      </c>
+      <c r="E1016" s="2" t="s">
+        <v>5016</v>
+      </c>
+      <c r="F1016" s="2" t="s">
+        <v>5017</v>
+      </c>
+      <c r="G1016" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1017" s="2" t="s">
+        <v>4914</v>
+      </c>
+      <c r="B1017" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1017" s="2" t="s">
+        <v>5018</v>
+      </c>
+      <c r="D1017" s="2" t="s">
+        <v>5019</v>
+      </c>
+      <c r="E1017" s="2" t="s">
+        <v>5020</v>
+      </c>
+      <c r="F1017" s="2" t="s">
+        <v>5021</v>
+      </c>
+      <c r="G1017" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1018" s="2" t="s">
+        <v>4915</v>
+      </c>
+      <c r="B1018" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1018" s="2" t="s">
+        <v>5022</v>
+      </c>
+      <c r="D1018" s="2" t="s">
+        <v>5023</v>
+      </c>
+      <c r="E1018" s="2" t="s">
+        <v>5024</v>
+      </c>
+      <c r="F1018" s="2" t="s">
+        <v>5025</v>
+      </c>
+      <c r="G1018" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1019" s="2" t="s">
+        <v>4916</v>
+      </c>
+      <c r="B1019" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1019" s="2" t="s">
+        <v>5026</v>
+      </c>
+      <c r="D1019" s="2" t="s">
+        <v>5027</v>
+      </c>
+      <c r="E1019" s="2" t="s">
+        <v>5028</v>
+      </c>
+      <c r="F1019" s="2" t="s">
+        <v>5029</v>
+      </c>
+      <c r="G1019" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1020" s="2" t="s">
+        <v>4917</v>
+      </c>
+      <c r="B1020" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1020" s="2" t="s">
+        <v>5030</v>
+      </c>
+      <c r="D1020" s="2" t="s">
+        <v>5031</v>
+      </c>
+      <c r="E1020" s="2" t="s">
+        <v>5032</v>
+      </c>
+      <c r="F1020" s="2" t="s">
+        <v>5033</v>
+      </c>
+      <c r="G1020" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1021" s="2" t="s">
+        <v>4918</v>
+      </c>
+      <c r="B1021" s="2">
+        <v>34</v>
+      </c>
+      <c r="C1021" s="2" t="s">
+        <v>5034</v>
+      </c>
+      <c r="D1021" s="2" t="s">
+        <v>5035</v>
+      </c>
+      <c r="E1021" s="2" t="s">
+        <v>5036</v>
+      </c>
+      <c r="F1021" s="2" t="s">
+        <v>5037</v>
+      </c>
+      <c r="G1021" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 35
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369FBD00-BA72-EC4E-ACAF-8BDA287E272C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DD0720-0C78-314E-A3D9-A8937F9D4F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5974" uniqueCount="5038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6154" uniqueCount="5187">
   <si>
     <t>ID</t>
   </si>
@@ -15144,6 +15144,453 @@
   </si>
   <si>
     <t>a moral issues / vấn đề đạo đức</t>
+  </si>
+  <si>
+    <t>U35_01</t>
+  </si>
+  <si>
+    <t>U35_02</t>
+  </si>
+  <si>
+    <t>U35_03</t>
+  </si>
+  <si>
+    <t>U35_04</t>
+  </si>
+  <si>
+    <t>U35_05</t>
+  </si>
+  <si>
+    <t>U35_06</t>
+  </si>
+  <si>
+    <t>U35_07</t>
+  </si>
+  <si>
+    <t>U35_08</t>
+  </si>
+  <si>
+    <t>U35_09</t>
+  </si>
+  <si>
+    <t>U35_10</t>
+  </si>
+  <si>
+    <t>U35_11</t>
+  </si>
+  <si>
+    <t>U35_12</t>
+  </si>
+  <si>
+    <t>U35_13</t>
+  </si>
+  <si>
+    <t>U35_14</t>
+  </si>
+  <si>
+    <t>U35_15</t>
+  </si>
+  <si>
+    <t>U35_16</t>
+  </si>
+  <si>
+    <t>U35_17</t>
+  </si>
+  <si>
+    <t>U35_18</t>
+  </si>
+  <si>
+    <t>U35_19</t>
+  </si>
+  <si>
+    <t>U35_20</t>
+  </si>
+  <si>
+    <t>U35_21</t>
+  </si>
+  <si>
+    <t>U35_22</t>
+  </si>
+  <si>
+    <t>U35_23</t>
+  </si>
+  <si>
+    <t>U35_24</t>
+  </si>
+  <si>
+    <t>U35_25</t>
+  </si>
+  <si>
+    <t>U35_26</t>
+  </si>
+  <si>
+    <t>U35_27</t>
+  </si>
+  <si>
+    <t>U35_28</t>
+  </si>
+  <si>
+    <t>U35_29</t>
+  </si>
+  <si>
+    <t>U35_30</t>
+  </si>
+  <si>
+    <t>Kỷ niệm</t>
+  </si>
+  <si>
+    <t>Anniversary</t>
+  </si>
+  <si>
+    <t>We are celebrating our wedding anniversary</t>
+  </si>
+  <si>
+    <t>A wedding anniversary</t>
+  </si>
+  <si>
+    <t>Cuộc hôn nhân</t>
+  </si>
+  <si>
+    <t>Marriage</t>
+  </si>
+  <si>
+    <t>There are arranged marriages in india</t>
+  </si>
+  <si>
+    <t>An arranged marriage / hôn nhân sắp đặt</t>
+  </si>
+  <si>
+    <t>Lãng mạn</t>
+  </si>
+  <si>
+    <t>Romantic</t>
+  </si>
+  <si>
+    <t>The couple has a beautiful romantic story</t>
+  </si>
+  <si>
+    <t>A romantic story</t>
+  </si>
+  <si>
+    <t>Đỏ mặt</t>
+  </si>
+  <si>
+    <t>Blush</t>
+  </si>
+  <si>
+    <t>His action made me blush with embarrassment</t>
+  </si>
+  <si>
+    <t>blush with embarrassment / đỏ mặt ngượng ngùng</t>
+  </si>
+  <si>
+    <t>Sự kết nối</t>
+  </si>
+  <si>
+    <t>Connection</t>
+  </si>
+  <si>
+    <t>The connection between them is strong</t>
+  </si>
+  <si>
+    <t>a connection between something or somebody</t>
+  </si>
+  <si>
+    <t>Instantly</t>
+  </si>
+  <si>
+    <t>Her voice is instantly recognizable.</t>
+  </si>
+  <si>
+    <t>instantly recognizable.</t>
+  </si>
+  <si>
+    <t>Rủ đi chơi</t>
+  </si>
+  <si>
+    <t>Ask out</t>
+  </si>
+  <si>
+    <t>Can I ask you out on a date?</t>
+  </si>
+  <si>
+    <t>Ask somebody out on a date / mời ai một buổi hẹn</t>
+  </si>
+  <si>
+    <t>Vững chắc</t>
+  </si>
+  <si>
+    <t>Steady</t>
+  </si>
+  <si>
+    <t>They try to maintain a steady relationship</t>
+  </si>
+  <si>
+    <t>steady relationship / mối quan hệ vững chắc</t>
+  </si>
+  <si>
+    <t>Phải lòng</t>
+  </si>
+  <si>
+    <t>Fall for</t>
+  </si>
+  <si>
+    <t>Don't make me fall for you.</t>
+  </si>
+  <si>
+    <t>fall for somebody</t>
+  </si>
+  <si>
+    <t>Hấp dẫn, quyến rũ</t>
+  </si>
+  <si>
+    <t>Attractive</t>
+  </si>
+  <si>
+    <t>She is an attractive person.</t>
+  </si>
+  <si>
+    <t>an attractive person / một người hấp dẫn</t>
+  </si>
+  <si>
+    <t>Rõ ràng</t>
+  </si>
+  <si>
+    <t>Obviously</t>
+  </si>
+  <si>
+    <t>Diet and exercise are obviously important.</t>
+  </si>
+  <si>
+    <t>to be obviously important</t>
+  </si>
+  <si>
+    <t>Chia tay</t>
+  </si>
+  <si>
+    <t>Break up</t>
+  </si>
+  <si>
+    <t>She cries when the actor breaks up with his girlfriend</t>
+  </si>
+  <si>
+    <t>break up with somebody</t>
+  </si>
+  <si>
+    <t>Liên hệ</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>We will contact you about the decision.</t>
+  </si>
+  <si>
+    <t>contact someone</t>
+  </si>
+  <si>
+    <t>Dịu dàng, nhẹ nhàng</t>
+  </si>
+  <si>
+    <t>Gentle</t>
+  </si>
+  <si>
+    <t>The singer has such a gentle voice.</t>
+  </si>
+  <si>
+    <t>a gentle voice / một chất giọng nhẹ nhàng</t>
+  </si>
+  <si>
+    <t>Lời nối dối</t>
+  </si>
+  <si>
+    <t>Lie</t>
+  </si>
+  <si>
+    <t>I don't think it's okay to tell a white lie.</t>
+  </si>
+  <si>
+    <t>a white lie / lời nói dối vô hại</t>
+  </si>
+  <si>
+    <t>Tình huống</t>
+  </si>
+  <si>
+    <t>Situation</t>
+  </si>
+  <si>
+    <t>I am facing a difficult situation now</t>
+  </si>
+  <si>
+    <t>a difficult situation</t>
+  </si>
+  <si>
+    <t>Lời bào chữa</t>
+  </si>
+  <si>
+    <t>Excuse</t>
+  </si>
+  <si>
+    <t>There is no excuse for arriving late.</t>
+  </si>
+  <si>
+    <t>an excuse for doing something / một cái cớ để làm một cái gì đó</t>
+  </si>
+  <si>
+    <t>Thư</t>
+  </si>
+  <si>
+    <t>Letter</t>
+  </si>
+  <si>
+    <t>I am sending a letter of complaint soon.</t>
+  </si>
+  <si>
+    <t>a letter of complaint / thư khiếu nại</t>
+  </si>
+  <si>
+    <t>Ý định</t>
+  </si>
+  <si>
+    <t>Intention</t>
+  </si>
+  <si>
+    <t>My intention of borrowing your car is to impress her</t>
+  </si>
+  <si>
+    <t>intention of doing something</t>
+  </si>
+  <si>
+    <t>Tha thứ</t>
+  </si>
+  <si>
+    <t>Forgive</t>
+  </si>
+  <si>
+    <t>Would you ever forgive me?</t>
+  </si>
+  <si>
+    <t>forgive somebody / tha thứ cho ai đó</t>
+  </si>
+  <si>
+    <t>Cô dâu</t>
+  </si>
+  <si>
+    <t>Bride</t>
+  </si>
+  <si>
+    <t>He introduces his new bride.</t>
+  </si>
+  <si>
+    <t>a new bride / vợ mới cưới</t>
+  </si>
+  <si>
+    <t>Chú rể</t>
+  </si>
+  <si>
+    <t>Groom</t>
+  </si>
+  <si>
+    <t>Let us toast to the (nâng ly chúc mừng) bride and groom.</t>
+  </si>
+  <si>
+    <t>The bride and groom / cô dâu chú rể</t>
+  </si>
+  <si>
+    <t>Hôn lễ</t>
+  </si>
+  <si>
+    <t>Wedding</t>
+  </si>
+  <si>
+    <t>Here is a wedding present for the bride.</t>
+  </si>
+  <si>
+    <t>a wedding present / một món quà cưới</t>
+  </si>
+  <si>
+    <t>Cặp đôi</t>
+  </si>
+  <si>
+    <t>Couple</t>
+  </si>
+  <si>
+    <t>We are officially a married couple.</t>
+  </si>
+  <si>
+    <t>a married couple / một cặp vợ chồng</t>
+  </si>
+  <si>
+    <t>Cảm xúc</t>
+  </si>
+  <si>
+    <t>Feeling</t>
+  </si>
+  <si>
+    <t>a feeling of sadness / cảm giác buồn bã</t>
+  </si>
+  <si>
+    <t>Losing (thất bại) gives me a feeling of sadness</t>
+  </si>
+  <si>
+    <t>Ấm áp, nồng nhiệt</t>
+  </si>
+  <si>
+    <t>Warm</t>
+  </si>
+  <si>
+    <t>The host extends a warm welcome to us.</t>
+  </si>
+  <si>
+    <t>a warm welcome / một sự chào đón nồng nhiệt</t>
+  </si>
+  <si>
+    <t>Đối diện</t>
+  </si>
+  <si>
+    <t>Opposite</t>
+  </si>
+  <si>
+    <t>he sits opposite you in class.</t>
+  </si>
+  <si>
+    <t>to be opposite something or someone</t>
+  </si>
+  <si>
+    <t>Kỳ cục</t>
+  </si>
+  <si>
+    <t>Weird</t>
+  </si>
+  <si>
+    <t>After lunch, my stomach had a weird feeling.</t>
+  </si>
+  <si>
+    <t>a weird feeling / một cảm giác kỳ lạ</t>
+  </si>
+  <si>
+    <t>Sẵn sàng</t>
+  </si>
+  <si>
+    <t>Willing</t>
+  </si>
+  <si>
+    <t>Would you be willing to help me?</t>
+  </si>
+  <si>
+    <t>To be willing to do something</t>
+  </si>
+  <si>
+    <t>Khoảnh khắc</t>
+  </si>
+  <si>
+    <t>Moment</t>
+  </si>
+  <si>
+    <t>She glanced at me for a brief moment</t>
+  </si>
+  <si>
+    <t>a brief moment / một khoảnh khắc ngắn ngủi</t>
   </si>
 </sst>
 </file>
@@ -15516,15 +15963,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1021"/>
+  <dimension ref="A1:G1051"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1001" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1022" sqref="C1022"/>
+    <sheetView tabSelected="1" topLeftCell="A1021" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1052" sqref="C1052"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -38710,6 +39157,696 @@
         <v>609</v>
       </c>
     </row>
+    <row r="1022" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1022" s="2" t="s">
+        <v>5038</v>
+      </c>
+      <c r="B1022" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1022" s="2" t="s">
+        <v>5068</v>
+      </c>
+      <c r="D1022" s="2" t="s">
+        <v>5069</v>
+      </c>
+      <c r="E1022" s="2" t="s">
+        <v>5070</v>
+      </c>
+      <c r="F1022" s="2" t="s">
+        <v>5071</v>
+      </c>
+      <c r="G1022" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1023" s="2" t="s">
+        <v>5039</v>
+      </c>
+      <c r="B1023" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1023" s="2" t="s">
+        <v>5072</v>
+      </c>
+      <c r="D1023" s="2" t="s">
+        <v>5073</v>
+      </c>
+      <c r="E1023" s="2" t="s">
+        <v>5074</v>
+      </c>
+      <c r="F1023" s="2" t="s">
+        <v>5075</v>
+      </c>
+      <c r="G1023" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1024" s="2" t="s">
+        <v>5040</v>
+      </c>
+      <c r="B1024" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1024" s="2" t="s">
+        <v>5076</v>
+      </c>
+      <c r="D1024" s="2" t="s">
+        <v>5077</v>
+      </c>
+      <c r="E1024" s="2" t="s">
+        <v>5078</v>
+      </c>
+      <c r="F1024" s="2" t="s">
+        <v>5079</v>
+      </c>
+      <c r="G1024" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1025" s="2" t="s">
+        <v>5041</v>
+      </c>
+      <c r="B1025" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1025" s="2" t="s">
+        <v>5080</v>
+      </c>
+      <c r="D1025" s="2" t="s">
+        <v>5081</v>
+      </c>
+      <c r="E1025" s="2" t="s">
+        <v>5082</v>
+      </c>
+      <c r="F1025" s="2" t="s">
+        <v>5083</v>
+      </c>
+      <c r="G1025" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1026" s="2" t="s">
+        <v>5042</v>
+      </c>
+      <c r="B1026" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1026" s="2" t="s">
+        <v>5084</v>
+      </c>
+      <c r="D1026" s="2" t="s">
+        <v>5085</v>
+      </c>
+      <c r="E1026" s="2" t="s">
+        <v>5086</v>
+      </c>
+      <c r="F1026" s="2" t="s">
+        <v>5087</v>
+      </c>
+      <c r="G1026" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1027" s="2" t="s">
+        <v>5043</v>
+      </c>
+      <c r="B1027" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1027" s="2" t="s">
+        <v>4110</v>
+      </c>
+      <c r="D1027" s="2" t="s">
+        <v>5088</v>
+      </c>
+      <c r="E1027" s="2" t="s">
+        <v>5089</v>
+      </c>
+      <c r="F1027" s="2" t="s">
+        <v>5090</v>
+      </c>
+      <c r="G1027" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1028" s="2" t="s">
+        <v>5044</v>
+      </c>
+      <c r="B1028" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1028" s="2" t="s">
+        <v>5091</v>
+      </c>
+      <c r="D1028" s="2" t="s">
+        <v>5092</v>
+      </c>
+      <c r="E1028" s="2" t="s">
+        <v>5093</v>
+      </c>
+      <c r="F1028" s="2" t="s">
+        <v>5094</v>
+      </c>
+      <c r="G1028" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1029" s="2" t="s">
+        <v>5045</v>
+      </c>
+      <c r="B1029" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1029" s="2" t="s">
+        <v>5095</v>
+      </c>
+      <c r="D1029" s="2" t="s">
+        <v>5096</v>
+      </c>
+      <c r="E1029" s="2" t="s">
+        <v>5097</v>
+      </c>
+      <c r="F1029" s="2" t="s">
+        <v>5098</v>
+      </c>
+      <c r="G1029" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1030" s="2" t="s">
+        <v>5046</v>
+      </c>
+      <c r="B1030" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1030" s="2" t="s">
+        <v>5099</v>
+      </c>
+      <c r="D1030" s="2" t="s">
+        <v>5100</v>
+      </c>
+      <c r="E1030" s="2" t="s">
+        <v>5101</v>
+      </c>
+      <c r="F1030" s="2" t="s">
+        <v>5102</v>
+      </c>
+      <c r="G1030" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1031" s="2" t="s">
+        <v>5047</v>
+      </c>
+      <c r="B1031" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1031" s="2" t="s">
+        <v>5103</v>
+      </c>
+      <c r="D1031" s="2" t="s">
+        <v>5104</v>
+      </c>
+      <c r="E1031" s="2" t="s">
+        <v>5105</v>
+      </c>
+      <c r="F1031" s="2" t="s">
+        <v>5106</v>
+      </c>
+      <c r="G1031" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1032" s="2" t="s">
+        <v>5048</v>
+      </c>
+      <c r="B1032" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1032" s="2" t="s">
+        <v>5107</v>
+      </c>
+      <c r="D1032" s="2" t="s">
+        <v>5108</v>
+      </c>
+      <c r="E1032" s="2" t="s">
+        <v>5109</v>
+      </c>
+      <c r="F1032" s="2" t="s">
+        <v>5110</v>
+      </c>
+      <c r="G1032" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1033" s="2" t="s">
+        <v>5049</v>
+      </c>
+      <c r="B1033" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1033" s="2" t="s">
+        <v>5111</v>
+      </c>
+      <c r="D1033" s="2" t="s">
+        <v>5112</v>
+      </c>
+      <c r="E1033" s="2" t="s">
+        <v>5113</v>
+      </c>
+      <c r="F1033" s="2" t="s">
+        <v>5114</v>
+      </c>
+      <c r="G1033" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1034" s="2" t="s">
+        <v>5050</v>
+      </c>
+      <c r="B1034" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1034" s="2" t="s">
+        <v>5115</v>
+      </c>
+      <c r="D1034" s="2" t="s">
+        <v>5116</v>
+      </c>
+      <c r="E1034" s="2" t="s">
+        <v>5117</v>
+      </c>
+      <c r="F1034" s="2" t="s">
+        <v>5118</v>
+      </c>
+      <c r="G1034" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1035" s="2" t="s">
+        <v>5051</v>
+      </c>
+      <c r="B1035" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1035" s="2" t="s">
+        <v>5119</v>
+      </c>
+      <c r="D1035" s="2" t="s">
+        <v>5120</v>
+      </c>
+      <c r="E1035" s="2" t="s">
+        <v>5121</v>
+      </c>
+      <c r="F1035" s="2" t="s">
+        <v>5122</v>
+      </c>
+      <c r="G1035" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1036" s="2" t="s">
+        <v>5052</v>
+      </c>
+      <c r="B1036" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1036" s="2" t="s">
+        <v>5123</v>
+      </c>
+      <c r="D1036" s="2" t="s">
+        <v>5124</v>
+      </c>
+      <c r="E1036" s="2" t="s">
+        <v>5125</v>
+      </c>
+      <c r="F1036" s="2" t="s">
+        <v>5126</v>
+      </c>
+      <c r="G1036" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1037" s="2" t="s">
+        <v>5053</v>
+      </c>
+      <c r="B1037" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1037" s="2" t="s">
+        <v>5127</v>
+      </c>
+      <c r="D1037" s="2" t="s">
+        <v>5128</v>
+      </c>
+      <c r="E1037" s="2" t="s">
+        <v>5129</v>
+      </c>
+      <c r="F1037" s="2" t="s">
+        <v>5130</v>
+      </c>
+      <c r="G1037" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1038" s="2" t="s">
+        <v>5054</v>
+      </c>
+      <c r="B1038" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1038" s="2" t="s">
+        <v>5131</v>
+      </c>
+      <c r="D1038" s="2" t="s">
+        <v>5132</v>
+      </c>
+      <c r="E1038" s="2" t="s">
+        <v>5133</v>
+      </c>
+      <c r="F1038" s="2" t="s">
+        <v>5134</v>
+      </c>
+      <c r="G1038" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1039" s="2" t="s">
+        <v>5055</v>
+      </c>
+      <c r="B1039" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1039" s="2" t="s">
+        <v>5135</v>
+      </c>
+      <c r="D1039" s="2" t="s">
+        <v>5136</v>
+      </c>
+      <c r="E1039" s="2" t="s">
+        <v>5137</v>
+      </c>
+      <c r="F1039" s="2" t="s">
+        <v>5138</v>
+      </c>
+      <c r="G1039" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1040" s="2" t="s">
+        <v>5056</v>
+      </c>
+      <c r="B1040" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1040" s="2" t="s">
+        <v>5139</v>
+      </c>
+      <c r="D1040" s="2" t="s">
+        <v>5140</v>
+      </c>
+      <c r="E1040" s="2" t="s">
+        <v>5141</v>
+      </c>
+      <c r="F1040" s="2" t="s">
+        <v>5142</v>
+      </c>
+      <c r="G1040" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1041" s="2" t="s">
+        <v>5057</v>
+      </c>
+      <c r="B1041" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1041" s="2" t="s">
+        <v>5143</v>
+      </c>
+      <c r="D1041" s="2" t="s">
+        <v>5144</v>
+      </c>
+      <c r="E1041" s="2" t="s">
+        <v>5145</v>
+      </c>
+      <c r="F1041" s="2" t="s">
+        <v>5146</v>
+      </c>
+      <c r="G1041" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1042" s="2" t="s">
+        <v>5058</v>
+      </c>
+      <c r="B1042" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1042" s="2" t="s">
+        <v>5147</v>
+      </c>
+      <c r="D1042" s="2" t="s">
+        <v>5148</v>
+      </c>
+      <c r="E1042" s="2" t="s">
+        <v>5149</v>
+      </c>
+      <c r="F1042" s="2" t="s">
+        <v>5150</v>
+      </c>
+      <c r="G1042" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1043" s="2" t="s">
+        <v>5059</v>
+      </c>
+      <c r="B1043" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1043" s="2" t="s">
+        <v>5151</v>
+      </c>
+      <c r="D1043" s="2" t="s">
+        <v>5152</v>
+      </c>
+      <c r="E1043" s="2" t="s">
+        <v>5153</v>
+      </c>
+      <c r="F1043" s="2" t="s">
+        <v>5154</v>
+      </c>
+      <c r="G1043" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1044" s="2" t="s">
+        <v>5060</v>
+      </c>
+      <c r="B1044" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1044" s="2" t="s">
+        <v>5155</v>
+      </c>
+      <c r="D1044" s="2" t="s">
+        <v>5156</v>
+      </c>
+      <c r="E1044" s="2" t="s">
+        <v>5157</v>
+      </c>
+      <c r="F1044" s="2" t="s">
+        <v>5158</v>
+      </c>
+      <c r="G1044" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1045" s="2" t="s">
+        <v>5061</v>
+      </c>
+      <c r="B1045" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1045" s="2" t="s">
+        <v>5159</v>
+      </c>
+      <c r="D1045" s="2" t="s">
+        <v>5160</v>
+      </c>
+      <c r="E1045" s="2" t="s">
+        <v>5161</v>
+      </c>
+      <c r="F1045" s="2" t="s">
+        <v>5162</v>
+      </c>
+      <c r="G1045" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1046" s="2" t="s">
+        <v>5062</v>
+      </c>
+      <c r="B1046" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1046" s="2" t="s">
+        <v>5163</v>
+      </c>
+      <c r="D1046" s="2" t="s">
+        <v>5164</v>
+      </c>
+      <c r="E1046" s="2" t="s">
+        <v>5166</v>
+      </c>
+      <c r="F1046" s="2" t="s">
+        <v>5165</v>
+      </c>
+      <c r="G1046" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1047" s="2" t="s">
+        <v>5063</v>
+      </c>
+      <c r="B1047" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1047" s="2" t="s">
+        <v>5167</v>
+      </c>
+      <c r="D1047" s="2" t="s">
+        <v>5168</v>
+      </c>
+      <c r="E1047" s="2" t="s">
+        <v>5169</v>
+      </c>
+      <c r="F1047" s="2" t="s">
+        <v>5170</v>
+      </c>
+      <c r="G1047" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1048" s="2" t="s">
+        <v>5064</v>
+      </c>
+      <c r="B1048" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1048" s="2" t="s">
+        <v>5171</v>
+      </c>
+      <c r="D1048" s="2" t="s">
+        <v>5172</v>
+      </c>
+      <c r="E1048" s="2" t="s">
+        <v>5173</v>
+      </c>
+      <c r="F1048" s="2" t="s">
+        <v>5174</v>
+      </c>
+      <c r="G1048" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1049" s="2" t="s">
+        <v>5065</v>
+      </c>
+      <c r="B1049" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1049" s="2" t="s">
+        <v>5175</v>
+      </c>
+      <c r="D1049" s="2" t="s">
+        <v>5176</v>
+      </c>
+      <c r="E1049" s="2" t="s">
+        <v>5177</v>
+      </c>
+      <c r="F1049" s="2" t="s">
+        <v>5178</v>
+      </c>
+      <c r="G1049" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1050" s="2" t="s">
+        <v>5066</v>
+      </c>
+      <c r="B1050" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1050" s="2" t="s">
+        <v>5179</v>
+      </c>
+      <c r="D1050" s="2" t="s">
+        <v>5180</v>
+      </c>
+      <c r="E1050" s="2" t="s">
+        <v>5181</v>
+      </c>
+      <c r="F1050" s="2" t="s">
+        <v>5182</v>
+      </c>
+      <c r="G1050" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1051" s="2" t="s">
+        <v>5067</v>
+      </c>
+      <c r="B1051" s="2">
+        <v>35</v>
+      </c>
+      <c r="C1051" s="2" t="s">
+        <v>5183</v>
+      </c>
+      <c r="D1051" s="2" t="s">
+        <v>5184</v>
+      </c>
+      <c r="E1051" s="2" t="s">
+        <v>5185</v>
+      </c>
+      <c r="F1051" s="2" t="s">
+        <v>5186</v>
+      </c>
+      <c r="G1051" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 36
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DD0720-0C78-314E-A3D9-A8937F9D4F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6BC4D7-D90F-7047-96AE-19B9A5726E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6154" uniqueCount="5187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6334" uniqueCount="5335">
   <si>
     <t>ID</t>
   </si>
@@ -15591,6 +15591,450 @@
   </si>
   <si>
     <t>a brief moment / một khoảnh khắc ngắn ngủi</t>
+  </si>
+  <si>
+    <t>U36_01</t>
+  </si>
+  <si>
+    <t>U36_02</t>
+  </si>
+  <si>
+    <t>U36_03</t>
+  </si>
+  <si>
+    <t>U36_04</t>
+  </si>
+  <si>
+    <t>U36_05</t>
+  </si>
+  <si>
+    <t>U36_06</t>
+  </si>
+  <si>
+    <t>U36_07</t>
+  </si>
+  <si>
+    <t>U36_08</t>
+  </si>
+  <si>
+    <t>U36_09</t>
+  </si>
+  <si>
+    <t>U36_10</t>
+  </si>
+  <si>
+    <t>U36_11</t>
+  </si>
+  <si>
+    <t>U36_12</t>
+  </si>
+  <si>
+    <t>U36_13</t>
+  </si>
+  <si>
+    <t>U36_14</t>
+  </si>
+  <si>
+    <t>U36_15</t>
+  </si>
+  <si>
+    <t>U36_16</t>
+  </si>
+  <si>
+    <t>U36_17</t>
+  </si>
+  <si>
+    <t>U36_18</t>
+  </si>
+  <si>
+    <t>U36_19</t>
+  </si>
+  <si>
+    <t>U36_20</t>
+  </si>
+  <si>
+    <t>U36_21</t>
+  </si>
+  <si>
+    <t>U36_22</t>
+  </si>
+  <si>
+    <t>U36_23</t>
+  </si>
+  <si>
+    <t>U36_24</t>
+  </si>
+  <si>
+    <t>U36_25</t>
+  </si>
+  <si>
+    <t>U36_26</t>
+  </si>
+  <si>
+    <t>U36_27</t>
+  </si>
+  <si>
+    <t>U36_28</t>
+  </si>
+  <si>
+    <t>U36_29</t>
+  </si>
+  <si>
+    <t>U36_30</t>
+  </si>
+  <si>
+    <t>Flight</t>
+  </si>
+  <si>
+    <t>Chuyến bay</t>
+  </si>
+  <si>
+    <t>International flights are currently delayed.</t>
+  </si>
+  <si>
+    <t>An international flight</t>
+  </si>
+  <si>
+    <t>Trả lại</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Please return the book to the library</t>
+  </si>
+  <si>
+    <t>Return something to somewhere</t>
+  </si>
+  <si>
+    <t>Cất cánh</t>
+  </si>
+  <si>
+    <t>Take off</t>
+  </si>
+  <si>
+    <t>The plane will take off soon</t>
+  </si>
+  <si>
+    <t>a plane takes off</t>
+  </si>
+  <si>
+    <t>Cổng</t>
+  </si>
+  <si>
+    <t>Gate</t>
+  </si>
+  <si>
+    <t>Please open the gate for my car.</t>
+  </si>
+  <si>
+    <t>open the gate</t>
+  </si>
+  <si>
+    <t>Nhập</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>Enter your password to log in.</t>
+  </si>
+  <si>
+    <t>Enter a password</t>
+  </si>
+  <si>
+    <t>Carry-on</t>
+  </si>
+  <si>
+    <t>Carry-on luggage can be stored under the seat.</t>
+  </si>
+  <si>
+    <t>carry-on luggage / hành lý xách tay</t>
+  </si>
+  <si>
+    <t>Hành lý</t>
+  </si>
+  <si>
+    <t>Xách tay</t>
+  </si>
+  <si>
+    <t>Luggage</t>
+  </si>
+  <si>
+    <t>You can only bring 2 pieces of luggage.</t>
+  </si>
+  <si>
+    <t>A piece of luggage / món hành lý</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>The long distance will make me tired.</t>
+  </si>
+  <si>
+    <t>Long distance / khoảng cách xa</t>
+  </si>
+  <si>
+    <t>Sự đến</t>
+  </si>
+  <si>
+    <t>Arrival</t>
+  </si>
+  <si>
+    <t>Upon arrival, they checked in at the reception.</t>
+  </si>
+  <si>
+    <t>On or upon arrival / khi đến nơi</t>
+  </si>
+  <si>
+    <t>Hành khách</t>
+  </si>
+  <si>
+    <t>Passenger</t>
+  </si>
+  <si>
+    <t>All passenger trains are currently full.</t>
+  </si>
+  <si>
+    <t>A passenger train / tàu chở khách</t>
+  </si>
+  <si>
+    <t>Cảng</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>port of entry / cảng nhập cảnh</t>
+  </si>
+  <si>
+    <t>We examine the goods (kiểm tra hàng hóa) at the port of entry.</t>
+  </si>
+  <si>
+    <t>Ferry</t>
+  </si>
+  <si>
+    <t>Phà</t>
+  </si>
+  <si>
+    <t>We take the ferry across the river every day.</t>
+  </si>
+  <si>
+    <t>Take the ferry / đi phà</t>
+  </si>
+  <si>
+    <t>Tuyến đường</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>The route to the hotel is dangerous.</t>
+  </si>
+  <si>
+    <t>The route to somewhere</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Flying from Hanoi to HCM city is a direct flight.</t>
+  </si>
+  <si>
+    <t>A direct flight / chuyến bay thẳng</t>
+  </si>
+  <si>
+    <t>Tai nạn</t>
+  </si>
+  <si>
+    <t>Accident</t>
+  </si>
+  <si>
+    <t>That family had a tragic accidient last month.</t>
+  </si>
+  <si>
+    <t>a tragic accident / tai nạn bi thảm</t>
+  </si>
+  <si>
+    <t>Tiếp tục</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>Continue reading on the next chapter</t>
+  </si>
+  <si>
+    <t>continue doing something</t>
+  </si>
+  <si>
+    <t>Dạo quanh</t>
+  </si>
+  <si>
+    <t>Get around</t>
+  </si>
+  <si>
+    <t>I need a car to get around town</t>
+  </si>
+  <si>
+    <t>get around town / dạo quanh thị trấn</t>
+  </si>
+  <si>
+    <t>Nhà ga</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Please take me to the train station</t>
+  </si>
+  <si>
+    <t>the train station / nhà ga tàu hỏa</t>
+  </si>
+  <si>
+    <t>Động cơ</t>
+  </si>
+  <si>
+    <t>Engine</t>
+  </si>
+  <si>
+    <t>We cannot move because the car engine is broken.</t>
+  </si>
+  <si>
+    <t>a car engine</t>
+  </si>
+  <si>
+    <t>Bánh xe</t>
+  </si>
+  <si>
+    <t>Wheel</t>
+  </si>
+  <si>
+    <t>Please have a spare wheel for your car</t>
+  </si>
+  <si>
+    <t>a spare wheel / một cái bánh xe dự phòng</t>
+  </si>
+  <si>
+    <t>Tốc độ</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>The athlete ran at the speed of light.</t>
+  </si>
+  <si>
+    <t>The speed of light / tốc độ ánh sáng</t>
+  </si>
+  <si>
+    <t>Mũ bảo hiểm</t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>Wear a safety helmet to prevent accidents</t>
+  </si>
+  <si>
+    <t>a safety helmet / mũ bảo hiểm</t>
+  </si>
+  <si>
+    <t>Băng qua</t>
+  </si>
+  <si>
+    <t>Cross</t>
+  </si>
+  <si>
+    <t>I helped an elderly woman cross the street</t>
+  </si>
+  <si>
+    <t>cross a street / sang đường</t>
+  </si>
+  <si>
+    <t>Nút giao thông</t>
+  </si>
+  <si>
+    <t>Intersection</t>
+  </si>
+  <si>
+    <t>There is traffic at the major intersection</t>
+  </si>
+  <si>
+    <t>A major intersection / Nút giao thông trọng yếu</t>
+  </si>
+  <si>
+    <t>Việc đỗ xe</t>
+  </si>
+  <si>
+    <t>Parking</t>
+  </si>
+  <si>
+    <t>She found a parking space for my car.</t>
+  </si>
+  <si>
+    <t>a parking space / một chổ đậu xe</t>
+  </si>
+  <si>
+    <t>Đường quốc lộ</t>
+  </si>
+  <si>
+    <t>Highway</t>
+  </si>
+  <si>
+    <t>We are driving on the highway to Vinh</t>
+  </si>
+  <si>
+    <t>On the highway / trên đường quốc lộ</t>
+  </si>
+  <si>
+    <t>Hướng</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>The car is coming from the opposite direction</t>
+  </si>
+  <si>
+    <t>the opposite direction / hướng đối diện</t>
+  </si>
+  <si>
+    <t>Một chiều</t>
+  </si>
+  <si>
+    <t>One-way</t>
+  </si>
+  <si>
+    <t>The one-way traffic prevents us from turning around</t>
+  </si>
+  <si>
+    <t>one-way traffic / giao thông một chiều</t>
+  </si>
+  <si>
+    <t>Xe tải</t>
+  </si>
+  <si>
+    <t>Truck</t>
+  </si>
+  <si>
+    <t>Truck drivers need a special license</t>
+  </si>
+  <si>
+    <t>a truck driver / tài xế xe tải</t>
+  </si>
+  <si>
+    <t>Cái phanh</t>
+  </si>
+  <si>
+    <t>Brake</t>
+  </si>
+  <si>
+    <t>The brake pedal is broken</t>
+  </si>
+  <si>
+    <t>The brake pedal / bàn đạp phanh</t>
   </si>
 </sst>
 </file>
@@ -15963,10 +16407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1051"/>
+  <dimension ref="A1:G1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1021" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1052" sqref="C1052"/>
+    <sheetView tabSelected="1" topLeftCell="B1058" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1082" sqref="C1082"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39847,6 +40291,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="1052" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1052" s="2" t="s">
+        <v>5187</v>
+      </c>
+      <c r="B1052" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1052" s="2" t="s">
+        <v>5218</v>
+      </c>
+      <c r="D1052" s="2" t="s">
+        <v>5217</v>
+      </c>
+      <c r="E1052" s="2" t="s">
+        <v>5219</v>
+      </c>
+      <c r="F1052" s="2" t="s">
+        <v>5220</v>
+      </c>
+      <c r="G1052" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1053" s="2" t="s">
+        <v>5188</v>
+      </c>
+      <c r="B1053" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1053" s="2" t="s">
+        <v>5221</v>
+      </c>
+      <c r="D1053" s="2" t="s">
+        <v>5222</v>
+      </c>
+      <c r="E1053" s="2" t="s">
+        <v>5223</v>
+      </c>
+      <c r="F1053" s="2" t="s">
+        <v>5224</v>
+      </c>
+      <c r="G1053" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1054" s="2" t="s">
+        <v>5189</v>
+      </c>
+      <c r="B1054" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1054" s="2" t="s">
+        <v>5225</v>
+      </c>
+      <c r="D1054" s="2" t="s">
+        <v>5226</v>
+      </c>
+      <c r="E1054" s="2" t="s">
+        <v>5227</v>
+      </c>
+      <c r="F1054" s="2" t="s">
+        <v>5228</v>
+      </c>
+      <c r="G1054" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1055" s="2" t="s">
+        <v>5190</v>
+      </c>
+      <c r="B1055" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1055" s="2" t="s">
+        <v>5229</v>
+      </c>
+      <c r="D1055" s="2" t="s">
+        <v>5230</v>
+      </c>
+      <c r="E1055" s="2" t="s">
+        <v>5231</v>
+      </c>
+      <c r="F1055" s="2" t="s">
+        <v>5232</v>
+      </c>
+      <c r="G1055" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1056" s="2" t="s">
+        <v>5191</v>
+      </c>
+      <c r="B1056" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1056" s="2" t="s">
+        <v>5233</v>
+      </c>
+      <c r="D1056" s="2" t="s">
+        <v>5234</v>
+      </c>
+      <c r="E1056" s="2" t="s">
+        <v>5235</v>
+      </c>
+      <c r="F1056" s="2" t="s">
+        <v>5236</v>
+      </c>
+      <c r="G1056" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1057" s="2" t="s">
+        <v>5192</v>
+      </c>
+      <c r="B1057" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1057" s="2" t="s">
+        <v>5241</v>
+      </c>
+      <c r="D1057" s="2" t="s">
+        <v>5237</v>
+      </c>
+      <c r="E1057" s="2" t="s">
+        <v>5238</v>
+      </c>
+      <c r="F1057" s="2" t="s">
+        <v>5239</v>
+      </c>
+      <c r="G1057" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1058" s="2" t="s">
+        <v>5193</v>
+      </c>
+      <c r="B1058" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1058" s="2" t="s">
+        <v>5240</v>
+      </c>
+      <c r="D1058" s="2" t="s">
+        <v>5242</v>
+      </c>
+      <c r="E1058" s="2" t="s">
+        <v>5243</v>
+      </c>
+      <c r="F1058" s="2" t="s">
+        <v>5244</v>
+      </c>
+      <c r="G1058" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1059" s="2" t="s">
+        <v>5194</v>
+      </c>
+      <c r="B1059" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1059" s="2" t="s">
+        <v>2495</v>
+      </c>
+      <c r="D1059" s="2" t="s">
+        <v>5245</v>
+      </c>
+      <c r="E1059" s="2" t="s">
+        <v>5246</v>
+      </c>
+      <c r="F1059" s="2" t="s">
+        <v>5247</v>
+      </c>
+      <c r="G1059" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1060" s="2" t="s">
+        <v>5195</v>
+      </c>
+      <c r="B1060" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1060" s="2" t="s">
+        <v>5248</v>
+      </c>
+      <c r="D1060" s="2" t="s">
+        <v>5249</v>
+      </c>
+      <c r="E1060" s="2" t="s">
+        <v>5250</v>
+      </c>
+      <c r="F1060" s="2" t="s">
+        <v>5251</v>
+      </c>
+      <c r="G1060" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1061" s="2" t="s">
+        <v>5196</v>
+      </c>
+      <c r="B1061" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1061" s="2" t="s">
+        <v>5252</v>
+      </c>
+      <c r="D1061" s="2" t="s">
+        <v>5253</v>
+      </c>
+      <c r="E1061" s="2" t="s">
+        <v>5254</v>
+      </c>
+      <c r="F1061" s="2" t="s">
+        <v>5255</v>
+      </c>
+      <c r="G1061" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1062" s="2" t="s">
+        <v>5197</v>
+      </c>
+      <c r="B1062" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1062" s="2" t="s">
+        <v>5256</v>
+      </c>
+      <c r="D1062" s="2" t="s">
+        <v>5257</v>
+      </c>
+      <c r="E1062" s="2" t="s">
+        <v>5259</v>
+      </c>
+      <c r="F1062" s="2" t="s">
+        <v>5258</v>
+      </c>
+      <c r="G1062" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1063" s="2" t="s">
+        <v>5198</v>
+      </c>
+      <c r="B1063" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1063" s="2" t="s">
+        <v>5261</v>
+      </c>
+      <c r="D1063" s="2" t="s">
+        <v>5260</v>
+      </c>
+      <c r="E1063" s="2" t="s">
+        <v>5262</v>
+      </c>
+      <c r="F1063" s="2" t="s">
+        <v>5263</v>
+      </c>
+      <c r="G1063" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1064" s="2" t="s">
+        <v>5199</v>
+      </c>
+      <c r="B1064" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1064" s="2" t="s">
+        <v>5264</v>
+      </c>
+      <c r="D1064" s="2" t="s">
+        <v>5265</v>
+      </c>
+      <c r="E1064" s="2" t="s">
+        <v>5266</v>
+      </c>
+      <c r="F1064" s="2" t="s">
+        <v>5267</v>
+      </c>
+      <c r="G1064" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1065" s="2" t="s">
+        <v>5200</v>
+      </c>
+      <c r="B1065" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1065" s="2" t="s">
+        <v>4434</v>
+      </c>
+      <c r="D1065" s="2" t="s">
+        <v>5268</v>
+      </c>
+      <c r="E1065" s="2" t="s">
+        <v>5269</v>
+      </c>
+      <c r="F1065" s="2" t="s">
+        <v>5270</v>
+      </c>
+      <c r="G1065" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1066" s="2" t="s">
+        <v>5201</v>
+      </c>
+      <c r="B1066" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1066" s="2" t="s">
+        <v>5271</v>
+      </c>
+      <c r="D1066" s="2" t="s">
+        <v>5272</v>
+      </c>
+      <c r="E1066" s="2" t="s">
+        <v>5273</v>
+      </c>
+      <c r="F1066" s="2" t="s">
+        <v>5274</v>
+      </c>
+      <c r="G1066" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1067" s="2" t="s">
+        <v>5202</v>
+      </c>
+      <c r="B1067" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1067" s="2" t="s">
+        <v>5275</v>
+      </c>
+      <c r="D1067" s="2" t="s">
+        <v>5276</v>
+      </c>
+      <c r="E1067" s="2" t="s">
+        <v>5277</v>
+      </c>
+      <c r="F1067" s="2" t="s">
+        <v>5278</v>
+      </c>
+      <c r="G1067" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1068" s="2" t="s">
+        <v>5203</v>
+      </c>
+      <c r="B1068" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1068" s="2" t="s">
+        <v>5279</v>
+      </c>
+      <c r="D1068" s="2" t="s">
+        <v>5280</v>
+      </c>
+      <c r="E1068" s="2" t="s">
+        <v>5281</v>
+      </c>
+      <c r="F1068" s="2" t="s">
+        <v>5282</v>
+      </c>
+      <c r="G1068" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1069" s="2" t="s">
+        <v>5204</v>
+      </c>
+      <c r="B1069" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1069" s="2" t="s">
+        <v>5283</v>
+      </c>
+      <c r="D1069" s="2" t="s">
+        <v>5284</v>
+      </c>
+      <c r="E1069" s="2" t="s">
+        <v>5285</v>
+      </c>
+      <c r="F1069" s="2" t="s">
+        <v>5286</v>
+      </c>
+      <c r="G1069" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1070" s="2" t="s">
+        <v>5205</v>
+      </c>
+      <c r="B1070" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1070" s="2" t="s">
+        <v>5287</v>
+      </c>
+      <c r="D1070" s="2" t="s">
+        <v>5288</v>
+      </c>
+      <c r="E1070" s="2" t="s">
+        <v>5289</v>
+      </c>
+      <c r="F1070" s="2" t="s">
+        <v>5290</v>
+      </c>
+      <c r="G1070" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1071" s="2" t="s">
+        <v>5206</v>
+      </c>
+      <c r="B1071" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1071" s="2" t="s">
+        <v>5291</v>
+      </c>
+      <c r="D1071" s="2" t="s">
+        <v>5292</v>
+      </c>
+      <c r="E1071" s="2" t="s">
+        <v>5293</v>
+      </c>
+      <c r="F1071" s="2" t="s">
+        <v>5294</v>
+      </c>
+      <c r="G1071" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1072" s="2" t="s">
+        <v>5207</v>
+      </c>
+      <c r="B1072" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1072" s="2" t="s">
+        <v>5295</v>
+      </c>
+      <c r="D1072" s="2" t="s">
+        <v>5296</v>
+      </c>
+      <c r="E1072" s="2" t="s">
+        <v>5297</v>
+      </c>
+      <c r="F1072" s="2" t="s">
+        <v>5298</v>
+      </c>
+      <c r="G1072" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1073" s="2" t="s">
+        <v>5208</v>
+      </c>
+      <c r="B1073" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1073" s="2" t="s">
+        <v>5299</v>
+      </c>
+      <c r="D1073" s="2" t="s">
+        <v>5300</v>
+      </c>
+      <c r="E1073" s="2" t="s">
+        <v>5301</v>
+      </c>
+      <c r="F1073" s="2" t="s">
+        <v>5302</v>
+      </c>
+      <c r="G1073" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1074" s="2" t="s">
+        <v>5209</v>
+      </c>
+      <c r="B1074" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1074" s="2" t="s">
+        <v>5303</v>
+      </c>
+      <c r="D1074" s="2" t="s">
+        <v>5304</v>
+      </c>
+      <c r="E1074" s="2" t="s">
+        <v>5305</v>
+      </c>
+      <c r="F1074" s="2" t="s">
+        <v>5306</v>
+      </c>
+      <c r="G1074" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1075" s="2" t="s">
+        <v>5210</v>
+      </c>
+      <c r="B1075" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1075" s="2" t="s">
+        <v>5307</v>
+      </c>
+      <c r="D1075" s="2" t="s">
+        <v>5308</v>
+      </c>
+      <c r="E1075" s="2" t="s">
+        <v>5309</v>
+      </c>
+      <c r="F1075" s="2" t="s">
+        <v>5310</v>
+      </c>
+      <c r="G1075" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1076" s="2" t="s">
+        <v>5211</v>
+      </c>
+      <c r="B1076" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1076" s="2" t="s">
+        <v>5311</v>
+      </c>
+      <c r="D1076" s="2" t="s">
+        <v>5312</v>
+      </c>
+      <c r="E1076" s="2" t="s">
+        <v>5313</v>
+      </c>
+      <c r="F1076" s="2" t="s">
+        <v>5314</v>
+      </c>
+      <c r="G1076" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1077" s="2" t="s">
+        <v>5212</v>
+      </c>
+      <c r="B1077" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1077" s="2" t="s">
+        <v>5315</v>
+      </c>
+      <c r="D1077" s="2" t="s">
+        <v>5316</v>
+      </c>
+      <c r="E1077" s="2" t="s">
+        <v>5317</v>
+      </c>
+      <c r="F1077" s="2" t="s">
+        <v>5318</v>
+      </c>
+      <c r="G1077" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1078" s="2" t="s">
+        <v>5213</v>
+      </c>
+      <c r="B1078" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1078" s="2" t="s">
+        <v>5319</v>
+      </c>
+      <c r="D1078" s="2" t="s">
+        <v>5320</v>
+      </c>
+      <c r="E1078" s="2" t="s">
+        <v>5321</v>
+      </c>
+      <c r="F1078" s="2" t="s">
+        <v>5322</v>
+      </c>
+      <c r="G1078" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1079" s="2" t="s">
+        <v>5214</v>
+      </c>
+      <c r="B1079" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1079" s="2" t="s">
+        <v>5323</v>
+      </c>
+      <c r="D1079" s="2" t="s">
+        <v>5324</v>
+      </c>
+      <c r="E1079" s="2" t="s">
+        <v>5325</v>
+      </c>
+      <c r="F1079" s="2" t="s">
+        <v>5326</v>
+      </c>
+      <c r="G1079" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1080" s="2" t="s">
+        <v>5215</v>
+      </c>
+      <c r="B1080" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1080" s="2" t="s">
+        <v>5327</v>
+      </c>
+      <c r="D1080" s="2" t="s">
+        <v>5328</v>
+      </c>
+      <c r="E1080" s="2" t="s">
+        <v>5329</v>
+      </c>
+      <c r="F1080" s="2" t="s">
+        <v>5330</v>
+      </c>
+      <c r="G1080" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1081" s="2" t="s">
+        <v>5216</v>
+      </c>
+      <c r="B1081" s="2">
+        <v>36</v>
+      </c>
+      <c r="C1081" s="2" t="s">
+        <v>5331</v>
+      </c>
+      <c r="D1081" s="2" t="s">
+        <v>5332</v>
+      </c>
+      <c r="E1081" s="2" t="s">
+        <v>5333</v>
+      </c>
+      <c r="F1081" s="2" t="s">
+        <v>5334</v>
+      </c>
+      <c r="G1081" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 37
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6BC4D7-D90F-7047-96AE-19B9A5726E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58786A82-35A2-4E47-B71A-DB29336F379D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6334" uniqueCount="5335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6514" uniqueCount="5484">
   <si>
     <t>ID</t>
   </si>
@@ -16035,6 +16035,453 @@
   </si>
   <si>
     <t>The brake pedal / bàn đạp phanh</t>
+  </si>
+  <si>
+    <t>U37_01</t>
+  </si>
+  <si>
+    <t>Khu dân cư</t>
+  </si>
+  <si>
+    <t>Neighborhood</t>
+  </si>
+  <si>
+    <t>There are no burglars in the neighborhood</t>
+  </si>
+  <si>
+    <t>In the neighborhood / trong khu phố</t>
+  </si>
+  <si>
+    <t>U37_02</t>
+  </si>
+  <si>
+    <t>U37_03</t>
+  </si>
+  <si>
+    <t>U37_04</t>
+  </si>
+  <si>
+    <t>U37_05</t>
+  </si>
+  <si>
+    <t>U37_06</t>
+  </si>
+  <si>
+    <t>U37_07</t>
+  </si>
+  <si>
+    <t>U37_08</t>
+  </si>
+  <si>
+    <t>U37_09</t>
+  </si>
+  <si>
+    <t>U37_10</t>
+  </si>
+  <si>
+    <t>U37_11</t>
+  </si>
+  <si>
+    <t>U37_12</t>
+  </si>
+  <si>
+    <t>U37_13</t>
+  </si>
+  <si>
+    <t>U37_14</t>
+  </si>
+  <si>
+    <t>U37_15</t>
+  </si>
+  <si>
+    <t>U37_16</t>
+  </si>
+  <si>
+    <t>U37_17</t>
+  </si>
+  <si>
+    <t>U37_18</t>
+  </si>
+  <si>
+    <t>U37_19</t>
+  </si>
+  <si>
+    <t>U37_20</t>
+  </si>
+  <si>
+    <t>U37_21</t>
+  </si>
+  <si>
+    <t>U37_22</t>
+  </si>
+  <si>
+    <t>U37_23</t>
+  </si>
+  <si>
+    <t>U37_24</t>
+  </si>
+  <si>
+    <t>U37_25</t>
+  </si>
+  <si>
+    <t>U37_26</t>
+  </si>
+  <si>
+    <t>U37_27</t>
+  </si>
+  <si>
+    <t>U37_28</t>
+  </si>
+  <si>
+    <t>U37_29</t>
+  </si>
+  <si>
+    <t>U37_30</t>
+  </si>
+  <si>
+    <t>Đi lang thang</t>
+  </si>
+  <si>
+    <t>Wander</t>
+  </si>
+  <si>
+    <t>I enjoy wandering around the city center</t>
+  </si>
+  <si>
+    <t>wander around / đi lang thang xung quanh</t>
+  </si>
+  <si>
+    <t>Sân chơi</t>
+  </si>
+  <si>
+    <t>Playground</t>
+  </si>
+  <si>
+    <t>Students can play at the school playground</t>
+  </si>
+  <si>
+    <t>a school playground / sân trường</t>
+  </si>
+  <si>
+    <t>Nhịp</t>
+  </si>
+  <si>
+    <t>Pace</t>
+  </si>
+  <si>
+    <t>She is learning at a steady pace</t>
+  </si>
+  <si>
+    <t>at a steady pace / ở một nhịp độ ổn định</t>
+  </si>
+  <si>
+    <t>Người đi đường</t>
+  </si>
+  <si>
+    <t>Pedestrian</t>
+  </si>
+  <si>
+    <t>We can walk on the pedestrian crossing</t>
+  </si>
+  <si>
+    <t>a pedestrian crossing / vạch kẻ đường cho người đi bộ</t>
+  </si>
+  <si>
+    <t>Vỉa hè</t>
+  </si>
+  <si>
+    <t>Sidewalk</t>
+  </si>
+  <si>
+    <t>At night, the city has busy sidewalks</t>
+  </si>
+  <si>
+    <t>a busy sidewalk</t>
+  </si>
+  <si>
+    <t>Làn đường</t>
+  </si>
+  <si>
+    <t>Lane</t>
+  </si>
+  <si>
+    <t>We drove in the right traffic lane.</t>
+  </si>
+  <si>
+    <t>a traffic lane / làn đường giao thông</t>
+  </si>
+  <si>
+    <t>Giao thông</t>
+  </si>
+  <si>
+    <t>Traffic</t>
+  </si>
+  <si>
+    <t>I want to avoid the rush-hour traffic</t>
+  </si>
+  <si>
+    <t>rush-hour traffic / giao thông giờ cao điểm</t>
+  </si>
+  <si>
+    <t>Rạp chiếu</t>
+  </si>
+  <si>
+    <t>Theater</t>
+  </si>
+  <si>
+    <t>There is a movie theater around the corner</t>
+  </si>
+  <si>
+    <t>a movie theater</t>
+  </si>
+  <si>
+    <t>Cửa hàng sách</t>
+  </si>
+  <si>
+    <t>Bookstore</t>
+  </si>
+  <si>
+    <t>Nowadays, we buy from online bookstores.</t>
+  </si>
+  <si>
+    <t>An online bookstore / hiệu sách trực tuyến</t>
+  </si>
+  <si>
+    <t>Tạp hóa</t>
+  </si>
+  <si>
+    <t>Grocery</t>
+  </si>
+  <si>
+    <t>Our grocery bill is too high</t>
+  </si>
+  <si>
+    <t>The grocery bill</t>
+  </si>
+  <si>
+    <t>Ngõ</t>
+  </si>
+  <si>
+    <t>Alley</t>
+  </si>
+  <si>
+    <t>My car cannot fit in the narrow alley</t>
+  </si>
+  <si>
+    <t>A narrow alley</t>
+  </si>
+  <si>
+    <t>Tòa nhà</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>The mausoleum is a historic building</t>
+  </si>
+  <si>
+    <t>a historic building / công trình lịch sử</t>
+  </si>
+  <si>
+    <t>Xuống cấp</t>
+  </si>
+  <si>
+    <t>Run-down</t>
+  </si>
+  <si>
+    <t>We can fix this run-down building</t>
+  </si>
+  <si>
+    <t>a run-down building</t>
+  </si>
+  <si>
+    <t>Tượng trưng cho</t>
+  </si>
+  <si>
+    <t>Represent</t>
+  </si>
+  <si>
+    <t>Roses represent remance and love</t>
+  </si>
+  <si>
+    <t>represent somebody or something / tượng trưng cho ai đó hoặc cái gì đó</t>
+  </si>
+  <si>
+    <t>Tháp</t>
+  </si>
+  <si>
+    <t>Tower</t>
+  </si>
+  <si>
+    <t>The eiffel tower is in Paris, France</t>
+  </si>
+  <si>
+    <t>The eiffel tower</t>
+  </si>
+  <si>
+    <t>Giao thông vận tải</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>What is your means of transportation to work every day</t>
+  </si>
+  <si>
+    <t>means of transportation / phương tiện giao thông</t>
+  </si>
+  <si>
+    <t>Dễ tiếp cận</t>
+  </si>
+  <si>
+    <t>Accessible</t>
+  </si>
+  <si>
+    <t>The library is accessible to everyone</t>
+  </si>
+  <si>
+    <t>accessible to somebody / Ai đó có thể tiếp cận được</t>
+  </si>
+  <si>
+    <t>Cảnh sát</t>
+  </si>
+  <si>
+    <t>Police</t>
+  </si>
+  <si>
+    <t>There is a police car outside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a police car </t>
+  </si>
+  <si>
+    <t>Dắt đi tham quan</t>
+  </si>
+  <si>
+    <t>Show around</t>
+  </si>
+  <si>
+    <t>I can show you around town sometime</t>
+  </si>
+  <si>
+    <t>show somebody around town / dắt ai đi tham quan thị trấn</t>
+  </si>
+  <si>
+    <t>Tài sản</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>This painting is government property</t>
+  </si>
+  <si>
+    <t>government property / tài sản chính phủ</t>
+  </si>
+  <si>
+    <t>Đông đúc</t>
+  </si>
+  <si>
+    <t>Crowded</t>
+  </si>
+  <si>
+    <t>We avoid going to crowded areas on the weekend</t>
+  </si>
+  <si>
+    <t>crowded areas</t>
+  </si>
+  <si>
+    <t>Tiếng ồn</t>
+  </si>
+  <si>
+    <t>Noise</t>
+  </si>
+  <si>
+    <t>Children tend to make noises</t>
+  </si>
+  <si>
+    <t>make a noise</t>
+  </si>
+  <si>
+    <t>chuyển vào</t>
+  </si>
+  <si>
+    <t>Move in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The family moved in a new apartment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">move in an apartment </t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Let's meet at a central location</t>
+  </si>
+  <si>
+    <t>a central location</t>
+  </si>
+  <si>
+    <t>Chuỗi</t>
+  </si>
+  <si>
+    <t>Chain</t>
+  </si>
+  <si>
+    <t>A chain of events happened throughout tonight</t>
+  </si>
+  <si>
+    <t>a chain of events</t>
+  </si>
+  <si>
+    <t>Đa dạng</t>
+  </si>
+  <si>
+    <t>Diverse</t>
+  </si>
+  <si>
+    <t>Our country has a diverse culture</t>
+  </si>
+  <si>
+    <t>A diverse culture</t>
+  </si>
+  <si>
+    <t>Ngẫu nhiên</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>We met on such a random occasion</t>
+  </si>
+  <si>
+    <t>A random accasion / một dịp ngẫu nhiên</t>
+  </si>
+  <si>
+    <t>Dày đặc</t>
+  </si>
+  <si>
+    <t>Dense</t>
+  </si>
+  <si>
+    <t>She can't pass through the dense crowd</t>
+  </si>
+  <si>
+    <t>a dense crowd</t>
+  </si>
+  <si>
+    <t>Dưới mặt đất</t>
+  </si>
+  <si>
+    <t>Underground</t>
+  </si>
+  <si>
+    <t>There is an underground basement here</t>
+  </si>
+  <si>
+    <t>an underground basement / một tầng hầm dưới mặt đất</t>
   </si>
 </sst>
 </file>
@@ -16407,10 +16854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1081"/>
+  <dimension ref="A1:G1111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1058" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1082" sqref="C1082"/>
+    <sheetView tabSelected="1" topLeftCell="C1083" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G1111" sqref="G1111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16418,7 +16865,7 @@
     <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
@@ -40981,6 +41428,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="1082" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1082" s="2" t="s">
+        <v>5335</v>
+      </c>
+      <c r="B1082" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1082" s="2" t="s">
+        <v>5336</v>
+      </c>
+      <c r="D1082" s="2" t="s">
+        <v>5337</v>
+      </c>
+      <c r="E1082" s="2" t="s">
+        <v>5338</v>
+      </c>
+      <c r="F1082" s="2" t="s">
+        <v>5339</v>
+      </c>
+      <c r="G1082" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1083" s="2" t="s">
+        <v>5340</v>
+      </c>
+      <c r="B1083" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1083" s="2" t="s">
+        <v>5369</v>
+      </c>
+      <c r="D1083" s="2" t="s">
+        <v>5370</v>
+      </c>
+      <c r="E1083" s="2" t="s">
+        <v>5371</v>
+      </c>
+      <c r="F1083" s="2" t="s">
+        <v>5372</v>
+      </c>
+      <c r="G1083" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1084" s="2" t="s">
+        <v>5341</v>
+      </c>
+      <c r="B1084" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1084" s="2" t="s">
+        <v>5373</v>
+      </c>
+      <c r="D1084" s="2" t="s">
+        <v>5374</v>
+      </c>
+      <c r="E1084" s="2" t="s">
+        <v>5375</v>
+      </c>
+      <c r="F1084" s="2" t="s">
+        <v>5376</v>
+      </c>
+      <c r="G1084" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1085" s="2" t="s">
+        <v>5342</v>
+      </c>
+      <c r="B1085" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1085" s="2" t="s">
+        <v>5377</v>
+      </c>
+      <c r="D1085" s="2" t="s">
+        <v>5378</v>
+      </c>
+      <c r="E1085" s="2" t="s">
+        <v>5379</v>
+      </c>
+      <c r="F1085" s="2" t="s">
+        <v>5380</v>
+      </c>
+      <c r="G1085" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1086" s="2" t="s">
+        <v>5343</v>
+      </c>
+      <c r="B1086" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1086" s="2" t="s">
+        <v>5381</v>
+      </c>
+      <c r="D1086" s="2" t="s">
+        <v>5382</v>
+      </c>
+      <c r="E1086" s="2" t="s">
+        <v>5383</v>
+      </c>
+      <c r="F1086" s="2" t="s">
+        <v>5384</v>
+      </c>
+      <c r="G1086" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1087" s="2" t="s">
+        <v>5344</v>
+      </c>
+      <c r="B1087" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1087" s="2" t="s">
+        <v>5385</v>
+      </c>
+      <c r="D1087" s="2" t="s">
+        <v>5386</v>
+      </c>
+      <c r="E1087" s="2" t="s">
+        <v>5387</v>
+      </c>
+      <c r="F1087" s="2" t="s">
+        <v>5388</v>
+      </c>
+      <c r="G1087" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1088" s="2" t="s">
+        <v>5345</v>
+      </c>
+      <c r="B1088" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1088" s="2" t="s">
+        <v>5389</v>
+      </c>
+      <c r="D1088" s="2" t="s">
+        <v>5390</v>
+      </c>
+      <c r="E1088" s="2" t="s">
+        <v>5391</v>
+      </c>
+      <c r="F1088" s="2" t="s">
+        <v>5392</v>
+      </c>
+      <c r="G1088" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1089" s="2" t="s">
+        <v>5346</v>
+      </c>
+      <c r="B1089" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1089" s="2" t="s">
+        <v>5393</v>
+      </c>
+      <c r="D1089" s="2" t="s">
+        <v>5394</v>
+      </c>
+      <c r="E1089" s="2" t="s">
+        <v>5395</v>
+      </c>
+      <c r="F1089" s="2" t="s">
+        <v>5396</v>
+      </c>
+      <c r="G1089" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1090" s="2" t="s">
+        <v>5347</v>
+      </c>
+      <c r="B1090" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1090" s="2" t="s">
+        <v>5397</v>
+      </c>
+      <c r="D1090" s="2" t="s">
+        <v>5398</v>
+      </c>
+      <c r="E1090" s="2" t="s">
+        <v>5399</v>
+      </c>
+      <c r="F1090" s="2" t="s">
+        <v>5400</v>
+      </c>
+      <c r="G1090" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1091" s="2" t="s">
+        <v>5348</v>
+      </c>
+      <c r="B1091" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1091" s="2" t="s">
+        <v>5401</v>
+      </c>
+      <c r="D1091" s="2" t="s">
+        <v>5402</v>
+      </c>
+      <c r="E1091" s="2" t="s">
+        <v>5403</v>
+      </c>
+      <c r="F1091" s="2" t="s">
+        <v>5404</v>
+      </c>
+      <c r="G1091" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1092" s="2" t="s">
+        <v>5349</v>
+      </c>
+      <c r="B1092" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1092" s="2" t="s">
+        <v>5405</v>
+      </c>
+      <c r="D1092" s="2" t="s">
+        <v>5406</v>
+      </c>
+      <c r="E1092" s="2" t="s">
+        <v>5407</v>
+      </c>
+      <c r="F1092" s="2" t="s">
+        <v>5408</v>
+      </c>
+      <c r="G1092" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1093" s="2" t="s">
+        <v>5350</v>
+      </c>
+      <c r="B1093" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1093" s="2" t="s">
+        <v>5409</v>
+      </c>
+      <c r="D1093" s="2" t="s">
+        <v>5410</v>
+      </c>
+      <c r="E1093" s="2" t="s">
+        <v>5411</v>
+      </c>
+      <c r="F1093" s="2" t="s">
+        <v>5412</v>
+      </c>
+      <c r="G1093" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1094" s="2" t="s">
+        <v>5351</v>
+      </c>
+      <c r="B1094" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1094" s="2" t="s">
+        <v>5413</v>
+      </c>
+      <c r="D1094" s="2" t="s">
+        <v>5414</v>
+      </c>
+      <c r="E1094" s="2" t="s">
+        <v>5415</v>
+      </c>
+      <c r="F1094" s="2" t="s">
+        <v>5416</v>
+      </c>
+      <c r="G1094" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1095" s="2" t="s">
+        <v>5352</v>
+      </c>
+      <c r="B1095" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1095" s="2" t="s">
+        <v>5417</v>
+      </c>
+      <c r="D1095" s="2" t="s">
+        <v>5418</v>
+      </c>
+      <c r="E1095" s="2" t="s">
+        <v>5419</v>
+      </c>
+      <c r="F1095" s="2" t="s">
+        <v>5420</v>
+      </c>
+      <c r="G1095" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1096" s="2" t="s">
+        <v>5353</v>
+      </c>
+      <c r="B1096" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1096" s="2" t="s">
+        <v>5421</v>
+      </c>
+      <c r="D1096" s="2" t="s">
+        <v>5422</v>
+      </c>
+      <c r="E1096" s="2" t="s">
+        <v>5423</v>
+      </c>
+      <c r="F1096" s="2" t="s">
+        <v>5424</v>
+      </c>
+      <c r="G1096" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1097" s="2" t="s">
+        <v>5354</v>
+      </c>
+      <c r="B1097" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1097" s="2" t="s">
+        <v>5425</v>
+      </c>
+      <c r="D1097" s="2" t="s">
+        <v>5426</v>
+      </c>
+      <c r="E1097" s="2" t="s">
+        <v>5427</v>
+      </c>
+      <c r="F1097" s="2" t="s">
+        <v>5428</v>
+      </c>
+      <c r="G1097" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1098" s="2" t="s">
+        <v>5355</v>
+      </c>
+      <c r="B1098" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1098" s="2" t="s">
+        <v>5429</v>
+      </c>
+      <c r="D1098" s="2" t="s">
+        <v>5430</v>
+      </c>
+      <c r="E1098" s="2" t="s">
+        <v>5431</v>
+      </c>
+      <c r="F1098" s="2" t="s">
+        <v>5432</v>
+      </c>
+      <c r="G1098" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1099" s="2" t="s">
+        <v>5356</v>
+      </c>
+      <c r="B1099" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1099" s="2" t="s">
+        <v>5433</v>
+      </c>
+      <c r="D1099" s="2" t="s">
+        <v>5434</v>
+      </c>
+      <c r="E1099" s="2" t="s">
+        <v>5435</v>
+      </c>
+      <c r="F1099" s="2" t="s">
+        <v>5436</v>
+      </c>
+      <c r="G1099" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1100" s="2" t="s">
+        <v>5357</v>
+      </c>
+      <c r="B1100" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1100" s="2" t="s">
+        <v>5437</v>
+      </c>
+      <c r="D1100" s="2" t="s">
+        <v>5438</v>
+      </c>
+      <c r="E1100" s="2" t="s">
+        <v>5439</v>
+      </c>
+      <c r="F1100" s="2" t="s">
+        <v>5440</v>
+      </c>
+      <c r="G1100" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1101" s="2" t="s">
+        <v>5358</v>
+      </c>
+      <c r="B1101" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1101" s="2" t="s">
+        <v>5441</v>
+      </c>
+      <c r="D1101" s="2" t="s">
+        <v>5442</v>
+      </c>
+      <c r="E1101" s="2" t="s">
+        <v>5443</v>
+      </c>
+      <c r="F1101" s="2" t="s">
+        <v>5444</v>
+      </c>
+      <c r="G1101" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1102" s="2" t="s">
+        <v>5359</v>
+      </c>
+      <c r="B1102" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1102" s="2" t="s">
+        <v>5445</v>
+      </c>
+      <c r="D1102" s="2" t="s">
+        <v>5446</v>
+      </c>
+      <c r="E1102" s="2" t="s">
+        <v>5447</v>
+      </c>
+      <c r="F1102" s="2" t="s">
+        <v>5448</v>
+      </c>
+      <c r="G1102" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1103" s="2" t="s">
+        <v>5360</v>
+      </c>
+      <c r="B1103" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1103" s="2" t="s">
+        <v>5449</v>
+      </c>
+      <c r="D1103" s="2" t="s">
+        <v>5450</v>
+      </c>
+      <c r="E1103" s="2" t="s">
+        <v>5451</v>
+      </c>
+      <c r="F1103" s="2" t="s">
+        <v>5452</v>
+      </c>
+      <c r="G1103" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1104" s="2" t="s">
+        <v>5361</v>
+      </c>
+      <c r="B1104" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1104" s="2" t="s">
+        <v>5453</v>
+      </c>
+      <c r="D1104" s="2" t="s">
+        <v>5454</v>
+      </c>
+      <c r="E1104" s="2" t="s">
+        <v>5455</v>
+      </c>
+      <c r="F1104" s="2" t="s">
+        <v>5456</v>
+      </c>
+      <c r="G1104" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1105" s="2" t="s">
+        <v>5362</v>
+      </c>
+      <c r="B1105" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1105" s="2" t="s">
+        <v>5457</v>
+      </c>
+      <c r="D1105" s="2" t="s">
+        <v>5458</v>
+      </c>
+      <c r="E1105" s="2" t="s">
+        <v>5459</v>
+      </c>
+      <c r="F1105" s="2" t="s">
+        <v>5460</v>
+      </c>
+      <c r="G1105" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1106" s="2" t="s">
+        <v>5363</v>
+      </c>
+      <c r="B1106" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1106" s="2" t="s">
+        <v>3944</v>
+      </c>
+      <c r="D1106" s="2" t="s">
+        <v>5461</v>
+      </c>
+      <c r="E1106" s="2" t="s">
+        <v>5462</v>
+      </c>
+      <c r="F1106" s="2" t="s">
+        <v>5463</v>
+      </c>
+      <c r="G1106" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1107" s="2" t="s">
+        <v>5364</v>
+      </c>
+      <c r="B1107" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1107" s="2" t="s">
+        <v>5464</v>
+      </c>
+      <c r="D1107" s="2" t="s">
+        <v>5465</v>
+      </c>
+      <c r="E1107" s="2" t="s">
+        <v>5466</v>
+      </c>
+      <c r="F1107" s="2" t="s">
+        <v>5467</v>
+      </c>
+      <c r="G1107" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1108" s="2" t="s">
+        <v>5365</v>
+      </c>
+      <c r="B1108" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1108" s="2" t="s">
+        <v>5468</v>
+      </c>
+      <c r="D1108" s="2" t="s">
+        <v>5469</v>
+      </c>
+      <c r="E1108" s="2" t="s">
+        <v>5470</v>
+      </c>
+      <c r="F1108" s="2" t="s">
+        <v>5471</v>
+      </c>
+      <c r="G1108" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1109" s="2" t="s">
+        <v>5366</v>
+      </c>
+      <c r="B1109" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1109" s="2" t="s">
+        <v>5472</v>
+      </c>
+      <c r="D1109" s="2" t="s">
+        <v>5473</v>
+      </c>
+      <c r="E1109" s="2" t="s">
+        <v>5474</v>
+      </c>
+      <c r="F1109" s="2" t="s">
+        <v>5475</v>
+      </c>
+      <c r="G1109" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1110" s="2" t="s">
+        <v>5367</v>
+      </c>
+      <c r="B1110" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1110" s="2" t="s">
+        <v>5476</v>
+      </c>
+      <c r="D1110" s="2" t="s">
+        <v>5477</v>
+      </c>
+      <c r="E1110" s="2" t="s">
+        <v>5478</v>
+      </c>
+      <c r="F1110" s="2" t="s">
+        <v>5479</v>
+      </c>
+      <c r="G1110" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1111" s="2" t="s">
+        <v>5368</v>
+      </c>
+      <c r="B1111" s="2">
+        <v>37</v>
+      </c>
+      <c r="C1111" s="2" t="s">
+        <v>5480</v>
+      </c>
+      <c r="D1111" s="2" t="s">
+        <v>5481</v>
+      </c>
+      <c r="E1111" s="2" t="s">
+        <v>5482</v>
+      </c>
+      <c r="F1111" s="2" t="s">
+        <v>5483</v>
+      </c>
+      <c r="G1111" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 39
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenlephong/Documents/Projects/english-app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EA561F-0913-9548-8294-3030050F38EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F180C8CC-0AC5-AE45-8608-47A57407ABF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="880" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6694" uniqueCount="5633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6874" uniqueCount="5782">
   <si>
     <t>ID</t>
   </si>
@@ -16929,6 +16929,453 @@
   </si>
   <si>
     <t>Throw away</t>
+  </si>
+  <si>
+    <t>U39_01</t>
+  </si>
+  <si>
+    <t>U39_02</t>
+  </si>
+  <si>
+    <t>U39_03</t>
+  </si>
+  <si>
+    <t>U39_04</t>
+  </si>
+  <si>
+    <t>U39_05</t>
+  </si>
+  <si>
+    <t>U39_06</t>
+  </si>
+  <si>
+    <t>U39_07</t>
+  </si>
+  <si>
+    <t>U39_08</t>
+  </si>
+  <si>
+    <t>U39_09</t>
+  </si>
+  <si>
+    <t>U39_10</t>
+  </si>
+  <si>
+    <t>U39_11</t>
+  </si>
+  <si>
+    <t>U39_12</t>
+  </si>
+  <si>
+    <t>U39_13</t>
+  </si>
+  <si>
+    <t>U39_14</t>
+  </si>
+  <si>
+    <t>U39_15</t>
+  </si>
+  <si>
+    <t>U39_16</t>
+  </si>
+  <si>
+    <t>U39_17</t>
+  </si>
+  <si>
+    <t>U39_18</t>
+  </si>
+  <si>
+    <t>U39_19</t>
+  </si>
+  <si>
+    <t>U39_20</t>
+  </si>
+  <si>
+    <t>U39_21</t>
+  </si>
+  <si>
+    <t>U39_22</t>
+  </si>
+  <si>
+    <t>U39_23</t>
+  </si>
+  <si>
+    <t>U39_24</t>
+  </si>
+  <si>
+    <t>U39_25</t>
+  </si>
+  <si>
+    <t>U39_26</t>
+  </si>
+  <si>
+    <t>U39_27</t>
+  </si>
+  <si>
+    <t>U39_28</t>
+  </si>
+  <si>
+    <t>U39_29</t>
+  </si>
+  <si>
+    <t>U39_30</t>
+  </si>
+  <si>
+    <t>Đáng yêu</t>
+  </si>
+  <si>
+    <t>Lovely</t>
+  </si>
+  <si>
+    <t>The singer has a lovely voice!</t>
+  </si>
+  <si>
+    <t>a lovely voice</t>
+  </si>
+  <si>
+    <t>Rực rỡ, sôi động</t>
+  </si>
+  <si>
+    <t>Vibrant</t>
+  </si>
+  <si>
+    <t>HCM City is a vibrant city in VN</t>
+  </si>
+  <si>
+    <t>a vibrant city / một thành phố sôi động</t>
+  </si>
+  <si>
+    <t>Hạt</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Plant a seed to grow a tree</t>
+  </si>
+  <si>
+    <t>plant a seed / gieo hạt giống</t>
+  </si>
+  <si>
+    <t>Đất</t>
+  </si>
+  <si>
+    <t>Soil</t>
+  </si>
+  <si>
+    <t>Flowers need fertile soil to grow well</t>
+  </si>
+  <si>
+    <t>fertile soil / đất đai màu mỡ</t>
+  </si>
+  <si>
+    <t>Tài nguyên</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Water is a natural resource to use</t>
+  </si>
+  <si>
+    <t>natural resource / tài nguyên thiên nhiên</t>
+  </si>
+  <si>
+    <t>Môi trường</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Animals need to live in a natural environment</t>
+  </si>
+  <si>
+    <t>a natural environment</t>
+  </si>
+  <si>
+    <t>Không khí</t>
+  </si>
+  <si>
+    <t>Atmosphere</t>
+  </si>
+  <si>
+    <t>The atmosphere of the room makes it hard to breathe</t>
+  </si>
+  <si>
+    <t>the atmosphere of / bầu không khí của</t>
+  </si>
+  <si>
+    <t>Cánh đồng</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>a field of something / cánh đồng trồng cái gì đó</t>
+  </si>
+  <si>
+    <t>Dalat has many fields of strawberries (dâu)</t>
+  </si>
+  <si>
+    <t>Nhánh, cành</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>There is a bird on the tree branch</t>
+  </si>
+  <si>
+    <t>a tree branch / cành cây</t>
+  </si>
+  <si>
+    <t>Thu hoạch</t>
+  </si>
+  <si>
+    <t>Harvest</t>
+  </si>
+  <si>
+    <t>It's time to harvest the crops</t>
+  </si>
+  <si>
+    <t>harvest the crops / thu hoạch cây trồng</t>
+  </si>
+  <si>
+    <t>Nông dân</t>
+  </si>
+  <si>
+    <t>Farmer</t>
+  </si>
+  <si>
+    <t>Local farmers in VN are hard workers</t>
+  </si>
+  <si>
+    <t>a local farmer / nông dân địa phương</t>
+  </si>
+  <si>
+    <t>Vùng thôn quê</t>
+  </si>
+  <si>
+    <t>Countryside</t>
+  </si>
+  <si>
+    <t>My grandparents live in the countryside</t>
+  </si>
+  <si>
+    <t>in the countryside / ở vùng nông thôn</t>
+  </si>
+  <si>
+    <t>Bùn</t>
+  </si>
+  <si>
+    <t>Mud</t>
+  </si>
+  <si>
+    <t>After playing, the boys are covered in mud</t>
+  </si>
+  <si>
+    <t>covered in mud / dính đầy bùn</t>
+  </si>
+  <si>
+    <t>Gia súc</t>
+  </si>
+  <si>
+    <t>Livestock</t>
+  </si>
+  <si>
+    <t>domestic livestock / gia súc chăn nuôi</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Herds of cattle are found in the countryside</t>
+  </si>
+  <si>
+    <t>a herd of cattle / đàn gia súc</t>
+  </si>
+  <si>
+    <t>Trâu</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Cows (Bò) are considered domestic livestock.</t>
+  </si>
+  <si>
+    <t>Buffalo meat is hard to chew on (rất dai)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffalo meat </t>
+  </si>
+  <si>
+    <t>Đi tới</t>
+  </si>
+  <si>
+    <t>Head to</t>
+  </si>
+  <si>
+    <t>I will head to the bank tomorrow.</t>
+  </si>
+  <si>
+    <t>Head to somewhere</t>
+  </si>
+  <si>
+    <t>Đồi</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>The house is on a hill</t>
+  </si>
+  <si>
+    <t>on a hill</t>
+  </si>
+  <si>
+    <t>Thung lũng</t>
+  </si>
+  <si>
+    <t>Valley</t>
+  </si>
+  <si>
+    <t>You can find many types of flowers in the valley.</t>
+  </si>
+  <si>
+    <t>in the valley</t>
+  </si>
+  <si>
+    <t>Dòng nước</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>The waterfall is a strong stream of water</t>
+  </si>
+  <si>
+    <t>stream of water / dòng nước</t>
+  </si>
+  <si>
+    <t>Thuộc nông thôn</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>Rural areas have fewer shopping malls</t>
+  </si>
+  <si>
+    <t>a rural area</t>
+  </si>
+  <si>
+    <t>Lối nhỏ, con đường</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Keep following the path until you reach the destination</t>
+  </si>
+  <si>
+    <t>follow the path / lần theo con đường</t>
+  </si>
+  <si>
+    <t>Nhà ở vùng thôn quê</t>
+  </si>
+  <si>
+    <t>Cottage</t>
+  </si>
+  <si>
+    <t>She lives a peaceful life in a cozy cottage</t>
+  </si>
+  <si>
+    <t>a cozy cottage / một ngôi nhà nhỏ ấm cúng ở miền quê</t>
+  </si>
+  <si>
+    <t>Rừng</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>There are not many dense forests left.</t>
+  </si>
+  <si>
+    <t>a dense forest / khu rừng rậm rạp</t>
+  </si>
+  <si>
+    <t>Vùng, khu vực</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>You cannot enter the danger zone</t>
+  </si>
+  <si>
+    <t>a danger zone</t>
+  </si>
+  <si>
+    <t>Thuộc nhiệt đới</t>
+  </si>
+  <si>
+    <t>Tropical</t>
+  </si>
+  <si>
+    <t>The mekong delta has many tropical fish</t>
+  </si>
+  <si>
+    <t>a tropical fish / loài cá vùng nhiệt đới</t>
+  </si>
+  <si>
+    <t>Nông nghiệp</t>
+  </si>
+  <si>
+    <t>Our country's strength is sustainable agriculture</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>sustainable agriculture/ nông nghiệp bền vững</t>
+  </si>
+  <si>
+    <t>Bình yên</t>
+  </si>
+  <si>
+    <t>Peaceful</t>
+  </si>
+  <si>
+    <t>The garden is quiet and peaceful</t>
+  </si>
+  <si>
+    <t>quiet and peaceful / yên tĩnh và bình yên</t>
+  </si>
+  <si>
+    <t>Kỳ Nghĩ</t>
+  </si>
+  <si>
+    <t>Vacation</t>
+  </si>
+  <si>
+    <t>I need to take a vacation to relax</t>
+  </si>
+  <si>
+    <t>take a vacation / đi nghỉ mát</t>
+  </si>
+  <si>
+    <t>Côn trùng</t>
+  </si>
+  <si>
+    <t>Insect</t>
+  </si>
+  <si>
+    <t>Ants are an insect species</t>
+  </si>
+  <si>
+    <t>insect species / loài côn trùng</t>
   </si>
 </sst>
 </file>
@@ -17294,10 +17741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1141"/>
+  <dimension ref="A1:G1171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1119" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1141" sqref="E1141"/>
+    <sheetView tabSelected="1" topLeftCell="A1161" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1172" sqref="C1172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -43095,6 +43542,696 @@
         <v>577</v>
       </c>
     </row>
+    <row r="1142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1142" s="1" t="s">
+        <v>5633</v>
+      </c>
+      <c r="B1142" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1142" s="1" t="s">
+        <v>5663</v>
+      </c>
+      <c r="D1142" s="1" t="s">
+        <v>5664</v>
+      </c>
+      <c r="E1142" s="1" t="s">
+        <v>5665</v>
+      </c>
+      <c r="F1142" s="1" t="s">
+        <v>5666</v>
+      </c>
+      <c r="G1142" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1143" s="1" t="s">
+        <v>5634</v>
+      </c>
+      <c r="B1143" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1143" s="1" t="s">
+        <v>5667</v>
+      </c>
+      <c r="D1143" s="1" t="s">
+        <v>5668</v>
+      </c>
+      <c r="E1143" s="1" t="s">
+        <v>5669</v>
+      </c>
+      <c r="F1143" s="1" t="s">
+        <v>5670</v>
+      </c>
+      <c r="G1143" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1144" s="1" t="s">
+        <v>5635</v>
+      </c>
+      <c r="B1144" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1144" s="1" t="s">
+        <v>5671</v>
+      </c>
+      <c r="D1144" s="1" t="s">
+        <v>5672</v>
+      </c>
+      <c r="E1144" s="1" t="s">
+        <v>5673</v>
+      </c>
+      <c r="F1144" s="1" t="s">
+        <v>5674</v>
+      </c>
+      <c r="G1144" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1145" s="1" t="s">
+        <v>5636</v>
+      </c>
+      <c r="B1145" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1145" s="1" t="s">
+        <v>5675</v>
+      </c>
+      <c r="D1145" s="1" t="s">
+        <v>5676</v>
+      </c>
+      <c r="E1145" s="1" t="s">
+        <v>5677</v>
+      </c>
+      <c r="F1145" s="1" t="s">
+        <v>5678</v>
+      </c>
+      <c r="G1145" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1146" s="1" t="s">
+        <v>5637</v>
+      </c>
+      <c r="B1146" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1146" s="1" t="s">
+        <v>5679</v>
+      </c>
+      <c r="D1146" s="1" t="s">
+        <v>5680</v>
+      </c>
+      <c r="E1146" s="1" t="s">
+        <v>5681</v>
+      </c>
+      <c r="F1146" s="1" t="s">
+        <v>5682</v>
+      </c>
+      <c r="G1146" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1147" s="1" t="s">
+        <v>5638</v>
+      </c>
+      <c r="B1147" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1147" s="1" t="s">
+        <v>5683</v>
+      </c>
+      <c r="D1147" s="1" t="s">
+        <v>5684</v>
+      </c>
+      <c r="E1147" s="1" t="s">
+        <v>5685</v>
+      </c>
+      <c r="F1147" s="1" t="s">
+        <v>5686</v>
+      </c>
+      <c r="G1147" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1148" s="1" t="s">
+        <v>5639</v>
+      </c>
+      <c r="B1148" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1148" s="1" t="s">
+        <v>5687</v>
+      </c>
+      <c r="D1148" s="1" t="s">
+        <v>5688</v>
+      </c>
+      <c r="E1148" s="1" t="s">
+        <v>5689</v>
+      </c>
+      <c r="F1148" s="1" t="s">
+        <v>5690</v>
+      </c>
+      <c r="G1148" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1149" s="1" t="s">
+        <v>5640</v>
+      </c>
+      <c r="B1149" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1149" s="1" t="s">
+        <v>5691</v>
+      </c>
+      <c r="D1149" s="1" t="s">
+        <v>5692</v>
+      </c>
+      <c r="E1149" s="1" t="s">
+        <v>5694</v>
+      </c>
+      <c r="F1149" s="1" t="s">
+        <v>5693</v>
+      </c>
+      <c r="G1149" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1150" s="1" t="s">
+        <v>5641</v>
+      </c>
+      <c r="B1150" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1150" s="1" t="s">
+        <v>5695</v>
+      </c>
+      <c r="D1150" s="1" t="s">
+        <v>5696</v>
+      </c>
+      <c r="E1150" s="1" t="s">
+        <v>5697</v>
+      </c>
+      <c r="F1150" s="1" t="s">
+        <v>5698</v>
+      </c>
+      <c r="G1150" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1151" s="1" t="s">
+        <v>5642</v>
+      </c>
+      <c r="B1151" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1151" s="1" t="s">
+        <v>5699</v>
+      </c>
+      <c r="D1151" s="1" t="s">
+        <v>5700</v>
+      </c>
+      <c r="E1151" s="1" t="s">
+        <v>5701</v>
+      </c>
+      <c r="F1151" s="1" t="s">
+        <v>5702</v>
+      </c>
+      <c r="G1151" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1152" s="1" t="s">
+        <v>5643</v>
+      </c>
+      <c r="B1152" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1152" s="1" t="s">
+        <v>5703</v>
+      </c>
+      <c r="D1152" s="1" t="s">
+        <v>5704</v>
+      </c>
+      <c r="E1152" s="1" t="s">
+        <v>5705</v>
+      </c>
+      <c r="F1152" s="1" t="s">
+        <v>5706</v>
+      </c>
+      <c r="G1152" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1153" s="1" t="s">
+        <v>5644</v>
+      </c>
+      <c r="B1153" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1153" s="1" t="s">
+        <v>5707</v>
+      </c>
+      <c r="D1153" s="1" t="s">
+        <v>5708</v>
+      </c>
+      <c r="E1153" s="1" t="s">
+        <v>5709</v>
+      </c>
+      <c r="F1153" s="1" t="s">
+        <v>5710</v>
+      </c>
+      <c r="G1153" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1154" s="1" t="s">
+        <v>5645</v>
+      </c>
+      <c r="B1154" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1154" s="1" t="s">
+        <v>5711</v>
+      </c>
+      <c r="D1154" s="1" t="s">
+        <v>5712</v>
+      </c>
+      <c r="E1154" s="1" t="s">
+        <v>5713</v>
+      </c>
+      <c r="F1154" s="1" t="s">
+        <v>5714</v>
+      </c>
+      <c r="G1154" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1155" s="1" t="s">
+        <v>5646</v>
+      </c>
+      <c r="B1155" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1155" s="1" t="s">
+        <v>5715</v>
+      </c>
+      <c r="D1155" s="1" t="s">
+        <v>5716</v>
+      </c>
+      <c r="E1155" s="1" t="s">
+        <v>5723</v>
+      </c>
+      <c r="F1155" s="1" t="s">
+        <v>5717</v>
+      </c>
+      <c r="G1155" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1156" s="1" t="s">
+        <v>5647</v>
+      </c>
+      <c r="B1156" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1156" s="1" t="s">
+        <v>5715</v>
+      </c>
+      <c r="D1156" s="1" t="s">
+        <v>5718</v>
+      </c>
+      <c r="E1156" s="1" t="s">
+        <v>5719</v>
+      </c>
+      <c r="F1156" s="1" t="s">
+        <v>5720</v>
+      </c>
+      <c r="G1156" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1157" s="1" t="s">
+        <v>5648</v>
+      </c>
+      <c r="B1157" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1157" s="1" t="s">
+        <v>5721</v>
+      </c>
+      <c r="D1157" s="1" t="s">
+        <v>5722</v>
+      </c>
+      <c r="E1157" s="1" t="s">
+        <v>5724</v>
+      </c>
+      <c r="F1157" s="1" t="s">
+        <v>5725</v>
+      </c>
+      <c r="G1157" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1158" s="1" t="s">
+        <v>5649</v>
+      </c>
+      <c r="B1158" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1158" s="1" t="s">
+        <v>5726</v>
+      </c>
+      <c r="D1158" s="1" t="s">
+        <v>5727</v>
+      </c>
+      <c r="E1158" s="1" t="s">
+        <v>5728</v>
+      </c>
+      <c r="F1158" s="1" t="s">
+        <v>5729</v>
+      </c>
+      <c r="G1158" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1159" s="1" t="s">
+        <v>5650</v>
+      </c>
+      <c r="B1159" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1159" s="1" t="s">
+        <v>5730</v>
+      </c>
+      <c r="D1159" s="1" t="s">
+        <v>5731</v>
+      </c>
+      <c r="E1159" s="1" t="s">
+        <v>5732</v>
+      </c>
+      <c r="F1159" s="1" t="s">
+        <v>5733</v>
+      </c>
+      <c r="G1159" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1160" s="1" t="s">
+        <v>5651</v>
+      </c>
+      <c r="B1160" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1160" s="1" t="s">
+        <v>5734</v>
+      </c>
+      <c r="D1160" s="1" t="s">
+        <v>5735</v>
+      </c>
+      <c r="E1160" s="1" t="s">
+        <v>5736</v>
+      </c>
+      <c r="F1160" s="1" t="s">
+        <v>5737</v>
+      </c>
+      <c r="G1160" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1161" s="1" t="s">
+        <v>5652</v>
+      </c>
+      <c r="B1161" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1161" s="1" t="s">
+        <v>5738</v>
+      </c>
+      <c r="D1161" s="1" t="s">
+        <v>5739</v>
+      </c>
+      <c r="E1161" s="1" t="s">
+        <v>5740</v>
+      </c>
+      <c r="F1161" s="1" t="s">
+        <v>5741</v>
+      </c>
+      <c r="G1161" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1162" s="1" t="s">
+        <v>5653</v>
+      </c>
+      <c r="B1162" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1162" s="1" t="s">
+        <v>5742</v>
+      </c>
+      <c r="D1162" s="1" t="s">
+        <v>5743</v>
+      </c>
+      <c r="E1162" s="1" t="s">
+        <v>5744</v>
+      </c>
+      <c r="F1162" s="1" t="s">
+        <v>5745</v>
+      </c>
+      <c r="G1162" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1163" s="1" t="s">
+        <v>5654</v>
+      </c>
+      <c r="B1163" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1163" s="1" t="s">
+        <v>5746</v>
+      </c>
+      <c r="D1163" s="1" t="s">
+        <v>5747</v>
+      </c>
+      <c r="E1163" s="1" t="s">
+        <v>5748</v>
+      </c>
+      <c r="F1163" s="1" t="s">
+        <v>5749</v>
+      </c>
+      <c r="G1163" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1164" s="1" t="s">
+        <v>5655</v>
+      </c>
+      <c r="B1164" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1164" s="1" t="s">
+        <v>5750</v>
+      </c>
+      <c r="D1164" s="1" t="s">
+        <v>5751</v>
+      </c>
+      <c r="E1164" s="1" t="s">
+        <v>5752</v>
+      </c>
+      <c r="F1164" s="1" t="s">
+        <v>5753</v>
+      </c>
+      <c r="G1164" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1165" s="1" t="s">
+        <v>5656</v>
+      </c>
+      <c r="B1165" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1165" s="1" t="s">
+        <v>5754</v>
+      </c>
+      <c r="D1165" s="1" t="s">
+        <v>5755</v>
+      </c>
+      <c r="E1165" s="1" t="s">
+        <v>5756</v>
+      </c>
+      <c r="F1165" s="1" t="s">
+        <v>5757</v>
+      </c>
+      <c r="G1165" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1166" s="1" t="s">
+        <v>5657</v>
+      </c>
+      <c r="B1166" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1166" s="1" t="s">
+        <v>5758</v>
+      </c>
+      <c r="D1166" s="1" t="s">
+        <v>5759</v>
+      </c>
+      <c r="E1166" s="1" t="s">
+        <v>5760</v>
+      </c>
+      <c r="F1166" s="1" t="s">
+        <v>5761</v>
+      </c>
+      <c r="G1166" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1167" s="1" t="s">
+        <v>5658</v>
+      </c>
+      <c r="B1167" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1167" s="1" t="s">
+        <v>5762</v>
+      </c>
+      <c r="D1167" s="1" t="s">
+        <v>5763</v>
+      </c>
+      <c r="E1167" s="1" t="s">
+        <v>5764</v>
+      </c>
+      <c r="F1167" s="1" t="s">
+        <v>5765</v>
+      </c>
+      <c r="G1167" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1168" s="1" t="s">
+        <v>5659</v>
+      </c>
+      <c r="B1168" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1168" s="1" t="s">
+        <v>5766</v>
+      </c>
+      <c r="D1168" s="1" t="s">
+        <v>5768</v>
+      </c>
+      <c r="E1168" s="1" t="s">
+        <v>5767</v>
+      </c>
+      <c r="F1168" s="1" t="s">
+        <v>5769</v>
+      </c>
+      <c r="G1168" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1169" s="1" t="s">
+        <v>5660</v>
+      </c>
+      <c r="B1169" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1169" s="1" t="s">
+        <v>5770</v>
+      </c>
+      <c r="D1169" s="1" t="s">
+        <v>5771</v>
+      </c>
+      <c r="E1169" s="1" t="s">
+        <v>5772</v>
+      </c>
+      <c r="F1169" s="1" t="s">
+        <v>5773</v>
+      </c>
+      <c r="G1169" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1170" s="1" t="s">
+        <v>5661</v>
+      </c>
+      <c r="B1170" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1170" s="1" t="s">
+        <v>5774</v>
+      </c>
+      <c r="D1170" s="1" t="s">
+        <v>5775</v>
+      </c>
+      <c r="E1170" s="1" t="s">
+        <v>5776</v>
+      </c>
+      <c r="F1170" s="1" t="s">
+        <v>5777</v>
+      </c>
+      <c r="G1170" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1171" s="1" t="s">
+        <v>5662</v>
+      </c>
+      <c r="B1171" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1171" s="1" t="s">
+        <v>5778</v>
+      </c>
+      <c r="D1171" s="1" t="s">
+        <v>5779</v>
+      </c>
+      <c r="E1171" s="1" t="s">
+        <v>5780</v>
+      </c>
+      <c r="F1171" s="1" t="s">
+        <v>5781</v>
+      </c>
+      <c r="G1171" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 40
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F180C8CC-0AC5-AE45-8608-47A57407ABF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C291F4-CECA-E740-80FF-91DE0218B560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6874" uniqueCount="5782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7054" uniqueCount="5930">
   <si>
     <t>ID</t>
   </si>
@@ -17376,6 +17376,450 @@
   </si>
   <si>
     <t>insect species / loài côn trùng</t>
+  </si>
+  <si>
+    <t>U40_01</t>
+  </si>
+  <si>
+    <t>U40_02</t>
+  </si>
+  <si>
+    <t>U40_03</t>
+  </si>
+  <si>
+    <t>U40_04</t>
+  </si>
+  <si>
+    <t>U40_05</t>
+  </si>
+  <si>
+    <t>U40_06</t>
+  </si>
+  <si>
+    <t>U40_07</t>
+  </si>
+  <si>
+    <t>U40_08</t>
+  </si>
+  <si>
+    <t>U40_09</t>
+  </si>
+  <si>
+    <t>U40_10</t>
+  </si>
+  <si>
+    <t>U40_11</t>
+  </si>
+  <si>
+    <t>U40_12</t>
+  </si>
+  <si>
+    <t>U40_13</t>
+  </si>
+  <si>
+    <t>U40_14</t>
+  </si>
+  <si>
+    <t>U40_15</t>
+  </si>
+  <si>
+    <t>U40_16</t>
+  </si>
+  <si>
+    <t>U40_17</t>
+  </si>
+  <si>
+    <t>U40_18</t>
+  </si>
+  <si>
+    <t>U40_19</t>
+  </si>
+  <si>
+    <t>U40_20</t>
+  </si>
+  <si>
+    <t>U40_21</t>
+  </si>
+  <si>
+    <t>U40_22</t>
+  </si>
+  <si>
+    <t>U40_23</t>
+  </si>
+  <si>
+    <t>U40_24</t>
+  </si>
+  <si>
+    <t>U40_25</t>
+  </si>
+  <si>
+    <t>U40_26</t>
+  </si>
+  <si>
+    <t>U40_27</t>
+  </si>
+  <si>
+    <t>U40_28</t>
+  </si>
+  <si>
+    <t>U40_29</t>
+  </si>
+  <si>
+    <t>U40_30</t>
+  </si>
+  <si>
+    <t>Cánh</t>
+  </si>
+  <si>
+    <t>Wing</t>
+  </si>
+  <si>
+    <t>chicken wing</t>
+  </si>
+  <si>
+    <t>KFC is known for its (nổi tiếng với) chicken wings</t>
+  </si>
+  <si>
+    <t>Chạm trán, gặp phải</t>
+  </si>
+  <si>
+    <t>Encounter</t>
+  </si>
+  <si>
+    <t>The detective(thám tử) encountered a hard case</t>
+  </si>
+  <si>
+    <t>encounter somebody or something</t>
+  </si>
+  <si>
+    <t>Sư tử</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>The lion cub follows its mother to learn hunting</t>
+  </si>
+  <si>
+    <t>lion cub / sư tử con</t>
+  </si>
+  <si>
+    <t>Vương quốc</t>
+  </si>
+  <si>
+    <t>Kingdom</t>
+  </si>
+  <si>
+    <t>The kingdom of Portugal(Bồ Đào Nha) does not exist anymore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The kingdom of </t>
+  </si>
+  <si>
+    <t>Khổng lồ</t>
+  </si>
+  <si>
+    <t>Giant</t>
+  </si>
+  <si>
+    <t>The aquarium(thủy cung) has a giant squid</t>
+  </si>
+  <si>
+    <t>a giant squid / một con mực khổng lồ</t>
+  </si>
+  <si>
+    <t>Hoang dã, hoang dại</t>
+  </si>
+  <si>
+    <t>Wild</t>
+  </si>
+  <si>
+    <t>Wild animals are hard to tame (thuần hóa)</t>
+  </si>
+  <si>
+    <t>Wild animals / động vật hoang dã</t>
+  </si>
+  <si>
+    <t>Kẻ thù</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>She is my sworn enemy</t>
+  </si>
+  <si>
+    <t>Somebody's sworn enemy / kẻ thù không đội trời chung</t>
+  </si>
+  <si>
+    <t>Săn</t>
+  </si>
+  <si>
+    <t>Hunt</t>
+  </si>
+  <si>
+    <t>hunt for something</t>
+  </si>
+  <si>
+    <t>People in that tribe(bộ tộc) hunt for deer (hươu)</t>
+  </si>
+  <si>
+    <t>Lồng, chuồng</t>
+  </si>
+  <si>
+    <t>Cage</t>
+  </si>
+  <si>
+    <t>He doesn't want to keep the dog in a cage.</t>
+  </si>
+  <si>
+    <t>keep something in a cage</t>
+  </si>
+  <si>
+    <t>Rộng rãi</t>
+  </si>
+  <si>
+    <t>Spacious</t>
+  </si>
+  <si>
+    <t>The spacious room allowed us to dance</t>
+  </si>
+  <si>
+    <t>a spacious room</t>
+  </si>
+  <si>
+    <t>Con dê</t>
+  </si>
+  <si>
+    <t>goat</t>
+  </si>
+  <si>
+    <t>There are no mountain goats here</t>
+  </si>
+  <si>
+    <t>a mountain goat / dê núi</t>
+  </si>
+  <si>
+    <t>Gãi, cào</t>
+  </si>
+  <si>
+    <t>Scratch</t>
+  </si>
+  <si>
+    <t>The cat scratched my face</t>
+  </si>
+  <si>
+    <t>scratch something</t>
+  </si>
+  <si>
+    <t>Chủng, giống</t>
+  </si>
+  <si>
+    <t>Breed</t>
+  </si>
+  <si>
+    <t>The farm has many breeds of sheep</t>
+  </si>
+  <si>
+    <t>A breed of sheep / giống cừu</t>
+  </si>
+  <si>
+    <t>Lông</t>
+  </si>
+  <si>
+    <t>Fur</t>
+  </si>
+  <si>
+    <t>I wear a fur coat because the weather is cold</t>
+  </si>
+  <si>
+    <t>a fur coat / áo khoác lông thú</t>
+  </si>
+  <si>
+    <t>Thô cứng</t>
+  </si>
+  <si>
+    <t>Rough</t>
+  </si>
+  <si>
+    <t>My father is used (đã quen) to driving on rough roads</t>
+  </si>
+  <si>
+    <t>rough roads / những con đường gồ ghề</t>
+  </si>
+  <si>
+    <t>Intelligent</t>
+  </si>
+  <si>
+    <t>He student are highly intelligent</t>
+  </si>
+  <si>
+    <t>Highly intelligent / cực kỳ thông minh</t>
+  </si>
+  <si>
+    <t>Môi trường sống</t>
+  </si>
+  <si>
+    <t>Habitat</t>
+  </si>
+  <si>
+    <t>The jungle (rừng già) is the monkey's natural habitat</t>
+  </si>
+  <si>
+    <t>natural habitat / môi trường sống tự  nhiên</t>
+  </si>
+  <si>
+    <t>Cỏ</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>Laying on (nằm trên) a field of grass is nice</t>
+  </si>
+  <si>
+    <t>a field of grass</t>
+  </si>
+  <si>
+    <t>Bẩn</t>
+  </si>
+  <si>
+    <t>Dirty</t>
+  </si>
+  <si>
+    <t>I have dirty hands after painting</t>
+  </si>
+  <si>
+    <t>dirty hands / tay bẩn</t>
+  </si>
+  <si>
+    <t>Dọn dẹp</t>
+  </si>
+  <si>
+    <t>Clean up</t>
+  </si>
+  <si>
+    <t>Clean this place up before he arrives</t>
+  </si>
+  <si>
+    <t>clean something up</t>
+  </si>
+  <si>
+    <t>Nhận nuôi</t>
+  </si>
+  <si>
+    <t>Adopt</t>
+  </si>
+  <si>
+    <t>They are going to adopt a child</t>
+  </si>
+  <si>
+    <t>adopt somebody / nhận nuôi một ai đó</t>
+  </si>
+  <si>
+    <t>Thú nuôi</t>
+  </si>
+  <si>
+    <t>Pet</t>
+  </si>
+  <si>
+    <t>Our family pet is a parrot (con vẹt)</t>
+  </si>
+  <si>
+    <t>a family pet / thú nuôi trong gia đình</t>
+  </si>
+  <si>
+    <t>Sinh học</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>I graduated with a degree in biology</t>
+  </si>
+  <si>
+    <t>a degree in biology / một tấm bằng ngành sinh học</t>
+  </si>
+  <si>
+    <t>Tận hưởng, yêu thích</t>
+  </si>
+  <si>
+    <t>Enjoy</t>
+  </si>
+  <si>
+    <t>Hope you enjoy the movie</t>
+  </si>
+  <si>
+    <t>enjoy something</t>
+  </si>
+  <si>
+    <t>Đua</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Five horses will race against each other in the Grand Finale (vòng chung kết)</t>
+  </si>
+  <si>
+    <t>race against / đua với</t>
+  </si>
+  <si>
+    <t>Yên lặng, trật tự</t>
+  </si>
+  <si>
+    <t>Silent</t>
+  </si>
+  <si>
+    <t>You must keep silent as everyone is asleep (đang ngủ)</t>
+  </si>
+  <si>
+    <t>keep silent</t>
+  </si>
+  <si>
+    <t>Điều chỉnh</t>
+  </si>
+  <si>
+    <t>Adjust</t>
+  </si>
+  <si>
+    <t>Can you adjust the seat belt for me?</t>
+  </si>
+  <si>
+    <t>adjust something</t>
+  </si>
+  <si>
+    <t>Đói</t>
+  </si>
+  <si>
+    <t>Hungry</t>
+  </si>
+  <si>
+    <t>He gives the hungry crowd enough bread and fish</t>
+  </si>
+  <si>
+    <t>a hungry crowd / một đám người đang đói</t>
+  </si>
+  <si>
+    <t>Cho ăn</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>My mother is feeding the baby</t>
+  </si>
+  <si>
+    <t>feed somebody</t>
+  </si>
+  <si>
+    <t>Run out of</t>
+  </si>
+  <si>
+    <t>We ran out of milk</t>
+  </si>
+  <si>
+    <t>run out of something</t>
   </si>
 </sst>
 </file>
@@ -17741,10 +18185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1171"/>
+  <dimension ref="A1:G1201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1161" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1172" sqref="C1172"/>
+    <sheetView tabSelected="1" topLeftCell="F1185" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G1201" sqref="G1201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -44232,6 +44676,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="1172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1172" s="1" t="s">
+        <v>5782</v>
+      </c>
+      <c r="B1172" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1172" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="D1172" s="1" t="s">
+        <v>5813</v>
+      </c>
+      <c r="E1172" s="1" t="s">
+        <v>5815</v>
+      </c>
+      <c r="F1172" s="1" t="s">
+        <v>5814</v>
+      </c>
+      <c r="G1172" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1173" s="1" t="s">
+        <v>5783</v>
+      </c>
+      <c r="B1173" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1173" s="1" t="s">
+        <v>5816</v>
+      </c>
+      <c r="D1173" s="1" t="s">
+        <v>5817</v>
+      </c>
+      <c r="E1173" s="1" t="s">
+        <v>5818</v>
+      </c>
+      <c r="F1173" s="1" t="s">
+        <v>5819</v>
+      </c>
+      <c r="G1173" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1174" s="1" t="s">
+        <v>5784</v>
+      </c>
+      <c r="B1174" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1174" s="1" t="s">
+        <v>5820</v>
+      </c>
+      <c r="D1174" s="1" t="s">
+        <v>5821</v>
+      </c>
+      <c r="E1174" s="1" t="s">
+        <v>5822</v>
+      </c>
+      <c r="F1174" s="1" t="s">
+        <v>5823</v>
+      </c>
+      <c r="G1174" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1175" s="1" t="s">
+        <v>5785</v>
+      </c>
+      <c r="B1175" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1175" s="1" t="s">
+        <v>5824</v>
+      </c>
+      <c r="D1175" s="1" t="s">
+        <v>5825</v>
+      </c>
+      <c r="E1175" s="1" t="s">
+        <v>5826</v>
+      </c>
+      <c r="F1175" s="1" t="s">
+        <v>5827</v>
+      </c>
+      <c r="G1175" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1176" s="1" t="s">
+        <v>5786</v>
+      </c>
+      <c r="B1176" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1176" s="1" t="s">
+        <v>5828</v>
+      </c>
+      <c r="D1176" s="1" t="s">
+        <v>5829</v>
+      </c>
+      <c r="E1176" s="1" t="s">
+        <v>5830</v>
+      </c>
+      <c r="F1176" s="1" t="s">
+        <v>5831</v>
+      </c>
+      <c r="G1176" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1177" s="1" t="s">
+        <v>5787</v>
+      </c>
+      <c r="B1177" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1177" s="1" t="s">
+        <v>5832</v>
+      </c>
+      <c r="D1177" s="1" t="s">
+        <v>5833</v>
+      </c>
+      <c r="E1177" s="1" t="s">
+        <v>5834</v>
+      </c>
+      <c r="F1177" s="1" t="s">
+        <v>5835</v>
+      </c>
+      <c r="G1177" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1178" s="1" t="s">
+        <v>5788</v>
+      </c>
+      <c r="B1178" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1178" s="1" t="s">
+        <v>5836</v>
+      </c>
+      <c r="D1178" s="1" t="s">
+        <v>5837</v>
+      </c>
+      <c r="E1178" s="1" t="s">
+        <v>5838</v>
+      </c>
+      <c r="F1178" s="1" t="s">
+        <v>5839</v>
+      </c>
+      <c r="G1178" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1179" s="1" t="s">
+        <v>5789</v>
+      </c>
+      <c r="B1179" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1179" s="1" t="s">
+        <v>5840</v>
+      </c>
+      <c r="D1179" s="1" t="s">
+        <v>5841</v>
+      </c>
+      <c r="E1179" s="1" t="s">
+        <v>5843</v>
+      </c>
+      <c r="F1179" s="1" t="s">
+        <v>5842</v>
+      </c>
+      <c r="G1179" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1180" s="1" t="s">
+        <v>5790</v>
+      </c>
+      <c r="B1180" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1180" s="1" t="s">
+        <v>5844</v>
+      </c>
+      <c r="D1180" s="1" t="s">
+        <v>5845</v>
+      </c>
+      <c r="E1180" s="1" t="s">
+        <v>5846</v>
+      </c>
+      <c r="F1180" s="1" t="s">
+        <v>5847</v>
+      </c>
+      <c r="G1180" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1181" s="1" t="s">
+        <v>5791</v>
+      </c>
+      <c r="B1181" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1181" s="1" t="s">
+        <v>5848</v>
+      </c>
+      <c r="D1181" s="1" t="s">
+        <v>5849</v>
+      </c>
+      <c r="E1181" s="1" t="s">
+        <v>5850</v>
+      </c>
+      <c r="F1181" s="1" t="s">
+        <v>5851</v>
+      </c>
+      <c r="G1181" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1182" s="1" t="s">
+        <v>5792</v>
+      </c>
+      <c r="B1182" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1182" s="1" t="s">
+        <v>5852</v>
+      </c>
+      <c r="D1182" s="1" t="s">
+        <v>5853</v>
+      </c>
+      <c r="E1182" s="1" t="s">
+        <v>5854</v>
+      </c>
+      <c r="F1182" s="1" t="s">
+        <v>5855</v>
+      </c>
+      <c r="G1182" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1183" s="1" t="s">
+        <v>5793</v>
+      </c>
+      <c r="B1183" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1183" s="1" t="s">
+        <v>5856</v>
+      </c>
+      <c r="D1183" s="1" t="s">
+        <v>5857</v>
+      </c>
+      <c r="E1183" s="1" t="s">
+        <v>5858</v>
+      </c>
+      <c r="F1183" s="1" t="s">
+        <v>5859</v>
+      </c>
+      <c r="G1183" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1184" s="1" t="s">
+        <v>5794</v>
+      </c>
+      <c r="B1184" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1184" s="1" t="s">
+        <v>5860</v>
+      </c>
+      <c r="D1184" s="1" t="s">
+        <v>5861</v>
+      </c>
+      <c r="E1184" s="1" t="s">
+        <v>5862</v>
+      </c>
+      <c r="F1184" s="1" t="s">
+        <v>5863</v>
+      </c>
+      <c r="G1184" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1185" s="1" t="s">
+        <v>5795</v>
+      </c>
+      <c r="B1185" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1185" s="1" t="s">
+        <v>5864</v>
+      </c>
+      <c r="D1185" s="1" t="s">
+        <v>5865</v>
+      </c>
+      <c r="E1185" s="1" t="s">
+        <v>5866</v>
+      </c>
+      <c r="F1185" s="1" t="s">
+        <v>5867</v>
+      </c>
+      <c r="G1185" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1186" s="1" t="s">
+        <v>5796</v>
+      </c>
+      <c r="B1186" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1186" s="1" t="s">
+        <v>5868</v>
+      </c>
+      <c r="D1186" s="1" t="s">
+        <v>5869</v>
+      </c>
+      <c r="E1186" s="1" t="s">
+        <v>5870</v>
+      </c>
+      <c r="F1186" s="1" t="s">
+        <v>5871</v>
+      </c>
+      <c r="G1186" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1187" s="1" t="s">
+        <v>5797</v>
+      </c>
+      <c r="B1187" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1187" s="1" t="s">
+        <v>2884</v>
+      </c>
+      <c r="D1187" s="1" t="s">
+        <v>5872</v>
+      </c>
+      <c r="E1187" s="1" t="s">
+        <v>5873</v>
+      </c>
+      <c r="F1187" s="1" t="s">
+        <v>5874</v>
+      </c>
+      <c r="G1187" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1188" s="1" t="s">
+        <v>5798</v>
+      </c>
+      <c r="B1188" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1188" s="1" t="s">
+        <v>5875</v>
+      </c>
+      <c r="D1188" s="1" t="s">
+        <v>5876</v>
+      </c>
+      <c r="E1188" s="1" t="s">
+        <v>5877</v>
+      </c>
+      <c r="F1188" s="1" t="s">
+        <v>5878</v>
+      </c>
+      <c r="G1188" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1189" s="1" t="s">
+        <v>5799</v>
+      </c>
+      <c r="B1189" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1189" s="1" t="s">
+        <v>5879</v>
+      </c>
+      <c r="D1189" s="1" t="s">
+        <v>5880</v>
+      </c>
+      <c r="E1189" s="1" t="s">
+        <v>5881</v>
+      </c>
+      <c r="F1189" s="1" t="s">
+        <v>5882</v>
+      </c>
+      <c r="G1189" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1190" s="1" t="s">
+        <v>5800</v>
+      </c>
+      <c r="B1190" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1190" s="1" t="s">
+        <v>5883</v>
+      </c>
+      <c r="D1190" s="1" t="s">
+        <v>5884</v>
+      </c>
+      <c r="E1190" s="1" t="s">
+        <v>5885</v>
+      </c>
+      <c r="F1190" s="1" t="s">
+        <v>5886</v>
+      </c>
+      <c r="G1190" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1191" s="1" t="s">
+        <v>5801</v>
+      </c>
+      <c r="B1191" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1191" s="1" t="s">
+        <v>5887</v>
+      </c>
+      <c r="D1191" s="1" t="s">
+        <v>5888</v>
+      </c>
+      <c r="E1191" s="1" t="s">
+        <v>5889</v>
+      </c>
+      <c r="F1191" s="1" t="s">
+        <v>5890</v>
+      </c>
+      <c r="G1191" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1192" s="1" t="s">
+        <v>5802</v>
+      </c>
+      <c r="B1192" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1192" s="1" t="s">
+        <v>5891</v>
+      </c>
+      <c r="D1192" s="1" t="s">
+        <v>5892</v>
+      </c>
+      <c r="E1192" s="1" t="s">
+        <v>5893</v>
+      </c>
+      <c r="F1192" s="1" t="s">
+        <v>5894</v>
+      </c>
+      <c r="G1192" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1193" s="1" t="s">
+        <v>5803</v>
+      </c>
+      <c r="B1193" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1193" s="1" t="s">
+        <v>5895</v>
+      </c>
+      <c r="D1193" s="1" t="s">
+        <v>5896</v>
+      </c>
+      <c r="E1193" s="1" t="s">
+        <v>5897</v>
+      </c>
+      <c r="F1193" s="1" t="s">
+        <v>5898</v>
+      </c>
+      <c r="G1193" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1194" s="1" t="s">
+        <v>5804</v>
+      </c>
+      <c r="B1194" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1194" s="1" t="s">
+        <v>5899</v>
+      </c>
+      <c r="D1194" s="1" t="s">
+        <v>5900</v>
+      </c>
+      <c r="E1194" s="1" t="s">
+        <v>5901</v>
+      </c>
+      <c r="F1194" s="1" t="s">
+        <v>5902</v>
+      </c>
+      <c r="G1194" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1195" s="1" t="s">
+        <v>5805</v>
+      </c>
+      <c r="B1195" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1195" s="1" t="s">
+        <v>5903</v>
+      </c>
+      <c r="D1195" s="1" t="s">
+        <v>5904</v>
+      </c>
+      <c r="E1195" s="1" t="s">
+        <v>5905</v>
+      </c>
+      <c r="F1195" s="1" t="s">
+        <v>5906</v>
+      </c>
+      <c r="G1195" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1196" s="1" t="s">
+        <v>5806</v>
+      </c>
+      <c r="B1196" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1196" s="1" t="s">
+        <v>5907</v>
+      </c>
+      <c r="D1196" s="1" t="s">
+        <v>5908</v>
+      </c>
+      <c r="E1196" s="1" t="s">
+        <v>5909</v>
+      </c>
+      <c r="F1196" s="1" t="s">
+        <v>5910</v>
+      </c>
+      <c r="G1196" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1197" s="1" t="s">
+        <v>5807</v>
+      </c>
+      <c r="B1197" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1197" s="1" t="s">
+        <v>5911</v>
+      </c>
+      <c r="D1197" s="1" t="s">
+        <v>5912</v>
+      </c>
+      <c r="E1197" s="1" t="s">
+        <v>5913</v>
+      </c>
+      <c r="F1197" s="1" t="s">
+        <v>5914</v>
+      </c>
+      <c r="G1197" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1198" s="1" t="s">
+        <v>5808</v>
+      </c>
+      <c r="B1198" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1198" s="1" t="s">
+        <v>5915</v>
+      </c>
+      <c r="D1198" s="1" t="s">
+        <v>5916</v>
+      </c>
+      <c r="E1198" s="1" t="s">
+        <v>5917</v>
+      </c>
+      <c r="F1198" s="1" t="s">
+        <v>5918</v>
+      </c>
+      <c r="G1198" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1199" s="1" t="s">
+        <v>5809</v>
+      </c>
+      <c r="B1199" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1199" s="1" t="s">
+        <v>5919</v>
+      </c>
+      <c r="D1199" s="1" t="s">
+        <v>5920</v>
+      </c>
+      <c r="E1199" s="1" t="s">
+        <v>5921</v>
+      </c>
+      <c r="F1199" s="1" t="s">
+        <v>5922</v>
+      </c>
+      <c r="G1199" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1200" s="1" t="s">
+        <v>5810</v>
+      </c>
+      <c r="B1200" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1200" s="1" t="s">
+        <v>5923</v>
+      </c>
+      <c r="D1200" s="1" t="s">
+        <v>5924</v>
+      </c>
+      <c r="E1200" s="1" t="s">
+        <v>5925</v>
+      </c>
+      <c r="F1200" s="1" t="s">
+        <v>5926</v>
+      </c>
+      <c r="G1200" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1201" s="1" t="s">
+        <v>5811</v>
+      </c>
+      <c r="B1201" s="1">
+        <v>40</v>
+      </c>
+      <c r="C1201" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="D1201" s="1" t="s">
+        <v>5927</v>
+      </c>
+      <c r="E1201" s="1" t="s">
+        <v>5928</v>
+      </c>
+      <c r="F1201" s="1" t="s">
+        <v>5929</v>
+      </c>
+      <c r="G1201" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 41
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C291F4-CECA-E740-80FF-91DE0218B560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8799BC-7AC6-F642-B0A5-E9CC3CC0BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7054" uniqueCount="5930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7234" uniqueCount="6078">
   <si>
     <t>ID</t>
   </si>
@@ -17820,6 +17820,450 @@
   </si>
   <si>
     <t>run out of something</t>
+  </si>
+  <si>
+    <t>U41_01</t>
+  </si>
+  <si>
+    <t>U41_02</t>
+  </si>
+  <si>
+    <t>U41_03</t>
+  </si>
+  <si>
+    <t>U41_04</t>
+  </si>
+  <si>
+    <t>U41_05</t>
+  </si>
+  <si>
+    <t>U41_06</t>
+  </si>
+  <si>
+    <t>U41_07</t>
+  </si>
+  <si>
+    <t>U41_08</t>
+  </si>
+  <si>
+    <t>U41_09</t>
+  </si>
+  <si>
+    <t>U41_10</t>
+  </si>
+  <si>
+    <t>U41_11</t>
+  </si>
+  <si>
+    <t>U41_12</t>
+  </si>
+  <si>
+    <t>U41_13</t>
+  </si>
+  <si>
+    <t>U41_14</t>
+  </si>
+  <si>
+    <t>U41_15</t>
+  </si>
+  <si>
+    <t>U41_16</t>
+  </si>
+  <si>
+    <t>U41_17</t>
+  </si>
+  <si>
+    <t>U41_18</t>
+  </si>
+  <si>
+    <t>U41_19</t>
+  </si>
+  <si>
+    <t>U41_20</t>
+  </si>
+  <si>
+    <t>U41_21</t>
+  </si>
+  <si>
+    <t>U41_22</t>
+  </si>
+  <si>
+    <t>U41_23</t>
+  </si>
+  <si>
+    <t>U41_24</t>
+  </si>
+  <si>
+    <t>U41_25</t>
+  </si>
+  <si>
+    <t>U41_26</t>
+  </si>
+  <si>
+    <t>U41_27</t>
+  </si>
+  <si>
+    <t>U41_28</t>
+  </si>
+  <si>
+    <t>U41_29</t>
+  </si>
+  <si>
+    <t>U41_30</t>
+  </si>
+  <si>
+    <t>Nhiều mây</t>
+  </si>
+  <si>
+    <t>Cloudy</t>
+  </si>
+  <si>
+    <t>We are having a cloudy day today.</t>
+  </si>
+  <si>
+    <t>cloudy day / ngày nhiều mây</t>
+  </si>
+  <si>
+    <t>Làm bừng sáng</t>
+  </si>
+  <si>
+    <t>Brighten up</t>
+  </si>
+  <si>
+    <t>Your smile brightens up my day</t>
+  </si>
+  <si>
+    <t>brighten up somebody's day / làm bừng sáng một ngày của ai đó</t>
+  </si>
+  <si>
+    <t>Dự báo</t>
+  </si>
+  <si>
+    <t>Predict</t>
+  </si>
+  <si>
+    <t>No one can predict the future</t>
+  </si>
+  <si>
+    <t>predict the future / dự đoán trước tương lai</t>
+  </si>
+  <si>
+    <t>Accurate</t>
+  </si>
+  <si>
+    <t>Was what you said accurate information?</t>
+  </si>
+  <si>
+    <t>accurate information</t>
+  </si>
+  <si>
+    <t>Ôn hòa</t>
+  </si>
+  <si>
+    <t>Mild</t>
+  </si>
+  <si>
+    <t>Dalat has such as mild climate</t>
+  </si>
+  <si>
+    <t>a mild climate / khí hậu ôn hòa</t>
+  </si>
+  <si>
+    <t>Bão</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>A tropical storm swept through the village.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A tropical storm </t>
+  </si>
+  <si>
+    <t>Mưa nặng hạt</t>
+  </si>
+  <si>
+    <t>Pour down</t>
+  </si>
+  <si>
+    <t>Suddenly, the rain pours down</t>
+  </si>
+  <si>
+    <t>rain pours down / mưa rơi tầm tã</t>
+  </si>
+  <si>
+    <t>Chớp</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>A bolt of lightning struck down the house</t>
+  </si>
+  <si>
+    <t>a bolt of lightning / một tia sét</t>
+  </si>
+  <si>
+    <t>Sấm</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>They suddenly heard a clap of thunder</t>
+  </si>
+  <si>
+    <t>a clap of thunder / một tiếng sấm</t>
+  </si>
+  <si>
+    <t>Sườn, dốc</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>on a slope / trên một dốc</t>
+  </si>
+  <si>
+    <t>We slid down the hill on a slope / Chúng tôi trượt xuống sườn đồi trên một con dốc</t>
+  </si>
+  <si>
+    <t>Nhiều nắng</t>
+  </si>
+  <si>
+    <t>Sunny</t>
+  </si>
+  <si>
+    <t>Let's not waste this sunny day / đừng lãng phí một ngày đầy nắng như thế này.</t>
+  </si>
+  <si>
+    <t>a sunny day</t>
+  </si>
+  <si>
+    <t>Mùa xuân</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Families do spring cleaning before Te holiday.</t>
+  </si>
+  <si>
+    <t>spring cleaning / tổng vệ sinh đầu xuân</t>
+  </si>
+  <si>
+    <t>Bất thường</t>
+  </si>
+  <si>
+    <t>unusual</t>
+  </si>
+  <si>
+    <t>She behaved in a highly unusual manner</t>
+  </si>
+  <si>
+    <t>highly unusual / rất bất thường</t>
+  </si>
+  <si>
+    <t>Nơi trú ẩn</t>
+  </si>
+  <si>
+    <t>Shelter</t>
+  </si>
+  <si>
+    <t>You can volunteer at the homeless shelter</t>
+  </si>
+  <si>
+    <t>a homeless shelter / chỗ ở cho người vô gia cư</t>
+  </si>
+  <si>
+    <t>Mùa</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>It's growing season for berries (quả mọng)</t>
+  </si>
+  <si>
+    <t>growing season / mùa gieo trồng</t>
+  </si>
+  <si>
+    <t>Sa mạc</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>It is hot like the sahara desert</t>
+  </si>
+  <si>
+    <t>the Sahara Desert / sa mạc Sahara</t>
+  </si>
+  <si>
+    <t>Mùa thu</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>Fall weather feels cooler than summer weather</t>
+  </si>
+  <si>
+    <t>fall weather</t>
+  </si>
+  <si>
+    <t>Sight</t>
+  </si>
+  <si>
+    <t>A traffic jam is a common sight in big cities</t>
+  </si>
+  <si>
+    <t>common sight / cảnh thường thấy</t>
+  </si>
+  <si>
+    <t>Địa lý</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>A degree in geography helps you understand the Earth</t>
+  </si>
+  <si>
+    <t>a degree in geography / một tấm bằng ngành địa lý</t>
+  </si>
+  <si>
+    <t>Nghiêm trọng, dữ dội</t>
+  </si>
+  <si>
+    <t>Severe</t>
+  </si>
+  <si>
+    <t>I took a pull for my severe headache</t>
+  </si>
+  <si>
+    <t>a severe headache / một cơn đau đầu dữ dội</t>
+  </si>
+  <si>
+    <t>Động đất</t>
+  </si>
+  <si>
+    <t>Earthquake</t>
+  </si>
+  <si>
+    <t>Volcanoes can cause a powerful earthquake.</t>
+  </si>
+  <si>
+    <t>powerful earthquake / trận động đất mạnh</t>
+  </si>
+  <si>
+    <t>Mặt đất</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>The ball is on the ground</t>
+  </si>
+  <si>
+    <t>Trái đất</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>The earth is round</t>
+  </si>
+  <si>
+    <t>the earth</t>
+  </si>
+  <si>
+    <t>Tai họa</t>
+  </si>
+  <si>
+    <t>Disaster</t>
+  </si>
+  <si>
+    <t>the flood was a natural disaster</t>
+  </si>
+  <si>
+    <t>a natural disaster / thiên tai</t>
+  </si>
+  <si>
+    <t>Sóng</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>Surfers love to ride the wave</t>
+  </si>
+  <si>
+    <t>ride the wave / cưỡi sóng</t>
+  </si>
+  <si>
+    <t>Bờ biển</t>
+  </si>
+  <si>
+    <t>Coast</t>
+  </si>
+  <si>
+    <t>I have a house on the coast</t>
+  </si>
+  <si>
+    <t>on the coast / trên bờ biển</t>
+  </si>
+  <si>
+    <t>Đóng băng</t>
+  </si>
+  <si>
+    <t>Freeze</t>
+  </si>
+  <si>
+    <t>You can freeze fruits to make smoothies later</t>
+  </si>
+  <si>
+    <t>freeze something</t>
+  </si>
+  <si>
+    <t>Hồ</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t>The campfire is by the lake</t>
+  </si>
+  <si>
+    <t>by the lake / Bên hồ</t>
+  </si>
+  <si>
+    <t>Phá hủy</t>
+  </si>
+  <si>
+    <t>Destroy</t>
+  </si>
+  <si>
+    <t>My niece (cháu gái) destroyed my toys</t>
+  </si>
+  <si>
+    <t>destroy something</t>
+  </si>
+  <si>
+    <t>Vụ mùa</t>
+  </si>
+  <si>
+    <t>Crop</t>
+  </si>
+  <si>
+    <t>We are short of food crops</t>
+  </si>
+  <si>
+    <t>food crop / cây lương thực</t>
+  </si>
+  <si>
+    <t>on the ground</t>
   </si>
 </sst>
 </file>
@@ -18185,10 +18629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1201"/>
+  <dimension ref="A1:G1231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1185" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G1201" sqref="G1201"/>
+    <sheetView tabSelected="1" topLeftCell="A1161" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1186" sqref="C1186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -45366,6 +45810,696 @@
         <v>577</v>
       </c>
     </row>
+    <row r="1202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1202" s="1" t="s">
+        <v>5930</v>
+      </c>
+      <c r="B1202" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1202" s="1" t="s">
+        <v>5960</v>
+      </c>
+      <c r="D1202" s="1" t="s">
+        <v>5961</v>
+      </c>
+      <c r="E1202" s="1" t="s">
+        <v>5962</v>
+      </c>
+      <c r="F1202" s="1" t="s">
+        <v>5963</v>
+      </c>
+      <c r="G1202" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1203" s="1" t="s">
+        <v>5931</v>
+      </c>
+      <c r="B1203" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1203" s="1" t="s">
+        <v>5964</v>
+      </c>
+      <c r="D1203" s="1" t="s">
+        <v>5965</v>
+      </c>
+      <c r="E1203" s="1" t="s">
+        <v>5966</v>
+      </c>
+      <c r="F1203" s="1" t="s">
+        <v>5967</v>
+      </c>
+      <c r="G1203" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1204" s="1" t="s">
+        <v>5932</v>
+      </c>
+      <c r="B1204" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1204" s="1" t="s">
+        <v>5968</v>
+      </c>
+      <c r="D1204" s="1" t="s">
+        <v>5969</v>
+      </c>
+      <c r="E1204" s="1" t="s">
+        <v>5970</v>
+      </c>
+      <c r="F1204" s="1" t="s">
+        <v>5971</v>
+      </c>
+      <c r="G1204" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1205" s="1" t="s">
+        <v>5933</v>
+      </c>
+      <c r="B1205" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1205" s="1" t="s">
+        <v>4058</v>
+      </c>
+      <c r="D1205" s="1" t="s">
+        <v>5972</v>
+      </c>
+      <c r="E1205" s="1" t="s">
+        <v>5973</v>
+      </c>
+      <c r="F1205" s="1" t="s">
+        <v>5974</v>
+      </c>
+      <c r="G1205" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1206" s="1" t="s">
+        <v>5934</v>
+      </c>
+      <c r="B1206" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1206" s="1" t="s">
+        <v>5975</v>
+      </c>
+      <c r="D1206" s="1" t="s">
+        <v>5976</v>
+      </c>
+      <c r="E1206" s="1" t="s">
+        <v>5977</v>
+      </c>
+      <c r="F1206" s="1" t="s">
+        <v>5978</v>
+      </c>
+      <c r="G1206" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1207" s="1" t="s">
+        <v>5935</v>
+      </c>
+      <c r="B1207" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1207" s="1" t="s">
+        <v>5979</v>
+      </c>
+      <c r="D1207" s="1" t="s">
+        <v>5980</v>
+      </c>
+      <c r="E1207" s="1" t="s">
+        <v>5981</v>
+      </c>
+      <c r="F1207" s="1" t="s">
+        <v>5982</v>
+      </c>
+      <c r="G1207" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1208" s="1" t="s">
+        <v>5936</v>
+      </c>
+      <c r="B1208" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1208" s="1" t="s">
+        <v>5983</v>
+      </c>
+      <c r="D1208" s="1" t="s">
+        <v>5984</v>
+      </c>
+      <c r="E1208" s="1" t="s">
+        <v>5985</v>
+      </c>
+      <c r="F1208" s="1" t="s">
+        <v>5986</v>
+      </c>
+      <c r="G1208" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1209" s="1" t="s">
+        <v>5937</v>
+      </c>
+      <c r="B1209" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1209" s="1" t="s">
+        <v>5987</v>
+      </c>
+      <c r="D1209" s="1" t="s">
+        <v>5988</v>
+      </c>
+      <c r="E1209" s="1" t="s">
+        <v>5989</v>
+      </c>
+      <c r="F1209" s="1" t="s">
+        <v>5990</v>
+      </c>
+      <c r="G1209" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1210" s="1" t="s">
+        <v>5938</v>
+      </c>
+      <c r="B1210" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1210" s="1" t="s">
+        <v>5991</v>
+      </c>
+      <c r="D1210" s="1" t="s">
+        <v>5992</v>
+      </c>
+      <c r="E1210" s="1" t="s">
+        <v>5993</v>
+      </c>
+      <c r="F1210" s="1" t="s">
+        <v>5994</v>
+      </c>
+      <c r="G1210" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1211" s="1" t="s">
+        <v>5939</v>
+      </c>
+      <c r="B1211" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1211" s="1" t="s">
+        <v>5995</v>
+      </c>
+      <c r="D1211" s="1" t="s">
+        <v>5996</v>
+      </c>
+      <c r="E1211" s="1" t="s">
+        <v>5998</v>
+      </c>
+      <c r="F1211" s="1" t="s">
+        <v>5997</v>
+      </c>
+      <c r="G1211" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1212" s="1" t="s">
+        <v>5940</v>
+      </c>
+      <c r="B1212" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1212" s="1" t="s">
+        <v>5999</v>
+      </c>
+      <c r="D1212" s="1" t="s">
+        <v>6000</v>
+      </c>
+      <c r="E1212" s="1" t="s">
+        <v>6001</v>
+      </c>
+      <c r="F1212" s="1" t="s">
+        <v>6002</v>
+      </c>
+      <c r="G1212" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1213" s="1" t="s">
+        <v>5941</v>
+      </c>
+      <c r="B1213" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1213" s="1" t="s">
+        <v>6003</v>
+      </c>
+      <c r="D1213" s="1" t="s">
+        <v>6004</v>
+      </c>
+      <c r="E1213" s="1" t="s">
+        <v>6005</v>
+      </c>
+      <c r="F1213" s="1" t="s">
+        <v>6006</v>
+      </c>
+      <c r="G1213" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1214" s="1" t="s">
+        <v>5942</v>
+      </c>
+      <c r="B1214" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1214" s="1" t="s">
+        <v>6007</v>
+      </c>
+      <c r="D1214" s="1" t="s">
+        <v>6008</v>
+      </c>
+      <c r="E1214" s="1" t="s">
+        <v>6009</v>
+      </c>
+      <c r="F1214" s="1" t="s">
+        <v>6010</v>
+      </c>
+      <c r="G1214" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1215" s="1" t="s">
+        <v>5943</v>
+      </c>
+      <c r="B1215" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1215" s="1" t="s">
+        <v>6011</v>
+      </c>
+      <c r="D1215" s="1" t="s">
+        <v>6012</v>
+      </c>
+      <c r="E1215" s="1" t="s">
+        <v>6013</v>
+      </c>
+      <c r="F1215" s="1" t="s">
+        <v>6014</v>
+      </c>
+      <c r="G1215" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1216" s="1" t="s">
+        <v>5944</v>
+      </c>
+      <c r="B1216" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1216" s="1" t="s">
+        <v>6015</v>
+      </c>
+      <c r="D1216" s="1" t="s">
+        <v>6016</v>
+      </c>
+      <c r="E1216" s="1" t="s">
+        <v>6017</v>
+      </c>
+      <c r="F1216" s="1" t="s">
+        <v>6018</v>
+      </c>
+      <c r="G1216" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1217" s="1" t="s">
+        <v>5945</v>
+      </c>
+      <c r="B1217" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1217" s="1" t="s">
+        <v>6019</v>
+      </c>
+      <c r="D1217" s="1" t="s">
+        <v>6020</v>
+      </c>
+      <c r="E1217" s="1" t="s">
+        <v>6021</v>
+      </c>
+      <c r="F1217" s="1" t="s">
+        <v>6022</v>
+      </c>
+      <c r="G1217" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1218" s="1" t="s">
+        <v>5946</v>
+      </c>
+      <c r="B1218" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1218" s="1" t="s">
+        <v>6023</v>
+      </c>
+      <c r="D1218" s="1" t="s">
+        <v>6024</v>
+      </c>
+      <c r="E1218" s="1" t="s">
+        <v>6025</v>
+      </c>
+      <c r="F1218" s="1" t="s">
+        <v>6026</v>
+      </c>
+      <c r="G1218" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1219" s="1" t="s">
+        <v>5947</v>
+      </c>
+      <c r="B1219" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1219" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1219" s="1" t="s">
+        <v>6027</v>
+      </c>
+      <c r="E1219" s="1" t="s">
+        <v>6028</v>
+      </c>
+      <c r="F1219" s="1" t="s">
+        <v>6029</v>
+      </c>
+      <c r="G1219" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1220" s="1" t="s">
+        <v>5948</v>
+      </c>
+      <c r="B1220" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1220" s="1" t="s">
+        <v>6030</v>
+      </c>
+      <c r="D1220" s="1" t="s">
+        <v>6031</v>
+      </c>
+      <c r="E1220" s="1" t="s">
+        <v>6032</v>
+      </c>
+      <c r="F1220" s="1" t="s">
+        <v>6033</v>
+      </c>
+      <c r="G1220" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1221" s="1" t="s">
+        <v>5949</v>
+      </c>
+      <c r="B1221" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1221" s="1" t="s">
+        <v>6034</v>
+      </c>
+      <c r="D1221" s="1" t="s">
+        <v>6035</v>
+      </c>
+      <c r="E1221" s="1" t="s">
+        <v>6036</v>
+      </c>
+      <c r="F1221" s="1" t="s">
+        <v>6037</v>
+      </c>
+      <c r="G1221" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1222" s="1" t="s">
+        <v>5950</v>
+      </c>
+      <c r="B1222" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1222" s="1" t="s">
+        <v>6038</v>
+      </c>
+      <c r="D1222" s="1" t="s">
+        <v>6039</v>
+      </c>
+      <c r="E1222" s="1" t="s">
+        <v>6040</v>
+      </c>
+      <c r="F1222" s="1" t="s">
+        <v>6041</v>
+      </c>
+      <c r="G1222" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1223" s="1" t="s">
+        <v>5951</v>
+      </c>
+      <c r="B1223" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1223" s="1" t="s">
+        <v>6042</v>
+      </c>
+      <c r="D1223" s="1" t="s">
+        <v>6043</v>
+      </c>
+      <c r="E1223" s="1" t="s">
+        <v>6044</v>
+      </c>
+      <c r="F1223" s="1" t="s">
+        <v>6077</v>
+      </c>
+      <c r="G1223" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1224" s="1" t="s">
+        <v>5952</v>
+      </c>
+      <c r="B1224" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1224" s="1" t="s">
+        <v>6045</v>
+      </c>
+      <c r="D1224" s="1" t="s">
+        <v>6046</v>
+      </c>
+      <c r="E1224" s="1" t="s">
+        <v>6047</v>
+      </c>
+      <c r="F1224" s="1" t="s">
+        <v>6048</v>
+      </c>
+      <c r="G1224" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1225" s="1" t="s">
+        <v>5953</v>
+      </c>
+      <c r="B1225" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1225" s="1" t="s">
+        <v>6049</v>
+      </c>
+      <c r="D1225" s="1" t="s">
+        <v>6050</v>
+      </c>
+      <c r="E1225" s="1" t="s">
+        <v>6051</v>
+      </c>
+      <c r="F1225" s="1" t="s">
+        <v>6052</v>
+      </c>
+      <c r="G1225" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1226" s="1" t="s">
+        <v>5954</v>
+      </c>
+      <c r="B1226" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1226" s="1" t="s">
+        <v>6053</v>
+      </c>
+      <c r="D1226" s="1" t="s">
+        <v>6054</v>
+      </c>
+      <c r="E1226" s="1" t="s">
+        <v>6055</v>
+      </c>
+      <c r="F1226" s="1" t="s">
+        <v>6056</v>
+      </c>
+      <c r="G1226" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1227" s="1" t="s">
+        <v>5955</v>
+      </c>
+      <c r="B1227" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1227" s="1" t="s">
+        <v>6057</v>
+      </c>
+      <c r="D1227" s="1" t="s">
+        <v>6058</v>
+      </c>
+      <c r="E1227" s="1" t="s">
+        <v>6059</v>
+      </c>
+      <c r="F1227" s="1" t="s">
+        <v>6060</v>
+      </c>
+      <c r="G1227" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1228" s="1" t="s">
+        <v>5956</v>
+      </c>
+      <c r="B1228" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1228" s="1" t="s">
+        <v>6061</v>
+      </c>
+      <c r="D1228" s="1" t="s">
+        <v>6062</v>
+      </c>
+      <c r="E1228" s="1" t="s">
+        <v>6063</v>
+      </c>
+      <c r="F1228" s="1" t="s">
+        <v>6064</v>
+      </c>
+      <c r="G1228" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1229" s="1" t="s">
+        <v>5957</v>
+      </c>
+      <c r="B1229" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1229" s="1" t="s">
+        <v>6065</v>
+      </c>
+      <c r="D1229" s="1" t="s">
+        <v>6066</v>
+      </c>
+      <c r="E1229" s="1" t="s">
+        <v>6067</v>
+      </c>
+      <c r="F1229" s="1" t="s">
+        <v>6068</v>
+      </c>
+      <c r="G1229" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1230" s="1" t="s">
+        <v>5958</v>
+      </c>
+      <c r="B1230" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1230" s="1" t="s">
+        <v>6069</v>
+      </c>
+      <c r="D1230" s="1" t="s">
+        <v>6070</v>
+      </c>
+      <c r="E1230" s="1" t="s">
+        <v>6071</v>
+      </c>
+      <c r="F1230" s="1" t="s">
+        <v>6072</v>
+      </c>
+      <c r="G1230" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1231" s="1" t="s">
+        <v>5959</v>
+      </c>
+      <c r="B1231" s="1">
+        <v>41</v>
+      </c>
+      <c r="C1231" s="1" t="s">
+        <v>6073</v>
+      </c>
+      <c r="D1231" s="1" t="s">
+        <v>6074</v>
+      </c>
+      <c r="E1231" s="1" t="s">
+        <v>6075</v>
+      </c>
+      <c r="F1231" s="1" t="s">
+        <v>6076</v>
+      </c>
+      <c r="G1231" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 42
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8799BC-7AC6-F642-B0A5-E9CC3CC0BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600AD382-507B-5B43-939F-7745BD421513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7234" uniqueCount="6078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7414" uniqueCount="6226">
   <si>
     <t>ID</t>
   </si>
@@ -18264,6 +18264,450 @@
   </si>
   <si>
     <t>on the ground</t>
+  </si>
+  <si>
+    <t>U42_01</t>
+  </si>
+  <si>
+    <t>U42_02</t>
+  </si>
+  <si>
+    <t>U42_03</t>
+  </si>
+  <si>
+    <t>U42_04</t>
+  </si>
+  <si>
+    <t>U42_05</t>
+  </si>
+  <si>
+    <t>U42_06</t>
+  </si>
+  <si>
+    <t>U42_07</t>
+  </si>
+  <si>
+    <t>U42_08</t>
+  </si>
+  <si>
+    <t>U42_09</t>
+  </si>
+  <si>
+    <t>U42_10</t>
+  </si>
+  <si>
+    <t>U42_11</t>
+  </si>
+  <si>
+    <t>U42_12</t>
+  </si>
+  <si>
+    <t>U42_13</t>
+  </si>
+  <si>
+    <t>U42_14</t>
+  </si>
+  <si>
+    <t>U42_15</t>
+  </si>
+  <si>
+    <t>U42_16</t>
+  </si>
+  <si>
+    <t>U42_17</t>
+  </si>
+  <si>
+    <t>U42_18</t>
+  </si>
+  <si>
+    <t>U42_19</t>
+  </si>
+  <si>
+    <t>U42_20</t>
+  </si>
+  <si>
+    <t>U42_21</t>
+  </si>
+  <si>
+    <t>U42_22</t>
+  </si>
+  <si>
+    <t>U42_23</t>
+  </si>
+  <si>
+    <t>U42_24</t>
+  </si>
+  <si>
+    <t>U42_25</t>
+  </si>
+  <si>
+    <t>U42_26</t>
+  </si>
+  <si>
+    <t>U42_27</t>
+  </si>
+  <si>
+    <t>U42_28</t>
+  </si>
+  <si>
+    <t>U42_29</t>
+  </si>
+  <si>
+    <t>U42_30</t>
+  </si>
+  <si>
+    <t>Tai nghe</t>
+  </si>
+  <si>
+    <t>Headphones</t>
+  </si>
+  <si>
+    <t>Use a set of headphones to listen clearly</t>
+  </si>
+  <si>
+    <t>set of headphones / bộ tai nghe</t>
+  </si>
+  <si>
+    <t>Cổ điển</t>
+  </si>
+  <si>
+    <t>Classical</t>
+  </si>
+  <si>
+    <t>The classical concert is at the HaNoi Opera House</t>
+  </si>
+  <si>
+    <t>A classical concert / buổi hòa nhạc cổ điển</t>
+  </si>
+  <si>
+    <t>Nhạc cụ</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Can you play any instrument?</t>
+  </si>
+  <si>
+    <t>play an instrument</t>
+  </si>
+  <si>
+    <t>Cuộc thi</t>
+  </si>
+  <si>
+    <t>Contest</t>
+  </si>
+  <si>
+    <t>The contest between Jack and Jill is exciting.</t>
+  </si>
+  <si>
+    <t>contest between A and B</t>
+  </si>
+  <si>
+    <t>Sáo</t>
+  </si>
+  <si>
+    <t>Flute</t>
+  </si>
+  <si>
+    <t>I am learning to play the flute</t>
+  </si>
+  <si>
+    <t>play the flute</t>
+  </si>
+  <si>
+    <t>Nhạc sĩ, nhạc công</t>
+  </si>
+  <si>
+    <t>Musicican</t>
+  </si>
+  <si>
+    <t>Professional musicians have to train very hard.</t>
+  </si>
+  <si>
+    <t>a professional musician / nhạc công chuyên nghiệp</t>
+  </si>
+  <si>
+    <t>Thu âm</t>
+  </si>
+  <si>
+    <t>Record</t>
+  </si>
+  <si>
+    <t>come to the studio to record music</t>
+  </si>
+  <si>
+    <t>record something</t>
+  </si>
+  <si>
+    <t>hát theo</t>
+  </si>
+  <si>
+    <t>Sing along</t>
+  </si>
+  <si>
+    <t>if you know this song, please sing along with us</t>
+  </si>
+  <si>
+    <t>sing along with somebody</t>
+  </si>
+  <si>
+    <t>Bảng sếp hạng, bảng biểu</t>
+  </si>
+  <si>
+    <t>Chart</t>
+  </si>
+  <si>
+    <t>This song is number one in music charts these days</t>
+  </si>
+  <si>
+    <t>The music charts / bảng sếp hạng âm nhạc</t>
+  </si>
+  <si>
+    <t>Tông giọng</t>
+  </si>
+  <si>
+    <t>Tone</t>
+  </si>
+  <si>
+    <t>You can guess her feelings through the tone of her voice</t>
+  </si>
+  <si>
+    <t>tone of one's voice / tông giọng của một người</t>
+  </si>
+  <si>
+    <t>Giai điệu</t>
+  </si>
+  <si>
+    <t>Tune</t>
+  </si>
+  <si>
+    <t>I can dance to the tune of any song.</t>
+  </si>
+  <si>
+    <t>to the tune of something / theo giai điệu của một cái gì đó</t>
+  </si>
+  <si>
+    <t>Buổi triển lãm</t>
+  </si>
+  <si>
+    <t>Exhibition</t>
+  </si>
+  <si>
+    <t>This is an exhibition of children's paintings.</t>
+  </si>
+  <si>
+    <t>an exhibition of something</t>
+  </si>
+  <si>
+    <t>Nghệ sĩ</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>She works as a solo artist</t>
+  </si>
+  <si>
+    <t>a solo artist / nghệ sĩ độc tấu</t>
+  </si>
+  <si>
+    <t>Họa sĩ</t>
+  </si>
+  <si>
+    <t>Painter</t>
+  </si>
+  <si>
+    <t>a landscape painter / họa sĩ tranh phong cảnh</t>
+  </si>
+  <si>
+    <t>Landscape painters paint natural scenery (vẽ cảnh quan thiên nhiên)</t>
+  </si>
+  <si>
+    <t>Tác phẩm điêu khắc</t>
+  </si>
+  <si>
+    <t>Sculpture</t>
+  </si>
+  <si>
+    <t>The museum is full of marble sculpture</t>
+  </si>
+  <si>
+    <t>a marble sculpture / một tác phẩm điêu khắc bằng đá cẩm thạch</t>
+  </si>
+  <si>
+    <t>Tượng</t>
+  </si>
+  <si>
+    <t>Statue</t>
+  </si>
+  <si>
+    <t>The bronze statues need polishing ( lau chùi)</t>
+  </si>
+  <si>
+    <t>a bronze statue / bức tượng đồng</t>
+  </si>
+  <si>
+    <t>Drum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can the musician play the drum? </t>
+  </si>
+  <si>
+    <t>Play the drum</t>
+  </si>
+  <si>
+    <t>Hòa trộn</t>
+  </si>
+  <si>
+    <t>Blend</t>
+  </si>
+  <si>
+    <t>This song is a great blend of modern and traditional music.</t>
+  </si>
+  <si>
+    <t>a blend of / một sự pha trộn của</t>
+  </si>
+  <si>
+    <t>Thuộc dân gian</t>
+  </si>
+  <si>
+    <t>Folk</t>
+  </si>
+  <si>
+    <t>We learned many folk songs in kindergarten (trường mẫu giáo)</t>
+  </si>
+  <si>
+    <t>folk song / bài dân ca</t>
+  </si>
+  <si>
+    <t>Nhịp điệu</t>
+  </si>
+  <si>
+    <t>Rhythm</t>
+  </si>
+  <si>
+    <t>Please dance in rhythm with the music</t>
+  </si>
+  <si>
+    <t>in rhythm with something / đúng nhịp với cái gì</t>
+  </si>
+  <si>
+    <t>Hoàn toàn</t>
+  </si>
+  <si>
+    <t>absolutely</t>
+  </si>
+  <si>
+    <t>Absolutely nothing can go wrong now (có thể sai sót được nữa)</t>
+  </si>
+  <si>
+    <t>Absolutely nothing / hoàn toàn không có gì</t>
+  </si>
+  <si>
+    <t>Thơ ca</t>
+  </si>
+  <si>
+    <t>Poetry</t>
+  </si>
+  <si>
+    <t>Some artists write poetry</t>
+  </si>
+  <si>
+    <t>write poetry / sáng tác thơ</t>
+  </si>
+  <si>
+    <t>Phi thường</t>
+  </si>
+  <si>
+    <t>Extraordinary</t>
+  </si>
+  <si>
+    <t>My hero is an extraordinary person</t>
+  </si>
+  <si>
+    <t>An extraordinary person / một người phi thường</t>
+  </si>
+  <si>
+    <t>Thế kỷ</t>
+  </si>
+  <si>
+    <t>Century</t>
+  </si>
+  <si>
+    <t>This device was invented a century ago</t>
+  </si>
+  <si>
+    <t>a century ago / một thế kỷ trước</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>The theme of the party is halloween</t>
+  </si>
+  <si>
+    <t>theme of something / chủ đề của một cái gì đó</t>
+  </si>
+  <si>
+    <t>Thiết kế</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>It costs money to design a logo</t>
+  </si>
+  <si>
+    <t>design something</t>
+  </si>
+  <si>
+    <t>Biểu tượng</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Green is the symbol of nature</t>
+  </si>
+  <si>
+    <t>Symbol of something</t>
+  </si>
+  <si>
+    <t>Con rối</t>
+  </si>
+  <si>
+    <t>Puppet</t>
+  </si>
+  <si>
+    <t>The party will have a puppet show</t>
+  </si>
+  <si>
+    <t>a puppet show / một mà biểu diễn múa rối</t>
+  </si>
+  <si>
+    <t>Tài năng</t>
+  </si>
+  <si>
+    <t>Talented</t>
+  </si>
+  <si>
+    <t>In basketball, he is a talented player</t>
+  </si>
+  <si>
+    <t>a talented player</t>
+  </si>
+  <si>
+    <t>Tâm hồn</t>
+  </si>
+  <si>
+    <t>Soul</t>
+  </si>
+  <si>
+    <t>a beautiful soul / tâm hồn đẹp</t>
+  </si>
+  <si>
+    <t>You have a heart of gold (trái tim nhân hậu) and a beautiful soul</t>
   </si>
 </sst>
 </file>
@@ -18629,10 +19073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1231"/>
+  <dimension ref="A1:G1261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1161" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1186" sqref="C1186"/>
+    <sheetView tabSelected="1" topLeftCell="A1237" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E1251" sqref="E1251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -46500,6 +46944,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="1232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1232" s="1" t="s">
+        <v>6078</v>
+      </c>
+      <c r="B1232" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1232" s="1" t="s">
+        <v>6108</v>
+      </c>
+      <c r="D1232" s="1" t="s">
+        <v>6109</v>
+      </c>
+      <c r="E1232" s="1" t="s">
+        <v>6110</v>
+      </c>
+      <c r="F1232" s="1" t="s">
+        <v>6111</v>
+      </c>
+      <c r="G1232" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1233" s="1" t="s">
+        <v>6079</v>
+      </c>
+      <c r="B1233" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1233" s="1" t="s">
+        <v>6112</v>
+      </c>
+      <c r="D1233" s="1" t="s">
+        <v>6113</v>
+      </c>
+      <c r="E1233" s="1" t="s">
+        <v>6114</v>
+      </c>
+      <c r="F1233" s="1" t="s">
+        <v>6115</v>
+      </c>
+      <c r="G1233" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1234" s="1" t="s">
+        <v>6080</v>
+      </c>
+      <c r="B1234" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1234" s="1" t="s">
+        <v>6116</v>
+      </c>
+      <c r="D1234" s="1" t="s">
+        <v>6117</v>
+      </c>
+      <c r="E1234" s="1" t="s">
+        <v>6118</v>
+      </c>
+      <c r="F1234" s="1" t="s">
+        <v>6119</v>
+      </c>
+      <c r="G1234" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1235" s="1" t="s">
+        <v>6081</v>
+      </c>
+      <c r="B1235" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1235" s="1" t="s">
+        <v>6120</v>
+      </c>
+      <c r="D1235" s="1" t="s">
+        <v>6121</v>
+      </c>
+      <c r="E1235" s="1" t="s">
+        <v>6122</v>
+      </c>
+      <c r="F1235" s="1" t="s">
+        <v>6123</v>
+      </c>
+      <c r="G1235" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1236" s="1" t="s">
+        <v>6082</v>
+      </c>
+      <c r="B1236" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1236" s="1" t="s">
+        <v>6124</v>
+      </c>
+      <c r="D1236" s="1" t="s">
+        <v>6125</v>
+      </c>
+      <c r="E1236" s="1" t="s">
+        <v>6126</v>
+      </c>
+      <c r="F1236" s="1" t="s">
+        <v>6127</v>
+      </c>
+      <c r="G1236" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1237" s="1" t="s">
+        <v>6083</v>
+      </c>
+      <c r="B1237" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1237" s="1" t="s">
+        <v>6128</v>
+      </c>
+      <c r="D1237" s="1" t="s">
+        <v>6129</v>
+      </c>
+      <c r="E1237" s="1" t="s">
+        <v>6130</v>
+      </c>
+      <c r="F1237" s="1" t="s">
+        <v>6131</v>
+      </c>
+      <c r="G1237" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1238" s="1" t="s">
+        <v>6084</v>
+      </c>
+      <c r="B1238" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1238" s="1" t="s">
+        <v>6132</v>
+      </c>
+      <c r="D1238" s="1" t="s">
+        <v>6133</v>
+      </c>
+      <c r="E1238" s="1" t="s">
+        <v>6134</v>
+      </c>
+      <c r="F1238" s="1" t="s">
+        <v>6135</v>
+      </c>
+      <c r="G1238" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1239" s="1" t="s">
+        <v>6085</v>
+      </c>
+      <c r="B1239" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1239" s="1" t="s">
+        <v>6136</v>
+      </c>
+      <c r="D1239" s="1" t="s">
+        <v>6137</v>
+      </c>
+      <c r="E1239" s="1" t="s">
+        <v>6138</v>
+      </c>
+      <c r="F1239" s="1" t="s">
+        <v>6139</v>
+      </c>
+      <c r="G1239" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1240" s="1" t="s">
+        <v>6086</v>
+      </c>
+      <c r="B1240" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1240" s="1" t="s">
+        <v>6140</v>
+      </c>
+      <c r="D1240" s="1" t="s">
+        <v>6141</v>
+      </c>
+      <c r="E1240" s="1" t="s">
+        <v>6142</v>
+      </c>
+      <c r="F1240" s="1" t="s">
+        <v>6143</v>
+      </c>
+      <c r="G1240" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1241" s="1" t="s">
+        <v>6087</v>
+      </c>
+      <c r="B1241" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1241" s="1" t="s">
+        <v>6144</v>
+      </c>
+      <c r="D1241" s="1" t="s">
+        <v>6145</v>
+      </c>
+      <c r="E1241" s="1" t="s">
+        <v>6146</v>
+      </c>
+      <c r="F1241" s="1" t="s">
+        <v>6147</v>
+      </c>
+      <c r="G1241" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1242" s="1" t="s">
+        <v>6088</v>
+      </c>
+      <c r="B1242" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1242" s="1" t="s">
+        <v>6148</v>
+      </c>
+      <c r="D1242" s="1" t="s">
+        <v>6149</v>
+      </c>
+      <c r="E1242" s="1" t="s">
+        <v>6150</v>
+      </c>
+      <c r="F1242" s="1" t="s">
+        <v>6151</v>
+      </c>
+      <c r="G1242" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1243" s="1" t="s">
+        <v>6089</v>
+      </c>
+      <c r="B1243" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1243" s="1" t="s">
+        <v>6152</v>
+      </c>
+      <c r="D1243" s="1" t="s">
+        <v>6153</v>
+      </c>
+      <c r="E1243" s="1" t="s">
+        <v>6154</v>
+      </c>
+      <c r="F1243" s="1" t="s">
+        <v>6155</v>
+      </c>
+      <c r="G1243" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1244" s="1" t="s">
+        <v>6090</v>
+      </c>
+      <c r="B1244" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1244" s="1" t="s">
+        <v>6156</v>
+      </c>
+      <c r="D1244" s="1" t="s">
+        <v>6157</v>
+      </c>
+      <c r="E1244" s="1" t="s">
+        <v>6158</v>
+      </c>
+      <c r="F1244" s="1" t="s">
+        <v>6159</v>
+      </c>
+      <c r="G1244" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1245" s="1" t="s">
+        <v>6091</v>
+      </c>
+      <c r="B1245" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1245" s="1" t="s">
+        <v>6160</v>
+      </c>
+      <c r="D1245" s="1" t="s">
+        <v>6161</v>
+      </c>
+      <c r="E1245" s="1" t="s">
+        <v>6163</v>
+      </c>
+      <c r="F1245" s="1" t="s">
+        <v>6162</v>
+      </c>
+      <c r="G1245" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1246" s="1" t="s">
+        <v>6092</v>
+      </c>
+      <c r="B1246" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1246" s="1" t="s">
+        <v>6164</v>
+      </c>
+      <c r="D1246" s="1" t="s">
+        <v>6165</v>
+      </c>
+      <c r="E1246" s="1" t="s">
+        <v>6166</v>
+      </c>
+      <c r="F1246" s="1" t="s">
+        <v>6167</v>
+      </c>
+      <c r="G1246" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1247" s="1" t="s">
+        <v>6093</v>
+      </c>
+      <c r="B1247" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1247" s="1" t="s">
+        <v>6168</v>
+      </c>
+      <c r="D1247" s="1" t="s">
+        <v>6169</v>
+      </c>
+      <c r="E1247" s="1" t="s">
+        <v>6170</v>
+      </c>
+      <c r="F1247" s="1" t="s">
+        <v>6171</v>
+      </c>
+      <c r="G1247" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1248" s="1" t="s">
+        <v>6094</v>
+      </c>
+      <c r="B1248" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1248" s="1" t="s">
+        <v>4407</v>
+      </c>
+      <c r="D1248" s="1" t="s">
+        <v>6172</v>
+      </c>
+      <c r="E1248" s="1" t="s">
+        <v>6173</v>
+      </c>
+      <c r="F1248" s="1" t="s">
+        <v>6174</v>
+      </c>
+      <c r="G1248" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1249" s="1" t="s">
+        <v>6095</v>
+      </c>
+      <c r="B1249" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1249" s="1" t="s">
+        <v>6175</v>
+      </c>
+      <c r="D1249" s="1" t="s">
+        <v>6176</v>
+      </c>
+      <c r="E1249" s="1" t="s">
+        <v>6177</v>
+      </c>
+      <c r="F1249" s="1" t="s">
+        <v>6178</v>
+      </c>
+      <c r="G1249" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1250" s="1" t="s">
+        <v>6096</v>
+      </c>
+      <c r="B1250" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1250" s="1" t="s">
+        <v>6179</v>
+      </c>
+      <c r="D1250" s="1" t="s">
+        <v>6180</v>
+      </c>
+      <c r="E1250" s="1" t="s">
+        <v>6181</v>
+      </c>
+      <c r="F1250" s="1" t="s">
+        <v>6182</v>
+      </c>
+      <c r="G1250" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1251" s="1" t="s">
+        <v>6097</v>
+      </c>
+      <c r="B1251" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1251" s="1" t="s">
+        <v>6183</v>
+      </c>
+      <c r="D1251" s="1" t="s">
+        <v>6184</v>
+      </c>
+      <c r="E1251" s="1" t="s">
+        <v>6185</v>
+      </c>
+      <c r="F1251" s="1" t="s">
+        <v>6186</v>
+      </c>
+      <c r="G1251" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1252" s="1" t="s">
+        <v>6098</v>
+      </c>
+      <c r="B1252" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1252" s="1" t="s">
+        <v>6187</v>
+      </c>
+      <c r="D1252" s="1" t="s">
+        <v>6188</v>
+      </c>
+      <c r="E1252" s="1" t="s">
+        <v>6189</v>
+      </c>
+      <c r="F1252" s="1" t="s">
+        <v>6190</v>
+      </c>
+      <c r="G1252" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1253" s="1" t="s">
+        <v>6099</v>
+      </c>
+      <c r="B1253" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1253" s="1" t="s">
+        <v>6191</v>
+      </c>
+      <c r="D1253" s="1" t="s">
+        <v>6192</v>
+      </c>
+      <c r="E1253" s="1" t="s">
+        <v>6193</v>
+      </c>
+      <c r="F1253" s="1" t="s">
+        <v>6194</v>
+      </c>
+      <c r="G1253" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1254" s="1" t="s">
+        <v>6100</v>
+      </c>
+      <c r="B1254" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1254" s="1" t="s">
+        <v>6195</v>
+      </c>
+      <c r="D1254" s="1" t="s">
+        <v>6196</v>
+      </c>
+      <c r="E1254" s="1" t="s">
+        <v>6197</v>
+      </c>
+      <c r="F1254" s="1" t="s">
+        <v>6198</v>
+      </c>
+      <c r="G1254" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1255" s="1" t="s">
+        <v>6101</v>
+      </c>
+      <c r="B1255" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1255" s="1" t="s">
+        <v>6199</v>
+      </c>
+      <c r="D1255" s="1" t="s">
+        <v>6200</v>
+      </c>
+      <c r="E1255" s="1" t="s">
+        <v>6201</v>
+      </c>
+      <c r="F1255" s="1" t="s">
+        <v>6202</v>
+      </c>
+      <c r="G1255" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1256" s="1" t="s">
+        <v>6102</v>
+      </c>
+      <c r="B1256" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1256" s="1" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D1256" s="1" t="s">
+        <v>6203</v>
+      </c>
+      <c r="E1256" s="1" t="s">
+        <v>6204</v>
+      </c>
+      <c r="F1256" s="1" t="s">
+        <v>6205</v>
+      </c>
+      <c r="G1256" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1257" s="1" t="s">
+        <v>6103</v>
+      </c>
+      <c r="B1257" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1257" s="1" t="s">
+        <v>6206</v>
+      </c>
+      <c r="D1257" s="1" t="s">
+        <v>6207</v>
+      </c>
+      <c r="E1257" s="1" t="s">
+        <v>6208</v>
+      </c>
+      <c r="F1257" s="1" t="s">
+        <v>6209</v>
+      </c>
+      <c r="G1257" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1258" s="1" t="s">
+        <v>6104</v>
+      </c>
+      <c r="B1258" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1258" s="1" t="s">
+        <v>6210</v>
+      </c>
+      <c r="D1258" s="1" t="s">
+        <v>6211</v>
+      </c>
+      <c r="E1258" s="1" t="s">
+        <v>6212</v>
+      </c>
+      <c r="F1258" s="1" t="s">
+        <v>6213</v>
+      </c>
+      <c r="G1258" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1259" s="1" t="s">
+        <v>6105</v>
+      </c>
+      <c r="B1259" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1259" s="1" t="s">
+        <v>6214</v>
+      </c>
+      <c r="D1259" s="1" t="s">
+        <v>6215</v>
+      </c>
+      <c r="E1259" s="1" t="s">
+        <v>6216</v>
+      </c>
+      <c r="F1259" s="1" t="s">
+        <v>6217</v>
+      </c>
+      <c r="G1259" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1260" s="1" t="s">
+        <v>6106</v>
+      </c>
+      <c r="B1260" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1260" s="1" t="s">
+        <v>6218</v>
+      </c>
+      <c r="D1260" s="1" t="s">
+        <v>6219</v>
+      </c>
+      <c r="E1260" s="1" t="s">
+        <v>6220</v>
+      </c>
+      <c r="F1260" s="1" t="s">
+        <v>6221</v>
+      </c>
+      <c r="G1260" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1261" s="1" t="s">
+        <v>6107</v>
+      </c>
+      <c r="B1261" s="1">
+        <v>42</v>
+      </c>
+      <c r="C1261" s="1" t="s">
+        <v>6222</v>
+      </c>
+      <c r="D1261" s="1" t="s">
+        <v>6223</v>
+      </c>
+      <c r="E1261" s="1" t="s">
+        <v>6225</v>
+      </c>
+      <c r="F1261" s="1" t="s">
+        <v>6224</v>
+      </c>
+      <c r="G1261" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 43
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600AD382-507B-5B43-939F-7745BD421513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6588E01F-AEAC-A448-8F0B-8F9E56C7027D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7414" uniqueCount="6226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7594" uniqueCount="6373">
   <si>
     <t>ID</t>
   </si>
@@ -18708,6 +18708,447 @@
   </si>
   <si>
     <t>You have a heart of gold (trái tim nhân hậu) and a beautiful soul</t>
+  </si>
+  <si>
+    <t>U43_01</t>
+  </si>
+  <si>
+    <t>U43_02</t>
+  </si>
+  <si>
+    <t>U43_03</t>
+  </si>
+  <si>
+    <t>U43_04</t>
+  </si>
+  <si>
+    <t>U43_05</t>
+  </si>
+  <si>
+    <t>U43_06</t>
+  </si>
+  <si>
+    <t>U43_07</t>
+  </si>
+  <si>
+    <t>U43_08</t>
+  </si>
+  <si>
+    <t>U43_09</t>
+  </si>
+  <si>
+    <t>U43_10</t>
+  </si>
+  <si>
+    <t>U43_11</t>
+  </si>
+  <si>
+    <t>U43_12</t>
+  </si>
+  <si>
+    <t>U43_13</t>
+  </si>
+  <si>
+    <t>U43_14</t>
+  </si>
+  <si>
+    <t>U43_15</t>
+  </si>
+  <si>
+    <t>U43_16</t>
+  </si>
+  <si>
+    <t>U43_17</t>
+  </si>
+  <si>
+    <t>U43_18</t>
+  </si>
+  <si>
+    <t>U43_19</t>
+  </si>
+  <si>
+    <t>U43_20</t>
+  </si>
+  <si>
+    <t>U43_21</t>
+  </si>
+  <si>
+    <t>U43_22</t>
+  </si>
+  <si>
+    <t>U43_23</t>
+  </si>
+  <si>
+    <t>U43_24</t>
+  </si>
+  <si>
+    <t>U43_25</t>
+  </si>
+  <si>
+    <t>U43_26</t>
+  </si>
+  <si>
+    <t>U43_27</t>
+  </si>
+  <si>
+    <t>U43_28</t>
+  </si>
+  <si>
+    <t>U43_29</t>
+  </si>
+  <si>
+    <t>U43_30</t>
+  </si>
+  <si>
+    <t>Bối rối</t>
+  </si>
+  <si>
+    <t>Frustrated</t>
+  </si>
+  <si>
+    <t>He is frustrated at this math question.</t>
+  </si>
+  <si>
+    <t>Frustrated at something</t>
+  </si>
+  <si>
+    <t>Giả định</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t>make an assumption / đưa ra giả định</t>
+  </si>
+  <si>
+    <t>They make assumptions about me being rude(rằng tôi là người thô lỗ)</t>
+  </si>
+  <si>
+    <t>Phép thuật</t>
+  </si>
+  <si>
+    <t>magic</t>
+  </si>
+  <si>
+    <t>She made it disappeer like magic</t>
+  </si>
+  <si>
+    <t>like magic / như phép màu</t>
+  </si>
+  <si>
+    <t>Chance</t>
+  </si>
+  <si>
+    <t>We met each other by chance / chúng tôi tình cờ gặp nhau</t>
+  </si>
+  <si>
+    <t>By chance / tình cờ</t>
+  </si>
+  <si>
+    <t>Yếu tố</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Have you considered all the important factors</t>
+  </si>
+  <si>
+    <t>an important factor / một yếu tố quan trọng</t>
+  </si>
+  <si>
+    <t>Bên trong</t>
+  </si>
+  <si>
+    <t>Inside</t>
+  </si>
+  <si>
+    <t>Your shirt is inside out</t>
+  </si>
+  <si>
+    <t>inside out / lộn ngược phần trong ra ngoài</t>
+  </si>
+  <si>
+    <t>Sự lo ngại</t>
+  </si>
+  <si>
+    <t>Concern</t>
+  </si>
+  <si>
+    <t>I have lots of concerns about my son</t>
+  </si>
+  <si>
+    <t>concern about something or somebody</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Please rate 5 star for that book on App Store</t>
+  </si>
+  <si>
+    <t>Rate something</t>
+  </si>
+  <si>
+    <t>Completely</t>
+  </si>
+  <si>
+    <t>He was a completely different person</t>
+  </si>
+  <si>
+    <t>completely different / hoàn toàn khác</t>
+  </si>
+  <si>
+    <t>Sự tồn tại</t>
+  </si>
+  <si>
+    <t>Existence</t>
+  </si>
+  <si>
+    <t>Dinosaurs are no longer in existence</t>
+  </si>
+  <si>
+    <t>in existence / tồn tại</t>
+  </si>
+  <si>
+    <t>Nghiên cứu, xem xét</t>
+  </si>
+  <si>
+    <t>The police will look into the files</t>
+  </si>
+  <si>
+    <t>Look into</t>
+  </si>
+  <si>
+    <t>Look into something</t>
+  </si>
+  <si>
+    <t>Kiểm soát</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>My father always tries to control me</t>
+  </si>
+  <si>
+    <t>control somebody or something</t>
+  </si>
+  <si>
+    <t>Bài viết</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Have you read the news article today?</t>
+  </si>
+  <si>
+    <t>a news article / bài báo</t>
+  </si>
+  <si>
+    <t>Tác giả</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Best-selling authors are skilled in writing</t>
+  </si>
+  <si>
+    <t>a best-selling author / tác giả bán chạy nhất</t>
+  </si>
+  <si>
+    <t>Đoạn</t>
+  </si>
+  <si>
+    <t>Passage</t>
+  </si>
+  <si>
+    <t>please read the message on page 24.</t>
+  </si>
+  <si>
+    <t>read a passage / đọc một đoạn</t>
+  </si>
+  <si>
+    <t>Thuyết phục</t>
+  </si>
+  <si>
+    <t>Convince</t>
+  </si>
+  <si>
+    <t>Please convince her to help me</t>
+  </si>
+  <si>
+    <t>convince somebody</t>
+  </si>
+  <si>
+    <t>Phần</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>I am a part of the team</t>
+  </si>
+  <si>
+    <t>part of something</t>
+  </si>
+  <si>
+    <t>Vừa đủ</t>
+  </si>
+  <si>
+    <t>Adequate</t>
+  </si>
+  <si>
+    <t>She show an adequate amout of skill.</t>
+  </si>
+  <si>
+    <t>An adequate amount / một lượng vừa đủ</t>
+  </si>
+  <si>
+    <t>Chọn</t>
+  </si>
+  <si>
+    <t>Pick</t>
+  </si>
+  <si>
+    <t>The team pucked him to be the leader</t>
+  </si>
+  <si>
+    <t>pick somebody or something</t>
+  </si>
+  <si>
+    <t>Thành thật, trung thực</t>
+  </si>
+  <si>
+    <t>Honest</t>
+  </si>
+  <si>
+    <t>Please be honest about your past.</t>
+  </si>
+  <si>
+    <t>honest about something / thành thật về một điều gì đó</t>
+  </si>
+  <si>
+    <t>Thất vọng</t>
+  </si>
+  <si>
+    <t>Disappointed</t>
+  </si>
+  <si>
+    <t>I am disappointed with what you did</t>
+  </si>
+  <si>
+    <t>disappointed with</t>
+  </si>
+  <si>
+    <t>Kết cấu</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>The structure of the company is complex</t>
+  </si>
+  <si>
+    <t>a structure of something</t>
+  </si>
+  <si>
+    <t>Tập phim</t>
+  </si>
+  <si>
+    <t>Episode</t>
+  </si>
+  <si>
+    <t>They broke up in the last episode</t>
+  </si>
+  <si>
+    <t>in an episode / trong tập phim</t>
+  </si>
+  <si>
+    <t>Thay thế</t>
+  </si>
+  <si>
+    <t>Replace</t>
+  </si>
+  <si>
+    <t>The school replaced the old building</t>
+  </si>
+  <si>
+    <t>replace somebody or something</t>
+  </si>
+  <si>
+    <t>Nguyên bản, độc đáo</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>He came up with an original idea.</t>
+  </si>
+  <si>
+    <t>an original idea / ý tưởng độc đáo</t>
+  </si>
+  <si>
+    <t>Sự phân tích</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>We need an expert in data analysis</t>
+  </si>
+  <si>
+    <t>data analysis / việc phân tích dữ liệu</t>
+  </si>
+  <si>
+    <t>Công lý</t>
+  </si>
+  <si>
+    <t>Justice</t>
+  </si>
+  <si>
+    <t>Justice will be served when he receives punishment(hình phạt)</t>
+  </si>
+  <si>
+    <t>justice is served / công lý được thực thi</t>
+  </si>
+  <si>
+    <t>Đại diện cho, ủng hộ cho</t>
+  </si>
+  <si>
+    <t>Stand for</t>
+  </si>
+  <si>
+    <t>We stand for equality</t>
+  </si>
+  <si>
+    <t>stand for something / ủng hộ cho một cái gì đó</t>
+  </si>
+  <si>
+    <t>Kết luận</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>In conclusion, this book is good</t>
+  </si>
+  <si>
+    <t>in conclusion / kết luận là</t>
+  </si>
+  <si>
+    <t>Khắp, suốt</t>
+  </si>
+  <si>
+    <t>Throughout</t>
+  </si>
+  <si>
+    <t>The school opens throughout the year</t>
+  </si>
+  <si>
+    <t>throughout the year / suốt cả năm</t>
   </si>
 </sst>
 </file>
@@ -19073,10 +19514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1261"/>
+  <dimension ref="A1:G1291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1237" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1251" sqref="E1251"/>
+    <sheetView tabSelected="1" topLeftCell="A1172" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1292" sqref="C1292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -47634,6 +48075,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="1262" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1262" s="1" t="s">
+        <v>6226</v>
+      </c>
+      <c r="B1262" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1262" s="1" t="s">
+        <v>6256</v>
+      </c>
+      <c r="D1262" s="1" t="s">
+        <v>6257</v>
+      </c>
+      <c r="E1262" s="1" t="s">
+        <v>6258</v>
+      </c>
+      <c r="F1262" s="1" t="s">
+        <v>6259</v>
+      </c>
+      <c r="G1262" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1263" s="1" t="s">
+        <v>6227</v>
+      </c>
+      <c r="B1263" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1263" s="1" t="s">
+        <v>6260</v>
+      </c>
+      <c r="D1263" s="1" t="s">
+        <v>6261</v>
+      </c>
+      <c r="E1263" s="1" t="s">
+        <v>6263</v>
+      </c>
+      <c r="F1263" s="1" t="s">
+        <v>6262</v>
+      </c>
+      <c r="G1263" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1264" s="1" t="s">
+        <v>6228</v>
+      </c>
+      <c r="B1264" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1264" s="1" t="s">
+        <v>6264</v>
+      </c>
+      <c r="D1264" s="1" t="s">
+        <v>6265</v>
+      </c>
+      <c r="E1264" s="1" t="s">
+        <v>6266</v>
+      </c>
+      <c r="F1264" s="1" t="s">
+        <v>6267</v>
+      </c>
+      <c r="G1264" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1265" s="1" t="s">
+        <v>6229</v>
+      </c>
+      <c r="B1265" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1265" s="1" t="s">
+        <v>4137</v>
+      </c>
+      <c r="D1265" s="1" t="s">
+        <v>6268</v>
+      </c>
+      <c r="E1265" s="1" t="s">
+        <v>6269</v>
+      </c>
+      <c r="F1265" s="1" t="s">
+        <v>6270</v>
+      </c>
+      <c r="G1265" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1266" s="1" t="s">
+        <v>6230</v>
+      </c>
+      <c r="B1266" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1266" s="1" t="s">
+        <v>6271</v>
+      </c>
+      <c r="D1266" s="1" t="s">
+        <v>6272</v>
+      </c>
+      <c r="E1266" s="1" t="s">
+        <v>6273</v>
+      </c>
+      <c r="F1266" s="1" t="s">
+        <v>6274</v>
+      </c>
+      <c r="G1266" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1267" s="1" t="s">
+        <v>6231</v>
+      </c>
+      <c r="B1267" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1267" s="1" t="s">
+        <v>6275</v>
+      </c>
+      <c r="D1267" s="1" t="s">
+        <v>6276</v>
+      </c>
+      <c r="E1267" s="1" t="s">
+        <v>6277</v>
+      </c>
+      <c r="F1267" s="1" t="s">
+        <v>6278</v>
+      </c>
+      <c r="G1267" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1268" s="1" t="s">
+        <v>6232</v>
+      </c>
+      <c r="B1268" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1268" s="1" t="s">
+        <v>6279</v>
+      </c>
+      <c r="D1268" s="1" t="s">
+        <v>6280</v>
+      </c>
+      <c r="E1268" s="1" t="s">
+        <v>6281</v>
+      </c>
+      <c r="F1268" s="1" t="s">
+        <v>6282</v>
+      </c>
+      <c r="G1268" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1269" s="1" t="s">
+        <v>6233</v>
+      </c>
+      <c r="B1269" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1269" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="D1269" s="1" t="s">
+        <v>6283</v>
+      </c>
+      <c r="E1269" s="1" t="s">
+        <v>6284</v>
+      </c>
+      <c r="F1269" s="1" t="s">
+        <v>6285</v>
+      </c>
+      <c r="G1269" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1270" s="1" t="s">
+        <v>6234</v>
+      </c>
+      <c r="B1270" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1270" s="1" t="s">
+        <v>6187</v>
+      </c>
+      <c r="D1270" s="1" t="s">
+        <v>6286</v>
+      </c>
+      <c r="E1270" s="1" t="s">
+        <v>6287</v>
+      </c>
+      <c r="F1270" s="1" t="s">
+        <v>6288</v>
+      </c>
+      <c r="G1270" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1271" s="1" t="s">
+        <v>6235</v>
+      </c>
+      <c r="B1271" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1271" s="1" t="s">
+        <v>6289</v>
+      </c>
+      <c r="D1271" s="1" t="s">
+        <v>6290</v>
+      </c>
+      <c r="E1271" s="1" t="s">
+        <v>6291</v>
+      </c>
+      <c r="F1271" s="1" t="s">
+        <v>6292</v>
+      </c>
+      <c r="G1271" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1272" s="1" t="s">
+        <v>6236</v>
+      </c>
+      <c r="B1272" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1272" s="1" t="s">
+        <v>6293</v>
+      </c>
+      <c r="D1272" s="1" t="s">
+        <v>6295</v>
+      </c>
+      <c r="E1272" s="1" t="s">
+        <v>6294</v>
+      </c>
+      <c r="F1272" s="1" t="s">
+        <v>6296</v>
+      </c>
+      <c r="G1272" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1273" s="1" t="s">
+        <v>6237</v>
+      </c>
+      <c r="B1273" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1273" s="1" t="s">
+        <v>6297</v>
+      </c>
+      <c r="D1273" s="1" t="s">
+        <v>6298</v>
+      </c>
+      <c r="E1273" s="1" t="s">
+        <v>6299</v>
+      </c>
+      <c r="F1273" s="1" t="s">
+        <v>6300</v>
+      </c>
+      <c r="G1273" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1274" s="1" t="s">
+        <v>6238</v>
+      </c>
+      <c r="B1274" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1274" s="1" t="s">
+        <v>6301</v>
+      </c>
+      <c r="D1274" s="1" t="s">
+        <v>6302</v>
+      </c>
+      <c r="E1274" s="1" t="s">
+        <v>6303</v>
+      </c>
+      <c r="F1274" s="1" t="s">
+        <v>6304</v>
+      </c>
+      <c r="G1274" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1275" s="1" t="s">
+        <v>6239</v>
+      </c>
+      <c r="B1275" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1275" s="1" t="s">
+        <v>6305</v>
+      </c>
+      <c r="D1275" s="1" t="s">
+        <v>6306</v>
+      </c>
+      <c r="E1275" s="1" t="s">
+        <v>6307</v>
+      </c>
+      <c r="F1275" s="1" t="s">
+        <v>6308</v>
+      </c>
+      <c r="G1275" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1276" s="1" t="s">
+        <v>6240</v>
+      </c>
+      <c r="B1276" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1276" s="1" t="s">
+        <v>6309</v>
+      </c>
+      <c r="D1276" s="1" t="s">
+        <v>6310</v>
+      </c>
+      <c r="E1276" s="1" t="s">
+        <v>6311</v>
+      </c>
+      <c r="F1276" s="1" t="s">
+        <v>6312</v>
+      </c>
+      <c r="G1276" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1277" s="1" t="s">
+        <v>6241</v>
+      </c>
+      <c r="B1277" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1277" s="1" t="s">
+        <v>6313</v>
+      </c>
+      <c r="D1277" s="1" t="s">
+        <v>6314</v>
+      </c>
+      <c r="E1277" s="1" t="s">
+        <v>6315</v>
+      </c>
+      <c r="F1277" s="1" t="s">
+        <v>6316</v>
+      </c>
+      <c r="G1277" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1278" s="1" t="s">
+        <v>6242</v>
+      </c>
+      <c r="B1278" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1278" s="1" t="s">
+        <v>6317</v>
+      </c>
+      <c r="D1278" s="1" t="s">
+        <v>6318</v>
+      </c>
+      <c r="E1278" s="1" t="s">
+        <v>6319</v>
+      </c>
+      <c r="F1278" s="1" t="s">
+        <v>6320</v>
+      </c>
+      <c r="G1278" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1279" s="1" t="s">
+        <v>6243</v>
+      </c>
+      <c r="B1279" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1279" s="1" t="s">
+        <v>6321</v>
+      </c>
+      <c r="D1279" s="1" t="s">
+        <v>6322</v>
+      </c>
+      <c r="E1279" s="1" t="s">
+        <v>6323</v>
+      </c>
+      <c r="F1279" s="1" t="s">
+        <v>6324</v>
+      </c>
+      <c r="G1279" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1280" s="1" t="s">
+        <v>6244</v>
+      </c>
+      <c r="B1280" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1280" s="1" t="s">
+        <v>6325</v>
+      </c>
+      <c r="D1280" s="1" t="s">
+        <v>6326</v>
+      </c>
+      <c r="E1280" s="1" t="s">
+        <v>6327</v>
+      </c>
+      <c r="F1280" s="1" t="s">
+        <v>6328</v>
+      </c>
+      <c r="G1280" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1281" s="1" t="s">
+        <v>6245</v>
+      </c>
+      <c r="B1281" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1281" s="1" t="s">
+        <v>6329</v>
+      </c>
+      <c r="D1281" s="1" t="s">
+        <v>6330</v>
+      </c>
+      <c r="E1281" s="1" t="s">
+        <v>6331</v>
+      </c>
+      <c r="F1281" s="1" t="s">
+        <v>6332</v>
+      </c>
+      <c r="G1281" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1282" s="1" t="s">
+        <v>6246</v>
+      </c>
+      <c r="B1282" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1282" s="1" t="s">
+        <v>6333</v>
+      </c>
+      <c r="D1282" s="1" t="s">
+        <v>6334</v>
+      </c>
+      <c r="E1282" s="1" t="s">
+        <v>6335</v>
+      </c>
+      <c r="F1282" s="1" t="s">
+        <v>6336</v>
+      </c>
+      <c r="G1282" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1283" s="1" t="s">
+        <v>6247</v>
+      </c>
+      <c r="B1283" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1283" s="1" t="s">
+        <v>6337</v>
+      </c>
+      <c r="D1283" s="1" t="s">
+        <v>6338</v>
+      </c>
+      <c r="E1283" s="1" t="s">
+        <v>6339</v>
+      </c>
+      <c r="F1283" s="1" t="s">
+        <v>6340</v>
+      </c>
+      <c r="G1283" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1284" s="1" t="s">
+        <v>6248</v>
+      </c>
+      <c r="B1284" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1284" s="1" t="s">
+        <v>6341</v>
+      </c>
+      <c r="D1284" s="1" t="s">
+        <v>6342</v>
+      </c>
+      <c r="E1284" s="1" t="s">
+        <v>6343</v>
+      </c>
+      <c r="F1284" s="1" t="s">
+        <v>6344</v>
+      </c>
+      <c r="G1284" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1285" s="1" t="s">
+        <v>6249</v>
+      </c>
+      <c r="B1285" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1285" s="1" t="s">
+        <v>6345</v>
+      </c>
+      <c r="D1285" s="1" t="s">
+        <v>6346</v>
+      </c>
+      <c r="E1285" s="1" t="s">
+        <v>6347</v>
+      </c>
+      <c r="F1285" s="1" t="s">
+        <v>6348</v>
+      </c>
+      <c r="G1285" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1286" s="1" t="s">
+        <v>6250</v>
+      </c>
+      <c r="B1286" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1286" s="1" t="s">
+        <v>6349</v>
+      </c>
+      <c r="D1286" s="1" t="s">
+        <v>6350</v>
+      </c>
+      <c r="E1286" s="1" t="s">
+        <v>6351</v>
+      </c>
+      <c r="F1286" s="1" t="s">
+        <v>6352</v>
+      </c>
+      <c r="G1286" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1287" s="1" t="s">
+        <v>6251</v>
+      </c>
+      <c r="B1287" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1287" s="1" t="s">
+        <v>6353</v>
+      </c>
+      <c r="D1287" s="1" t="s">
+        <v>6354</v>
+      </c>
+      <c r="E1287" s="1" t="s">
+        <v>6355</v>
+      </c>
+      <c r="F1287" s="1" t="s">
+        <v>6356</v>
+      </c>
+      <c r="G1287" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1288" s="1" t="s">
+        <v>6252</v>
+      </c>
+      <c r="B1288" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1288" s="1" t="s">
+        <v>6357</v>
+      </c>
+      <c r="D1288" s="1" t="s">
+        <v>6358</v>
+      </c>
+      <c r="E1288" s="1" t="s">
+        <v>6359</v>
+      </c>
+      <c r="F1288" s="1" t="s">
+        <v>6360</v>
+      </c>
+      <c r="G1288" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1289" s="1" t="s">
+        <v>6253</v>
+      </c>
+      <c r="B1289" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1289" s="1" t="s">
+        <v>6361</v>
+      </c>
+      <c r="D1289" s="1" t="s">
+        <v>6362</v>
+      </c>
+      <c r="E1289" s="1" t="s">
+        <v>6363</v>
+      </c>
+      <c r="F1289" s="1" t="s">
+        <v>6364</v>
+      </c>
+      <c r="G1289" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1290" s="1" t="s">
+        <v>6254</v>
+      </c>
+      <c r="B1290" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1290" s="1" t="s">
+        <v>6365</v>
+      </c>
+      <c r="D1290" s="1" t="s">
+        <v>6366</v>
+      </c>
+      <c r="E1290" s="1" t="s">
+        <v>6367</v>
+      </c>
+      <c r="F1290" s="1" t="s">
+        <v>6368</v>
+      </c>
+      <c r="G1290" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1291" s="1" t="s">
+        <v>6255</v>
+      </c>
+      <c r="B1291" s="1">
+        <v>43</v>
+      </c>
+      <c r="C1291" s="1" t="s">
+        <v>6369</v>
+      </c>
+      <c r="D1291" s="1" t="s">
+        <v>6370</v>
+      </c>
+      <c r="E1291" s="1" t="s">
+        <v>6371</v>
+      </c>
+      <c r="F1291" s="1" t="s">
+        <v>6372</v>
+      </c>
+      <c r="G1291" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 44
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6588E01F-AEAC-A448-8F0B-8F9E56C7027D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC55A42D-0A78-A54B-AFAC-AD83D98C8486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7594" uniqueCount="6373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7774" uniqueCount="6523">
   <si>
     <t>ID</t>
   </si>
@@ -19149,6 +19149,456 @@
   </si>
   <si>
     <t>throughout the year / suốt cả năm</t>
+  </si>
+  <si>
+    <t>U44_01</t>
+  </si>
+  <si>
+    <t>U44_02</t>
+  </si>
+  <si>
+    <t>U44_03</t>
+  </si>
+  <si>
+    <t>U44_04</t>
+  </si>
+  <si>
+    <t>U44_05</t>
+  </si>
+  <si>
+    <t>U44_06</t>
+  </si>
+  <si>
+    <t>U44_07</t>
+  </si>
+  <si>
+    <t>U44_08</t>
+  </si>
+  <si>
+    <t>U44_09</t>
+  </si>
+  <si>
+    <t>U44_10</t>
+  </si>
+  <si>
+    <t>U44_11</t>
+  </si>
+  <si>
+    <t>U44_12</t>
+  </si>
+  <si>
+    <t>U44_13</t>
+  </si>
+  <si>
+    <t>U44_14</t>
+  </si>
+  <si>
+    <t>U44_15</t>
+  </si>
+  <si>
+    <t>U44_16</t>
+  </si>
+  <si>
+    <t>U44_17</t>
+  </si>
+  <si>
+    <t>U44_18</t>
+  </si>
+  <si>
+    <t>U44_19</t>
+  </si>
+  <si>
+    <t>U44_20</t>
+  </si>
+  <si>
+    <t>U44_21</t>
+  </si>
+  <si>
+    <t>U44_22</t>
+  </si>
+  <si>
+    <t>U44_23</t>
+  </si>
+  <si>
+    <t>U44_24</t>
+  </si>
+  <si>
+    <t>U44_25</t>
+  </si>
+  <si>
+    <t>U44_26</t>
+  </si>
+  <si>
+    <t>U44_27</t>
+  </si>
+  <si>
+    <t>U44_28</t>
+  </si>
+  <si>
+    <t>U44_29</t>
+  </si>
+  <si>
+    <t>U44_30</t>
+  </si>
+  <si>
+    <t>Thuộc kinh tế</t>
+  </si>
+  <si>
+    <t>Economic</t>
+  </si>
+  <si>
+    <t>Economic growth is projected to be high (dự báo tăng trưởng kinh tế cao)</t>
+  </si>
+  <si>
+    <t>economic growth</t>
+  </si>
+  <si>
+    <t>Tài chính</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>I need financial support from you</t>
+  </si>
+  <si>
+    <t>Financial support</t>
+  </si>
+  <si>
+    <t>Tiền mặt</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Can I pay in cash</t>
+  </si>
+  <si>
+    <t>in cash / bằng tiền mặt</t>
+  </si>
+  <si>
+    <t>cổ phiếu</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>You need to research before investing in stock</t>
+  </si>
+  <si>
+    <t>invest in stocks / đầu tư vào cổ phiếu</t>
+  </si>
+  <si>
+    <t>Sự đầu tư</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>My parents made a large investment in me</t>
+  </si>
+  <si>
+    <t>make an investment / đầu tư</t>
+  </si>
+  <si>
+    <t>Ngành công nghiệp</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>We should network more within the industry</t>
+  </si>
+  <si>
+    <t>within an industry / trong ngành</t>
+  </si>
+  <si>
+    <t>Thành lập, thiết lập</t>
+  </si>
+  <si>
+    <t>Set up</t>
+  </si>
+  <si>
+    <t>How do I set up an account on this site?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set up an account </t>
+  </si>
+  <si>
+    <t>Giao dịch</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>They refuse (từ chối) to trade stock with our company</t>
+  </si>
+  <si>
+    <t>trade stock / giao dịch chứng khoán</t>
+  </si>
+  <si>
+    <t>Kiếm tiền</t>
+  </si>
+  <si>
+    <t>Earn</t>
+  </si>
+  <si>
+    <t>He earns a living as a dentist</t>
+  </si>
+  <si>
+    <t>Earn a living / kiếm sống</t>
+  </si>
+  <si>
+    <t>Lợi nhuận</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>The business made a huge profit last year</t>
+  </si>
+  <si>
+    <t>make a profit / tạo ra lợi nhuận</t>
+  </si>
+  <si>
+    <t>Nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Japan is a leading supplier of salmon</t>
+  </si>
+  <si>
+    <t>a leading supplier / nhà cung cấp hàng đầu</t>
+  </si>
+  <si>
+    <t>Đạt được, có được</t>
+  </si>
+  <si>
+    <t>Obtain</t>
+  </si>
+  <si>
+    <t>After paying the fee, I will obtain a new tourist visa.</t>
+  </si>
+  <si>
+    <t>obtain something / có được một cái gì đó</t>
+  </si>
+  <si>
+    <t>Dự định, mục tiêu</t>
+  </si>
+  <si>
+    <t>Aim</t>
+  </si>
+  <si>
+    <t>I exercise a lot with the aim to lose weight.</t>
+  </si>
+  <si>
+    <t>with the aim / với mục tiêu</t>
+  </si>
+  <si>
+    <t>Phần trăm</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>The percentage of your grade is 20%</t>
+  </si>
+  <si>
+    <t>percentage of something / tỷ lệ phần trăm của something</t>
+  </si>
+  <si>
+    <t>Giấy phép</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>You need a license to drive cars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">license to do something </t>
+  </si>
+  <si>
+    <t>Sự thiếu hụt</t>
+  </si>
+  <si>
+    <t>Shortage</t>
+  </si>
+  <si>
+    <t>There is no shortage of food during Tet.</t>
+  </si>
+  <si>
+    <t>a shortage of food / tình trạng thiếu lương thực</t>
+  </si>
+  <si>
+    <t>Đóng góp</t>
+  </si>
+  <si>
+    <t>Contribute</t>
+  </si>
+  <si>
+    <t>We all contribute towards economic growth.</t>
+  </si>
+  <si>
+    <t>Contribute to/towards something (đóng góp vào một cái gì đó)</t>
+  </si>
+  <si>
+    <t>Thử nghiệm</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Scientists conduct experiments regularly</t>
+  </si>
+  <si>
+    <t>conduct an experiment / tiến hành thí nghiệm</t>
+  </si>
+  <si>
+    <t>Trận chiến, trận đấu</t>
+  </si>
+  <si>
+    <t>Battle</t>
+  </si>
+  <si>
+    <t>The battle between the fighters(võ sĩ) is on tonight</t>
+  </si>
+  <si>
+    <t>Battle between A and B / trận đấu giữa A và B</t>
+  </si>
+  <si>
+    <t>Điều khoản</t>
+  </si>
+  <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>Read the terms and conditions carefully</t>
+  </si>
+  <si>
+    <t>terms and conditions / các điều khoản và điều kiện</t>
+  </si>
+  <si>
+    <t>Hàng hóa</t>
+  </si>
+  <si>
+    <t>Goods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The store sells luxury goods </t>
+  </si>
+  <si>
+    <t>Luxury goods / hàng hóa cao cấp</t>
+  </si>
+  <si>
+    <t>Hiếm</t>
+  </si>
+  <si>
+    <t>Scarce</t>
+  </si>
+  <si>
+    <t>Scarce resources prevent us from continuing</t>
+  </si>
+  <si>
+    <t>scarce resources / Tài nguyên khan hiếm</t>
+  </si>
+  <si>
+    <t>Mở rộng</t>
+  </si>
+  <si>
+    <t>Extend</t>
+  </si>
+  <si>
+    <t>Can you extend the deadline?</t>
+  </si>
+  <si>
+    <t>Extend the deadline / gia hạn hạn chót</t>
+  </si>
+  <si>
+    <t>Khu vực</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Here is the latest news from the Southeast Asian region</t>
+  </si>
+  <si>
+    <t>from the region / từ khu vực</t>
+  </si>
+  <si>
+    <t>Lãnh đạo</t>
+  </si>
+  <si>
+    <t>Leader</t>
+  </si>
+  <si>
+    <t>A world leader / nhà lãnh đạo thế giới</t>
+  </si>
+  <si>
+    <t>World leaders will discuss this in the upcoming conference. / Các nhà lãnh đạo thế giới sẽ thảo luận vấn đề này trong hội nghị sắp tới</t>
+  </si>
+  <si>
+    <t>Trả hết nợ</t>
+  </si>
+  <si>
+    <t>Pay off</t>
+  </si>
+  <si>
+    <t>Can you pay off the debt?</t>
+  </si>
+  <si>
+    <t>pay of the debt / trả hết nợ</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Quy mô</t>
+  </si>
+  <si>
+    <t>We are distributing(đang phân phối) on a large scale</t>
+  </si>
+  <si>
+    <t>on a large scale / trên một quy mô lớn</t>
+  </si>
+  <si>
+    <t>Tiền tệ</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>In VN, US dollar is a foreign currency.</t>
+  </si>
+  <si>
+    <t>foreign currency / ngoại tệ</t>
+  </si>
+  <si>
+    <t>Thuế</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>There is a tax on buying products</t>
+  </si>
+  <si>
+    <t>tax on something / thuế cho một thứ gì đó</t>
+  </si>
+  <si>
+    <t>Nhấn mạnh</t>
+  </si>
+  <si>
+    <t>Emphasize</t>
+  </si>
+  <si>
+    <t>Emphasize something / nhấn mạnh một cái gì đó</t>
+  </si>
+  <si>
+    <t>The writer emphasized the bravery (quả cảm) of his characters</t>
   </si>
 </sst>
 </file>
@@ -19514,10 +19964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1291"/>
+  <dimension ref="A1:G1321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1172" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1292" sqref="C1292"/>
+    <sheetView tabSelected="1" topLeftCell="A1301" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A1322" sqref="A1322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -48765,6 +49215,696 @@
         <v>720</v>
       </c>
     </row>
+    <row r="1292" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1292" s="1" t="s">
+        <v>6373</v>
+      </c>
+      <c r="B1292" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1292" s="1" t="s">
+        <v>6403</v>
+      </c>
+      <c r="D1292" s="1" t="s">
+        <v>6404</v>
+      </c>
+      <c r="E1292" s="1" t="s">
+        <v>6405</v>
+      </c>
+      <c r="F1292" s="1" t="s">
+        <v>6406</v>
+      </c>
+      <c r="G1292" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1293" s="1" t="s">
+        <v>6374</v>
+      </c>
+      <c r="B1293" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1293" s="1" t="s">
+        <v>6407</v>
+      </c>
+      <c r="D1293" s="1" t="s">
+        <v>6408</v>
+      </c>
+      <c r="E1293" s="1" t="s">
+        <v>6409</v>
+      </c>
+      <c r="F1293" s="1" t="s">
+        <v>6410</v>
+      </c>
+      <c r="G1293" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1294" s="1" t="s">
+        <v>6375</v>
+      </c>
+      <c r="B1294" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1294" s="1" t="s">
+        <v>6411</v>
+      </c>
+      <c r="D1294" s="1" t="s">
+        <v>6412</v>
+      </c>
+      <c r="E1294" s="1" t="s">
+        <v>6413</v>
+      </c>
+      <c r="F1294" s="1" t="s">
+        <v>6414</v>
+      </c>
+      <c r="G1294" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1295" s="1" t="s">
+        <v>6376</v>
+      </c>
+      <c r="B1295" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1295" s="1" t="s">
+        <v>6415</v>
+      </c>
+      <c r="D1295" s="1" t="s">
+        <v>6416</v>
+      </c>
+      <c r="E1295" s="1" t="s">
+        <v>6417</v>
+      </c>
+      <c r="F1295" s="1" t="s">
+        <v>6418</v>
+      </c>
+      <c r="G1295" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1296" s="1" t="s">
+        <v>6377</v>
+      </c>
+      <c r="B1296" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1296" s="1" t="s">
+        <v>6419</v>
+      </c>
+      <c r="D1296" s="1" t="s">
+        <v>6420</v>
+      </c>
+      <c r="E1296" s="1" t="s">
+        <v>6421</v>
+      </c>
+      <c r="F1296" s="1" t="s">
+        <v>6422</v>
+      </c>
+      <c r="G1296" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1297" s="1" t="s">
+        <v>6378</v>
+      </c>
+      <c r="B1297" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1297" s="1" t="s">
+        <v>6423</v>
+      </c>
+      <c r="D1297" s="1" t="s">
+        <v>6424</v>
+      </c>
+      <c r="E1297" s="1" t="s">
+        <v>6425</v>
+      </c>
+      <c r="F1297" s="1" t="s">
+        <v>6426</v>
+      </c>
+      <c r="G1297" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1298" s="1" t="s">
+        <v>6379</v>
+      </c>
+      <c r="B1298" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1298" s="1" t="s">
+        <v>6427</v>
+      </c>
+      <c r="D1298" s="1" t="s">
+        <v>6428</v>
+      </c>
+      <c r="E1298" s="1" t="s">
+        <v>6429</v>
+      </c>
+      <c r="F1298" s="1" t="s">
+        <v>6430</v>
+      </c>
+      <c r="G1298" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1299" s="1" t="s">
+        <v>6380</v>
+      </c>
+      <c r="B1299" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1299" s="1" t="s">
+        <v>6431</v>
+      </c>
+      <c r="D1299" s="1" t="s">
+        <v>6432</v>
+      </c>
+      <c r="E1299" s="1" t="s">
+        <v>6433</v>
+      </c>
+      <c r="F1299" s="1" t="s">
+        <v>6434</v>
+      </c>
+      <c r="G1299" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1300" s="1" t="s">
+        <v>6381</v>
+      </c>
+      <c r="B1300" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1300" s="1" t="s">
+        <v>6435</v>
+      </c>
+      <c r="D1300" s="1" t="s">
+        <v>6436</v>
+      </c>
+      <c r="E1300" s="1" t="s">
+        <v>6437</v>
+      </c>
+      <c r="F1300" s="1" t="s">
+        <v>6438</v>
+      </c>
+      <c r="G1300" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1301" s="1" t="s">
+        <v>6382</v>
+      </c>
+      <c r="B1301" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1301" s="1" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D1301" s="1" t="s">
+        <v>6440</v>
+      </c>
+      <c r="E1301" s="1" t="s">
+        <v>6441</v>
+      </c>
+      <c r="F1301" s="1" t="s">
+        <v>6442</v>
+      </c>
+      <c r="G1301" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1302" s="1" t="s">
+        <v>6383</v>
+      </c>
+      <c r="B1302" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1302" s="1" t="s">
+        <v>6443</v>
+      </c>
+      <c r="D1302" s="1" t="s">
+        <v>6444</v>
+      </c>
+      <c r="E1302" s="1" t="s">
+        <v>6445</v>
+      </c>
+      <c r="F1302" s="1" t="s">
+        <v>6446</v>
+      </c>
+      <c r="G1302" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1303" s="1" t="s">
+        <v>6384</v>
+      </c>
+      <c r="B1303" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1303" s="1" t="s">
+        <v>6447</v>
+      </c>
+      <c r="D1303" s="1" t="s">
+        <v>6448</v>
+      </c>
+      <c r="E1303" s="1" t="s">
+        <v>6449</v>
+      </c>
+      <c r="F1303" s="1" t="s">
+        <v>6450</v>
+      </c>
+      <c r="G1303" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1304" s="1" t="s">
+        <v>6385</v>
+      </c>
+      <c r="B1304" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1304" s="1" t="s">
+        <v>6451</v>
+      </c>
+      <c r="D1304" s="1" t="s">
+        <v>6452</v>
+      </c>
+      <c r="E1304" s="1" t="s">
+        <v>6453</v>
+      </c>
+      <c r="F1304" s="1" t="s">
+        <v>6454</v>
+      </c>
+      <c r="G1304" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1305" s="1" t="s">
+        <v>6386</v>
+      </c>
+      <c r="B1305" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1305" s="1" t="s">
+        <v>6455</v>
+      </c>
+      <c r="D1305" s="1" t="s">
+        <v>6456</v>
+      </c>
+      <c r="E1305" s="1" t="s">
+        <v>6457</v>
+      </c>
+      <c r="F1305" s="1" t="s">
+        <v>6458</v>
+      </c>
+      <c r="G1305" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1306" s="1" t="s">
+        <v>6387</v>
+      </c>
+      <c r="B1306" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1306" s="1" t="s">
+        <v>6459</v>
+      </c>
+      <c r="D1306" s="1" t="s">
+        <v>6460</v>
+      </c>
+      <c r="E1306" s="1" t="s">
+        <v>6461</v>
+      </c>
+      <c r="F1306" s="1" t="s">
+        <v>6462</v>
+      </c>
+      <c r="G1306" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1307" s="1" t="s">
+        <v>6388</v>
+      </c>
+      <c r="B1307" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1307" s="1" t="s">
+        <v>6463</v>
+      </c>
+      <c r="D1307" s="1" t="s">
+        <v>6464</v>
+      </c>
+      <c r="E1307" s="1" t="s">
+        <v>6465</v>
+      </c>
+      <c r="F1307" s="1" t="s">
+        <v>6466</v>
+      </c>
+      <c r="G1307" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1308" s="1" t="s">
+        <v>6389</v>
+      </c>
+      <c r="B1308" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1308" s="1" t="s">
+        <v>6467</v>
+      </c>
+      <c r="D1308" s="1" t="s">
+        <v>6468</v>
+      </c>
+      <c r="E1308" s="1" t="s">
+        <v>6469</v>
+      </c>
+      <c r="F1308" s="1" t="s">
+        <v>6470</v>
+      </c>
+      <c r="G1308" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1309" s="1" t="s">
+        <v>6390</v>
+      </c>
+      <c r="B1309" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1309" s="1" t="s">
+        <v>6471</v>
+      </c>
+      <c r="D1309" s="1" t="s">
+        <v>6472</v>
+      </c>
+      <c r="E1309" s="1" t="s">
+        <v>6473</v>
+      </c>
+      <c r="F1309" s="1" t="s">
+        <v>6474</v>
+      </c>
+      <c r="G1309" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1310" s="1" t="s">
+        <v>6391</v>
+      </c>
+      <c r="B1310" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1310" s="1" t="s">
+        <v>6475</v>
+      </c>
+      <c r="D1310" s="1" t="s">
+        <v>6476</v>
+      </c>
+      <c r="E1310" s="1" t="s">
+        <v>6477</v>
+      </c>
+      <c r="F1310" s="1" t="s">
+        <v>6478</v>
+      </c>
+      <c r="G1310" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1311" s="1" t="s">
+        <v>6392</v>
+      </c>
+      <c r="B1311" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1311" s="1" t="s">
+        <v>6479</v>
+      </c>
+      <c r="D1311" s="1" t="s">
+        <v>6480</v>
+      </c>
+      <c r="E1311" s="1" t="s">
+        <v>6481</v>
+      </c>
+      <c r="F1311" s="1" t="s">
+        <v>6482</v>
+      </c>
+      <c r="G1311" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1312" s="1" t="s">
+        <v>6393</v>
+      </c>
+      <c r="B1312" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1312" s="1" t="s">
+        <v>6483</v>
+      </c>
+      <c r="D1312" s="1" t="s">
+        <v>6484</v>
+      </c>
+      <c r="E1312" s="1" t="s">
+        <v>6485</v>
+      </c>
+      <c r="F1312" s="1" t="s">
+        <v>6486</v>
+      </c>
+      <c r="G1312" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1313" s="1" t="s">
+        <v>6394</v>
+      </c>
+      <c r="B1313" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1313" s="1" t="s">
+        <v>6487</v>
+      </c>
+      <c r="D1313" s="1" t="s">
+        <v>6488</v>
+      </c>
+      <c r="E1313" s="1" t="s">
+        <v>6489</v>
+      </c>
+      <c r="F1313" s="1" t="s">
+        <v>6490</v>
+      </c>
+      <c r="G1313" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1314" s="1" t="s">
+        <v>6395</v>
+      </c>
+      <c r="B1314" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1314" s="1" t="s">
+        <v>6491</v>
+      </c>
+      <c r="D1314" s="1" t="s">
+        <v>6492</v>
+      </c>
+      <c r="E1314" s="1" t="s">
+        <v>6493</v>
+      </c>
+      <c r="F1314" s="1" t="s">
+        <v>6494</v>
+      </c>
+      <c r="G1314" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1315" s="1" t="s">
+        <v>6396</v>
+      </c>
+      <c r="B1315" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1315" s="1" t="s">
+        <v>6495</v>
+      </c>
+      <c r="D1315" s="1" t="s">
+        <v>6496</v>
+      </c>
+      <c r="E1315" s="1" t="s">
+        <v>6497</v>
+      </c>
+      <c r="F1315" s="1" t="s">
+        <v>6498</v>
+      </c>
+      <c r="G1315" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1316" s="1" t="s">
+        <v>6397</v>
+      </c>
+      <c r="B1316" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1316" s="1" t="s">
+        <v>6499</v>
+      </c>
+      <c r="D1316" s="1" t="s">
+        <v>6500</v>
+      </c>
+      <c r="E1316" s="1" t="s">
+        <v>6502</v>
+      </c>
+      <c r="F1316" s="1" t="s">
+        <v>6501</v>
+      </c>
+      <c r="G1316" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1317" s="1" t="s">
+        <v>6398</v>
+      </c>
+      <c r="B1317" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1317" s="1" t="s">
+        <v>6503</v>
+      </c>
+      <c r="D1317" s="1" t="s">
+        <v>6504</v>
+      </c>
+      <c r="E1317" s="1" t="s">
+        <v>6505</v>
+      </c>
+      <c r="F1317" s="1" t="s">
+        <v>6506</v>
+      </c>
+      <c r="G1317" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1318" s="1" t="s">
+        <v>6399</v>
+      </c>
+      <c r="B1318" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1318" s="1" t="s">
+        <v>6508</v>
+      </c>
+      <c r="D1318" s="1" t="s">
+        <v>6507</v>
+      </c>
+      <c r="E1318" s="1" t="s">
+        <v>6509</v>
+      </c>
+      <c r="F1318" s="1" t="s">
+        <v>6510</v>
+      </c>
+      <c r="G1318" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1319" s="1" t="s">
+        <v>6400</v>
+      </c>
+      <c r="B1319" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1319" s="1" t="s">
+        <v>6511</v>
+      </c>
+      <c r="D1319" s="1" t="s">
+        <v>6512</v>
+      </c>
+      <c r="E1319" s="1" t="s">
+        <v>6513</v>
+      </c>
+      <c r="F1319" s="1" t="s">
+        <v>6514</v>
+      </c>
+      <c r="G1319" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1320" s="1" t="s">
+        <v>6401</v>
+      </c>
+      <c r="B1320" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1320" s="1" t="s">
+        <v>6515</v>
+      </c>
+      <c r="D1320" s="1" t="s">
+        <v>6516</v>
+      </c>
+      <c r="E1320" s="1" t="s">
+        <v>6517</v>
+      </c>
+      <c r="F1320" s="1" t="s">
+        <v>6518</v>
+      </c>
+      <c r="G1320" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1321" s="1" t="s">
+        <v>6402</v>
+      </c>
+      <c r="B1321" s="1">
+        <v>44</v>
+      </c>
+      <c r="C1321" s="1" t="s">
+        <v>6519</v>
+      </c>
+      <c r="D1321" s="1" t="s">
+        <v>6520</v>
+      </c>
+      <c r="E1321" s="1" t="s">
+        <v>6522</v>
+      </c>
+      <c r="F1321" s="1" t="s">
+        <v>6521</v>
+      </c>
+      <c r="G1321" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 45
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC55A42D-0A78-A54B-AFAC-AD83D98C8486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2167D193-57FF-7249-86D6-6051FE478E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7774" uniqueCount="6523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7954" uniqueCount="6669">
   <si>
     <t>ID</t>
   </si>
@@ -19599,6 +19599,444 @@
   </si>
   <si>
     <t>The writer emphasized the bravery (quả cảm) of his characters</t>
+  </si>
+  <si>
+    <t>U45_01</t>
+  </si>
+  <si>
+    <t>U45_02</t>
+  </si>
+  <si>
+    <t>U45_03</t>
+  </si>
+  <si>
+    <t>U45_04</t>
+  </si>
+  <si>
+    <t>U45_05</t>
+  </si>
+  <si>
+    <t>U45_06</t>
+  </si>
+  <si>
+    <t>U45_07</t>
+  </si>
+  <si>
+    <t>U45_08</t>
+  </si>
+  <si>
+    <t>U45_09</t>
+  </si>
+  <si>
+    <t>U45_10</t>
+  </si>
+  <si>
+    <t>U45_11</t>
+  </si>
+  <si>
+    <t>U45_12</t>
+  </si>
+  <si>
+    <t>U45_13</t>
+  </si>
+  <si>
+    <t>U45_14</t>
+  </si>
+  <si>
+    <t>U45_15</t>
+  </si>
+  <si>
+    <t>U45_16</t>
+  </si>
+  <si>
+    <t>U45_17</t>
+  </si>
+  <si>
+    <t>U45_18</t>
+  </si>
+  <si>
+    <t>U45_19</t>
+  </si>
+  <si>
+    <t>U45_20</t>
+  </si>
+  <si>
+    <t>U45_21</t>
+  </si>
+  <si>
+    <t>U45_22</t>
+  </si>
+  <si>
+    <t>U45_23</t>
+  </si>
+  <si>
+    <t>U45_24</t>
+  </si>
+  <si>
+    <t>U45_25</t>
+  </si>
+  <si>
+    <t>U45_26</t>
+  </si>
+  <si>
+    <t>U45_27</t>
+  </si>
+  <si>
+    <t>U45_28</t>
+  </si>
+  <si>
+    <t>U45_29</t>
+  </si>
+  <si>
+    <t>U45_30</t>
+  </si>
+  <si>
+    <t>Cảm nhận, cảm giác</t>
+  </si>
+  <si>
+    <t>Sense</t>
+  </si>
+  <si>
+    <t>Success gave me a sense of happiness</t>
+  </si>
+  <si>
+    <t>a sense of something</t>
+  </si>
+  <si>
+    <t>Quan điểm</t>
+  </si>
+  <si>
+    <t>Opinion</t>
+  </si>
+  <si>
+    <t>He has opinions about everything</t>
+  </si>
+  <si>
+    <t>have an opinion about something</t>
+  </si>
+  <si>
+    <t>Hữu ích</t>
+  </si>
+  <si>
+    <t>Useful</t>
+  </si>
+  <si>
+    <t>Your insight (hiểu biết của cậu) was useful for my research</t>
+  </si>
+  <si>
+    <t>useful for somebody or something</t>
+  </si>
+  <si>
+    <t>Có lẽ</t>
+  </si>
+  <si>
+    <t>Perhaps</t>
+  </si>
+  <si>
+    <t>Perhaps we should tell him the truth</t>
+  </si>
+  <si>
+    <t>Perhaps somebody should do something</t>
+  </si>
+  <si>
+    <t>Definitely</t>
+  </si>
+  <si>
+    <t>This is definitely not her first time lying.</t>
+  </si>
+  <si>
+    <t>definitely not / chắc chắn không phải</t>
+  </si>
+  <si>
+    <t>Sự thật</t>
+  </si>
+  <si>
+    <t>Truth</t>
+  </si>
+  <si>
+    <t>The truth is, I lied to you</t>
+  </si>
+  <si>
+    <t>the truth is / sự thật là</t>
+  </si>
+  <si>
+    <t>Bình luận</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Please leave a comment if you have any questions</t>
+  </si>
+  <si>
+    <t>leave a comment / để lại bình luận</t>
+  </si>
+  <si>
+    <t>Tin</t>
+  </si>
+  <si>
+    <t>Believe</t>
+  </si>
+  <si>
+    <t>Do you believe in me</t>
+  </si>
+  <si>
+    <t>believe in somebody / tin vào ai đó</t>
+  </si>
+  <si>
+    <t>Totally</t>
+  </si>
+  <si>
+    <t>What you said was totally unacceptable</t>
+  </si>
+  <si>
+    <t>totally unacceptable / hoàn toàn không thể chấp nhận được</t>
+  </si>
+  <si>
+    <t>Thấy phiền</t>
+  </si>
+  <si>
+    <t>Mind</t>
+  </si>
+  <si>
+    <t>Would you mind if I ask you something?</t>
+  </si>
+  <si>
+    <t>would you mind / bạn có phiền</t>
+  </si>
+  <si>
+    <t>Sự tự do</t>
+  </si>
+  <si>
+    <t>Freedom</t>
+  </si>
+  <si>
+    <t>Children need the freedom to make mistakes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freedom to do something </t>
+  </si>
+  <si>
+    <t>Lý lẽ, cuộc tranh cãi</t>
+  </si>
+  <si>
+    <t>Argument</t>
+  </si>
+  <si>
+    <t>I had an argument with her yesterday</t>
+  </si>
+  <si>
+    <t>an argument with somebody / một cuộc tranh luận với ai đó</t>
+  </si>
+  <si>
+    <t>Cuộc tranh biện</t>
+  </si>
+  <si>
+    <t>debate</t>
+  </si>
+  <si>
+    <t>We were having a debate on justice (công lý)</t>
+  </si>
+  <si>
+    <t>a debate on something</t>
+  </si>
+  <si>
+    <t>Dường như</t>
+  </si>
+  <si>
+    <t>Seem</t>
+  </si>
+  <si>
+    <t>They seem to be scared at first (lúc đầu họ dường như là bị sợ sệt)</t>
+  </si>
+  <si>
+    <t>seem to be / dường như là</t>
+  </si>
+  <si>
+    <t>Sự lựa chọn</t>
+  </si>
+  <si>
+    <t>Choice</t>
+  </si>
+  <si>
+    <t>Make a choice between apples and oranges</t>
+  </si>
+  <si>
+    <t>choice between A and B</t>
+  </si>
+  <si>
+    <t>Đồng ý</t>
+  </si>
+  <si>
+    <t>Agree</t>
+  </si>
+  <si>
+    <t>I agree with her on moving forward (tiếp tục triển khai)</t>
+  </si>
+  <si>
+    <t>agree with somebody</t>
+  </si>
+  <si>
+    <t>Thực tế</t>
+  </si>
+  <si>
+    <t>Realistic</t>
+  </si>
+  <si>
+    <t>Be realistic about your expectations / Hãy thực tế về những sự kỳ vọng của mình</t>
+  </si>
+  <si>
+    <t>To be realistic about something</t>
+  </si>
+  <si>
+    <t>Divide</t>
+  </si>
+  <si>
+    <t>Divide the apples into 4 servings (phần)</t>
+  </si>
+  <si>
+    <t>divide into something / chia thành cái gì đó</t>
+  </si>
+  <si>
+    <t>fair</t>
+  </si>
+  <si>
+    <t>Công bằng</t>
+  </si>
+  <si>
+    <t>My teacher is fair to all students</t>
+  </si>
+  <si>
+    <t>to be fair to somebody / công bằng với ai đó</t>
+  </si>
+  <si>
+    <t>Nhân chứng</t>
+  </si>
+  <si>
+    <t>Witness</t>
+  </si>
+  <si>
+    <t>I was a witness to his crime</t>
+  </si>
+  <si>
+    <t>a witness to something</t>
+  </si>
+  <si>
+    <t>Phiên bản</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Here is the latest version of the iPhone.</t>
+  </si>
+  <si>
+    <t>version of something</t>
+  </si>
+  <si>
+    <t>Lời tuyên bố</t>
+  </si>
+  <si>
+    <t>statement</t>
+  </si>
+  <si>
+    <t>The film was a statement about fairness.</t>
+  </si>
+  <si>
+    <t>statement about something</t>
+  </si>
+  <si>
+    <t>Về mặt cá nhân</t>
+  </si>
+  <si>
+    <t>Personally</t>
+  </si>
+  <si>
+    <t>Personally speaking, I feel offended by the question (câu hỏi có phần xúc phạm)</t>
+  </si>
+  <si>
+    <t>personally speaking / về mặt cá nhân mà nói</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>From my point of view, you seem nice</t>
+  </si>
+  <si>
+    <t>from my point of view / theo quan điểm của tôi</t>
+  </si>
+  <si>
+    <t>Lý thuyết</t>
+  </si>
+  <si>
+    <t>Theory</t>
+  </si>
+  <si>
+    <t>Hawking discovered the theory of black holes</t>
+  </si>
+  <si>
+    <t>Theory of something</t>
+  </si>
+  <si>
+    <t>Cho là, tự nhận là</t>
+  </si>
+  <si>
+    <t>Claim</t>
+  </si>
+  <si>
+    <t>He claims to be an honest man</t>
+  </si>
+  <si>
+    <t>claim to be something</t>
+  </si>
+  <si>
+    <t>Lạc quan</t>
+  </si>
+  <si>
+    <t>Optimistic</t>
+  </si>
+  <si>
+    <t>We are optimistic about the future</t>
+  </si>
+  <si>
+    <t>optimistic about something</t>
+  </si>
+  <si>
+    <t>Khá</t>
+  </si>
+  <si>
+    <t>Quite</t>
+  </si>
+  <si>
+    <t>quite good/ khá tốt, khá ngon</t>
+  </si>
+  <si>
+    <t>Đáng kinh ngạc, khó tin</t>
+  </si>
+  <si>
+    <t>Incredible</t>
+  </si>
+  <si>
+    <t>He told us an incredible story</t>
+  </si>
+  <si>
+    <t>an incredible story</t>
+  </si>
+  <si>
+    <t>Sự đồng cảm</t>
+  </si>
+  <si>
+    <t>Sympathy</t>
+  </si>
+  <si>
+    <t>Have sympathy for her loss (sự mất mát của cô ấy)</t>
+  </si>
+  <si>
+    <t>Have sympathy for somebody</t>
+  </si>
+  <si>
+    <t>The meal was quired good</t>
   </si>
 </sst>
 </file>
@@ -19964,10 +20402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1321"/>
+  <dimension ref="A1:G1351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1301" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A1322" sqref="A1322"/>
+    <sheetView tabSelected="1" topLeftCell="A1341" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E1350" sqref="E1350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -49905,6 +50343,696 @@
         <v>577</v>
       </c>
     </row>
+    <row r="1322" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1322" s="1" t="s">
+        <v>6523</v>
+      </c>
+      <c r="B1322" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1322" s="1" t="s">
+        <v>6553</v>
+      </c>
+      <c r="D1322" s="1" t="s">
+        <v>6554</v>
+      </c>
+      <c r="E1322" s="1" t="s">
+        <v>6555</v>
+      </c>
+      <c r="F1322" s="1" t="s">
+        <v>6556</v>
+      </c>
+      <c r="G1322" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1323" s="1" t="s">
+        <v>6524</v>
+      </c>
+      <c r="B1323" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1323" s="1" t="s">
+        <v>6557</v>
+      </c>
+      <c r="D1323" s="1" t="s">
+        <v>6558</v>
+      </c>
+      <c r="E1323" s="1" t="s">
+        <v>6559</v>
+      </c>
+      <c r="F1323" s="1" t="s">
+        <v>6560</v>
+      </c>
+      <c r="G1323" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1324" s="1" t="s">
+        <v>6525</v>
+      </c>
+      <c r="B1324" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1324" s="1" t="s">
+        <v>6561</v>
+      </c>
+      <c r="D1324" s="1" t="s">
+        <v>6562</v>
+      </c>
+      <c r="E1324" s="1" t="s">
+        <v>6563</v>
+      </c>
+      <c r="F1324" s="1" t="s">
+        <v>6564</v>
+      </c>
+      <c r="G1324" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1325" s="1" t="s">
+        <v>6526</v>
+      </c>
+      <c r="B1325" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1325" s="1" t="s">
+        <v>6565</v>
+      </c>
+      <c r="D1325" s="1" t="s">
+        <v>6566</v>
+      </c>
+      <c r="E1325" s="1" t="s">
+        <v>6567</v>
+      </c>
+      <c r="F1325" s="1" t="s">
+        <v>6568</v>
+      </c>
+      <c r="G1325" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1326" s="1" t="s">
+        <v>6527</v>
+      </c>
+      <c r="B1326" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1326" s="1" t="s">
+        <v>2750</v>
+      </c>
+      <c r="D1326" s="1" t="s">
+        <v>6569</v>
+      </c>
+      <c r="E1326" s="1" t="s">
+        <v>6570</v>
+      </c>
+      <c r="F1326" s="1" t="s">
+        <v>6571</v>
+      </c>
+      <c r="G1326" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1327" s="1" t="s">
+        <v>6528</v>
+      </c>
+      <c r="B1327" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1327" s="1" t="s">
+        <v>6572</v>
+      </c>
+      <c r="D1327" s="1" t="s">
+        <v>6573</v>
+      </c>
+      <c r="E1327" s="1" t="s">
+        <v>6574</v>
+      </c>
+      <c r="F1327" s="1" t="s">
+        <v>6575</v>
+      </c>
+      <c r="G1327" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1328" s="1" t="s">
+        <v>6529</v>
+      </c>
+      <c r="B1328" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1328" s="1" t="s">
+        <v>6576</v>
+      </c>
+      <c r="D1328" s="1" t="s">
+        <v>6577</v>
+      </c>
+      <c r="E1328" s="1" t="s">
+        <v>6578</v>
+      </c>
+      <c r="F1328" s="1" t="s">
+        <v>6579</v>
+      </c>
+      <c r="G1328" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1329" s="1" t="s">
+        <v>6530</v>
+      </c>
+      <c r="B1329" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1329" s="1" t="s">
+        <v>6580</v>
+      </c>
+      <c r="D1329" s="1" t="s">
+        <v>6581</v>
+      </c>
+      <c r="E1329" s="1" t="s">
+        <v>6582</v>
+      </c>
+      <c r="F1329" s="1" t="s">
+        <v>6583</v>
+      </c>
+      <c r="G1329" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1330" s="1" t="s">
+        <v>6531</v>
+      </c>
+      <c r="B1330" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1330" s="1" t="s">
+        <v>6187</v>
+      </c>
+      <c r="D1330" s="1" t="s">
+        <v>6584</v>
+      </c>
+      <c r="E1330" s="1" t="s">
+        <v>6585</v>
+      </c>
+      <c r="F1330" s="1" t="s">
+        <v>6586</v>
+      </c>
+      <c r="G1330" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1331" s="1" t="s">
+        <v>6532</v>
+      </c>
+      <c r="B1331" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1331" s="1" t="s">
+        <v>6587</v>
+      </c>
+      <c r="D1331" s="1" t="s">
+        <v>6588</v>
+      </c>
+      <c r="E1331" s="1" t="s">
+        <v>6589</v>
+      </c>
+      <c r="F1331" s="1" t="s">
+        <v>6590</v>
+      </c>
+      <c r="G1331" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1332" s="1" t="s">
+        <v>6533</v>
+      </c>
+      <c r="B1332" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1332" s="1" t="s">
+        <v>6591</v>
+      </c>
+      <c r="D1332" s="1" t="s">
+        <v>6592</v>
+      </c>
+      <c r="E1332" s="1" t="s">
+        <v>6593</v>
+      </c>
+      <c r="F1332" s="1" t="s">
+        <v>6594</v>
+      </c>
+      <c r="G1332" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1333" s="1" t="s">
+        <v>6534</v>
+      </c>
+      <c r="B1333" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1333" s="1" t="s">
+        <v>6595</v>
+      </c>
+      <c r="D1333" s="1" t="s">
+        <v>6596</v>
+      </c>
+      <c r="E1333" s="1" t="s">
+        <v>6597</v>
+      </c>
+      <c r="F1333" s="1" t="s">
+        <v>6598</v>
+      </c>
+      <c r="G1333" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1334" s="1" t="s">
+        <v>6535</v>
+      </c>
+      <c r="B1334" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1334" s="1" t="s">
+        <v>6599</v>
+      </c>
+      <c r="D1334" s="1" t="s">
+        <v>6600</v>
+      </c>
+      <c r="E1334" s="1" t="s">
+        <v>6601</v>
+      </c>
+      <c r="F1334" s="1" t="s">
+        <v>6602</v>
+      </c>
+      <c r="G1334" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1335" s="1" t="s">
+        <v>6536</v>
+      </c>
+      <c r="B1335" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1335" s="1" t="s">
+        <v>6603</v>
+      </c>
+      <c r="D1335" s="1" t="s">
+        <v>6604</v>
+      </c>
+      <c r="E1335" s="1" t="s">
+        <v>6605</v>
+      </c>
+      <c r="F1335" s="1" t="s">
+        <v>6606</v>
+      </c>
+      <c r="G1335" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1336" s="1" t="s">
+        <v>6537</v>
+      </c>
+      <c r="B1336" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1336" s="1" t="s">
+        <v>6607</v>
+      </c>
+      <c r="D1336" s="1" t="s">
+        <v>6608</v>
+      </c>
+      <c r="E1336" s="1" t="s">
+        <v>6609</v>
+      </c>
+      <c r="F1336" s="1" t="s">
+        <v>6610</v>
+      </c>
+      <c r="G1336" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1337" s="1" t="s">
+        <v>6538</v>
+      </c>
+      <c r="B1337" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1337" s="1" t="s">
+        <v>6611</v>
+      </c>
+      <c r="D1337" s="1" t="s">
+        <v>6612</v>
+      </c>
+      <c r="E1337" s="1" t="s">
+        <v>6613</v>
+      </c>
+      <c r="F1337" s="1" t="s">
+        <v>6614</v>
+      </c>
+      <c r="G1337" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1338" s="1" t="s">
+        <v>6539</v>
+      </c>
+      <c r="B1338" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1338" s="1" t="s">
+        <v>6615</v>
+      </c>
+      <c r="D1338" s="1" t="s">
+        <v>6616</v>
+      </c>
+      <c r="E1338" s="1" t="s">
+        <v>6617</v>
+      </c>
+      <c r="F1338" s="1" t="s">
+        <v>6618</v>
+      </c>
+      <c r="G1338" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1339" s="1" t="s">
+        <v>6540</v>
+      </c>
+      <c r="B1339" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1339" s="1" t="s">
+        <v>2279</v>
+      </c>
+      <c r="D1339" s="1" t="s">
+        <v>6619</v>
+      </c>
+      <c r="E1339" s="1" t="s">
+        <v>6620</v>
+      </c>
+      <c r="F1339" s="1" t="s">
+        <v>6621</v>
+      </c>
+      <c r="G1339" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1340" s="1" t="s">
+        <v>6541</v>
+      </c>
+      <c r="B1340" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1340" s="1" t="s">
+        <v>6623</v>
+      </c>
+      <c r="D1340" s="1" t="s">
+        <v>6622</v>
+      </c>
+      <c r="E1340" s="1" t="s">
+        <v>6624</v>
+      </c>
+      <c r="F1340" s="1" t="s">
+        <v>6625</v>
+      </c>
+      <c r="G1340" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1341" s="1" t="s">
+        <v>6542</v>
+      </c>
+      <c r="B1341" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1341" s="1" t="s">
+        <v>6626</v>
+      </c>
+      <c r="D1341" s="1" t="s">
+        <v>6627</v>
+      </c>
+      <c r="E1341" s="1" t="s">
+        <v>6628</v>
+      </c>
+      <c r="F1341" s="1" t="s">
+        <v>6629</v>
+      </c>
+      <c r="G1341" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1342" s="1" t="s">
+        <v>6543</v>
+      </c>
+      <c r="B1342" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1342" s="1" t="s">
+        <v>6630</v>
+      </c>
+      <c r="D1342" s="1" t="s">
+        <v>6631</v>
+      </c>
+      <c r="E1342" s="1" t="s">
+        <v>6632</v>
+      </c>
+      <c r="F1342" s="1" t="s">
+        <v>6633</v>
+      </c>
+      <c r="G1342" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1343" s="1" t="s">
+        <v>6544</v>
+      </c>
+      <c r="B1343" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1343" s="1" t="s">
+        <v>6634</v>
+      </c>
+      <c r="D1343" s="1" t="s">
+        <v>6635</v>
+      </c>
+      <c r="E1343" s="1" t="s">
+        <v>6636</v>
+      </c>
+      <c r="F1343" s="1" t="s">
+        <v>6637</v>
+      </c>
+      <c r="G1343" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1344" s="1" t="s">
+        <v>6545</v>
+      </c>
+      <c r="B1344" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1344" s="1" t="s">
+        <v>6638</v>
+      </c>
+      <c r="D1344" s="1" t="s">
+        <v>6639</v>
+      </c>
+      <c r="E1344" s="1" t="s">
+        <v>6640</v>
+      </c>
+      <c r="F1344" s="1" t="s">
+        <v>6641</v>
+      </c>
+      <c r="G1344" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1345" s="1" t="s">
+        <v>6546</v>
+      </c>
+      <c r="B1345" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1345" s="1" t="s">
+        <v>6557</v>
+      </c>
+      <c r="D1345" s="1" t="s">
+        <v>6642</v>
+      </c>
+      <c r="E1345" s="1" t="s">
+        <v>6643</v>
+      </c>
+      <c r="F1345" s="1" t="s">
+        <v>6644</v>
+      </c>
+      <c r="G1345" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1346" s="1" t="s">
+        <v>6547</v>
+      </c>
+      <c r="B1346" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1346" s="1" t="s">
+        <v>6645</v>
+      </c>
+      <c r="D1346" s="1" t="s">
+        <v>6646</v>
+      </c>
+      <c r="E1346" s="1" t="s">
+        <v>6647</v>
+      </c>
+      <c r="F1346" s="1" t="s">
+        <v>6648</v>
+      </c>
+      <c r="G1346" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1347" s="1" t="s">
+        <v>6548</v>
+      </c>
+      <c r="B1347" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1347" s="1" t="s">
+        <v>6649</v>
+      </c>
+      <c r="D1347" s="1" t="s">
+        <v>6650</v>
+      </c>
+      <c r="E1347" s="1" t="s">
+        <v>6651</v>
+      </c>
+      <c r="F1347" s="1" t="s">
+        <v>6652</v>
+      </c>
+      <c r="G1347" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1348" s="1" t="s">
+        <v>6549</v>
+      </c>
+      <c r="B1348" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1348" s="1" t="s">
+        <v>6653</v>
+      </c>
+      <c r="D1348" s="1" t="s">
+        <v>6654</v>
+      </c>
+      <c r="E1348" s="1" t="s">
+        <v>6655</v>
+      </c>
+      <c r="F1348" s="1" t="s">
+        <v>6656</v>
+      </c>
+      <c r="G1348" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1349" s="1" t="s">
+        <v>6550</v>
+      </c>
+      <c r="B1349" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1349" s="1" t="s">
+        <v>6657</v>
+      </c>
+      <c r="D1349" s="1" t="s">
+        <v>6658</v>
+      </c>
+      <c r="E1349" s="1" t="s">
+        <v>6668</v>
+      </c>
+      <c r="F1349" s="1" t="s">
+        <v>6659</v>
+      </c>
+      <c r="G1349" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1350" s="1" t="s">
+        <v>6551</v>
+      </c>
+      <c r="B1350" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1350" s="1" t="s">
+        <v>6660</v>
+      </c>
+      <c r="D1350" s="1" t="s">
+        <v>6661</v>
+      </c>
+      <c r="E1350" s="1" t="s">
+        <v>6662</v>
+      </c>
+      <c r="F1350" s="1" t="s">
+        <v>6663</v>
+      </c>
+      <c r="G1350" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1351" s="1" t="s">
+        <v>6552</v>
+      </c>
+      <c r="B1351" s="1">
+        <v>45</v>
+      </c>
+      <c r="C1351" s="1" t="s">
+        <v>6664</v>
+      </c>
+      <c r="D1351" s="1" t="s">
+        <v>6665</v>
+      </c>
+      <c r="E1351" s="1" t="s">
+        <v>6666</v>
+      </c>
+      <c r="F1351" s="1" t="s">
+        <v>6667</v>
+      </c>
+      <c r="G1351" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 46
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2167D193-57FF-7249-86D6-6051FE478E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2C8262-391B-BD41-B3E0-45A25BB761BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7954" uniqueCount="6669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8134" uniqueCount="6816">
   <si>
     <t>ID</t>
   </si>
@@ -20037,6 +20037,447 @@
   </si>
   <si>
     <t>The meal was quired good</t>
+  </si>
+  <si>
+    <t>U46_01</t>
+  </si>
+  <si>
+    <t>U46_02</t>
+  </si>
+  <si>
+    <t>U46_03</t>
+  </si>
+  <si>
+    <t>U46_04</t>
+  </si>
+  <si>
+    <t>U46_05</t>
+  </si>
+  <si>
+    <t>U46_06</t>
+  </si>
+  <si>
+    <t>U46_07</t>
+  </si>
+  <si>
+    <t>U46_08</t>
+  </si>
+  <si>
+    <t>U46_09</t>
+  </si>
+  <si>
+    <t>U46_10</t>
+  </si>
+  <si>
+    <t>U46_11</t>
+  </si>
+  <si>
+    <t>U46_12</t>
+  </si>
+  <si>
+    <t>U46_13</t>
+  </si>
+  <si>
+    <t>U46_14</t>
+  </si>
+  <si>
+    <t>U46_15</t>
+  </si>
+  <si>
+    <t>U46_16</t>
+  </si>
+  <si>
+    <t>U46_17</t>
+  </si>
+  <si>
+    <t>U46_18</t>
+  </si>
+  <si>
+    <t>U46_19</t>
+  </si>
+  <si>
+    <t>U46_20</t>
+  </si>
+  <si>
+    <t>U46_21</t>
+  </si>
+  <si>
+    <t>U46_22</t>
+  </si>
+  <si>
+    <t>U46_23</t>
+  </si>
+  <si>
+    <t>U46_24</t>
+  </si>
+  <si>
+    <t>U46_25</t>
+  </si>
+  <si>
+    <t>U46_26</t>
+  </si>
+  <si>
+    <t>U46_27</t>
+  </si>
+  <si>
+    <t>U46_28</t>
+  </si>
+  <si>
+    <t>U46_29</t>
+  </si>
+  <si>
+    <t>U46_30</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>English is a foreign language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign language </t>
+  </si>
+  <si>
+    <t>Thuộc nước ngoài</t>
+  </si>
+  <si>
+    <t>Foreign</t>
+  </si>
+  <si>
+    <t>We haven't been to foreign countries</t>
+  </si>
+  <si>
+    <t>a foreign country / nước ngoài</t>
+  </si>
+  <si>
+    <t>Hành trình, chuyến đi</t>
+  </si>
+  <si>
+    <t>Journey</t>
+  </si>
+  <si>
+    <t>Take me on a journey with you</t>
+  </si>
+  <si>
+    <t>on a journey</t>
+  </si>
+  <si>
+    <t>Người mới bắt đầu</t>
+  </si>
+  <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>This level is easy for a beginner</t>
+  </si>
+  <si>
+    <t>for a beginner</t>
+  </si>
+  <si>
+    <t>Từ, lời nói</t>
+  </si>
+  <si>
+    <t>My leader has the last word on team decisions (quyết định)</t>
+  </si>
+  <si>
+    <t>have the last word on something / đưa lời nói cuối cùng về việc gì đó</t>
+  </si>
+  <si>
+    <t>Lưu loát</t>
+  </si>
+  <si>
+    <t>Fluent</t>
+  </si>
+  <si>
+    <t>she is fluent in French</t>
+  </si>
+  <si>
+    <t>fluent in something</t>
+  </si>
+  <si>
+    <t>Bản địa</t>
+  </si>
+  <si>
+    <t>Native</t>
+  </si>
+  <si>
+    <t>Native language / tiếng mẹ đẻ</t>
+  </si>
+  <si>
+    <t>My native language is Vietnamese</t>
+  </si>
+  <si>
+    <t>người nói</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>She was a brilliant public speaker</t>
+  </si>
+  <si>
+    <t>a public speaker / một diễn giả</t>
+  </si>
+  <si>
+    <t>Dài hạn</t>
+  </si>
+  <si>
+    <t>long-term</t>
+  </si>
+  <si>
+    <t>A long-term goal often takes years to achieve</t>
+  </si>
+  <si>
+    <t>long-term goal</t>
+  </si>
+  <si>
+    <t>Khái niệm, ý tưởng chủ đạo</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>The concept of this event is experimental (Đang được thử nghiệm)</t>
+  </si>
+  <si>
+    <t>Concept of something / ý tưởng chủ đạo của something</t>
+  </si>
+  <si>
+    <t>Ghi lại</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>I often note down new words in my handbook</t>
+  </si>
+  <si>
+    <t>note down something</t>
+  </si>
+  <si>
+    <t>Đánh vần</t>
+  </si>
+  <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Please spell your name for me</t>
+  </si>
+  <si>
+    <t>spell something / đánh vần một cái gì đó</t>
+  </si>
+  <si>
+    <t>Ngữ pháp</t>
+  </si>
+  <si>
+    <t>Grammar</t>
+  </si>
+  <si>
+    <t>English grammar is easy to learn</t>
+  </si>
+  <si>
+    <t>English grammar</t>
+  </si>
+  <si>
+    <t>Kỷ thuật</t>
+  </si>
+  <si>
+    <t>Technique</t>
+  </si>
+  <si>
+    <t>You must learn the technique for baking.</t>
+  </si>
+  <si>
+    <t>technique for doing something / kỷ thuật làm một cái gì đó</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>I am the restaurant's regular customer</t>
+  </si>
+  <si>
+    <t>a regular customer / khách quen</t>
+  </si>
+  <si>
+    <t>Dịch</t>
+  </si>
+  <si>
+    <t>Translate</t>
+  </si>
+  <si>
+    <t>Can you translate english into vietnamese?</t>
+  </si>
+  <si>
+    <t>Translate something into something / dịch một cái gì thành một cái gì</t>
+  </si>
+  <si>
+    <t>Bối cảnh</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>in or within the context of something / trong bối cảnh gì đó</t>
+  </si>
+  <si>
+    <t>In the context of funerals(đám tang), wear dark clothing.</t>
+  </si>
+  <si>
+    <t>Định nghĩa</t>
+  </si>
+  <si>
+    <t>Define</t>
+  </si>
+  <si>
+    <t>Please define this work for me</t>
+  </si>
+  <si>
+    <t>define a word / định nghĩa một từ</t>
+  </si>
+  <si>
+    <t>Từ điển</t>
+  </si>
+  <si>
+    <t>Dictionary</t>
+  </si>
+  <si>
+    <t>You can look it up in the dictionary</t>
+  </si>
+  <si>
+    <t>look it up in the dictionary / tra cứu trong từ điển</t>
+  </si>
+  <si>
+    <t>Động từ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"To be" is an irregular verb </t>
+  </si>
+  <si>
+    <t>irregular verb / động từ bất quy tắc</t>
+  </si>
+  <si>
+    <t>Tương tác</t>
+  </si>
+  <si>
+    <t>Interact</t>
+  </si>
+  <si>
+    <t>I love interacting with people</t>
+  </si>
+  <si>
+    <t>interact with somebody / tương tác với ai đó</t>
+  </si>
+  <si>
+    <t>Cụm từ</t>
+  </si>
+  <si>
+    <t>Phrase</t>
+  </si>
+  <si>
+    <t>Catchy phrase help me study better</t>
+  </si>
+  <si>
+    <t>catchy phrase / cụm từ dễ nhớ</t>
+  </si>
+  <si>
+    <t>Giảm tốc độ</t>
+  </si>
+  <si>
+    <t>Slow down</t>
+  </si>
+  <si>
+    <t>slow the car down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slow somebody of something down </t>
+  </si>
+  <si>
+    <t>Căn bản, cơ bản</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Lions have basic instincts in hunting</t>
+  </si>
+  <si>
+    <t>basic instinct / bản năng căn bản</t>
+  </si>
+  <si>
+    <t>Quên</t>
+  </si>
+  <si>
+    <t>Forget</t>
+  </si>
+  <si>
+    <t>I forgot about you</t>
+  </si>
+  <si>
+    <t>forget about something or someone / quên đi một cái gì đó hoặc ai đó</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Nghe</t>
+  </si>
+  <si>
+    <t>Does my accent sound right?</t>
+  </si>
+  <si>
+    <t>sound right / nghe đúng, nghe chuẩn</t>
+  </si>
+  <si>
+    <t>Trò chuyện</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>She is chatting with someone at the bar</t>
+  </si>
+  <si>
+    <t>chat with somebody</t>
+  </si>
+  <si>
+    <t>Câu</t>
+  </si>
+  <si>
+    <t>Sentence</t>
+  </si>
+  <si>
+    <t>English only has a few basic sentence structures</t>
+  </si>
+  <si>
+    <t>sentence structure / cấu trúc câu</t>
+  </si>
+  <si>
+    <t>Tự tin</t>
+  </si>
+  <si>
+    <t>Confident</t>
+  </si>
+  <si>
+    <t>Are you confident about your performance?</t>
+  </si>
+  <si>
+    <t>confident about something</t>
+  </si>
+  <si>
+    <t>Ý nghĩa</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>What is the meaning of life =</t>
+  </si>
+  <si>
+    <t>meaning of something</t>
   </si>
 </sst>
 </file>
@@ -20402,10 +20843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1351"/>
+  <dimension ref="A1:G1381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1341" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1350" sqref="E1350"/>
+    <sheetView tabSelected="1" topLeftCell="F1346" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F1366" sqref="F1366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -51033,6 +51474,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="1352" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1352" s="1" t="s">
+        <v>6669</v>
+      </c>
+      <c r="B1352" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1352" s="1" t="s">
+        <v>6699</v>
+      </c>
+      <c r="D1352" s="1" t="s">
+        <v>6700</v>
+      </c>
+      <c r="E1352" s="1" t="s">
+        <v>6701</v>
+      </c>
+      <c r="F1352" s="1" t="s">
+        <v>6702</v>
+      </c>
+      <c r="G1352" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1353" s="1" t="s">
+        <v>6670</v>
+      </c>
+      <c r="B1353" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1353" s="1" t="s">
+        <v>6703</v>
+      </c>
+      <c r="D1353" s="1" t="s">
+        <v>6704</v>
+      </c>
+      <c r="E1353" s="1" t="s">
+        <v>6705</v>
+      </c>
+      <c r="F1353" s="1" t="s">
+        <v>6706</v>
+      </c>
+      <c r="G1353" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1354" s="1" t="s">
+        <v>6671</v>
+      </c>
+      <c r="B1354" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1354" s="1" t="s">
+        <v>6707</v>
+      </c>
+      <c r="D1354" s="1" t="s">
+        <v>6708</v>
+      </c>
+      <c r="E1354" s="1" t="s">
+        <v>6709</v>
+      </c>
+      <c r="F1354" s="1" t="s">
+        <v>6710</v>
+      </c>
+      <c r="G1354" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1355" s="1" t="s">
+        <v>6672</v>
+      </c>
+      <c r="B1355" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1355" s="1" t="s">
+        <v>6711</v>
+      </c>
+      <c r="D1355" s="1" t="s">
+        <v>6712</v>
+      </c>
+      <c r="E1355" s="1" t="s">
+        <v>6713</v>
+      </c>
+      <c r="F1355" s="1" t="s">
+        <v>6714</v>
+      </c>
+      <c r="G1355" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1356" s="1" t="s">
+        <v>6673</v>
+      </c>
+      <c r="B1356" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1356" s="1" t="s">
+        <v>6715</v>
+      </c>
+      <c r="D1356" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1356" s="1" t="s">
+        <v>6716</v>
+      </c>
+      <c r="F1356" s="1" t="s">
+        <v>6717</v>
+      </c>
+      <c r="G1356" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1357" s="1" t="s">
+        <v>6674</v>
+      </c>
+      <c r="B1357" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1357" s="1" t="s">
+        <v>6718</v>
+      </c>
+      <c r="D1357" s="1" t="s">
+        <v>6719</v>
+      </c>
+      <c r="E1357" s="1" t="s">
+        <v>6720</v>
+      </c>
+      <c r="F1357" s="1" t="s">
+        <v>6721</v>
+      </c>
+      <c r="G1357" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1358" s="1" t="s">
+        <v>6675</v>
+      </c>
+      <c r="B1358" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1358" s="1" t="s">
+        <v>6722</v>
+      </c>
+      <c r="D1358" s="1" t="s">
+        <v>6723</v>
+      </c>
+      <c r="E1358" s="1" t="s">
+        <v>6725</v>
+      </c>
+      <c r="F1358" s="1" t="s">
+        <v>6724</v>
+      </c>
+      <c r="G1358" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1359" s="1" t="s">
+        <v>6676</v>
+      </c>
+      <c r="B1359" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1359" s="1" t="s">
+        <v>6726</v>
+      </c>
+      <c r="D1359" s="1" t="s">
+        <v>6727</v>
+      </c>
+      <c r="E1359" s="1" t="s">
+        <v>6728</v>
+      </c>
+      <c r="F1359" s="1" t="s">
+        <v>6729</v>
+      </c>
+      <c r="G1359" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1360" s="1" t="s">
+        <v>6677</v>
+      </c>
+      <c r="B1360" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1360" s="1" t="s">
+        <v>6730</v>
+      </c>
+      <c r="D1360" s="1" t="s">
+        <v>6731</v>
+      </c>
+      <c r="E1360" s="1" t="s">
+        <v>6732</v>
+      </c>
+      <c r="F1360" s="1" t="s">
+        <v>6733</v>
+      </c>
+      <c r="G1360" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1361" s="1" t="s">
+        <v>6678</v>
+      </c>
+      <c r="B1361" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1361" s="1" t="s">
+        <v>6734</v>
+      </c>
+      <c r="D1361" s="1" t="s">
+        <v>6735</v>
+      </c>
+      <c r="E1361" s="1" t="s">
+        <v>6736</v>
+      </c>
+      <c r="F1361" s="1" t="s">
+        <v>6737</v>
+      </c>
+      <c r="G1361" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1362" s="1" t="s">
+        <v>6679</v>
+      </c>
+      <c r="B1362" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1362" s="1" t="s">
+        <v>6738</v>
+      </c>
+      <c r="D1362" s="1" t="s">
+        <v>6739</v>
+      </c>
+      <c r="E1362" s="1" t="s">
+        <v>6740</v>
+      </c>
+      <c r="F1362" s="1" t="s">
+        <v>6741</v>
+      </c>
+      <c r="G1362" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1363" s="1" t="s">
+        <v>6680</v>
+      </c>
+      <c r="B1363" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1363" s="1" t="s">
+        <v>6742</v>
+      </c>
+      <c r="D1363" s="1" t="s">
+        <v>6743</v>
+      </c>
+      <c r="E1363" s="1" t="s">
+        <v>6744</v>
+      </c>
+      <c r="F1363" s="1" t="s">
+        <v>6745</v>
+      </c>
+      <c r="G1363" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1364" s="1" t="s">
+        <v>6681</v>
+      </c>
+      <c r="B1364" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1364" s="1" t="s">
+        <v>6746</v>
+      </c>
+      <c r="D1364" s="1" t="s">
+        <v>6747</v>
+      </c>
+      <c r="E1364" s="1" t="s">
+        <v>6748</v>
+      </c>
+      <c r="F1364" s="1" t="s">
+        <v>6749</v>
+      </c>
+      <c r="G1364" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1365" s="1" t="s">
+        <v>6682</v>
+      </c>
+      <c r="B1365" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1365" s="1" t="s">
+        <v>6750</v>
+      </c>
+      <c r="D1365" s="1" t="s">
+        <v>6751</v>
+      </c>
+      <c r="E1365" s="1" t="s">
+        <v>6752</v>
+      </c>
+      <c r="F1365" s="1" t="s">
+        <v>6753</v>
+      </c>
+      <c r="G1365" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1366" s="1" t="s">
+        <v>6683</v>
+      </c>
+      <c r="B1366" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1366" s="1" t="s">
+        <v>3680</v>
+      </c>
+      <c r="D1366" s="1" t="s">
+        <v>6754</v>
+      </c>
+      <c r="E1366" s="1" t="s">
+        <v>6755</v>
+      </c>
+      <c r="F1366" s="1" t="s">
+        <v>6756</v>
+      </c>
+      <c r="G1366" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1367" s="1" t="s">
+        <v>6684</v>
+      </c>
+      <c r="B1367" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1367" s="1" t="s">
+        <v>6757</v>
+      </c>
+      <c r="D1367" s="1" t="s">
+        <v>6758</v>
+      </c>
+      <c r="E1367" s="1" t="s">
+        <v>6759</v>
+      </c>
+      <c r="F1367" s="1" t="s">
+        <v>6760</v>
+      </c>
+      <c r="G1367" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1368" s="1" t="s">
+        <v>6685</v>
+      </c>
+      <c r="B1368" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1368" s="1" t="s">
+        <v>6761</v>
+      </c>
+      <c r="D1368" s="1" t="s">
+        <v>6762</v>
+      </c>
+      <c r="E1368" s="1" t="s">
+        <v>6764</v>
+      </c>
+      <c r="F1368" s="1" t="s">
+        <v>6763</v>
+      </c>
+      <c r="G1368" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1369" s="1" t="s">
+        <v>6686</v>
+      </c>
+      <c r="B1369" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1369" s="1" t="s">
+        <v>6765</v>
+      </c>
+      <c r="D1369" s="1" t="s">
+        <v>6766</v>
+      </c>
+      <c r="E1369" s="1" t="s">
+        <v>6767</v>
+      </c>
+      <c r="F1369" s="1" t="s">
+        <v>6768</v>
+      </c>
+      <c r="G1369" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1370" s="1" t="s">
+        <v>6687</v>
+      </c>
+      <c r="B1370" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1370" s="1" t="s">
+        <v>6769</v>
+      </c>
+      <c r="D1370" s="1" t="s">
+        <v>6770</v>
+      </c>
+      <c r="E1370" s="1" t="s">
+        <v>6771</v>
+      </c>
+      <c r="F1370" s="1" t="s">
+        <v>6772</v>
+      </c>
+      <c r="G1370" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1371" s="1" t="s">
+        <v>6688</v>
+      </c>
+      <c r="B1371" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1371" s="1" t="s">
+        <v>6773</v>
+      </c>
+      <c r="D1371" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="E1371" s="1" t="s">
+        <v>6774</v>
+      </c>
+      <c r="F1371" s="1" t="s">
+        <v>6775</v>
+      </c>
+      <c r="G1371" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1372" s="1" t="s">
+        <v>6689</v>
+      </c>
+      <c r="B1372" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1372" s="1" t="s">
+        <v>6776</v>
+      </c>
+      <c r="D1372" s="1" t="s">
+        <v>6777</v>
+      </c>
+      <c r="E1372" s="1" t="s">
+        <v>6778</v>
+      </c>
+      <c r="F1372" s="1" t="s">
+        <v>6779</v>
+      </c>
+      <c r="G1372" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1373" s="1" t="s">
+        <v>6690</v>
+      </c>
+      <c r="B1373" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1373" s="1" t="s">
+        <v>6780</v>
+      </c>
+      <c r="D1373" s="1" t="s">
+        <v>6781</v>
+      </c>
+      <c r="E1373" s="1" t="s">
+        <v>6782</v>
+      </c>
+      <c r="F1373" s="1" t="s">
+        <v>6783</v>
+      </c>
+      <c r="G1373" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1374" s="1" t="s">
+        <v>6691</v>
+      </c>
+      <c r="B1374" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1374" s="1" t="s">
+        <v>6784</v>
+      </c>
+      <c r="D1374" s="1" t="s">
+        <v>6785</v>
+      </c>
+      <c r="E1374" s="1" t="s">
+        <v>6786</v>
+      </c>
+      <c r="F1374" s="1" t="s">
+        <v>6787</v>
+      </c>
+      <c r="G1374" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1375" s="1" t="s">
+        <v>6692</v>
+      </c>
+      <c r="B1375" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1375" s="1" t="s">
+        <v>6788</v>
+      </c>
+      <c r="D1375" s="1" t="s">
+        <v>6789</v>
+      </c>
+      <c r="E1375" s="1" t="s">
+        <v>6790</v>
+      </c>
+      <c r="F1375" s="1" t="s">
+        <v>6791</v>
+      </c>
+      <c r="G1375" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1376" s="1" t="s">
+        <v>6693</v>
+      </c>
+      <c r="B1376" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1376" s="1" t="s">
+        <v>6792</v>
+      </c>
+      <c r="D1376" s="1" t="s">
+        <v>6793</v>
+      </c>
+      <c r="E1376" s="1" t="s">
+        <v>6794</v>
+      </c>
+      <c r="F1376" s="1" t="s">
+        <v>6795</v>
+      </c>
+      <c r="G1376" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1377" s="1" t="s">
+        <v>6694</v>
+      </c>
+      <c r="B1377" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1377" s="1" t="s">
+        <v>6797</v>
+      </c>
+      <c r="D1377" s="1" t="s">
+        <v>6796</v>
+      </c>
+      <c r="E1377" s="1" t="s">
+        <v>6798</v>
+      </c>
+      <c r="F1377" s="1" t="s">
+        <v>6799</v>
+      </c>
+      <c r="G1377" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1378" s="1" t="s">
+        <v>6695</v>
+      </c>
+      <c r="B1378" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1378" s="1" t="s">
+        <v>6800</v>
+      </c>
+      <c r="D1378" s="1" t="s">
+        <v>6801</v>
+      </c>
+      <c r="E1378" s="1" t="s">
+        <v>6802</v>
+      </c>
+      <c r="F1378" s="1" t="s">
+        <v>6803</v>
+      </c>
+      <c r="G1378" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1379" s="1" t="s">
+        <v>6696</v>
+      </c>
+      <c r="B1379" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1379" s="1" t="s">
+        <v>6804</v>
+      </c>
+      <c r="D1379" s="1" t="s">
+        <v>6805</v>
+      </c>
+      <c r="E1379" s="1" t="s">
+        <v>6806</v>
+      </c>
+      <c r="F1379" s="1" t="s">
+        <v>6807</v>
+      </c>
+      <c r="G1379" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1380" s="1" t="s">
+        <v>6697</v>
+      </c>
+      <c r="B1380" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1380" s="1" t="s">
+        <v>6808</v>
+      </c>
+      <c r="D1380" s="1" t="s">
+        <v>6809</v>
+      </c>
+      <c r="E1380" s="1" t="s">
+        <v>6810</v>
+      </c>
+      <c r="F1380" s="1" t="s">
+        <v>6811</v>
+      </c>
+      <c r="G1380" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1381" s="1" t="s">
+        <v>6698</v>
+      </c>
+      <c r="B1381" s="1">
+        <v>46</v>
+      </c>
+      <c r="C1381" s="1" t="s">
+        <v>6812</v>
+      </c>
+      <c r="D1381" s="1" t="s">
+        <v>6813</v>
+      </c>
+      <c r="E1381" s="1" t="s">
+        <v>6814</v>
+      </c>
+      <c r="F1381" s="1" t="s">
+        <v>6815</v>
+      </c>
+      <c r="G1381" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 47
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2C8262-391B-BD41-B3E0-45A25BB761BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E71F2D6-F53E-3A4D-9900-F29E93121C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8134" uniqueCount="6816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8314" uniqueCount="6962">
   <si>
     <t>ID</t>
   </si>
@@ -20478,6 +20478,444 @@
   </si>
   <si>
     <t>meaning of something</t>
+  </si>
+  <si>
+    <t>U47_01</t>
+  </si>
+  <si>
+    <t>U47_02</t>
+  </si>
+  <si>
+    <t>U47_03</t>
+  </si>
+  <si>
+    <t>U47_04</t>
+  </si>
+  <si>
+    <t>U47_05</t>
+  </si>
+  <si>
+    <t>U47_06</t>
+  </si>
+  <si>
+    <t>U47_07</t>
+  </si>
+  <si>
+    <t>U47_08</t>
+  </si>
+  <si>
+    <t>U47_09</t>
+  </si>
+  <si>
+    <t>U47_10</t>
+  </si>
+  <si>
+    <t>U47_11</t>
+  </si>
+  <si>
+    <t>U47_12</t>
+  </si>
+  <si>
+    <t>U47_13</t>
+  </si>
+  <si>
+    <t>U47_14</t>
+  </si>
+  <si>
+    <t>U47_15</t>
+  </si>
+  <si>
+    <t>U47_16</t>
+  </si>
+  <si>
+    <t>U47_17</t>
+  </si>
+  <si>
+    <t>U47_18</t>
+  </si>
+  <si>
+    <t>U47_19</t>
+  </si>
+  <si>
+    <t>U47_20</t>
+  </si>
+  <si>
+    <t>U47_21</t>
+  </si>
+  <si>
+    <t>U47_22</t>
+  </si>
+  <si>
+    <t>U47_23</t>
+  </si>
+  <si>
+    <t>U47_24</t>
+  </si>
+  <si>
+    <t>U47_25</t>
+  </si>
+  <si>
+    <t>U47_26</t>
+  </si>
+  <si>
+    <t>U47_27</t>
+  </si>
+  <si>
+    <t>U47_28</t>
+  </si>
+  <si>
+    <t>U47_29</t>
+  </si>
+  <si>
+    <t>U47_30</t>
+  </si>
+  <si>
+    <t>Đăng</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>She posted a picture on Instagram</t>
+  </si>
+  <si>
+    <t>post something / đăng một cái gì đó</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>I turned off notifications on FB</t>
+  </si>
+  <si>
+    <t>turn on or off notifications</t>
+  </si>
+  <si>
+    <t>Phần mềm</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Software developers help me update my computer</t>
+  </si>
+  <si>
+    <t>a software developer / nhà phát triển phần mềm</t>
+  </si>
+  <si>
+    <t>Cập nhật</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>You should update your phone</t>
+  </si>
+  <si>
+    <t>update something / cập nhật một cái gì đó</t>
+  </si>
+  <si>
+    <t>Đường dẫn, liên kết</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Click on this link to download the document</t>
+  </si>
+  <si>
+    <t>click the link / nhấn vào liên kết</t>
+  </si>
+  <si>
+    <t>Ngón tay</t>
+  </si>
+  <si>
+    <t>Finger</t>
+  </si>
+  <si>
+    <t>He points his finger in her direction</t>
+  </si>
+  <si>
+    <t>point the finger / chỉ tay</t>
+  </si>
+  <si>
+    <t>Nhấn chuột</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>Click on the button to stop</t>
+  </si>
+  <si>
+    <t>click on something / nhấp vào một cái gì đó</t>
+  </si>
+  <si>
+    <t>Tải xuống</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>Download the program to start</t>
+  </si>
+  <si>
+    <t>download something / tải về một cái gì đó</t>
+  </si>
+  <si>
+    <t>Công nghệ</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Modern technology makes our lives better</t>
+  </si>
+  <si>
+    <t>modern technology / công nghệ hiện đại</t>
+  </si>
+  <si>
+    <t>Sự giao tiếp</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>We must have clear communication within the team</t>
+  </si>
+  <si>
+    <t>clear communication / sự giao tiếp rõ ràng</t>
+  </si>
+  <si>
+    <t>Trang mạng</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>FB is one of the most popular social media sites</t>
+  </si>
+  <si>
+    <t>a social media site / một trang mạng xã hội</t>
+  </si>
+  <si>
+    <t>Trang nhật ký</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>My online blog is about make-up</t>
+  </si>
+  <si>
+    <t>an online blog / trang nhật ký trực tuyến</t>
+  </si>
+  <si>
+    <t>Đổi</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>You can press here to switch between your email accounts</t>
+  </si>
+  <si>
+    <t>Truy cập</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>We can access the Internet</t>
+  </si>
+  <si>
+    <t>access something or somebody / truy cập một cái gì đó hoặc ai đó</t>
+  </si>
+  <si>
+    <t>Khách ghé thăm, khách truy cập</t>
+  </si>
+  <si>
+    <t>Visitor</t>
+  </si>
+  <si>
+    <t>This site has a growing number of first-time visitors</t>
+  </si>
+  <si>
+    <t>first-time visitor / khách truy cập lần đầu</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Click on the app icon to start</t>
+  </si>
+  <si>
+    <t>app icon / biểu tưởng ứng dụng</t>
+  </si>
+  <si>
+    <t>Sign up</t>
+  </si>
+  <si>
+    <t>Please sign up for dance class</t>
+  </si>
+  <si>
+    <t>sign up for something</t>
+  </si>
+  <si>
+    <t>Tân tiến, đột phá</t>
+  </si>
+  <si>
+    <t>Innovative</t>
+  </si>
+  <si>
+    <t>The architecture has an innovative design</t>
+  </si>
+  <si>
+    <t>innovative design / thiết kế mang tính đột phá</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>Online shopping is popular in these times(rất phổ biến hiện nay)</t>
+  </si>
+  <si>
+    <t>online shopping / mua sắm trực tuyến</t>
+  </si>
+  <si>
+    <t>Mạng lưới</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>I have a network of business contacts</t>
+  </si>
+  <si>
+    <t>network of something / mạng lưới của cái gì đó</t>
+  </si>
+  <si>
+    <t>Tín hiệu</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>It was a signal for me to run</t>
+  </si>
+  <si>
+    <t>a signal to do something / một tín hiệu đê làm một cái gì đó</t>
+  </si>
+  <si>
+    <t>Bảng</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>The teacher writes a question on the board</t>
+  </si>
+  <si>
+    <t>on the board</t>
+  </si>
+  <si>
+    <t>Tiên tiến</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Advanced technology connects us easier</t>
+  </si>
+  <si>
+    <t>advanced technology / công nghệ tiên tiến</t>
+  </si>
+  <si>
+    <t>Trả lời</t>
+  </si>
+  <si>
+    <t>Reply</t>
+  </si>
+  <si>
+    <t>She replied to me yesterday</t>
+  </si>
+  <si>
+    <t>reply to somebody or something</t>
+  </si>
+  <si>
+    <t>Không gian</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>My phone needs extra space for storage</t>
+  </si>
+  <si>
+    <t>extra space</t>
+  </si>
+  <si>
+    <t>Dây cáp</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>The mouse bit(cắn) the power cable</t>
+  </si>
+  <si>
+    <t>A power cable / dây cáp điện</t>
+  </si>
+  <si>
+    <t>Kết nối</t>
+  </si>
+  <si>
+    <t>Connect</t>
+  </si>
+  <si>
+    <t>Connect the phone to the charger</t>
+  </si>
+  <si>
+    <t>connect a to b</t>
+  </si>
+  <si>
+    <t>Giải quyết</t>
+  </si>
+  <si>
+    <t>Solve</t>
+  </si>
+  <si>
+    <t>Solve this puzzle for me</t>
+  </si>
+  <si>
+    <t>solve a puzzle / giải một câu đố</t>
+  </si>
+  <si>
+    <t>Tra cứu</t>
+  </si>
+  <si>
+    <t>Look up</t>
+  </si>
+  <si>
+    <t>Can you look up this word for me?</t>
+  </si>
+  <si>
+    <t>look up something</t>
+  </si>
+  <si>
+    <t>Từ khóa</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Find the keyword of this text</t>
+  </si>
+  <si>
+    <t>find the keyword / tìm ra từ khóa</t>
+  </si>
+  <si>
+    <t>Switch between something / đổi giữa cái gì đó</t>
   </si>
 </sst>
 </file>
@@ -20843,10 +21281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1381"/>
+  <dimension ref="A1:G1411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1346" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F1366" sqref="F1366"/>
+    <sheetView tabSelected="1" topLeftCell="A1400" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1409" sqref="C1409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -52164,6 +52602,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="1382" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1382" s="1" t="s">
+        <v>6816</v>
+      </c>
+      <c r="B1382" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1382" s="1" t="s">
+        <v>6846</v>
+      </c>
+      <c r="D1382" s="1" t="s">
+        <v>6847</v>
+      </c>
+      <c r="E1382" s="1" t="s">
+        <v>6848</v>
+      </c>
+      <c r="F1382" s="1" t="s">
+        <v>6849</v>
+      </c>
+      <c r="G1382" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1383" s="1" t="s">
+        <v>6817</v>
+      </c>
+      <c r="B1383" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1383" s="1" t="s">
+        <v>3873</v>
+      </c>
+      <c r="D1383" s="1" t="s">
+        <v>6850</v>
+      </c>
+      <c r="E1383" s="1" t="s">
+        <v>6851</v>
+      </c>
+      <c r="F1383" s="1" t="s">
+        <v>6852</v>
+      </c>
+      <c r="G1383" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1384" s="1" t="s">
+        <v>6818</v>
+      </c>
+      <c r="B1384" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1384" s="1" t="s">
+        <v>6853</v>
+      </c>
+      <c r="D1384" s="1" t="s">
+        <v>6854</v>
+      </c>
+      <c r="E1384" s="1" t="s">
+        <v>6855</v>
+      </c>
+      <c r="F1384" s="1" t="s">
+        <v>6856</v>
+      </c>
+      <c r="G1384" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1385" s="1" t="s">
+        <v>6819</v>
+      </c>
+      <c r="B1385" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1385" s="1" t="s">
+        <v>6857</v>
+      </c>
+      <c r="D1385" s="1" t="s">
+        <v>6858</v>
+      </c>
+      <c r="E1385" s="1" t="s">
+        <v>6859</v>
+      </c>
+      <c r="F1385" s="1" t="s">
+        <v>6860</v>
+      </c>
+      <c r="G1385" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1386" s="1" t="s">
+        <v>6820</v>
+      </c>
+      <c r="B1386" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1386" s="1" t="s">
+        <v>6861</v>
+      </c>
+      <c r="D1386" s="1" t="s">
+        <v>6862</v>
+      </c>
+      <c r="E1386" s="1" t="s">
+        <v>6863</v>
+      </c>
+      <c r="F1386" s="1" t="s">
+        <v>6864</v>
+      </c>
+      <c r="G1386" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1387" s="1" t="s">
+        <v>6821</v>
+      </c>
+      <c r="B1387" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1387" s="1" t="s">
+        <v>6865</v>
+      </c>
+      <c r="D1387" s="1" t="s">
+        <v>6866</v>
+      </c>
+      <c r="E1387" s="1" t="s">
+        <v>6867</v>
+      </c>
+      <c r="F1387" s="1" t="s">
+        <v>6868</v>
+      </c>
+      <c r="G1387" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1388" s="1" t="s">
+        <v>6822</v>
+      </c>
+      <c r="B1388" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1388" s="1" t="s">
+        <v>6869</v>
+      </c>
+      <c r="D1388" s="1" t="s">
+        <v>6870</v>
+      </c>
+      <c r="E1388" s="1" t="s">
+        <v>6871</v>
+      </c>
+      <c r="F1388" s="1" t="s">
+        <v>6872</v>
+      </c>
+      <c r="G1388" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1389" s="1" t="s">
+        <v>6823</v>
+      </c>
+      <c r="B1389" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1389" s="1" t="s">
+        <v>6873</v>
+      </c>
+      <c r="D1389" s="1" t="s">
+        <v>6874</v>
+      </c>
+      <c r="E1389" s="1" t="s">
+        <v>6875</v>
+      </c>
+      <c r="F1389" s="1" t="s">
+        <v>6876</v>
+      </c>
+      <c r="G1389" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1390" s="1" t="s">
+        <v>6824</v>
+      </c>
+      <c r="B1390" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1390" s="1" t="s">
+        <v>6877</v>
+      </c>
+      <c r="D1390" s="1" t="s">
+        <v>6878</v>
+      </c>
+      <c r="E1390" s="1" t="s">
+        <v>6879</v>
+      </c>
+      <c r="F1390" s="1" t="s">
+        <v>6880</v>
+      </c>
+      <c r="G1390" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1391" s="1" t="s">
+        <v>6825</v>
+      </c>
+      <c r="B1391" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1391" s="1" t="s">
+        <v>6881</v>
+      </c>
+      <c r="D1391" s="1" t="s">
+        <v>6882</v>
+      </c>
+      <c r="E1391" s="1" t="s">
+        <v>6883</v>
+      </c>
+      <c r="F1391" s="1" t="s">
+        <v>6884</v>
+      </c>
+      <c r="G1391" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1392" s="1" t="s">
+        <v>6826</v>
+      </c>
+      <c r="B1392" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1392" s="1" t="s">
+        <v>6885</v>
+      </c>
+      <c r="D1392" s="1" t="s">
+        <v>6886</v>
+      </c>
+      <c r="E1392" s="1" t="s">
+        <v>6887</v>
+      </c>
+      <c r="F1392" s="1" t="s">
+        <v>6888</v>
+      </c>
+      <c r="G1392" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1393" s="1" t="s">
+        <v>6827</v>
+      </c>
+      <c r="B1393" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1393" s="1" t="s">
+        <v>6889</v>
+      </c>
+      <c r="D1393" s="1" t="s">
+        <v>6890</v>
+      </c>
+      <c r="E1393" s="1" t="s">
+        <v>6891</v>
+      </c>
+      <c r="F1393" s="1" t="s">
+        <v>6892</v>
+      </c>
+      <c r="G1393" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1394" s="1" t="s">
+        <v>6828</v>
+      </c>
+      <c r="B1394" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1394" s="1" t="s">
+        <v>6893</v>
+      </c>
+      <c r="D1394" s="1" t="s">
+        <v>6894</v>
+      </c>
+      <c r="E1394" s="1" t="s">
+        <v>6895</v>
+      </c>
+      <c r="F1394" s="1" t="s">
+        <v>6961</v>
+      </c>
+      <c r="G1394" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1395" s="1" t="s">
+        <v>6829</v>
+      </c>
+      <c r="B1395" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1395" s="1" t="s">
+        <v>6896</v>
+      </c>
+      <c r="D1395" s="1" t="s">
+        <v>6897</v>
+      </c>
+      <c r="E1395" s="1" t="s">
+        <v>6898</v>
+      </c>
+      <c r="F1395" s="1" t="s">
+        <v>6899</v>
+      </c>
+      <c r="G1395" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1396" s="1" t="s">
+        <v>6830</v>
+      </c>
+      <c r="B1396" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1396" s="1" t="s">
+        <v>6900</v>
+      </c>
+      <c r="D1396" s="1" t="s">
+        <v>6901</v>
+      </c>
+      <c r="E1396" s="1" t="s">
+        <v>6902</v>
+      </c>
+      <c r="F1396" s="1" t="s">
+        <v>6903</v>
+      </c>
+      <c r="G1396" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1397" s="1" t="s">
+        <v>6831</v>
+      </c>
+      <c r="B1397" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1397" s="1" t="s">
+        <v>6210</v>
+      </c>
+      <c r="D1397" s="1" t="s">
+        <v>6904</v>
+      </c>
+      <c r="E1397" s="1" t="s">
+        <v>6905</v>
+      </c>
+      <c r="F1397" s="1" t="s">
+        <v>6906</v>
+      </c>
+      <c r="G1397" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1398" s="1" t="s">
+        <v>6832</v>
+      </c>
+      <c r="B1398" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1398" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1398" s="1" t="s">
+        <v>6907</v>
+      </c>
+      <c r="E1398" s="1" t="s">
+        <v>6908</v>
+      </c>
+      <c r="F1398" s="1" t="s">
+        <v>6909</v>
+      </c>
+      <c r="G1398" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1399" s="1" t="s">
+        <v>6833</v>
+      </c>
+      <c r="B1399" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1399" s="1" t="s">
+        <v>6910</v>
+      </c>
+      <c r="D1399" s="1" t="s">
+        <v>6911</v>
+      </c>
+      <c r="E1399" s="1" t="s">
+        <v>6912</v>
+      </c>
+      <c r="F1399" s="1" t="s">
+        <v>6913</v>
+      </c>
+      <c r="G1399" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1400" s="1" t="s">
+        <v>6834</v>
+      </c>
+      <c r="B1400" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1400" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1400" s="1" t="s">
+        <v>6914</v>
+      </c>
+      <c r="E1400" s="1" t="s">
+        <v>6915</v>
+      </c>
+      <c r="F1400" s="1" t="s">
+        <v>6916</v>
+      </c>
+      <c r="G1400" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1401" s="1" t="s">
+        <v>6835</v>
+      </c>
+      <c r="B1401" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1401" s="1" t="s">
+        <v>6917</v>
+      </c>
+      <c r="D1401" s="1" t="s">
+        <v>6918</v>
+      </c>
+      <c r="E1401" s="1" t="s">
+        <v>6919</v>
+      </c>
+      <c r="F1401" s="1" t="s">
+        <v>6920</v>
+      </c>
+      <c r="G1401" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1402" s="1" t="s">
+        <v>6836</v>
+      </c>
+      <c r="B1402" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1402" s="1" t="s">
+        <v>6921</v>
+      </c>
+      <c r="D1402" s="1" t="s">
+        <v>6922</v>
+      </c>
+      <c r="E1402" s="1" t="s">
+        <v>6923</v>
+      </c>
+      <c r="F1402" s="1" t="s">
+        <v>6924</v>
+      </c>
+      <c r="G1402" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1403" s="1" t="s">
+        <v>6837</v>
+      </c>
+      <c r="B1403" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1403" s="1" t="s">
+        <v>6925</v>
+      </c>
+      <c r="D1403" s="1" t="s">
+        <v>6926</v>
+      </c>
+      <c r="E1403" s="1" t="s">
+        <v>6927</v>
+      </c>
+      <c r="F1403" s="1" t="s">
+        <v>6928</v>
+      </c>
+      <c r="G1403" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1404" s="1" t="s">
+        <v>6838</v>
+      </c>
+      <c r="B1404" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1404" s="1" t="s">
+        <v>6929</v>
+      </c>
+      <c r="D1404" s="1" t="s">
+        <v>6930</v>
+      </c>
+      <c r="E1404" s="1" t="s">
+        <v>6931</v>
+      </c>
+      <c r="F1404" s="1" t="s">
+        <v>6932</v>
+      </c>
+      <c r="G1404" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1405" s="1" t="s">
+        <v>6839</v>
+      </c>
+      <c r="B1405" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1405" s="1" t="s">
+        <v>6933</v>
+      </c>
+      <c r="D1405" s="1" t="s">
+        <v>6934</v>
+      </c>
+      <c r="E1405" s="1" t="s">
+        <v>6935</v>
+      </c>
+      <c r="F1405" s="1" t="s">
+        <v>6936</v>
+      </c>
+      <c r="G1405" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1406" s="1" t="s">
+        <v>6840</v>
+      </c>
+      <c r="B1406" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1406" s="1" t="s">
+        <v>6937</v>
+      </c>
+      <c r="D1406" s="1" t="s">
+        <v>6938</v>
+      </c>
+      <c r="E1406" s="1" t="s">
+        <v>6939</v>
+      </c>
+      <c r="F1406" s="1" t="s">
+        <v>6940</v>
+      </c>
+      <c r="G1406" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1407" s="1" t="s">
+        <v>6841</v>
+      </c>
+      <c r="B1407" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1407" s="1" t="s">
+        <v>6941</v>
+      </c>
+      <c r="D1407" s="1" t="s">
+        <v>6942</v>
+      </c>
+      <c r="E1407" s="1" t="s">
+        <v>6943</v>
+      </c>
+      <c r="F1407" s="1" t="s">
+        <v>6944</v>
+      </c>
+      <c r="G1407" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1408" s="1" t="s">
+        <v>6842</v>
+      </c>
+      <c r="B1408" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1408" s="1" t="s">
+        <v>6945</v>
+      </c>
+      <c r="D1408" s="1" t="s">
+        <v>6946</v>
+      </c>
+      <c r="E1408" s="1" t="s">
+        <v>6947</v>
+      </c>
+      <c r="F1408" s="1" t="s">
+        <v>6948</v>
+      </c>
+      <c r="G1408" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1409" s="1" t="s">
+        <v>6843</v>
+      </c>
+      <c r="B1409" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1409" s="1" t="s">
+        <v>6949</v>
+      </c>
+      <c r="D1409" s="1" t="s">
+        <v>6950</v>
+      </c>
+      <c r="E1409" s="1" t="s">
+        <v>6951</v>
+      </c>
+      <c r="F1409" s="1" t="s">
+        <v>6952</v>
+      </c>
+      <c r="G1409" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1410" s="1" t="s">
+        <v>6844</v>
+      </c>
+      <c r="B1410" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1410" s="1" t="s">
+        <v>6953</v>
+      </c>
+      <c r="D1410" s="1" t="s">
+        <v>6954</v>
+      </c>
+      <c r="E1410" s="1" t="s">
+        <v>6955</v>
+      </c>
+      <c r="F1410" s="1" t="s">
+        <v>6956</v>
+      </c>
+      <c r="G1410" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1411" s="1" t="s">
+        <v>6845</v>
+      </c>
+      <c r="B1411" s="1">
+        <v>47</v>
+      </c>
+      <c r="C1411" s="1" t="s">
+        <v>6957</v>
+      </c>
+      <c r="D1411" s="1" t="s">
+        <v>6958</v>
+      </c>
+      <c r="E1411" s="1" t="s">
+        <v>6959</v>
+      </c>
+      <c r="F1411" s="1" t="s">
+        <v>6960</v>
+      </c>
+      <c r="G1411" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 48
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E71F2D6-F53E-3A4D-9900-F29E93121C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDAC7AD-13E2-0E4D-B3F4-4732377C64EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8314" uniqueCount="6962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8494" uniqueCount="7108">
   <si>
     <t>ID</t>
   </si>
@@ -20916,6 +20916,444 @@
   </si>
   <si>
     <t>Switch between something / đổi giữa cái gì đó</t>
+  </si>
+  <si>
+    <t>U48_01</t>
+  </si>
+  <si>
+    <t>U48_02</t>
+  </si>
+  <si>
+    <t>U48_03</t>
+  </si>
+  <si>
+    <t>U48_04</t>
+  </si>
+  <si>
+    <t>U48_05</t>
+  </si>
+  <si>
+    <t>U48_06</t>
+  </si>
+  <si>
+    <t>U48_07</t>
+  </si>
+  <si>
+    <t>U48_08</t>
+  </si>
+  <si>
+    <t>U48_09</t>
+  </si>
+  <si>
+    <t>U48_10</t>
+  </si>
+  <si>
+    <t>U48_11</t>
+  </si>
+  <si>
+    <t>U48_12</t>
+  </si>
+  <si>
+    <t>U48_13</t>
+  </si>
+  <si>
+    <t>U48_14</t>
+  </si>
+  <si>
+    <t>U48_15</t>
+  </si>
+  <si>
+    <t>U48_16</t>
+  </si>
+  <si>
+    <t>U48_17</t>
+  </si>
+  <si>
+    <t>U48_18</t>
+  </si>
+  <si>
+    <t>U48_19</t>
+  </si>
+  <si>
+    <t>U48_20</t>
+  </si>
+  <si>
+    <t>U48_21</t>
+  </si>
+  <si>
+    <t>U48_22</t>
+  </si>
+  <si>
+    <t>U48_23</t>
+  </si>
+  <si>
+    <t>U48_24</t>
+  </si>
+  <si>
+    <t>U48_25</t>
+  </si>
+  <si>
+    <t>U48_26</t>
+  </si>
+  <si>
+    <t>U48_27</t>
+  </si>
+  <si>
+    <t>U48_28</t>
+  </si>
+  <si>
+    <t>U48_29</t>
+  </si>
+  <si>
+    <t>U48_30</t>
+  </si>
+  <si>
+    <t>Xuất bản</t>
+  </si>
+  <si>
+    <t>Publish</t>
+  </si>
+  <si>
+    <t>The author published one novel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publish something </t>
+  </si>
+  <si>
+    <t>Người máy</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>I always sing without emotion like a robot</t>
+  </si>
+  <si>
+    <t>like a robot / như một cái máy</t>
+  </si>
+  <si>
+    <t>Máy móc</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>The watch was made by machine</t>
+  </si>
+  <si>
+    <t>by machine / bằng máy</t>
+  </si>
+  <si>
+    <t>able</t>
+  </si>
+  <si>
+    <t>She is able to play the piano</t>
+  </si>
+  <si>
+    <t>able to do something / có thể làm một cái gì đó</t>
+  </si>
+  <si>
+    <t>Tự động</t>
+  </si>
+  <si>
+    <t>Automatic</t>
+  </si>
+  <si>
+    <t>The car is fully automatic</t>
+  </si>
+  <si>
+    <t>fully automatic / hoàn toàn tự động</t>
+  </si>
+  <si>
+    <t>Respond</t>
+  </si>
+  <si>
+    <t>Please respond to my email by morning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">respond to something or somebody </t>
+  </si>
+  <si>
+    <t>Khảo sát</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>We conducted a survey for research</t>
+  </si>
+  <si>
+    <t>conduct a survey / tiến hành một cuộc khảo sát</t>
+  </si>
+  <si>
+    <t>Dòng trạng thái</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>I recently posted a status on FB</t>
+  </si>
+  <si>
+    <t>post a status / đăng tải một dòng trạng thái</t>
+  </si>
+  <si>
+    <t>Đính</t>
+  </si>
+  <si>
+    <t>Attach</t>
+  </si>
+  <si>
+    <t>Could you attach the file with your email?</t>
+  </si>
+  <si>
+    <t>attach something to something / đính một cái gì đó vào một cái gì đó</t>
+  </si>
+  <si>
+    <t>Tài khoản</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>I am opening up a bank account</t>
+  </si>
+  <si>
+    <t>a bank account</t>
+  </si>
+  <si>
+    <t>Chính sách</t>
+  </si>
+  <si>
+    <t>Policy</t>
+  </si>
+  <si>
+    <t>What is your policy on education?</t>
+  </si>
+  <si>
+    <t>policy on something / chính sách về một cái gì đó</t>
+  </si>
+  <si>
+    <t>Trang</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Turn to page 25 and read</t>
+  </si>
+  <si>
+    <t>turn to page / lật sang trang</t>
+  </si>
+  <si>
+    <t>Permit</t>
+  </si>
+  <si>
+    <t>My parents do not permit me to come home late</t>
+  </si>
+  <si>
+    <t>permit somebody to do something / cho pe ai đó làm một cái gì đó</t>
+  </si>
+  <si>
+    <t>Hợp lệ, có hiệu lực</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>A valid passport is needed for traveling</t>
+  </si>
+  <si>
+    <t>valid passport / hộ chiếu có hiệu lực</t>
+  </si>
+  <si>
+    <t>Ổn định</t>
+  </si>
+  <si>
+    <t>Stable</t>
+  </si>
+  <si>
+    <t>The petrol price remains stable in recent times</t>
+  </si>
+  <si>
+    <t>remain stable / vẫn ổn định</t>
+  </si>
+  <si>
+    <t>Kẻ trộm</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>Stealing makes you a petty thief</t>
+  </si>
+  <si>
+    <t>petty thief / kẻ cắp vặt</t>
+  </si>
+  <si>
+    <t>Vệ tinh</t>
+  </si>
+  <si>
+    <t>Satellite</t>
+  </si>
+  <si>
+    <t>We can watch TV via satallite</t>
+  </si>
+  <si>
+    <t>via satellite / thông qua vệ tinh</t>
+  </si>
+  <si>
+    <t>Tên lửa</t>
+  </si>
+  <si>
+    <t>Rocket</t>
+  </si>
+  <si>
+    <t>Little boys love space rockets</t>
+  </si>
+  <si>
+    <t>space rocket / tên lửa vũ trụ</t>
+  </si>
+  <si>
+    <t>Vũ khí</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Police are armed (trang bị) with weapons</t>
+  </si>
+  <si>
+    <t>with a weapon / với một vũ khí</t>
+  </si>
+  <si>
+    <t>Lời cảnh cáo, cảnh báo</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>I received a warning for my mistake</t>
+  </si>
+  <si>
+    <t>receive a warning / nhận được một lời cảnh cáo</t>
+  </si>
+  <si>
+    <t>Hồ sơ</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>I set up a profile on FB</t>
+  </si>
+  <si>
+    <t>set up a profile / thiết lập hồ sơ cá nhân</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>I will help you select an option for your travel plan</t>
+  </si>
+  <si>
+    <t>select something / lựa chọn một cái gì đó</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Can you edit my essay?</t>
+  </si>
+  <si>
+    <t>edit something / chỉnh sửa một cái gì đó</t>
+  </si>
+  <si>
+    <t>Giới hạn</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Mother limited me to playing once a day.</t>
+  </si>
+  <si>
+    <t>limit somebody to something / giới hạn ai đó trong một việc gì đó</t>
+  </si>
+  <si>
+    <t>Sao lưu dữ liệu</t>
+  </si>
+  <si>
+    <t>Back up</t>
+  </si>
+  <si>
+    <t>You should back up your data</t>
+  </si>
+  <si>
+    <t>back up the data</t>
+  </si>
+  <si>
+    <t>Dữ liệu</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scientists gather data for research </t>
+  </si>
+  <si>
+    <t>gather data / thu thập dữ liệu</t>
+  </si>
+  <si>
+    <t>Thư viện</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Return the library book in 1 day</t>
+  </si>
+  <si>
+    <t>library book / sách thư viện</t>
+  </si>
+  <si>
+    <t>Tìm kiếm</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>I search for love</t>
+  </si>
+  <si>
+    <t>search for somebody or something</t>
+  </si>
+  <si>
+    <t>Tiêu chuẩn</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>All products must meet the quality standards</t>
+  </si>
+  <si>
+    <t>quality standards / các tiêu chuẩn chất lượng</t>
+  </si>
+  <si>
+    <t>Kho</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>The bags are still in storage</t>
+  </si>
+  <si>
+    <t>in storage / trong kho</t>
   </si>
 </sst>
 </file>
@@ -21281,10 +21719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1411"/>
+  <dimension ref="A1:G1441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1400" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1409" sqref="C1409"/>
+    <sheetView tabSelected="1" topLeftCell="A1436" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1455" sqref="C1455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -53292,6 +53730,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="1412" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1412" s="1" t="s">
+        <v>6962</v>
+      </c>
+      <c r="B1412" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1412" s="1" t="s">
+        <v>6992</v>
+      </c>
+      <c r="D1412" s="1" t="s">
+        <v>6993</v>
+      </c>
+      <c r="E1412" s="1" t="s">
+        <v>6994</v>
+      </c>
+      <c r="F1412" s="1" t="s">
+        <v>6995</v>
+      </c>
+      <c r="G1412" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1413" s="1" t="s">
+        <v>6963</v>
+      </c>
+      <c r="B1413" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1413" s="1" t="s">
+        <v>6996</v>
+      </c>
+      <c r="D1413" s="1" t="s">
+        <v>6997</v>
+      </c>
+      <c r="E1413" s="1" t="s">
+        <v>6998</v>
+      </c>
+      <c r="F1413" s="1" t="s">
+        <v>6999</v>
+      </c>
+      <c r="G1413" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1414" s="1" t="s">
+        <v>6964</v>
+      </c>
+      <c r="B1414" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1414" s="1" t="s">
+        <v>7000</v>
+      </c>
+      <c r="D1414" s="1" t="s">
+        <v>7001</v>
+      </c>
+      <c r="E1414" s="1" t="s">
+        <v>7002</v>
+      </c>
+      <c r="F1414" s="1" t="s">
+        <v>7003</v>
+      </c>
+      <c r="G1414" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1415" s="1" t="s">
+        <v>6965</v>
+      </c>
+      <c r="B1415" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1415" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="D1415" s="1" t="s">
+        <v>7004</v>
+      </c>
+      <c r="E1415" s="1" t="s">
+        <v>7005</v>
+      </c>
+      <c r="F1415" s="1" t="s">
+        <v>7006</v>
+      </c>
+      <c r="G1415" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1416" s="1" t="s">
+        <v>6966</v>
+      </c>
+      <c r="B1416" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1416" s="1" t="s">
+        <v>7007</v>
+      </c>
+      <c r="D1416" s="1" t="s">
+        <v>7008</v>
+      </c>
+      <c r="E1416" s="1" t="s">
+        <v>7009</v>
+      </c>
+      <c r="F1416" s="1" t="s">
+        <v>7010</v>
+      </c>
+      <c r="G1416" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1417" s="1" t="s">
+        <v>6967</v>
+      </c>
+      <c r="B1417" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1417" s="1" t="s">
+        <v>6933</v>
+      </c>
+      <c r="D1417" s="1" t="s">
+        <v>7011</v>
+      </c>
+      <c r="E1417" s="1" t="s">
+        <v>7012</v>
+      </c>
+      <c r="F1417" s="1" t="s">
+        <v>7013</v>
+      </c>
+      <c r="G1417" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1418" s="1" t="s">
+        <v>6968</v>
+      </c>
+      <c r="B1418" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1418" s="1" t="s">
+        <v>7014</v>
+      </c>
+      <c r="D1418" s="1" t="s">
+        <v>7015</v>
+      </c>
+      <c r="E1418" s="1" t="s">
+        <v>7016</v>
+      </c>
+      <c r="F1418" s="1" t="s">
+        <v>7017</v>
+      </c>
+      <c r="G1418" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1419" s="1" t="s">
+        <v>6969</v>
+      </c>
+      <c r="B1419" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1419" s="1" t="s">
+        <v>7018</v>
+      </c>
+      <c r="D1419" s="1" t="s">
+        <v>7019</v>
+      </c>
+      <c r="E1419" s="1" t="s">
+        <v>7020</v>
+      </c>
+      <c r="F1419" s="1" t="s">
+        <v>7021</v>
+      </c>
+      <c r="G1419" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1420" s="1" t="s">
+        <v>6970</v>
+      </c>
+      <c r="B1420" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1420" s="1" t="s">
+        <v>7022</v>
+      </c>
+      <c r="D1420" s="1" t="s">
+        <v>7023</v>
+      </c>
+      <c r="E1420" s="1" t="s">
+        <v>7024</v>
+      </c>
+      <c r="F1420" s="1" t="s">
+        <v>7025</v>
+      </c>
+      <c r="G1420" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1421" s="1" t="s">
+        <v>6971</v>
+      </c>
+      <c r="B1421" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1421" s="1" t="s">
+        <v>7026</v>
+      </c>
+      <c r="D1421" s="1" t="s">
+        <v>7027</v>
+      </c>
+      <c r="E1421" s="1" t="s">
+        <v>7028</v>
+      </c>
+      <c r="F1421" s="1" t="s">
+        <v>7029</v>
+      </c>
+      <c r="G1421" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1422" s="1" t="s">
+        <v>6972</v>
+      </c>
+      <c r="B1422" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1422" s="1" t="s">
+        <v>7030</v>
+      </c>
+      <c r="D1422" s="1" t="s">
+        <v>7031</v>
+      </c>
+      <c r="E1422" s="1" t="s">
+        <v>7032</v>
+      </c>
+      <c r="F1422" s="1" t="s">
+        <v>7033</v>
+      </c>
+      <c r="G1422" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1423" s="1" t="s">
+        <v>6973</v>
+      </c>
+      <c r="B1423" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1423" s="1" t="s">
+        <v>7034</v>
+      </c>
+      <c r="D1423" s="1" t="s">
+        <v>7035</v>
+      </c>
+      <c r="E1423" s="1" t="s">
+        <v>7036</v>
+      </c>
+      <c r="F1423" s="1" t="s">
+        <v>7037</v>
+      </c>
+      <c r="G1423" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1424" s="1" t="s">
+        <v>6974</v>
+      </c>
+      <c r="B1424" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1424" s="1" t="s">
+        <v>2407</v>
+      </c>
+      <c r="D1424" s="1" t="s">
+        <v>7038</v>
+      </c>
+      <c r="E1424" s="1" t="s">
+        <v>7039</v>
+      </c>
+      <c r="F1424" s="1" t="s">
+        <v>7040</v>
+      </c>
+      <c r="G1424" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1425" s="1" t="s">
+        <v>6975</v>
+      </c>
+      <c r="B1425" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1425" s="1" t="s">
+        <v>7041</v>
+      </c>
+      <c r="D1425" s="1" t="s">
+        <v>7042</v>
+      </c>
+      <c r="E1425" s="1" t="s">
+        <v>7043</v>
+      </c>
+      <c r="F1425" s="1" t="s">
+        <v>7044</v>
+      </c>
+      <c r="G1425" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1426" s="1" t="s">
+        <v>6976</v>
+      </c>
+      <c r="B1426" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1426" s="1" t="s">
+        <v>7045</v>
+      </c>
+      <c r="D1426" s="1" t="s">
+        <v>7046</v>
+      </c>
+      <c r="E1426" s="1" t="s">
+        <v>7047</v>
+      </c>
+      <c r="F1426" s="1" t="s">
+        <v>7048</v>
+      </c>
+      <c r="G1426" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1427" s="1" t="s">
+        <v>6977</v>
+      </c>
+      <c r="B1427" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1427" s="1" t="s">
+        <v>7049</v>
+      </c>
+      <c r="D1427" s="1" t="s">
+        <v>7050</v>
+      </c>
+      <c r="E1427" s="1" t="s">
+        <v>7051</v>
+      </c>
+      <c r="F1427" s="1" t="s">
+        <v>7052</v>
+      </c>
+      <c r="G1427" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1428" s="1" t="s">
+        <v>6978</v>
+      </c>
+      <c r="B1428" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1428" s="1" t="s">
+        <v>7053</v>
+      </c>
+      <c r="D1428" s="1" t="s">
+        <v>7054</v>
+      </c>
+      <c r="E1428" s="1" t="s">
+        <v>7055</v>
+      </c>
+      <c r="F1428" s="1" t="s">
+        <v>7056</v>
+      </c>
+      <c r="G1428" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1429" s="1" t="s">
+        <v>6979</v>
+      </c>
+      <c r="B1429" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1429" s="1" t="s">
+        <v>7057</v>
+      </c>
+      <c r="D1429" s="1" t="s">
+        <v>7058</v>
+      </c>
+      <c r="E1429" s="1" t="s">
+        <v>7059</v>
+      </c>
+      <c r="F1429" s="1" t="s">
+        <v>7060</v>
+      </c>
+      <c r="G1429" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1430" s="1" t="s">
+        <v>6980</v>
+      </c>
+      <c r="B1430" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1430" s="1" t="s">
+        <v>7061</v>
+      </c>
+      <c r="D1430" s="1" t="s">
+        <v>7062</v>
+      </c>
+      <c r="E1430" s="1" t="s">
+        <v>7063</v>
+      </c>
+      <c r="F1430" s="1" t="s">
+        <v>7064</v>
+      </c>
+      <c r="G1430" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1431" s="1" t="s">
+        <v>6981</v>
+      </c>
+      <c r="B1431" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1431" s="1" t="s">
+        <v>7065</v>
+      </c>
+      <c r="D1431" s="1" t="s">
+        <v>7066</v>
+      </c>
+      <c r="E1431" s="1" t="s">
+        <v>7067</v>
+      </c>
+      <c r="F1431" s="1" t="s">
+        <v>7068</v>
+      </c>
+      <c r="G1431" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1432" s="1" t="s">
+        <v>6982</v>
+      </c>
+      <c r="B1432" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1432" s="1" t="s">
+        <v>7069</v>
+      </c>
+      <c r="D1432" s="1" t="s">
+        <v>7070</v>
+      </c>
+      <c r="E1432" s="1" t="s">
+        <v>7071</v>
+      </c>
+      <c r="F1432" s="1" t="s">
+        <v>7072</v>
+      </c>
+      <c r="G1432" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1433" s="1" t="s">
+        <v>6983</v>
+      </c>
+      <c r="B1433" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1433" s="1" t="s">
+        <v>6325</v>
+      </c>
+      <c r="D1433" s="1" t="s">
+        <v>7073</v>
+      </c>
+      <c r="E1433" s="1" t="s">
+        <v>7074</v>
+      </c>
+      <c r="F1433" s="1" t="s">
+        <v>7075</v>
+      </c>
+      <c r="G1433" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1434" s="1" t="s">
+        <v>6984</v>
+      </c>
+      <c r="B1434" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1434" s="1" t="s">
+        <v>7076</v>
+      </c>
+      <c r="D1434" s="1" t="s">
+        <v>7077</v>
+      </c>
+      <c r="E1434" s="1" t="s">
+        <v>7078</v>
+      </c>
+      <c r="F1434" s="1" t="s">
+        <v>7079</v>
+      </c>
+      <c r="G1434" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1435" s="1" t="s">
+        <v>6985</v>
+      </c>
+      <c r="B1435" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1435" s="1" t="s">
+        <v>7080</v>
+      </c>
+      <c r="D1435" s="1" t="s">
+        <v>7081</v>
+      </c>
+      <c r="E1435" s="1" t="s">
+        <v>7082</v>
+      </c>
+      <c r="F1435" s="1" t="s">
+        <v>7083</v>
+      </c>
+      <c r="G1435" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1436" s="1" t="s">
+        <v>6986</v>
+      </c>
+      <c r="B1436" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1436" s="1" t="s">
+        <v>7084</v>
+      </c>
+      <c r="D1436" s="1" t="s">
+        <v>7085</v>
+      </c>
+      <c r="E1436" s="1" t="s">
+        <v>7086</v>
+      </c>
+      <c r="F1436" s="1" t="s">
+        <v>7087</v>
+      </c>
+      <c r="G1436" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1437" s="1" t="s">
+        <v>6987</v>
+      </c>
+      <c r="B1437" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1437" s="1" t="s">
+        <v>7088</v>
+      </c>
+      <c r="D1437" s="1" t="s">
+        <v>7089</v>
+      </c>
+      <c r="E1437" s="1" t="s">
+        <v>7090</v>
+      </c>
+      <c r="F1437" s="1" t="s">
+        <v>7091</v>
+      </c>
+      <c r="G1437" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1438" s="1" t="s">
+        <v>6988</v>
+      </c>
+      <c r="B1438" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1438" s="1" t="s">
+        <v>7092</v>
+      </c>
+      <c r="D1438" s="1" t="s">
+        <v>7093</v>
+      </c>
+      <c r="E1438" s="1" t="s">
+        <v>7094</v>
+      </c>
+      <c r="F1438" s="1" t="s">
+        <v>7095</v>
+      </c>
+      <c r="G1438" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1439" s="1" t="s">
+        <v>6989</v>
+      </c>
+      <c r="B1439" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1439" s="1" t="s">
+        <v>7096</v>
+      </c>
+      <c r="D1439" s="1" t="s">
+        <v>7097</v>
+      </c>
+      <c r="E1439" s="1" t="s">
+        <v>7098</v>
+      </c>
+      <c r="F1439" s="1" t="s">
+        <v>7099</v>
+      </c>
+      <c r="G1439" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1440" s="1" t="s">
+        <v>6990</v>
+      </c>
+      <c r="B1440" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1440" s="1" t="s">
+        <v>7100</v>
+      </c>
+      <c r="D1440" s="1" t="s">
+        <v>7101</v>
+      </c>
+      <c r="E1440" s="1" t="s">
+        <v>7102</v>
+      </c>
+      <c r="F1440" s="1" t="s">
+        <v>7103</v>
+      </c>
+      <c r="G1440" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1441" s="1" t="s">
+        <v>6991</v>
+      </c>
+      <c r="B1441" s="1">
+        <v>48</v>
+      </c>
+      <c r="C1441" s="1" t="s">
+        <v>7104</v>
+      </c>
+      <c r="D1441" s="1" t="s">
+        <v>7105</v>
+      </c>
+      <c r="E1441" s="1" t="s">
+        <v>7106</v>
+      </c>
+      <c r="F1441" s="1" t="s">
+        <v>7107</v>
+      </c>
+      <c r="G1441" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 49
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDAC7AD-13E2-0E4D-B3F4-4732377C64EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F79D6B-004C-594B-A43C-8F8189DAA12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8494" uniqueCount="7108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8674" uniqueCount="7256">
   <si>
     <t>ID</t>
   </si>
@@ -21354,6 +21354,450 @@
   </si>
   <si>
     <t>in storage / trong kho</t>
+  </si>
+  <si>
+    <t>U49_01</t>
+  </si>
+  <si>
+    <t>U49_02</t>
+  </si>
+  <si>
+    <t>U49_03</t>
+  </si>
+  <si>
+    <t>U49_04</t>
+  </si>
+  <si>
+    <t>U49_05</t>
+  </si>
+  <si>
+    <t>U49_06</t>
+  </si>
+  <si>
+    <t>U49_07</t>
+  </si>
+  <si>
+    <t>U49_08</t>
+  </si>
+  <si>
+    <t>U49_09</t>
+  </si>
+  <si>
+    <t>U49_10</t>
+  </si>
+  <si>
+    <t>U49_11</t>
+  </si>
+  <si>
+    <t>U49_12</t>
+  </si>
+  <si>
+    <t>U49_13</t>
+  </si>
+  <si>
+    <t>U49_14</t>
+  </si>
+  <si>
+    <t>U49_15</t>
+  </si>
+  <si>
+    <t>U49_16</t>
+  </si>
+  <si>
+    <t>U49_17</t>
+  </si>
+  <si>
+    <t>U49_18</t>
+  </si>
+  <si>
+    <t>U49_19</t>
+  </si>
+  <si>
+    <t>U49_20</t>
+  </si>
+  <si>
+    <t>U49_21</t>
+  </si>
+  <si>
+    <t>U49_22</t>
+  </si>
+  <si>
+    <t>U49_23</t>
+  </si>
+  <si>
+    <t>U49_24</t>
+  </si>
+  <si>
+    <t>U49_25</t>
+  </si>
+  <si>
+    <t>U49_26</t>
+  </si>
+  <si>
+    <t>U49_27</t>
+  </si>
+  <si>
+    <t>U49_28</t>
+  </si>
+  <si>
+    <t>U49_29</t>
+  </si>
+  <si>
+    <t>U49_30</t>
+  </si>
+  <si>
+    <t>Nhà tù</t>
+  </si>
+  <si>
+    <t>Prison</t>
+  </si>
+  <si>
+    <t>He will be in prison for murder</t>
+  </si>
+  <si>
+    <t>in prison for doing something / phải vào tù vì tội gì đó</t>
+  </si>
+  <si>
+    <t>Trốn thoát, thoát khỏi</t>
+  </si>
+  <si>
+    <t>Escape</t>
+  </si>
+  <si>
+    <t>She must escape from him</t>
+  </si>
+  <si>
+    <t>escape from somebody or something</t>
+  </si>
+  <si>
+    <t>Cướp</t>
+  </si>
+  <si>
+    <t>Rob</t>
+  </si>
+  <si>
+    <t>rob somebody or something</t>
+  </si>
+  <si>
+    <t>It is wrong to rob people / trộm cướp tài sản là điều sai trái</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đột nhập vào </t>
+  </si>
+  <si>
+    <t>Break into</t>
+  </si>
+  <si>
+    <t>Someone broke into my house</t>
+  </si>
+  <si>
+    <t>break into something / đột nhập vào một cái gì đó</t>
+  </si>
+  <si>
+    <t>Đuổi theo</t>
+  </si>
+  <si>
+    <t>Chase</t>
+  </si>
+  <si>
+    <t>Cats chase mice (chuột)</t>
+  </si>
+  <si>
+    <t>chase somebody or something / đuổi theo ai đó hoặc cái gì đó</t>
+  </si>
+  <si>
+    <t>Che giấu</t>
+  </si>
+  <si>
+    <t>Hide</t>
+  </si>
+  <si>
+    <t>hide somebody or something</t>
+  </si>
+  <si>
+    <t>They hide their money throughout the house (khắp nhà)</t>
+  </si>
+  <si>
+    <t>Tội phạm</t>
+  </si>
+  <si>
+    <t>Criminal</t>
+  </si>
+  <si>
+    <t>The convicted criminal pleaded guilty (nhận tội)</t>
+  </si>
+  <si>
+    <t>Convicted criminal / tội phạm bị kết án</t>
+  </si>
+  <si>
+    <t>Nạn nhân</t>
+  </si>
+  <si>
+    <t>Victim</t>
+  </si>
+  <si>
+    <t>He is a victim of his own greed (Anh ta là nạn nhân của lòng tham của chính mình)</t>
+  </si>
+  <si>
+    <t>a victim of something / nạn nhân của một cái gì đó</t>
+  </si>
+  <si>
+    <t>Luật sư</t>
+  </si>
+  <si>
+    <t>Lawyer</t>
+  </si>
+  <si>
+    <t>He needs to hire a criminal lawyer</t>
+  </si>
+  <si>
+    <t>a criminal lawyer / một luật sư hình sự</t>
+  </si>
+  <si>
+    <t>Có tội, có lỗi</t>
+  </si>
+  <si>
+    <t>Guilty</t>
+  </si>
+  <si>
+    <t>I feel guilty about lying to you</t>
+  </si>
+  <si>
+    <t>guilty about doing something / có lỗi vì làm điều gì đó</t>
+  </si>
+  <si>
+    <t>Tòa án</t>
+  </si>
+  <si>
+    <t>Court</t>
+  </si>
+  <si>
+    <t>He can be a witness in a civil court case</t>
+  </si>
+  <si>
+    <t>a civil court case / tòa án dân sự</t>
+  </si>
+  <si>
+    <t>Trường hợp</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>In case of emergency, here is my number</t>
+  </si>
+  <si>
+    <t>in case of something / trong trường hợp nào đó</t>
+  </si>
+  <si>
+    <t>Bằng chứng</t>
+  </si>
+  <si>
+    <t>Evidence</t>
+  </si>
+  <si>
+    <t>Scientists are looking for evidence of life on other planets (hành tinh)</t>
+  </si>
+  <si>
+    <t>evidence of something / bằng chứng của một cái gì đó</t>
+  </si>
+  <si>
+    <t>Sự có mặt, sự hiện diện</t>
+  </si>
+  <si>
+    <t>Presence</t>
+  </si>
+  <si>
+    <t>In the presence of her, I feel safe</t>
+  </si>
+  <si>
+    <t>in the presence of something or somebody</t>
+  </si>
+  <si>
+    <t>Seek</t>
+  </si>
+  <si>
+    <t>Make sure you seek help if you feel overwhelmed (quá tải)</t>
+  </si>
+  <si>
+    <t>Seek something or somebody / tìm kiếm một cái gì đó</t>
+  </si>
+  <si>
+    <t>An ninh</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>National security is a duty of government</t>
+  </si>
+  <si>
+    <t>Nation security / an ninh quốc gia</t>
+  </si>
+  <si>
+    <t>Độc ác, tàn nhẫn</t>
+  </si>
+  <si>
+    <t>Cruel</t>
+  </si>
+  <si>
+    <t>I am sorry that I was cruel to you</t>
+  </si>
+  <si>
+    <t>to be cruel to somebody or something</t>
+  </si>
+  <si>
+    <t>Liberty</t>
+  </si>
+  <si>
+    <t>Citizens have the liberty to voice concerns</t>
+  </si>
+  <si>
+    <t>Liberty to do something / tự do làm cái gì đó</t>
+  </si>
+  <si>
+    <t>Tấn công</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>attack somebody / tấn công ai đó</t>
+  </si>
+  <si>
+    <t>The burglar (tên trộm) attacked the civilian (người dân)</t>
+  </si>
+  <si>
+    <t>bạo lực</t>
+  </si>
+  <si>
+    <t>Violent</t>
+  </si>
+  <si>
+    <t>We don't have to be violent towards one another</t>
+  </si>
+  <si>
+    <t>violent towards or to somebody</t>
+  </si>
+  <si>
+    <t>Lan truyền</t>
+  </si>
+  <si>
+    <t>Spread</t>
+  </si>
+  <si>
+    <t>He spreads the word about her promotion</t>
+  </si>
+  <si>
+    <t>spread the word / loan tin</t>
+  </si>
+  <si>
+    <t>Lạm dụng, lợi dụng</t>
+  </si>
+  <si>
+    <t>Abuse</t>
+  </si>
+  <si>
+    <t>Be careful not to abuse alcohol</t>
+  </si>
+  <si>
+    <t>abuse alcohol / lạm dụng rượu</t>
+  </si>
+  <si>
+    <t>Chính phủ</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>There will be a high-level meeting among government officials</t>
+  </si>
+  <si>
+    <t>a government official / quan chức chính phủ</t>
+  </si>
+  <si>
+    <t>Luật, quy định</t>
+  </si>
+  <si>
+    <t>What is the law on drinking age?</t>
+  </si>
+  <si>
+    <t>law on something</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>Nhanh chóng</t>
+  </si>
+  <si>
+    <t>Rapid</t>
+  </si>
+  <si>
+    <t>The company is experiencing a rapid growth</t>
+  </si>
+  <si>
+    <t>rapid growth / sự tăng trưởng nhanh chóng</t>
+  </si>
+  <si>
+    <t>Theo pháp luật</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>We rely on (dựa vào) the legal system for justice</t>
+  </si>
+  <si>
+    <t>the legal system / hệ thống luật pháp</t>
+  </si>
+  <si>
+    <t>Sau cùng</t>
+  </si>
+  <si>
+    <t>Ultimate</t>
+  </si>
+  <si>
+    <t>Having a meaningful life is the ultimate target</t>
+  </si>
+  <si>
+    <t>ultimate target / mục tiêu cuối cùng</t>
+  </si>
+  <si>
+    <t>Cảnh nghèo nàn</t>
+  </si>
+  <si>
+    <t>Poverty</t>
+  </si>
+  <si>
+    <t>Some countries have extreme poverty</t>
+  </si>
+  <si>
+    <t>extreme poverty / tình trạng nghèo đói cùng cực</t>
+  </si>
+  <si>
+    <t>Ly dị</t>
+  </si>
+  <si>
+    <t>Divorce</t>
+  </si>
+  <si>
+    <t>In the past, wives of kings could never divorce their husbands</t>
+  </si>
+  <si>
+    <t>divorce someone</t>
+  </si>
+  <si>
+    <t>Tội giết người</t>
+  </si>
+  <si>
+    <t>Murder</t>
+  </si>
+  <si>
+    <t>The detective found out who murdered the victim</t>
+  </si>
+  <si>
+    <t>murder somebody / giết ai đó</t>
   </si>
 </sst>
 </file>
@@ -21719,10 +22163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1441"/>
+  <dimension ref="A1:G1471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1436" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1455" sqref="C1455"/>
+    <sheetView tabSelected="1" topLeftCell="C1451" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1472" sqref="C1472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -54420,6 +54864,696 @@
         <v>593</v>
       </c>
     </row>
+    <row r="1442" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1442" s="1" t="s">
+        <v>7108</v>
+      </c>
+      <c r="B1442" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1442" s="1" t="s">
+        <v>7138</v>
+      </c>
+      <c r="D1442" s="1" t="s">
+        <v>7139</v>
+      </c>
+      <c r="E1442" s="1" t="s">
+        <v>7140</v>
+      </c>
+      <c r="F1442" s="1" t="s">
+        <v>7141</v>
+      </c>
+      <c r="G1442" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1443" s="1" t="s">
+        <v>7109</v>
+      </c>
+      <c r="B1443" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1443" s="1" t="s">
+        <v>7142</v>
+      </c>
+      <c r="D1443" s="1" t="s">
+        <v>7143</v>
+      </c>
+      <c r="E1443" s="1" t="s">
+        <v>7144</v>
+      </c>
+      <c r="F1443" s="1" t="s">
+        <v>7145</v>
+      </c>
+      <c r="G1443" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1444" s="1" t="s">
+        <v>7110</v>
+      </c>
+      <c r="B1444" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1444" s="1" t="s">
+        <v>7146</v>
+      </c>
+      <c r="D1444" s="1" t="s">
+        <v>7147</v>
+      </c>
+      <c r="E1444" s="1" t="s">
+        <v>7149</v>
+      </c>
+      <c r="F1444" s="1" t="s">
+        <v>7148</v>
+      </c>
+      <c r="G1444" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1445" s="1" t="s">
+        <v>7111</v>
+      </c>
+      <c r="B1445" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1445" s="1" t="s">
+        <v>7150</v>
+      </c>
+      <c r="D1445" s="1" t="s">
+        <v>7151</v>
+      </c>
+      <c r="E1445" s="1" t="s">
+        <v>7152</v>
+      </c>
+      <c r="F1445" s="1" t="s">
+        <v>7153</v>
+      </c>
+      <c r="G1445" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1446" s="1" t="s">
+        <v>7112</v>
+      </c>
+      <c r="B1446" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1446" s="1" t="s">
+        <v>7154</v>
+      </c>
+      <c r="D1446" s="1" t="s">
+        <v>7155</v>
+      </c>
+      <c r="E1446" s="1" t="s">
+        <v>7156</v>
+      </c>
+      <c r="F1446" s="1" t="s">
+        <v>7157</v>
+      </c>
+      <c r="G1446" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1447" s="1" t="s">
+        <v>7113</v>
+      </c>
+      <c r="B1447" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1447" s="1" t="s">
+        <v>7158</v>
+      </c>
+      <c r="D1447" s="1" t="s">
+        <v>7159</v>
+      </c>
+      <c r="E1447" s="1" t="s">
+        <v>7161</v>
+      </c>
+      <c r="F1447" s="1" t="s">
+        <v>7160</v>
+      </c>
+      <c r="G1447" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1448" s="1" t="s">
+        <v>7114</v>
+      </c>
+      <c r="B1448" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1448" s="1" t="s">
+        <v>7162</v>
+      </c>
+      <c r="D1448" s="1" t="s">
+        <v>7163</v>
+      </c>
+      <c r="E1448" s="1" t="s">
+        <v>7164</v>
+      </c>
+      <c r="F1448" s="1" t="s">
+        <v>7165</v>
+      </c>
+      <c r="G1448" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1449" s="1" t="s">
+        <v>7115</v>
+      </c>
+      <c r="B1449" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1449" s="1" t="s">
+        <v>7166</v>
+      </c>
+      <c r="D1449" s="1" t="s">
+        <v>7167</v>
+      </c>
+      <c r="E1449" s="1" t="s">
+        <v>7168</v>
+      </c>
+      <c r="F1449" s="1" t="s">
+        <v>7169</v>
+      </c>
+      <c r="G1449" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1450" s="1" t="s">
+        <v>7116</v>
+      </c>
+      <c r="B1450" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1450" s="1" t="s">
+        <v>7170</v>
+      </c>
+      <c r="D1450" s="1" t="s">
+        <v>7171</v>
+      </c>
+      <c r="E1450" s="1" t="s">
+        <v>7172</v>
+      </c>
+      <c r="F1450" s="1" t="s">
+        <v>7173</v>
+      </c>
+      <c r="G1450" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1451" s="1" t="s">
+        <v>7117</v>
+      </c>
+      <c r="B1451" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1451" s="1" t="s">
+        <v>7174</v>
+      </c>
+      <c r="D1451" s="1" t="s">
+        <v>7175</v>
+      </c>
+      <c r="E1451" s="1" t="s">
+        <v>7176</v>
+      </c>
+      <c r="F1451" s="1" t="s">
+        <v>7177</v>
+      </c>
+      <c r="G1451" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1452" s="1" t="s">
+        <v>7118</v>
+      </c>
+      <c r="B1452" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1452" s="1" t="s">
+        <v>7178</v>
+      </c>
+      <c r="D1452" s="1" t="s">
+        <v>7179</v>
+      </c>
+      <c r="E1452" s="1" t="s">
+        <v>7180</v>
+      </c>
+      <c r="F1452" s="1" t="s">
+        <v>7181</v>
+      </c>
+      <c r="G1452" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1453" s="1" t="s">
+        <v>7119</v>
+      </c>
+      <c r="B1453" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1453" s="1" t="s">
+        <v>7182</v>
+      </c>
+      <c r="D1453" s="1" t="s">
+        <v>7183</v>
+      </c>
+      <c r="E1453" s="1" t="s">
+        <v>7184</v>
+      </c>
+      <c r="F1453" s="1" t="s">
+        <v>7185</v>
+      </c>
+      <c r="G1453" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1454" s="1" t="s">
+        <v>7120</v>
+      </c>
+      <c r="B1454" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1454" s="1" t="s">
+        <v>7186</v>
+      </c>
+      <c r="D1454" s="1" t="s">
+        <v>7187</v>
+      </c>
+      <c r="E1454" s="1" t="s">
+        <v>7188</v>
+      </c>
+      <c r="F1454" s="1" t="s">
+        <v>7189</v>
+      </c>
+      <c r="G1454" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1455" s="1" t="s">
+        <v>7121</v>
+      </c>
+      <c r="B1455" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1455" s="1" t="s">
+        <v>7190</v>
+      </c>
+      <c r="D1455" s="1" t="s">
+        <v>7191</v>
+      </c>
+      <c r="E1455" s="1" t="s">
+        <v>7192</v>
+      </c>
+      <c r="F1455" s="1" t="s">
+        <v>7193</v>
+      </c>
+      <c r="G1455" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1456" s="1" t="s">
+        <v>7122</v>
+      </c>
+      <c r="B1456" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1456" s="1" t="s">
+        <v>7096</v>
+      </c>
+      <c r="D1456" s="1" t="s">
+        <v>7194</v>
+      </c>
+      <c r="E1456" s="1" t="s">
+        <v>7195</v>
+      </c>
+      <c r="F1456" s="1" t="s">
+        <v>7196</v>
+      </c>
+      <c r="G1456" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1457" s="1" t="s">
+        <v>7123</v>
+      </c>
+      <c r="B1457" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1457" s="1" t="s">
+        <v>7197</v>
+      </c>
+      <c r="D1457" s="1" t="s">
+        <v>7198</v>
+      </c>
+      <c r="E1457" s="1" t="s">
+        <v>7199</v>
+      </c>
+      <c r="F1457" s="1" t="s">
+        <v>7200</v>
+      </c>
+      <c r="G1457" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1458" s="1" t="s">
+        <v>7124</v>
+      </c>
+      <c r="B1458" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1458" s="1" t="s">
+        <v>7201</v>
+      </c>
+      <c r="D1458" s="1" t="s">
+        <v>7202</v>
+      </c>
+      <c r="E1458" s="1" t="s">
+        <v>7203</v>
+      </c>
+      <c r="F1458" s="1" t="s">
+        <v>7204</v>
+      </c>
+      <c r="G1458" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1459" s="1" t="s">
+        <v>7125</v>
+      </c>
+      <c r="B1459" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1459" s="1" t="s">
+        <v>6591</v>
+      </c>
+      <c r="D1459" s="1" t="s">
+        <v>7205</v>
+      </c>
+      <c r="E1459" s="1" t="s">
+        <v>7206</v>
+      </c>
+      <c r="F1459" s="1" t="s">
+        <v>7207</v>
+      </c>
+      <c r="G1459" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1460" s="1" t="s">
+        <v>7126</v>
+      </c>
+      <c r="B1460" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1460" s="1" t="s">
+        <v>7208</v>
+      </c>
+      <c r="D1460" s="1" t="s">
+        <v>7209</v>
+      </c>
+      <c r="E1460" s="1" t="s">
+        <v>7211</v>
+      </c>
+      <c r="F1460" s="1" t="s">
+        <v>7210</v>
+      </c>
+      <c r="G1460" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1461" s="1" t="s">
+        <v>7127</v>
+      </c>
+      <c r="B1461" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1461" s="1" t="s">
+        <v>7212</v>
+      </c>
+      <c r="D1461" s="1" t="s">
+        <v>7213</v>
+      </c>
+      <c r="E1461" s="1" t="s">
+        <v>7214</v>
+      </c>
+      <c r="F1461" s="1" t="s">
+        <v>7215</v>
+      </c>
+      <c r="G1461" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1462" s="1" t="s">
+        <v>7128</v>
+      </c>
+      <c r="B1462" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1462" s="1" t="s">
+        <v>7216</v>
+      </c>
+      <c r="D1462" s="1" t="s">
+        <v>7217</v>
+      </c>
+      <c r="E1462" s="1" t="s">
+        <v>7218</v>
+      </c>
+      <c r="F1462" s="1" t="s">
+        <v>7219</v>
+      </c>
+      <c r="G1462" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1463" s="1" t="s">
+        <v>7129</v>
+      </c>
+      <c r="B1463" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1463" s="1" t="s">
+        <v>7220</v>
+      </c>
+      <c r="D1463" s="1" t="s">
+        <v>7221</v>
+      </c>
+      <c r="E1463" s="1" t="s">
+        <v>7222</v>
+      </c>
+      <c r="F1463" s="1" t="s">
+        <v>7223</v>
+      </c>
+      <c r="G1463" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1464" s="1" t="s">
+        <v>7130</v>
+      </c>
+      <c r="B1464" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1464" s="1" t="s">
+        <v>7224</v>
+      </c>
+      <c r="D1464" s="1" t="s">
+        <v>7225</v>
+      </c>
+      <c r="E1464" s="1" t="s">
+        <v>7226</v>
+      </c>
+      <c r="F1464" s="1" t="s">
+        <v>7227</v>
+      </c>
+      <c r="G1464" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1465" s="1" t="s">
+        <v>7131</v>
+      </c>
+      <c r="B1465" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1465" s="1" t="s">
+        <v>7228</v>
+      </c>
+      <c r="D1465" s="1" t="s">
+        <v>7231</v>
+      </c>
+      <c r="E1465" s="1" t="s">
+        <v>7229</v>
+      </c>
+      <c r="F1465" s="1" t="s">
+        <v>7230</v>
+      </c>
+      <c r="G1465" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1466" s="1" t="s">
+        <v>7132</v>
+      </c>
+      <c r="B1466" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1466" s="1" t="s">
+        <v>7232</v>
+      </c>
+      <c r="D1466" s="1" t="s">
+        <v>7233</v>
+      </c>
+      <c r="E1466" s="1" t="s">
+        <v>7234</v>
+      </c>
+      <c r="F1466" s="1" t="s">
+        <v>7235</v>
+      </c>
+      <c r="G1466" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1467" s="1" t="s">
+        <v>7133</v>
+      </c>
+      <c r="B1467" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1467" s="1" t="s">
+        <v>7236</v>
+      </c>
+      <c r="D1467" s="1" t="s">
+        <v>7237</v>
+      </c>
+      <c r="E1467" s="1" t="s">
+        <v>7238</v>
+      </c>
+      <c r="F1467" s="1" t="s">
+        <v>7239</v>
+      </c>
+      <c r="G1467" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1468" s="1" t="s">
+        <v>7134</v>
+      </c>
+      <c r="B1468" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1468" s="1" t="s">
+        <v>7240</v>
+      </c>
+      <c r="D1468" s="1" t="s">
+        <v>7241</v>
+      </c>
+      <c r="E1468" s="1" t="s">
+        <v>7242</v>
+      </c>
+      <c r="F1468" s="1" t="s">
+        <v>7243</v>
+      </c>
+      <c r="G1468" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1469" s="1" t="s">
+        <v>7135</v>
+      </c>
+      <c r="B1469" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1469" s="1" t="s">
+        <v>7244</v>
+      </c>
+      <c r="D1469" s="1" t="s">
+        <v>7245</v>
+      </c>
+      <c r="E1469" s="1" t="s">
+        <v>7246</v>
+      </c>
+      <c r="F1469" s="1" t="s">
+        <v>7247</v>
+      </c>
+      <c r="G1469" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1470" s="1" t="s">
+        <v>7136</v>
+      </c>
+      <c r="B1470" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1470" s="1" t="s">
+        <v>7248</v>
+      </c>
+      <c r="D1470" s="1" t="s">
+        <v>7249</v>
+      </c>
+      <c r="E1470" s="1" t="s">
+        <v>7250</v>
+      </c>
+      <c r="F1470" s="1" t="s">
+        <v>7251</v>
+      </c>
+      <c r="G1470" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1471" s="1" t="s">
+        <v>7137</v>
+      </c>
+      <c r="B1471" s="1">
+        <v>49</v>
+      </c>
+      <c r="C1471" s="1" t="s">
+        <v>7252</v>
+      </c>
+      <c r="D1471" s="1" t="s">
+        <v>7253</v>
+      </c>
+      <c r="E1471" s="1" t="s">
+        <v>7254</v>
+      </c>
+      <c r="F1471" s="1" t="s">
+        <v>7255</v>
+      </c>
+      <c r="G1471" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add list of words for unit 50
</commit_message>
<xml_diff>
--- a/data/WordStudy.xlsx
+++ b/data/WordStudy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Documents/Dom/english-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F79D6B-004C-594B-A43C-8F8189DAA12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B727ED24-7C53-4142-9FBA-7118AC594ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="500" windowWidth="20820" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8674" uniqueCount="7256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8854" uniqueCount="7404">
   <si>
     <t>ID</t>
   </si>
@@ -21798,6 +21798,450 @@
   </si>
   <si>
     <t>murder somebody / giết ai đó</t>
+  </si>
+  <si>
+    <t>U50_01</t>
+  </si>
+  <si>
+    <t>U50_02</t>
+  </si>
+  <si>
+    <t>U50_03</t>
+  </si>
+  <si>
+    <t>U50_04</t>
+  </si>
+  <si>
+    <t>U50_05</t>
+  </si>
+  <si>
+    <t>U50_06</t>
+  </si>
+  <si>
+    <t>U50_07</t>
+  </si>
+  <si>
+    <t>U50_08</t>
+  </si>
+  <si>
+    <t>U50_09</t>
+  </si>
+  <si>
+    <t>U50_10</t>
+  </si>
+  <si>
+    <t>U50_11</t>
+  </si>
+  <si>
+    <t>U50_12</t>
+  </si>
+  <si>
+    <t>U50_13</t>
+  </si>
+  <si>
+    <t>U50_14</t>
+  </si>
+  <si>
+    <t>U50_15</t>
+  </si>
+  <si>
+    <t>U50_16</t>
+  </si>
+  <si>
+    <t>U50_17</t>
+  </si>
+  <si>
+    <t>U50_18</t>
+  </si>
+  <si>
+    <t>U50_19</t>
+  </si>
+  <si>
+    <t>U50_20</t>
+  </si>
+  <si>
+    <t>U50_21</t>
+  </si>
+  <si>
+    <t>U50_22</t>
+  </si>
+  <si>
+    <t>U50_23</t>
+  </si>
+  <si>
+    <t>U50_24</t>
+  </si>
+  <si>
+    <t>U50_25</t>
+  </si>
+  <si>
+    <t>U50_26</t>
+  </si>
+  <si>
+    <t>U50_27</t>
+  </si>
+  <si>
+    <t>U50_28</t>
+  </si>
+  <si>
+    <t>U50_29</t>
+  </si>
+  <si>
+    <t>U50_30</t>
+  </si>
+  <si>
+    <t>Tạp chí</t>
+  </si>
+  <si>
+    <t>magazine</t>
+  </si>
+  <si>
+    <t>Online magazines are convenient to read</t>
+  </si>
+  <si>
+    <t>online magazine / tạp chí điện tử</t>
+  </si>
+  <si>
+    <t>Loài động vật</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Many fish species are in the ocean</t>
+  </si>
+  <si>
+    <t>fish species / loài cá</t>
+  </si>
+  <si>
+    <t>extinction</t>
+  </si>
+  <si>
+    <t>Tigers are on the verge of extinction</t>
+  </si>
+  <si>
+    <t>on the verge of extinction / trên bờ vực tuyệt chủng</t>
+  </si>
+  <si>
+    <t>Sự tuyệt chủng</t>
+  </si>
+  <si>
+    <t>Hành tinh</t>
+  </si>
+  <si>
+    <t>Planet</t>
+  </si>
+  <si>
+    <t>The planet Earth is warming up</t>
+  </si>
+  <si>
+    <t>the planet earth / hành tinh trái đất</t>
+  </si>
+  <si>
+    <t>Quyên góp</t>
+  </si>
+  <si>
+    <t>Donate</t>
+  </si>
+  <si>
+    <t>Will you donate money to charity?</t>
+  </si>
+  <si>
+    <t>donate something to somebody or something</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổ chức </t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>The WHO is an international organization.</t>
+  </si>
+  <si>
+    <t>International organization / tổ chức quốc tế</t>
+  </si>
+  <si>
+    <t>Dân số</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>The working population is increasing each year</t>
+  </si>
+  <si>
+    <t>working population / số người lao động</t>
+  </si>
+  <si>
+    <t>Khí hậu</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>Dalat is famous for its mild climate</t>
+  </si>
+  <si>
+    <t>mild climate / khí hậu ôn hòa</t>
+  </si>
+  <si>
+    <t>Nước thải</t>
+  </si>
+  <si>
+    <t>Sewage</t>
+  </si>
+  <si>
+    <t>Raw sewage is dangerous to human health</t>
+  </si>
+  <si>
+    <t>raw sewage / nước thải chưa qua xử lý</t>
+  </si>
+  <si>
+    <t>Sự bảo tồn</t>
+  </si>
+  <si>
+    <t>Conservation</t>
+  </si>
+  <si>
+    <t>Wildlife conservation is necessary to save animals</t>
+  </si>
+  <si>
+    <t>wildlife conservation / bảo tồn động vật hoang dã</t>
+  </si>
+  <si>
+    <t>Tồn tại</t>
+  </si>
+  <si>
+    <t>Exist</t>
+  </si>
+  <si>
+    <t>Trees exist to provide oxygen</t>
+  </si>
+  <si>
+    <t>exist to do something / tồn tại để làm cái gì đó</t>
+  </si>
+  <si>
+    <t>Cuộc bầu cử</t>
+  </si>
+  <si>
+    <t>Election</t>
+  </si>
+  <si>
+    <t>Citizens can vote at the national election</t>
+  </si>
+  <si>
+    <t>national election / cuộc bầu cử toàn quốc</t>
+  </si>
+  <si>
+    <t>Bầu chọn</t>
+  </si>
+  <si>
+    <t>Vote</t>
+  </si>
+  <si>
+    <t>I voted for the new president (tổng thống)</t>
+  </si>
+  <si>
+    <t>vote for somebody / bầu chọn cho ai đó</t>
+  </si>
+  <si>
+    <t>Chính trị</t>
+  </si>
+  <si>
+    <t>Politics</t>
+  </si>
+  <si>
+    <t>Employees should avoid office politics</t>
+  </si>
+  <si>
+    <t>office politics / chính trị công sở</t>
+  </si>
+  <si>
+    <t>Tổng thống</t>
+  </si>
+  <si>
+    <t>President</t>
+  </si>
+  <si>
+    <t>an acting president / quyền tổng thống</t>
+  </si>
+  <si>
+    <t>He is serving as acting president of the country (ông ấy đang đảm nhiệm chức vụ quyền tổng thống của đất nước)</t>
+  </si>
+  <si>
+    <t>Chiến dịch</t>
+  </si>
+  <si>
+    <t>Campaign</t>
+  </si>
+  <si>
+    <t>We should start a campaign to save animals</t>
+  </si>
+  <si>
+    <t>a campaign to do something</t>
+  </si>
+  <si>
+    <t>Lính</t>
+  </si>
+  <si>
+    <t>Soldier</t>
+  </si>
+  <si>
+    <t>There are soldiers on duty around the embassy (đại sứ quán)</t>
+  </si>
+  <si>
+    <t>a soldier on duty / một người lính đang làm nhiệm vụ</t>
+  </si>
+  <si>
+    <t>Quân đội</t>
+  </si>
+  <si>
+    <t>Army</t>
+  </si>
+  <si>
+    <t>My brother is in the army</t>
+  </si>
+  <si>
+    <t>in the army / trong quân đội</t>
+  </si>
+  <si>
+    <t>Medal</t>
+  </si>
+  <si>
+    <t>Huân chương</t>
+  </si>
+  <si>
+    <t>She was given a medal of honor</t>
+  </si>
+  <si>
+    <t>a medal of honor / một huân chương danh dự</t>
+  </si>
+  <si>
+    <t>Phi công</t>
+  </si>
+  <si>
+    <t>Pilot</t>
+  </si>
+  <si>
+    <t>I am studying to be an airline pilot</t>
+  </si>
+  <si>
+    <t>an airline pilot / một phi công hàng không</t>
+  </si>
+  <si>
+    <t>Ví dụ, mẫu</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Doctors will take a sample of your blood</t>
+  </si>
+  <si>
+    <t>a sample of something / một mẫu của một cái gì đó</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>This section of the book is interesting</t>
+  </si>
+  <si>
+    <t>a section of something</t>
+  </si>
+  <si>
+    <t>Ồ ạt</t>
+  </si>
+  <si>
+    <t>Massive</t>
+  </si>
+  <si>
+    <t>a massive attack / một cuộc tấn công lớn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The army launched (phát động) a massive attack on the enemy </t>
+  </si>
+  <si>
+    <t>Occur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earthquakes occur frequently in Japan </t>
+  </si>
+  <si>
+    <t>Occur frequently / xãy ra thường xuyên</t>
+  </si>
+  <si>
+    <t>Mạnh mẽ, đầy uy lực</t>
+  </si>
+  <si>
+    <t>Powerful</t>
+  </si>
+  <si>
+    <t>The speaker had a  powerful voice</t>
+  </si>
+  <si>
+    <t>a powerful voice / một giọng nói đầy uy lực</t>
+  </si>
+  <si>
+    <t>Phong trào</t>
+  </si>
+  <si>
+    <t>Movement</t>
+  </si>
+  <si>
+    <t>A social movement can significantly (ảnh hưởng) shape a society</t>
+  </si>
+  <si>
+    <t>a social movement / một phong trào xã hội</t>
+  </si>
+  <si>
+    <t>Cuộc cách mạng</t>
+  </si>
+  <si>
+    <t>Revolution</t>
+  </si>
+  <si>
+    <t>The activists (nhà hoạt động xã hội) started a revolution</t>
+  </si>
+  <si>
+    <t>start a revolution / bắt đầu một cuộc cách mạng</t>
+  </si>
+  <si>
+    <t>Hiệp hội</t>
+  </si>
+  <si>
+    <t>Union</t>
+  </si>
+  <si>
+    <t>You can join a labor union</t>
+  </si>
+  <si>
+    <t>labor union / công đoàn</t>
+  </si>
+  <si>
+    <t>Giải cứu</t>
+  </si>
+  <si>
+    <t>Rescue</t>
+  </si>
+  <si>
+    <t>The koala (Chú gấu) was rescued from the fire</t>
+  </si>
+  <si>
+    <t>rescue from something / giải cứu khỏi cái gì đó</t>
+  </si>
+  <si>
+    <t>Bắt buộc</t>
+  </si>
+  <si>
+    <t>force</t>
+  </si>
+  <si>
+    <t>They forced me to clean the dishes</t>
+  </si>
+  <si>
+    <t>force something or someone / bắt buộc một cái gì đó hoặc ai đó</t>
   </si>
 </sst>
 </file>
@@ -22163,10 +22607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1471"/>
+  <dimension ref="A1:G1501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1451" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1472" sqref="C1472"/>
+    <sheetView tabSelected="1" topLeftCell="A1478" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1514" sqref="C1488:C1514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -55554,6 +55998,696 @@
         <v>577</v>
       </c>
     </row>
+    <row r="1472" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1472" s="1" t="s">
+        <v>7256</v>
+      </c>
+      <c r="B1472" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1472" s="1" t="s">
+        <v>7286</v>
+      </c>
+      <c r="D1472" s="1" t="s">
+        <v>7287</v>
+      </c>
+      <c r="E1472" s="1" t="s">
+        <v>7288</v>
+      </c>
+      <c r="F1472" s="1" t="s">
+        <v>7289</v>
+      </c>
+      <c r="G1472" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1473" s="1" t="s">
+        <v>7257</v>
+      </c>
+      <c r="B1473" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1473" s="1" t="s">
+        <v>7290</v>
+      </c>
+      <c r="D1473" s="1" t="s">
+        <v>7291</v>
+      </c>
+      <c r="E1473" s="1" t="s">
+        <v>7292</v>
+      </c>
+      <c r="F1473" s="1" t="s">
+        <v>7293</v>
+      </c>
+      <c r="G1473" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1474" s="1" t="s">
+        <v>7258</v>
+      </c>
+      <c r="B1474" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1474" s="1" t="s">
+        <v>7297</v>
+      </c>
+      <c r="D1474" s="1" t="s">
+        <v>7294</v>
+      </c>
+      <c r="E1474" s="1" t="s">
+        <v>7295</v>
+      </c>
+      <c r="F1474" s="1" t="s">
+        <v>7296</v>
+      </c>
+      <c r="G1474" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1475" s="1" t="s">
+        <v>7259</v>
+      </c>
+      <c r="B1475" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1475" s="1" t="s">
+        <v>7298</v>
+      </c>
+      <c r="D1475" s="1" t="s">
+        <v>7299</v>
+      </c>
+      <c r="E1475" s="1" t="s">
+        <v>7300</v>
+      </c>
+      <c r="F1475" s="1" t="s">
+        <v>7301</v>
+      </c>
+      <c r="G1475" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1476" s="1" t="s">
+        <v>7260</v>
+      </c>
+      <c r="B1476" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1476" s="1" t="s">
+        <v>7302</v>
+      </c>
+      <c r="D1476" s="1" t="s">
+        <v>7303</v>
+      </c>
+      <c r="E1476" s="1" t="s">
+        <v>7304</v>
+      </c>
+      <c r="F1476" s="1" t="s">
+        <v>7305</v>
+      </c>
+      <c r="G1476" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1477" s="1" t="s">
+        <v>7261</v>
+      </c>
+      <c r="B1477" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1477" s="1" t="s">
+        <v>7306</v>
+      </c>
+      <c r="D1477" s="1" t="s">
+        <v>7307</v>
+      </c>
+      <c r="E1477" s="1" t="s">
+        <v>7308</v>
+      </c>
+      <c r="F1477" s="1" t="s">
+        <v>7309</v>
+      </c>
+      <c r="G1477" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1478" s="1" t="s">
+        <v>7262</v>
+      </c>
+      <c r="B1478" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1478" s="1" t="s">
+        <v>7310</v>
+      </c>
+      <c r="D1478" s="1" t="s">
+        <v>7311</v>
+      </c>
+      <c r="E1478" s="1" t="s">
+        <v>7312</v>
+      </c>
+      <c r="F1478" s="1" t="s">
+        <v>7313</v>
+      </c>
+      <c r="G1478" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1479" s="1" t="s">
+        <v>7263</v>
+      </c>
+      <c r="B1479" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1479" s="1" t="s">
+        <v>7314</v>
+      </c>
+      <c r="D1479" s="1" t="s">
+        <v>7315</v>
+      </c>
+      <c r="E1479" s="1" t="s">
+        <v>7316</v>
+      </c>
+      <c r="F1479" s="1" t="s">
+        <v>7317</v>
+      </c>
+      <c r="G1479" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1480" s="1" t="s">
+        <v>7264</v>
+      </c>
+      <c r="B1480" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1480" s="1" t="s">
+        <v>7318</v>
+      </c>
+      <c r="D1480" s="1" t="s">
+        <v>7319</v>
+      </c>
+      <c r="E1480" s="1" t="s">
+        <v>7320</v>
+      </c>
+      <c r="F1480" s="1" t="s">
+        <v>7321</v>
+      </c>
+      <c r="G1480" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1481" s="1" t="s">
+        <v>7265</v>
+      </c>
+      <c r="B1481" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1481" s="1" t="s">
+        <v>7322</v>
+      </c>
+      <c r="D1481" s="1" t="s">
+        <v>7323</v>
+      </c>
+      <c r="E1481" s="1" t="s">
+        <v>7324</v>
+      </c>
+      <c r="F1481" s="1" t="s">
+        <v>7325</v>
+      </c>
+      <c r="G1481" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1482" s="1" t="s">
+        <v>7266</v>
+      </c>
+      <c r="B1482" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1482" s="1" t="s">
+        <v>7326</v>
+      </c>
+      <c r="D1482" s="1" t="s">
+        <v>7327</v>
+      </c>
+      <c r="E1482" s="1" t="s">
+        <v>7328</v>
+      </c>
+      <c r="F1482" s="1" t="s">
+        <v>7329</v>
+      </c>
+      <c r="G1482" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1483" s="1" t="s">
+        <v>7267</v>
+      </c>
+      <c r="B1483" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1483" s="1" t="s">
+        <v>7330</v>
+      </c>
+      <c r="D1483" s="1" t="s">
+        <v>7331</v>
+      </c>
+      <c r="E1483" s="1" t="s">
+        <v>7332</v>
+      </c>
+      <c r="F1483" s="1" t="s">
+        <v>7333</v>
+      </c>
+      <c r="G1483" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1484" s="1" t="s">
+        <v>7268</v>
+      </c>
+      <c r="B1484" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1484" s="1" t="s">
+        <v>7334</v>
+      </c>
+      <c r="D1484" s="1" t="s">
+        <v>7335</v>
+      </c>
+      <c r="E1484" s="1" t="s">
+        <v>7336</v>
+      </c>
+      <c r="F1484" s="1" t="s">
+        <v>7337</v>
+      </c>
+      <c r="G1484" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1485" s="1" t="s">
+        <v>7269</v>
+      </c>
+      <c r="B1485" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1485" s="1" t="s">
+        <v>7338</v>
+      </c>
+      <c r="D1485" s="1" t="s">
+        <v>7339</v>
+      </c>
+      <c r="E1485" s="1" t="s">
+        <v>7340</v>
+      </c>
+      <c r="F1485" s="1" t="s">
+        <v>7341</v>
+      </c>
+      <c r="G1485" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1486" s="1" t="s">
+        <v>7270</v>
+      </c>
+      <c r="B1486" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1486" s="1" t="s">
+        <v>7342</v>
+      </c>
+      <c r="D1486" s="1" t="s">
+        <v>7343</v>
+      </c>
+      <c r="E1486" s="1" t="s">
+        <v>7345</v>
+      </c>
+      <c r="F1486" s="1" t="s">
+        <v>7344</v>
+      </c>
+      <c r="G1486" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1487" s="1" t="s">
+        <v>7271</v>
+      </c>
+      <c r="B1487" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1487" s="1" t="s">
+        <v>7346</v>
+      </c>
+      <c r="D1487" s="1" t="s">
+        <v>7347</v>
+      </c>
+      <c r="E1487" s="1" t="s">
+        <v>7348</v>
+      </c>
+      <c r="F1487" s="1" t="s">
+        <v>7349</v>
+      </c>
+      <c r="G1487" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1488" s="1" t="s">
+        <v>7272</v>
+      </c>
+      <c r="B1488" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1488" s="1" t="s">
+        <v>7350</v>
+      </c>
+      <c r="D1488" s="1" t="s">
+        <v>7351</v>
+      </c>
+      <c r="E1488" s="1" t="s">
+        <v>7352</v>
+      </c>
+      <c r="F1488" s="1" t="s">
+        <v>7353</v>
+      </c>
+      <c r="G1488" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1489" s="1" t="s">
+        <v>7273</v>
+      </c>
+      <c r="B1489" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1489" s="1" t="s">
+        <v>7354</v>
+      </c>
+      <c r="D1489" s="1" t="s">
+        <v>7355</v>
+      </c>
+      <c r="E1489" s="1" t="s">
+        <v>7356</v>
+      </c>
+      <c r="F1489" s="1" t="s">
+        <v>7357</v>
+      </c>
+      <c r="G1489" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1490" s="1" t="s">
+        <v>7274</v>
+      </c>
+      <c r="B1490" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1490" s="1" t="s">
+        <v>7359</v>
+      </c>
+      <c r="D1490" s="1" t="s">
+        <v>7358</v>
+      </c>
+      <c r="E1490" s="1" t="s">
+        <v>7360</v>
+      </c>
+      <c r="F1490" s="1" t="s">
+        <v>7361</v>
+      </c>
+      <c r="G1490" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1491" s="1" t="s">
+        <v>7275</v>
+      </c>
+      <c r="B1491" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1491" s="1" t="s">
+        <v>7362</v>
+      </c>
+      <c r="D1491" s="1" t="s">
+        <v>7363</v>
+      </c>
+      <c r="E1491" s="1" t="s">
+        <v>7364</v>
+      </c>
+      <c r="F1491" s="1" t="s">
+        <v>7365</v>
+      </c>
+      <c r="G1491" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1492" s="1" t="s">
+        <v>7276</v>
+      </c>
+      <c r="B1492" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1492" s="1" t="s">
+        <v>7366</v>
+      </c>
+      <c r="D1492" s="1" t="s">
+        <v>7367</v>
+      </c>
+      <c r="E1492" s="1" t="s">
+        <v>7368</v>
+      </c>
+      <c r="F1492" s="1" t="s">
+        <v>7369</v>
+      </c>
+      <c r="G1492" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1493" s="1" t="s">
+        <v>7277</v>
+      </c>
+      <c r="B1493" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1493" s="1" t="s">
+        <v>6317</v>
+      </c>
+      <c r="D1493" s="1" t="s">
+        <v>7370</v>
+      </c>
+      <c r="E1493" s="1" t="s">
+        <v>7371</v>
+      </c>
+      <c r="F1493" s="1" t="s">
+        <v>7372</v>
+      </c>
+      <c r="G1493" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1494" s="1" t="s">
+        <v>7278</v>
+      </c>
+      <c r="B1494" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1494" s="1" t="s">
+        <v>7373</v>
+      </c>
+      <c r="D1494" s="1" t="s">
+        <v>7374</v>
+      </c>
+      <c r="E1494" s="1" t="s">
+        <v>7376</v>
+      </c>
+      <c r="F1494" s="1" t="s">
+        <v>7375</v>
+      </c>
+      <c r="G1494" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1495" s="1" t="s">
+        <v>7279</v>
+      </c>
+      <c r="B1495" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1495" s="1" t="s">
+        <v>4098</v>
+      </c>
+      <c r="D1495" s="1" t="s">
+        <v>7377</v>
+      </c>
+      <c r="E1495" s="1" t="s">
+        <v>7378</v>
+      </c>
+      <c r="F1495" s="1" t="s">
+        <v>7379</v>
+      </c>
+      <c r="G1495" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1496" s="1" t="s">
+        <v>7280</v>
+      </c>
+      <c r="B1496" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1496" s="1" t="s">
+        <v>7380</v>
+      </c>
+      <c r="D1496" s="1" t="s">
+        <v>7381</v>
+      </c>
+      <c r="E1496" s="1" t="s">
+        <v>7382</v>
+      </c>
+      <c r="F1496" s="1" t="s">
+        <v>7383</v>
+      </c>
+      <c r="G1496" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1497" s="1" t="s">
+        <v>7281</v>
+      </c>
+      <c r="B1497" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1497" s="1" t="s">
+        <v>7384</v>
+      </c>
+      <c r="D1497" s="1" t="s">
+        <v>7385</v>
+      </c>
+      <c r="E1497" s="1" t="s">
+        <v>7386</v>
+      </c>
+      <c r="F1497" s="1" t="s">
+        <v>7387</v>
+      </c>
+      <c r="G1497" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1498" s="1" t="s">
+        <v>7282</v>
+      </c>
+      <c r="B1498" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1498" s="1" t="s">
+        <v>7388</v>
+      </c>
+      <c r="D1498" s="1" t="s">
+        <v>7389</v>
+      </c>
+      <c r="E1498" s="1" t="s">
+        <v>7390</v>
+      </c>
+      <c r="F1498" s="1" t="s">
+        <v>7391</v>
+      </c>
+      <c r="G1498" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1499" s="1" t="s">
+        <v>7283</v>
+      </c>
+      <c r="B1499" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1499" s="1" t="s">
+        <v>7392</v>
+      </c>
+      <c r="D1499" s="1" t="s">
+        <v>7393</v>
+      </c>
+      <c r="E1499" s="1" t="s">
+        <v>7394</v>
+      </c>
+      <c r="F1499" s="1" t="s">
+        <v>7395</v>
+      </c>
+      <c r="G1499" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1500" s="1" t="s">
+        <v>7284</v>
+      </c>
+      <c r="B1500" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1500" s="1" t="s">
+        <v>7396</v>
+      </c>
+      <c r="D1500" s="1" t="s">
+        <v>7397</v>
+      </c>
+      <c r="E1500" s="1" t="s">
+        <v>7398</v>
+      </c>
+      <c r="F1500" s="1" t="s">
+        <v>7399</v>
+      </c>
+      <c r="G1500" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1501" s="1" t="s">
+        <v>7285</v>
+      </c>
+      <c r="B1501" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1501" s="1" t="s">
+        <v>7400</v>
+      </c>
+      <c r="D1501" s="1" t="s">
+        <v>7401</v>
+      </c>
+      <c r="E1501" s="1" t="s">
+        <v>7402</v>
+      </c>
+      <c r="F1501" s="1" t="s">
+        <v>7403</v>
+      </c>
+      <c r="G1501" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>